<commit_message>
added in basic language translation substitution with proof of concept for Spanish.  The current deja vu font does not support Chinese characters, so support for font substitution is next step.
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,19 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15CFB13D-B035-4113-AAFE-63B39D797BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{340D042C-E89A-4D0B-B262-7EFD4E0BB180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
+    <sheet name="languages" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">languages!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="314">
   <si>
     <t>name</t>
   </si>
@@ -646,9 +650,6 @@
     <t>Street connectivity is an important aspect of walkability, as it affects proximity and convenient routes to destinations.</t>
   </si>
   <si>
-    <t>Walkable neighbourhoods underpin a liveable city, providing opportunities for healthy sustainable lifestyles.  Walkability encompasses accessibility of services and amenities and is influenced by policies determining land use mix and population density, as well as street connectivity.  Sufficient density of dwellings and population is critical for walkability, because it determines the viability of local destinations and adequate public transport service.</t>
-  </si>
-  <si>
     <t>infographic</t>
   </si>
   <si>
@@ -668,6 +669,306 @@
   </si>
   <si>
     <t>Insert some content here maybe??</t>
+  </si>
+  <si>
+    <t>El informe completo, incluidos los datos y los métodos, se ha publicado en INSERTAR LA CITA DE LA SERIE Y LA URL | Datos de población: Schiavina, M. et al. (2019): GHS population grid multitemporal (1975, 1990, 2000, 2015) R2019A. European Commission, Joint Research Centre (JRC). https://doi.org/10.2905/42E8BE89-54FF-464E-BE7B-BF9E64DA5218 | Límites urbanos: Florczyk, A. et al. (2019): GHS Urban Centre Database 2015, multitemporal and multidimensional attributes, R2019A. European Commission, Joint Research Centre (JRC). https://data.jrc.ec.europa.eu/dataset/53473144-b88c-44bc-b4a3-4583ed1f547e | Características urbanas: OpenStreetMap contributors. Openstreetmap (2020). https://planet.osm.org/pbf/planet-200803.osm.pbf.torrent | Escala de colores: Crameri, F. (2018). Scientific colour-maps (3.0.4). Zenodo. https://doi.org/10.5281/zenodo.1287763</t>
+  </si>
+  <si>
+    <t>Las estrategias de diseño urbano pueden crear vecindarios aptos para caminar y andar en bicicleta con espacios públicos abiertos accesibles, que se asocian con mayores niveles de actividad física y menor riesgo de enfermedades crónicas. Un objetivo de política para el acceso residencial a espacios públicos abiertos dentro de los 400 m es ampliamente consistente con la evidencia sobre el fomento de caminar. Sin embargo, el acceso a parques más grandes también puede ser importante, y se deben considerar diferentes velocidades y habilidades para caminar.</t>
+  </si>
+  <si>
+    <t>Objetivos para el uso del transporte público</t>
+  </si>
+  <si>
+    <t>Requisitos mínimos para acceder al transporte público</t>
+  </si>
+  <si>
+    <t>Requisitos para la distribución del empleo en la ciudad</t>
+  </si>
+  <si>
+    <t>Requisitos para el acceso del transporte público al empleo y las infraestructuras</t>
+  </si>
+  <si>
+    <t>Evidencia de salud respaldada</t>
+  </si>
+  <si>
+    <t>Objetivo medible</t>
+  </si>
+  <si>
+    <t>Estándar específico</t>
+  </si>
+  <si>
+    <t>Política identificada</t>
+  </si>
+  <si>
+    <t>El fácil acceso al transporte público frecuente es un determinante clave de los sistemas de transporte saludables y sostenibles. La ubicación de la vivienda y el empleo cerca del transporte público aumenta la participación modal de los viajes en transporte público, lo que fomenta la caminata relacionada con el transporte; ofrecer acceso a empleos y servicios regionales; mejorar la salud, el desarrollo económico y la inclusión social; y reducir la contaminación y las emisiones de carbono.</t>
+  </si>
+  <si>
+    <t>Easy access to frequent public transport is a key determinant of healthy and sustainable transport systems. Placing housing and employment near public transport increases the mode share of public transport trips, thus encouraging transport-related walking; offering access to regional jobs and services; improving health, economic development, and social inclusiveness; and reducing pollution and carbon emissions.</t>
+  </si>
+  <si>
+    <t>¿Insertar algún contenido aquí tal vez?</t>
+  </si>
+  <si>
+    <t>La conectividad de las calles es un aspecto importante de la caminabilidad, ya que afecta la proximidad y las rutas convenientes a los destinos.</t>
+  </si>
+  <si>
+    <t>Acceso al transporte público entre semana a 500 m</t>
+  </si>
+  <si>
+    <t>Densidad de intersección de calles</t>
+  </si>
+  <si>
+    <t>Objetivos de participación ciclista</t>
+  </si>
+  <si>
+    <t>Objetivos de participación a pie</t>
+  </si>
+  <si>
+    <t>Provisión de infraestructura ciclista</t>
+  </si>
+  <si>
+    <t>Provisión de infraestructura peatonal</t>
+  </si>
+  <si>
+    <t>Restricciones de estacionamiento para desalentar el uso del automóvil</t>
+  </si>
+  <si>
+    <t>Conectividad de calles o proporción de pedshed</t>
+  </si>
+  <si>
+    <t>Requisitos de densidad de vivienda</t>
+  </si>
+  <si>
+    <t>Políticas de contaminación del aire relacionadas con el transporte y la planificación del uso del suelo</t>
+  </si>
+  <si>
+    <t>¿Información sobre el gasto público en infraestructura para diferentes modos de transporte?</t>
+  </si>
+  <si>
+    <t>¿Se ha incorporado la evaluación del impacto en la salud en la política o legislación urbana/de transporte?</t>
+  </si>
+  <si>
+    <t>¿Las políticas metropolitanas de transporte  especifica acciones enfocadas en la salud?</t>
+  </si>
+  <si>
+    <t>¿Las políticas urbanas metropolitanas especifica acciones enfocadas en la salud?</t>
+  </si>
+  <si>
+    <t>¿La transporte y planificación urbana combinados en un departamento gubernamental?</t>
+  </si>
+  <si>
+    <t>Comparación de 25 ciudades</t>
+  </si>
+  <si>
+    <t>La presencia de las politícas de transporte</t>
+  </si>
+  <si>
+    <t>¹ La clasificacíon de la calidad de las políticas se recompensa las políticas específicas, mensurables y alineados con evidencia de consenso de las ciudades saludes</t>
+  </si>
+  <si>
+    <t>La calidad de las políticas ¹</t>
+  </si>
+  <si>
+    <t>La presencia de las políticas</t>
+  </si>
+  <si>
+    <t>Políticas Urbanas y Salud</t>
+  </si>
+  <si>
+    <t>Densidad poblacional</t>
+  </si>
+  <si>
+    <t>Caminabilidad</t>
+  </si>
+  <si>
+    <t>(arriba) Las estimaciones de la ciudad para el porcentaje de población con acceso a servicios dentro de los 500 metros (m) se pueden comparar con el desempeño de otras ciudades en nuestro estudio global.</t>
+  </si>
+  <si>
+    <t>Diseño urbano y características del transporte.</t>
+  </si>
+  <si>
+    <t>Infografía para insertar aquí…</t>
+  </si>
+  <si>
+    <t>Urban Policy and Built Environment Scorecard 2020</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Walkable neighbourhoods underpin a liveable city, providing opportunities for healthy sustainable lifestyles.  Walkability encompasses accessibility of services and amenities and is influenced by policies determining land use mix and population density, as well as street connectivity. Sufficient density of dwellings and population is critical for walkability, because it determines the viability of local destinations and adequate public transport service.\n\nThe below checklist reports on an analysis of {city} urban policies supporting walkable neighbourhoods, evaluating: policy presence; whether the policy had a specific aim or standard; whether it had a measurable target; and whether it was consistent with evidence on health supportive environments.</t>
+  </si>
+  <si>
+    <t>Walkable neighbourhoods underpin a liveable city, providing opportunities for healthy sustainable lifestyles.  Walkability encompasses accessibility of services and amenities and is influenced by policies determining land use mix and population density, as well as street connectivity. Sufficient density of dwellings and population is critical for walkability, because it determines the viability of local destinations and adequate public transport service.
+The below checklist reports on an analysis of {city} urban policies supporting walkable neighbourhoods, evaluating: policy presence; whether the policy had a specific aim or standard; whether it had a measurable target; and whether it was consistent with evidence on health supportive environments.</t>
+  </si>
+  <si>
+    <t>Los vecindarios transitables sustentan una ciudad habitable y brindan oportunidades para estilos de vida sostenibles y saludables. La accesibilidad para peatones abarca la accesibilidad de los servicios y las comodidades y está influenciada por las políticas que determinan la combinación de usos del suelo y la densidad de población, así como la conectividad de las calles. Una densidad suficiente de viviendas y población es fundamental para la transitabilidad, ya que determina la viabilidad de los destinos locales y un servicio de transporte público adecuado.
+La siguiente lista de verificación informa sobre un análisis de las políticas urbanas de {city} que apoyan los vecindarios transitables, evaluando: la presencia de políticas; si la política tenía un objetivo o estándar específico; si tenía un objetivo medible; y si era consistente con la evidencia sobre entornos de apoyo a la salud.</t>
+  </si>
+  <si>
+    <t>Large public open space access within 500m</t>
+  </si>
+  <si>
+    <t>Acceso a gran espacio público abierto a 500 m</t>
+  </si>
+  <si>
+    <t>Please provide a high resolution 'hero image' for this city, ideally with dimensions in the ratio of 21:10 (e.g. 2100px by 1000px)</t>
+  </si>
+  <si>
+    <t>Citation: Global Healthy &amp; Sustainable Cities Indicators Collaboration. 2022. Urban Policy and Built Environment Scorecard 2020: {city}. https://doi.org/INSERT-DOI-HERE</t>
+  </si>
+  <si>
+    <t>Tanteador de Política Urbana y Entorno Construido 2020</t>
+  </si>
+  <si>
+    <t>Ciudades Globales Saludables y Sostenibles</t>
+  </si>
+  <si>
+    <t>Citación: Global Healthy &amp; Sustainable Cities Indicators Collaboration. 2022. Urban Policy and Built Environment Scorecard 2020: {city}  (Spanish). https://doi.org/INSERT-DOI-HERE</t>
+  </si>
+  <si>
+    <t>全球健康与可持续城市</t>
+  </si>
+  <si>
+    <t>城市政策和建筑环境记分卡2020</t>
+  </si>
+  <si>
+    <t>信息图将在此处插入...</t>
+  </si>
+  <si>
+    <t>城市设计和交通特色</t>
+  </si>
+  <si>
+    <t>（上图）在我们的全球研究中，城市估计的500米（m）范围内获得便利设施的人口百分比可以与其他城市的表现进行比较。</t>
+  </si>
+  <si>
+    <t>步行性</t>
+  </si>
+  <si>
+    <t>人口密度</t>
+  </si>
+  <si>
+    <t>与卫生相关的城市政策</t>
+  </si>
+  <si>
+    <t>策略存在</t>
+  </si>
+  <si>
+    <t>政策质量¹</t>
+  </si>
+  <si>
+    <t>¹ 政策质量评级奖励与健康城市共识证据相一致的特定、可衡量的政策</t>
+  </si>
+  <si>
+    <t>传输策略清单</t>
+  </si>
+  <si>
+    <t>25 城市比较</t>
+  </si>
+  <si>
+    <t>交通和规划合并在一个政府部门？</t>
+  </si>
+  <si>
+    <t>大都市城市政策具体规定了以卫生为重点的行动？</t>
+  </si>
+  <si>
+    <t>大都市交通政策规定了以卫生为重点的行动？</t>
+  </si>
+  <si>
+    <t>将健康影响评估纳入城市/交通政策或立法？</t>
+  </si>
+  <si>
+    <t>关于政府对不同运输方式的基础设施支出的信息？</t>
+  </si>
+  <si>
+    <t>与运输和土地使用规划有关的空气污染政策</t>
+  </si>
+  <si>
+    <t>已确定策略</t>
+  </si>
+  <si>
+    <t>具体标准</t>
+  </si>
+  <si>
+    <t>可衡量的目标</t>
+  </si>
+  <si>
+    <t>健康证据支持</t>
+  </si>
+  <si>
+    <t>外壳密度要求</t>
+  </si>
+  <si>
+    <t>街道连通性或 附装 比例</t>
+  </si>
+  <si>
+    <t>停车限制，以阻止汽车使用</t>
+  </si>
+  <si>
+    <t>提供行人基础设施</t>
+  </si>
+  <si>
+    <t>提供自行车基础设施</t>
+  </si>
+  <si>
+    <t>步行参与目标</t>
+  </si>
+  <si>
+    <t>自行车参与目标</t>
+  </si>
+  <si>
+    <t>街道交叉口密度</t>
+  </si>
+  <si>
+    <t>500米范围内的平日公共交通</t>
+  </si>
+  <si>
+    <t>500米范围内的大型公共开放空间通道</t>
+  </si>
+  <si>
+    <t>街道连通性是可步行性的一个重要方面，因为它会影响到目的地的距离和便捷路线。</t>
+  </si>
+  <si>
+    <t>在这里插入一些内容也许？？</t>
+  </si>
+  <si>
+    <t>方便使用频繁的公共交通工具是健康和可持续交通系统的关键决定因素。 将住房和就业安置在公共交通工具附近会增加公共交通旅行的方式份额，从而鼓励与交通相关的步行;提供获得区域工作和服务的机会;改善健康，经济发展和社会包容性;减少污染和碳排放。</t>
+  </si>
+  <si>
+    <t>公共交通获得就业和基础设施的要求</t>
+  </si>
+  <si>
+    <t>全市就业分配要求</t>
+  </si>
+  <si>
+    <t>公共交通的最低要求</t>
+  </si>
+  <si>
+    <t>公共交通使用目标</t>
+  </si>
+  <si>
+    <t>城市设计策略可以创建步行和骑自行车友好的社区，拥有无障碍的公共开放空间，这与增加身体活动水平和降低慢性病风险有关。   住宅进入400米以内公共开放空间的政策目标与鼓励步行的证据大致一致。 但是，进入较大的公园可能也很重要，应该考虑不同的步行速度和能力。</t>
+  </si>
+  <si>
+    <t>公共开放空间出入的最低要求</t>
+  </si>
+  <si>
+    <t>包括数据和方法的完整报告已发表在INSERT SERIES CITATION &amp; URL |人口数据：Schiavina，M. et al. （2019）： GHS人口网格多期（1975， 1990， 2000， 2015） R2019A.欧盟委员会，联合研究中心（JRC）。https://doi.org/10.2905/42E8BE89-54FF-464E-BE7B-BF9E64DA5218 |城市边界：Florczyk， A. et al. （2019）：GHS城市中心数据库2015，多时间和多维属性，R2019A。欧盟委员会，联合研究中心（JRC）。https://data.jrc.ec.europa.eu/dataset/53473144-b88c-44bc-b4a3-4583ed1f547e |城市特色： OpenStreetMap 贡献者.打开街道地图 （2020）.https://planet.osm.org/pbf/planet-200803.osm.pbf.torrent |色阶： 克拉梅里， F. （2018）.科学色图 （3.0.4）.泽诺多.https://doi.org/10.5281/zenodo.1287763</t>
+  </si>
+  <si>
+    <t>适合步行的社区支撑着一个宜居的城市，为健康的可持续生活方式提供了机会。 步行性包括服务和便利设施的可访问性，并受到确定土地使用组合和人口密度以及街道连通性的政策的影响。 足够的住宅密度和人口对于 步行能力至关重要，因为它 决定了当地目的地的可行性和足够的公共交通服务。
+下面的清单报告了对支持步行社区的{city}城市政策的分析， 评估： 政策存在;政策是否有特定的目标或标准;它是否有可衡量的目标;以及它是否与健康支持环境的证据一致。</t>
+  </si>
+  <si>
+    <t>引文：全球健康与可持续城市指标合作。 城市政策与建筑环境记分卡2020：{city}. https://doi.org/INSERT-DOI-HERE</t>
+  </si>
+  <si>
+    <t>Chinese (NOT SUPPORTED)</t>
   </si>
 </sst>
 </file>
@@ -1151,10 +1452,29 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1201,7 +1521,18 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1513,8 +1844,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P155" sqref="P155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,62 +1855,62 @@
     <col min="16" max="16" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="7" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1841,8 +2173,11 @@
       <c r="O6" t="s">
         <v>29</v>
       </c>
+      <c r="P6" t="s">
+        <v>263</v>
+      </c>
       <c r="Q6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R6" t="b">
         <v>1</v>
@@ -1903,7 +2238,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1945,7 +2280,7 @@
         <v>42</v>
       </c>
       <c r="P8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Q8">
         <v>2</v>
@@ -3881,7 +4216,7 @@
         <v>42</v>
       </c>
       <c r="P42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Q42">
         <v>3</v>
@@ -3995,7 +4330,7 @@
         <v>29</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>208</v>
+        <v>258</v>
       </c>
       <c r="Q44">
         <v>2</v>
@@ -6697,7 +7032,7 @@
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B92">
         <v>4</v>
@@ -6910,7 +7245,7 @@
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B96">
         <v>4</v>
@@ -6952,7 +7287,7 @@
         <v>42</v>
       </c>
       <c r="P96" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q96">
         <v>2</v>
@@ -10208,7 +10543,7 @@
     </row>
     <row r="155" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B155">
         <v>5</v>
@@ -10250,7 +10585,9 @@
       <c r="O155" t="s">
         <v>29</v>
       </c>
-      <c r="P155" s="1"/>
+      <c r="P155" s="1" t="s">
+        <v>264</v>
+      </c>
       <c r="Q155">
         <v>2</v>
       </c>
@@ -10265,4 +10602,674 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" style="2" customWidth="1"/>
+    <col min="2" max="4" width="55" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="270" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="255" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated template with some portuguese trnaslations
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{665B66F4-9D96-4137-98BE-EA1E7F48C416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2E0B9225-0DEF-4228-B351-4C5AC8167E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="549">
   <si>
     <t>name</t>
   </si>
@@ -1679,6 +1679,18 @@
   </si>
   <si>
     <t>waree</t>
+  </si>
+  <si>
+    <t>Install</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Portuguese - Brazilian</t>
   </si>
 </sst>
 </file>
@@ -11404,11 +11416,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F62" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G63" sqref="G63"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13129,270 +13141,451 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="67" customWidth="1"/>
-    <col min="5" max="5" width="78.7109375" customWidth="1"/>
+    <col min="1" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="67" customWidth="1"/>
+    <col min="6" max="6" width="78.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>315</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>258</v>
       </c>
       <c r="B2" t="s">
+        <v>546</v>
+      </c>
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>258</v>
       </c>
       <c r="B3" t="s">
+        <v>546</v>
+      </c>
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>258</v>
       </c>
       <c r="B4" t="s">
+        <v>546</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>258</v>
       </c>
       <c r="B5" t="s">
+        <v>546</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>319</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>257</v>
       </c>
       <c r="B6" t="s">
+        <v>546</v>
+      </c>
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>257</v>
       </c>
       <c r="B7" t="s">
+        <v>546</v>
+      </c>
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>41</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>257</v>
       </c>
       <c r="B8" t="s">
+        <v>546</v>
+      </c>
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>257</v>
       </c>
       <c r="B9" t="s">
+        <v>546</v>
+      </c>
+      <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>319</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>548</v>
+      </c>
+      <c r="B10" t="s">
+        <v>546</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>548</v>
+      </c>
+      <c r="B11" t="s">
+        <v>546</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>548</v>
+      </c>
+      <c r="B12" t="s">
+        <v>546</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>548</v>
+      </c>
+      <c r="B13" t="s">
+        <v>546</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>319</v>
+      </c>
+      <c r="E13" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>414</v>
+      </c>
+      <c r="B14" t="s">
+        <v>546</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>414</v>
+      </c>
+      <c r="B15" t="s">
+        <v>546</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>414</v>
+      </c>
+      <c r="B16" t="s">
+        <v>546</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>414</v>
+      </c>
+      <c r="B17" t="s">
+        <v>546</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>319</v>
+      </c>
+      <c r="E17" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>312</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B18" t="s">
+        <v>546</v>
+      </c>
+      <c r="C18" t="s">
         <v>328</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E18" t="s">
         <v>326</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F18" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>312</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B19" t="s">
+        <v>546</v>
+      </c>
+      <c r="C19" t="s">
         <v>328</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D19" t="s">
         <v>41</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E19" t="s">
         <v>325</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F19" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>312</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B20" t="s">
+        <v>546</v>
+      </c>
+      <c r="C20" t="s">
         <v>328</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D20" t="s">
         <v>28</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E20" t="s">
         <v>327</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F20" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>312</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B21" t="s">
+        <v>546</v>
+      </c>
+      <c r="C21" t="s">
         <v>328</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D21" t="s">
         <v>319</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E21" t="s">
         <v>324</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F21" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>475</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B22" t="s">
+        <v>547</v>
+      </c>
+      <c r="C22" t="s">
         <v>544</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E22" t="s">
         <v>540</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F22" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>475</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B23" t="s">
+        <v>547</v>
+      </c>
+      <c r="C23" t="s">
         <v>544</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D23" t="s">
         <v>41</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E23" t="s">
         <v>541</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F23" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>475</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B24" t="s">
+        <v>547</v>
+      </c>
+      <c r="C24" t="s">
         <v>544</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D24" t="s">
         <v>28</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E24" t="s">
         <v>542</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F24" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>475</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B25" t="s">
+        <v>547</v>
+      </c>
+      <c r="C25" t="s">
         <v>544</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D25" t="s">
         <v>319</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E25" t="s">
         <v>543</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F25" t="s">
         <v>539</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated with justified font and example placeholder text for city description
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B2551C-216C-4905-B445-D63E2A866D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355F3C38-11E9-49D6-B7C5-148140E2728C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1567" uniqueCount="605">
   <si>
     <t>name</t>
   </si>
@@ -1862,7 +1862,13 @@
     <t>Auckland</t>
   </si>
   <si>
-    <t>Melbourne is a coastal Australian port city developed through the nineteenth to twenty-first centuries with temperate climate with rapid population growth, sprawling from relatively flat, moderately dense and well-serviced inner suburbs to peri-urban rural and bush fringe areas challenged with a lack of amenities, local employment opportunities and transport infrastructure.</t>
+    <t>Melbourne is a coastal Australian port city developed through the nineteenth to twenty-first centuries with temperate climate experiencing rapid population growth, sprawling from relatively flat, moderately dense and well-serviced inner suburbs to peri-urban rural and bush fringe areas challenged with a lack of amenities, local employment opportunities and transport infrastructure.</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Thailand's capital city Bangkok has a long history as a vibrant cultural and economic hub of the South East Asian region, undergoing dramatic growth and development since the late 20th century.</t>
   </si>
 </sst>
 </file>
@@ -2866,9 +2872,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U164"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3536,7 +3542,7 @@
         <v>21</v>
       </c>
       <c r="O12" t="s">
-        <v>27</v>
+        <v>603</v>
       </c>
       <c r="P12" t="s">
         <v>566</v>
@@ -3599,7 +3605,7 @@
         <v>21</v>
       </c>
       <c r="O13" t="s">
-        <v>27</v>
+        <v>603</v>
       </c>
       <c r="P13" t="s">
         <v>564</v>
@@ -3810,7 +3816,7 @@
         <v>20</v>
       </c>
       <c r="I17">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -3922,7 +3928,7 @@
         <v>20</v>
       </c>
       <c r="I19">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -5545,7 +5551,7 @@
         <v>165</v>
       </c>
       <c r="F47">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="G47">
         <f>E47+4</f>
@@ -5570,7 +5576,7 @@
         <v>21</v>
       </c>
       <c r="O47" t="s">
-        <v>27</v>
+        <v>603</v>
       </c>
       <c r="P47" s="1" t="s">
         <v>251</v>
@@ -8652,7 +8658,7 @@
         <v>21</v>
       </c>
       <c r="O101" t="s">
-        <v>27</v>
+        <v>603</v>
       </c>
       <c r="P101" s="1" t="s">
         <v>203</v>
@@ -10544,7 +10550,7 @@
         <v>21</v>
       </c>
       <c r="O134" t="s">
-        <v>27</v>
+        <v>603</v>
       </c>
       <c r="P134" s="1" t="s">
         <v>202</v>
@@ -12181,7 +12187,7 @@
         <v>21</v>
       </c>
       <c r="O164" t="s">
-        <v>27</v>
+        <v>603</v>
       </c>
       <c r="P164" s="1" t="s">
         <v>255</v>
@@ -12206,11 +12212,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C71" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C86" sqref="C86"/>
+      <selection pane="bottomRight" activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14021,12 +14027,15 @@
         <v>586</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>562</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed up some encoding issues for non-Latin languages, and ensured that the basic dejavu font set is loaded in addition to custom fonts for specific languages
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355F3C38-11E9-49D6-B7C5-148140E2728C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA81A23-DF04-4318-85DA-CFEA8CF9BE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">languages!$B$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scorecard_template_elements!$A$1:$S$164</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1567" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="607">
   <si>
     <t>name</t>
   </si>
@@ -1757,21 +1758,12 @@
     <t>This policy report presents findings for {city} arising from a collaborative study of 25 cities from diverse settings globally.  An analysis of policies supporting urban and transport features contributing which contribute to health, wellbeing and sustainability was conducted, and their presence in local neighbourhoods was also evaluated.</t>
   </si>
   <si>
-    <t>Urban Design and Transport Features and Policy for Health Report, {year}</t>
-  </si>
-  <si>
-    <t>Urban design and transport for health in {city}, {year}</t>
-  </si>
-  <si>
     <t>title_year</t>
   </si>
   <si>
     <t>year</t>
   </si>
   <si>
-    <t>This policy report presents findings for {city} arising from a collaborative study of 25 cities from diverse settings globally.  An analysis of policies supporting urban and transport features which contribute to health, wellbeing and sustainability was conducted, and their presence in local neighbourhoods was also evaluated.</t>
-  </si>
-  <si>
     <t>city_header</t>
   </si>
   <si>
@@ -1862,13 +1854,28 @@
     <t>Auckland</t>
   </si>
   <si>
-    <t>Melbourne is a coastal Australian port city developed through the nineteenth to twenty-first centuries with temperate climate experiencing rapid population growth, sprawling from relatively flat, moderately dense and well-serviced inner suburbs to peri-urban rural and bush fringe areas challenged with a lack of amenities, local employment opportunities and transport infrastructure.</t>
-  </si>
-  <si>
     <t>J</t>
   </si>
   <si>
-    <t>Thailand's capital city Bangkok has a long history as a vibrant cultural and economic hub of the South East Asian region, undergoing dramatic growth and development since the late 20th century.</t>
+    <t>*Please provide executive summary in Languages configuration sheet for this city*</t>
+  </si>
+  <si>
+    <t>Urban Design and Transport Indicators for Healthy and Sustainable Cities</t>
+  </si>
+  <si>
+    <t>Urban design and transport for health in {city}</t>
+  </si>
+  <si>
+    <t>This policy report presents findings for {city} arising from a collaborative study of 25 cities from diverse settings globally in {year}.  An analysis of policies supporting urban and transport features which contribute to health, wellbeing and sustainability was conducted, and their presence in local neighbourhoods was also evaluated.</t>
+  </si>
+  <si>
+    <t>25 city median</t>
+  </si>
+  <si>
+    <t>TO DO: translate series_intro</t>
+  </si>
+  <si>
+    <t>custom</t>
   </si>
 </sst>
 </file>
@@ -2872,9 +2879,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U164"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H162" sqref="H162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2965,7 +2972,7 @@
         <v>118</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I2">
         <v>20</v>
@@ -3023,7 +3030,7 @@
         <v>127</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I3">
         <v>12</v>
@@ -3082,7 +3089,7 @@
         <v>134</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I4">
         <v>12</v>
@@ -3104,7 +3111,7 @@
       </c>
       <c r="P4" t="str">
         <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(scorecard_template_elements!A4,languages!B:B,0)),"")</f>
-        <v>Urban Design and Transport Features and Policy for Health Report, {year}</v>
+        <v>Urban Design and Transport Indicators for Healthy and Sustainable Cities</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -3118,7 +3125,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3141,7 +3148,7 @@
         <v>141</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I5">
         <v>12</v>
@@ -3162,7 +3169,7 @@
         <v>22</v>
       </c>
       <c r="P5" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -3248,7 +3255,7 @@
         <v>215</v>
       </c>
       <c r="H7" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I7">
         <v>12</v>
@@ -3355,7 +3362,7 @@
         <v>280</v>
       </c>
       <c r="H9" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -3410,9 +3417,6 @@
       <c r="G10">
         <v>289</v>
       </c>
-      <c r="H10" t="s">
-        <v>20</v>
-      </c>
       <c r="I10">
         <v>0</v>
       </c>
@@ -3464,7 +3468,7 @@
         <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I11">
         <v>14</v>
@@ -3524,7 +3528,7 @@
         <v>25</v>
       </c>
       <c r="H12" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I12">
         <v>9</v>
@@ -3542,7 +3546,7 @@
         <v>21</v>
       </c>
       <c r="O12" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="P12" t="s">
         <v>566</v>
@@ -3587,7 +3591,7 @@
         <v>45</v>
       </c>
       <c r="H13" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I13">
         <v>9</v>
@@ -3605,7 +3609,7 @@
         <v>21</v>
       </c>
       <c r="O13" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="P13" t="s">
         <v>564</v>
@@ -3701,7 +3705,7 @@
         <v>68</v>
       </c>
       <c r="H15" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I15">
         <v>8</v>
@@ -3757,7 +3761,7 @@
         <v>16</v>
       </c>
       <c r="H16" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I16">
         <v>14</v>
@@ -3813,7 +3817,7 @@
         <v>24</v>
       </c>
       <c r="H17" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I17">
         <v>8</v>
@@ -3925,7 +3929,7 @@
         <v>46</v>
       </c>
       <c r="H19" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I19">
         <v>8</v>
@@ -4038,7 +4042,7 @@
         <v>62</v>
       </c>
       <c r="H21" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I21">
         <v>8</v>
@@ -4152,7 +4156,7 @@
         <v>78</v>
       </c>
       <c r="H23" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I23">
         <v>8</v>
@@ -4187,7 +4191,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -4212,7 +4216,7 @@
         <v>85</v>
       </c>
       <c r="H24" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I24">
         <v>8</v>
@@ -4233,7 +4237,7 @@
         <v>22</v>
       </c>
       <c r="P24" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="Q24">
         <v>2</v>
@@ -4272,7 +4276,7 @@
         <v>79</v>
       </c>
       <c r="H25" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I25">
         <v>8</v>
@@ -4439,7 +4443,7 @@
         <v>92</v>
       </c>
       <c r="H28" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I28">
         <v>8</v>
@@ -4499,7 +4503,7 @@
         <v>92</v>
       </c>
       <c r="H29" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I29">
         <v>8</v>
@@ -4616,7 +4620,7 @@
         <v>103</v>
       </c>
       <c r="H31" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I31">
         <v>8</v>
@@ -4676,7 +4680,7 @@
         <v>103</v>
       </c>
       <c r="H32" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I32">
         <v>8</v>
@@ -4793,7 +4797,7 @@
         <v>114</v>
       </c>
       <c r="H34" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I34">
         <v>8</v>
@@ -4853,7 +4857,7 @@
         <v>114</v>
       </c>
       <c r="H35" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I35">
         <v>8</v>
@@ -4970,7 +4974,7 @@
         <v>125</v>
       </c>
       <c r="H37" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I37">
         <v>8</v>
@@ -5030,7 +5034,7 @@
         <v>125</v>
       </c>
       <c r="H38" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I38">
         <v>8</v>
@@ -5147,7 +5151,7 @@
         <v>136</v>
       </c>
       <c r="H40" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I40">
         <v>8</v>
@@ -5207,7 +5211,7 @@
         <v>136</v>
       </c>
       <c r="H41" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I41">
         <v>8</v>
@@ -5324,7 +5328,7 @@
         <v>147</v>
       </c>
       <c r="H43" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I43">
         <v>8</v>
@@ -5384,7 +5388,7 @@
         <v>147</v>
       </c>
       <c r="H44" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I44">
         <v>8</v>
@@ -5499,7 +5503,7 @@
         <v>161</v>
       </c>
       <c r="H46" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I46">
         <v>12</v>
@@ -5558,7 +5562,7 @@
         <v>169</v>
       </c>
       <c r="H47" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I47">
         <v>9</v>
@@ -5576,7 +5580,7 @@
         <v>21</v>
       </c>
       <c r="O47" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="P47" s="1" t="s">
         <v>251</v>
@@ -5726,7 +5730,7 @@
         <v>198</v>
       </c>
       <c r="H50" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I50">
         <v>8</v>
@@ -5786,7 +5790,7 @@
         <v>203</v>
       </c>
       <c r="H51" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I51">
         <v>8</v>
@@ -5846,7 +5850,7 @@
         <v>203</v>
       </c>
       <c r="H52" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I52">
         <v>8</v>
@@ -5906,7 +5910,7 @@
         <v>203</v>
       </c>
       <c r="H53" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I53">
         <v>8</v>
@@ -5966,7 +5970,7 @@
         <v>203</v>
       </c>
       <c r="H54" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I54">
         <v>8</v>
@@ -6242,7 +6246,7 @@
         <v>216</v>
       </c>
       <c r="H59" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I59">
         <v>8</v>
@@ -6530,7 +6534,7 @@
         <v>227</v>
       </c>
       <c r="H64" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I64">
         <v>8</v>
@@ -6818,7 +6822,7 @@
         <v>238</v>
       </c>
       <c r="H69" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I69">
         <v>8</v>
@@ -7106,7 +7110,7 @@
         <v>249</v>
       </c>
       <c r="H74" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I74">
         <v>8</v>
@@ -7394,7 +7398,7 @@
         <v>260</v>
       </c>
       <c r="H79" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I79">
         <v>8</v>
@@ -7682,7 +7686,7 @@
         <v>271</v>
       </c>
       <c r="H84" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I84">
         <v>8</v>
@@ -7970,7 +7974,7 @@
         <v>282</v>
       </c>
       <c r="H89" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I89">
         <v>8</v>
@@ -8255,7 +8259,7 @@
         <v>16</v>
       </c>
       <c r="H94" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I94">
         <v>12</v>
@@ -8364,7 +8368,7 @@
         <v>16</v>
       </c>
       <c r="H96" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I96">
         <v>12</v>
@@ -8452,7 +8456,7 @@
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B98">
         <v>3</v>
@@ -8504,7 +8508,7 @@
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B99">
         <v>3</v>
@@ -8526,7 +8530,7 @@
         <v>215</v>
       </c>
       <c r="H99" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I99">
         <v>12</v>
@@ -8547,7 +8551,7 @@
         <v>27</v>
       </c>
       <c r="P99" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="Q99">
         <v>0</v>
@@ -8582,7 +8586,7 @@
         <v>16</v>
       </c>
       <c r="H100" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I100">
         <v>12</v>
@@ -8640,7 +8644,7 @@
         <v>24</v>
       </c>
       <c r="H101" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I101">
         <v>9</v>
@@ -8658,7 +8662,7 @@
         <v>21</v>
       </c>
       <c r="O101" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="P101" s="1" t="s">
         <v>203</v>
@@ -8809,7 +8813,7 @@
         <v>65</v>
       </c>
       <c r="H104" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I104">
         <v>12</v>
@@ -8869,7 +8873,7 @@
         <v>70</v>
       </c>
       <c r="H105" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I105">
         <v>8</v>
@@ -8929,7 +8933,7 @@
         <v>70</v>
       </c>
       <c r="H106" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I106">
         <v>8</v>
@@ -8989,7 +8993,7 @@
         <v>70</v>
       </c>
       <c r="H107" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I107">
         <v>8</v>
@@ -9049,7 +9053,7 @@
         <v>70</v>
       </c>
       <c r="H108" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I108">
         <v>8</v>
@@ -9324,7 +9328,7 @@
         <v>83</v>
       </c>
       <c r="H113" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I113">
         <v>8</v>
@@ -9612,7 +9616,7 @@
         <v>94</v>
       </c>
       <c r="H118" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I118">
         <v>8</v>
@@ -9900,7 +9904,7 @@
         <v>105</v>
       </c>
       <c r="H123" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I123">
         <v>8</v>
@@ -10188,7 +10192,7 @@
         <v>116</v>
       </c>
       <c r="H128" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I128">
         <v>8</v>
@@ -10474,7 +10478,7 @@
         <v>135</v>
       </c>
       <c r="H133" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I133">
         <v>12</v>
@@ -10532,7 +10536,7 @@
         <v>143</v>
       </c>
       <c r="H134" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I134">
         <v>9</v>
@@ -10550,7 +10554,7 @@
         <v>21</v>
       </c>
       <c r="O134" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="P134" s="1" t="s">
         <v>202</v>
@@ -10700,7 +10704,7 @@
         <v>196</v>
       </c>
       <c r="H137" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I137">
         <v>12</v>
@@ -10760,7 +10764,7 @@
         <v>201</v>
       </c>
       <c r="H138" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I138">
         <v>8</v>
@@ -10820,7 +10824,7 @@
         <v>201</v>
       </c>
       <c r="H139" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I139">
         <v>8</v>
@@ -10880,7 +10884,7 @@
         <v>201</v>
       </c>
       <c r="H140" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I140">
         <v>8</v>
@@ -10940,7 +10944,7 @@
         <v>201</v>
       </c>
       <c r="H141" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I141">
         <v>8</v>
@@ -11216,7 +11220,7 @@
         <v>214</v>
       </c>
       <c r="H146" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I146">
         <v>8</v>
@@ -11501,7 +11505,7 @@
         <v>23</v>
       </c>
       <c r="H151" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I151">
         <v>6</v>
@@ -12169,7 +12173,7 @@
         <v>241</v>
       </c>
       <c r="H164" t="s">
-        <v>20</v>
+        <v>606</v>
       </c>
       <c r="I164">
         <v>12</v>
@@ -12187,7 +12191,7 @@
         <v>21</v>
       </c>
       <c r="O164" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="P164" s="1" t="s">
         <v>255</v>
@@ -12203,6 +12207,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:S164" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -12212,11 +12217,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C68" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C79" sqref="C79"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12387,13 +12392,13 @@
         <v>416</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="H7" s="9"/>
     </row>
@@ -12717,7 +12722,7 @@
         <v>64</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>64</v>
+        <v>604</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>442</v>
@@ -12767,7 +12772,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>567</v>
+        <v>601</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>256</v>
@@ -12819,7 +12824,7 @@
         <v>43</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>568</v>
+        <v>602</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>247</v>
@@ -12845,7 +12850,7 @@
         <v>46</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>246</v>
@@ -13960,74 +13965,233 @@
         <v>565</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+        <v>577</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C71" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+        <v>578</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+        <v>579</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+        <v>580</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+        <v>581</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+        <v>582</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>583</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>321</v>
       </c>
@@ -14035,114 +14199,363 @@
         <v>562</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+        <v>600</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+        <v>584</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H79" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>585</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>586</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>587</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+        <v>588</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <v>589</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>590</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <v>592</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>593</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+        <v>594</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>321</v>
       </c>
@@ -14150,23 +14563,74 @@
         <v>560</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+        <v>600</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="C93" s="3" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>601</v>
+        <v>598</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed annoted band for threshold plots, instead including text for target range; also improved display of policy ratings, now label not included (so colour bar can be full height)
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A5DA16-8E7A-4B3B-8159-560AD56FE200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF553B6A-AB0C-49C8-A41D-F06839C2E480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="625">
   <si>
     <t>name</t>
   </si>
@@ -1818,9 +1818,6 @@
     <t>*Please provide executive summary in Languages configuration sheet for this city*</t>
   </si>
   <si>
-    <t>Urban Design and Transport Indicators for Healthy and Sustainable Cities</t>
-  </si>
-  <si>
     <t>Urban design and transport for health in {city}</t>
   </si>
   <si>
@@ -1869,9 +1866,6 @@
     <t>การให้คะแนนคุณภาพนโยบายให้รางวัลเฉพาะนโยบายที่วัดได้ซึ่งสอดคล้องกับหลักฐานฉันทามติในเมืองที่มีสุขภาพดี</t>
   </si>
   <si>
-    <t>Policy quality rating for having specific, measurable policies aligned with consensus evidence on healthy cities</t>
-  </si>
-  <si>
     <t>La clasificacíon de la calidad de las políticas se recompensa las políticas específicas, mensurables y alineados con evidencia de consenso de las ciudades saludes</t>
   </si>
   <si>
@@ -1896,40 +1890,51 @@
     <t>25 cities comparison by income group</t>
   </si>
   <si>
-    <t>Middle</t>
-  </si>
-  <si>
-    <t>Upper</t>
-  </si>
-  <si>
-    <t>0/6</t>
-  </si>
-  <si>
-    <t>7/19</t>
-  </si>
-  <si>
-    <t>16/19</t>
-  </si>
-  <si>
-    <t>18/19</t>
-  </si>
-  <si>
-    <t>5/6</t>
-  </si>
-  <si>
-    <t>2/6</t>
-  </si>
-  <si>
-    <t>2/19</t>
-  </si>
-  <si>
     <t xml:space="preserve">44% (11/25) </t>
   </si>
   <si>
-    <t>9/19</t>
-  </si>
-  <si>
-    <t>15/19</t>
+    <t>Upper
+/19</t>
+  </si>
+  <si>
+    <t>Middle
+/6</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>28%</t>
+  </si>
+  <si>
+    <t>64%</t>
+  </si>
+  <si>
+    <t>83%</t>
+  </si>
+  <si>
+    <t>72%</t>
+  </si>
+  <si>
+    <t>33%</t>
+  </si>
+  <si>
+    <t>8%</t>
+  </si>
+  <si>
+    <t>36%</t>
+  </si>
+  <si>
+    <t>60%</t>
+  </si>
+  <si>
+    <t>Urban Indicators and Policy for Healthy, Sustainable Cities</t>
+  </si>
+  <si>
+    <t>% of population in target range</t>
+  </si>
+  <si>
+    <t>Policy quality rating for specific, measurable policies aligned with consensus evidence on healthy cities</t>
   </si>
 </sst>
 </file>
@@ -2422,7 +2427,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2456,8 +2461,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2957,8 +2961,8 @@
   <dimension ref="A1:U180"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P62" sqref="P62"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3049,7 +3053,7 @@
         <v>118</v>
       </c>
       <c r="H2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I2">
         <v>20</v>
@@ -3107,7 +3111,7 @@
         <v>127</v>
       </c>
       <c r="H3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I3">
         <v>12</v>
@@ -3166,7 +3170,7 @@
         <v>134</v>
       </c>
       <c r="H4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I4">
         <v>12</v>
@@ -3188,7 +3192,7 @@
       </c>
       <c r="P4" t="str">
         <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(scorecard_template_elements!A4,languages!B:B,0)),"")</f>
-        <v>Urban Design and Transport Indicators for Healthy and Sustainable Cities</v>
+        <v>Urban Indicators and Policy for Healthy, Sustainable Cities</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -3205,7 +3209,7 @@
         <v>553</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>-666</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -3225,7 +3229,7 @@
         <v>141</v>
       </c>
       <c r="H5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I5">
         <v>12</v>
@@ -3332,7 +3336,7 @@
         <v>215</v>
       </c>
       <c r="H7" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I7">
         <v>12</v>
@@ -3439,7 +3443,7 @@
         <v>280</v>
       </c>
       <c r="H9" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -3545,7 +3549,7 @@
         <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I11">
         <v>14</v>
@@ -3605,7 +3609,7 @@
         <v>25</v>
       </c>
       <c r="H12" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I12">
         <v>9</v>
@@ -3668,7 +3672,7 @@
         <v>49</v>
       </c>
       <c r="H13" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I13">
         <v>9</v>
@@ -3782,7 +3786,7 @@
         <v>70</v>
       </c>
       <c r="H15" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I15">
         <v>8</v>
@@ -3838,7 +3842,7 @@
         <v>16</v>
       </c>
       <c r="H16" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I16">
         <v>14</v>
@@ -3894,7 +3898,7 @@
         <v>24</v>
       </c>
       <c r="H17" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I17">
         <v>8</v>
@@ -3929,7 +3933,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -3946,14 +3950,14 @@
         <v>25</v>
       </c>
       <c r="F18">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G18">
         <f>E18+3</f>
         <v>28</v>
       </c>
       <c r="H18" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I18">
         <v>8</v>
@@ -3971,7 +3975,7 @@
         <v>21</v>
       </c>
       <c r="O18" t="s">
-        <v>27</v>
+        <v>585</v>
       </c>
       <c r="P18" t="s">
         <v>128</v>
@@ -4066,7 +4070,7 @@
         <v>50</v>
       </c>
       <c r="H20" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I20">
         <v>8</v>
@@ -4101,7 +4105,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -4118,14 +4122,14 @@
         <v>51</v>
       </c>
       <c r="F21">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G21">
         <f>E21+3</f>
         <v>54</v>
       </c>
       <c r="H21" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I21">
         <v>8</v>
@@ -4143,7 +4147,7 @@
         <v>21</v>
       </c>
       <c r="O21" t="s">
-        <v>27</v>
+        <v>585</v>
       </c>
       <c r="P21" t="s">
         <v>128</v>
@@ -4234,7 +4238,7 @@
       </c>
       <c r="G23">
         <f>G61+3</f>
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -4293,7 +4297,7 @@
         <v>80</v>
       </c>
       <c r="H24" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I24">
         <v>8</v>
@@ -4353,7 +4357,7 @@
         <v>91</v>
       </c>
       <c r="H25" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I25">
         <v>8</v>
@@ -4413,7 +4417,7 @@
         <v>81</v>
       </c>
       <c r="H26" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I26">
         <v>8</v>
@@ -4446,123 +4450,125 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>610</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
+    <row r="27" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
         <f>D29</f>
         <v>179</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <f>E25</f>
         <v>88</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <f>D30</f>
         <v>192</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="2">
         <f>G25</f>
         <v>91</v>
       </c>
-      <c r="H27" t="s">
-        <v>592</v>
-      </c>
-      <c r="I27">
-        <v>8</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="N27" t="s">
+      <c r="H27" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="I27" s="2">
+        <v>7</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="O27" t="s">
+      <c r="O27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="P27" t="s">
+      <c r="P27" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="Q27">
-        <v>2</v>
-      </c>
-      <c r="R27" t="b">
+      <c r="Q27" s="2">
+        <v>2</v>
+      </c>
+      <c r="R27" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="S27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>609</v>
-      </c>
-      <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="S27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="2">
         <f>D30</f>
         <v>192</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <f>E27</f>
         <v>88</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <f>F23</f>
         <v>204</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="2">
         <f>G27</f>
         <v>91</v>
       </c>
-      <c r="H28" t="s">
-        <v>592</v>
-      </c>
-      <c r="I28">
-        <v>8</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="N28" t="s">
+      <c r="H28" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="I28" s="2">
+        <v>7</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2">
+        <v>0</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="O28" t="s">
+      <c r="O28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="P28" t="s">
-        <v>613</v>
-      </c>
-      <c r="Q28">
-        <v>2</v>
-      </c>
-      <c r="R28" t="b">
+      <c r="P28" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>2</v>
+      </c>
+      <c r="R28" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="S28">
+      <c r="S28" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4590,7 +4596,7 @@
       </c>
       <c r="G29">
         <f>G23-2</f>
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -4643,7 +4649,7 @@
       </c>
       <c r="G30">
         <f>G29</f>
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -4687,8 +4693,8 @@
         <v>100</v>
       </c>
       <c r="E31">
-        <f>E26+13</f>
-        <v>91</v>
+        <f>E26+16</f>
+        <v>94</v>
       </c>
       <c r="F31">
         <f>F26</f>
@@ -4696,7 +4702,7 @@
       </c>
       <c r="G31">
         <f>E31</f>
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -4742,7 +4748,7 @@
       </c>
       <c r="E32">
         <f>E31+2</f>
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F32">
         <f>D32+68</f>
@@ -4750,10 +4756,10 @@
       </c>
       <c r="G32">
         <f>E32+4</f>
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H32" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I32">
         <v>8</v>
@@ -4802,7 +4808,7 @@
       </c>
       <c r="E33">
         <f>E32</f>
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F33">
         <f>$F$23</f>
@@ -4810,10 +4816,10 @@
       </c>
       <c r="G33">
         <f>G32</f>
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H33" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I33">
         <v>8</v>
@@ -4863,7 +4869,7 @@
       </c>
       <c r="E34">
         <f>E33</f>
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F34">
         <f>$F$27</f>
@@ -4871,10 +4877,10 @@
       </c>
       <c r="G34">
         <f>G33</f>
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H34" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I34">
         <v>8</v>
@@ -4894,8 +4900,8 @@
       <c r="O34" t="s">
         <v>40</v>
       </c>
-      <c r="P34" t="s">
-        <v>614</v>
+      <c r="P34" s="12" t="s">
+        <v>613</v>
       </c>
       <c r="Q34">
         <v>3</v>
@@ -4924,7 +4930,7 @@
       </c>
       <c r="E35">
         <f>E34</f>
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F35">
         <f>$F$28</f>
@@ -4932,10 +4938,10 @@
       </c>
       <c r="G35">
         <f>G34</f>
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H35" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I35">
         <v>8</v>
@@ -4955,8 +4961,8 @@
       <c r="O35" t="s">
         <v>40</v>
       </c>
-      <c r="P35" s="12" t="s">
-        <v>615</v>
+      <c r="P35" s="13" t="s">
+        <v>614</v>
       </c>
       <c r="Q35">
         <v>3</v>
@@ -4984,7 +4990,7 @@
       </c>
       <c r="E36">
         <f>E33</f>
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F36">
         <f>D36+4</f>
@@ -4992,7 +4998,7 @@
       </c>
       <c r="G36">
         <f>E36+6</f>
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H36" t="s">
         <v>20</v>
@@ -5041,7 +5047,7 @@
       </c>
       <c r="E37">
         <f>E36+11</f>
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F37">
         <f>D37+68</f>
@@ -5049,10 +5055,10 @@
       </c>
       <c r="G37">
         <f>E37+4</f>
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H37" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I37">
         <v>8</v>
@@ -5101,7 +5107,7 @@
       </c>
       <c r="E38">
         <f>E37</f>
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F38">
         <f>$F$23</f>
@@ -5109,10 +5115,10 @@
       </c>
       <c r="G38">
         <f>G37</f>
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H38" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I38">
         <v>8</v>
@@ -5162,7 +5168,7 @@
       </c>
       <c r="E39">
         <f>E38</f>
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F39">
         <f>$F$27</f>
@@ -5170,10 +5176,10 @@
       </c>
       <c r="G39">
         <f>G38</f>
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H39" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I39">
         <v>8</v>
@@ -5193,8 +5199,8 @@
       <c r="O39" t="s">
         <v>40</v>
       </c>
-      <c r="P39" t="s">
-        <v>614</v>
+      <c r="P39" s="12" t="s">
+        <v>613</v>
       </c>
       <c r="Q39">
         <v>3</v>
@@ -5223,7 +5229,7 @@
       </c>
       <c r="E40">
         <f>E39</f>
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F40">
         <f>$F$28</f>
@@ -5231,10 +5237,10 @@
       </c>
       <c r="G40">
         <f>G39</f>
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H40" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I40">
         <v>8</v>
@@ -5254,8 +5260,8 @@
       <c r="O40" t="s">
         <v>40</v>
       </c>
-      <c r="P40" s="12" t="s">
-        <v>616</v>
+      <c r="P40" s="13" t="s">
+        <v>615</v>
       </c>
       <c r="Q40">
         <v>3</v>
@@ -5283,7 +5289,7 @@
       </c>
       <c r="E41">
         <f>E38</f>
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F41">
         <f>D41+4</f>
@@ -5291,7 +5297,7 @@
       </c>
       <c r="G41">
         <f>E41+6</f>
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H41" t="s">
         <v>20</v>
@@ -5340,7 +5346,7 @@
       </c>
       <c r="E42">
         <f>E41+11</f>
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F42">
         <f>D42+68</f>
@@ -5348,10 +5354,10 @@
       </c>
       <c r="G42">
         <f>E42+4</f>
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H42" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I42">
         <v>8</v>
@@ -5400,7 +5406,7 @@
       </c>
       <c r="E43">
         <f>E42</f>
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F43">
         <f>$F$23</f>
@@ -5408,10 +5414,10 @@
       </c>
       <c r="G43">
         <f>G42</f>
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H43" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I43">
         <v>8</v>
@@ -5461,7 +5467,7 @@
       </c>
       <c r="E44">
         <f>E43</f>
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F44">
         <f>$F$27</f>
@@ -5469,10 +5475,10 @@
       </c>
       <c r="G44">
         <f>G43</f>
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H44" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I44">
         <v>8</v>
@@ -5493,7 +5499,7 @@
         <v>40</v>
       </c>
       <c r="P44" s="13" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="Q44">
         <v>3</v>
@@ -5522,7 +5528,7 @@
       </c>
       <c r="E45">
         <f>E44</f>
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F45">
         <f>$F$28</f>
@@ -5530,10 +5536,10 @@
       </c>
       <c r="G45">
         <f>G44</f>
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H45" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I45">
         <v>8</v>
@@ -5553,7 +5559,7 @@
       <c r="O45" t="s">
         <v>40</v>
       </c>
-      <c r="P45" s="12" t="s">
+      <c r="P45" s="13" t="s">
         <v>617</v>
       </c>
       <c r="Q45">
@@ -5582,7 +5588,7 @@
       </c>
       <c r="E46">
         <f>E43</f>
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F46">
         <f>D46+4</f>
@@ -5590,7 +5596,7 @@
       </c>
       <c r="G46">
         <f>E46+6</f>
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H46" t="s">
         <v>20</v>
@@ -5639,7 +5645,7 @@
       </c>
       <c r="E47">
         <f>E46+11</f>
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F47">
         <f>D47+68</f>
@@ -5647,10 +5653,10 @@
       </c>
       <c r="G47">
         <f>E47+4</f>
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H47" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I47">
         <v>8</v>
@@ -5699,7 +5705,7 @@
       </c>
       <c r="E48">
         <f>E47</f>
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F48">
         <f>$F$23</f>
@@ -5707,10 +5713,10 @@
       </c>
       <c r="G48">
         <f>G47</f>
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H48" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I48">
         <v>8</v>
@@ -5760,7 +5766,7 @@
       </c>
       <c r="E49">
         <f>E48</f>
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F49">
         <f>$F$27</f>
@@ -5768,10 +5774,10 @@
       </c>
       <c r="G49">
         <f>G48</f>
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H49" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I49">
         <v>8</v>
@@ -5792,7 +5798,7 @@
         <v>40</v>
       </c>
       <c r="P49" s="13" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="Q49">
         <v>3</v>
@@ -5821,7 +5827,7 @@
       </c>
       <c r="E50">
         <f>E49</f>
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F50">
         <f>$F$28</f>
@@ -5829,10 +5835,10 @@
       </c>
       <c r="G50">
         <f>G49</f>
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H50" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I50">
         <v>8</v>
@@ -5852,8 +5858,8 @@
       <c r="O50" t="s">
         <v>40</v>
       </c>
-      <c r="P50" s="12" t="s">
-        <v>620</v>
+      <c r="P50" s="13" t="s">
+        <v>619</v>
       </c>
       <c r="Q50">
         <v>3</v>
@@ -5881,7 +5887,7 @@
       </c>
       <c r="E51">
         <f>E48</f>
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F51">
         <f>D51+4</f>
@@ -5889,7 +5895,7 @@
       </c>
       <c r="G51">
         <f>E51+6</f>
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H51" t="s">
         <v>20</v>
@@ -5938,7 +5944,7 @@
       </c>
       <c r="E52">
         <f>E47+11</f>
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F52">
         <f>D52+68</f>
@@ -5946,10 +5952,10 @@
       </c>
       <c r="G52">
         <f>E52+4</f>
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H52" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I52">
         <v>8</v>
@@ -5998,7 +6004,7 @@
       </c>
       <c r="E53">
         <f>E52</f>
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F53">
         <f>$F$23</f>
@@ -6006,10 +6012,10 @@
       </c>
       <c r="G53">
         <f>G52</f>
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H53" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I53">
         <v>8</v>
@@ -6030,7 +6036,7 @@
         <v>40</v>
       </c>
       <c r="P53" t="s">
-        <v>621</v>
+        <v>610</v>
       </c>
       <c r="Q53">
         <v>3</v>
@@ -6059,7 +6065,7 @@
       </c>
       <c r="E54">
         <f>E53</f>
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F54">
         <f>$F$27</f>
@@ -6067,10 +6073,10 @@
       </c>
       <c r="G54">
         <f>G53</f>
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H54" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I54">
         <v>8</v>
@@ -6091,7 +6097,7 @@
         <v>40</v>
       </c>
       <c r="P54" s="13" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="Q54">
         <v>3</v>
@@ -6120,7 +6126,7 @@
       </c>
       <c r="E55">
         <f>E54</f>
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F55">
         <f>$F$28</f>
@@ -6128,10 +6134,10 @@
       </c>
       <c r="G55">
         <f>G54</f>
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H55" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I55">
         <v>8</v>
@@ -6151,8 +6157,8 @@
       <c r="O55" t="s">
         <v>40</v>
       </c>
-      <c r="P55" s="14" t="s">
-        <v>622</v>
+      <c r="P55" s="13" t="s">
+        <v>620</v>
       </c>
       <c r="Q55">
         <v>3</v>
@@ -6180,7 +6186,7 @@
       </c>
       <c r="E56">
         <f>E53</f>
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F56">
         <f>D56+4</f>
@@ -6188,7 +6194,7 @@
       </c>
       <c r="G56">
         <f>E56+6</f>
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="H56" t="s">
         <v>20</v>
@@ -6237,7 +6243,7 @@
       </c>
       <c r="E57">
         <f>E52+11</f>
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F57">
         <f>D57+68</f>
@@ -6245,10 +6251,10 @@
       </c>
       <c r="G57">
         <f>E57+4</f>
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H57" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I57">
         <v>8</v>
@@ -6297,7 +6303,7 @@
       </c>
       <c r="E58">
         <f>E57</f>
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F58">
         <f>$F$23</f>
@@ -6305,10 +6311,10 @@
       </c>
       <c r="G58">
         <f>G57</f>
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H58" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I58">
         <v>8</v>
@@ -6358,7 +6364,7 @@
       </c>
       <c r="E59">
         <f>E58</f>
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F59">
         <f>$F$27</f>
@@ -6366,10 +6372,10 @@
       </c>
       <c r="G59">
         <f>G58</f>
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H59" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I59">
         <v>8</v>
@@ -6389,8 +6395,8 @@
       <c r="O59" t="s">
         <v>40</v>
       </c>
-      <c r="P59" s="12" t="s">
-        <v>619</v>
+      <c r="P59" s="13" t="s">
+        <v>618</v>
       </c>
       <c r="Q59">
         <v>3</v>
@@ -6419,7 +6425,7 @@
       </c>
       <c r="E60">
         <f>E59</f>
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F60">
         <f>$F$28</f>
@@ -6427,10 +6433,10 @@
       </c>
       <c r="G60">
         <f>G59</f>
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H60" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I60">
         <v>8</v>
@@ -6450,8 +6456,8 @@
       <c r="O60" t="s">
         <v>40</v>
       </c>
-      <c r="P60" s="12" t="s">
-        <v>623</v>
+      <c r="P60" s="13" t="s">
+        <v>621</v>
       </c>
       <c r="Q60">
         <v>3</v>
@@ -6479,7 +6485,7 @@
       </c>
       <c r="E61">
         <f>E58</f>
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F61">
         <f>D61+4</f>
@@ -6487,7 +6493,7 @@
       </c>
       <c r="G61">
         <f>E61+6</f>
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="H61" t="s">
         <v>20</v>
@@ -6535,17 +6541,17 @@
       </c>
       <c r="E62">
         <f>G23+6</f>
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F62">
         <v>94</v>
       </c>
       <c r="G62">
         <f>E62+3</f>
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="H62" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I62">
         <v>12</v>
@@ -6594,17 +6600,17 @@
       </c>
       <c r="E63">
         <f>G62+4</f>
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="F63">
         <v>203</v>
       </c>
       <c r="G63">
         <f>E63+4</f>
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="H63" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I63">
         <v>9</v>
@@ -6772,7 +6778,7 @@
         <v>198</v>
       </c>
       <c r="H66" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I66">
         <v>8</v>
@@ -6832,7 +6838,7 @@
         <v>203</v>
       </c>
       <c r="H67" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I67">
         <v>8</v>
@@ -6892,7 +6898,7 @@
         <v>203</v>
       </c>
       <c r="H68" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I68">
         <v>8</v>
@@ -6952,7 +6958,7 @@
         <v>203</v>
       </c>
       <c r="H69" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I69">
         <v>8</v>
@@ -7012,7 +7018,7 @@
         <v>203</v>
       </c>
       <c r="H70" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I70">
         <v>8</v>
@@ -7288,7 +7294,7 @@
         <v>216</v>
       </c>
       <c r="H75" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I75">
         <v>8</v>
@@ -7576,7 +7582,7 @@
         <v>227</v>
       </c>
       <c r="H80" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I80">
         <v>8</v>
@@ -7864,7 +7870,7 @@
         <v>238</v>
       </c>
       <c r="H85" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I85">
         <v>8</v>
@@ -8152,7 +8158,7 @@
         <v>249</v>
       </c>
       <c r="H90" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I90">
         <v>8</v>
@@ -8440,7 +8446,7 @@
         <v>260</v>
       </c>
       <c r="H95" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I95">
         <v>8</v>
@@ -8728,7 +8734,7 @@
         <v>271</v>
       </c>
       <c r="H100" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I100">
         <v>8</v>
@@ -9016,7 +9022,7 @@
         <v>282</v>
       </c>
       <c r="H105" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I105">
         <v>8</v>
@@ -9301,7 +9307,7 @@
         <v>16</v>
       </c>
       <c r="H110" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I110">
         <v>12</v>
@@ -9410,7 +9416,7 @@
         <v>16</v>
       </c>
       <c r="H112" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I112">
         <v>12</v>
@@ -9572,7 +9578,7 @@
         <v>215</v>
       </c>
       <c r="H115" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I115">
         <v>12</v>
@@ -9628,7 +9634,7 @@
         <v>16</v>
       </c>
       <c r="H116" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I116">
         <v>12</v>
@@ -9686,7 +9692,7 @@
         <v>24</v>
       </c>
       <c r="H117" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I117">
         <v>9</v>
@@ -9855,7 +9861,7 @@
         <v>65</v>
       </c>
       <c r="H120" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I120">
         <v>12</v>
@@ -9915,7 +9921,7 @@
         <v>70</v>
       </c>
       <c r="H121" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I121">
         <v>8</v>
@@ -9975,7 +9981,7 @@
         <v>70</v>
       </c>
       <c r="H122" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I122">
         <v>8</v>
@@ -10035,7 +10041,7 @@
         <v>70</v>
       </c>
       <c r="H123" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I123">
         <v>8</v>
@@ -10095,7 +10101,7 @@
         <v>70</v>
       </c>
       <c r="H124" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I124">
         <v>8</v>
@@ -10370,7 +10376,7 @@
         <v>83</v>
       </c>
       <c r="H129" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I129">
         <v>8</v>
@@ -10658,7 +10664,7 @@
         <v>94</v>
       </c>
       <c r="H134" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I134">
         <v>8</v>
@@ -10946,7 +10952,7 @@
         <v>105</v>
       </c>
       <c r="H139" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I139">
         <v>8</v>
@@ -11234,7 +11240,7 @@
         <v>116</v>
       </c>
       <c r="H144" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I144">
         <v>8</v>
@@ -11520,7 +11526,7 @@
         <v>135</v>
       </c>
       <c r="H149" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I149">
         <v>12</v>
@@ -11578,7 +11584,7 @@
         <v>143</v>
       </c>
       <c r="H150" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I150">
         <v>9</v>
@@ -11746,7 +11752,7 @@
         <v>196</v>
       </c>
       <c r="H153" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I153">
         <v>12</v>
@@ -11806,7 +11812,7 @@
         <v>201</v>
       </c>
       <c r="H154" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I154">
         <v>8</v>
@@ -11866,7 +11872,7 @@
         <v>201</v>
       </c>
       <c r="H155" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I155">
         <v>8</v>
@@ -11926,7 +11932,7 @@
         <v>201</v>
       </c>
       <c r="H156" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I156">
         <v>8</v>
@@ -11986,7 +11992,7 @@
         <v>201</v>
       </c>
       <c r="H157" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I157">
         <v>8</v>
@@ -12262,7 +12268,7 @@
         <v>214</v>
       </c>
       <c r="H162" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I162">
         <v>8</v>
@@ -12547,7 +12553,7 @@
         <v>23</v>
       </c>
       <c r="H167" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I167">
         <v>6</v>
@@ -13215,7 +13221,7 @@
         <v>241</v>
       </c>
       <c r="H180" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I180">
         <v>12</v>
@@ -13260,10 +13266,10 @@
   <dimension ref="A1:H97"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13644,7 +13650,7 @@
         <v>415</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>415</v>
+        <v>623</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>423</v>
@@ -13704,7 +13710,7 @@
         <v>449</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="H18" s="9"/>
     </row>
@@ -13761,10 +13767,10 @@
         <v>315</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>433</v>
@@ -13814,7 +13820,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>587</v>
+        <v>622</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>251</v>
@@ -13866,7 +13872,7 @@
         <v>43</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>242</v>
@@ -14016,25 +14022,25 @@
         <v>314</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>365</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -14045,10 +14051,10 @@
         <v>58</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>597</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>598</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>364</v>
@@ -14057,10 +14063,10 @@
         <v>364</v>
       </c>
       <c r="G32" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="H32" s="3" t="s">
         <v>599</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -14068,25 +14074,25 @@
         <v>314</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>603</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>604</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>605</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>365</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -14123,7 +14129,7 @@
         <v>62</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>235</v>
@@ -14141,56 +14147,56 @@
         <v>264</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>314</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>612</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>314</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -15085,22 +15091,22 @@
         <v>551</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added in draft alignment of cities with potential translation languages
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF553B6A-AB0C-49C8-A41D-F06839C2E480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C41A6B-ABDB-4B6C-924D-B18A9BD60A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
     <sheet name="languages" sheetId="2" r:id="rId2"/>
     <sheet name="fonts" sheetId="3" r:id="rId3"/>
+    <sheet name="translations" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">languages!$B$1:$D$1</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="640">
   <si>
     <t>name</t>
   </si>
@@ -1901,9 +1902,6 @@
 /6</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>28%</t>
   </si>
   <si>
@@ -1935,13 +1933,61 @@
   </si>
   <si>
     <t>Policy quality rating for specific, measurable policies aligned with consensus evidence on healthy cities</t>
+  </si>
+  <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Vietnamese</t>
+  </si>
+  <si>
+    <t>Tamil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portuguese </t>
+  </si>
+  <si>
+    <t>Māori</t>
+  </si>
+  <si>
+    <t>Kanuri</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Gaelic</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Dutch</t>
+  </si>
+  <si>
+    <t>Danish</t>
+  </si>
+  <si>
+    <t>Czech</t>
+  </si>
+  <si>
+    <t>Chinese (traditional)</t>
+  </si>
+  <si>
+    <t>Catalan / Valencian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2072,6 +2118,26 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2258,7 +2324,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2382,6 +2448,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2427,7 +2508,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2460,8 +2541,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2960,9 +3073,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U180"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O22" sqref="O22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P39" sqref="P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4900,8 +5013,8 @@
       <c r="O34" t="s">
         <v>40</v>
       </c>
-      <c r="P34" s="12" t="s">
-        <v>613</v>
+      <c r="P34" s="13" t="s">
+        <v>624</v>
       </c>
       <c r="Q34">
         <v>3</v>
@@ -4962,7 +5075,7 @@
         <v>40</v>
       </c>
       <c r="P35" s="13" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="Q35">
         <v>3</v>
@@ -5199,8 +5312,8 @@
       <c r="O39" t="s">
         <v>40</v>
       </c>
-      <c r="P39" s="12" t="s">
-        <v>613</v>
+      <c r="P39" s="13" t="s">
+        <v>624</v>
       </c>
       <c r="Q39">
         <v>3</v>
@@ -5261,7 +5374,7 @@
         <v>40</v>
       </c>
       <c r="P40" s="13" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="Q40">
         <v>3</v>
@@ -5499,7 +5612,7 @@
         <v>40</v>
       </c>
       <c r="P44" s="13" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="Q44">
         <v>3</v>
@@ -5560,7 +5673,7 @@
         <v>40</v>
       </c>
       <c r="P45" s="13" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Q45">
         <v>3</v>
@@ -5798,7 +5911,7 @@
         <v>40</v>
       </c>
       <c r="P49" s="13" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Q49">
         <v>3</v>
@@ -5859,7 +5972,7 @@
         <v>40</v>
       </c>
       <c r="P50" s="13" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="Q50">
         <v>3</v>
@@ -6097,7 +6210,7 @@
         <v>40</v>
       </c>
       <c r="P54" s="13" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Q54">
         <v>3</v>
@@ -6158,7 +6271,7 @@
         <v>40</v>
       </c>
       <c r="P55" s="13" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="Q55">
         <v>3</v>
@@ -6396,7 +6509,7 @@
         <v>40</v>
       </c>
       <c r="P59" s="13" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Q59">
         <v>3</v>
@@ -6457,7 +6570,7 @@
         <v>40</v>
       </c>
       <c r="P60" s="13" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q60">
         <v>3</v>
@@ -6540,15 +6653,15 @@
         <v>7</v>
       </c>
       <c r="E62">
-        <f>G23+6</f>
-        <v>166</v>
+        <f>G23+3</f>
+        <v>163</v>
       </c>
       <c r="F62">
         <v>94</v>
       </c>
       <c r="G62">
         <f>E62+3</f>
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H62" t="s">
         <v>591</v>
@@ -6600,14 +6713,14 @@
       </c>
       <c r="E63">
         <f>G62+4</f>
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F63">
         <v>203</v>
       </c>
       <c r="G63">
         <f>E63+4</f>
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H63" t="s">
         <v>591</v>
@@ -13269,7 +13382,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
+      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13650,7 +13763,7 @@
         <v>415</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>423</v>
@@ -13820,7 +13933,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>251</v>
@@ -14077,7 +14190,7 @@
         <v>595</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>602</v>
@@ -16259,4 +16372,695 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4326381-5013-44C7-92E7-E6B9FE8B43CF}">
+  <dimension ref="A1:Q26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="17" width="11.42578125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="23"/>
+      <c r="B1" s="22" t="s">
+        <v>639</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>638</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>637</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>636</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>635</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>634</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>633</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>632</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>631</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>630</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>629</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>628</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q1" s="21" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>564</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>565</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>582</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>546</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>583</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>584</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14" t="s">
+        <v>625</v>
+      </c>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>573</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>625</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+    </row>
+    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>571</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>572</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>580</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14" t="s">
+        <v>625</v>
+      </c>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>625</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+    </row>
+    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>578</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>625</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+    </row>
+    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>579</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>625</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+    </row>
+    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>581</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>574</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14" t="s">
+        <v>625</v>
+      </c>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+    </row>
+    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>568</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>549</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+    </row>
+    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="B22" s="15"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+    </row>
+    <row r="23" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>548</v>
+      </c>
+      <c r="B23" s="15"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="Q23" s="14"/>
+    </row>
+    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>570</v>
+      </c>
+      <c r="B24" s="15"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>563</v>
+      </c>
+      <c r="B25" s="15"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14" t="s">
+        <v>625</v>
+      </c>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="14"/>
+    </row>
+    <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>569</v>
+      </c>
+      <c r="B26" s="15"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14" t="s">
+        <v>625</v>
+      </c>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
saved mock translation of Danish undertaken using MS Word as example for how this could work
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593496A3-A0EC-42A6-96B1-7251CDBE959F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489A25F1-3DB0-4502-A15E-BCA43FAD251B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3885" yWindow="4365" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="translations" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">languages!$B$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">languages!$B$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scorecard_template_elements!$A$1:$T$170</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="466">
   <si>
     <t>name</t>
   </si>
@@ -1225,6 +1225,225 @@
   </si>
   <si>
     <t>Please provide a high resolution 'hero image' for this city, ideally in .jpg format with dimensions in the ratio of 21:10 (e.g. 2100px by 1000px)</t>
+  </si>
+  <si>
+    <t>Fødevaremarkedet</t>
+  </si>
+  <si>
+    <t>Bekvemmelighed</t>
+  </si>
+  <si>
+    <t>Ethvert offentligt åbent rum</t>
+  </si>
+  <si>
+    <t>Stort offentligt åbent rum</t>
+  </si>
+  <si>
+    <t>Stop for offentlig transport</t>
+  </si>
+  <si>
+    <t>Offentlig transport med rutekørsel</t>
+  </si>
+  <si>
+    <t>Offentlig transport med rutekørsel (ikke evalueret)</t>
+  </si>
+  <si>
+    <t>Nabolag walkability i forhold til 25 byer</t>
+  </si>
+  <si>
+    <t>Lav</t>
+  </si>
+  <si>
+    <t>Gennemsnitlig</t>
+  </si>
+  <si>
+    <t>Høj</t>
+  </si>
+  <si>
+    <t>Procentdel af befolkningen med adgang til offentlig transport</t>
+  </si>
+  <si>
+    <t>% befolkning inden for 500 mio. offentlig transport med 20 min eller bedre gennemsnitlig ugedagsfrekvens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% befolkning inden for 500 m af det offentlige åbne område på 1,5 ha eller derover </t>
+  </si>
+  <si>
+    <t>% af befolkningen i optimalt interval</t>
+  </si>
+  <si>
+    <t>Identificerede politikker</t>
+  </si>
+  <si>
+    <t>Befolkning %med adgangmed i500m til...</t>
+  </si>
+  <si>
+    <t>Befolkningstætheden i nabolaget (pr. km²)</t>
+  </si>
+  <si>
+    <t>Tæthed i vejkryds i nabolaget (pr. km²)</t>
+  </si>
+  <si>
+    <t>25 by median</t>
+  </si>
+  <si>
+    <t>Globalt samarbejde om sunde og bæredygtige byindikatorer</t>
+  </si>
+  <si>
+    <t>Indikatorer for sunde og bæredygtige byer: Kort rapport</t>
+  </si>
+  <si>
+    <t>Infografik, der skal indsættes her ...</t>
+  </si>
+  <si>
+    <t>Indikatorer for sunde og bæredygtige byer: {city}</t>
+  </si>
+  <si>
+    <t>(nedenfor) By skøn for procentdel af befolkningen med adgang til faciliteter inden for 500 meter (m).</t>
+  </si>
+  <si>
+    <t>Befolkningstæthed</t>
+  </si>
+  <si>
+    <t>Optimale intervaller, der er nævnt i ovenstående plottekster, er baseret på modellering af Cerin et al. (2022) af de byggede miljøfunktioner, der er nødvendige for at nå Verdenssundhedsorganisationens mål om en ≥15% relativ reduktion i utilstrækkelig fysisk aktivitet gennem gang (se https://www.who.int/news-room/initiatives/gappa ).</t>
+  </si>
+  <si>
+    <t>Politisk tilstedeværelse</t>
+  </si>
+  <si>
+    <t>Bydesign- og transportpolitik, der støtter sundhed og sustinabilitet, og som er</t>
+  </si>
+  <si>
+    <t>Politikkvalitet</t>
+  </si>
+  <si>
+    <t>Politikkvalitetsvurdering for specifikke, målbare politikker, der er i overensstemmelse med konsensusbevis om sunde byer</t>
+  </si>
+  <si>
+    <t>Krav til byplanlægning</t>
+  </si>
+  <si>
+    <t>25 byer sammenligning efter indkomstgruppe</t>
+  </si>
+  <si>
+    <t>Midt/6</t>
+  </si>
+  <si>
+    <t>Høj/19</t>
+  </si>
+  <si>
+    <t>Specifikke sundhedsfokuserede foranstaltninger i storbyens bypolitik</t>
+  </si>
+  <si>
+    <t>Specifikke sundhedsfokuserede foranstaltninger i storbyens transportpolitik</t>
+  </si>
+  <si>
+    <t>Krav til sundhedskonsekvensanalyse i by-/transportpolitik/lovgivning</t>
+  </si>
+  <si>
+    <t>Oplysninger om de offentlige udgifter til infrastruktur for forskellige transportformer</t>
+  </si>
+  <si>
+    <t>Luftforureningspolitikker i forbindelse med transportplanlægning</t>
+  </si>
+  <si>
+    <t>Luftforureningspolitikker i forbindelse med fysisk planlægning</t>
+  </si>
+  <si>
+    <t>Walkable kvarterer giver muligheder for en sund, bæredygtig livsstil og opfyldelse af retningslinjer for fysisk aktivitet. Walkable neighourhoods har tilstrækkelig tæthed af boliger og befolkning (men ikke hyper-tæthed) til at støtte lokale destinationer og passende offentlig transport. Walkable kvarterer har også blandet arealanvendelse og high street tilslutningsmuligheder, for at sikre nærliggende og bekvem adgang til destinationer. Fodgængerinfrastruktur af høj kvalitet og reduktion af trafikken gennem styring af efterspørgslen efter brug af biler kan også tilskynde til at gå til transport.</t>
+  </si>
+  <si>
+    <t>Gangbarhedspolitik</t>
+  </si>
+  <si>
+    <t>Politik for offentlig transport</t>
+  </si>
+  <si>
+    <t>Politik for offentligt åbent rum</t>
+  </si>
+  <si>
+    <t>Politik identificeret</t>
+  </si>
+  <si>
+    <t>Specifik standard eller mål</t>
+  </si>
+  <si>
+    <t>Målbart mål</t>
+  </si>
+  <si>
+    <t>I overensstemmelse med sundhedsbeviser</t>
+  </si>
+  <si>
+    <t>Krav til boligtæthed</t>
+  </si>
+  <si>
+    <t>Krav til gadeforbindelse</t>
+  </si>
+  <si>
+    <t>Parkeringsrestriktioner for at modvirke bilbrug</t>
+  </si>
+  <si>
+    <t>Levering af fodgængerinfrastruktur</t>
+  </si>
+  <si>
+    <t>Levering af cykelinfrastruktur</t>
+  </si>
+  <si>
+    <t>Gå deltagelse mål</t>
+  </si>
+  <si>
+    <t>Mål for cykeldeltagelse</t>
+  </si>
+  <si>
+    <t>Vejkryds tæthed</t>
+  </si>
+  <si>
+    <t>Adgang til offentlig transport</t>
+  </si>
+  <si>
+    <t>Adgang til offentlige åbne rum</t>
+  </si>
+  <si>
+    <t>Indsæt noget indhold her måske?</t>
+  </si>
+  <si>
+    <t>Nem adgang til hyppig offentlig transport er en afgørende faktor for sunde og bæredygtige transportsystemer. Offentlig transport i nærheden af boliger og beskæftigelse øger andelen af offentlige transporter og tilskynder dermed til transportrelateret gang. at tilbyde adgang til regionale job og tjenester; forbedring af sundhed, økonomisk udvikling og social inklusion; og reducere forurening og CO2-emissioner. Hyppigheden af tjenester tilskynder også til brug af offentlig transport ud over nærheden af stationer eller stop.</t>
+  </si>
+  <si>
+    <t>Krav til offentlig transport adgang til beskæftigelse/infrastruktur</t>
+  </si>
+  <si>
+    <t>Krav til fordeling af beskæftigelsen</t>
+  </si>
+  <si>
+    <t>Minimumskrav til adgang til offentlig transport</t>
+  </si>
+  <si>
+    <t>Mål for brug af offentlig transport</t>
+  </si>
+  <si>
+    <t>Lokal adgang til offentlige åbne rum af høj kvalitet fremmer rekreativ fysisk aktivitet og mental sundhed. Nærliggende offentlige åbne rum skaber hyggelige, attraktive miljøer, hjælper med at afkøle byen og beskytter biodiversiteten. Som byer fortætne og private åbne rum falder, giver mere offentlige åbne rum er afgørende for befolkningens sundhed. At have offentligt åbent rum inden for 400 m fra hjemmet kan tilskynde til at gå. Adgang til større parker kan også være vigtig.</t>
+  </si>
+  <si>
+    <t>Minimumskrav til adgang til offentlige åbne områder</t>
+  </si>
+  <si>
+    <t>Den fulde rapport med data, metoder og begrænsninger er blevet offentliggjort i INSERT SERIES CITATION &amp;URL | Befolkningsdata: Schiavina, M. et al. (2019): GHS-befolkningsgitter multitemporal (1975, 1990, 2000, 2015) R2019A. Europa-Kommissionen, Det Fælles Forskningscenter (FFC). https://doi.org/10.2905/42E8BE89-54FF-464E-BE7B-BF9E64DA5218 | Bygrænser: Florczyk, A. et al. (2019): GHS Urban Centre Database 2015, multitemporale og flerdimensionelle egenskaber, R2019A. Europa-Kommissionen, Det Fælles Forskningscenter (FFC). https://data.jrc.ec.europa.eu/dataset/53473144-b88c-44bc-b4a3-4583ed1f547e | Urban funktioner: OpenStreetMap bidragydere. Openstreetmap (2020). https://planet.osm.org/pbf/planet-200803.osm.pbf.torrent | Farveskala: Crameri, F. (2018). Videnskabelige farvekort (3.0.4). Zenodo. https://doi.org/10.5281/zenodo.1287763</t>
+  </si>
+  <si>
+    <t>Citat: Globalt samarbejde om sunde og bæredygtige byindikatorer. 2022. Indikatorer for sunde og bæredygtige byer: Kort rapport, {city}. https://doi.org/INSERT-DOI-HERE</t>
+  </si>
+  <si>
+    <t>Denne korte rapport skitserer, hvordan {city} klarer sig på rumlige og politiske indikatorer for sunde og bæredygtige byer. Global Healthy and Sustainable City-Indicators Collaboration-undersøgelsen undersøgte den rumlige fordeling af bydesign og transportfunktioner og tilstedeværelsen og kvaliteten af byplanlægningspolitikker, der fremmer sundhed og bæredygtighed for 25 byer på tværs af 19 lande internationalt. Yderligere oplysninger om undersøgelsen kan fås på https://doi.org/INSERT-DOI-HERE.</t>
+  </si>
+  <si>
+    <t>*Angiv en oversigt i konfigurationsarket Sprog for denne by*</t>
+  </si>
+  <si>
+    <t>Melbourne havde relativt god adgang til offentlige transportstop og åbne rum og en række byplanlægningspolitikker, der støttede walkable kvarterer med god adgang til offentlige åbne rum. Men walkability og adgang til hyppig offentlig transport blev uretfærdigt fordelt, til fordel for indre byområder. Kravene til boligtæthed skulle øges for bedre at kunne understøtte walkability.</t>
+  </si>
+  <si>
+    <t>Danish - Word translation</t>
   </si>
 </sst>
 </file>
@@ -1869,7 +2088,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1945,9 +2164,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1959,9 +2175,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2038,298 +2251,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -13827,24 +13753,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M97"/>
+  <dimension ref="A1:N97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H71" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C73" sqref="C73"/>
+      <selection pane="bottomRight" activeCell="D73" sqref="C1:D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="21" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" style="21" customWidth="1"/>
-    <col min="3" max="9" width="55" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="2" width="31.5703125" style="21" hidden="1" customWidth="1"/>
+    <col min="3" max="10" width="55" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>229</v>
       </c>
@@ -13854,2047 +13780,2338 @@
       <c r="C1" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>354</v>
       </c>
       <c r="E1" s="24" t="s">
+        <v>465</v>
+      </c>
+      <c r="F1" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="G1" s="24" t="s">
         <v>232</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="H1" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="I1" s="24" t="s">
         <v>255</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="J1" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="J1" s="25"/>
       <c r="K1" s="25"/>
       <c r="L1" s="25"/>
-      <c r="M1" s="26"/>
-    </row>
-    <row r="2" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M1" s="25"/>
+      <c r="N1" s="26"/>
+    </row>
+    <row r="2" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="30" t="s">
         <v>234</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="27" t="s">
+        <v>393</v>
+      </c>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
       <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="30"/>
-    </row>
-    <row r="3" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="29"/>
+    </row>
+    <row r="3" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="30" t="s">
         <v>235</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="27" t="s">
+        <v>394</v>
+      </c>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
       <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="30"/>
-    </row>
-    <row r="4" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="29"/>
+    </row>
+    <row r="4" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="30" t="s">
         <v>236</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="27" t="s">
+        <v>395</v>
+      </c>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
       <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="30"/>
-    </row>
-    <row r="5" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="29"/>
+    </row>
+    <row r="5" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="30" t="s">
         <v>237</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="27" t="s">
+        <v>396</v>
+      </c>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
       <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="30"/>
-    </row>
-    <row r="6" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="29"/>
+    </row>
+    <row r="6" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="27" t="s">
+        <v>397</v>
+      </c>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
       <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="30"/>
-    </row>
-    <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="29"/>
+    </row>
+    <row r="7" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="30" t="s">
         <v>240</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="27" t="s">
+        <v>398</v>
+      </c>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
       <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="30"/>
-    </row>
-    <row r="8" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="29"/>
+    </row>
+    <row r="8" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="30" t="s">
         <v>239</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="27" t="s">
+        <v>399</v>
+      </c>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
       <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="30"/>
-    </row>
-    <row r="9" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="29"/>
+    </row>
+    <row r="9" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="30" t="s">
         <v>364</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="27" t="s">
+        <v>400</v>
+      </c>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
       <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="30"/>
-    </row>
-    <row r="10" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="29"/>
+    </row>
+    <row r="10" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="27" t="s">
+        <v>401</v>
+      </c>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
       <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="30"/>
-    </row>
-    <row r="11" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="29"/>
+    </row>
+    <row r="11" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="27" t="s">
+        <v>402</v>
+      </c>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
       <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="30"/>
-    </row>
-    <row r="12" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="29"/>
+    </row>
+    <row r="12" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="27" t="s">
+        <v>403</v>
+      </c>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
       <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="30"/>
-    </row>
-    <row r="13" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="29"/>
+    </row>
+    <row r="13" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="27" t="s">
+        <v>404</v>
+      </c>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
       <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="30"/>
-    </row>
-    <row r="14" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="29"/>
+    </row>
+    <row r="14" spans="1:14" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="30" t="s">
         <v>368</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="28" t="s">
+        <v>405</v>
+      </c>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
       <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="30"/>
-    </row>
-    <row r="15" spans="1:13" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="29"/>
+    </row>
+    <row r="15" spans="1:14" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="30" t="s">
         <v>370</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="28" t="s">
+        <v>406</v>
+      </c>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
       <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="30"/>
-    </row>
-    <row r="16" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="29"/>
+    </row>
+    <row r="16" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="30" t="s">
         <v>366</v>
       </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="27" t="s">
+        <v>407</v>
+      </c>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
       <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="30"/>
-    </row>
-    <row r="17" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="29"/>
+    </row>
+    <row r="17" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B17" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="30" t="s">
         <v>249</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="27" t="s">
+        <v>408</v>
+      </c>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
       <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="30"/>
-    </row>
-    <row r="18" spans="1:13" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="29"/>
+    </row>
+    <row r="18" spans="1:14" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="30" t="s">
         <v>250</v>
       </c>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="28" t="s">
+        <v>409</v>
+      </c>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
       <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="30"/>
-    </row>
-    <row r="19" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="29"/>
+    </row>
+    <row r="19" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B19" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="28" t="s">
+        <v>410</v>
+      </c>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
       <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="30"/>
-    </row>
-    <row r="20" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="29"/>
+    </row>
+    <row r="20" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="30" t="s">
         <v>365</v>
       </c>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="28" t="s">
+        <v>411</v>
+      </c>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
       <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="30"/>
-    </row>
-    <row r="21" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="29"/>
+    </row>
+    <row r="21" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>231</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>322</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="30" t="s">
         <v>320</v>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="27" t="s">
+        <v>412</v>
+      </c>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
       <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="30"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="29"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="34" t="s">
         <v>266</v>
       </c>
-      <c r="D22" s="33"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="35"/>
-    </row>
-    <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="34"/>
+      <c r="E22" s="31" t="s">
+        <v>413</v>
+      </c>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="33"/>
+    </row>
+    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="34" t="s">
         <v>358</v>
       </c>
-      <c r="D23" s="33"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="35"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D23" s="34"/>
+      <c r="E23" s="31" t="s">
+        <v>414</v>
+      </c>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="33"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="34" t="s">
         <v>202</v>
       </c>
       <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="35"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E24" s="32" t="s">
+        <v>415</v>
+      </c>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="33"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="34" t="s">
         <v>359</v>
       </c>
       <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="35"/>
-    </row>
-    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E25" s="32" t="s">
+        <v>416</v>
+      </c>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="33"/>
+    </row>
+    <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="36" t="s">
+      <c r="C26" s="34" t="s">
         <v>295</v>
       </c>
       <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="35"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E26" s="32" t="s">
+        <v>417</v>
+      </c>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="33"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B27" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="34" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="35"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E27" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="33"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B28" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="34" t="s">
         <v>52</v>
       </c>
       <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="35"/>
-    </row>
-    <row r="29" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="E28" s="32" t="s">
+        <v>418</v>
+      </c>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="33"/>
+    </row>
+    <row r="29" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B29" s="21" t="s">
         <v>375</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="34" t="s">
         <v>376</v>
       </c>
       <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="35"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E29" s="32" t="s">
+        <v>419</v>
+      </c>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="33"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B30" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="C30" s="34" t="s">
         <v>57</v>
       </c>
       <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="35"/>
-    </row>
-    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E30" s="32" t="s">
+        <v>420</v>
+      </c>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="33"/>
+    </row>
+    <row r="31" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B31" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="34" t="s">
         <v>326</v>
       </c>
       <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="35"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E31" s="32" t="s">
+        <v>421</v>
+      </c>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="33"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B32" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="36" t="s">
+      <c r="C32" s="34" t="s">
         <v>325</v>
       </c>
       <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="33"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="35"/>
-    </row>
-    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E32" s="32" t="s">
+        <v>422</v>
+      </c>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+      <c r="N32" s="33"/>
+    </row>
+    <row r="33" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B33" s="21" t="s">
         <v>324</v>
       </c>
-      <c r="C33" s="36" t="s">
+      <c r="C33" s="34" t="s">
         <v>341</v>
       </c>
       <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="35"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E33" s="32" t="s">
+        <v>423</v>
+      </c>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="31"/>
+      <c r="M33" s="31"/>
+      <c r="N33" s="33"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B34" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="36" t="s">
+      <c r="C34" s="34" t="s">
         <v>268</v>
       </c>
       <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="33"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="35"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E34" s="32" t="s">
+        <v>424</v>
+      </c>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="31"/>
+      <c r="N34" s="33"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B35" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="34" t="s">
         <v>329</v>
       </c>
       <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="33"/>
-      <c r="K35" s="33"/>
-      <c r="L35" s="33"/>
-      <c r="M35" s="35"/>
-    </row>
-    <row r="36" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E35" s="32" t="s">
+        <v>425</v>
+      </c>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
+      <c r="N35" s="33"/>
+    </row>
+    <row r="36" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B36" s="21" t="s">
         <v>328</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="C36" s="34" t="s">
         <v>332</v>
       </c>
       <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="33"/>
-      <c r="K36" s="33"/>
-      <c r="L36" s="33"/>
-      <c r="M36" s="35"/>
-    </row>
-    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E36" s="32" t="s">
+        <v>426</v>
+      </c>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
+      <c r="N36" s="33"/>
+    </row>
+    <row r="37" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B37" s="21" t="s">
         <v>327</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="34" t="s">
         <v>361</v>
       </c>
       <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="33"/>
-      <c r="K37" s="33"/>
-      <c r="L37" s="33"/>
-      <c r="M37" s="35"/>
-    </row>
-    <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E37" s="32" t="s">
+        <v>427</v>
+      </c>
+      <c r="F37" s="32"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="31"/>
+      <c r="N37" s="33"/>
+    </row>
+    <row r="38" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B38" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="36" t="s">
+      <c r="C38" s="34" t="s">
         <v>387</v>
       </c>
       <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="33"/>
-      <c r="K38" s="33"/>
-      <c r="L38" s="33"/>
-      <c r="M38" s="35"/>
-    </row>
-    <row r="39" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E38" s="32" t="s">
+        <v>428</v>
+      </c>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="32"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="31"/>
+      <c r="N38" s="33"/>
+    </row>
+    <row r="39" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B39" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="36" t="s">
+      <c r="C39" s="34" t="s">
         <v>388</v>
       </c>
       <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="33"/>
-      <c r="K39" s="33"/>
-      <c r="L39" s="33"/>
-      <c r="M39" s="35"/>
-    </row>
-    <row r="40" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E39" s="32" t="s">
+        <v>429</v>
+      </c>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="31"/>
+      <c r="N39" s="33"/>
+    </row>
+    <row r="40" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B40" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="36" t="s">
+      <c r="C40" s="34" t="s">
         <v>389</v>
       </c>
       <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="33"/>
-      <c r="K40" s="33"/>
-      <c r="L40" s="33"/>
-      <c r="M40" s="35"/>
-    </row>
-    <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E40" s="32" t="s">
+        <v>430</v>
+      </c>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="33"/>
+    </row>
+    <row r="41" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B41" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="36" t="s">
+      <c r="C41" s="34" t="s">
         <v>390</v>
       </c>
       <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="34"/>
-      <c r="J41" s="33"/>
-      <c r="K41" s="33"/>
-      <c r="L41" s="33"/>
-      <c r="M41" s="35"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E41" s="32" t="s">
+        <v>431</v>
+      </c>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="33"/>
+    </row>
+    <row r="42" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B42" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C42" s="34" t="s">
         <v>362</v>
       </c>
       <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="33"/>
-      <c r="K42" s="33"/>
-      <c r="L42" s="33"/>
-      <c r="M42" s="35"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E42" s="32" t="s">
+        <v>432</v>
+      </c>
+      <c r="F42" s="32"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="31"/>
+      <c r="M42" s="31"/>
+      <c r="N42" s="33"/>
+    </row>
+    <row r="43" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B43" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="36" t="s">
+      <c r="C43" s="34" t="s">
         <v>373</v>
       </c>
       <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="33"/>
-      <c r="K43" s="33"/>
-      <c r="L43" s="33"/>
-      <c r="M43" s="35"/>
-    </row>
-    <row r="44" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+      <c r="E43" s="32" t="s">
+        <v>433</v>
+      </c>
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="31"/>
+      <c r="L43" s="31"/>
+      <c r="M43" s="31"/>
+      <c r="N43" s="33"/>
+    </row>
+    <row r="44" spans="1:14" ht="165" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B44" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C44" s="37" t="s">
+      <c r="C44" s="35" t="s">
         <v>363</v>
       </c>
-      <c r="D44" s="38"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="34"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="33"/>
-      <c r="K44" s="33"/>
-      <c r="L44" s="33"/>
-      <c r="M44" s="35"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D44" s="35"/>
+      <c r="E44" s="36" t="s">
+        <v>434</v>
+      </c>
+      <c r="F44" s="32"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
+      <c r="J44" s="32"/>
+      <c r="K44" s="31"/>
+      <c r="L44" s="31"/>
+      <c r="M44" s="31"/>
+      <c r="N44" s="33"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B45" s="21" t="s">
         <v>272</v>
       </c>
-      <c r="C45" s="36" t="s">
+      <c r="C45" s="34" t="s">
         <v>273</v>
       </c>
       <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="34"/>
-      <c r="H45" s="34"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="33"/>
-      <c r="K45" s="33"/>
-      <c r="L45" s="33"/>
-      <c r="M45" s="35"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E45" s="32" t="s">
+        <v>435</v>
+      </c>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="31"/>
+      <c r="L45" s="31"/>
+      <c r="M45" s="31"/>
+      <c r="N45" s="33"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B46" s="21" t="s">
         <v>277</v>
       </c>
-      <c r="C46" s="36" t="s">
+      <c r="C46" s="34" t="s">
         <v>280</v>
       </c>
       <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="34"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="33"/>
-      <c r="K46" s="33"/>
-      <c r="L46" s="33"/>
-      <c r="M46" s="35"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E46" s="32" t="s">
+        <v>436</v>
+      </c>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
+      <c r="K46" s="31"/>
+      <c r="L46" s="31"/>
+      <c r="M46" s="31"/>
+      <c r="N46" s="33"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B47" s="21" t="s">
         <v>278</v>
       </c>
-      <c r="C47" s="36" t="s">
+      <c r="C47" s="34" t="s">
         <v>279</v>
       </c>
       <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="33"/>
-      <c r="K47" s="33"/>
-      <c r="L47" s="33"/>
-      <c r="M47" s="35"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E47" s="32" t="s">
+        <v>437</v>
+      </c>
+      <c r="F47" s="32"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="32"/>
+      <c r="J47" s="32"/>
+      <c r="K47" s="31"/>
+      <c r="L47" s="31"/>
+      <c r="M47" s="31"/>
+      <c r="N47" s="33"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B48" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="C48" s="36" t="s">
+      <c r="C48" s="34" t="s">
         <v>122</v>
       </c>
       <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="34"/>
-      <c r="H48" s="34"/>
-      <c r="I48" s="34"/>
-      <c r="J48" s="33"/>
-      <c r="K48" s="33"/>
-      <c r="L48" s="33"/>
-      <c r="M48" s="35"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E48" s="32" t="s">
+        <v>438</v>
+      </c>
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="32"/>
+      <c r="J48" s="32"/>
+      <c r="K48" s="31"/>
+      <c r="L48" s="31"/>
+      <c r="M48" s="31"/>
+      <c r="N48" s="33"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B49" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="C49" s="36" t="s">
+      <c r="C49" s="34" t="s">
         <v>274</v>
       </c>
       <c r="D49" s="34"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="34"/>
-      <c r="I49" s="34"/>
-      <c r="J49" s="33"/>
-      <c r="K49" s="33"/>
-      <c r="L49" s="33"/>
-      <c r="M49" s="35"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E49" s="32" t="s">
+        <v>439</v>
+      </c>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="32"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="31"/>
+      <c r="M49" s="31"/>
+      <c r="N49" s="33"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B50" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="C50" s="36" t="s">
+      <c r="C50" s="34" t="s">
         <v>119</v>
       </c>
       <c r="D50" s="34"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="34"/>
-      <c r="H50" s="34"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="33"/>
-      <c r="K50" s="33"/>
-      <c r="L50" s="33"/>
-      <c r="M50" s="35"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E50" s="32" t="s">
+        <v>440</v>
+      </c>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="32"/>
+      <c r="J50" s="32"/>
+      <c r="K50" s="31"/>
+      <c r="L50" s="31"/>
+      <c r="M50" s="31"/>
+      <c r="N50" s="33"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B51" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C51" s="36" t="s">
+      <c r="C51" s="34" t="s">
         <v>275</v>
       </c>
       <c r="D51" s="34"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="34"/>
-      <c r="H51" s="34"/>
-      <c r="I51" s="34"/>
-      <c r="J51" s="33"/>
-      <c r="K51" s="33"/>
-      <c r="L51" s="33"/>
-      <c r="M51" s="35"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E51" s="32" t="s">
+        <v>441</v>
+      </c>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
+      <c r="J51" s="32"/>
+      <c r="K51" s="31"/>
+      <c r="L51" s="31"/>
+      <c r="M51" s="31"/>
+      <c r="N51" s="33"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B52" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="C52" s="36" t="s">
+      <c r="C52" s="34" t="s">
         <v>107</v>
       </c>
       <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="34"/>
-      <c r="H52" s="34"/>
-      <c r="I52" s="34"/>
-      <c r="J52" s="33"/>
-      <c r="K52" s="33"/>
-      <c r="L52" s="33"/>
-      <c r="M52" s="35"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E52" s="32" t="s">
+        <v>442</v>
+      </c>
+      <c r="F52" s="32"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
+      <c r="J52" s="32"/>
+      <c r="K52" s="31"/>
+      <c r="L52" s="31"/>
+      <c r="M52" s="31"/>
+      <c r="N52" s="33"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B53" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="C53" s="36" t="s">
+      <c r="C53" s="34" t="s">
         <v>385</v>
       </c>
       <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="34"/>
-      <c r="H53" s="34"/>
-      <c r="I53" s="34"/>
-      <c r="J53" s="33"/>
-      <c r="K53" s="33"/>
-      <c r="L53" s="33"/>
-      <c r="M53" s="35"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E53" s="32" t="s">
+        <v>443</v>
+      </c>
+      <c r="F53" s="32"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="32"/>
+      <c r="J53" s="32"/>
+      <c r="K53" s="31"/>
+      <c r="L53" s="31"/>
+      <c r="M53" s="31"/>
+      <c r="N53" s="33"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B54" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="C54" s="36" t="s">
+      <c r="C54" s="34" t="s">
         <v>109</v>
       </c>
       <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="34"/>
-      <c r="H54" s="34"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="33"/>
-      <c r="K54" s="33"/>
-      <c r="L54" s="33"/>
-      <c r="M54" s="35"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E54" s="32" t="s">
+        <v>444</v>
+      </c>
+      <c r="F54" s="32"/>
+      <c r="G54" s="32"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="32"/>
+      <c r="J54" s="32"/>
+      <c r="K54" s="31"/>
+      <c r="L54" s="31"/>
+      <c r="M54" s="31"/>
+      <c r="N54" s="33"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B55" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="C55" s="36" t="s">
+      <c r="C55" s="34" t="s">
         <v>110</v>
       </c>
       <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="34"/>
-      <c r="G55" s="34"/>
-      <c r="H55" s="34"/>
-      <c r="I55" s="34"/>
-      <c r="J55" s="33"/>
-      <c r="K55" s="33"/>
-      <c r="L55" s="33"/>
-      <c r="M55" s="35"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E55" s="32" t="s">
+        <v>445</v>
+      </c>
+      <c r="F55" s="32"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="32"/>
+      <c r="J55" s="32"/>
+      <c r="K55" s="31"/>
+      <c r="L55" s="31"/>
+      <c r="M55" s="31"/>
+      <c r="N55" s="33"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B56" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="C56" s="36" t="s">
+      <c r="C56" s="34" t="s">
         <v>111</v>
       </c>
       <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="34"/>
-      <c r="H56" s="34"/>
-      <c r="I56" s="34"/>
-      <c r="J56" s="33"/>
-      <c r="K56" s="33"/>
-      <c r="L56" s="33"/>
-      <c r="M56" s="35"/>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E56" s="32" t="s">
+        <v>446</v>
+      </c>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
+      <c r="I56" s="32"/>
+      <c r="J56" s="32"/>
+      <c r="K56" s="31"/>
+      <c r="L56" s="31"/>
+      <c r="M56" s="31"/>
+      <c r="N56" s="33"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B57" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="C57" s="36" t="s">
+      <c r="C57" s="34" t="s">
         <v>112</v>
       </c>
       <c r="D57" s="34"/>
-      <c r="E57" s="34"/>
-      <c r="F57" s="34"/>
-      <c r="G57" s="34"/>
-      <c r="H57" s="34"/>
-      <c r="I57" s="34"/>
-      <c r="J57" s="33"/>
-      <c r="K57" s="33"/>
-      <c r="L57" s="33"/>
-      <c r="M57" s="35"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E57" s="32" t="s">
+        <v>447</v>
+      </c>
+      <c r="F57" s="32"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="32"/>
+      <c r="J57" s="32"/>
+      <c r="K57" s="31"/>
+      <c r="L57" s="31"/>
+      <c r="M57" s="31"/>
+      <c r="N57" s="33"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B58" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="C58" s="36" t="s">
+      <c r="C58" s="34" t="s">
         <v>113</v>
       </c>
       <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="34"/>
-      <c r="H58" s="34"/>
-      <c r="I58" s="34"/>
-      <c r="J58" s="33"/>
-      <c r="K58" s="33"/>
-      <c r="L58" s="33"/>
-      <c r="M58" s="35"/>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E58" s="32" t="s">
+        <v>448</v>
+      </c>
+      <c r="F58" s="32"/>
+      <c r="G58" s="32"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="32"/>
+      <c r="J58" s="32"/>
+      <c r="K58" s="31"/>
+      <c r="L58" s="31"/>
+      <c r="M58" s="31"/>
+      <c r="N58" s="33"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B59" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="C59" s="36" t="s">
+      <c r="C59" s="34" t="s">
         <v>93</v>
       </c>
       <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="34"/>
-      <c r="H59" s="34"/>
-      <c r="I59" s="34"/>
-      <c r="J59" s="33"/>
-      <c r="K59" s="33"/>
-      <c r="L59" s="33"/>
-      <c r="M59" s="35"/>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E59" s="32" t="s">
+        <v>449</v>
+      </c>
+      <c r="F59" s="32"/>
+      <c r="G59" s="32"/>
+      <c r="H59" s="32"/>
+      <c r="I59" s="32"/>
+      <c r="J59" s="32"/>
+      <c r="K59" s="31"/>
+      <c r="L59" s="31"/>
+      <c r="M59" s="31"/>
+      <c r="N59" s="33"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B60" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="C60" s="36" t="s">
+      <c r="C60" s="34" t="s">
         <v>269</v>
       </c>
       <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="34"/>
-      <c r="H60" s="34"/>
-      <c r="I60" s="38"/>
-      <c r="J60" s="33"/>
-      <c r="K60" s="33"/>
-      <c r="L60" s="33"/>
-      <c r="M60" s="35"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E60" s="32" t="s">
+        <v>450</v>
+      </c>
+      <c r="F60" s="32"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="32"/>
+      <c r="I60" s="32"/>
+      <c r="J60" s="36"/>
+      <c r="K60" s="31"/>
+      <c r="L60" s="31"/>
+      <c r="M60" s="31"/>
+      <c r="N60" s="33"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B61" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C61" s="36" t="s">
+      <c r="C61" s="34" t="s">
         <v>270</v>
       </c>
       <c r="D61" s="34"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="34"/>
-      <c r="H61" s="34"/>
-      <c r="I61" s="34"/>
-      <c r="J61" s="33"/>
-      <c r="K61" s="33"/>
-      <c r="L61" s="33"/>
-      <c r="M61" s="35"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E61" s="32" t="s">
+        <v>451</v>
+      </c>
+      <c r="F61" s="32"/>
+      <c r="G61" s="32"/>
+      <c r="H61" s="32"/>
+      <c r="I61" s="32"/>
+      <c r="J61" s="32"/>
+      <c r="K61" s="31"/>
+      <c r="L61" s="31"/>
+      <c r="M61" s="31"/>
+      <c r="N61" s="33"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B62" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="C62" s="36" t="s">
+      <c r="C62" s="34" t="s">
         <v>207</v>
       </c>
       <c r="D62" s="34"/>
-      <c r="E62" s="34"/>
-      <c r="F62" s="34"/>
-      <c r="G62" s="34"/>
-      <c r="H62" s="34"/>
-      <c r="I62" s="34"/>
-      <c r="J62" s="33"/>
-      <c r="K62" s="33"/>
-      <c r="L62" s="33"/>
-      <c r="M62" s="35"/>
-    </row>
-    <row r="63" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+      <c r="E62" s="32" t="s">
+        <v>452</v>
+      </c>
+      <c r="F62" s="32"/>
+      <c r="G62" s="32"/>
+      <c r="H62" s="32"/>
+      <c r="I62" s="32"/>
+      <c r="J62" s="32"/>
+      <c r="K62" s="31"/>
+      <c r="L62" s="31"/>
+      <c r="M62" s="31"/>
+      <c r="N62" s="33"/>
+    </row>
+    <row r="63" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A63" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B63" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="C63" s="37" t="s">
+      <c r="C63" s="35" t="s">
         <v>367</v>
       </c>
-      <c r="D63" s="38"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="34"/>
-      <c r="H63" s="34"/>
-      <c r="I63" s="34"/>
-      <c r="J63" s="33"/>
-      <c r="K63" s="33"/>
-      <c r="L63" s="33"/>
-      <c r="M63" s="35"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D63" s="35"/>
+      <c r="E63" s="36" t="s">
+        <v>453</v>
+      </c>
+      <c r="F63" s="32"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="32"/>
+      <c r="J63" s="32"/>
+      <c r="K63" s="31"/>
+      <c r="L63" s="31"/>
+      <c r="M63" s="31"/>
+      <c r="N63" s="33"/>
+    </row>
+    <row r="64" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B64" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="C64" s="32" t="s">
+      <c r="C64" s="34" t="s">
         <v>386</v>
       </c>
-      <c r="D64" s="33"/>
-      <c r="E64" s="34"/>
-      <c r="F64" s="34"/>
-      <c r="G64" s="34"/>
-      <c r="H64" s="34"/>
-      <c r="I64" s="34"/>
-      <c r="J64" s="33"/>
-      <c r="K64" s="33"/>
-      <c r="L64" s="33"/>
-      <c r="M64" s="35"/>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D64" s="34"/>
+      <c r="E64" s="31" t="s">
+        <v>454</v>
+      </c>
+      <c r="F64" s="32"/>
+      <c r="G64" s="32"/>
+      <c r="H64" s="32"/>
+      <c r="I64" s="32"/>
+      <c r="J64" s="32"/>
+      <c r="K64" s="31"/>
+      <c r="L64" s="31"/>
+      <c r="M64" s="31"/>
+      <c r="N64" s="33"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B65" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="C65" s="32" t="s">
+      <c r="C65" s="34" t="s">
         <v>281</v>
       </c>
-      <c r="D65" s="33"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="34"/>
-      <c r="H65" s="34"/>
-      <c r="I65" s="34"/>
-      <c r="J65" s="33"/>
-      <c r="K65" s="33"/>
-      <c r="L65" s="33"/>
-      <c r="M65" s="35"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D65" s="34"/>
+      <c r="E65" s="31" t="s">
+        <v>455</v>
+      </c>
+      <c r="F65" s="32"/>
+      <c r="G65" s="32"/>
+      <c r="H65" s="32"/>
+      <c r="I65" s="32"/>
+      <c r="J65" s="32"/>
+      <c r="K65" s="31"/>
+      <c r="L65" s="31"/>
+      <c r="M65" s="31"/>
+      <c r="N65" s="33"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B66" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="C66" s="36" t="s">
+      <c r="C66" s="34" t="s">
         <v>188</v>
       </c>
       <c r="D66" s="34"/>
-      <c r="E66" s="34"/>
-      <c r="F66" s="34"/>
-      <c r="G66" s="34"/>
-      <c r="H66" s="34"/>
-      <c r="I66" s="38"/>
-      <c r="J66" s="33"/>
-      <c r="K66" s="33"/>
-      <c r="L66" s="33"/>
-      <c r="M66" s="35"/>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E66" s="32" t="s">
+        <v>456</v>
+      </c>
+      <c r="F66" s="32"/>
+      <c r="G66" s="32"/>
+      <c r="H66" s="32"/>
+      <c r="I66" s="32"/>
+      <c r="J66" s="36"/>
+      <c r="K66" s="31"/>
+      <c r="L66" s="31"/>
+      <c r="M66" s="31"/>
+      <c r="N66" s="33"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B67" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C67" s="36" t="s">
+      <c r="C67" s="34" t="s">
         <v>189</v>
       </c>
       <c r="D67" s="34"/>
-      <c r="E67" s="34"/>
-      <c r="F67" s="34"/>
-      <c r="G67" s="34"/>
-      <c r="H67" s="34"/>
-      <c r="I67" s="34"/>
-      <c r="J67" s="33"/>
-      <c r="K67" s="33"/>
-      <c r="L67" s="33"/>
-      <c r="M67" s="35"/>
-    </row>
-    <row r="68" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+      <c r="E67" s="32" t="s">
+        <v>457</v>
+      </c>
+      <c r="F67" s="32"/>
+      <c r="G67" s="32"/>
+      <c r="H67" s="32"/>
+      <c r="I67" s="32"/>
+      <c r="J67" s="32"/>
+      <c r="K67" s="31"/>
+      <c r="L67" s="31"/>
+      <c r="M67" s="31"/>
+      <c r="N67" s="33"/>
+    </row>
+    <row r="68" spans="1:14" ht="135" x14ac:dyDescent="0.25">
       <c r="A68" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B68" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="C68" s="37" t="s">
+      <c r="C68" s="35" t="s">
         <v>369</v>
       </c>
-      <c r="D68" s="38"/>
-      <c r="E68" s="34"/>
-      <c r="F68" s="34"/>
-      <c r="G68" s="34"/>
-      <c r="H68" s="34"/>
-      <c r="I68" s="34"/>
-      <c r="J68" s="33"/>
-      <c r="K68" s="33"/>
-      <c r="L68" s="33"/>
-      <c r="M68" s="35"/>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D68" s="35"/>
+      <c r="E68" s="36" t="s">
+        <v>458</v>
+      </c>
+      <c r="F68" s="32"/>
+      <c r="G68" s="32"/>
+      <c r="H68" s="32"/>
+      <c r="I68" s="32"/>
+      <c r="J68" s="32"/>
+      <c r="K68" s="31"/>
+      <c r="L68" s="31"/>
+      <c r="M68" s="31"/>
+      <c r="N68" s="33"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B69" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="C69" s="36" t="s">
+      <c r="C69" s="34" t="s">
         <v>195</v>
       </c>
       <c r="D69" s="34"/>
-      <c r="E69" s="34"/>
-      <c r="F69" s="34"/>
-      <c r="G69" s="34"/>
-      <c r="H69" s="34"/>
-      <c r="I69" s="34"/>
-      <c r="J69" s="33"/>
-      <c r="K69" s="33"/>
-      <c r="L69" s="33"/>
-      <c r="M69" s="35"/>
-    </row>
-    <row r="70" spans="1:13" ht="255" x14ac:dyDescent="0.25">
+      <c r="E69" s="32" t="s">
+        <v>459</v>
+      </c>
+      <c r="F69" s="32"/>
+      <c r="G69" s="32"/>
+      <c r="H69" s="32"/>
+      <c r="I69" s="32"/>
+      <c r="J69" s="32"/>
+      <c r="K69" s="31"/>
+      <c r="L69" s="31"/>
+      <c r="M69" s="31"/>
+      <c r="N69" s="33"/>
+    </row>
+    <row r="70" spans="1:14" ht="240" x14ac:dyDescent="0.25">
       <c r="A70" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B70" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C70" s="36" t="s">
+      <c r="C70" s="34" t="s">
         <v>271</v>
       </c>
       <c r="D70" s="34"/>
-      <c r="E70" s="34"/>
-      <c r="F70" s="34"/>
-      <c r="G70" s="34"/>
-      <c r="H70" s="34"/>
-      <c r="I70" s="34"/>
-      <c r="J70" s="33"/>
-      <c r="K70" s="33"/>
-      <c r="L70" s="33"/>
-      <c r="M70" s="35"/>
-    </row>
-    <row r="71" spans="1:13" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E70" s="32" t="s">
+        <v>460</v>
+      </c>
+      <c r="F70" s="32"/>
+      <c r="G70" s="32"/>
+      <c r="H70" s="32"/>
+      <c r="I70" s="32"/>
+      <c r="J70" s="32"/>
+      <c r="K70" s="31"/>
+      <c r="L70" s="31"/>
+      <c r="M70" s="31"/>
+      <c r="N70" s="33"/>
+    </row>
+    <row r="71" spans="1:14" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B71" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="C71" s="36" t="s">
+      <c r="C71" s="34" t="s">
         <v>371</v>
       </c>
       <c r="D71" s="34"/>
-      <c r="E71" s="34"/>
-      <c r="F71" s="34"/>
-      <c r="G71" s="34"/>
-      <c r="H71" s="34"/>
-      <c r="I71" s="34"/>
-      <c r="J71" s="33"/>
-      <c r="K71" s="33"/>
-      <c r="L71" s="33"/>
-      <c r="M71" s="35"/>
-    </row>
-    <row r="72" spans="1:13" ht="177.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E71" s="32" t="s">
+        <v>461</v>
+      </c>
+      <c r="F71" s="32"/>
+      <c r="G71" s="32"/>
+      <c r="H71" s="32"/>
+      <c r="I71" s="32"/>
+      <c r="J71" s="32"/>
+      <c r="K71" s="31"/>
+      <c r="L71" s="31"/>
+      <c r="M71" s="31"/>
+      <c r="N71" s="33"/>
+    </row>
+    <row r="72" spans="1:14" ht="177.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B72" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="C72" s="36" t="s">
+      <c r="C72" s="34" t="s">
         <v>372</v>
       </c>
       <c r="D72" s="34"/>
-      <c r="E72" s="34"/>
-      <c r="F72" s="34"/>
-      <c r="G72" s="34"/>
-      <c r="H72" s="34"/>
-      <c r="I72" s="34"/>
-      <c r="J72" s="33"/>
-      <c r="K72" s="33"/>
-      <c r="L72" s="33"/>
-      <c r="M72" s="35"/>
-    </row>
-    <row r="73" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E72" s="32" t="s">
+        <v>462</v>
+      </c>
+      <c r="F72" s="32"/>
+      <c r="G72" s="32"/>
+      <c r="H72" s="32"/>
+      <c r="I72" s="32"/>
+      <c r="J72" s="32"/>
+      <c r="K72" s="31"/>
+      <c r="L72" s="31"/>
+      <c r="M72" s="31"/>
+      <c r="N72" s="33"/>
+    </row>
+    <row r="73" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B73" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="C73" s="36" t="s">
+      <c r="C73" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D73" s="34"/>
-      <c r="E73" s="34"/>
-      <c r="F73" s="34"/>
-      <c r="G73" s="34"/>
-      <c r="H73" s="34"/>
-      <c r="I73" s="34"/>
-      <c r="J73" s="33"/>
-      <c r="K73" s="33"/>
-      <c r="L73" s="33"/>
-      <c r="M73" s="35"/>
-    </row>
-    <row r="74" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E73" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F73" s="32"/>
+      <c r="G73" s="32"/>
+      <c r="H73" s="32"/>
+      <c r="I73" s="32"/>
+      <c r="J73" s="32"/>
+      <c r="K73" s="31"/>
+      <c r="L73" s="31"/>
+      <c r="M73" s="31"/>
+      <c r="N73" s="33"/>
+    </row>
+    <row r="74" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B74" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="C74" s="36" t="s">
+      <c r="C74" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D74" s="34"/>
-      <c r="E74" s="34"/>
-      <c r="F74" s="34"/>
-      <c r="G74" s="34"/>
-      <c r="H74" s="34"/>
-      <c r="I74" s="34"/>
-      <c r="J74" s="33"/>
-      <c r="K74" s="33"/>
-      <c r="L74" s="33"/>
-      <c r="M74" s="35"/>
-    </row>
-    <row r="75" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E74" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F74" s="32"/>
+      <c r="G74" s="32"/>
+      <c r="H74" s="32"/>
+      <c r="I74" s="32"/>
+      <c r="J74" s="32"/>
+      <c r="K74" s="31"/>
+      <c r="L74" s="31"/>
+      <c r="M74" s="31"/>
+      <c r="N74" s="33"/>
+    </row>
+    <row r="75" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B75" s="21" t="s">
         <v>297</v>
       </c>
-      <c r="C75" s="36" t="s">
+      <c r="C75" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D75" s="34"/>
-      <c r="E75" s="34"/>
-      <c r="F75" s="34"/>
-      <c r="G75" s="34"/>
-      <c r="H75" s="34"/>
-      <c r="I75" s="34"/>
-      <c r="J75" s="33"/>
-      <c r="K75" s="33"/>
-      <c r="L75" s="33"/>
-      <c r="M75" s="35"/>
-    </row>
-    <row r="76" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E75" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F75" s="32"/>
+      <c r="G75" s="32"/>
+      <c r="H75" s="32"/>
+      <c r="I75" s="32"/>
+      <c r="J75" s="32"/>
+      <c r="K75" s="31"/>
+      <c r="L75" s="31"/>
+      <c r="M75" s="31"/>
+      <c r="N75" s="33"/>
+    </row>
+    <row r="76" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B76" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="C76" s="36" t="s">
+      <c r="C76" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D76" s="34"/>
-      <c r="E76" s="34"/>
-      <c r="F76" s="34"/>
-      <c r="G76" s="34"/>
-      <c r="H76" s="34"/>
-      <c r="I76" s="34"/>
-      <c r="J76" s="33"/>
-      <c r="K76" s="33"/>
-      <c r="L76" s="33"/>
-      <c r="M76" s="35"/>
-    </row>
-    <row r="77" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E76" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F76" s="32"/>
+      <c r="G76" s="32"/>
+      <c r="H76" s="32"/>
+      <c r="I76" s="32"/>
+      <c r="J76" s="32"/>
+      <c r="K76" s="31"/>
+      <c r="L76" s="31"/>
+      <c r="M76" s="31"/>
+      <c r="N76" s="33"/>
+    </row>
+    <row r="77" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B77" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="C77" s="36" t="s">
+      <c r="C77" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D77" s="34"/>
-      <c r="E77" s="34"/>
-      <c r="F77" s="34"/>
-      <c r="G77" s="34"/>
-      <c r="H77" s="34"/>
-      <c r="I77" s="34"/>
-      <c r="J77" s="33"/>
-      <c r="K77" s="33"/>
-      <c r="L77" s="33"/>
-      <c r="M77" s="35"/>
-    </row>
-    <row r="78" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E77" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F77" s="32"/>
+      <c r="G77" s="32"/>
+      <c r="H77" s="32"/>
+      <c r="I77" s="32"/>
+      <c r="J77" s="32"/>
+      <c r="K77" s="31"/>
+      <c r="L77" s="31"/>
+      <c r="M77" s="31"/>
+      <c r="N77" s="33"/>
+    </row>
+    <row r="78" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B78" s="21" t="s">
         <v>300</v>
       </c>
-      <c r="C78" s="36" t="s">
+      <c r="C78" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D78" s="34"/>
-      <c r="E78" s="34"/>
-      <c r="F78" s="34"/>
-      <c r="G78" s="34"/>
-      <c r="H78" s="34"/>
-      <c r="I78" s="34"/>
-      <c r="J78" s="33"/>
-      <c r="K78" s="33"/>
-      <c r="L78" s="33"/>
-      <c r="M78" s="35"/>
-    </row>
-    <row r="79" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E78" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F78" s="32"/>
+      <c r="G78" s="32"/>
+      <c r="H78" s="32"/>
+      <c r="I78" s="32"/>
+      <c r="J78" s="32"/>
+      <c r="K78" s="31"/>
+      <c r="L78" s="31"/>
+      <c r="M78" s="31"/>
+      <c r="N78" s="33"/>
+    </row>
+    <row r="79" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B79" s="21" t="s">
         <v>301</v>
       </c>
-      <c r="C79" s="36" t="s">
+      <c r="C79" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D79" s="34"/>
-      <c r="E79" s="34"/>
-      <c r="F79" s="34"/>
-      <c r="G79" s="34"/>
-      <c r="H79" s="34"/>
-      <c r="I79" s="34"/>
-      <c r="J79" s="33"/>
-      <c r="K79" s="33"/>
-      <c r="L79" s="33"/>
-      <c r="M79" s="35"/>
-    </row>
-    <row r="80" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E79" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F79" s="32"/>
+      <c r="G79" s="32"/>
+      <c r="H79" s="32"/>
+      <c r="I79" s="32"/>
+      <c r="J79" s="32"/>
+      <c r="K79" s="31"/>
+      <c r="L79" s="31"/>
+      <c r="M79" s="31"/>
+      <c r="N79" s="33"/>
+    </row>
+    <row r="80" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B80" s="21" t="s">
         <v>302</v>
       </c>
-      <c r="C80" s="36" t="s">
+      <c r="C80" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D80" s="34"/>
-      <c r="E80" s="34"/>
-      <c r="F80" s="34"/>
-      <c r="G80" s="34"/>
-      <c r="H80" s="34"/>
-      <c r="I80" s="34"/>
-      <c r="J80" s="33"/>
-      <c r="K80" s="33"/>
-      <c r="L80" s="33"/>
-      <c r="M80" s="35"/>
-    </row>
-    <row r="81" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E80" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F80" s="32"/>
+      <c r="G80" s="32"/>
+      <c r="H80" s="32"/>
+      <c r="I80" s="32"/>
+      <c r="J80" s="32"/>
+      <c r="K80" s="31"/>
+      <c r="L80" s="31"/>
+      <c r="M80" s="31"/>
+      <c r="N80" s="33"/>
+    </row>
+    <row r="81" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B81" s="21" t="s">
         <v>284</v>
       </c>
-      <c r="C81" s="36" t="s">
+      <c r="C81" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D81" s="34"/>
-      <c r="E81" s="34"/>
-      <c r="F81" s="34"/>
-      <c r="G81" s="34"/>
-      <c r="H81" s="34"/>
-      <c r="I81" s="34"/>
-      <c r="J81" s="33"/>
-      <c r="K81" s="33"/>
-      <c r="L81" s="33"/>
-      <c r="M81" s="35"/>
-    </row>
-    <row r="82" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E81" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F81" s="32"/>
+      <c r="G81" s="32"/>
+      <c r="H81" s="32"/>
+      <c r="I81" s="32"/>
+      <c r="J81" s="32"/>
+      <c r="K81" s="31"/>
+      <c r="L81" s="31"/>
+      <c r="M81" s="31"/>
+      <c r="N81" s="33"/>
+    </row>
+    <row r="82" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B82" s="21" t="s">
         <v>303</v>
       </c>
-      <c r="C82" s="36" t="s">
+      <c r="C82" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D82" s="34"/>
-      <c r="E82" s="34"/>
-      <c r="F82" s="34"/>
-      <c r="G82" s="34"/>
-      <c r="H82" s="34"/>
-      <c r="I82" s="34"/>
-      <c r="J82" s="33"/>
-      <c r="K82" s="33"/>
-      <c r="L82" s="33"/>
-      <c r="M82" s="35"/>
-    </row>
-    <row r="83" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E82" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F82" s="32"/>
+      <c r="G82" s="32"/>
+      <c r="H82" s="32"/>
+      <c r="I82" s="32"/>
+      <c r="J82" s="32"/>
+      <c r="K82" s="31"/>
+      <c r="L82" s="31"/>
+      <c r="M82" s="31"/>
+      <c r="N82" s="33"/>
+    </row>
+    <row r="83" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B83" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="C83" s="36" t="s">
+      <c r="C83" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D83" s="34"/>
-      <c r="E83" s="34"/>
-      <c r="F83" s="34"/>
-      <c r="G83" s="34"/>
-      <c r="H83" s="34"/>
-      <c r="I83" s="34"/>
-      <c r="J83" s="33"/>
-      <c r="K83" s="33"/>
-      <c r="L83" s="33"/>
-      <c r="M83" s="35"/>
-    </row>
-    <row r="84" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E83" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F83" s="32"/>
+      <c r="G83" s="32"/>
+      <c r="H83" s="32"/>
+      <c r="I83" s="32"/>
+      <c r="J83" s="32"/>
+      <c r="K83" s="31"/>
+      <c r="L83" s="31"/>
+      <c r="M83" s="31"/>
+      <c r="N83" s="33"/>
+    </row>
+    <row r="84" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B84" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="C84" s="36" t="s">
+      <c r="C84" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D84" s="34"/>
-      <c r="E84" s="34"/>
-      <c r="F84" s="34"/>
-      <c r="G84" s="34"/>
-      <c r="H84" s="34"/>
-      <c r="I84" s="34"/>
-      <c r="J84" s="33"/>
-      <c r="K84" s="33"/>
-      <c r="L84" s="33"/>
-      <c r="M84" s="35"/>
-    </row>
-    <row r="85" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E84" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F84" s="32"/>
+      <c r="G84" s="32"/>
+      <c r="H84" s="32"/>
+      <c r="I84" s="32"/>
+      <c r="J84" s="32"/>
+      <c r="K84" s="31"/>
+      <c r="L84" s="31"/>
+      <c r="M84" s="31"/>
+      <c r="N84" s="33"/>
+    </row>
+    <row r="85" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B85" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="C85" s="36" t="s">
+      <c r="C85" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D85" s="34"/>
-      <c r="E85" s="34"/>
-      <c r="F85" s="34"/>
-      <c r="G85" s="34"/>
-      <c r="H85" s="34"/>
-      <c r="I85" s="34"/>
-      <c r="J85" s="33"/>
-      <c r="K85" s="33"/>
-      <c r="L85" s="33"/>
-      <c r="M85" s="35"/>
-    </row>
-    <row r="86" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E85" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F85" s="32"/>
+      <c r="G85" s="32"/>
+      <c r="H85" s="32"/>
+      <c r="I85" s="32"/>
+      <c r="J85" s="32"/>
+      <c r="K85" s="31"/>
+      <c r="L85" s="31"/>
+      <c r="M85" s="31"/>
+      <c r="N85" s="33"/>
+    </row>
+    <row r="86" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B86" s="21" t="s">
         <v>307</v>
       </c>
-      <c r="C86" s="36" t="s">
+      <c r="C86" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D86" s="34"/>
-      <c r="E86" s="34"/>
-      <c r="F86" s="34"/>
-      <c r="G86" s="34"/>
-      <c r="H86" s="34"/>
-      <c r="I86" s="34"/>
-      <c r="J86" s="33"/>
-      <c r="K86" s="33"/>
-      <c r="L86" s="33"/>
-      <c r="M86" s="35"/>
-    </row>
-    <row r="87" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E86" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F86" s="32"/>
+      <c r="G86" s="32"/>
+      <c r="H86" s="32"/>
+      <c r="I86" s="32"/>
+      <c r="J86" s="32"/>
+      <c r="K86" s="31"/>
+      <c r="L86" s="31"/>
+      <c r="M86" s="31"/>
+      <c r="N86" s="33"/>
+    </row>
+    <row r="87" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B87" s="21" t="s">
         <v>308</v>
       </c>
-      <c r="C87" s="36" t="s">
+      <c r="C87" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D87" s="34"/>
-      <c r="E87" s="34"/>
-      <c r="F87" s="34"/>
-      <c r="G87" s="34"/>
-      <c r="H87" s="34"/>
-      <c r="I87" s="34"/>
-      <c r="J87" s="33"/>
-      <c r="K87" s="33"/>
-      <c r="L87" s="33"/>
-      <c r="M87" s="35"/>
-    </row>
-    <row r="88" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E87" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F87" s="32"/>
+      <c r="G87" s="32"/>
+      <c r="H87" s="32"/>
+      <c r="I87" s="32"/>
+      <c r="J87" s="32"/>
+      <c r="K87" s="31"/>
+      <c r="L87" s="31"/>
+      <c r="M87" s="31"/>
+      <c r="N87" s="33"/>
+    </row>
+    <row r="88" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B88" s="21" t="s">
         <v>309</v>
       </c>
-      <c r="C88" s="36" t="s">
+      <c r="C88" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D88" s="34"/>
-      <c r="E88" s="34"/>
-      <c r="F88" s="34"/>
-      <c r="G88" s="34"/>
-      <c r="H88" s="34"/>
-      <c r="I88" s="34"/>
-      <c r="J88" s="33"/>
-      <c r="K88" s="33"/>
-      <c r="L88" s="33"/>
-      <c r="M88" s="35"/>
-    </row>
-    <row r="89" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E88" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F88" s="32"/>
+      <c r="G88" s="32"/>
+      <c r="H88" s="32"/>
+      <c r="I88" s="32"/>
+      <c r="J88" s="32"/>
+      <c r="K88" s="31"/>
+      <c r="L88" s="31"/>
+      <c r="M88" s="31"/>
+      <c r="N88" s="33"/>
+    </row>
+    <row r="89" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B89" s="21" t="s">
         <v>310</v>
       </c>
-      <c r="C89" s="36" t="s">
+      <c r="C89" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D89" s="34"/>
-      <c r="E89" s="34"/>
-      <c r="F89" s="34"/>
-      <c r="G89" s="34"/>
-      <c r="H89" s="34"/>
-      <c r="I89" s="34"/>
-      <c r="J89" s="33"/>
-      <c r="K89" s="33"/>
-      <c r="L89" s="33"/>
-      <c r="M89" s="35"/>
-    </row>
-    <row r="90" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E89" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F89" s="32"/>
+      <c r="G89" s="32"/>
+      <c r="H89" s="32"/>
+      <c r="I89" s="32"/>
+      <c r="J89" s="32"/>
+      <c r="K89" s="31"/>
+      <c r="L89" s="31"/>
+      <c r="M89" s="31"/>
+      <c r="N89" s="33"/>
+    </row>
+    <row r="90" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B90" s="21" t="s">
         <v>311</v>
       </c>
-      <c r="C90" s="36" t="s">
+      <c r="C90" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D90" s="34"/>
-      <c r="E90" s="34"/>
-      <c r="F90" s="34"/>
-      <c r="G90" s="34"/>
-      <c r="H90" s="34"/>
-      <c r="I90" s="34"/>
-      <c r="J90" s="33"/>
-      <c r="K90" s="33"/>
-      <c r="L90" s="33"/>
-      <c r="M90" s="35"/>
-    </row>
-    <row r="91" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E90" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F90" s="32"/>
+      <c r="G90" s="32"/>
+      <c r="H90" s="32"/>
+      <c r="I90" s="32"/>
+      <c r="J90" s="32"/>
+      <c r="K90" s="31"/>
+      <c r="L90" s="31"/>
+      <c r="M90" s="31"/>
+      <c r="N90" s="33"/>
+    </row>
+    <row r="91" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B91" s="21" t="s">
         <v>312</v>
       </c>
-      <c r="C91" s="36" t="s">
+      <c r="C91" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D91" s="34"/>
-      <c r="E91" s="34"/>
-      <c r="F91" s="34"/>
-      <c r="G91" s="34"/>
-      <c r="H91" s="34"/>
-      <c r="I91" s="34"/>
-      <c r="J91" s="33"/>
-      <c r="K91" s="33"/>
-      <c r="L91" s="33"/>
-      <c r="M91" s="35"/>
-    </row>
-    <row r="92" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E91" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F91" s="32"/>
+      <c r="G91" s="32"/>
+      <c r="H91" s="32"/>
+      <c r="I91" s="32"/>
+      <c r="J91" s="32"/>
+      <c r="K91" s="31"/>
+      <c r="L91" s="31"/>
+      <c r="M91" s="31"/>
+      <c r="N91" s="33"/>
+    </row>
+    <row r="92" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B92" s="21" t="s">
         <v>313</v>
       </c>
-      <c r="C92" s="36" t="s">
+      <c r="C92" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D92" s="34"/>
-      <c r="E92" s="34"/>
-      <c r="F92" s="34"/>
-      <c r="G92" s="34"/>
-      <c r="H92" s="34"/>
-      <c r="I92" s="34"/>
-      <c r="J92" s="33"/>
-      <c r="K92" s="33"/>
-      <c r="L92" s="33"/>
-      <c r="M92" s="35"/>
-    </row>
-    <row r="93" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E92" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F92" s="32"/>
+      <c r="G92" s="32"/>
+      <c r="H92" s="32"/>
+      <c r="I92" s="32"/>
+      <c r="J92" s="32"/>
+      <c r="K92" s="31"/>
+      <c r="L92" s="31"/>
+      <c r="M92" s="31"/>
+      <c r="N92" s="33"/>
+    </row>
+    <row r="93" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B93" s="21" t="s">
         <v>314</v>
       </c>
-      <c r="C93" s="36" t="s">
+      <c r="C93" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D93" s="34"/>
-      <c r="E93" s="34"/>
-      <c r="F93" s="34"/>
-      <c r="G93" s="34"/>
-      <c r="H93" s="34"/>
-      <c r="I93" s="34"/>
-      <c r="J93" s="33"/>
-      <c r="K93" s="33"/>
-      <c r="L93" s="33"/>
-      <c r="M93" s="35"/>
-    </row>
-    <row r="94" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E93" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F93" s="32"/>
+      <c r="G93" s="32"/>
+      <c r="H93" s="32"/>
+      <c r="I93" s="32"/>
+      <c r="J93" s="32"/>
+      <c r="K93" s="31"/>
+      <c r="L93" s="31"/>
+      <c r="M93" s="31"/>
+      <c r="N93" s="33"/>
+    </row>
+    <row r="94" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B94" s="22" t="s">
         <v>315</v>
       </c>
-      <c r="C94" s="36" t="s">
+      <c r="C94" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D94" s="34"/>
-      <c r="E94" s="34"/>
-      <c r="F94" s="34"/>
-      <c r="G94" s="34"/>
-      <c r="H94" s="34"/>
-      <c r="I94" s="34"/>
-      <c r="J94" s="33"/>
-      <c r="K94" s="33"/>
-      <c r="L94" s="33"/>
-      <c r="M94" s="35"/>
-    </row>
-    <row r="95" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="E94" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F94" s="32"/>
+      <c r="G94" s="32"/>
+      <c r="H94" s="32"/>
+      <c r="I94" s="32"/>
+      <c r="J94" s="32"/>
+      <c r="K94" s="31"/>
+      <c r="L94" s="31"/>
+      <c r="M94" s="31"/>
+      <c r="N94" s="33"/>
+    </row>
+    <row r="95" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A95" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B95" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="C95" s="36" t="s">
+      <c r="C95" s="34" t="s">
         <v>360</v>
       </c>
       <c r="D95" s="34"/>
-      <c r="E95" s="34"/>
-      <c r="F95" s="34"/>
-      <c r="G95" s="34"/>
-      <c r="H95" s="34"/>
-      <c r="I95" s="34"/>
-      <c r="J95" s="33"/>
-      <c r="K95" s="33"/>
-      <c r="L95" s="33"/>
-      <c r="M95" s="35"/>
-    </row>
-    <row r="96" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E95" s="32" t="s">
+        <v>464</v>
+      </c>
+      <c r="F95" s="32"/>
+      <c r="G95" s="32"/>
+      <c r="H95" s="32"/>
+      <c r="I95" s="32"/>
+      <c r="J95" s="32"/>
+      <c r="K95" s="31"/>
+      <c r="L95" s="31"/>
+      <c r="M95" s="31"/>
+      <c r="N95" s="33"/>
+    </row>
+    <row r="96" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B96" s="21" t="s">
         <v>316</v>
       </c>
-      <c r="C96" s="36" t="s">
+      <c r="C96" s="34" t="s">
         <v>319</v>
       </c>
       <c r="D96" s="34"/>
-      <c r="E96" s="34"/>
-      <c r="F96" s="34"/>
-      <c r="G96" s="34"/>
-      <c r="H96" s="34"/>
-      <c r="I96" s="34"/>
-      <c r="J96" s="33"/>
-      <c r="K96" s="33"/>
-      <c r="L96" s="33"/>
-      <c r="M96" s="35"/>
-    </row>
-    <row r="97" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="E96" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F96" s="32"/>
+      <c r="G96" s="32"/>
+      <c r="H96" s="32"/>
+      <c r="I96" s="32"/>
+      <c r="J96" s="32"/>
+      <c r="K96" s="31"/>
+      <c r="L96" s="31"/>
+      <c r="M96" s="31"/>
+      <c r="N96" s="33"/>
+    </row>
+    <row r="97" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="21" t="s">
         <v>230</v>
       </c>
       <c r="B97" s="21" t="s">
         <v>317</v>
       </c>
-      <c r="C97" s="39" t="s">
+      <c r="C97" s="37" t="s">
         <v>319</v>
       </c>
-      <c r="D97" s="40"/>
-      <c r="E97" s="40"/>
-      <c r="F97" s="40"/>
-      <c r="G97" s="40"/>
-      <c r="H97" s="40"/>
-      <c r="I97" s="40"/>
-      <c r="J97" s="41"/>
-      <c r="K97" s="41"/>
-      <c r="L97" s="41"/>
-      <c r="M97" s="42"/>
+      <c r="D97" s="37"/>
+      <c r="E97" s="38" t="s">
+        <v>463</v>
+      </c>
+      <c r="F97" s="38"/>
+      <c r="G97" s="38"/>
+      <c r="H97" s="38"/>
+      <c r="I97" s="38"/>
+      <c r="J97" s="38"/>
+      <c r="K97" s="39"/>
+      <c r="L97" s="39"/>
+      <c r="M97" s="39"/>
+      <c r="N97" s="40"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:D2">
+  <conditionalFormatting sqref="C2:E2">
     <cfRule type="duplicateValues" dxfId="14" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
@@ -15903,19 +16120,19 @@
   <conditionalFormatting sqref="B48:B1048576 B22:B30 B1:B2 B32:B36 B38:B44">
     <cfRule type="duplicateValues" dxfId="12" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:D12">
+  <conditionalFormatting sqref="C9:E12">
     <cfRule type="duplicateValues" dxfId="11" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:D13">
+  <conditionalFormatting sqref="C13:E13">
     <cfRule type="duplicateValues" dxfId="10" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:D21">
+  <conditionalFormatting sqref="C21:E21">
     <cfRule type="duplicateValues" dxfId="9" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6 B8:B21">
     <cfRule type="duplicateValues" dxfId="8" priority="23"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:D6 C8:D8 C14:D20">
+  <conditionalFormatting sqref="C3:E6 C8:E8 C14:E20">
     <cfRule type="duplicateValues" dxfId="7" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
@@ -15927,7 +16144,7 @@
   <conditionalFormatting sqref="B47">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:D7">
+  <conditionalFormatting sqref="C7:E7">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
@@ -15936,21 +16153,22 @@
   <conditionalFormatting sqref="B37">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:M97">
+  <conditionalFormatting sqref="E1:N97">
     <cfRule type="containsBlanks" dxfId="0" priority="26">
-      <formula>LEN(TRIM(D1))=0</formula>
+      <formula>LEN(TRIM(E1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16048,7 +16266,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>208</v>
+        <v>354</v>
       </c>
       <c r="B6" t="s">
         <v>263</v>
@@ -16062,7 +16280,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>208</v>
+        <v>354</v>
       </c>
       <c r="B7" t="s">
         <v>263</v>
@@ -16079,7 +16297,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>208</v>
+        <v>354</v>
       </c>
       <c r="B8" t="s">
         <v>263</v>
@@ -16096,7 +16314,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>208</v>
+        <v>354</v>
       </c>
       <c r="B9" t="s">
         <v>263</v>
@@ -16113,7 +16331,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>265</v>
+        <v>208</v>
       </c>
       <c r="B10" t="s">
         <v>263</v>
@@ -16127,7 +16345,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>265</v>
+        <v>208</v>
       </c>
       <c r="B11" t="s">
         <v>263</v>
@@ -16144,7 +16362,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>265</v>
+        <v>208</v>
       </c>
       <c r="B12" t="s">
         <v>263</v>
@@ -16161,7 +16379,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>265</v>
+        <v>208</v>
       </c>
       <c r="B13" t="s">
         <v>263</v>
@@ -16178,7 +16396,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>233</v>
+        <v>265</v>
       </c>
       <c r="B14" t="s">
         <v>263</v>
@@ -16192,7 +16410,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>233</v>
+        <v>265</v>
       </c>
       <c r="B15" t="s">
         <v>263</v>
@@ -16209,7 +16427,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>233</v>
+        <v>265</v>
       </c>
       <c r="B16" t="s">
         <v>263</v>
@@ -16226,7 +16444,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>233</v>
+        <v>265</v>
       </c>
       <c r="B17" t="s">
         <v>263</v>
@@ -16243,155 +16461,220 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
       <c r="B18" t="s">
         <v>263</v>
       </c>
       <c r="C18" t="s">
-        <v>226</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>224</v>
-      </c>
-      <c r="F18" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
       <c r="B19" t="s">
         <v>263</v>
       </c>
       <c r="C19" t="s">
-        <v>226</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
         <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>223</v>
-      </c>
-      <c r="F19" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
       <c r="B20" t="s">
         <v>263</v>
       </c>
       <c r="C20" t="s">
-        <v>226</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
         <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>225</v>
-      </c>
-      <c r="F20" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
       <c r="B21" t="s">
         <v>263</v>
       </c>
       <c r="C21" t="s">
-        <v>226</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
         <v>217</v>
       </c>
       <c r="E21" t="s">
-        <v>222</v>
-      </c>
-      <c r="F21" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>255</v>
+        <v>212</v>
       </c>
       <c r="B22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C22" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
       <c r="E22" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
       <c r="F22" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>255</v>
+        <v>212</v>
       </c>
       <c r="B23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C23" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
       <c r="D23" t="s">
         <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>258</v>
+        <v>223</v>
       </c>
       <c r="F23" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>255</v>
+        <v>212</v>
       </c>
       <c r="B24" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C24" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
       </c>
       <c r="E24" t="s">
-        <v>259</v>
+        <v>225</v>
       </c>
       <c r="F24" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>255</v>
+        <v>212</v>
       </c>
       <c r="B25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C25" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
       <c r="D25" t="s">
         <v>217</v>
       </c>
       <c r="E25" t="s">
+        <v>222</v>
+      </c>
+      <c r="F25" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>255</v>
+      </c>
+      <c r="B26" t="s">
+        <v>264</v>
+      </c>
+      <c r="C26" t="s">
+        <v>261</v>
+      </c>
+      <c r="E26" t="s">
+        <v>257</v>
+      </c>
+      <c r="F26" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>255</v>
+      </c>
+      <c r="B27" t="s">
+        <v>264</v>
+      </c>
+      <c r="C27" t="s">
+        <v>261</v>
+      </c>
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" t="s">
+        <v>258</v>
+      </c>
+      <c r="F27" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>255</v>
+      </c>
+      <c r="B28" t="s">
+        <v>264</v>
+      </c>
+      <c r="C28" t="s">
+        <v>261</v>
+      </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" t="s">
+        <v>259</v>
+      </c>
+      <c r="F28" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>255</v>
+      </c>
+      <c r="B29" t="s">
+        <v>264</v>
+      </c>
+      <c r="C29" t="s">
+        <v>261</v>
+      </c>
+      <c r="D29" t="s">
+        <v>217</v>
+      </c>
+      <c r="E29" t="s">
         <v>260</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F29" t="s">
         <v>256</v>
       </c>
     </row>

</xml_diff>

<commit_message>
located and set up a Tamil font Aaram which also includes latin glyphs (eg for units in plot axis), developed by Tharique Azeez @enathu https://github.com/enathu/aaram
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560733C4-A623-4ED5-BF1B-96458A513174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20F2D7B-3A81-4D7F-9788-106976FB7277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2717" uniqueCount="1138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2725" uniqueCount="1140">
   <si>
     <t>name</t>
   </si>
@@ -2868,9 +2868,6 @@
     <t>இன்போ இங்கே செருகப்பட வேண்டும் ...</t>
   </si>
   <si>
-    <t>ஆரோக்கியமான மற்றும் நிலையான நகரங்களின் குறிகாட்டிகள்: {நகரம்}</t>
-  </si>
-  <si>
     <t>நடைப்பயணம்</t>
   </si>
   <si>
@@ -2989,12 +2986,6 @@
   </si>
   <si>
     <t>தரவு, முறைகள் மற்றும் வரம்புகள் உள்ளிட்ட முழு அறிக்கை செருகு தொடர் மேற்கோள் &amp; | மக்கள் தொகை தரவு: ஷியாவினா, எம் மற்றும் பலர். (2019): ஜிஹெச்எஸ் மக்கள் தொகை கட்டம் மல்டிடெம்போரல் (1975, 1990, 2000, 2015) ஆர் 2019ஏ. ஐரோப்பிய ஆணையம், கூட்டு ஆராய்ச்சி மையம் (ஜே.ஆர்.சி.). https://doi.org/10.2905/42E8BE89-54FF-464E-BE7B-BF9E64DA5218 | நகர்ப்புற எல்லைகள்: ஃப்ளோர்சிக், ஏ. மற்றும் பலர். (2019): ஜிஹெச்எஸ் நகர்ப்புற மையம் தரவுத்தளம் 2015, மல்டிடெம்போரல் மற்றும் பல பரிமாண பண்புகள், ஆர்2019ஏ. ஐரோப்பிய ஆணையம், கூட்டு ஆராய்ச்சி மையம் (ஜே.ஆர்.சி.). https://data.jrc.ec.europa.eu/dataset/53473144-b88c-44bc-b4a3-4583ed1f547e | நகர்ப்புற அம்சங்கள்: ஓபன்ஸ்ட்ரீட்மேப் பங்களிப்பாளர்கள். ஓபன்ஸ்ட்ரீட்மேப் (2020). https://planet.osm.org/pbf/planet-200803.osm.pbf.torrent | வண்ண அளவு: க்ராமரி, எஃப் (2018). அறிவியல் வண்ண வரைபடங்கள் (3.0.4). ஜெனோடோ. https://doi.org/10.5281/zenodo.1287763</t>
-  </si>
-  <si>
-    <t xml:space="preserve">இந்த சுருக்கமான அறிக்கை {நகரம்} ஆரோக்கியமான மற்றும் நிலையான நகரங்களின் இடம் சார்ந்த மற்றும் கொள்கை குறிகாட்டிகளின் தேர்வை எவ்வாறு செய்கிறது என்பதை கோடிட்டுக் காட்டுகிறது. எங்கள் கூட்டு ஆய்வு நகர்ப்புற வடிவமைப்பு மற்றும் போக்குவரத்து அம்சங்கள் இடம் சார்ந்த விநியோகம் மற்றும் சர்வதேச அளவில் 19 நாடுகளில் 25 நகரங்களில் சுகாதார மற்றும் நிலைத்தன்மை ஊக்குவிக்கும் நகர திட்டமிடல் கொள்கைகள் முன்னிலையில் மற்றும் தரம் ஆய்வு. ஆய்வின் கூடுதல் விவரங்கள் https://doi.org/INSERT-DOI-HERE கிடைக்கின்றன.  </t>
-  </si>
-  <si>
-    <t>ஆய்வில் சேர்க்கப்பட்டுள்ள நகரங்கள் முழுவதும் சராசரி (வழக்கமான கவனிக்கப்பட்ட மதிப்பு) ஒப்பீடுகள் நகர கொள்கைகளை தெரிவிக்க பயன்படுத்தப்படலாம். {நகரம்}முழுவதும் சுற்றுச்சூழல் அம்சங்களின் விநியோகத்தை வரைபடங்கள் காட்டுகின்றன, இது மிகவும் சமமான சூழல்களை வழங்கும் மாற்றங்களிலிருந்து மிகவும் பயனடையக்கூடிய பகுதிகளை அடையாளம் காண பயன்படுத்தப்படலாம்.</t>
   </si>
   <si>
     <t>நிர்வாக சுருக்கம்</t>
@@ -3494,35 +3485,50 @@
     <t>மக்கள் தொகையில் % குறைந்தபட்ச வரம்பை பூர்த்தி செய்யுங்கள்*</t>
   </si>
   <si>
-    <t>(கீழே) {நகரம்} 500 மீட்டர் (மீ) க்குள் வசதிகளை அணுகுவதற்கான மக்கள் தொகை சதவீதத்திற்கான மதிப்பீடுகள்.</t>
-  </si>
-  <si>
     <t>* வரம்புகள் நடைபயிற்சி (https://www.who.int/news-room/initiatives/gappa) மூலம் போதுமான பொதுஜன முன்னணி 15% ஒப்பீட்டளவில் குறைப்பு உலக சுகாதார அமைப்பின் இலக்கை அடைய தேவைகளை எங்கள் மாடலிங் அடிப்படையாக கொண்டது.  அதிஅடர்த்தியான சுற்றுப்புறங்கள் (எ.கா. &gt;15,000 நபர்கள் ஒரு கி.மீ²) உடல் செயல்பாடுகளுக்கான நன்மைகளைக் குறைக்கலாம்; இது எதிர்கால ஆராய்ச்சிக்கு ஒரு முக்கியமான தலைப்பு.</t>
   </si>
   <si>
-    <t>{நகரத்தில்} நடைப்பயணக் கொள்கை</t>
-  </si>
-  <si>
-    <t>{நகரத்தில்} பொது போக்குவரத்து கொள்கை</t>
-  </si>
-  <si>
-    <t>{நகரத்தில்} பொது திறந்த வெளி கொள்கை</t>
-  </si>
-  <si>
-    <t>மேற்கோள்: உலகளாவிய ஆரோக்கியமான மற்றும் நிலையான நகரம்-குறிகாட்டிகள் ஒத்துழைப்பு. 2022. ஆரோக்கியமான மற்றும் நிலையான நகரம் குறிகாட்டிகள் சர்வதேச ஒப்பீடு அறிக்கை: {நகரம்}. https://doi.org/INSERT-DOI-HERE</t>
-  </si>
-  <si>
-    <t>fonts/fpdf_unicode_font_pack/font/gargi.ttf</t>
-  </si>
-  <si>
-    <t>gargi</t>
+    <t>ஆரோக்கியமான மற்றும் நிலையான நகரங்களின் குறிகாட்டிகள்: {city}</t>
+  </si>
+  <si>
+    <t>(கீழே) {city} 500 மீட்டர் (மீ) க்குள் வசதிகளை அணுகுவதற்கான மக்கள் தொகை சதவீதத்திற்கான மதிப்பீடுகள்.</t>
+  </si>
+  <si>
+    <t>மேற்கோள்: உலகளாவிய ஆரோக்கியமான மற்றும் நிலையான நகரம்-குறிகாட்டிகள் ஒத்துழைப்பு. 2022. ஆரோக்கியமான மற்றும் நிலையான நகரம் குறிகாட்டிகள் சர்வதேச ஒப்பீடு அறிக்கை: {city}. https://doi.org/INSERT-DOI-HERE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">இந்த சுருக்கமான அறிக்கை {city} ஆரோக்கியமான மற்றும் நிலையான நகரங்களின் இடம் சார்ந்த மற்றும் கொள்கை குறிகாட்டிகளின் தேர்வை எவ்வாறு செய்கிறது என்பதை கோடிட்டுக் காட்டுகிறது. எங்கள் கூட்டு ஆய்வு நகர்ப்புற வடிவமைப்பு மற்றும் போக்குவரத்து அம்சங்கள் இடம் சார்ந்த விநியோகம் மற்றும் சர்வதேச அளவில் 19 நாடுகளில் 25 நகரங்களில் சுகாதார மற்றும் நிலைத்தன்மை ஊக்குவிக்கும் நகர திட்டமிடல் கொள்கைகள் முன்னிலையில் மற்றும் தரம் ஆய்வு. ஆய்வின் கூடுதல் விவரங்கள் https://doi.org/INSERT-DOI-HERE கிடைக்கின்றன.  </t>
+  </si>
+  <si>
+    <t>ஆய்வில் சேர்க்கப்பட்டுள்ள நகரங்கள் முழுவதும் சராசரி (வழக்கமான கவனிக்கப்பட்ட மதிப்பு) ஒப்பீடுகள் நகர கொள்கைகளை தெரிவிக்க பயன்படுத்தப்படலாம். {city}முழுவதும் சுற்றுச்சூழல் அம்சங்களின் விநியோகத்தை வரைபடங்கள் காட்டுகின்றன, இது மிகவும் சமமான சூழல்களை வழங்கும் மாற்றங்களிலிருந்து மிகவும் பயனடையக்கூடிய பகுதிகளை அடையாளம் காண பயன்படுத்தப்படலாம்.</t>
+  </si>
+  <si>
+    <t>{city} நடைப்பயணக் கொள்கை</t>
+  </si>
+  <si>
+    <t>{city} பொது போக்குவரத்து கொள்கை</t>
+  </si>
+  <si>
+    <t>{city} பொது திறந்த வெளி கொள்கை</t>
+  </si>
+  <si>
+    <t>noto_sans_tamil</t>
+  </si>
+  <si>
+    <t>fonts/Aaram-Regular.ttf</t>
+  </si>
+  <si>
+    <t>https://github.com/dejavu-fonts/dejavu-fonts/releases</t>
+  </si>
+  <si>
+    <t>https://github.com/enathu/aaram/blob/gh-pages/build/Aaram-Regular.ttf  (may have a missing glyph; unclear which)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3717,6 +3723,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Noto Sans Tamil"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Noto Sans Tamil"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -4186,7 +4205,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4307,6 +4326,25 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4389,19 +4427,19 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -15945,20 +15983,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="P43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="T100" sqref="T100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="33" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" style="33" customWidth="1"/>
     <col min="3" max="8" width="55" style="3" customWidth="1"/>
     <col min="9" max="9" width="67" style="3" customWidth="1"/>
-    <col min="10" max="20" width="55" style="3" customWidth="1"/>
+    <col min="10" max="19" width="55" style="3" customWidth="1"/>
+    <col min="20" max="20" width="55" style="47" customWidth="1"/>
     <col min="21" max="24" width="43.140625" style="3" customWidth="1"/>
     <col min="25" max="16384" width="9.140625" style="3"/>
   </cols>
@@ -15983,13 +16022,13 @@
         <v>305</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="H1" s="19" t="s">
         <v>185</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
       <c r="J1" s="19" t="s">
         <v>787</v>
@@ -16021,7 +16060,7 @@
       <c r="S1" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="T1" s="42" t="s">
         <v>909</v>
       </c>
       <c r="U1" s="19" t="s">
@@ -16031,10 +16070,10 @@
         <v>826</v>
       </c>
       <c r="W1" s="19" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="X1" s="19" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="Y1" s="19"/>
       <c r="Z1" s="31"/>
@@ -16061,7 +16100,7 @@
         <v>786</v>
       </c>
       <c r="I2" s="40" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="J2" s="29" t="s">
         <v>793</v>
@@ -16091,8 +16130,8 @@
         <v>801</v>
       </c>
       <c r="S2" s="29"/>
-      <c r="T2" s="29" t="s">
-        <v>1125</v>
+      <c r="T2" s="43" t="s">
+        <v>1122</v>
       </c>
       <c r="U2" s="29"/>
       <c r="V2" s="29" t="s">
@@ -16100,7 +16139,7 @@
       </c>
       <c r="W2" s="29"/>
       <c r="X2" s="29" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="Y2" s="29"/>
       <c r="Z2" s="34"/>
@@ -16113,7 +16152,7 @@
         <v>772</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="22" t="s">
@@ -16145,8 +16184,8 @@
         <v>774</v>
       </c>
       <c r="S3" s="22"/>
-      <c r="T3" s="22" t="s">
-        <v>1126</v>
+      <c r="T3" s="44" t="s">
+        <v>1123</v>
       </c>
       <c r="U3" s="22"/>
       <c r="V3" s="22" t="s">
@@ -16154,7 +16193,7 @@
       </c>
       <c r="W3" s="22"/>
       <c r="X3" s="22" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="Y3" s="22"/>
       <c r="Z3" s="36"/>
@@ -16167,7 +16206,7 @@
         <v>773</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="22" t="s">
@@ -16177,7 +16216,7 @@
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
       <c r="I4" s="22" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>781</v>
@@ -16199,8 +16238,8 @@
         <v>775</v>
       </c>
       <c r="S4" s="22"/>
-      <c r="T4" s="22" t="s">
-        <v>1127</v>
+      <c r="T4" s="44" t="s">
+        <v>1124</v>
       </c>
       <c r="U4" s="22"/>
       <c r="V4" s="22" t="s">
@@ -16208,12 +16247,12 @@
       </c>
       <c r="W4" s="22"/>
       <c r="X4" s="22" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
       <c r="Y4" s="22"/>
       <c r="Z4" s="36"/>
     </row>
-    <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="33" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>198</v>
       </c>
@@ -16231,7 +16270,7 @@
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
       <c r="I5" s="22" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="J5" s="22" t="s">
         <v>434</v>
@@ -16253,7 +16292,7 @@
         <v>682</v>
       </c>
       <c r="S5" s="22"/>
-      <c r="T5" s="22" t="s">
+      <c r="T5" s="44" t="s">
         <v>910</v>
       </c>
       <c r="U5" s="22"/>
@@ -16262,7 +16301,7 @@
       </c>
       <c r="W5" s="22"/>
       <c r="X5" s="22" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="Y5" s="22"/>
       <c r="Z5" s="36"/>
@@ -16293,7 +16332,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
+      <c r="T6" s="44"/>
       <c r="U6" s="22"/>
       <c r="V6" s="22"/>
       <c r="W6" s="22"/>
@@ -16331,7 +16370,7 @@
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
+      <c r="T7" s="44"/>
       <c r="U7" s="22"/>
       <c r="V7" s="22"/>
       <c r="W7" s="22"/>
@@ -16365,7 +16404,7 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="22"/>
-      <c r="T8" s="22"/>
+      <c r="T8" s="44"/>
       <c r="U8" s="22"/>
       <c r="V8" s="22"/>
       <c r="W8" s="22"/>
@@ -16399,7 +16438,7 @@
       <c r="Q9" s="22"/>
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
-      <c r="T9" s="22"/>
+      <c r="T9" s="44"/>
       <c r="U9" s="22"/>
       <c r="V9" s="22"/>
       <c r="W9" s="22"/>
@@ -16433,7 +16472,7 @@
       <c r="Q10" s="22"/>
       <c r="R10" s="22"/>
       <c r="S10" s="22"/>
-      <c r="T10" s="22"/>
+      <c r="T10" s="44"/>
       <c r="U10" s="22"/>
       <c r="V10" s="22"/>
       <c r="W10" s="22"/>
@@ -16469,7 +16508,7 @@
       <c r="Q11" s="22"/>
       <c r="R11" s="22"/>
       <c r="S11" s="22"/>
-      <c r="T11" s="22"/>
+      <c r="T11" s="44"/>
       <c r="U11" s="22"/>
       <c r="V11" s="22"/>
       <c r="W11" s="22"/>
@@ -16505,7 +16544,7 @@
         <v>825</v>
       </c>
       <c r="S12" s="22"/>
-      <c r="T12" s="22"/>
+      <c r="T12" s="44"/>
       <c r="U12" s="22"/>
       <c r="V12" s="22"/>
       <c r="W12" s="22"/>
@@ -16539,7 +16578,7 @@
       <c r="Q13" s="22"/>
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
-      <c r="T13" s="22" t="s">
+      <c r="T13" s="44" t="s">
         <v>911</v>
       </c>
       <c r="U13" s="22"/>
@@ -16577,7 +16616,7 @@
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="22"/>
-      <c r="T14" s="22"/>
+      <c r="T14" s="44"/>
       <c r="U14" s="22"/>
       <c r="V14" s="22"/>
       <c r="W14" s="22"/>
@@ -16611,7 +16650,7 @@
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
-      <c r="T15" s="22"/>
+      <c r="T15" s="44"/>
       <c r="U15" s="22"/>
       <c r="V15" s="22" t="s">
         <v>831</v>
@@ -16649,7 +16688,7 @@
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
-      <c r="T16" s="22"/>
+      <c r="T16" s="44"/>
       <c r="U16" s="22"/>
       <c r="V16" s="22"/>
       <c r="W16" s="22"/>
@@ -16683,7 +16722,7 @@
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="22"/>
-      <c r="T17" s="22"/>
+      <c r="T17" s="44"/>
       <c r="U17" s="22"/>
       <c r="V17" s="22"/>
       <c r="W17" s="22"/>
@@ -16719,7 +16758,7 @@
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
       <c r="S18" s="22"/>
-      <c r="T18" s="22"/>
+      <c r="T18" s="44"/>
       <c r="U18" s="22"/>
       <c r="V18" s="22"/>
       <c r="W18" s="22"/>
@@ -16753,7 +16792,7 @@
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="22"/>
-      <c r="T19" s="22"/>
+      <c r="T19" s="44"/>
       <c r="U19" s="22"/>
       <c r="V19" s="22"/>
       <c r="W19" s="22"/>
@@ -16775,7 +16814,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
       <c r="G20" s="22" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="H20" s="22"/>
       <c r="I20" s="22"/>
@@ -16789,7 +16828,7 @@
       <c r="Q20" s="22"/>
       <c r="R20" s="22"/>
       <c r="S20" s="22"/>
-      <c r="T20" s="22"/>
+      <c r="T20" s="44"/>
       <c r="U20" s="22"/>
       <c r="V20" s="22"/>
       <c r="W20" s="22"/>
@@ -16823,7 +16862,7 @@
       <c r="Q21" s="22"/>
       <c r="R21" s="22"/>
       <c r="S21" s="22"/>
-      <c r="T21" s="22"/>
+      <c r="T21" s="44"/>
       <c r="U21" s="22"/>
       <c r="V21" s="22"/>
       <c r="W21" s="22"/>
@@ -16861,7 +16900,7 @@
       <c r="Q22" s="22"/>
       <c r="R22" s="22"/>
       <c r="S22" s="22"/>
-      <c r="T22" s="22"/>
+      <c r="T22" s="44"/>
       <c r="U22" s="22"/>
       <c r="V22" s="22"/>
       <c r="W22" s="22"/>
@@ -16901,12 +16940,12 @@
       <c r="Q23" s="22"/>
       <c r="R23" s="22"/>
       <c r="S23" s="22"/>
-      <c r="T23" s="22"/>
+      <c r="T23" s="44"/>
       <c r="U23" s="22"/>
       <c r="V23" s="22"/>
       <c r="W23" s="22"/>
       <c r="X23" s="22" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="Y23" s="22"/>
       <c r="Z23" s="36"/>
@@ -16941,7 +16980,7 @@
       <c r="Q24" s="22"/>
       <c r="R24" s="22"/>
       <c r="S24" s="22"/>
-      <c r="T24" s="22"/>
+      <c r="T24" s="44"/>
       <c r="U24" s="22"/>
       <c r="V24" s="22"/>
       <c r="W24" s="22"/>
@@ -16977,7 +17016,7 @@
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
       <c r="S25" s="22"/>
-      <c r="T25" s="22"/>
+      <c r="T25" s="44"/>
       <c r="U25" s="22"/>
       <c r="V25" s="22"/>
       <c r="W25" s="22"/>
@@ -17013,7 +17052,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="22"/>
-      <c r="T26" s="22"/>
+      <c r="T26" s="44"/>
       <c r="U26" s="22"/>
       <c r="V26" s="22"/>
       <c r="W26" s="22"/>
@@ -17047,7 +17086,7 @@
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="22"/>
-      <c r="T27" s="22"/>
+      <c r="T27" s="44"/>
       <c r="U27" s="22"/>
       <c r="V27" s="22"/>
       <c r="W27" s="22"/>
@@ -17081,7 +17120,7 @@
       <c r="Q28" s="22"/>
       <c r="R28" s="22"/>
       <c r="S28" s="22"/>
-      <c r="T28" s="22"/>
+      <c r="T28" s="44"/>
       <c r="U28" s="22"/>
       <c r="V28" s="22"/>
       <c r="W28" s="22"/>
@@ -17115,7 +17154,7 @@
       <c r="Q29" s="22"/>
       <c r="R29" s="22"/>
       <c r="S29" s="22"/>
-      <c r="T29" s="22"/>
+      <c r="T29" s="44"/>
       <c r="U29" s="22"/>
       <c r="V29" s="22"/>
       <c r="W29" s="22"/>
@@ -17149,7 +17188,7 @@
       <c r="Q30" s="27"/>
       <c r="R30" s="27"/>
       <c r="S30" s="27"/>
-      <c r="T30" s="27"/>
+      <c r="T30" s="45"/>
       <c r="U30" s="27"/>
       <c r="V30" s="27"/>
       <c r="W30" s="27"/>
@@ -17175,7 +17214,7 @@
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
       <c r="I31" s="22" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="J31" s="20" t="s">
         <v>417</v>
@@ -17197,7 +17236,7 @@
         <v>664</v>
       </c>
       <c r="S31" s="20"/>
-      <c r="T31" s="20" t="s">
+      <c r="T31" s="44" t="s">
         <v>912</v>
       </c>
       <c r="U31" s="20"/>
@@ -17206,7 +17245,7 @@
       </c>
       <c r="W31" s="20"/>
       <c r="X31" s="20" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="Y31" s="20"/>
       <c r="Z31" s="39"/>
@@ -17229,7 +17268,7 @@
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
       <c r="I32" s="22" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="J32" s="20" t="s">
         <v>418</v>
@@ -17251,7 +17290,7 @@
         <v>665</v>
       </c>
       <c r="S32" s="20"/>
-      <c r="T32" s="20" t="s">
+      <c r="T32" s="44" t="s">
         <v>913</v>
       </c>
       <c r="U32" s="20"/>
@@ -17260,7 +17299,7 @@
       </c>
       <c r="W32" s="20"/>
       <c r="X32" s="20" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="Y32" s="20"/>
       <c r="Z32" s="39"/>
@@ -17305,7 +17344,7 @@
         <v>666</v>
       </c>
       <c r="S33" s="20"/>
-      <c r="T33" s="20" t="s">
+      <c r="T33" s="44" t="s">
         <v>914</v>
       </c>
       <c r="U33" s="20"/>
@@ -17314,7 +17353,7 @@
       </c>
       <c r="W33" s="20"/>
       <c r="X33" s="20" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="Y33" s="20"/>
       <c r="Z33" s="39"/>
@@ -17337,7 +17376,7 @@
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
       <c r="I34" s="22" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="J34" s="20" t="s">
         <v>420</v>
@@ -17359,7 +17398,7 @@
         <v>667</v>
       </c>
       <c r="S34" s="20"/>
-      <c r="T34" s="20" t="s">
+      <c r="T34" s="44" t="s">
         <v>915</v>
       </c>
       <c r="U34" s="20"/>
@@ -17368,7 +17407,7 @@
       </c>
       <c r="W34" s="20"/>
       <c r="X34" s="20" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="Y34" s="20"/>
       <c r="Z34" s="39"/>
@@ -17413,7 +17452,7 @@
         <v>668</v>
       </c>
       <c r="S35" s="20"/>
-      <c r="T35" s="20" t="s">
+      <c r="T35" s="44" t="s">
         <v>916</v>
       </c>
       <c r="U35" s="20"/>
@@ -17422,12 +17461,12 @@
       </c>
       <c r="W35" s="20"/>
       <c r="X35" s="20" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="Y35" s="20"/>
       <c r="Z35" s="39"/>
     </row>
-    <row r="36" spans="1:26" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" s="35" customFormat="1" ht="33" x14ac:dyDescent="0.25">
       <c r="A36" s="33" t="s">
         <v>199</v>
       </c>
@@ -17467,7 +17506,7 @@
         <v>669</v>
       </c>
       <c r="S36" s="20"/>
-      <c r="T36" s="20" t="s">
+      <c r="T36" s="44" t="s">
         <v>917</v>
       </c>
       <c r="U36" s="20"/>
@@ -17476,12 +17515,12 @@
       </c>
       <c r="W36" s="20"/>
       <c r="X36" s="20" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="Y36" s="20"/>
       <c r="Z36" s="39"/>
     </row>
-    <row r="37" spans="1:26" s="35" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" s="35" customFormat="1" ht="33" x14ac:dyDescent="0.25">
       <c r="A37" s="33" t="s">
         <v>199</v>
       </c>
@@ -17521,7 +17560,7 @@
         <v>670</v>
       </c>
       <c r="S37" s="20"/>
-      <c r="T37" s="20" t="s">
+      <c r="T37" s="44" t="s">
         <v>918</v>
       </c>
       <c r="U37" s="20"/>
@@ -17530,12 +17569,12 @@
       </c>
       <c r="W37" s="20"/>
       <c r="X37" s="20" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="Y37" s="20"/>
       <c r="Z37" s="39"/>
     </row>
-    <row r="38" spans="1:26" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" s="35" customFormat="1" ht="33" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
         <v>199</v>
       </c>
@@ -17553,7 +17592,7 @@
       <c r="G38" s="20"/>
       <c r="H38" s="20"/>
       <c r="I38" s="22" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="J38" s="20" t="s">
         <v>424</v>
@@ -17575,7 +17614,7 @@
         <v>671</v>
       </c>
       <c r="S38" s="20"/>
-      <c r="T38" s="20" t="s">
+      <c r="T38" s="44" t="s">
         <v>919</v>
       </c>
       <c r="U38" s="20"/>
@@ -17584,7 +17623,7 @@
       </c>
       <c r="W38" s="20"/>
       <c r="X38" s="20" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="Y38" s="20"/>
       <c r="Z38" s="39"/>
@@ -17629,7 +17668,7 @@
         <v>672</v>
       </c>
       <c r="S39" s="20"/>
-      <c r="T39" s="20" t="s">
+      <c r="T39" s="44" t="s">
         <v>920</v>
       </c>
       <c r="U39" s="20"/>
@@ -17638,7 +17677,7 @@
       </c>
       <c r="W39" s="20"/>
       <c r="X39" s="20" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="Y39" s="20"/>
       <c r="Z39" s="39"/>
@@ -17683,7 +17722,7 @@
         <v>673</v>
       </c>
       <c r="S40" s="20"/>
-      <c r="T40" s="20" t="s">
+      <c r="T40" s="44" t="s">
         <v>921</v>
       </c>
       <c r="U40" s="20"/>
@@ -17692,7 +17731,7 @@
       </c>
       <c r="W40" s="20"/>
       <c r="X40" s="20" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="Y40" s="20"/>
       <c r="Z40" s="39"/>
@@ -17737,7 +17776,7 @@
         <v>674</v>
       </c>
       <c r="S41" s="20"/>
-      <c r="T41" s="20" t="s">
+      <c r="T41" s="44" t="s">
         <v>922</v>
       </c>
       <c r="U41" s="20"/>
@@ -17746,12 +17785,12 @@
       </c>
       <c r="W41" s="20"/>
       <c r="X41" s="20" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="Y41" s="20"/>
       <c r="Z41" s="39"/>
     </row>
-    <row r="42" spans="1:26" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" s="35" customFormat="1" ht="33" x14ac:dyDescent="0.25">
       <c r="A42" s="33" t="s">
         <v>199</v>
       </c>
@@ -17759,7 +17798,7 @@
         <v>213</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="D42" s="21"/>
       <c r="E42" s="20" t="s">
@@ -17769,10 +17808,10 @@
       <c r="G42" s="20"/>
       <c r="H42" s="20"/>
       <c r="I42" s="22" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
       <c r="J42" s="20" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="K42" s="20"/>
       <c r="L42" s="20" t="s">
@@ -17791,8 +17830,8 @@
         <v>675</v>
       </c>
       <c r="S42" s="20"/>
-      <c r="T42" s="20" t="s">
-        <v>1128</v>
+      <c r="T42" s="44" t="s">
+        <v>1125</v>
       </c>
       <c r="U42" s="20"/>
       <c r="V42" s="20" t="s">
@@ -17800,7 +17839,7 @@
       </c>
       <c r="W42" s="20"/>
       <c r="X42" s="20" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="Y42" s="20"/>
       <c r="Z42" s="39"/>
@@ -17823,7 +17862,7 @@
       <c r="G43" s="20"/>
       <c r="H43" s="20"/>
       <c r="I43" s="22" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="J43" s="20" t="s">
         <v>428</v>
@@ -17845,7 +17884,7 @@
         <v>676</v>
       </c>
       <c r="S43" s="20"/>
-      <c r="T43" s="20" t="s">
+      <c r="T43" s="44" t="s">
         <v>923</v>
       </c>
       <c r="U43" s="20"/>
@@ -17854,12 +17893,12 @@
       </c>
       <c r="W43" s="20"/>
       <c r="X43" s="20" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="Y43" s="20"/>
       <c r="Z43" s="39"/>
     </row>
-    <row r="44" spans="1:26" s="35" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" s="35" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A44" s="33" t="s">
         <v>199</v>
       </c>
@@ -17877,7 +17916,7 @@
       <c r="G44" s="20"/>
       <c r="H44" s="20"/>
       <c r="I44" s="22" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
       <c r="J44" s="20" t="s">
         <v>429</v>
@@ -17899,7 +17938,7 @@
         <v>677</v>
       </c>
       <c r="S44" s="20"/>
-      <c r="T44" s="20" t="s">
+      <c r="T44" s="44" t="s">
         <v>924</v>
       </c>
       <c r="U44" s="20"/>
@@ -17908,12 +17947,12 @@
       </c>
       <c r="W44" s="20"/>
       <c r="X44" s="20" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="Y44" s="20"/>
       <c r="Z44" s="39"/>
     </row>
-    <row r="45" spans="1:26" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" s="35" customFormat="1" ht="33" x14ac:dyDescent="0.25">
       <c r="A45" s="33" t="s">
         <v>199</v>
       </c>
@@ -17921,7 +17960,7 @@
         <v>803</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="D45" s="21"/>
       <c r="E45" s="20" t="s">
@@ -17931,7 +17970,7 @@
       <c r="G45" s="20"/>
       <c r="H45" s="20"/>
       <c r="I45" s="22" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="J45" s="20" t="s">
         <v>804</v>
@@ -17953,8 +17992,8 @@
         <v>809</v>
       </c>
       <c r="S45" s="20"/>
-      <c r="T45" s="20" t="s">
-        <v>1129</v>
+      <c r="T45" s="44" t="s">
+        <v>1126</v>
       </c>
       <c r="U45" s="20"/>
       <c r="V45" s="20" t="s">
@@ -17962,7 +18001,7 @@
       </c>
       <c r="W45" s="20"/>
       <c r="X45" s="20" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="Y45" s="20"/>
       <c r="Z45" s="39"/>
@@ -18007,7 +18046,7 @@
         <v>678</v>
       </c>
       <c r="S46" s="20"/>
-      <c r="T46" s="20" t="s">
+      <c r="T46" s="44" t="s">
         <v>925</v>
       </c>
       <c r="U46" s="20"/>
@@ -18016,7 +18055,7 @@
       </c>
       <c r="W46" s="20"/>
       <c r="X46" s="20" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="Y46" s="20"/>
       <c r="Z46" s="39"/>
@@ -18039,7 +18078,7 @@
       <c r="G47" s="20"/>
       <c r="H47" s="20"/>
       <c r="I47" s="22" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="J47" s="20" t="s">
         <v>811</v>
@@ -18061,7 +18100,7 @@
         <v>815</v>
       </c>
       <c r="S47" s="20"/>
-      <c r="T47" s="20" t="s">
+      <c r="T47" s="44" t="s">
         <v>926</v>
       </c>
       <c r="U47" s="20"/>
@@ -18070,12 +18109,12 @@
       </c>
       <c r="W47" s="20"/>
       <c r="X47" s="20" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="Y47" s="20"/>
       <c r="Z47" s="39"/>
     </row>
-    <row r="48" spans="1:26" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" s="35" customFormat="1" ht="33" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
         <v>199</v>
       </c>
@@ -18093,7 +18132,7 @@
       <c r="G48" s="20"/>
       <c r="H48" s="20"/>
       <c r="I48" s="22" t="s">
-        <v>1084</v>
+        <v>1081</v>
       </c>
       <c r="J48" s="20" t="s">
         <v>431</v>
@@ -18115,7 +18154,7 @@
         <v>679</v>
       </c>
       <c r="S48" s="20"/>
-      <c r="T48" s="20" t="s">
+      <c r="T48" s="44" t="s">
         <v>927</v>
       </c>
       <c r="U48" s="20"/>
@@ -18124,7 +18163,7 @@
       </c>
       <c r="W48" s="20"/>
       <c r="X48" s="20" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="Y48" s="20"/>
       <c r="Z48" s="39"/>
@@ -18147,7 +18186,7 @@
       <c r="G49" s="20"/>
       <c r="H49" s="20"/>
       <c r="I49" s="22" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="J49" s="20" t="s">
         <v>432</v>
@@ -18169,7 +18208,7 @@
         <v>680</v>
       </c>
       <c r="S49" s="20"/>
-      <c r="T49" s="20" t="s">
+      <c r="T49" s="44" t="s">
         <v>928</v>
       </c>
       <c r="U49" s="20"/>
@@ -18178,7 +18217,7 @@
       </c>
       <c r="W49" s="20"/>
       <c r="X49" s="20" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="Y49" s="20"/>
       <c r="Z49" s="39"/>
@@ -18201,7 +18240,7 @@
       <c r="G50" s="20"/>
       <c r="H50" s="20"/>
       <c r="I50" s="22" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="J50" s="20" t="s">
         <v>433</v>
@@ -18223,7 +18262,7 @@
         <v>681</v>
       </c>
       <c r="S50" s="20"/>
-      <c r="T50" s="20" t="s">
+      <c r="T50" s="44" t="s">
         <v>929</v>
       </c>
       <c r="U50" s="20"/>
@@ -18232,7 +18271,7 @@
       </c>
       <c r="W50" s="20"/>
       <c r="X50" s="20" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="Y50" s="20"/>
       <c r="Z50" s="39"/>
@@ -18255,7 +18294,7 @@
       <c r="G51" s="22"/>
       <c r="H51" s="22"/>
       <c r="I51" s="22" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="J51" s="22" t="s">
         <v>733</v>
@@ -18277,7 +18316,7 @@
         <v>748</v>
       </c>
       <c r="S51" s="22"/>
-      <c r="T51" s="22" t="s">
+      <c r="T51" s="44" t="s">
         <v>930</v>
       </c>
       <c r="U51" s="22"/>
@@ -18286,7 +18325,7 @@
       </c>
       <c r="W51" s="22"/>
       <c r="X51" s="22" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="Y51" s="22"/>
       <c r="Z51" s="36"/>
@@ -18309,7 +18348,7 @@
       <c r="G52" s="22"/>
       <c r="H52" s="22"/>
       <c r="I52" s="22" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="J52" s="22" t="s">
         <v>746</v>
@@ -18331,7 +18370,7 @@
         <v>749</v>
       </c>
       <c r="S52" s="22"/>
-      <c r="T52" s="22" t="s">
+      <c r="T52" s="44" t="s">
         <v>931</v>
       </c>
       <c r="U52" s="22"/>
@@ -18340,7 +18379,7 @@
       </c>
       <c r="W52" s="22"/>
       <c r="X52" s="22" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="Y52" s="22"/>
       <c r="Z52" s="36"/>
@@ -18385,7 +18424,7 @@
         <v>750</v>
       </c>
       <c r="S53" s="22"/>
-      <c r="T53" s="22" t="s">
+      <c r="T53" s="44" t="s">
         <v>932</v>
       </c>
       <c r="U53" s="22"/>
@@ -18394,7 +18433,7 @@
       </c>
       <c r="W53" s="22"/>
       <c r="X53" s="22" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="Y53" s="22"/>
       <c r="Z53" s="36"/>
@@ -18417,7 +18456,7 @@
       <c r="G54" s="22"/>
       <c r="H54" s="22"/>
       <c r="I54" s="22" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="J54" s="22" t="s">
         <v>435</v>
@@ -18439,7 +18478,7 @@
         <v>683</v>
       </c>
       <c r="S54" s="22"/>
-      <c r="T54" s="22" t="s">
+      <c r="T54" s="44" t="s">
         <v>933</v>
       </c>
       <c r="U54" s="22"/>
@@ -18448,12 +18487,12 @@
       </c>
       <c r="W54" s="22"/>
       <c r="X54" s="22" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="Y54" s="22"/>
       <c r="Z54" s="36"/>
     </row>
-    <row r="55" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" ht="33" x14ac:dyDescent="0.25">
       <c r="A55" s="33" t="s">
         <v>198</v>
       </c>
@@ -18493,8 +18532,8 @@
         <v>768</v>
       </c>
       <c r="S55" s="22"/>
-      <c r="T55" s="22" t="s">
-        <v>934</v>
+      <c r="T55" s="44" t="s">
+        <v>1128</v>
       </c>
       <c r="U55" s="22"/>
       <c r="V55" s="22" t="s">
@@ -18502,12 +18541,12 @@
       </c>
       <c r="W55" s="22"/>
       <c r="X55" s="22" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="Y55" s="22"/>
       <c r="Z55" s="36"/>
     </row>
-    <row r="56" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A56" s="33" t="s">
         <v>198</v>
       </c>
@@ -18515,7 +18554,7 @@
         <v>44</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="D56" s="23"/>
       <c r="E56" s="22" t="s">
@@ -18525,7 +18564,7 @@
       <c r="G56" s="22"/>
       <c r="H56" s="22"/>
       <c r="I56" s="22" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="J56" s="22" t="s">
         <v>437</v>
@@ -18547,8 +18586,8 @@
         <v>684</v>
       </c>
       <c r="S56" s="22"/>
-      <c r="T56" s="22" t="s">
-        <v>1130</v>
+      <c r="T56" s="44" t="s">
+        <v>1129</v>
       </c>
       <c r="U56" s="22"/>
       <c r="V56" s="22" t="s">
@@ -18556,7 +18595,7 @@
       </c>
       <c r="W56" s="22"/>
       <c r="X56" s="22" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="Y56" s="22"/>
       <c r="Z56" s="36"/>
@@ -18579,7 +18618,7 @@
       <c r="G57" s="22"/>
       <c r="H57" s="22"/>
       <c r="I57" s="22" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="J57" s="22" t="s">
         <v>438</v>
@@ -18601,8 +18640,8 @@
         <v>685</v>
       </c>
       <c r="S57" s="22"/>
-      <c r="T57" s="22" t="s">
-        <v>935</v>
+      <c r="T57" s="44" t="s">
+        <v>934</v>
       </c>
       <c r="U57" s="22"/>
       <c r="V57" s="22" t="s">
@@ -18610,7 +18649,7 @@
       </c>
       <c r="W57" s="22"/>
       <c r="X57" s="22" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="Y57" s="22"/>
       <c r="Z57" s="36"/>
@@ -18655,8 +18694,8 @@
         <v>686</v>
       </c>
       <c r="S58" s="22"/>
-      <c r="T58" s="22" t="s">
-        <v>936</v>
+      <c r="T58" s="44" t="s">
+        <v>935</v>
       </c>
       <c r="U58" s="22"/>
       <c r="V58" s="22" t="s">
@@ -18664,12 +18703,12 @@
       </c>
       <c r="W58" s="22"/>
       <c r="X58" s="22" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="Y58" s="22"/>
       <c r="Z58" s="36"/>
     </row>
-    <row r="59" spans="1:26" ht="165" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" ht="181.5" x14ac:dyDescent="0.25">
       <c r="A59" s="33" t="s">
         <v>198</v>
       </c>
@@ -18677,7 +18716,7 @@
         <v>326</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="D59" s="23"/>
       <c r="E59" s="22" t="s">
@@ -18687,7 +18726,7 @@
       <c r="G59" s="22"/>
       <c r="H59" s="22"/>
       <c r="I59" s="22" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="J59" s="22" t="s">
         <v>817</v>
@@ -18709,8 +18748,8 @@
         <v>821</v>
       </c>
       <c r="S59" s="22"/>
-      <c r="T59" s="22" t="s">
-        <v>1131</v>
+      <c r="T59" s="44" t="s">
+        <v>1127</v>
       </c>
       <c r="U59" s="22"/>
       <c r="V59" s="22" t="s">
@@ -18718,7 +18757,7 @@
       </c>
       <c r="W59" s="22"/>
       <c r="X59" s="22" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="Y59" s="22"/>
       <c r="Z59" s="36"/>
@@ -18763,8 +18802,8 @@
         <v>687</v>
       </c>
       <c r="S60" s="22"/>
-      <c r="T60" s="22" t="s">
-        <v>937</v>
+      <c r="T60" s="44" t="s">
+        <v>936</v>
       </c>
       <c r="U60" s="22"/>
       <c r="V60" s="22" t="s">
@@ -18772,12 +18811,12 @@
       </c>
       <c r="W60" s="22"/>
       <c r="X60" s="22" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="Y60" s="22"/>
       <c r="Z60" s="36"/>
     </row>
-    <row r="61" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" ht="66" x14ac:dyDescent="0.25">
       <c r="A61" s="33" t="s">
         <v>198</v>
       </c>
@@ -18795,7 +18834,7 @@
       <c r="G61" s="22"/>
       <c r="H61" s="22"/>
       <c r="I61" s="22" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
       <c r="J61" s="22" t="s">
         <v>441</v>
@@ -18817,8 +18856,8 @@
         <v>688</v>
       </c>
       <c r="S61" s="22"/>
-      <c r="T61" s="22" t="s">
-        <v>938</v>
+      <c r="T61" s="44" t="s">
+        <v>937</v>
       </c>
       <c r="U61" s="22"/>
       <c r="V61" s="22" t="s">
@@ -18826,7 +18865,7 @@
       </c>
       <c r="W61" s="22"/>
       <c r="X61" s="22" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="Y61" s="22"/>
       <c r="Z61" s="36"/>
@@ -18849,7 +18888,7 @@
       <c r="G62" s="22"/>
       <c r="H62" s="22"/>
       <c r="I62" s="22" t="s">
-        <v>1094</v>
+        <v>1091</v>
       </c>
       <c r="J62" s="22" t="s">
         <v>442</v>
@@ -18871,8 +18910,8 @@
         <v>689</v>
       </c>
       <c r="S62" s="22"/>
-      <c r="T62" s="22" t="s">
-        <v>939</v>
+      <c r="T62" s="44" t="s">
+        <v>938</v>
       </c>
       <c r="U62" s="22"/>
       <c r="V62" s="22" t="s">
@@ -18880,12 +18919,12 @@
       </c>
       <c r="W62" s="22"/>
       <c r="X62" s="22" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="Y62" s="22"/>
       <c r="Z62" s="36"/>
     </row>
-    <row r="63" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" ht="66" x14ac:dyDescent="0.25">
       <c r="A63" s="33" t="s">
         <v>198</v>
       </c>
@@ -18903,7 +18942,7 @@
       <c r="G63" s="22"/>
       <c r="H63" s="22"/>
       <c r="I63" s="22" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
       <c r="J63" s="22" t="s">
         <v>443</v>
@@ -18925,8 +18964,8 @@
         <v>690</v>
       </c>
       <c r="S63" s="22"/>
-      <c r="T63" s="22" t="s">
-        <v>940</v>
+      <c r="T63" s="44" t="s">
+        <v>939</v>
       </c>
       <c r="U63" s="22"/>
       <c r="V63" s="22" t="s">
@@ -18934,7 +18973,7 @@
       </c>
       <c r="W63" s="22"/>
       <c r="X63" s="22" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Y63" s="22"/>
       <c r="Z63" s="36"/>
@@ -18957,7 +18996,7 @@
       <c r="G64" s="22"/>
       <c r="H64" s="22"/>
       <c r="I64" s="22" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
       <c r="J64" s="22" t="s">
         <v>444</v>
@@ -18979,8 +19018,8 @@
         <v>691</v>
       </c>
       <c r="S64" s="22"/>
-      <c r="T64" s="22" t="s">
-        <v>941</v>
+      <c r="T64" s="44" t="s">
+        <v>940</v>
       </c>
       <c r="U64" s="22"/>
       <c r="V64" s="22" t="s">
@@ -18988,12 +19027,12 @@
       </c>
       <c r="W64" s="22"/>
       <c r="X64" s="22" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="Y64" s="22"/>
       <c r="Z64" s="36"/>
     </row>
-    <row r="65" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" ht="33" x14ac:dyDescent="0.25">
       <c r="A65" s="33" t="s">
         <v>198</v>
       </c>
@@ -19011,7 +19050,7 @@
       <c r="G65" s="22"/>
       <c r="H65" s="22"/>
       <c r="I65" s="22" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="J65" s="22" t="s">
         <v>445</v>
@@ -19033,8 +19072,8 @@
         <v>692</v>
       </c>
       <c r="S65" s="22"/>
-      <c r="T65" s="22" t="s">
-        <v>942</v>
+      <c r="T65" s="44" t="s">
+        <v>941</v>
       </c>
       <c r="U65" s="22"/>
       <c r="V65" s="22" t="s">
@@ -19042,7 +19081,7 @@
       </c>
       <c r="W65" s="22"/>
       <c r="X65" s="22" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="Y65" s="22"/>
       <c r="Z65" s="36"/>
@@ -19065,7 +19104,7 @@
       <c r="G66" s="22"/>
       <c r="H66" s="22"/>
       <c r="I66" s="23" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="J66" s="22" t="s">
         <v>446</v>
@@ -19087,8 +19126,8 @@
         <v>693</v>
       </c>
       <c r="S66" s="22"/>
-      <c r="T66" s="22" t="s">
-        <v>943</v>
+      <c r="T66" s="44" t="s">
+        <v>942</v>
       </c>
       <c r="U66" s="22"/>
       <c r="V66" s="22" t="s">
@@ -19096,7 +19135,7 @@
       </c>
       <c r="W66" s="22"/>
       <c r="X66" s="22" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="Y66" s="22"/>
       <c r="Z66" s="36"/>
@@ -19119,7 +19158,7 @@
       <c r="G67" s="22"/>
       <c r="H67" s="22"/>
       <c r="I67" s="23" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="J67" s="22" t="s">
         <v>447</v>
@@ -19141,8 +19180,8 @@
         <v>694</v>
       </c>
       <c r="S67" s="22"/>
-      <c r="T67" s="22" t="s">
-        <v>944</v>
+      <c r="T67" s="44" t="s">
+        <v>943</v>
       </c>
       <c r="U67" s="22"/>
       <c r="V67" s="22" t="s">
@@ -19150,12 +19189,12 @@
       </c>
       <c r="W67" s="22"/>
       <c r="X67" s="22" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="Y67" s="22"/>
       <c r="Z67" s="36"/>
     </row>
-    <row r="68" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" ht="33" x14ac:dyDescent="0.25">
       <c r="A68" s="33" t="s">
         <v>198</v>
       </c>
@@ -19173,7 +19212,7 @@
       <c r="G68" s="22"/>
       <c r="H68" s="22"/>
       <c r="I68" s="22" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="J68" s="22" t="s">
         <v>448</v>
@@ -19195,8 +19234,8 @@
         <v>695</v>
       </c>
       <c r="S68" s="22"/>
-      <c r="T68" s="22" t="s">
-        <v>945</v>
+      <c r="T68" s="44" t="s">
+        <v>944</v>
       </c>
       <c r="U68" s="22"/>
       <c r="V68" s="22" t="s">
@@ -19204,12 +19243,12 @@
       </c>
       <c r="W68" s="22"/>
       <c r="X68" s="22" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="Y68" s="22"/>
       <c r="Z68" s="36"/>
     </row>
-    <row r="69" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A69" s="33" t="s">
         <v>198</v>
       </c>
@@ -19227,7 +19266,7 @@
       <c r="G69" s="22"/>
       <c r="H69" s="22"/>
       <c r="I69" s="22" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="J69" s="22" t="s">
         <v>449</v>
@@ -19249,8 +19288,8 @@
         <v>696</v>
       </c>
       <c r="S69" s="22"/>
-      <c r="T69" s="22" t="s">
-        <v>946</v>
+      <c r="T69" s="44" t="s">
+        <v>945</v>
       </c>
       <c r="U69" s="22"/>
       <c r="V69" s="22" t="s">
@@ -19258,12 +19297,12 @@
       </c>
       <c r="W69" s="22"/>
       <c r="X69" s="22" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="Y69" s="22"/>
       <c r="Z69" s="36"/>
     </row>
-    <row r="70" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A70" s="33" t="s">
         <v>198</v>
       </c>
@@ -19281,7 +19320,7 @@
       <c r="G70" s="22"/>
       <c r="H70" s="22"/>
       <c r="I70" s="22" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="J70" s="22" t="s">
         <v>450</v>
@@ -19303,8 +19342,8 @@
         <v>697</v>
       </c>
       <c r="S70" s="22"/>
-      <c r="T70" s="22" t="s">
-        <v>947</v>
+      <c r="T70" s="44" t="s">
+        <v>946</v>
       </c>
       <c r="U70" s="22"/>
       <c r="V70" s="22" t="s">
@@ -19312,12 +19351,12 @@
       </c>
       <c r="W70" s="22"/>
       <c r="X70" s="22" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="Y70" s="22"/>
       <c r="Z70" s="36"/>
     </row>
-    <row r="71" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A71" s="33" t="s">
         <v>198</v>
       </c>
@@ -19357,8 +19396,8 @@
         <v>698</v>
       </c>
       <c r="S71" s="22"/>
-      <c r="T71" s="22" t="s">
-        <v>948</v>
+      <c r="T71" s="44" t="s">
+        <v>947</v>
       </c>
       <c r="U71" s="22"/>
       <c r="V71" s="22" t="s">
@@ -19366,12 +19405,12 @@
       </c>
       <c r="W71" s="22"/>
       <c r="X71" s="22" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="Y71" s="22"/>
       <c r="Z71" s="36"/>
     </row>
-    <row r="72" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" ht="33" x14ac:dyDescent="0.25">
       <c r="A72" s="33" t="s">
         <v>198</v>
       </c>
@@ -19411,8 +19450,8 @@
         <v>699</v>
       </c>
       <c r="S72" s="22"/>
-      <c r="T72" s="22" t="s">
-        <v>949</v>
+      <c r="T72" s="44" t="s">
+        <v>948</v>
       </c>
       <c r="U72" s="22"/>
       <c r="V72" s="22" t="s">
@@ -19420,12 +19459,12 @@
       </c>
       <c r="W72" s="22"/>
       <c r="X72" s="22" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="Y72" s="22"/>
       <c r="Z72" s="36"/>
     </row>
-    <row r="73" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" ht="33" x14ac:dyDescent="0.25">
       <c r="A73" s="33" t="s">
         <v>198</v>
       </c>
@@ -19465,8 +19504,8 @@
         <v>700</v>
       </c>
       <c r="S73" s="22"/>
-      <c r="T73" s="22" t="s">
-        <v>950</v>
+      <c r="T73" s="44" t="s">
+        <v>949</v>
       </c>
       <c r="U73" s="22"/>
       <c r="V73" s="22" t="s">
@@ -19474,12 +19513,12 @@
       </c>
       <c r="W73" s="22"/>
       <c r="X73" s="22" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="Y73" s="22"/>
       <c r="Z73" s="36"/>
     </row>
-    <row r="74" spans="1:26" ht="315" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" ht="346.5" x14ac:dyDescent="0.25">
       <c r="A74" s="33" t="s">
         <v>198</v>
       </c>
@@ -19497,7 +19536,7 @@
       <c r="G74" s="25"/>
       <c r="H74" s="22"/>
       <c r="I74" s="24" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="J74" s="22" t="s">
         <v>454</v>
@@ -19519,8 +19558,8 @@
         <v>701</v>
       </c>
       <c r="S74" s="22"/>
-      <c r="T74" s="22" t="s">
-        <v>951</v>
+      <c r="T74" s="44" t="s">
+        <v>950</v>
       </c>
       <c r="U74" s="22"/>
       <c r="V74" s="22" t="s">
@@ -19528,7 +19567,7 @@
       </c>
       <c r="W74" s="22"/>
       <c r="X74" s="22" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="Y74" s="22"/>
       <c r="Z74" s="36"/>
@@ -19541,7 +19580,7 @@
         <v>237</v>
       </c>
       <c r="C75" s="23" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="D75" s="23"/>
       <c r="E75" s="22" t="s">
@@ -19551,7 +19590,7 @@
       <c r="G75" s="22"/>
       <c r="H75" s="22"/>
       <c r="I75" s="41" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="J75" s="22" t="s">
         <v>455</v>
@@ -19573,8 +19612,8 @@
         <v>702</v>
       </c>
       <c r="S75" s="22"/>
-      <c r="T75" s="22" t="s">
-        <v>1132</v>
+      <c r="T75" s="44" t="s">
+        <v>1133</v>
       </c>
       <c r="U75" s="22"/>
       <c r="V75" s="22" t="s">
@@ -19582,7 +19621,7 @@
       </c>
       <c r="W75" s="22"/>
       <c r="X75" s="22" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="Y75" s="22"/>
       <c r="Z75" s="36"/>
@@ -19595,7 +19634,7 @@
         <v>240</v>
       </c>
       <c r="C76" s="23" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="D76" s="23"/>
       <c r="E76" s="22" t="s">
@@ -19627,8 +19666,8 @@
         <v>703</v>
       </c>
       <c r="S76" s="22"/>
-      <c r="T76" s="22" t="s">
-        <v>1133</v>
+      <c r="T76" s="44" t="s">
+        <v>1134</v>
       </c>
       <c r="U76" s="22"/>
       <c r="V76" s="22" t="s">
@@ -19636,7 +19675,7 @@
       </c>
       <c r="W76" s="22"/>
       <c r="X76" s="22" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="Y76" s="22"/>
       <c r="Z76" s="36"/>
@@ -19649,7 +19688,7 @@
         <v>241</v>
       </c>
       <c r="C77" s="23" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="D77" s="23"/>
       <c r="E77" s="22" t="s">
@@ -19681,8 +19720,8 @@
         <v>704</v>
       </c>
       <c r="S77" s="22"/>
-      <c r="T77" s="22" t="s">
-        <v>1134</v>
+      <c r="T77" s="44" t="s">
+        <v>1135</v>
       </c>
       <c r="U77" s="22"/>
       <c r="V77" s="22" t="s">
@@ -19690,7 +19729,7 @@
       </c>
       <c r="W77" s="22"/>
       <c r="X77" s="22" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="Y77" s="22"/>
       <c r="Z77" s="36"/>
@@ -19735,8 +19774,8 @@
         <v>705</v>
       </c>
       <c r="S78" s="22"/>
-      <c r="T78" s="22" t="s">
-        <v>952</v>
+      <c r="T78" s="44" t="s">
+        <v>951</v>
       </c>
       <c r="U78" s="22"/>
       <c r="V78" s="22" t="s">
@@ -19767,7 +19806,7 @@
       <c r="G79" s="22"/>
       <c r="H79" s="22"/>
       <c r="I79" s="22" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="J79" s="22" t="s">
         <v>459</v>
@@ -19789,8 +19828,8 @@
         <v>706</v>
       </c>
       <c r="S79" s="22"/>
-      <c r="T79" s="22" t="s">
-        <v>953</v>
+      <c r="T79" s="44" t="s">
+        <v>952</v>
       </c>
       <c r="U79" s="22"/>
       <c r="V79" s="22" t="s">
@@ -19798,7 +19837,7 @@
       </c>
       <c r="W79" s="22"/>
       <c r="X79" s="22" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="Y79" s="22"/>
       <c r="Z79" s="36"/>
@@ -19843,8 +19882,8 @@
         <v>707</v>
       </c>
       <c r="S80" s="22"/>
-      <c r="T80" s="22" t="s">
-        <v>954</v>
+      <c r="T80" s="44" t="s">
+        <v>953</v>
       </c>
       <c r="U80" s="22"/>
       <c r="V80" s="22" t="s">
@@ -19852,7 +19891,7 @@
       </c>
       <c r="W80" s="22"/>
       <c r="X80" s="22" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="Y80" s="22"/>
       <c r="Z80" s="36"/>
@@ -19897,8 +19936,8 @@
         <v>708</v>
       </c>
       <c r="S81" s="22"/>
-      <c r="T81" s="22" t="s">
-        <v>955</v>
+      <c r="T81" s="44" t="s">
+        <v>954</v>
       </c>
       <c r="U81" s="22"/>
       <c r="V81" s="22" t="s">
@@ -19906,7 +19945,7 @@
       </c>
       <c r="W81" s="22"/>
       <c r="X81" s="22" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="Y81" s="22"/>
       <c r="Z81" s="36"/>
@@ -19929,7 +19968,7 @@
       <c r="G82" s="22"/>
       <c r="H82" s="22"/>
       <c r="I82" s="22" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="J82" s="22" t="s">
         <v>462</v>
@@ -19951,8 +19990,8 @@
         <v>709</v>
       </c>
       <c r="S82" s="22"/>
-      <c r="T82" s="22" t="s">
-        <v>956</v>
+      <c r="T82" s="44" t="s">
+        <v>955</v>
       </c>
       <c r="U82" s="22"/>
       <c r="V82" s="22" t="s">
@@ -19960,7 +19999,7 @@
       </c>
       <c r="W82" s="22"/>
       <c r="X82" s="22" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="Y82" s="22"/>
       <c r="Z82" s="36"/>
@@ -20005,8 +20044,8 @@
         <v>710</v>
       </c>
       <c r="S83" s="22"/>
-      <c r="T83" s="22" t="s">
-        <v>957</v>
+      <c r="T83" s="44" t="s">
+        <v>956</v>
       </c>
       <c r="U83" s="22"/>
       <c r="V83" s="22" t="s">
@@ -20014,12 +20053,12 @@
       </c>
       <c r="W83" s="22"/>
       <c r="X83" s="22" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
       <c r="Y83" s="22"/>
       <c r="Z83" s="36"/>
     </row>
-    <row r="84" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" ht="33" x14ac:dyDescent="0.25">
       <c r="A84" s="33" t="s">
         <v>198</v>
       </c>
@@ -20059,8 +20098,8 @@
         <v>711</v>
       </c>
       <c r="S84" s="22"/>
-      <c r="T84" s="22" t="s">
-        <v>958</v>
+      <c r="T84" s="44" t="s">
+        <v>957</v>
       </c>
       <c r="U84" s="22"/>
       <c r="V84" s="22" t="s">
@@ -20068,7 +20107,7 @@
       </c>
       <c r="W84" s="22"/>
       <c r="X84" s="22" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
       <c r="Y84" s="22"/>
       <c r="Z84" s="36"/>
@@ -20113,8 +20152,8 @@
         <v>712</v>
       </c>
       <c r="S85" s="22"/>
-      <c r="T85" s="22" t="s">
-        <v>959</v>
+      <c r="T85" s="44" t="s">
+        <v>958</v>
       </c>
       <c r="U85" s="22"/>
       <c r="V85" s="22" t="s">
@@ -20122,7 +20161,7 @@
       </c>
       <c r="W85" s="22"/>
       <c r="X85" s="22" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
       <c r="Y85" s="22"/>
       <c r="Z85" s="36"/>
@@ -20167,8 +20206,8 @@
         <v>713</v>
       </c>
       <c r="S86" s="22"/>
-      <c r="T86" s="22" t="s">
-        <v>960</v>
+      <c r="T86" s="44" t="s">
+        <v>959</v>
       </c>
       <c r="U86" s="22"/>
       <c r="V86" s="22" t="s">
@@ -20176,7 +20215,7 @@
       </c>
       <c r="W86" s="22"/>
       <c r="X86" s="22" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="Y86" s="22"/>
       <c r="Z86" s="36"/>
@@ -20221,8 +20260,8 @@
         <v>714</v>
       </c>
       <c r="S87" s="22"/>
-      <c r="T87" s="22" t="s">
-        <v>961</v>
+      <c r="T87" s="44" t="s">
+        <v>960</v>
       </c>
       <c r="U87" s="22"/>
       <c r="V87" s="22" t="s">
@@ -20230,7 +20269,7 @@
       </c>
       <c r="W87" s="22"/>
       <c r="X87" s="22" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
       <c r="Y87" s="22"/>
       <c r="Z87" s="36"/>
@@ -20275,8 +20314,8 @@
         <v>715</v>
       </c>
       <c r="S88" s="22"/>
-      <c r="T88" s="22" t="s">
-        <v>962</v>
+      <c r="T88" s="44" t="s">
+        <v>961</v>
       </c>
       <c r="U88" s="22"/>
       <c r="V88" s="22" t="s">
@@ -20284,7 +20323,7 @@
       </c>
       <c r="W88" s="22"/>
       <c r="X88" s="22" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="Y88" s="22"/>
       <c r="Z88" s="36"/>
@@ -20329,8 +20368,8 @@
         <v>716</v>
       </c>
       <c r="S89" s="22"/>
-      <c r="T89" s="22" t="s">
-        <v>963</v>
+      <c r="T89" s="44" t="s">
+        <v>962</v>
       </c>
       <c r="U89" s="22"/>
       <c r="V89" s="22" t="s">
@@ -20338,7 +20377,7 @@
       </c>
       <c r="W89" s="22"/>
       <c r="X89" s="22" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
       <c r="Y89" s="22"/>
       <c r="Z89" s="36"/>
@@ -20361,7 +20400,7 @@
       <c r="G90" s="22"/>
       <c r="H90" s="22"/>
       <c r="I90" s="22" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="J90" s="22" t="s">
         <v>470</v>
@@ -20383,8 +20422,8 @@
         <v>717</v>
       </c>
       <c r="S90" s="25"/>
-      <c r="T90" s="25" t="s">
-        <v>964</v>
+      <c r="T90" s="46" t="s">
+        <v>963</v>
       </c>
       <c r="U90" s="22"/>
       <c r="V90" s="22" t="s">
@@ -20392,7 +20431,7 @@
       </c>
       <c r="W90" s="22"/>
       <c r="X90" s="22" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
       <c r="Y90" s="22"/>
       <c r="Z90" s="36"/>
@@ -20415,7 +20454,7 @@
       <c r="G91" s="22"/>
       <c r="H91" s="22"/>
       <c r="I91" s="22" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="J91" s="22" t="s">
         <v>471</v>
@@ -20437,8 +20476,8 @@
         <v>718</v>
       </c>
       <c r="S91" s="22"/>
-      <c r="T91" s="22" t="s">
-        <v>965</v>
+      <c r="T91" s="44" t="s">
+        <v>964</v>
       </c>
       <c r="U91" s="22"/>
       <c r="V91" s="22" t="s">
@@ -20446,7 +20485,7 @@
       </c>
       <c r="W91" s="22"/>
       <c r="X91" s="22" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="Y91" s="22"/>
       <c r="Z91" s="36"/>
@@ -20491,8 +20530,8 @@
         <v>719</v>
       </c>
       <c r="S92" s="22"/>
-      <c r="T92" s="22" t="s">
-        <v>966</v>
+      <c r="T92" s="44" t="s">
+        <v>965</v>
       </c>
       <c r="U92" s="22"/>
       <c r="V92" s="22" t="s">
@@ -20500,12 +20539,12 @@
       </c>
       <c r="W92" s="22"/>
       <c r="X92" s="22" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="Y92" s="22"/>
       <c r="Z92" s="36"/>
     </row>
-    <row r="93" spans="1:26" ht="285" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" ht="297" x14ac:dyDescent="0.25">
       <c r="A93" s="33" t="s">
         <v>198</v>
       </c>
@@ -20523,7 +20562,7 @@
       <c r="G93" s="25"/>
       <c r="H93" s="22"/>
       <c r="I93" s="24" t="s">
-        <v>1109</v>
+        <v>1106</v>
       </c>
       <c r="J93" s="22" t="s">
         <v>473</v>
@@ -20545,8 +20584,8 @@
         <v>720</v>
       </c>
       <c r="S93" s="22"/>
-      <c r="T93" s="22" t="s">
-        <v>967</v>
+      <c r="T93" s="44" t="s">
+        <v>966</v>
       </c>
       <c r="U93" s="22"/>
       <c r="V93" s="22" t="s">
@@ -20554,12 +20593,12 @@
       </c>
       <c r="W93" s="22"/>
       <c r="X93" s="22" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="Y93" s="22"/>
       <c r="Z93" s="36"/>
     </row>
-    <row r="94" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" ht="33" x14ac:dyDescent="0.25">
       <c r="A94" s="33" t="s">
         <v>198</v>
       </c>
@@ -20599,8 +20638,8 @@
         <v>721</v>
       </c>
       <c r="S94" s="22"/>
-      <c r="T94" s="22" t="s">
-        <v>968</v>
+      <c r="T94" s="44" t="s">
+        <v>967</v>
       </c>
       <c r="U94" s="22"/>
       <c r="V94" s="22" t="s">
@@ -20608,7 +20647,7 @@
       </c>
       <c r="W94" s="22"/>
       <c r="X94" s="22" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="Y94" s="22"/>
       <c r="Z94" s="36"/>
@@ -20653,8 +20692,8 @@
         <v>722</v>
       </c>
       <c r="S95" s="22"/>
-      <c r="T95" s="22" t="s">
-        <v>969</v>
+      <c r="T95" s="44" t="s">
+        <v>968</v>
       </c>
       <c r="U95" s="22"/>
       <c r="V95" s="22" t="s">
@@ -20662,12 +20701,12 @@
       </c>
       <c r="W95" s="22"/>
       <c r="X95" s="22" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="Y95" s="22"/>
       <c r="Z95" s="36"/>
     </row>
-    <row r="96" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" ht="33" x14ac:dyDescent="0.25">
       <c r="A96" s="33" t="s">
         <v>198</v>
       </c>
@@ -20707,8 +20746,8 @@
         <v>723</v>
       </c>
       <c r="S96" s="25"/>
-      <c r="T96" s="25" t="s">
-        <v>970</v>
+      <c r="T96" s="46" t="s">
+        <v>969</v>
       </c>
       <c r="U96" s="22"/>
       <c r="V96" s="22" t="s">
@@ -20716,12 +20755,12 @@
       </c>
       <c r="W96" s="22"/>
       <c r="X96" s="22" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="Y96" s="22"/>
       <c r="Z96" s="36"/>
     </row>
-    <row r="97" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" ht="33" x14ac:dyDescent="0.25">
       <c r="A97" s="33" t="s">
         <v>198</v>
       </c>
@@ -20761,8 +20800,8 @@
         <v>724</v>
       </c>
       <c r="S97" s="22"/>
-      <c r="T97" s="22" t="s">
-        <v>971</v>
+      <c r="T97" s="44" t="s">
+        <v>970</v>
       </c>
       <c r="U97" s="22"/>
       <c r="V97" s="22" t="s">
@@ -20770,12 +20809,12 @@
       </c>
       <c r="W97" s="22"/>
       <c r="X97" s="22" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="Y97" s="22"/>
       <c r="Z97" s="36"/>
     </row>
-    <row r="98" spans="1:26" ht="240" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" ht="264" x14ac:dyDescent="0.25">
       <c r="A98" s="33" t="s">
         <v>198</v>
       </c>
@@ -20793,7 +20832,7 @@
       <c r="G98" s="25"/>
       <c r="H98" s="22"/>
       <c r="I98" s="24" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="J98" s="22" t="s">
         <v>478</v>
@@ -20815,8 +20854,8 @@
         <v>725</v>
       </c>
       <c r="S98" s="22"/>
-      <c r="T98" s="22" t="s">
-        <v>972</v>
+      <c r="T98" s="44" t="s">
+        <v>971</v>
       </c>
       <c r="U98" s="22"/>
       <c r="V98" s="22" t="s">
@@ -20824,12 +20863,12 @@
       </c>
       <c r="W98" s="22"/>
       <c r="X98" s="22" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="Y98" s="22"/>
       <c r="Z98" s="36"/>
     </row>
-    <row r="99" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" ht="33" x14ac:dyDescent="0.25">
       <c r="A99" s="33" t="s">
         <v>198</v>
       </c>
@@ -20847,7 +20886,7 @@
       <c r="G99" s="22"/>
       <c r="H99" s="22"/>
       <c r="I99" s="22" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="J99" s="22" t="s">
         <v>479</v>
@@ -20869,8 +20908,8 @@
         <v>726</v>
       </c>
       <c r="S99" s="22"/>
-      <c r="T99" s="22" t="s">
-        <v>973</v>
+      <c r="T99" s="44" t="s">
+        <v>972</v>
       </c>
       <c r="U99" s="22"/>
       <c r="V99" s="22" t="s">
@@ -20878,12 +20917,12 @@
       </c>
       <c r="W99" s="22"/>
       <c r="X99" s="22" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="Y99" s="22"/>
       <c r="Z99" s="36"/>
     </row>
-    <row r="100" spans="1:26" ht="345" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:26" ht="396" x14ac:dyDescent="0.25">
       <c r="A100" s="33" t="s">
         <v>198</v>
       </c>
@@ -20901,7 +20940,7 @@
       <c r="G100" s="22"/>
       <c r="H100" s="22"/>
       <c r="I100" s="22" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="J100" s="22" t="s">
         <v>480</v>
@@ -20923,8 +20962,8 @@
         <v>727</v>
       </c>
       <c r="S100" s="22"/>
-      <c r="T100" s="22" t="s">
-        <v>974</v>
+      <c r="T100" s="44" t="s">
+        <v>973</v>
       </c>
       <c r="U100" s="22"/>
       <c r="V100" s="22" t="s">
@@ -20932,7 +20971,7 @@
       </c>
       <c r="W100" s="22"/>
       <c r="X100" s="22" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="Y100" s="22"/>
       <c r="Z100" s="36"/>
@@ -20945,7 +20984,7 @@
         <v>180</v>
       </c>
       <c r="C101" s="23" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="D101" s="23"/>
       <c r="E101" s="22" t="s">
@@ -20955,7 +20994,7 @@
       <c r="G101" s="22"/>
       <c r="H101" s="22"/>
       <c r="I101" s="22" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
       <c r="J101" s="22" t="s">
         <v>765</v>
@@ -20977,8 +21016,8 @@
         <v>769</v>
       </c>
       <c r="S101" s="22"/>
-      <c r="T101" s="22" t="s">
-        <v>1135</v>
+      <c r="T101" s="44" t="s">
+        <v>1130</v>
       </c>
       <c r="U101" s="22"/>
       <c r="V101" s="22" t="s">
@@ -20986,7 +21025,7 @@
       </c>
       <c r="W101" s="22"/>
       <c r="X101" s="22" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="Y101" s="22"/>
       <c r="Z101" s="36"/>
@@ -21009,7 +21048,7 @@
       <c r="G102" s="22"/>
       <c r="H102" s="22"/>
       <c r="I102" s="22" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="J102" s="22" t="s">
         <v>766</v>
@@ -21031,8 +21070,8 @@
         <v>770</v>
       </c>
       <c r="S102" s="22"/>
-      <c r="T102" s="22" t="s">
-        <v>975</v>
+      <c r="T102" s="44" t="s">
+        <v>1131</v>
       </c>
       <c r="U102" s="22"/>
       <c r="V102" s="22" t="s">
@@ -21040,7 +21079,7 @@
       </c>
       <c r="W102" s="22"/>
       <c r="X102" s="22" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="Y102" s="22"/>
       <c r="Z102" s="36"/>
@@ -21063,7 +21102,7 @@
       <c r="G103" s="22"/>
       <c r="H103" s="22"/>
       <c r="I103" s="22" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="J103" s="22" t="s">
         <v>767</v>
@@ -21085,8 +21124,8 @@
         <v>771</v>
       </c>
       <c r="S103" s="22"/>
-      <c r="T103" s="22" t="s">
-        <v>976</v>
+      <c r="T103" s="44" t="s">
+        <v>1132</v>
       </c>
       <c r="U103" s="22"/>
       <c r="V103" s="22" t="s">
@@ -21094,7 +21133,7 @@
       </c>
       <c r="W103" s="22"/>
       <c r="X103" s="22" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="Y103" s="22"/>
       <c r="Z103" s="36"/>
@@ -21139,8 +21178,8 @@
         <v>751</v>
       </c>
       <c r="S104" s="22"/>
-      <c r="T104" s="22" t="s">
-        <v>977</v>
+      <c r="T104" s="44" t="s">
+        <v>974</v>
       </c>
       <c r="U104" s="22"/>
       <c r="V104" s="22" t="s">
@@ -21148,7 +21187,7 @@
       </c>
       <c r="W104" s="22"/>
       <c r="X104" s="22" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="Y104" s="22"/>
       <c r="Z104" s="36"/>
@@ -21193,8 +21232,8 @@
         <v>757</v>
       </c>
       <c r="S105" s="22"/>
-      <c r="T105" s="22" t="s">
-        <v>978</v>
+      <c r="T105" s="44" t="s">
+        <v>975</v>
       </c>
       <c r="U105" s="22"/>
       <c r="V105" s="22" t="s">
@@ -21202,7 +21241,7 @@
       </c>
       <c r="W105" s="22"/>
       <c r="X105" s="22" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="Y105" s="22"/>
       <c r="Z105" s="36"/>
@@ -21248,14 +21287,14 @@
         <v>728</v>
       </c>
       <c r="S106" s="22"/>
-      <c r="T106" s="22"/>
+      <c r="T106" s="44"/>
       <c r="U106" s="22"/>
       <c r="V106" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W106" s="22"/>
       <c r="X106" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y106" s="22"/>
       <c r="Z106" s="36"/>
@@ -21301,14 +21340,14 @@
         <v>728</v>
       </c>
       <c r="S107" s="22"/>
-      <c r="T107" s="22"/>
+      <c r="T107" s="44"/>
       <c r="U107" s="22"/>
       <c r="V107" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W107" s="22"/>
       <c r="X107" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y107" s="22"/>
       <c r="Z107" s="36"/>
@@ -21354,14 +21393,14 @@
         <v>728</v>
       </c>
       <c r="S108" s="22"/>
-      <c r="T108" s="22"/>
+      <c r="T108" s="44"/>
       <c r="U108" s="22"/>
       <c r="V108" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W108" s="22"/>
       <c r="X108" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y108" s="22"/>
       <c r="Z108" s="36"/>
@@ -21407,14 +21446,14 @@
         <v>728</v>
       </c>
       <c r="S109" s="22"/>
-      <c r="T109" s="22"/>
+      <c r="T109" s="44"/>
       <c r="U109" s="22"/>
       <c r="V109" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W109" s="22"/>
       <c r="X109" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y109" s="22"/>
       <c r="Z109" s="36"/>
@@ -21460,14 +21499,14 @@
         <v>728</v>
       </c>
       <c r="S110" s="22"/>
-      <c r="T110" s="22"/>
+      <c r="T110" s="44"/>
       <c r="U110" s="22"/>
       <c r="V110" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W110" s="22"/>
       <c r="X110" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y110" s="22"/>
       <c r="Z110" s="36"/>
@@ -21513,14 +21552,14 @@
         <v>728</v>
       </c>
       <c r="S111" s="22"/>
-      <c r="T111" s="22"/>
+      <c r="T111" s="44"/>
       <c r="U111" s="22"/>
       <c r="V111" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W111" s="22"/>
       <c r="X111" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y111" s="22"/>
       <c r="Z111" s="36"/>
@@ -21566,19 +21605,19 @@
         <v>728</v>
       </c>
       <c r="S112" s="22"/>
-      <c r="T112" s="22"/>
+      <c r="T112" s="44"/>
       <c r="U112" s="22"/>
       <c r="V112" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W112" s="22"/>
       <c r="X112" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y112" s="22"/>
       <c r="Z112" s="36"/>
     </row>
-    <row r="113" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:26" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A113" s="33" t="s">
         <v>198</v>
       </c>
@@ -21619,8 +21658,8 @@
         <v>728</v>
       </c>
       <c r="S113" s="22"/>
-      <c r="T113" s="22" t="s">
-        <v>979</v>
+      <c r="T113" s="44" t="s">
+        <v>976</v>
       </c>
       <c r="U113" s="22"/>
       <c r="V113" s="22" t="s">
@@ -21628,7 +21667,7 @@
       </c>
       <c r="W113" s="22"/>
       <c r="X113" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y113" s="22"/>
       <c r="Z113" s="36"/>
@@ -21674,14 +21713,14 @@
         <v>728</v>
       </c>
       <c r="S114" s="22"/>
-      <c r="T114" s="22"/>
+      <c r="T114" s="44"/>
       <c r="U114" s="22"/>
       <c r="V114" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W114" s="22"/>
       <c r="X114" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y114" s="22"/>
       <c r="Z114" s="36"/>
@@ -21727,14 +21766,14 @@
         <v>728</v>
       </c>
       <c r="S115" s="22"/>
-      <c r="T115" s="22"/>
+      <c r="T115" s="44"/>
       <c r="U115" s="22"/>
       <c r="V115" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W115" s="22"/>
       <c r="X115" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y115" s="22"/>
       <c r="Z115" s="36"/>
@@ -21780,14 +21819,14 @@
         <v>728</v>
       </c>
       <c r="S116" s="22"/>
-      <c r="T116" s="22"/>
+      <c r="T116" s="44"/>
       <c r="U116" s="22"/>
       <c r="V116" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W116" s="22"/>
       <c r="X116" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y116" s="22"/>
       <c r="Z116" s="36"/>
@@ -21833,14 +21872,14 @@
         <v>728</v>
       </c>
       <c r="S117" s="22"/>
-      <c r="T117" s="22"/>
+      <c r="T117" s="44"/>
       <c r="U117" s="22"/>
       <c r="V117" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W117" s="22"/>
       <c r="X117" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y117" s="22"/>
       <c r="Z117" s="36"/>
@@ -21886,14 +21925,14 @@
         <v>728</v>
       </c>
       <c r="S118" s="22"/>
-      <c r="T118" s="22"/>
+      <c r="T118" s="44"/>
       <c r="U118" s="22"/>
       <c r="V118" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W118" s="22"/>
       <c r="X118" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y118" s="22"/>
       <c r="Z118" s="36"/>
@@ -21939,14 +21978,14 @@
         <v>728</v>
       </c>
       <c r="S119" s="22"/>
-      <c r="T119" s="22"/>
+      <c r="T119" s="44"/>
       <c r="U119" s="22"/>
       <c r="V119" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W119" s="22"/>
       <c r="X119" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y119" s="22"/>
       <c r="Z119" s="36"/>
@@ -21992,14 +22031,14 @@
         <v>728</v>
       </c>
       <c r="S120" s="22"/>
-      <c r="T120" s="22"/>
+      <c r="T120" s="44"/>
       <c r="U120" s="22"/>
       <c r="V120" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W120" s="22"/>
       <c r="X120" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y120" s="22"/>
       <c r="Z120" s="36"/>
@@ -22045,14 +22084,14 @@
         <v>728</v>
       </c>
       <c r="S121" s="22"/>
-      <c r="T121" s="22"/>
+      <c r="T121" s="44"/>
       <c r="U121" s="22"/>
       <c r="V121" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W121" s="22"/>
       <c r="X121" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y121" s="22"/>
       <c r="Z121" s="36"/>
@@ -22098,14 +22137,14 @@
         <v>728</v>
       </c>
       <c r="S122" s="22"/>
-      <c r="T122" s="22"/>
+      <c r="T122" s="44"/>
       <c r="U122" s="22"/>
       <c r="V122" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W122" s="22"/>
       <c r="X122" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y122" s="22"/>
       <c r="Z122" s="36"/>
@@ -22151,14 +22190,14 @@
         <v>728</v>
       </c>
       <c r="S123" s="22"/>
-      <c r="T123" s="22"/>
+      <c r="T123" s="44"/>
       <c r="U123" s="22"/>
       <c r="V123" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W123" s="22"/>
       <c r="X123" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y123" s="22"/>
       <c r="Z123" s="36"/>
@@ -22204,14 +22243,14 @@
         <v>728</v>
       </c>
       <c r="S124" s="22"/>
-      <c r="T124" s="22"/>
+      <c r="T124" s="44"/>
       <c r="U124" s="22"/>
       <c r="V124" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W124" s="22"/>
       <c r="X124" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y124" s="22"/>
       <c r="Z124" s="36"/>
@@ -22257,14 +22296,14 @@
         <v>728</v>
       </c>
       <c r="S125" s="22"/>
-      <c r="T125" s="22"/>
+      <c r="T125" s="44"/>
       <c r="U125" s="22"/>
       <c r="V125" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W125" s="22"/>
       <c r="X125" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y125" s="22"/>
       <c r="Z125" s="36"/>
@@ -22310,14 +22349,14 @@
         <v>728</v>
       </c>
       <c r="S126" s="22"/>
-      <c r="T126" s="22"/>
+      <c r="T126" s="44"/>
       <c r="U126" s="22"/>
       <c r="V126" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W126" s="22"/>
       <c r="X126" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y126" s="22"/>
       <c r="Z126" s="36"/>
@@ -22363,19 +22402,19 @@
         <v>728</v>
       </c>
       <c r="S127" s="22"/>
-      <c r="T127" s="22"/>
+      <c r="T127" s="44"/>
       <c r="U127" s="22"/>
       <c r="V127" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W127" s="22"/>
       <c r="X127" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y127" s="22"/>
       <c r="Z127" s="36"/>
     </row>
-    <row r="128" spans="1:26" ht="210" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:26" ht="231" x14ac:dyDescent="0.25">
       <c r="A128" s="33" t="s">
         <v>198</v>
       </c>
@@ -22416,8 +22455,8 @@
         <v>729</v>
       </c>
       <c r="S128" s="22"/>
-      <c r="T128" s="22" t="s">
-        <v>980</v>
+      <c r="T128" s="44" t="s">
+        <v>977</v>
       </c>
       <c r="U128" s="22"/>
       <c r="V128" s="22" t="s">
@@ -22425,7 +22464,7 @@
       </c>
       <c r="W128" s="22"/>
       <c r="X128" s="22" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="Y128" s="22"/>
       <c r="Z128" s="36"/>
@@ -22471,14 +22510,14 @@
         <v>728</v>
       </c>
       <c r="S129" s="22"/>
-      <c r="T129" s="22"/>
+      <c r="T129" s="44"/>
       <c r="U129" s="22"/>
       <c r="V129" s="22" t="s">
         <v>907</v>
       </c>
       <c r="W129" s="22"/>
       <c r="X129" s="22" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y129" s="22"/>
       <c r="Z129" s="36"/>
@@ -22524,14 +22563,14 @@
         <v>728</v>
       </c>
       <c r="S130" s="27"/>
-      <c r="T130" s="27"/>
+      <c r="T130" s="45"/>
       <c r="U130" s="27"/>
       <c r="V130" s="27" t="s">
         <v>907</v>
       </c>
       <c r="W130" s="27"/>
       <c r="X130" s="27" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="Y130" s="27"/>
       <c r="Z130" s="38"/>
@@ -22577,40 +22616,40 @@
     <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:H130 J1:Z130">
-    <cfRule type="containsBlanks" dxfId="6" priority="31">
+    <cfRule type="containsBlanks" dxfId="0" priority="31">
       <formula>LEN(TRIM(C1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62:B66 B68:B74 B51:B60 B78:B1048576 B1:B31">
-    <cfRule type="duplicateValues" dxfId="5" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I44 I46:I73 I94:I97 I76:I92 I99:I130">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="5" priority="5">
       <formula>LEN(TRIM(I1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="4" priority="4">
       <formula>LEN(TRIM(I45))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I74">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="3" priority="3">
       <formula>LEN(TRIM(I74))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I93">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(I93))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I98">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(I98))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -22618,8 +22657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22664,6 +22703,9 @@
       <c r="E2" t="s">
         <v>192</v>
       </c>
+      <c r="F2" t="s">
+        <v>1138</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -22681,6 +22723,9 @@
       <c r="E3" t="s">
         <v>193</v>
       </c>
+      <c r="F3" t="s">
+        <v>1138</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -22698,6 +22743,9 @@
       <c r="E4" t="s">
         <v>194</v>
       </c>
+      <c r="F4" t="s">
+        <v>1138</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -22715,6 +22763,9 @@
       <c r="E5" t="s">
         <v>195</v>
       </c>
+      <c r="F5" t="s">
+        <v>1138</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -22724,13 +22775,13 @@
         <v>230</v>
       </c>
       <c r="C6" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="E6" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="F6" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -22741,16 +22792,16 @@
         <v>230</v>
       </c>
       <c r="C7" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="D7" t="s">
         <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>1065</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1066</v>
+        <v>1062</v>
+      </c>
+      <c r="F7" s="48" t="s">
+        <v>1063</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -22761,16 +22812,16 @@
         <v>230</v>
       </c>
       <c r="C8" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="D8" t="s">
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="F8" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -22781,16 +22832,16 @@
         <v>230</v>
       </c>
       <c r="C9" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="D9" t="s">
         <v>191</v>
       </c>
       <c r="E9" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="F9" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -22872,67 +22923,79 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>909</v>
+        <v>301</v>
       </c>
       <c r="B14" t="s">
         <v>230</v>
       </c>
       <c r="C14" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E14" t="s">
         <v>1137</v>
       </c>
-      <c r="E14" t="s">
-        <v>1136</v>
+      <c r="F14" t="s">
+        <v>1139</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>909</v>
+        <v>301</v>
       </c>
       <c r="B15" t="s">
         <v>230</v>
       </c>
       <c r="C15" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D15" t="s">
         <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>1136</v>
+        <v>1137</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1139</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>909</v>
+        <v>301</v>
       </c>
       <c r="B16" t="s">
         <v>230</v>
       </c>
       <c r="C16" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>1136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1137</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>909</v>
+        <v>301</v>
       </c>
       <c r="B17" t="s">
         <v>230</v>
       </c>
       <c r="C17" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D17" t="s">
         <v>191</v>
       </c>
       <c r="E17" t="s">
-        <v>1136</v>
+        <v>1137</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some prose changes; but there is a new bug with languages requiring non-Latin font
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD9BF27-ECC8-4B06-B9C5-D51B6B5F550F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9A6243-87D4-4B4E-BEBD-FC9321574941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3083" uniqueCount="1387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3084" uniqueCount="1398">
   <si>
     <t>name</t>
   </si>
@@ -1964,7 +1964,7 @@
     <t>Proporcione una "imagen de héroe" de alta resolución para esta ciudad, idealmente en formato .jpg con dimensiones en la proporción de 21:10 (por ejemplo, 2100px por 1000px)</t>
   </si>
   <si>
-    <t>Resumen ejecutivo</t>
+    <t>Resumé</t>
   </si>
   <si>
     <t>แทรกโลโก้</t>
@@ -2853,6 +2853,9 @@
   </si>
   <si>
     <t>* Thresholds are based on our modelling  of built environment features requiremed to reach the World Health Organization's Global Action Plan for Physica Activity target of a 15% relative reduction in insufficient physical activity through walking.  We found preliminary evidence that street intersection density above xx and ultra-dense neighbourhoods ( &gt;15,000 persons per km²) may have decreasing benefits for physical activity.  This is an important topic for future research.</t>
+  </si>
+  <si>
+    <t>Summary</t>
   </si>
   <si>
     <t>Citation: Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {city} Healthy and Sustainable City Indicators  Report: Comparisons with 25 cities internationally. https://doi.org/INSERT-DOI-HERE</t>
@@ -4285,6 +4288,36 @@
   </si>
   <si>
     <t>Trích dẫn: Hợp tác các Chỉ số Thành phố Bền vững &amp; Khỏe mạnh Toàn cầu. 2022. {city} Báo cáo Chỉ số Thành phố Bền vững và Khỏe mạnh: So sánh với 25 thành phố trên thế giới. https://doi.org/INSERT-DOI-HERE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Resum</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 概括</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> souhrn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overzicht </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zusammenfassung</t>
+  </si>
+  <si>
+    <t>Resumen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Resumo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">சுருக்கம் </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> สรุป</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tóm lược</t>
   </si>
 </sst>
 </file>
@@ -5082,19 +5115,19 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -16640,10 +16673,10 @@
   <dimension ref="A1:AD131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D103" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A104" sqref="A104"/>
+      <selection pane="bottomRight" activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16687,7 +16720,7 @@
         <v>307</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="J1" s="18" t="s">
         <v>306</v>
@@ -16699,7 +16732,7 @@
         <v>305</v>
       </c>
       <c r="M1" s="19" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="N1" s="19" t="s">
         <v>302</v>
@@ -16711,7 +16744,7 @@
         <v>184</v>
       </c>
       <c r="Q1" s="19" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="R1" s="19" t="s">
         <v>660</v>
@@ -16770,10 +16803,10 @@
         <v>674</v>
       </c>
       <c r="H2" s="27" t="s">
+        <v>1176</v>
+      </c>
+      <c r="I2" s="27" t="s">
         <v>1175</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>1174</v>
       </c>
       <c r="J2" s="20" t="s">
         <v>658</v>
@@ -16782,14 +16815,14 @@
         <v>667</v>
       </c>
       <c r="L2" s="20" t="s">
+        <v>1173</v>
+      </c>
+      <c r="M2" s="20" t="s">
         <v>1172</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>1171</v>
       </c>
       <c r="N2" s="20"/>
       <c r="O2" s="20" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="P2" s="20" t="s">
         <v>659</v>
@@ -16841,54 +16874,54 @@
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="F3" s="22"/>
       <c r="G3" s="22" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="H3" s="23"/>
       <c r="I3" s="23" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="J3" s="22"/>
       <c r="K3" s="34" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="L3" s="34"/>
       <c r="M3" s="34" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="N3" s="22"/>
       <c r="O3" s="34" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="P3" s="22"/>
       <c r="Q3" s="22" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="R3" s="22" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="S3" s="22"/>
       <c r="T3" s="34" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="U3" s="22"/>
       <c r="V3" s="34" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="W3" s="22"/>
       <c r="X3" s="34" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="Y3" s="22"/>
       <c r="Z3" s="22" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="AA3" s="22"/>
       <c r="AB3" s="22" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="AC3" s="22"/>
       <c r="AD3" s="22"/>
@@ -16905,54 +16938,54 @@
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="22" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="22" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="H4" s="23"/>
       <c r="I4" s="23" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="J4" s="22"/>
       <c r="K4" s="34" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="L4" s="34"/>
       <c r="M4" s="34" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="N4" s="22"/>
       <c r="O4" s="34" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="P4" s="22"/>
       <c r="Q4" s="22" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="R4" s="22" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="S4" s="22"/>
       <c r="T4" s="34" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="U4" s="22"/>
       <c r="V4" s="34" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="W4" s="22"/>
       <c r="X4" s="34" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="Y4" s="22"/>
       <c r="Z4" s="22" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="AA4" s="22"/>
       <c r="AB4" s="22" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="AC4" s="22"/>
       <c r="AD4" s="22"/>
@@ -16977,7 +17010,7 @@
       </c>
       <c r="H5" s="23"/>
       <c r="I5" s="23" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="J5" s="22"/>
       <c r="K5" s="34" t="s">
@@ -16985,11 +17018,11 @@
       </c>
       <c r="L5" s="34"/>
       <c r="M5" s="34" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="N5" s="22"/>
       <c r="O5" s="34" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="P5" s="22"/>
       <c r="Q5" s="22" t="s">
@@ -17475,7 +17508,7 @@
       <c r="K17" s="34"/>
       <c r="L17" s="34"/>
       <c r="M17" s="34" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="N17" s="22"/>
       <c r="O17" s="34"/>
@@ -17551,7 +17584,7 @@
       <c r="G19" s="22"/>
       <c r="H19" s="23"/>
       <c r="I19" s="23" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="J19" s="22"/>
       <c r="K19" s="34"/>
@@ -18035,7 +18068,7 @@
       <c r="G31" s="20"/>
       <c r="H31" s="21"/>
       <c r="I31" s="21" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="J31" s="20"/>
       <c r="K31" s="34" t="s">
@@ -18043,11 +18076,11 @@
       </c>
       <c r="L31" s="34"/>
       <c r="M31" s="34" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="N31" s="20"/>
       <c r="O31" s="34" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="P31" s="20"/>
       <c r="Q31" s="22" t="s">
@@ -18099,19 +18132,19 @@
       </c>
       <c r="H32" s="21"/>
       <c r="I32" s="21" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="J32" s="20"/>
       <c r="K32" s="34" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="L32" s="34"/>
       <c r="M32" s="34" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="N32" s="20"/>
       <c r="O32" s="34" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="P32" s="20"/>
       <c r="Q32" s="22" t="s">
@@ -18163,7 +18196,7 @@
       </c>
       <c r="H33" s="21"/>
       <c r="I33" s="21" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="J33" s="20"/>
       <c r="K33" s="34" t="s">
@@ -18171,11 +18204,11 @@
       </c>
       <c r="L33" s="34"/>
       <c r="M33" s="34" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="N33" s="20"/>
       <c r="O33" s="34" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="P33" s="20"/>
       <c r="Q33" s="22" t="s">
@@ -18227,7 +18260,7 @@
       </c>
       <c r="H34" s="21"/>
       <c r="I34" s="21" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="J34" s="20"/>
       <c r="K34" s="34" t="s">
@@ -18235,11 +18268,11 @@
       </c>
       <c r="L34" s="34"/>
       <c r="M34" s="34" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="N34" s="20"/>
       <c r="O34" s="34" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="P34" s="20"/>
       <c r="Q34" s="22" t="s">
@@ -18291,7 +18324,7 @@
       </c>
       <c r="H35" s="21"/>
       <c r="I35" s="21" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="J35" s="20"/>
       <c r="K35" s="34" t="s">
@@ -18299,11 +18332,11 @@
       </c>
       <c r="L35" s="34"/>
       <c r="M35" s="34" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="N35" s="20"/>
       <c r="O35" s="34" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="P35" s="20"/>
       <c r="Q35" s="22" t="s">
@@ -18355,7 +18388,7 @@
       </c>
       <c r="H36" s="21"/>
       <c r="I36" s="21" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="J36" s="20"/>
       <c r="K36" s="34" t="s">
@@ -18363,11 +18396,11 @@
       </c>
       <c r="L36" s="34"/>
       <c r="M36" s="34" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="N36" s="20"/>
       <c r="O36" s="34" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="P36" s="20"/>
       <c r="Q36" s="22" t="s">
@@ -18419,7 +18452,7 @@
       </c>
       <c r="H37" s="21"/>
       <c r="I37" s="21" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="J37" s="20"/>
       <c r="K37" s="34" t="s">
@@ -18427,11 +18460,11 @@
       </c>
       <c r="L37" s="34"/>
       <c r="M37" s="34" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="N37" s="20"/>
       <c r="O37" s="34" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="P37" s="20"/>
       <c r="Q37" s="22" t="s">
@@ -18483,7 +18516,7 @@
       </c>
       <c r="H38" s="21"/>
       <c r="I38" s="21" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="J38" s="20"/>
       <c r="K38" s="34" t="s">
@@ -18491,11 +18524,11 @@
       </c>
       <c r="L38" s="34"/>
       <c r="M38" s="34" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="N38" s="20"/>
       <c r="O38" s="34" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="P38" s="20"/>
       <c r="Q38" s="22" t="s">
@@ -18547,7 +18580,7 @@
       </c>
       <c r="H39" s="21"/>
       <c r="I39" s="21" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="J39" s="20"/>
       <c r="K39" s="34" t="s">
@@ -18555,11 +18588,11 @@
       </c>
       <c r="L39" s="34"/>
       <c r="M39" s="34" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="N39" s="20"/>
       <c r="O39" s="34" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="P39" s="20"/>
       <c r="Q39" s="22" t="s">
@@ -18611,7 +18644,7 @@
       </c>
       <c r="H40" s="21"/>
       <c r="I40" s="21" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="J40" s="20"/>
       <c r="K40" s="34" t="s">
@@ -18619,11 +18652,11 @@
       </c>
       <c r="L40" s="34"/>
       <c r="M40" s="34" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="N40" s="20"/>
       <c r="O40" s="34" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="P40" s="20"/>
       <c r="Q40" s="22" t="s">
@@ -18675,7 +18708,7 @@
       </c>
       <c r="H41" s="21"/>
       <c r="I41" s="21" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="J41" s="20"/>
       <c r="K41" s="34" t="s">
@@ -18683,11 +18716,11 @@
       </c>
       <c r="L41" s="34"/>
       <c r="M41" s="34" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="N41" s="20"/>
       <c r="O41" s="34" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="P41" s="20"/>
       <c r="Q41" s="22" t="s">
@@ -18731,7 +18764,7 @@
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="20" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="F42" s="20"/>
       <c r="G42" s="20" t="s">
@@ -18739,19 +18772,19 @@
       </c>
       <c r="H42" s="21"/>
       <c r="I42" s="21" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="J42" s="20"/>
       <c r="K42" s="34" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="L42" s="34"/>
       <c r="M42" s="34" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="N42" s="20"/>
       <c r="O42" s="34" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="P42" s="20"/>
       <c r="Q42" s="22" t="s">
@@ -18762,11 +18795,11 @@
       </c>
       <c r="S42" s="20"/>
       <c r="T42" s="34" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="U42" s="20"/>
       <c r="V42" s="34" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="W42" s="20"/>
       <c r="X42" s="34" t="s">
@@ -18774,11 +18807,11 @@
       </c>
       <c r="Y42" s="20"/>
       <c r="Z42" s="20" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="AA42" s="20"/>
       <c r="AB42" s="20" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="AC42" s="20"/>
       <c r="AD42" s="20"/>
@@ -18795,7 +18828,7 @@
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="20" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="F43" s="20"/>
       <c r="G43" s="20" t="s">
@@ -18803,26 +18836,26 @@
       </c>
       <c r="H43" s="21"/>
       <c r="I43" s="21" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="J43" s="20"/>
       <c r="K43" s="34" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="L43" s="34"/>
       <c r="M43" s="34" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="N43" s="20"/>
       <c r="O43" s="34" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="P43" s="20"/>
       <c r="Q43" s="22" t="s">
         <v>905</v>
       </c>
       <c r="R43" s="20" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="S43" s="20"/>
       <c r="T43" s="34" t="s">
@@ -18830,19 +18863,19 @@
       </c>
       <c r="U43" s="20"/>
       <c r="V43" s="34" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="W43" s="20"/>
       <c r="X43" s="34" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="Y43" s="20"/>
       <c r="Z43" s="20" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="AA43" s="20"/>
       <c r="AB43" s="20" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="AC43" s="20"/>
       <c r="AD43" s="20"/>
@@ -18859,7 +18892,7 @@
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="20" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="F44" s="20"/>
       <c r="G44" s="20" t="s">
@@ -18867,46 +18900,46 @@
       </c>
       <c r="H44" s="21"/>
       <c r="I44" s="21" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="J44" s="20"/>
       <c r="K44" s="34" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="L44" s="34"/>
       <c r="M44" s="34" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="N44" s="20"/>
       <c r="O44" s="34" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="P44" s="20"/>
       <c r="Q44" s="22" t="s">
         <v>904</v>
       </c>
       <c r="R44" s="20" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="S44" s="20"/>
       <c r="T44" s="34" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="U44" s="20"/>
       <c r="V44" s="34" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="W44" s="20"/>
       <c r="X44" s="34" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="Y44" s="20"/>
       <c r="Z44" s="20" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="AA44" s="20"/>
       <c r="AB44" s="20" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="AC44" s="20"/>
       <c r="AD44" s="20"/>
@@ -18923,42 +18956,42 @@
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="20" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="F45" s="20"/>
       <c r="G45" s="20" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="H45" s="21"/>
       <c r="I45" s="21" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="J45" s="20"/>
       <c r="K45" s="34" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="L45" s="34"/>
       <c r="M45" s="34" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="N45" s="20"/>
       <c r="O45" s="34" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="P45" s="20"/>
       <c r="Q45" s="22" t="s">
         <v>871</v>
       </c>
       <c r="R45" s="20" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="S45" s="20"/>
       <c r="T45" s="34" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="U45" s="20"/>
       <c r="V45" s="34" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="W45" s="20"/>
       <c r="X45" s="34" t="s">
@@ -18966,11 +18999,11 @@
       </c>
       <c r="Y45" s="20"/>
       <c r="Z45" s="20" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="AA45" s="20"/>
       <c r="AB45" s="20" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="AC45" s="20"/>
       <c r="AD45" s="20"/>
@@ -18995,7 +19028,7 @@
       </c>
       <c r="H46" s="21"/>
       <c r="I46" s="21" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="J46" s="20"/>
       <c r="K46" s="34" t="s">
@@ -19003,11 +19036,11 @@
       </c>
       <c r="L46" s="34"/>
       <c r="M46" s="34" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="N46" s="20"/>
       <c r="O46" s="34" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="P46" s="20"/>
       <c r="Q46" s="22" t="s">
@@ -19051,54 +19084,54 @@
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="20" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="F47" s="20"/>
       <c r="G47" s="20" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="H47" s="21"/>
       <c r="I47" s="21" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="J47" s="20"/>
       <c r="K47" s="34" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="L47" s="34"/>
       <c r="M47" s="34" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="N47" s="20"/>
       <c r="O47" s="34" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="P47" s="20"/>
       <c r="Q47" s="22" t="s">
         <v>872</v>
       </c>
       <c r="R47" s="20" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="S47" s="20"/>
       <c r="T47" s="34" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="U47" s="20"/>
       <c r="V47" s="34" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="W47" s="20"/>
       <c r="X47" s="34" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="Y47" s="20"/>
       <c r="Z47" s="20" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="AA47" s="20"/>
       <c r="AB47" s="20" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="AC47" s="20"/>
       <c r="AD47" s="20"/>
@@ -19119,15 +19152,15 @@
       </c>
       <c r="F48" s="20"/>
       <c r="G48" s="20" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="H48" s="21"/>
       <c r="I48" s="21" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="J48" s="20"/>
       <c r="K48" s="34" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="L48" s="34"/>
       <c r="M48" s="34" t="s">
@@ -19135,32 +19168,34 @@
       </c>
       <c r="N48" s="20"/>
       <c r="O48" s="34" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="P48" s="20"/>
-      <c r="Q48" s="22"/>
+      <c r="Q48" s="20" t="s">
+        <v>1032</v>
+      </c>
       <c r="R48" s="20" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="S48" s="20"/>
       <c r="T48" s="34" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="U48" s="20"/>
       <c r="V48" s="34" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="W48" s="20"/>
       <c r="X48" s="34" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="Y48" s="20"/>
       <c r="Z48" s="20" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="AA48" s="20"/>
       <c r="AB48" s="20" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="AC48" s="20"/>
       <c r="AD48" s="20"/>
@@ -19177,54 +19212,54 @@
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="20" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="F49" s="20"/>
       <c r="G49" s="20" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="H49" s="21"/>
       <c r="I49" s="21" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="J49" s="20"/>
       <c r="K49" s="34" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="L49" s="34"/>
       <c r="M49" s="34" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="N49" s="20"/>
       <c r="O49" s="34" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="P49" s="20"/>
       <c r="Q49" s="22" t="s">
         <v>873</v>
       </c>
       <c r="R49" s="20" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="S49" s="20"/>
       <c r="T49" s="34" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="U49" s="20"/>
       <c r="V49" s="34" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="W49" s="20"/>
       <c r="X49" s="34" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="Y49" s="20"/>
       <c r="Z49" s="20" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="AA49" s="20"/>
       <c r="AB49" s="20" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="AC49" s="20"/>
       <c r="AD49" s="20"/>
@@ -19241,54 +19276,54 @@
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="20" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="F50" s="20"/>
       <c r="G50" s="20" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="H50" s="21"/>
       <c r="I50" s="21" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="J50" s="20"/>
       <c r="K50" s="34" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="L50" s="34"/>
       <c r="M50" s="34" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="N50" s="20"/>
       <c r="O50" s="34" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="P50" s="20"/>
       <c r="Q50" s="22" t="s">
         <v>874</v>
       </c>
       <c r="R50" s="20" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="S50" s="20"/>
       <c r="T50" s="34" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="U50" s="20"/>
       <c r="V50" s="34" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="W50" s="20"/>
       <c r="X50" s="34" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="Y50" s="20"/>
       <c r="Z50" s="20" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="AA50" s="20"/>
       <c r="AB50" s="20" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="AC50" s="20"/>
       <c r="AD50" s="20"/>
@@ -19313,7 +19348,7 @@
       </c>
       <c r="H51" s="21"/>
       <c r="I51" s="21" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="J51" s="20"/>
       <c r="K51" s="34" t="s">
@@ -19321,11 +19356,11 @@
       </c>
       <c r="L51" s="34"/>
       <c r="M51" s="34" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="N51" s="20"/>
       <c r="O51" s="34" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="P51" s="20"/>
       <c r="Q51" s="22" t="s">
@@ -19373,23 +19408,23 @@
       </c>
       <c r="F52" s="22"/>
       <c r="G52" s="22" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="H52" s="23"/>
       <c r="I52" s="23" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="J52" s="22"/>
       <c r="K52" s="34" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="L52" s="34"/>
       <c r="M52" s="34" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="N52" s="22"/>
       <c r="O52" s="34" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="P52" s="22"/>
       <c r="Q52" s="22" t="s">
@@ -19400,7 +19435,7 @@
       </c>
       <c r="S52" s="22"/>
       <c r="T52" s="34" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="U52" s="22"/>
       <c r="V52" s="34" t="s">
@@ -19408,11 +19443,11 @@
       </c>
       <c r="W52" s="22"/>
       <c r="X52" s="34" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="Y52" s="22"/>
       <c r="Z52" s="22" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="AA52" s="22"/>
       <c r="AB52" s="22" t="s">
@@ -19437,23 +19472,23 @@
       </c>
       <c r="F53" s="22"/>
       <c r="G53" s="22" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="H53" s="23"/>
       <c r="I53" s="23" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="J53" s="22"/>
       <c r="K53" s="34" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="L53" s="34"/>
       <c r="M53" s="34" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="N53" s="22"/>
       <c r="O53" s="34" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="P53" s="22"/>
       <c r="Q53" s="22" t="s">
@@ -19468,7 +19503,7 @@
       </c>
       <c r="U53" s="22"/>
       <c r="V53" s="34" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="W53" s="22"/>
       <c r="X53" s="34" t="s">
@@ -19476,7 +19511,7 @@
       </c>
       <c r="Y53" s="22"/>
       <c r="Z53" s="22" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="AA53" s="22"/>
       <c r="AB53" s="22" t="s">
@@ -19505,7 +19540,7 @@
       </c>
       <c r="H54" s="23"/>
       <c r="I54" s="23" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="J54" s="22"/>
       <c r="K54" s="34" t="s">
@@ -19513,11 +19548,11 @@
       </c>
       <c r="L54" s="34"/>
       <c r="M54" s="34" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="N54" s="22"/>
       <c r="O54" s="34" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="P54" s="22"/>
       <c r="Q54" s="22" t="s">
@@ -19569,7 +19604,7 @@
       </c>
       <c r="H55" s="23"/>
       <c r="I55" s="23" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="J55" s="22"/>
       <c r="K55" s="34" t="s">
@@ -19577,11 +19612,11 @@
       </c>
       <c r="L55" s="34"/>
       <c r="M55" s="34" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="N55" s="22"/>
       <c r="O55" s="34" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="P55" s="22"/>
       <c r="Q55" s="22" t="s">
@@ -19625,54 +19660,54 @@
       </c>
       <c r="D56" s="22"/>
       <c r="E56" s="22" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="F56" s="22"/>
       <c r="G56" s="22" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="H56" s="23"/>
       <c r="I56" s="23" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="J56" s="22"/>
       <c r="K56" s="34" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="L56" s="34"/>
       <c r="M56" s="34" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="N56" s="22"/>
       <c r="O56" s="34" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="P56" s="22"/>
       <c r="Q56" s="22" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="R56" s="22" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="S56" s="22"/>
       <c r="T56" s="34" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="U56" s="22"/>
       <c r="V56" s="34" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="W56" s="22"/>
       <c r="X56" s="34" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="Y56" s="22"/>
       <c r="Z56" s="22" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="AA56" s="22"/>
       <c r="AB56" s="22" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="AC56" s="22"/>
       <c r="AD56" s="22"/>
@@ -19689,54 +19724,54 @@
       </c>
       <c r="D57" s="22"/>
       <c r="E57" s="22" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="F57" s="22"/>
       <c r="G57" s="22" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="H57" s="23"/>
       <c r="I57" s="23" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="J57" s="22"/>
       <c r="K57" s="34" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="L57" s="34"/>
       <c r="M57" s="34" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="N57" s="22"/>
       <c r="O57" s="34" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="P57" s="22"/>
       <c r="Q57" s="22" t="s">
         <v>899</v>
       </c>
       <c r="R57" s="22" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="S57" s="22"/>
       <c r="T57" s="34" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="U57" s="22"/>
       <c r="V57" s="34" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="W57" s="22"/>
       <c r="X57" s="34" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="Y57" s="22"/>
       <c r="Z57" s="22" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="AA57" s="22"/>
       <c r="AB57" s="22" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="AC57" s="22"/>
       <c r="AD57" s="22"/>
@@ -19753,54 +19788,54 @@
       </c>
       <c r="D58" s="22"/>
       <c r="E58" s="22" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="F58" s="22"/>
       <c r="G58" s="22" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="H58" s="23"/>
       <c r="I58" s="23" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="J58" s="22"/>
       <c r="K58" s="34" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="L58" s="34"/>
       <c r="M58" s="34" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="N58" s="22"/>
       <c r="O58" s="34" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="P58" s="22"/>
       <c r="Q58" s="22" t="s">
         <v>900</v>
       </c>
       <c r="R58" s="22" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="S58" s="22"/>
       <c r="T58" s="34" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="U58" s="22"/>
       <c r="V58" s="34" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="W58" s="22"/>
       <c r="X58" s="34" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="Y58" s="22"/>
       <c r="Z58" s="22" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="AA58" s="22"/>
       <c r="AB58" s="22" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="AC58" s="22"/>
       <c r="AD58" s="22"/>
@@ -19817,42 +19852,42 @@
       </c>
       <c r="D59" s="22"/>
       <c r="E59" s="22" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="F59" s="22"/>
       <c r="G59" s="22" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="H59" s="23"/>
       <c r="I59" s="23" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="J59" s="22"/>
       <c r="K59" s="34" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="L59" s="34"/>
       <c r="M59" s="34" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="N59" s="22"/>
       <c r="O59" s="34" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="P59" s="22"/>
       <c r="Q59" s="22" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="R59" s="22" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="S59" s="22"/>
       <c r="T59" s="34" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="U59" s="22"/>
       <c r="V59" s="34" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="W59" s="22"/>
       <c r="X59" s="34" t="s">
@@ -19860,11 +19895,11 @@
       </c>
       <c r="Y59" s="22"/>
       <c r="Z59" s="22" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="AA59" s="22"/>
       <c r="AB59" s="22" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="AC59" s="22"/>
       <c r="AD59" s="22"/>
@@ -19889,7 +19924,7 @@
       </c>
       <c r="H60" s="23"/>
       <c r="I60" s="23" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="J60" s="22"/>
       <c r="K60" s="34" t="s">
@@ -19897,11 +19932,11 @@
       </c>
       <c r="L60" s="34"/>
       <c r="M60" s="34" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="N60" s="22"/>
       <c r="O60" s="34" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="P60" s="22"/>
       <c r="Q60" s="22" t="s">
@@ -19953,7 +19988,7 @@
       </c>
       <c r="H61" s="23"/>
       <c r="I61" s="23" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="J61" s="22"/>
       <c r="K61" s="34" t="s">
@@ -19961,11 +19996,11 @@
       </c>
       <c r="L61" s="34"/>
       <c r="M61" s="34" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="N61" s="22"/>
       <c r="O61" s="34" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="P61" s="22"/>
       <c r="Q61" s="22" t="s">
@@ -20009,54 +20044,54 @@
       </c>
       <c r="D62" s="22"/>
       <c r="E62" s="22" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="F62" s="22"/>
       <c r="G62" s="22" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="H62" s="23"/>
       <c r="I62" s="23" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="J62" s="22"/>
       <c r="K62" s="34" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="L62" s="34"/>
       <c r="M62" s="34" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="N62" s="22"/>
       <c r="O62" s="34" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="P62" s="22"/>
       <c r="Q62" s="22" t="s">
         <v>880</v>
       </c>
       <c r="R62" s="22" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="S62" s="22"/>
       <c r="T62" s="34" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="U62" s="22"/>
       <c r="V62" s="34" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="W62" s="22"/>
       <c r="X62" s="34" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="Y62" s="22"/>
       <c r="Z62" s="22" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="AA62" s="22"/>
       <c r="AB62" s="22" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="AC62" s="22"/>
       <c r="AD62" s="22"/>
@@ -20073,54 +20108,54 @@
       </c>
       <c r="D63" s="22"/>
       <c r="E63" s="22" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="F63" s="22"/>
       <c r="G63" s="22" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="H63" s="23"/>
       <c r="I63" s="23" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="J63" s="22"/>
       <c r="K63" s="34" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="L63" s="34"/>
       <c r="M63" s="34" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="N63" s="22"/>
       <c r="O63" s="34" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="P63" s="22"/>
       <c r="Q63" s="22" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="R63" s="22" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="S63" s="22"/>
       <c r="T63" s="34" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="U63" s="22"/>
       <c r="V63" s="34" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="W63" s="22"/>
       <c r="X63" s="34" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="Y63" s="22"/>
       <c r="Z63" s="22" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="AA63" s="22"/>
       <c r="AB63" s="22" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="AC63" s="22"/>
       <c r="AD63" s="22"/>
@@ -20145,7 +20180,7 @@
       </c>
       <c r="H64" s="23"/>
       <c r="I64" s="23" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="J64" s="22"/>
       <c r="K64" s="34" t="s">
@@ -20153,11 +20188,11 @@
       </c>
       <c r="L64" s="34"/>
       <c r="M64" s="34" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="N64" s="22"/>
       <c r="O64" s="34" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="P64" s="22"/>
       <c r="Q64" s="22" t="s">
@@ -20201,54 +20236,54 @@
       </c>
       <c r="D65" s="22"/>
       <c r="E65" s="22" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="F65" s="22"/>
       <c r="G65" s="22" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="H65" s="23"/>
       <c r="I65" s="23" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="J65" s="22"/>
       <c r="K65" s="34" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="L65" s="34"/>
       <c r="M65" s="34" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="N65" s="22"/>
       <c r="O65" s="34" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="P65" s="22"/>
       <c r="Q65" s="22" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="R65" s="22" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="S65" s="22"/>
       <c r="T65" s="34" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="U65" s="22"/>
       <c r="V65" s="34" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="W65" s="22"/>
       <c r="X65" s="34" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="Y65" s="22"/>
       <c r="Z65" s="22" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="AA65" s="22"/>
       <c r="AB65" s="22" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="AC65" s="22"/>
       <c r="AD65" s="22"/>
@@ -20273,7 +20308,7 @@
       </c>
       <c r="H66" s="23"/>
       <c r="I66" s="23" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="J66" s="22"/>
       <c r="K66" s="34" t="s">
@@ -20281,11 +20316,11 @@
       </c>
       <c r="L66" s="34"/>
       <c r="M66" s="34" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="N66" s="22"/>
       <c r="O66" s="34" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="P66" s="22"/>
       <c r="Q66" s="22" t="s">
@@ -20337,7 +20372,7 @@
       </c>
       <c r="H67" s="23"/>
       <c r="I67" s="23" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="J67" s="22"/>
       <c r="K67" s="34" t="s">
@@ -20345,11 +20380,11 @@
       </c>
       <c r="L67" s="34"/>
       <c r="M67" s="34" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="N67" s="22"/>
       <c r="O67" s="34" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="P67" s="22"/>
       <c r="Q67" s="22" t="s">
@@ -20393,54 +20428,54 @@
       </c>
       <c r="D68" s="22"/>
       <c r="E68" s="22" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="F68" s="22"/>
       <c r="G68" s="22" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="H68" s="23"/>
       <c r="I68" s="23" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="J68" s="22"/>
       <c r="K68" s="34" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="L68" s="34"/>
       <c r="M68" s="34" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="N68" s="22"/>
       <c r="O68" s="34" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="P68" s="22"/>
       <c r="Q68" s="22" t="s">
         <v>884</v>
       </c>
       <c r="R68" s="22" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="S68" s="22"/>
       <c r="T68" s="34" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="U68" s="22"/>
       <c r="V68" s="34" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="W68" s="22"/>
       <c r="X68" s="34" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="Y68" s="22"/>
       <c r="Z68" s="22" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="AA68" s="22"/>
       <c r="AB68" s="22" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="AC68" s="22"/>
       <c r="AD68" s="22"/>
@@ -20465,7 +20500,7 @@
       </c>
       <c r="H69" s="23"/>
       <c r="I69" s="23" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="J69" s="22"/>
       <c r="K69" s="34" t="s">
@@ -20473,11 +20508,11 @@
       </c>
       <c r="L69" s="34"/>
       <c r="M69" s="34" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="N69" s="22"/>
       <c r="O69" s="34" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="P69" s="22"/>
       <c r="Q69" s="22" t="s">
@@ -20529,7 +20564,7 @@
       </c>
       <c r="H70" s="23"/>
       <c r="I70" s="23" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="J70" s="22"/>
       <c r="K70" s="34" t="s">
@@ -20537,11 +20572,11 @@
       </c>
       <c r="L70" s="34"/>
       <c r="M70" s="34" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="N70" s="22"/>
       <c r="O70" s="34" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="P70" s="22"/>
       <c r="Q70" s="22" t="s">
@@ -20593,7 +20628,7 @@
       </c>
       <c r="H71" s="23"/>
       <c r="I71" s="23" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="J71" s="22"/>
       <c r="K71" s="34" t="s">
@@ -20601,11 +20636,11 @@
       </c>
       <c r="L71" s="34"/>
       <c r="M71" s="34" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="N71" s="22"/>
       <c r="O71" s="34" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="P71" s="22"/>
       <c r="Q71" s="22" t="s">
@@ -20657,7 +20692,7 @@
       </c>
       <c r="H72" s="23"/>
       <c r="I72" s="23" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="J72" s="22"/>
       <c r="K72" s="34" t="s">
@@ -20665,11 +20700,11 @@
       </c>
       <c r="L72" s="34"/>
       <c r="M72" s="34" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="N72" s="22"/>
       <c r="O72" s="34" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="P72" s="22"/>
       <c r="Q72" s="22" t="s">
@@ -20721,7 +20756,7 @@
       </c>
       <c r="H73" s="23"/>
       <c r="I73" s="23" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="J73" s="22"/>
       <c r="K73" s="34" t="s">
@@ -20729,11 +20764,11 @@
       </c>
       <c r="L73" s="34"/>
       <c r="M73" s="34" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="N73" s="22"/>
       <c r="O73" s="34" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="P73" s="22"/>
       <c r="Q73" s="22" t="s">
@@ -20785,7 +20820,7 @@
       </c>
       <c r="H74" s="23"/>
       <c r="I74" s="23" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="J74" s="22"/>
       <c r="K74" s="34" t="s">
@@ -20793,11 +20828,11 @@
       </c>
       <c r="L74" s="34"/>
       <c r="M74" s="34" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="N74" s="22"/>
       <c r="O74" s="34" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="P74" s="22"/>
       <c r="Q74" s="22" t="s">
@@ -20849,7 +20884,7 @@
       </c>
       <c r="H75" s="23"/>
       <c r="I75" s="23" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="J75" s="22"/>
       <c r="K75" s="34" t="s">
@@ -20857,11 +20892,11 @@
       </c>
       <c r="L75" s="34"/>
       <c r="M75" s="34" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="N75" s="22"/>
       <c r="O75" s="34" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="P75" s="22"/>
       <c r="Q75" s="22" t="s">
@@ -20913,7 +20948,7 @@
       </c>
       <c r="H76" s="23"/>
       <c r="I76" s="23" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="J76" s="22"/>
       <c r="K76" s="34" t="s">
@@ -20921,11 +20956,11 @@
       </c>
       <c r="L76" s="34"/>
       <c r="M76" s="34" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="N76" s="22"/>
       <c r="O76" s="34" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="P76" s="22"/>
       <c r="Q76" s="22" t="s">
@@ -20965,58 +21000,58 @@
         <v>87</v>
       </c>
       <c r="C77" s="24" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="D77" s="22"/>
       <c r="E77" s="22" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="F77" s="22"/>
       <c r="G77" s="22" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="H77" s="24"/>
       <c r="I77" s="24" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="J77" s="25"/>
       <c r="K77" s="34" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="L77" s="34"/>
       <c r="M77" s="34" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="N77" s="25"/>
       <c r="O77" s="34" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="P77" s="22"/>
       <c r="Q77" s="25" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="R77" s="22" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="S77" s="22"/>
       <c r="T77" s="34" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="U77" s="22"/>
       <c r="V77" s="34" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="W77" s="22"/>
       <c r="X77" s="34" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="Y77" s="22"/>
       <c r="Z77" s="22" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="AA77" s="22"/>
       <c r="AB77" s="22" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="AC77" s="22"/>
       <c r="AD77" s="22"/>
@@ -21033,42 +21068,42 @@
       </c>
       <c r="D78" s="22"/>
       <c r="E78" s="22" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="F78" s="22"/>
       <c r="G78" s="22" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="H78" s="23"/>
       <c r="I78" s="23" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="J78" s="22"/>
       <c r="K78" s="34" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="L78" s="34"/>
       <c r="M78" s="34" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="N78" s="22"/>
       <c r="O78" s="34" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="P78" s="22"/>
       <c r="Q78" s="22" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="R78" s="22" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="S78" s="22"/>
       <c r="T78" s="34" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="U78" s="22"/>
       <c r="V78" s="34" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="W78" s="22"/>
       <c r="X78" s="34" t="s">
@@ -21076,11 +21111,11 @@
       </c>
       <c r="Y78" s="22"/>
       <c r="Z78" s="22" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="AA78" s="22"/>
       <c r="AB78" s="22" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="AC78" s="22"/>
       <c r="AD78" s="22"/>
@@ -21097,42 +21132,42 @@
       </c>
       <c r="D79" s="22"/>
       <c r="E79" s="22" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="F79" s="22"/>
       <c r="G79" s="22" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="H79" s="23"/>
       <c r="I79" s="23" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="J79" s="22"/>
       <c r="K79" s="34" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="L79" s="34"/>
       <c r="M79" s="34" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="N79" s="22"/>
       <c r="O79" s="34" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="P79" s="22"/>
       <c r="Q79" s="22" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="R79" s="22" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="S79" s="22"/>
       <c r="T79" s="34" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="U79" s="22"/>
       <c r="V79" s="34" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="W79" s="22"/>
       <c r="X79" s="34" t="s">
@@ -21140,11 +21175,11 @@
       </c>
       <c r="Y79" s="22"/>
       <c r="Z79" s="22" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="AA79" s="22"/>
       <c r="AB79" s="22" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="AC79" s="22"/>
       <c r="AD79" s="22"/>
@@ -21161,42 +21196,42 @@
       </c>
       <c r="D80" s="22"/>
       <c r="E80" s="22" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="F80" s="22"/>
       <c r="G80" s="22" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="H80" s="23"/>
       <c r="I80" s="23" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="J80" s="22"/>
       <c r="K80" s="34" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="L80" s="34"/>
       <c r="M80" s="34" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="N80" s="22"/>
       <c r="O80" s="34" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="P80" s="22"/>
       <c r="Q80" s="22" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="R80" s="22" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="S80" s="22"/>
       <c r="T80" s="34" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="U80" s="22"/>
       <c r="V80" s="34" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="W80" s="22"/>
       <c r="X80" s="34" t="s">
@@ -21204,11 +21239,11 @@
       </c>
       <c r="Y80" s="22"/>
       <c r="Z80" s="22" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="AA80" s="22"/>
       <c r="AB80" s="22" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="AC80" s="22"/>
       <c r="AD80" s="22"/>
@@ -21233,7 +21268,7 @@
       </c>
       <c r="H81" s="23"/>
       <c r="I81" s="23" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="J81" s="22"/>
       <c r="K81" s="34" t="s">
@@ -21241,11 +21276,11 @@
       </c>
       <c r="L81" s="34"/>
       <c r="M81" s="34" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="N81" s="22"/>
       <c r="O81" s="34" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="P81" s="22"/>
       <c r="Q81" s="22" t="s">
@@ -21297,7 +21332,7 @@
       </c>
       <c r="H82" s="23"/>
       <c r="I82" s="23" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="J82" s="22"/>
       <c r="K82" s="34" t="s">
@@ -21305,11 +21340,11 @@
       </c>
       <c r="L82" s="34"/>
       <c r="M82" s="34" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="N82" s="22"/>
       <c r="O82" s="34" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="P82" s="22"/>
       <c r="Q82" s="22" t="s">
@@ -21361,7 +21396,7 @@
       </c>
       <c r="H83" s="23"/>
       <c r="I83" s="23" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="J83" s="22"/>
       <c r="K83" s="34" t="s">
@@ -21369,11 +21404,11 @@
       </c>
       <c r="L83" s="34"/>
       <c r="M83" s="34" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="N83" s="22"/>
       <c r="O83" s="34" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="P83" s="22"/>
       <c r="Q83" s="22" t="s">
@@ -21425,7 +21460,7 @@
       </c>
       <c r="H84" s="23"/>
       <c r="I84" s="23" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="J84" s="22"/>
       <c r="K84" s="34" t="s">
@@ -21433,11 +21468,11 @@
       </c>
       <c r="L84" s="34"/>
       <c r="M84" s="34" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="N84" s="22"/>
       <c r="O84" s="34" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="P84" s="22"/>
       <c r="Q84" s="22" t="s">
@@ -21489,7 +21524,7 @@
       </c>
       <c r="H85" s="23"/>
       <c r="I85" s="23" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="J85" s="22"/>
       <c r="K85" s="34" t="s">
@@ -21497,11 +21532,11 @@
       </c>
       <c r="L85" s="34"/>
       <c r="M85" s="34" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="N85" s="22"/>
       <c r="O85" s="34" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="P85" s="22"/>
       <c r="Q85" s="22" t="s">
@@ -21553,7 +21588,7 @@
       </c>
       <c r="H86" s="23"/>
       <c r="I86" s="23" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="J86" s="22"/>
       <c r="K86" s="34" t="s">
@@ -21561,11 +21596,11 @@
       </c>
       <c r="L86" s="34"/>
       <c r="M86" s="34" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="N86" s="22"/>
       <c r="O86" s="34" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="P86" s="22"/>
       <c r="Q86" s="22" t="s">
@@ -21617,7 +21652,7 @@
       </c>
       <c r="H87" s="23"/>
       <c r="I87" s="23" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="J87" s="22"/>
       <c r="K87" s="34" t="s">
@@ -21625,11 +21660,11 @@
       </c>
       <c r="L87" s="34"/>
       <c r="M87" s="34" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="N87" s="22"/>
       <c r="O87" s="34" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="P87" s="22"/>
       <c r="Q87" s="22" t="s">
@@ -21681,7 +21716,7 @@
       </c>
       <c r="H88" s="23"/>
       <c r="I88" s="23" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="J88" s="22"/>
       <c r="K88" s="34" t="s">
@@ -21689,11 +21724,11 @@
       </c>
       <c r="L88" s="34"/>
       <c r="M88" s="34" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="N88" s="22"/>
       <c r="O88" s="34" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="P88" s="22"/>
       <c r="Q88" s="22" t="s">
@@ -21745,7 +21780,7 @@
       </c>
       <c r="H89" s="23"/>
       <c r="I89" s="23" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="J89" s="22"/>
       <c r="K89" s="34" t="s">
@@ -21753,11 +21788,11 @@
       </c>
       <c r="L89" s="34"/>
       <c r="M89" s="34" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="N89" s="22"/>
       <c r="O89" s="34" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="P89" s="22"/>
       <c r="Q89" s="22" t="s">
@@ -21809,7 +21844,7 @@
       </c>
       <c r="H90" s="23"/>
       <c r="I90" s="23" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="J90" s="22"/>
       <c r="K90" s="34" t="s">
@@ -21817,11 +21852,11 @@
       </c>
       <c r="L90" s="34"/>
       <c r="M90" s="34" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="N90" s="22"/>
       <c r="O90" s="34" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="P90" s="22"/>
       <c r="Q90" s="22" t="s">
@@ -21873,7 +21908,7 @@
       </c>
       <c r="H91" s="23"/>
       <c r="I91" s="23" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="J91" s="22"/>
       <c r="K91" s="34" t="s">
@@ -21881,11 +21916,11 @@
       </c>
       <c r="L91" s="34"/>
       <c r="M91" s="34" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="N91" s="22"/>
       <c r="O91" s="34" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="P91" s="22"/>
       <c r="Q91" s="22" t="s">
@@ -21937,7 +21972,7 @@
       </c>
       <c r="H92" s="23"/>
       <c r="I92" s="23" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="J92" s="22"/>
       <c r="K92" s="34" t="s">
@@ -21945,11 +21980,11 @@
       </c>
       <c r="L92" s="34"/>
       <c r="M92" s="34" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="N92" s="22"/>
       <c r="O92" s="34" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="P92" s="22"/>
       <c r="Q92" s="22" t="s">
@@ -22001,7 +22036,7 @@
       </c>
       <c r="H93" s="23"/>
       <c r="I93" s="23" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="J93" s="22"/>
       <c r="K93" s="34" t="s">
@@ -22009,11 +22044,11 @@
       </c>
       <c r="L93" s="34"/>
       <c r="M93" s="34" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="N93" s="22"/>
       <c r="O93" s="34" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="P93" s="22"/>
       <c r="Q93" s="22" t="s">
@@ -22065,7 +22100,7 @@
       </c>
       <c r="H94" s="23"/>
       <c r="I94" s="23" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="J94" s="22"/>
       <c r="K94" s="34" t="s">
@@ -22073,11 +22108,11 @@
       </c>
       <c r="L94" s="34"/>
       <c r="M94" s="34" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="N94" s="22"/>
       <c r="O94" s="34" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="P94" s="22"/>
       <c r="Q94" s="22" t="s">
@@ -22129,7 +22164,7 @@
       </c>
       <c r="H95" s="23"/>
       <c r="I95" s="23" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="J95" s="22"/>
       <c r="K95" s="34" t="s">
@@ -22137,11 +22172,11 @@
       </c>
       <c r="L95" s="34"/>
       <c r="M95" s="34" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="N95" s="22"/>
       <c r="O95" s="34" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="P95" s="22"/>
       <c r="Q95" s="22" t="s">
@@ -22193,7 +22228,7 @@
       </c>
       <c r="H96" s="24"/>
       <c r="I96" s="24" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="J96" s="25"/>
       <c r="K96" s="34" t="s">
@@ -22201,11 +22236,11 @@
       </c>
       <c r="L96" s="34"/>
       <c r="M96" s="34" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="N96" s="25"/>
       <c r="O96" s="34" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="P96" s="22"/>
       <c r="Q96" s="25" t="s">
@@ -22257,7 +22292,7 @@
       </c>
       <c r="H97" s="23"/>
       <c r="I97" s="23" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="J97" s="22"/>
       <c r="K97" s="34" t="s">
@@ -22265,11 +22300,11 @@
       </c>
       <c r="L97" s="34"/>
       <c r="M97" s="34" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="N97" s="22"/>
       <c r="O97" s="34" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="P97" s="22"/>
       <c r="Q97" s="22" t="s">
@@ -22321,7 +22356,7 @@
       </c>
       <c r="H98" s="23"/>
       <c r="I98" s="23" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="J98" s="22"/>
       <c r="K98" s="34" t="s">
@@ -22329,11 +22364,11 @@
       </c>
       <c r="L98" s="34"/>
       <c r="M98" s="34" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="N98" s="22"/>
       <c r="O98" s="34" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="P98" s="22"/>
       <c r="Q98" s="22" t="s">
@@ -22385,7 +22420,7 @@
       </c>
       <c r="H99" s="23"/>
       <c r="I99" s="23" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="J99" s="22"/>
       <c r="K99" s="34" t="s">
@@ -22393,11 +22428,11 @@
       </c>
       <c r="L99" s="34"/>
       <c r="M99" s="34" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="N99" s="22"/>
       <c r="O99" s="34" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="P99" s="22"/>
       <c r="Q99" s="22" t="s">
@@ -22449,7 +22484,7 @@
       </c>
       <c r="H100" s="23"/>
       <c r="I100" s="23" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="J100" s="22"/>
       <c r="K100" s="34" t="s">
@@ -22457,11 +22492,11 @@
       </c>
       <c r="L100" s="34"/>
       <c r="M100" s="34" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="N100" s="22"/>
       <c r="O100" s="34" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="P100" s="22"/>
       <c r="Q100" s="22" t="s">
@@ -22513,7 +22548,7 @@
       </c>
       <c r="H101" s="24"/>
       <c r="I101" s="24" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="J101" s="25"/>
       <c r="K101" s="34" t="s">
@@ -22521,11 +22556,11 @@
       </c>
       <c r="L101" s="34"/>
       <c r="M101" s="34" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="N101" s="25"/>
       <c r="O101" s="34" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="P101" s="22"/>
       <c r="Q101" s="25" t="s">
@@ -22577,7 +22612,7 @@
       </c>
       <c r="H102" s="23"/>
       <c r="I102" s="23" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="J102" s="22"/>
       <c r="K102" s="34" t="s">
@@ -22585,11 +22620,11 @@
       </c>
       <c r="L102" s="34"/>
       <c r="M102" s="34" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="N102" s="22"/>
       <c r="O102" s="34" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="P102" s="22"/>
       <c r="Q102" s="22" t="s">
@@ -22641,7 +22676,7 @@
       </c>
       <c r="H103" s="23"/>
       <c r="I103" s="23" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="J103" s="22"/>
       <c r="K103" s="34" t="s">
@@ -22649,11 +22684,11 @@
       </c>
       <c r="L103" s="34"/>
       <c r="M103" s="34" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="N103" s="22"/>
       <c r="O103" s="34" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="P103" s="22"/>
       <c r="Q103" s="22" t="s">
@@ -22676,7 +22711,7 @@
       </c>
       <c r="Y103" s="22"/>
       <c r="Z103" s="22" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="AA103" s="22"/>
       <c r="AB103" s="22" t="s">
@@ -22693,58 +22728,58 @@
         <v>179</v>
       </c>
       <c r="C104" s="23" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="D104" s="22"/>
       <c r="E104" s="22" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="F104" s="22"/>
       <c r="G104" s="22" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="H104" s="23"/>
       <c r="I104" s="23" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="J104" s="22"/>
       <c r="K104" s="34" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="L104" s="34"/>
       <c r="M104" s="34" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="N104" s="22"/>
       <c r="O104" s="34" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="P104" s="22"/>
       <c r="Q104" s="22" t="s">
         <v>898</v>
       </c>
       <c r="R104" s="22" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="S104" s="22"/>
       <c r="T104" s="34" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="U104" s="22"/>
       <c r="V104" s="34" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="W104" s="22"/>
       <c r="X104" s="34" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="Y104" s="22"/>
       <c r="Z104" s="22" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="AA104" s="22"/>
       <c r="AB104" s="22" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="AC104" s="22"/>
       <c r="AD104" s="22"/>
@@ -22757,58 +22792,58 @@
         <v>391</v>
       </c>
       <c r="C105" s="23" t="s">
-        <v>325</v>
+        <v>934</v>
       </c>
       <c r="D105" s="22"/>
       <c r="E105" s="22" t="s">
-        <v>325</v>
+        <v>1388</v>
       </c>
       <c r="F105" s="22"/>
       <c r="G105" s="22" t="s">
-        <v>325</v>
+        <v>1389</v>
       </c>
       <c r="H105" s="23"/>
       <c r="I105" s="23" t="s">
-        <v>325</v>
+        <v>1390</v>
       </c>
       <c r="J105" s="22"/>
       <c r="K105" s="35" t="s">
-        <v>325</v>
+        <v>639</v>
       </c>
       <c r="L105" s="35"/>
       <c r="M105" s="35" t="s">
-        <v>325</v>
+        <v>1391</v>
       </c>
       <c r="N105" s="22"/>
       <c r="O105" s="35" t="s">
-        <v>325</v>
+        <v>1392</v>
       </c>
       <c r="P105" s="22"/>
       <c r="Q105" s="22" t="s">
-        <v>639</v>
+        <v>1393</v>
       </c>
       <c r="R105" s="22" t="s">
-        <v>325</v>
+        <v>1393</v>
       </c>
       <c r="S105" s="22"/>
       <c r="T105" s="35" t="s">
-        <v>325</v>
+        <v>1394</v>
       </c>
       <c r="U105" s="22"/>
       <c r="V105" s="35" t="s">
-        <v>325</v>
+        <v>1394</v>
       </c>
       <c r="W105" s="22"/>
       <c r="X105" s="35" t="s">
-        <v>325</v>
+        <v>1395</v>
       </c>
       <c r="Y105" s="22"/>
       <c r="Z105" s="22" t="s">
-        <v>325</v>
+        <v>1396</v>
       </c>
       <c r="AA105" s="22"/>
       <c r="AB105" s="22" t="s">
-        <v>325</v>
+        <v>1397</v>
       </c>
       <c r="AC105" s="22"/>
       <c r="AD105" s="22"/>
@@ -22833,7 +22868,7 @@
       </c>
       <c r="H106" s="23"/>
       <c r="I106" s="23" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="J106" s="22"/>
       <c r="K106" s="34" t="s">
@@ -22841,11 +22876,11 @@
       </c>
       <c r="L106" s="34"/>
       <c r="M106" s="34" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="N106" s="22"/>
       <c r="O106" s="34" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="P106" s="22"/>
       <c r="Q106" s="22" t="s">
@@ -22898,7 +22933,7 @@
       </c>
       <c r="H107" s="23"/>
       <c r="I107" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J107" s="22"/>
       <c r="K107" s="34" t="s">
@@ -22906,11 +22941,11 @@
       </c>
       <c r="L107" s="34"/>
       <c r="M107" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N107" s="22"/>
       <c r="O107" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P107" s="22"/>
       <c r="Q107" s="22" t="s">
@@ -22963,7 +22998,7 @@
       </c>
       <c r="H108" s="23"/>
       <c r="I108" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J108" s="22"/>
       <c r="K108" s="34" t="s">
@@ -22971,11 +23006,11 @@
       </c>
       <c r="L108" s="34"/>
       <c r="M108" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N108" s="22"/>
       <c r="O108" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P108" s="22"/>
       <c r="Q108" s="22" t="s">
@@ -23028,7 +23063,7 @@
       </c>
       <c r="H109" s="23"/>
       <c r="I109" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J109" s="22"/>
       <c r="K109" s="34" t="s">
@@ -23036,11 +23071,11 @@
       </c>
       <c r="L109" s="34"/>
       <c r="M109" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N109" s="22"/>
       <c r="O109" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P109" s="22"/>
       <c r="Q109" s="22" t="s">
@@ -23093,7 +23128,7 @@
       </c>
       <c r="H110" s="23"/>
       <c r="I110" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J110" s="22"/>
       <c r="K110" s="34" t="s">
@@ -23101,11 +23136,11 @@
       </c>
       <c r="L110" s="34"/>
       <c r="M110" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N110" s="22"/>
       <c r="O110" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P110" s="22"/>
       <c r="Q110" s="22" t="s">
@@ -23158,7 +23193,7 @@
       </c>
       <c r="H111" s="23"/>
       <c r="I111" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J111" s="22"/>
       <c r="K111" s="34" t="s">
@@ -23166,11 +23201,11 @@
       </c>
       <c r="L111" s="34"/>
       <c r="M111" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N111" s="22"/>
       <c r="O111" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P111" s="22"/>
       <c r="Q111" s="22" t="s">
@@ -23223,7 +23258,7 @@
       </c>
       <c r="H112" s="23"/>
       <c r="I112" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J112" s="22"/>
       <c r="K112" s="34" t="s">
@@ -23231,11 +23266,11 @@
       </c>
       <c r="L112" s="34"/>
       <c r="M112" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N112" s="22"/>
       <c r="O112" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P112" s="22"/>
       <c r="Q112" s="22" t="s">
@@ -23288,7 +23323,7 @@
       </c>
       <c r="H113" s="23"/>
       <c r="I113" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J113" s="22"/>
       <c r="K113" s="34" t="s">
@@ -23296,11 +23331,11 @@
       </c>
       <c r="L113" s="34"/>
       <c r="M113" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N113" s="22"/>
       <c r="O113" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P113" s="22"/>
       <c r="Q113" s="22" t="s">
@@ -23353,7 +23388,7 @@
       </c>
       <c r="H114" s="23"/>
       <c r="I114" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J114" s="22"/>
       <c r="K114" s="34" t="s">
@@ -23361,11 +23396,11 @@
       </c>
       <c r="L114" s="34"/>
       <c r="M114" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N114" s="22"/>
       <c r="O114" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P114" s="22"/>
       <c r="Q114" s="22" t="s">
@@ -23418,7 +23453,7 @@
       </c>
       <c r="H115" s="23"/>
       <c r="I115" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J115" s="22"/>
       <c r="K115" s="34" t="s">
@@ -23426,11 +23461,11 @@
       </c>
       <c r="L115" s="34"/>
       <c r="M115" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N115" s="22"/>
       <c r="O115" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P115" s="22"/>
       <c r="Q115" s="22" t="s">
@@ -23483,7 +23518,7 @@
       </c>
       <c r="H116" s="23"/>
       <c r="I116" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J116" s="22"/>
       <c r="K116" s="34" t="s">
@@ -23491,11 +23526,11 @@
       </c>
       <c r="L116" s="34"/>
       <c r="M116" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N116" s="22"/>
       <c r="O116" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P116" s="22"/>
       <c r="Q116" s="22" t="s">
@@ -23548,7 +23583,7 @@
       </c>
       <c r="H117" s="23"/>
       <c r="I117" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J117" s="22"/>
       <c r="K117" s="34" t="s">
@@ -23556,11 +23591,11 @@
       </c>
       <c r="L117" s="34"/>
       <c r="M117" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N117" s="22"/>
       <c r="O117" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P117" s="22"/>
       <c r="Q117" s="22" t="s">
@@ -23613,7 +23648,7 @@
       </c>
       <c r="H118" s="23"/>
       <c r="I118" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J118" s="22"/>
       <c r="K118" s="34" t="s">
@@ -23621,11 +23656,11 @@
       </c>
       <c r="L118" s="34"/>
       <c r="M118" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N118" s="22"/>
       <c r="O118" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P118" s="22"/>
       <c r="Q118" s="22" t="s">
@@ -23678,7 +23713,7 @@
       </c>
       <c r="H119" s="23"/>
       <c r="I119" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J119" s="22"/>
       <c r="K119" s="34" t="s">
@@ -23686,11 +23721,11 @@
       </c>
       <c r="L119" s="34"/>
       <c r="M119" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N119" s="22"/>
       <c r="O119" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P119" s="22"/>
       <c r="Q119" s="22" t="s">
@@ -23743,7 +23778,7 @@
       </c>
       <c r="H120" s="23"/>
       <c r="I120" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J120" s="22"/>
       <c r="K120" s="34" t="s">
@@ -23751,11 +23786,11 @@
       </c>
       <c r="L120" s="34"/>
       <c r="M120" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N120" s="22"/>
       <c r="O120" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P120" s="22"/>
       <c r="Q120" s="22" t="s">
@@ -23808,7 +23843,7 @@
       </c>
       <c r="H121" s="23"/>
       <c r="I121" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J121" s="22"/>
       <c r="K121" s="34" t="s">
@@ -23816,11 +23851,11 @@
       </c>
       <c r="L121" s="34"/>
       <c r="M121" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N121" s="22"/>
       <c r="O121" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P121" s="22"/>
       <c r="Q121" s="22" t="s">
@@ -23873,7 +23908,7 @@
       </c>
       <c r="H122" s="23"/>
       <c r="I122" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J122" s="22"/>
       <c r="K122" s="34" t="s">
@@ -23881,11 +23916,11 @@
       </c>
       <c r="L122" s="34"/>
       <c r="M122" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N122" s="22"/>
       <c r="O122" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P122" s="22"/>
       <c r="Q122" s="22" t="s">
@@ -23938,7 +23973,7 @@
       </c>
       <c r="H123" s="23"/>
       <c r="I123" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J123" s="22"/>
       <c r="K123" s="34" t="s">
@@ -23946,11 +23981,11 @@
       </c>
       <c r="L123" s="34"/>
       <c r="M123" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N123" s="22"/>
       <c r="O123" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P123" s="22"/>
       <c r="Q123" s="22" t="s">
@@ -24003,7 +24038,7 @@
       </c>
       <c r="H124" s="23"/>
       <c r="I124" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J124" s="22"/>
       <c r="K124" s="34" t="s">
@@ -24011,11 +24046,11 @@
       </c>
       <c r="L124" s="34"/>
       <c r="M124" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N124" s="22"/>
       <c r="O124" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P124" s="22"/>
       <c r="Q124" s="22" t="s">
@@ -24068,7 +24103,7 @@
       </c>
       <c r="H125" s="23"/>
       <c r="I125" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J125" s="22"/>
       <c r="K125" s="34" t="s">
@@ -24076,11 +24111,11 @@
       </c>
       <c r="L125" s="34"/>
       <c r="M125" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N125" s="22"/>
       <c r="O125" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P125" s="22"/>
       <c r="Q125" s="22" t="s">
@@ -24133,7 +24168,7 @@
       </c>
       <c r="H126" s="23"/>
       <c r="I126" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J126" s="22"/>
       <c r="K126" s="34" t="s">
@@ -24141,11 +24176,11 @@
       </c>
       <c r="L126" s="34"/>
       <c r="M126" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N126" s="22"/>
       <c r="O126" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P126" s="22"/>
       <c r="Q126" s="22" t="s">
@@ -24198,7 +24233,7 @@
       </c>
       <c r="H127" s="23"/>
       <c r="I127" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J127" s="22"/>
       <c r="K127" s="34" t="s">
@@ -24206,11 +24241,11 @@
       </c>
       <c r="L127" s="34"/>
       <c r="M127" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N127" s="22"/>
       <c r="O127" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P127" s="22"/>
       <c r="Q127" s="22" t="s">
@@ -24263,7 +24298,7 @@
       </c>
       <c r="H128" s="23"/>
       <c r="I128" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J128" s="22"/>
       <c r="K128" s="34" t="s">
@@ -24271,11 +24306,11 @@
       </c>
       <c r="L128" s="34"/>
       <c r="M128" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N128" s="22"/>
       <c r="O128" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P128" s="22"/>
       <c r="Q128" s="22" t="s">
@@ -24328,7 +24363,7 @@
       </c>
       <c r="H129" s="23"/>
       <c r="I129" s="23" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="J129" s="22"/>
       <c r="K129" s="34" t="s">
@@ -24336,11 +24371,11 @@
       </c>
       <c r="L129" s="34"/>
       <c r="M129" s="34" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="N129" s="22"/>
       <c r="O129" s="34" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="P129" s="22"/>
       <c r="Q129" s="22" t="s">
@@ -24393,7 +24428,7 @@
       </c>
       <c r="H130" s="23"/>
       <c r="I130" s="23" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J130" s="22"/>
       <c r="K130" s="34" t="s">
@@ -24401,11 +24436,11 @@
       </c>
       <c r="L130" s="34"/>
       <c r="M130" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N130" s="22"/>
       <c r="O130" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P130" s="22"/>
       <c r="Q130" s="22" t="s">
@@ -24458,7 +24493,7 @@
       </c>
       <c r="H131" s="26"/>
       <c r="I131" s="26" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="J131" s="22"/>
       <c r="K131" s="34" t="s">
@@ -24466,11 +24501,11 @@
       </c>
       <c r="L131" s="34"/>
       <c r="M131" s="34" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="N131" s="22"/>
       <c r="O131" s="34" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="P131" s="22"/>
       <c r="Q131" s="22" t="s">
@@ -24543,35 +24578,35 @@
     <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:AD131">
-    <cfRule type="containsBlanks" dxfId="6" priority="31">
+    <cfRule type="containsBlanks" dxfId="0" priority="31">
       <formula>LEN(TRIM(C1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65:B69 B71:B77 B81:B1048576 B52:B63 B1:B31">
-    <cfRule type="duplicateValues" dxfId="5" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q44 Q46:Q76 Q97:Q100 Q78:Q95">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="5" priority="5">
       <formula>LEN(TRIM(Q1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q45">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="4" priority="4">
       <formula>LEN(TRIM(Q45))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q77">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="3" priority="3">
       <formula>LEN(TRIM(Q77))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q96">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(Q96))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q101">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(Q101))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24585,7 +24620,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
amended urban header on second page for better readability in different languages
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC4E877-ADA4-4E97-8E67-A64748736F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F494BB9-BB76-4BF6-8248-798833FD3329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2762,9 +2762,6 @@
     <t>Comparisons with 25 cities internationally</t>
   </si>
   <si>
-    <t>{city} Healthy and Sustainable City Indicators Report</t>
-  </si>
-  <si>
     <t>Policy presence in {city}</t>
   </si>
   <si>
@@ -4445,6 +4442,9 @@
   </si>
   <si>
     <t xml:space="preserve">Densidad de intersección de calles por km²  en el barrio </t>
+  </si>
+  <si>
+    <t>Healthy and Sustainable City Indicators Report: {city}, {country}</t>
   </si>
 </sst>
 </file>
@@ -16822,10 +16822,10 @@
   <dimension ref="A1:AD156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D137" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A137" sqref="A137"/>
+      <selection pane="bottomRight" activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -16869,7 +16869,7 @@
         <v>302</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J1" s="18" t="s">
         <v>301</v>
@@ -16881,7 +16881,7 @@
         <v>300</v>
       </c>
       <c r="M1" s="19" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="N1" s="19" t="s">
         <v>297</v>
@@ -16890,10 +16890,10 @@
         <v>847</v>
       </c>
       <c r="P1" s="19" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="Q1" s="19" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="R1" s="19" t="s">
         <v>647</v>
@@ -16952,10 +16952,10 @@
         <v>661</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J2" s="20" t="s">
         <v>646</v>
@@ -16964,14 +16964,14 @@
         <v>654</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="N2" s="20"/>
       <c r="O2" s="20" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="P2" s="20" t="s">
         <v>849</v>
@@ -17019,60 +17019,60 @@
         <v>643</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="F3" s="22"/>
       <c r="G3" s="22" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="H3" s="23"/>
       <c r="I3" s="23" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="J3" s="22"/>
       <c r="K3" s="37" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="L3" s="37"/>
       <c r="M3" s="37" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="N3" s="22"/>
       <c r="O3" s="37" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="P3" s="22" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="Q3" s="22" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="R3" s="22" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="S3" s="22"/>
       <c r="T3" s="37" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="U3" s="22"/>
       <c r="V3" s="37" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="W3" s="22"/>
       <c r="X3" s="39" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="Y3" s="22"/>
       <c r="Z3" s="22" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="AA3" s="22"/>
       <c r="AB3" s="22" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="AC3" s="22"/>
       <c r="AD3" s="22"/>
@@ -17089,56 +17089,56 @@
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="22" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="22" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="H4" s="23"/>
       <c r="I4" s="23" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="J4" s="22"/>
       <c r="K4" s="37" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="L4" s="37"/>
       <c r="M4" s="37" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="N4" s="22"/>
       <c r="O4" s="37" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="P4" s="22" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="Q4" s="22" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="R4" s="22" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="S4" s="22"/>
       <c r="T4" s="37" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="U4" s="22"/>
       <c r="V4" s="37" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="W4" s="22"/>
       <c r="X4" s="39" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="Y4" s="22"/>
       <c r="Z4" s="22" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="AA4" s="22"/>
       <c r="AB4" s="22" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="AC4" s="22"/>
       <c r="AD4" s="22"/>
@@ -17163,7 +17163,7 @@
       </c>
       <c r="H5" s="23"/>
       <c r="I5" s="23" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="J5" s="22"/>
       <c r="K5" s="37" t="s">
@@ -17171,11 +17171,11 @@
       </c>
       <c r="L5" s="37"/>
       <c r="M5" s="37" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="N5" s="22"/>
       <c r="O5" s="37" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="P5" s="22" t="s">
         <v>850</v>
@@ -17663,7 +17663,7 @@
       <c r="K17" s="37"/>
       <c r="L17" s="37"/>
       <c r="M17" s="37" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="N17" s="22"/>
       <c r="O17" s="37"/>
@@ -17739,7 +17739,7 @@
       <c r="G19" s="22"/>
       <c r="H19" s="23"/>
       <c r="I19" s="23" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="J19" s="22"/>
       <c r="K19" s="37"/>
@@ -18210,10 +18210,10 @@
         <v>195</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
@@ -18248,10 +18248,10 @@
         <v>195</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
@@ -18266,11 +18266,11 @@
       <c r="N32" s="22"/>
       <c r="O32" s="37"/>
       <c r="P32" s="22" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="Q32" s="22"/>
       <c r="R32" s="22" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="S32" s="22"/>
       <c r="T32" s="37"/>
@@ -18290,10 +18290,10 @@
         <v>195</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
@@ -18328,10 +18328,10 @@
         <v>195</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
@@ -18366,10 +18366,10 @@
         <v>195</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
@@ -18404,10 +18404,10 @@
         <v>195</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
@@ -18426,7 +18426,7 @@
       <c r="R36" s="22"/>
       <c r="S36" s="22"/>
       <c r="T36" s="37" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="U36" s="22"/>
       <c r="V36" s="37"/>
@@ -18444,16 +18444,16 @@
         <v>195</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
       <c r="G37" s="22" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="H37" s="23"/>
       <c r="I37" s="23"/>
@@ -18484,10 +18484,10 @@
         <v>195</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="D38" s="22"/>
       <c r="E38" s="22"/>
@@ -18510,7 +18510,7 @@
       <c r="V38" s="37"/>
       <c r="W38" s="22"/>
       <c r="X38" s="39" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="Y38" s="22"/>
       <c r="Z38" s="22"/>
@@ -18524,10 +18524,10 @@
         <v>195</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
@@ -18552,7 +18552,7 @@
       <c r="X39" s="39"/>
       <c r="Y39" s="22"/>
       <c r="Z39" s="22" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="AA39" s="22"/>
       <c r="AB39" s="22"/>
@@ -18564,10 +18564,10 @@
         <v>195</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
@@ -18594,7 +18594,7 @@
       <c r="Z40" s="22"/>
       <c r="AA40" s="22"/>
       <c r="AB40" s="22" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="AC40" s="22"/>
       <c r="AD40" s="22"/>
@@ -18604,10 +18604,10 @@
         <v>195</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
@@ -18621,7 +18621,7 @@
       <c r="M41" s="37"/>
       <c r="N41" s="22"/>
       <c r="O41" s="37" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="P41" s="22"/>
       <c r="Q41" s="22"/>
@@ -18644,10 +18644,10 @@
         <v>195</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="D42" s="22"/>
       <c r="E42" s="22"/>
@@ -18659,7 +18659,7 @@
       <c r="K42" s="37"/>
       <c r="L42" s="37"/>
       <c r="M42" s="37" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="N42" s="22"/>
       <c r="O42" s="37"/>
@@ -18684,10 +18684,10 @@
         <v>195</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
@@ -18701,7 +18701,7 @@
       <c r="M43" s="37"/>
       <c r="N43" s="22"/>
       <c r="O43" s="37" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="P43" s="22"/>
       <c r="Q43" s="22"/>
@@ -18724,10 +18724,10 @@
         <v>195</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
@@ -18735,7 +18735,7 @@
       <c r="G44" s="22"/>
       <c r="H44" s="23"/>
       <c r="I44" s="23" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="J44" s="22"/>
       <c r="K44" s="37"/>
@@ -18764,10 +18764,10 @@
         <v>195</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="C45" s="23" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
@@ -18781,7 +18781,7 @@
       <c r="M45" s="37"/>
       <c r="N45" s="22"/>
       <c r="O45" s="37" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="P45" s="22"/>
       <c r="Q45" s="22"/>
@@ -18804,10 +18804,10 @@
         <v>195</v>
       </c>
       <c r="B46" s="30" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
@@ -18817,7 +18817,7 @@
       <c r="I46" s="23"/>
       <c r="J46" s="22"/>
       <c r="K46" s="37" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="L46" s="37"/>
       <c r="M46" s="37"/>
@@ -18844,14 +18844,14 @@
         <v>195</v>
       </c>
       <c r="B47" s="30" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="22" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="F47" s="22"/>
       <c r="G47" s="22"/>
@@ -18865,10 +18865,10 @@
       <c r="O47" s="37"/>
       <c r="P47" s="22"/>
       <c r="Q47" s="22" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="R47" s="22" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="S47" s="22"/>
       <c r="T47" s="37"/>
@@ -18888,14 +18888,14 @@
         <v>195</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="22" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="F48" s="22"/>
       <c r="G48" s="22"/>
@@ -18909,10 +18909,10 @@
       <c r="O48" s="37"/>
       <c r="P48" s="22"/>
       <c r="Q48" s="22" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="R48" s="22" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="S48" s="22"/>
       <c r="T48" s="37"/>
@@ -18932,14 +18932,14 @@
         <v>195</v>
       </c>
       <c r="B49" s="30" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="D49" s="22"/>
       <c r="E49" s="22" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="F49" s="22"/>
       <c r="G49" s="22"/>
@@ -18953,10 +18953,10 @@
       <c r="O49" s="37"/>
       <c r="P49" s="22"/>
       <c r="Q49" s="22" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="R49" s="22" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="S49" s="22"/>
       <c r="T49" s="37"/>
@@ -18976,10 +18976,10 @@
         <v>195</v>
       </c>
       <c r="B50" s="30" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
@@ -19014,10 +19014,10 @@
         <v>195</v>
       </c>
       <c r="B51" s="30" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
@@ -19038,7 +19038,7 @@
       <c r="T51" s="37"/>
       <c r="U51" s="22"/>
       <c r="V51" s="37" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="W51" s="22"/>
       <c r="X51" s="39"/>
@@ -19054,10 +19054,10 @@
         <v>195</v>
       </c>
       <c r="B52" s="32" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
@@ -19092,10 +19092,10 @@
         <v>195</v>
       </c>
       <c r="B53" s="30" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
@@ -19130,10 +19130,10 @@
         <v>195</v>
       </c>
       <c r="B54" s="30" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="D54" s="22"/>
       <c r="E54" s="22"/>
@@ -19168,10 +19168,10 @@
         <v>195</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="D55" s="22"/>
       <c r="E55" s="22"/>
@@ -19219,7 +19219,7 @@
       <c r="G56" s="20"/>
       <c r="H56" s="21"/>
       <c r="I56" s="21" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="J56" s="20"/>
       <c r="K56" s="37" t="s">
@@ -19227,11 +19227,11 @@
       </c>
       <c r="L56" s="37"/>
       <c r="M56" s="37" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="N56" s="20"/>
       <c r="O56" s="37" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="P56" s="20" t="s">
         <v>851</v>
@@ -19285,19 +19285,19 @@
       </c>
       <c r="H57" s="21"/>
       <c r="I57" s="21" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="J57" s="20"/>
       <c r="K57" s="37" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="L57" s="37"/>
       <c r="M57" s="37" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="N57" s="20"/>
       <c r="O57" s="37" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="P57" s="20" t="s">
         <v>852</v>
@@ -19351,7 +19351,7 @@
       </c>
       <c r="H58" s="21"/>
       <c r="I58" s="21" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="J58" s="20"/>
       <c r="K58" s="37" t="s">
@@ -19359,11 +19359,11 @@
       </c>
       <c r="L58" s="37"/>
       <c r="M58" s="37" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="N58" s="20"/>
       <c r="O58" s="37" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="P58" s="20" t="s">
         <v>387</v>
@@ -19417,7 +19417,7 @@
       </c>
       <c r="H59" s="21"/>
       <c r="I59" s="21" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="J59" s="20"/>
       <c r="K59" s="37" t="s">
@@ -19425,11 +19425,11 @@
       </c>
       <c r="L59" s="37"/>
       <c r="M59" s="37" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="N59" s="20"/>
       <c r="O59" s="37" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="P59" s="20" t="s">
         <v>853</v>
@@ -19483,7 +19483,7 @@
       </c>
       <c r="H60" s="21"/>
       <c r="I60" s="21" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="J60" s="20"/>
       <c r="K60" s="37" t="s">
@@ -19491,11 +19491,11 @@
       </c>
       <c r="L60" s="37"/>
       <c r="M60" s="37" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="N60" s="20"/>
       <c r="O60" s="37" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="P60" s="20" t="s">
         <v>389</v>
@@ -19549,7 +19549,7 @@
       </c>
       <c r="H61" s="21"/>
       <c r="I61" s="21" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="J61" s="20"/>
       <c r="K61" s="37" t="s">
@@ -19557,11 +19557,11 @@
       </c>
       <c r="L61" s="37"/>
       <c r="M61" s="37" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="N61" s="20"/>
       <c r="O61" s="37" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="P61" s="20" t="s">
         <v>390</v>
@@ -19615,7 +19615,7 @@
       </c>
       <c r="H62" s="21"/>
       <c r="I62" s="21" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="J62" s="20"/>
       <c r="K62" s="37" t="s">
@@ -19623,11 +19623,11 @@
       </c>
       <c r="L62" s="37"/>
       <c r="M62" s="37" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="N62" s="20"/>
       <c r="O62" s="37" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="P62" s="20" t="s">
         <v>391</v>
@@ -19669,7 +19669,7 @@
         <v>206</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="D63" s="20"/>
       <c r="E63" s="20" t="s">
@@ -19681,7 +19681,7 @@
       </c>
       <c r="H63" s="21"/>
       <c r="I63" s="21" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="J63" s="20"/>
       <c r="K63" s="37" t="s">
@@ -19689,17 +19689,17 @@
       </c>
       <c r="L63" s="37"/>
       <c r="M63" s="37" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="N63" s="20"/>
       <c r="O63" s="37" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="P63" s="20" t="s">
         <v>854</v>
       </c>
       <c r="Q63" s="22" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="R63" s="20" t="s">
         <v>392</v>
@@ -19747,7 +19747,7 @@
       </c>
       <c r="H64" s="21"/>
       <c r="I64" s="21" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="J64" s="20"/>
       <c r="K64" s="37" t="s">
@@ -19755,11 +19755,11 @@
       </c>
       <c r="L64" s="37"/>
       <c r="M64" s="37" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="N64" s="20"/>
       <c r="O64" s="37" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="P64" s="20" t="s">
         <v>393</v>
@@ -19813,7 +19813,7 @@
       </c>
       <c r="H65" s="21"/>
       <c r="I65" s="21" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="J65" s="20"/>
       <c r="K65" s="37" t="s">
@@ -19821,11 +19821,11 @@
       </c>
       <c r="L65" s="37"/>
       <c r="M65" s="37" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="N65" s="20"/>
       <c r="O65" s="37" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="P65" s="20" t="s">
         <v>394</v>
@@ -19879,7 +19879,7 @@
       </c>
       <c r="H66" s="21"/>
       <c r="I66" s="21" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="J66" s="20"/>
       <c r="K66" s="37" t="s">
@@ -19887,11 +19887,11 @@
       </c>
       <c r="L66" s="37"/>
       <c r="M66" s="37" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="N66" s="20"/>
       <c r="O66" s="37" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="P66" s="20" t="s">
         <v>395</v>
@@ -19937,7 +19937,7 @@
       </c>
       <c r="D67" s="20"/>
       <c r="E67" s="20" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="F67" s="20"/>
       <c r="G67" s="20" t="s">
@@ -19945,19 +19945,19 @@
       </c>
       <c r="H67" s="21"/>
       <c r="I67" s="21" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="J67" s="20"/>
       <c r="K67" s="37" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="L67" s="37"/>
       <c r="M67" s="37" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="N67" s="20"/>
       <c r="O67" s="37" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="P67" s="20" t="s">
         <v>883</v>
@@ -19970,11 +19970,11 @@
       </c>
       <c r="S67" s="20"/>
       <c r="T67" s="37" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="U67" s="20"/>
       <c r="V67" s="37" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="W67" s="20"/>
       <c r="X67" s="39" t="s">
@@ -19982,11 +19982,11 @@
       </c>
       <c r="Y67" s="20"/>
       <c r="Z67" s="20" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="AA67" s="20"/>
       <c r="AB67" s="20" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="AC67" s="20"/>
       <c r="AD67" s="20"/>
@@ -20003,7 +20003,7 @@
       </c>
       <c r="D68" s="20"/>
       <c r="E68" s="20" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="F68" s="20"/>
       <c r="G68" s="20" t="s">
@@ -20011,19 +20011,19 @@
       </c>
       <c r="H68" s="21"/>
       <c r="I68" s="21" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="J68" s="20"/>
       <c r="K68" s="37" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="L68" s="37"/>
       <c r="M68" s="37" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="N68" s="20"/>
       <c r="O68" s="37" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="P68" s="20" t="s">
         <v>887</v>
@@ -20032,7 +20032,7 @@
         <v>887</v>
       </c>
       <c r="R68" s="20" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="S68" s="20"/>
       <c r="T68" s="37" t="s">
@@ -20040,19 +20040,19 @@
       </c>
       <c r="U68" s="20"/>
       <c r="V68" s="37" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="W68" s="20"/>
       <c r="X68" s="39" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="Y68" s="20"/>
       <c r="Z68" s="20" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="AA68" s="20"/>
       <c r="AB68" s="20" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="AC68" s="20"/>
       <c r="AD68" s="20"/>
@@ -20069,7 +20069,7 @@
       </c>
       <c r="D69" s="20"/>
       <c r="E69" s="20" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="F69" s="20"/>
       <c r="G69" s="20" t="s">
@@ -20077,19 +20077,19 @@
       </c>
       <c r="H69" s="21"/>
       <c r="I69" s="21" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="J69" s="20"/>
       <c r="K69" s="37" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="L69" s="37"/>
       <c r="M69" s="37" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="N69" s="20"/>
       <c r="O69" s="37" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="P69" s="20" t="s">
         <v>886</v>
@@ -20098,27 +20098,27 @@
         <v>886</v>
       </c>
       <c r="R69" s="20" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="S69" s="20"/>
       <c r="T69" s="37" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="U69" s="20"/>
       <c r="V69" s="37" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="W69" s="20"/>
       <c r="X69" s="39" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="Y69" s="20"/>
       <c r="Z69" s="20" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="AA69" s="20"/>
       <c r="AB69" s="20" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="AC69" s="20"/>
       <c r="AD69" s="20"/>
@@ -20135,27 +20135,27 @@
       </c>
       <c r="D70" s="20"/>
       <c r="E70" s="20" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="F70" s="20"/>
       <c r="G70" s="20" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="H70" s="21"/>
       <c r="I70" s="21" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="J70" s="20"/>
       <c r="K70" s="37" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="L70" s="37"/>
       <c r="M70" s="37" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="N70" s="20"/>
       <c r="O70" s="37" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="P70" s="20" t="s">
         <v>855</v>
@@ -20164,15 +20164,15 @@
         <v>855</v>
       </c>
       <c r="R70" s="20" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="S70" s="20"/>
       <c r="T70" s="37" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="U70" s="20"/>
       <c r="V70" s="37" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="W70" s="20"/>
       <c r="X70" s="39" t="s">
@@ -20180,11 +20180,11 @@
       </c>
       <c r="Y70" s="20"/>
       <c r="Z70" s="20" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="AA70" s="20"/>
       <c r="AB70" s="20" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="AC70" s="20"/>
       <c r="AD70" s="20"/>
@@ -20209,7 +20209,7 @@
       </c>
       <c r="H71" s="21"/>
       <c r="I71" s="21" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="J71" s="20"/>
       <c r="K71" s="37" t="s">
@@ -20217,11 +20217,11 @@
       </c>
       <c r="L71" s="37"/>
       <c r="M71" s="37" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="N71" s="20"/>
       <c r="O71" s="37" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="P71" s="20" t="s">
         <v>396</v>
@@ -20267,27 +20267,27 @@
       </c>
       <c r="D72" s="20"/>
       <c r="E72" s="20" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="F72" s="20"/>
       <c r="G72" s="20" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="H72" s="21"/>
       <c r="I72" s="21" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="J72" s="20"/>
       <c r="K72" s="37" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="L72" s="37"/>
       <c r="M72" s="37" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="N72" s="20"/>
       <c r="O72" s="37" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="P72" s="20" t="s">
         <v>856</v>
@@ -20296,27 +20296,27 @@
         <v>856</v>
       </c>
       <c r="R72" s="20" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="S72" s="20"/>
       <c r="T72" s="37" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="U72" s="20"/>
       <c r="V72" s="37" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="W72" s="20"/>
       <c r="X72" s="39" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="Y72" s="20"/>
       <c r="Z72" s="20" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="AA72" s="20"/>
       <c r="AB72" s="20" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="AC72" s="20"/>
       <c r="AD72" s="20"/>
@@ -20326,63 +20326,63 @@
         <v>196</v>
       </c>
       <c r="B73" s="30" t="s">
+        <v>907</v>
+      </c>
+      <c r="C73" s="21" t="s">
         <v>908</v>
-      </c>
-      <c r="C73" s="21" t="s">
-        <v>909</v>
       </c>
       <c r="D73" s="20"/>
       <c r="E73" s="20" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="F73" s="20"/>
       <c r="G73" s="20" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="H73" s="21"/>
       <c r="I73" s="21" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="J73" s="20"/>
       <c r="K73" s="37" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="L73" s="37"/>
       <c r="M73" s="37" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="N73" s="20"/>
       <c r="O73" s="37" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="P73" s="20" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="Q73" s="20" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="R73" s="20" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="S73" s="20"/>
       <c r="T73" s="37" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="U73" s="20"/>
       <c r="V73" s="37" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="W73" s="20"/>
       <c r="X73" s="39" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="Y73" s="20"/>
       <c r="Z73" s="20" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="AA73" s="20"/>
       <c r="AB73" s="20" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="AC73" s="20"/>
       <c r="AD73" s="20"/>
@@ -20395,60 +20395,60 @@
         <v>215</v>
       </c>
       <c r="C74" s="21" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D74" s="20"/>
       <c r="E74" s="20" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="F74" s="20"/>
       <c r="G74" s="20" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="H74" s="21"/>
       <c r="I74" s="21" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="J74" s="20"/>
       <c r="K74" s="37" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="L74" s="37"/>
       <c r="M74" s="37" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="N74" s="20"/>
       <c r="O74" s="37" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="P74" s="20" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="Q74" s="22" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="R74" s="20" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="S74" s="20"/>
       <c r="T74" s="37" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="U74" s="20"/>
       <c r="V74" s="37" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="W74" s="20"/>
       <c r="X74" s="39" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="Y74" s="20"/>
       <c r="Z74" s="20" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="AA74" s="20"/>
       <c r="AB74" s="20" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AC74" s="20"/>
       <c r="AD74" s="20"/>
@@ -20461,60 +20461,60 @@
         <v>216</v>
       </c>
       <c r="C75" s="21" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="D75" s="20"/>
       <c r="E75" s="20" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="F75" s="20"/>
       <c r="G75" s="20" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="H75" s="21"/>
       <c r="I75" s="21" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="J75" s="20"/>
       <c r="K75" s="37" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="L75" s="37"/>
       <c r="M75" s="37" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="N75" s="20"/>
       <c r="O75" s="37" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="P75" s="20" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="Q75" s="22" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="R75" s="20" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="S75" s="20"/>
       <c r="T75" s="37" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="U75" s="20"/>
       <c r="V75" s="37" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="W75" s="20"/>
       <c r="X75" s="39" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="Y75" s="20"/>
       <c r="Z75" s="20" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="AA75" s="20"/>
       <c r="AB75" s="20" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="AC75" s="20"/>
       <c r="AD75" s="20"/>
@@ -20527,7 +20527,7 @@
         <v>272</v>
       </c>
       <c r="C76" s="21" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="D76" s="20"/>
       <c r="E76" s="20" t="s">
@@ -20539,7 +20539,7 @@
       </c>
       <c r="H76" s="21"/>
       <c r="I76" s="21" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="J76" s="20"/>
       <c r="K76" s="37" t="s">
@@ -20547,11 +20547,11 @@
       </c>
       <c r="L76" s="37"/>
       <c r="M76" s="37" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="N76" s="20"/>
       <c r="O76" s="37" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="P76" s="20" t="s">
         <v>857</v>
@@ -20601,23 +20601,23 @@
       </c>
       <c r="F77" s="22"/>
       <c r="G77" s="22" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="H77" s="23"/>
       <c r="I77" s="23" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="J77" s="22"/>
       <c r="K77" s="37" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="L77" s="37"/>
       <c r="M77" s="37" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="N77" s="22"/>
       <c r="O77" s="37" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="P77" s="22" t="s">
         <v>858</v>
@@ -20630,7 +20630,7 @@
       </c>
       <c r="S77" s="22"/>
       <c r="T77" s="37" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="U77" s="22"/>
       <c r="V77" s="37" t="s">
@@ -20638,11 +20638,11 @@
       </c>
       <c r="W77" s="22"/>
       <c r="X77" s="39" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="Y77" s="22"/>
       <c r="Z77" s="22" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="AA77" s="22"/>
       <c r="AB77" s="22" t="s">
@@ -20667,23 +20667,23 @@
       </c>
       <c r="F78" s="22"/>
       <c r="G78" s="22" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="H78" s="23"/>
       <c r="I78" s="23" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="J78" s="22"/>
       <c r="K78" s="37" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="L78" s="37"/>
       <c r="M78" s="37" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="N78" s="22"/>
       <c r="O78" s="37" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="P78" s="22" t="s">
         <v>859</v>
@@ -20700,7 +20700,7 @@
       </c>
       <c r="U78" s="22"/>
       <c r="V78" s="37" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="W78" s="22"/>
       <c r="X78" s="39" t="s">
@@ -20708,7 +20708,7 @@
       </c>
       <c r="Y78" s="22"/>
       <c r="Z78" s="22" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="AA78" s="22"/>
       <c r="AB78" s="22" t="s">
@@ -20737,7 +20737,7 @@
       </c>
       <c r="H79" s="23"/>
       <c r="I79" s="23" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="J79" s="22"/>
       <c r="K79" s="37" t="s">
@@ -20745,11 +20745,11 @@
       </c>
       <c r="L79" s="37"/>
       <c r="M79" s="37" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="N79" s="22"/>
       <c r="O79" s="37" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="P79" s="22" t="s">
         <v>630</v>
@@ -20803,7 +20803,7 @@
       </c>
       <c r="H80" s="23"/>
       <c r="I80" s="23" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="J80" s="22"/>
       <c r="K80" s="37" t="s">
@@ -20811,11 +20811,11 @@
       </c>
       <c r="L80" s="37"/>
       <c r="M80" s="37" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="N80" s="22"/>
       <c r="O80" s="37" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="P80" s="22" t="s">
         <v>860</v>
@@ -20857,60 +20857,60 @@
         <v>42</v>
       </c>
       <c r="C81" s="23" t="s">
-        <v>903</v>
+        <v>1446</v>
       </c>
       <c r="D81" s="22"/>
       <c r="E81" s="22" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="F81" s="22"/>
       <c r="G81" s="22" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="H81" s="23"/>
       <c r="I81" s="23" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="J81" s="22"/>
       <c r="K81" s="37" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="L81" s="37"/>
       <c r="M81" s="37" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="N81" s="22"/>
       <c r="O81" s="37" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="P81" s="22" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="Q81" s="22" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="R81" s="22" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="S81" s="22"/>
       <c r="T81" s="37" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="U81" s="22"/>
       <c r="V81" s="37" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="W81" s="22"/>
       <c r="X81" s="39" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="Y81" s="22"/>
       <c r="Z81" s="22" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="AA81" s="22"/>
       <c r="AB81" s="22" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="AC81" s="22"/>
       <c r="AD81" s="22"/>
@@ -20923,31 +20923,31 @@
         <v>242</v>
       </c>
       <c r="C82" s="23" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="D82" s="22"/>
       <c r="E82" s="22" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="F82" s="22"/>
       <c r="G82" s="22" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="H82" s="23"/>
       <c r="I82" s="23" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="J82" s="22"/>
       <c r="K82" s="37" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="L82" s="37"/>
       <c r="M82" s="37" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="N82" s="22"/>
       <c r="O82" s="37" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="P82" s="22" t="s">
         <v>881</v>
@@ -20956,27 +20956,27 @@
         <v>881</v>
       </c>
       <c r="R82" s="22" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="S82" s="22"/>
       <c r="T82" s="37" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="U82" s="22"/>
       <c r="V82" s="37" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="W82" s="22"/>
       <c r="X82" s="39" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="Y82" s="22"/>
       <c r="Z82" s="22" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="AA82" s="22"/>
       <c r="AB82" s="22" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="AC82" s="22"/>
       <c r="AD82" s="22"/>
@@ -20989,31 +20989,31 @@
         <v>382</v>
       </c>
       <c r="C83" s="23" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="D83" s="22"/>
       <c r="E83" s="22" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="F83" s="22"/>
       <c r="G83" s="22" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="H83" s="23"/>
       <c r="I83" s="23" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="J83" s="22"/>
       <c r="K83" s="37" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="L83" s="37"/>
       <c r="M83" s="37" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="N83" s="22"/>
       <c r="O83" s="37" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="P83" s="22" t="s">
         <v>882</v>
@@ -21022,27 +21022,27 @@
         <v>882</v>
       </c>
       <c r="R83" s="22" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="S83" s="22"/>
       <c r="T83" s="37" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="U83" s="22"/>
       <c r="V83" s="37" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="W83" s="22"/>
       <c r="X83" s="39" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="Y83" s="22"/>
       <c r="Z83" s="22" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="AA83" s="22"/>
       <c r="AB83" s="22" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="AC83" s="22"/>
       <c r="AD83" s="22"/>
@@ -21055,48 +21055,48 @@
         <v>44</v>
       </c>
       <c r="C84" s="23" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="D84" s="22"/>
       <c r="E84" s="22" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="F84" s="22"/>
       <c r="G84" s="22" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="H84" s="23"/>
       <c r="I84" s="23" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="J84" s="22"/>
       <c r="K84" s="37" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="L84" s="37"/>
       <c r="M84" s="37" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="N84" s="22"/>
       <c r="O84" s="37" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="P84" s="22" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="Q84" s="22" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="R84" s="22" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="S84" s="22"/>
       <c r="T84" s="37" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="U84" s="22"/>
       <c r="V84" s="37" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="W84" s="22"/>
       <c r="X84" s="39" t="s">
@@ -21104,11 +21104,11 @@
       </c>
       <c r="Y84" s="22"/>
       <c r="Z84" s="22" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="AA84" s="22"/>
       <c r="AB84" s="22" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="AC84" s="22"/>
       <c r="AD84" s="22"/>
@@ -21121,7 +21121,7 @@
         <v>45</v>
       </c>
       <c r="C85" s="23" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="D85" s="22"/>
       <c r="E85" s="22" t="s">
@@ -21133,7 +21133,7 @@
       </c>
       <c r="H85" s="23"/>
       <c r="I85" s="23" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="J85" s="22"/>
       <c r="K85" s="37" t="s">
@@ -21141,11 +21141,11 @@
       </c>
       <c r="L85" s="37"/>
       <c r="M85" s="37" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="N85" s="22"/>
       <c r="O85" s="37" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="P85" s="22" t="s">
         <v>861</v>
@@ -21187,7 +21187,7 @@
         <v>48</v>
       </c>
       <c r="C86" s="23" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="D86" s="22"/>
       <c r="E86" s="22" t="s">
@@ -21199,7 +21199,7 @@
       </c>
       <c r="H86" s="23"/>
       <c r="I86" s="23" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="J86" s="22"/>
       <c r="K86" s="37" t="s">
@@ -21207,11 +21207,11 @@
       </c>
       <c r="L86" s="37"/>
       <c r="M86" s="37" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="N86" s="22"/>
       <c r="O86" s="37" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="P86" s="22" t="s">
         <v>401</v>
@@ -21253,31 +21253,31 @@
         <v>314</v>
       </c>
       <c r="C87" s="23" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="D87" s="22"/>
       <c r="E87" s="22" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="F87" s="22"/>
       <c r="G87" s="22" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="H87" s="23"/>
       <c r="I87" s="23" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="J87" s="22"/>
       <c r="K87" s="37" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="L87" s="37"/>
       <c r="M87" s="37" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="N87" s="22"/>
       <c r="O87" s="37" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="P87" s="22" t="s">
         <v>862</v>
@@ -21286,27 +21286,27 @@
         <v>862</v>
       </c>
       <c r="R87" s="22" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="S87" s="22"/>
       <c r="T87" s="37" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="U87" s="22"/>
       <c r="V87" s="37" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="W87" s="22"/>
       <c r="X87" s="39" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="Y87" s="22"/>
       <c r="Z87" s="22" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="AA87" s="22"/>
       <c r="AB87" s="22" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="AC87" s="22"/>
       <c r="AD87" s="22"/>
@@ -21319,60 +21319,60 @@
         <v>51</v>
       </c>
       <c r="C88" s="23" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D88" s="22"/>
       <c r="E88" s="22" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="F88" s="22"/>
       <c r="G88" s="22" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="H88" s="23"/>
       <c r="I88" s="23" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="J88" s="22"/>
       <c r="K88" s="37" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="L88" s="37"/>
       <c r="M88" s="37" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="N88" s="22"/>
       <c r="O88" s="37" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="P88" s="22" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="Q88" s="22" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="R88" s="22" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="S88" s="22"/>
       <c r="T88" s="37" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="U88" s="22"/>
       <c r="V88" s="37" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="W88" s="22"/>
       <c r="X88" s="39" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="Y88" s="22"/>
       <c r="Z88" s="22" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="AA88" s="22"/>
       <c r="AB88" s="22" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="AC88" s="22"/>
       <c r="AD88" s="22"/>
@@ -21397,7 +21397,7 @@
       </c>
       <c r="H89" s="23"/>
       <c r="I89" s="23" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="J89" s="22"/>
       <c r="K89" s="37" t="s">
@@ -21405,11 +21405,11 @@
       </c>
       <c r="L89" s="37"/>
       <c r="M89" s="37" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="N89" s="22"/>
       <c r="O89" s="37" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="P89" s="22" t="s">
         <v>863</v>
@@ -21451,60 +21451,60 @@
         <v>52</v>
       </c>
       <c r="C90" s="23" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D90" s="22"/>
       <c r="E90" s="22" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="F90" s="22"/>
       <c r="G90" s="22" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="H90" s="23"/>
       <c r="I90" s="23" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="J90" s="22"/>
       <c r="K90" s="37" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="L90" s="37"/>
       <c r="M90" s="37" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="N90" s="22"/>
       <c r="O90" s="37" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="P90" s="22" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="Q90" s="22" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="R90" s="22" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="S90" s="22"/>
       <c r="T90" s="37" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="U90" s="22"/>
       <c r="V90" s="37" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="W90" s="22"/>
       <c r="X90" s="39" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="Y90" s="22"/>
       <c r="Z90" s="22" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="AA90" s="22"/>
       <c r="AB90" s="22" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="AC90" s="22"/>
       <c r="AD90" s="22"/>
@@ -21529,7 +21529,7 @@
       </c>
       <c r="H91" s="23"/>
       <c r="I91" s="23" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="J91" s="22"/>
       <c r="K91" s="37" t="s">
@@ -21537,11 +21537,11 @@
       </c>
       <c r="L91" s="37"/>
       <c r="M91" s="37" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="N91" s="22"/>
       <c r="O91" s="37" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="P91" s="22" t="s">
         <v>864</v>
@@ -21595,7 +21595,7 @@
       </c>
       <c r="H92" s="23"/>
       <c r="I92" s="23" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="J92" s="22"/>
       <c r="K92" s="37" t="s">
@@ -21603,11 +21603,11 @@
       </c>
       <c r="L92" s="37"/>
       <c r="M92" s="37" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="N92" s="22"/>
       <c r="O92" s="37" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="P92" s="22" t="s">
         <v>865</v>
@@ -21649,31 +21649,31 @@
         <v>55</v>
       </c>
       <c r="C93" s="23" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D93" s="22"/>
       <c r="E93" s="22" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="F93" s="22"/>
       <c r="G93" s="22" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="H93" s="23"/>
       <c r="I93" s="23" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="J93" s="22"/>
       <c r="K93" s="37" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="L93" s="37"/>
       <c r="M93" s="37" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="N93" s="22"/>
       <c r="O93" s="37" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="P93" s="22" t="s">
         <v>866</v>
@@ -21682,27 +21682,27 @@
         <v>866</v>
       </c>
       <c r="R93" s="22" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="S93" s="22"/>
       <c r="T93" s="37" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="U93" s="22"/>
       <c r="V93" s="37" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="W93" s="22"/>
       <c r="X93" s="39" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="Y93" s="22"/>
       <c r="Z93" s="22" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="AA93" s="22"/>
       <c r="AB93" s="22" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="AC93" s="22"/>
       <c r="AD93" s="22"/>
@@ -21727,7 +21727,7 @@
       </c>
       <c r="H94" s="23"/>
       <c r="I94" s="23" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="J94" s="22"/>
       <c r="K94" s="37" t="s">
@@ -21735,11 +21735,11 @@
       </c>
       <c r="L94" s="37"/>
       <c r="M94" s="37" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="N94" s="22"/>
       <c r="O94" s="37" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="P94" s="22" t="s">
         <v>867</v>
@@ -21793,7 +21793,7 @@
       </c>
       <c r="H95" s="23"/>
       <c r="I95" s="23" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="J95" s="22"/>
       <c r="K95" s="37" t="s">
@@ -21801,11 +21801,11 @@
       </c>
       <c r="L95" s="37"/>
       <c r="M95" s="37" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="N95" s="22"/>
       <c r="O95" s="37" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="P95" s="22" t="s">
         <v>868</v>
@@ -21859,7 +21859,7 @@
       </c>
       <c r="H96" s="23"/>
       <c r="I96" s="23" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="J96" s="22"/>
       <c r="K96" s="37" t="s">
@@ -21867,11 +21867,11 @@
       </c>
       <c r="L96" s="37"/>
       <c r="M96" s="37" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="N96" s="22"/>
       <c r="O96" s="37" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="P96" s="22" t="s">
         <v>869</v>
@@ -21925,7 +21925,7 @@
       </c>
       <c r="H97" s="23"/>
       <c r="I97" s="23" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="J97" s="22"/>
       <c r="K97" s="37" t="s">
@@ -21933,11 +21933,11 @@
       </c>
       <c r="L97" s="37"/>
       <c r="M97" s="37" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="N97" s="22"/>
       <c r="O97" s="37" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="P97" s="22" t="s">
         <v>870</v>
@@ -21991,7 +21991,7 @@
       </c>
       <c r="H98" s="23"/>
       <c r="I98" s="23" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="J98" s="22"/>
       <c r="K98" s="37" t="s">
@@ -21999,11 +21999,11 @@
       </c>
       <c r="L98" s="37"/>
       <c r="M98" s="37" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="N98" s="22"/>
       <c r="O98" s="37" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="P98" s="22" t="s">
         <v>871</v>
@@ -22057,7 +22057,7 @@
       </c>
       <c r="H99" s="23"/>
       <c r="I99" s="23" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="J99" s="22"/>
       <c r="K99" s="37" t="s">
@@ -22065,11 +22065,11 @@
       </c>
       <c r="L99" s="37"/>
       <c r="M99" s="37" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="N99" s="22"/>
       <c r="O99" s="37" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="P99" s="22" t="s">
         <v>410</v>
@@ -22123,7 +22123,7 @@
       </c>
       <c r="H100" s="23"/>
       <c r="I100" s="23" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="J100" s="22"/>
       <c r="K100" s="37" t="s">
@@ -22131,11 +22131,11 @@
       </c>
       <c r="L100" s="37"/>
       <c r="M100" s="37" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="N100" s="22"/>
       <c r="O100" s="37" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="P100" s="22" t="s">
         <v>411</v>
@@ -22189,7 +22189,7 @@
       </c>
       <c r="H101" s="23"/>
       <c r="I101" s="23" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="J101" s="22"/>
       <c r="K101" s="37" t="s">
@@ -22197,11 +22197,11 @@
       </c>
       <c r="L101" s="37"/>
       <c r="M101" s="37" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="N101" s="22"/>
       <c r="O101" s="37" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="P101" s="22" t="s">
         <v>412</v>
@@ -22243,60 +22243,60 @@
         <v>85</v>
       </c>
       <c r="C102" s="24" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="D102" s="22"/>
       <c r="E102" s="22" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="F102" s="22"/>
       <c r="G102" s="22" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="H102" s="24"/>
       <c r="I102" s="24" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="J102" s="25"/>
       <c r="K102" s="37" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="L102" s="37"/>
       <c r="M102" s="37" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="N102" s="25"/>
       <c r="O102" s="37" t="s">
+        <v>1112</v>
+      </c>
+      <c r="P102" s="22" t="s">
+        <v>1437</v>
+      </c>
+      <c r="Q102" s="25" t="s">
+        <v>1440</v>
+      </c>
+      <c r="R102" s="22" t="s">
         <v>1113</v>
-      </c>
-      <c r="P102" s="22" t="s">
-        <v>1438</v>
-      </c>
-      <c r="Q102" s="25" t="s">
-        <v>1441</v>
-      </c>
-      <c r="R102" s="22" t="s">
-        <v>1114</v>
       </c>
       <c r="S102" s="22"/>
       <c r="T102" s="37" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="U102" s="22"/>
       <c r="V102" s="37" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="W102" s="22"/>
       <c r="X102" s="39" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="Y102" s="22"/>
       <c r="Z102" s="22" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="AA102" s="22"/>
       <c r="AB102" s="22" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="AC102" s="22"/>
       <c r="AD102" s="22"/>
@@ -22313,44 +22313,44 @@
       </c>
       <c r="D103" s="22"/>
       <c r="E103" s="22" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="F103" s="22"/>
       <c r="G103" s="22" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="H103" s="23"/>
       <c r="I103" s="23" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="J103" s="22"/>
       <c r="K103" s="37" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="L103" s="37"/>
       <c r="M103" s="37" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="N103" s="22"/>
       <c r="O103" s="37" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="P103" s="22" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="Q103" s="22" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="R103" s="22" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="S103" s="22"/>
       <c r="T103" s="37" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="U103" s="22"/>
       <c r="V103" s="37" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="W103" s="22"/>
       <c r="X103" s="39" t="s">
@@ -22358,11 +22358,11 @@
       </c>
       <c r="Y103" s="22"/>
       <c r="Z103" s="22" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="AA103" s="22"/>
       <c r="AB103" s="22" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="AC103" s="22"/>
       <c r="AD103" s="22"/>
@@ -22379,44 +22379,44 @@
       </c>
       <c r="D104" s="22"/>
       <c r="E104" s="22" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="F104" s="22"/>
       <c r="G104" s="22" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="H104" s="23"/>
       <c r="I104" s="23" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="J104" s="22"/>
       <c r="K104" s="37" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="L104" s="37"/>
       <c r="M104" s="37" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="N104" s="22"/>
       <c r="O104" s="37" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="P104" s="22" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="Q104" s="22" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="R104" s="22" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="S104" s="22"/>
       <c r="T104" s="37" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="U104" s="22"/>
       <c r="V104" s="37" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="W104" s="22"/>
       <c r="X104" s="39" t="s">
@@ -22424,11 +22424,11 @@
       </c>
       <c r="Y104" s="22"/>
       <c r="Z104" s="22" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="AA104" s="22"/>
       <c r="AB104" s="22" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="AC104" s="22"/>
       <c r="AD104" s="22"/>
@@ -22445,44 +22445,44 @@
       </c>
       <c r="D105" s="22"/>
       <c r="E105" s="22" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="F105" s="22"/>
       <c r="G105" s="22" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="H105" s="23"/>
       <c r="I105" s="23" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="J105" s="22"/>
       <c r="K105" s="37" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="L105" s="37"/>
       <c r="M105" s="37" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="N105" s="22"/>
       <c r="O105" s="37" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="P105" s="22" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="Q105" s="22" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="R105" s="22" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="S105" s="22"/>
       <c r="T105" s="37" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="U105" s="22"/>
       <c r="V105" s="37" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="W105" s="22"/>
       <c r="X105" s="39" t="s">
@@ -22490,11 +22490,11 @@
       </c>
       <c r="Y105" s="22"/>
       <c r="Z105" s="22" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="AA105" s="22"/>
       <c r="AB105" s="22" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="AC105" s="22"/>
       <c r="AD105" s="22"/>
@@ -22519,7 +22519,7 @@
       </c>
       <c r="H106" s="23"/>
       <c r="I106" s="23" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="J106" s="22"/>
       <c r="K106" s="37" t="s">
@@ -22527,11 +22527,11 @@
       </c>
       <c r="L106" s="37"/>
       <c r="M106" s="37" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="N106" s="22"/>
       <c r="O106" s="37" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="P106" s="22" t="s">
         <v>413</v>
@@ -22585,7 +22585,7 @@
       </c>
       <c r="H107" s="23"/>
       <c r="I107" s="23" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="J107" s="22"/>
       <c r="K107" s="37" t="s">
@@ -22593,11 +22593,11 @@
       </c>
       <c r="L107" s="37"/>
       <c r="M107" s="37" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="N107" s="22"/>
       <c r="O107" s="37" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="P107" s="22" t="s">
         <v>872</v>
@@ -22651,7 +22651,7 @@
       </c>
       <c r="H108" s="23"/>
       <c r="I108" s="23" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="J108" s="22"/>
       <c r="K108" s="37" t="s">
@@ -22659,11 +22659,11 @@
       </c>
       <c r="L108" s="37"/>
       <c r="M108" s="37" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="N108" s="22"/>
       <c r="O108" s="37" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="P108" s="22" t="s">
         <v>415</v>
@@ -22717,7 +22717,7 @@
       </c>
       <c r="H109" s="23"/>
       <c r="I109" s="23" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="J109" s="22"/>
       <c r="K109" s="37" t="s">
@@ -22725,11 +22725,11 @@
       </c>
       <c r="L109" s="37"/>
       <c r="M109" s="37" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="N109" s="22"/>
       <c r="O109" s="37" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="P109" s="22" t="s">
         <v>416</v>
@@ -22783,7 +22783,7 @@
       </c>
       <c r="H110" s="23"/>
       <c r="I110" s="23" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="J110" s="22"/>
       <c r="K110" s="37" t="s">
@@ -22791,11 +22791,11 @@
       </c>
       <c r="L110" s="37"/>
       <c r="M110" s="37" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="N110" s="22"/>
       <c r="O110" s="37" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="P110" s="22" t="s">
         <v>873</v>
@@ -22849,7 +22849,7 @@
       </c>
       <c r="H111" s="23"/>
       <c r="I111" s="23" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="J111" s="22"/>
       <c r="K111" s="37" t="s">
@@ -22857,11 +22857,11 @@
       </c>
       <c r="L111" s="37"/>
       <c r="M111" s="37" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="N111" s="22"/>
       <c r="O111" s="37" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="P111" s="22" t="s">
         <v>418</v>
@@ -22915,7 +22915,7 @@
       </c>
       <c r="H112" s="23"/>
       <c r="I112" s="23" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="J112" s="22"/>
       <c r="K112" s="37" t="s">
@@ -22923,11 +22923,11 @@
       </c>
       <c r="L112" s="37"/>
       <c r="M112" s="37" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="N112" s="22"/>
       <c r="O112" s="37" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="P112" s="22" t="s">
         <v>419</v>
@@ -22981,7 +22981,7 @@
       </c>
       <c r="H113" s="23"/>
       <c r="I113" s="23" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="J113" s="22"/>
       <c r="K113" s="37" t="s">
@@ -22989,11 +22989,11 @@
       </c>
       <c r="L113" s="37"/>
       <c r="M113" s="37" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="N113" s="22"/>
       <c r="O113" s="37" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="P113" s="22" t="s">
         <v>420</v>
@@ -23047,7 +23047,7 @@
       </c>
       <c r="H114" s="23"/>
       <c r="I114" s="23" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="J114" s="22"/>
       <c r="K114" s="37" t="s">
@@ -23055,11 +23055,11 @@
       </c>
       <c r="L114" s="37"/>
       <c r="M114" s="37" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="N114" s="22"/>
       <c r="O114" s="37" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="P114" s="22" t="s">
         <v>421</v>
@@ -23113,7 +23113,7 @@
       </c>
       <c r="H115" s="23"/>
       <c r="I115" s="23" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="J115" s="22"/>
       <c r="K115" s="37" t="s">
@@ -23121,11 +23121,11 @@
       </c>
       <c r="L115" s="37"/>
       <c r="M115" s="37" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="N115" s="22"/>
       <c r="O115" s="37" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="P115" s="22" t="s">
         <v>422</v>
@@ -23179,7 +23179,7 @@
       </c>
       <c r="H116" s="23"/>
       <c r="I116" s="23" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="J116" s="22"/>
       <c r="K116" s="37" t="s">
@@ -23187,11 +23187,11 @@
       </c>
       <c r="L116" s="37"/>
       <c r="M116" s="37" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="N116" s="22"/>
       <c r="O116" s="37" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="P116" s="22" t="s">
         <v>423</v>
@@ -23233,7 +23233,7 @@
         <v>79</v>
       </c>
       <c r="C117" s="23" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="D117" s="22"/>
       <c r="E117" s="22" t="s">
@@ -23245,7 +23245,7 @@
       </c>
       <c r="H117" s="23"/>
       <c r="I117" s="23" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="J117" s="22"/>
       <c r="K117" s="37" t="s">
@@ -23253,11 +23253,11 @@
       </c>
       <c r="L117" s="37"/>
       <c r="M117" s="37" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="N117" s="22"/>
       <c r="O117" s="37" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="P117" s="22" t="s">
         <v>424</v>
@@ -23299,7 +23299,7 @@
         <v>81</v>
       </c>
       <c r="C118" s="23" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="D118" s="22"/>
       <c r="E118" s="22" t="s">
@@ -23311,7 +23311,7 @@
       </c>
       <c r="H118" s="23"/>
       <c r="I118" s="23" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="J118" s="22"/>
       <c r="K118" s="37" t="s">
@@ -23319,11 +23319,11 @@
       </c>
       <c r="L118" s="37"/>
       <c r="M118" s="37" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="N118" s="22"/>
       <c r="O118" s="37" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="P118" s="22" t="s">
         <v>874</v>
@@ -23365,7 +23365,7 @@
         <v>82</v>
       </c>
       <c r="C119" s="23" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="D119" s="22"/>
       <c r="E119" s="22" t="s">
@@ -23377,7 +23377,7 @@
       </c>
       <c r="H119" s="23"/>
       <c r="I119" s="23" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="J119" s="22"/>
       <c r="K119" s="37" t="s">
@@ -23385,11 +23385,11 @@
       </c>
       <c r="L119" s="37"/>
       <c r="M119" s="37" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="N119" s="22"/>
       <c r="O119" s="37" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="P119" s="22" t="s">
         <v>875</v>
@@ -23443,7 +23443,7 @@
       </c>
       <c r="H120" s="23"/>
       <c r="I120" s="23" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="J120" s="22"/>
       <c r="K120" s="37" t="s">
@@ -23451,11 +23451,11 @@
       </c>
       <c r="L120" s="37"/>
       <c r="M120" s="37" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="N120" s="22"/>
       <c r="O120" s="37" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="P120" s="22" t="s">
         <v>427</v>
@@ -23509,7 +23509,7 @@
       </c>
       <c r="H121" s="24"/>
       <c r="I121" s="24" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="J121" s="25"/>
       <c r="K121" s="37" t="s">
@@ -23517,11 +23517,11 @@
       </c>
       <c r="L121" s="37"/>
       <c r="M121" s="37" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="N121" s="25"/>
       <c r="O121" s="37" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="P121" s="22" t="s">
         <v>876</v>
@@ -23575,7 +23575,7 @@
       </c>
       <c r="H122" s="23"/>
       <c r="I122" s="23" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="J122" s="22"/>
       <c r="K122" s="37" t="s">
@@ -23583,11 +23583,11 @@
       </c>
       <c r="L122" s="37"/>
       <c r="M122" s="37" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="N122" s="22"/>
       <c r="O122" s="37" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="P122" s="22" t="s">
         <v>429</v>
@@ -23641,7 +23641,7 @@
       </c>
       <c r="H123" s="23"/>
       <c r="I123" s="23" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="J123" s="22"/>
       <c r="K123" s="37" t="s">
@@ -23649,11 +23649,11 @@
       </c>
       <c r="L123" s="37"/>
       <c r="M123" s="37" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="N123" s="22"/>
       <c r="O123" s="37" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="P123" s="22" t="s">
         <v>430</v>
@@ -23707,7 +23707,7 @@
       </c>
       <c r="H124" s="23"/>
       <c r="I124" s="23" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="J124" s="22"/>
       <c r="K124" s="37" t="s">
@@ -23715,11 +23715,11 @@
       </c>
       <c r="L124" s="37"/>
       <c r="M124" s="37" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="N124" s="22"/>
       <c r="O124" s="37" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="P124" s="22" t="s">
         <v>431</v>
@@ -23773,7 +23773,7 @@
       </c>
       <c r="H125" s="23"/>
       <c r="I125" s="23" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="J125" s="22"/>
       <c r="K125" s="37" t="s">
@@ -23781,11 +23781,11 @@
       </c>
       <c r="L125" s="37"/>
       <c r="M125" s="37" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="N125" s="22"/>
       <c r="O125" s="37" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="P125" s="22" t="s">
         <v>432</v>
@@ -23839,7 +23839,7 @@
       </c>
       <c r="H126" s="24"/>
       <c r="I126" s="24" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="J126" s="25"/>
       <c r="K126" s="37" t="s">
@@ -23847,11 +23847,11 @@
       </c>
       <c r="L126" s="37"/>
       <c r="M126" s="37" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="N126" s="25"/>
       <c r="O126" s="37" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="P126" s="22" t="s">
         <v>877</v>
@@ -23905,7 +23905,7 @@
       </c>
       <c r="H127" s="23"/>
       <c r="I127" s="23" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="J127" s="22"/>
       <c r="K127" s="37" t="s">
@@ -23913,11 +23913,11 @@
       </c>
       <c r="L127" s="37"/>
       <c r="M127" s="37" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="N127" s="22"/>
       <c r="O127" s="37" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="P127" s="22" t="s">
         <v>878</v>
@@ -23971,7 +23971,7 @@
       </c>
       <c r="H128" s="23"/>
       <c r="I128" s="23" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="J128" s="22"/>
       <c r="K128" s="37" t="s">
@@ -23979,11 +23979,11 @@
       </c>
       <c r="L128" s="37"/>
       <c r="M128" s="37" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="N128" s="22"/>
       <c r="O128" s="37" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="P128" s="22" t="s">
         <v>879</v>
@@ -24008,7 +24008,7 @@
       </c>
       <c r="Y128" s="22"/>
       <c r="Z128" s="22" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="AA128" s="22"/>
       <c r="AB128" s="22" t="s">
@@ -24025,31 +24025,31 @@
         <v>177</v>
       </c>
       <c r="C129" s="23" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D129" s="22"/>
       <c r="E129" s="22" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="F129" s="22"/>
       <c r="G129" s="22" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="H129" s="23"/>
       <c r="I129" s="23" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="J129" s="22"/>
       <c r="K129" s="37" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="L129" s="37"/>
       <c r="M129" s="37" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="N129" s="22"/>
       <c r="O129" s="37" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="P129" s="22" t="s">
         <v>880</v>
@@ -24058,27 +24058,27 @@
         <v>880</v>
       </c>
       <c r="R129" s="22" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="S129" s="22"/>
       <c r="T129" s="37" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="U129" s="22"/>
       <c r="V129" s="37" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="W129" s="22"/>
       <c r="X129" s="39" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="Y129" s="22"/>
       <c r="Z129" s="22" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="AA129" s="22"/>
       <c r="AB129" s="22" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="AC129" s="22"/>
       <c r="AD129" s="22"/>
@@ -24091,19 +24091,19 @@
         <v>384</v>
       </c>
       <c r="C130" s="23" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D130" s="22"/>
       <c r="E130" s="22" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="F130" s="22"/>
       <c r="G130" s="22" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="H130" s="23"/>
       <c r="I130" s="23" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="J130" s="22"/>
       <c r="K130" s="38" t="s">
@@ -24111,40 +24111,40 @@
       </c>
       <c r="L130" s="38"/>
       <c r="M130" s="38" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="N130" s="22"/>
       <c r="O130" s="38" t="s">
+        <v>1364</v>
+      </c>
+      <c r="P130" s="22" t="s">
         <v>1365</v>
       </c>
-      <c r="P130" s="22" t="s">
-        <v>1366</v>
-      </c>
       <c r="Q130" s="22" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="R130" s="22" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="S130" s="22"/>
       <c r="T130" s="38" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="U130" s="22"/>
       <c r="V130" s="38" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="W130" s="22"/>
       <c r="X130" s="40" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="Y130" s="22"/>
       <c r="Z130" s="22" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="AA130" s="22"/>
       <c r="AB130" s="22" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="AC130" s="22"/>
       <c r="AD130" s="22"/>
@@ -24169,7 +24169,7 @@
       </c>
       <c r="H131" s="23"/>
       <c r="I131" s="23" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="J131" s="22"/>
       <c r="K131" s="37" t="s">
@@ -24177,11 +24177,11 @@
       </c>
       <c r="L131" s="37"/>
       <c r="M131" s="37" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="N131" s="22"/>
       <c r="O131" s="37" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="P131" s="22" t="s">
         <v>636</v>
@@ -24642,7 +24642,7 @@
       <c r="M142" s="37"/>
       <c r="N142" s="22"/>
       <c r="O142" s="37" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="P142" s="22"/>
       <c r="Q142" s="22"/>
@@ -24681,7 +24681,7 @@
       <c r="K143" s="37"/>
       <c r="L143" s="37"/>
       <c r="M143" s="37" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="N143" s="22"/>
       <c r="O143" s="37"/>
@@ -24724,7 +24724,7 @@
       <c r="M144" s="37"/>
       <c r="N144" s="22"/>
       <c r="O144" s="37" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="P144" s="22"/>
       <c r="Q144" s="22"/>
@@ -24759,7 +24759,7 @@
       <c r="G145" s="22"/>
       <c r="H145" s="23"/>
       <c r="I145" s="23" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="J145" s="22"/>
       <c r="K145" s="37"/>
@@ -24806,7 +24806,7 @@
       <c r="M146" s="37"/>
       <c r="N146" s="22"/>
       <c r="O146" s="37" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="P146" s="22"/>
       <c r="Q146" s="22"/>

</xml_diff>

<commit_message>
removed parameterised city bracket from walkability plot label
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F494BB9-BB76-4BF6-8248-798833FD3329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89F6744-6E9C-4D78-8E8A-3135285880EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4396,9 +4396,6 @@
     <t>Walkable neighbourhoods provide opportunities for active,  healthy, and sustainable lifestyles. Walkable neighourhoods have sufficient but not excessive population density to support adequate provision of local amenities including public transport services. Walkable neighbourhoods also have mixed land uses and well-connected streets, to ensure proximate and convenient access to destinations. High-quality pedestrian infrastructure and reducing traffic through managing demand for car use can also encourage walking for transport.</t>
   </si>
   <si>
-    <t>Neighbourhood walkability in {city} relative to 25 cities</t>
-  </si>
-  <si>
     <t>Population density in {city}</t>
   </si>
   <si>
@@ -4445,6 +4442,9 @@
   </si>
   <si>
     <t>Healthy and Sustainable City Indicators Report: {city}, {country}</t>
+  </si>
+  <si>
+    <t>Neighbourhood walkability in relative to 25 cities</t>
   </si>
 </sst>
 </file>
@@ -16822,10 +16822,10 @@
   <dimension ref="A1:AD156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C82" sqref="C82"/>
+      <selection pane="bottomRight" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -16890,10 +16890,10 @@
         <v>847</v>
       </c>
       <c r="P1" s="19" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="Q1" s="19" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="R1" s="19" t="s">
         <v>647</v>
@@ -19669,7 +19669,7 @@
         <v>206</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>1430</v>
+        <v>1446</v>
       </c>
       <c r="D63" s="20"/>
       <c r="E63" s="20" t="s">
@@ -19699,7 +19699,7 @@
         <v>854</v>
       </c>
       <c r="Q63" s="22" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="R63" s="20" t="s">
         <v>392</v>
@@ -20422,10 +20422,10 @@
         <v>950</v>
       </c>
       <c r="P74" s="20" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="Q74" s="22" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="R74" s="20" t="s">
         <v>1010</v>
@@ -20488,10 +20488,10 @@
         <v>951</v>
       </c>
       <c r="P75" s="20" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="Q75" s="22" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="R75" s="20" t="s">
         <v>1011</v>
@@ -20527,7 +20527,7 @@
         <v>272</v>
       </c>
       <c r="C76" s="21" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="D76" s="20"/>
       <c r="E76" s="20" t="s">
@@ -20857,7 +20857,7 @@
         <v>42</v>
       </c>
       <c r="C81" s="23" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="D81" s="22"/>
       <c r="E81" s="22" t="s">
@@ -21121,7 +21121,7 @@
         <v>45</v>
       </c>
       <c r="C85" s="23" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="D85" s="22"/>
       <c r="E85" s="22" t="s">
@@ -21187,7 +21187,7 @@
         <v>48</v>
       </c>
       <c r="C86" s="23" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="D86" s="22"/>
       <c r="E86" s="22" t="s">
@@ -22270,10 +22270,10 @@
         <v>1112</v>
       </c>
       <c r="P102" s="22" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="Q102" s="25" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="R102" s="22" t="s">
         <v>1113</v>
@@ -23233,7 +23233,7 @@
         <v>79</v>
       </c>
       <c r="C117" s="23" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="D117" s="22"/>
       <c r="E117" s="22" t="s">
@@ -23299,7 +23299,7 @@
         <v>81</v>
       </c>
       <c r="C118" s="23" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="D118" s="22"/>
       <c r="E118" s="22" t="s">
@@ -23365,7 +23365,7 @@
         <v>82</v>
       </c>
       <c r="C119" s="23" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="D119" s="22"/>
       <c r="E119" s="22" t="s">

</xml_diff>

<commit_message>
minor clean up of spreadsheet formatting
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89F6744-6E9C-4D78-8E8A-3135285880EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F52905-041B-4B9A-A222-D15F343909EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5227,176 +5227,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -16810,7 +16645,7 @@
   </sheetData>
   <autoFilter ref="A1:T174" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A118">
-    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -16822,10 +16657,10 @@
   <dimension ref="A1:AD156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C65" sqref="C65"/>
+      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -25237,76 +25072,12 @@
       <c r="AD156" s="22"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H56:J56 C56 N56">
-    <cfRule type="duplicateValues" dxfId="19" priority="19"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B61">
-    <cfRule type="duplicateValues" dxfId="18" priority="17"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63:C66 H63:J66 N63:N66">
-    <cfRule type="duplicateValues" dxfId="17" priority="15"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H67:J67 C67 N67">
-    <cfRule type="duplicateValues" dxfId="16" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H76:J76 C76 N76">
-    <cfRule type="duplicateValues" dxfId="15" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B57:B60 B62:B76">
-    <cfRule type="duplicateValues" dxfId="14" priority="28"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C60 H57:J60 H62:J62 C62 C68:C75 H68:J75 N68:N75 N62 N57:N60">
-    <cfRule type="duplicateValues" dxfId="13" priority="30"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B103">
-    <cfRule type="duplicateValues" dxfId="12" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B104">
-    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B105">
-    <cfRule type="duplicateValues" dxfId="10" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H61:J61 C61 N61">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B89">
-    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B95">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:AD156">
     <cfRule type="containsBlanks" dxfId="0" priority="31">
       <formula>LEN(TRIM(C1))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B90:B94 B96:B102 B106:B1048576 B77:B88 B1:B56">
-    <cfRule type="duplicateValues" dxfId="6" priority="32"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q71:Q101 Q122:Q125 Q103:Q120 Q1:Q69">
-    <cfRule type="containsBlanks" dxfId="5" priority="5">
-      <formula>LEN(TRIM(Q1))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q70">
-    <cfRule type="containsBlanks" dxfId="4" priority="4">
-      <formula>LEN(TRIM(Q70))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q102">
-    <cfRule type="containsBlanks" dxfId="3" priority="3">
-      <formula>LEN(TRIM(Q102))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q121">
-    <cfRule type="containsBlanks" dxfId="2" priority="2">
-      <formula>LEN(TRIM(Q121))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q126">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(Q126))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed typo in prose
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\global-indicators\analysis\global_scorecards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C19038-1118-4967-A212-2FBB3DFA2B0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC5E39D-D9B9-4855-B07A-D7297F9F222F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
@@ -4432,9 +4432,6 @@
     <t>Please provide a high resolution 'hero image' photo showing a convivial, walkable city steet or public space for this city, ideally in .jpg format with dimensions in the ratio of 1:1 (e.g. 1000px by 1000px)</t>
   </si>
   <si>
-    <t>Urban design and transport policies supporting health and sustinability</t>
-  </si>
-  <si>
     <t>Comparisons with the median values for all cities included in this international study could inform changes needed for local city policies. The maps show the distribution of urban design and transport features across {city}, and identify areas that could benefit the most from interventions to create healthy and sustainable environments.</t>
   </si>
   <si>
@@ -4445,13 +4442,16 @@
   </si>
   <si>
     <t>fonts/dejavu-fonts-ttf-2.37/ttf/DejaVuSansCondensed.ttf</t>
+  </si>
+  <si>
+    <t>Urban design and transport policies supporting health and sustainability</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5572,13 +5572,13 @@
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.140625" customWidth="1"/>
     <col min="16" max="16" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="4" customFormat="1">
+    <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -5640,7 +5640,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>639</v>
       </c>
@@ -5757,7 +5757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>640</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -5870,7 +5870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>242</v>
       </c>
@@ -5928,7 +5928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -5981,7 +5981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>107</v>
       </c>
@@ -6038,7 +6038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -6091,7 +6091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>228</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>228</v>
       </c>
@@ -6201,7 +6201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -6257,7 +6257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>241</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>378</v>
       </c>
@@ -6380,7 +6380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>379</v>
       </c>
@@ -6436,7 +6436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>380</v>
       </c>
@@ -6493,7 +6493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>238</v>
       </c>
@@ -6553,7 +6553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -6613,7 +6613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -6782,7 +6782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>272</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>105</v>
       </c>
@@ -6898,7 +6898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -6957,7 +6957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>273</v>
       </c>
@@ -7016,7 +7016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>106</v>
       </c>
@@ -7073,7 +7073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -7132,7 +7132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -7191,7 +7191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>243</v>
       </c>
@@ -7251,7 +7251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -7311,7 +7311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>275</v>
       </c>
@@ -7373,7 +7373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>274</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -7492,7 +7492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -7548,7 +7548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -7604,7 +7604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -7667,7 +7667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -7730,7 +7730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A37,LEN("policy2_text")+1,1),"_middle")</f>
         <v>policy2_text1_middle</v>
@@ -7794,7 +7794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A38,LEN("policy2_text")+1,1),"_upper")</f>
         <v>policy2_text1_upper</v>
@@ -7858,7 +7858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>59</v>
       </c>
@@ -7918,7 +7918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>60</v>
       </c>
@@ -7981,7 +7981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>61</v>
       </c>
@@ -8044,7 +8044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A42,LEN("policy2_text")+1,1),"_middle")</f>
         <v>policy2_text2_middle</v>
@@ -8108,7 +8108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A43,LEN("policy2_text")+1,1),"_upper")</f>
         <v>policy2_text2_upper</v>
@@ -8172,7 +8172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>63</v>
       </c>
@@ -8232,7 +8232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>64</v>
       </c>
@@ -8295,7 +8295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>65</v>
       </c>
@@ -8358,7 +8358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A47,LEN("policy2_text")+1,1),"_middle")</f>
         <v>policy2_text3_middle</v>
@@ -8422,7 +8422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A48,LEN("policy2_text")+1,1),"_upper")</f>
         <v>policy2_text3_upper</v>
@@ -8486,7 +8486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>67</v>
       </c>
@@ -8546,7 +8546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -8609,7 +8609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:20">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>69</v>
       </c>
@@ -8672,7 +8672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:20">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A52,LEN("policy2_text")+1,1),"_middle")</f>
         <v>policy2_text4_middle</v>
@@ -8736,7 +8736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:20">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A53,LEN("policy2_text")+1,1),"_upper")</f>
         <v>policy2_text4_upper</v>
@@ -8800,7 +8800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:20">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>71</v>
       </c>
@@ -8860,7 +8860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:20">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>72</v>
       </c>
@@ -8923,7 +8923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:20">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>73</v>
       </c>
@@ -8986,7 +8986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:20">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A57,LEN("policy2_text")+1,1),"_middle")</f>
         <v>policy2_text5_middle</v>
@@ -9050,7 +9050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:20">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A58,LEN("policy2_text")+1,1),"_upper")</f>
         <v>policy2_text5_upper</v>
@@ -9114,7 +9114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:20">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>74</v>
       </c>
@@ -9174,7 +9174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:20">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>75</v>
       </c>
@@ -9237,7 +9237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:20">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>76</v>
       </c>
@@ -9300,7 +9300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:20">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A62,LEN("policy2_text")+1,1),"_middle")</f>
         <v>policy2_text6_middle</v>
@@ -9364,7 +9364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:20">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A63,LEN("policy2_text")+1,1),"_upper")</f>
         <v>policy2_text6_upper</v>
@@ -9428,7 +9428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:20">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -9488,7 +9488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:20">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>45</v>
       </c>
@@ -9546,7 +9546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:20">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>85</v>
       </c>
@@ -9606,7 +9606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:20">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>47</v>
       </c>
@@ -9662,7 +9662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:20">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>78</v>
       </c>
@@ -9720,7 +9720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:20">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>231</v>
       </c>
@@ -9780,7 +9780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:20">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>97</v>
       </c>
@@ -9840,7 +9840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:20">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>98</v>
       </c>
@@ -9900,7 +9900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:20">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>99</v>
       </c>
@@ -9960,7 +9960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:20">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>100</v>
       </c>
@@ -10020,7 +10020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:20">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>87</v>
       </c>
@@ -10077,7 +10077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:20">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>88</v>
       </c>
@@ -10134,7 +10134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:20">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>89</v>
       </c>
@@ -10191,7 +10191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:20">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>103</v>
       </c>
@@ -10248,7 +10248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:20">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>108</v>
       </c>
@@ -10308,7 +10308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:20">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>109</v>
       </c>
@@ -10368,7 +10368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:20">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>110</v>
       </c>
@@ -10428,7 +10428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:20">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>111</v>
       </c>
@@ -10488,7 +10488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:20">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>112</v>
       </c>
@@ -10548,7 +10548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:20">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>113</v>
       </c>
@@ -10608,7 +10608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:20">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>114</v>
       </c>
@@ -10668,7 +10668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:20">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>115</v>
       </c>
@@ -10728,7 +10728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:20">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>116</v>
       </c>
@@ -10788,7 +10788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:20">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>117</v>
       </c>
@@ -10848,7 +10848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:20">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>118</v>
       </c>
@@ -10908,7 +10908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:20">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>119</v>
       </c>
@@ -10968,7 +10968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:20">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>120</v>
       </c>
@@ -11028,7 +11028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:20">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>121</v>
       </c>
@@ -11088,7 +11088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:20">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>122</v>
       </c>
@@ -11148,7 +11148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:20">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>123</v>
       </c>
@@ -11208,7 +11208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:20">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>124</v>
       </c>
@@ -11268,7 +11268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:20">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>125</v>
       </c>
@@ -11328,7 +11328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:20">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>126</v>
       </c>
@@ -11388,7 +11388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:20">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>127</v>
       </c>
@@ -11448,7 +11448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:20">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>128</v>
       </c>
@@ -11508,7 +11508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:20">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>129</v>
       </c>
@@ -11568,7 +11568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:20">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>130</v>
       </c>
@@ -11628,7 +11628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:20">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>131</v>
       </c>
@@ -11688,7 +11688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:20">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>132</v>
       </c>
@@ -11748,7 +11748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:20">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>133</v>
       </c>
@@ -11808,7 +11808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:20">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>134</v>
       </c>
@@ -11868,7 +11868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:20">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>135</v>
       </c>
@@ -11928,7 +11928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:20">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>136</v>
       </c>
@@ -11988,7 +11988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:20">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>137</v>
       </c>
@@ -12048,7 +12048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:20">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>138</v>
       </c>
@@ -12108,7 +12108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:20">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>139</v>
       </c>
@@ -12168,7 +12168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:20">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>140</v>
       </c>
@@ -12228,7 +12228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:20">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>141</v>
       </c>
@@ -12288,7 +12288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:20">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>142</v>
       </c>
@@ -12348,7 +12348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:20">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>48</v>
       </c>
@@ -12405,7 +12405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:20">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>49</v>
       </c>
@@ -12460,7 +12460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:20">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>79</v>
       </c>
@@ -12517,7 +12517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:20">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>80</v>
       </c>
@@ -12573,7 +12573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:20">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>312</v>
       </c>
@@ -12633,7 +12633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:20">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>244</v>
       </c>
@@ -12687,7 +12687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:20">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>245</v>
       </c>
@@ -12744,7 +12744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:20">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>81</v>
       </c>
@@ -12800,7 +12800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:20">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>163</v>
       </c>
@@ -12859,7 +12859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:20">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>179</v>
       </c>
@@ -12915,7 +12915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:20">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>172</v>
       </c>
@@ -12974,7 +12974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:20">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>234</v>
       </c>
@@ -13034,7 +13034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:20">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>97</v>
       </c>
@@ -13094,7 +13094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:20">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>98</v>
       </c>
@@ -13154,7 +13154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:20">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>99</v>
       </c>
@@ -13214,7 +13214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:20">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>100</v>
       </c>
@@ -13274,7 +13274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:20">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>87</v>
       </c>
@@ -13331,7 +13331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:20">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>88</v>
       </c>
@@ -13388,7 +13388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:20">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>89</v>
       </c>
@@ -13445,7 +13445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:20">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>103</v>
       </c>
@@ -13501,7 +13501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:20">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>143</v>
       </c>
@@ -13561,7 +13561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:20">
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>144</v>
       </c>
@@ -13621,7 +13621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:20">
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>145</v>
       </c>
@@ -13681,7 +13681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:20">
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>146</v>
       </c>
@@ -13741,7 +13741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:20">
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>147</v>
       </c>
@@ -13801,7 +13801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:20">
+    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>148</v>
       </c>
@@ -13861,7 +13861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:20">
+    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>149</v>
       </c>
@@ -13921,7 +13921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:20">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>150</v>
       </c>
@@ -13981,7 +13981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:20">
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>151</v>
       </c>
@@ -14041,7 +14041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:20">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>152</v>
       </c>
@@ -14101,7 +14101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:20">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>153</v>
       </c>
@@ -14161,7 +14161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:20">
+    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>154</v>
       </c>
@@ -14221,7 +14221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:20">
+    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>155</v>
       </c>
@@ -14281,7 +14281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:20">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>156</v>
       </c>
@@ -14341,7 +14341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:20">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>157</v>
       </c>
@@ -14401,7 +14401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:20">
+    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>158</v>
       </c>
@@ -14461,7 +14461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:20">
+    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>159</v>
       </c>
@@ -14521,7 +14521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:20">
+    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>160</v>
       </c>
@@ -14581,7 +14581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:20">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>161</v>
       </c>
@@ -14641,7 +14641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:20">
+    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>162</v>
       </c>
@@ -14701,7 +14701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:20">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>82</v>
       </c>
@@ -14759,7 +14759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:20">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>174</v>
       </c>
@@ -14818,7 +14818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:20">
+    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>83</v>
       </c>
@@ -14874,7 +14874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:20">
+    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>173</v>
       </c>
@@ -14933,7 +14933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:20">
+    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>235</v>
       </c>
@@ -14992,7 +14992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:20">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>97</v>
       </c>
@@ -15052,7 +15052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:20">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>98</v>
       </c>
@@ -15112,7 +15112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:20">
+    <row r="161" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>99</v>
       </c>
@@ -15172,7 +15172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:20">
+    <row r="162" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>100</v>
       </c>
@@ -15232,7 +15232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:20">
+    <row r="163" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>87</v>
       </c>
@@ -15289,7 +15289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:20">
+    <row r="164" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>88</v>
       </c>
@@ -15346,7 +15346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:20">
+    <row r="165" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>89</v>
       </c>
@@ -15403,7 +15403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:20">
+    <row r="166" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>103</v>
       </c>
@@ -15460,7 +15460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:20">
+    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -15520,7 +15520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:20">
+    <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -15580,7 +15580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:20">
+    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -15640,7 +15640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:20">
+    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -15700,7 +15700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:20">
+    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -15760,7 +15760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:20">
+    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>84</v>
       </c>
@@ -15817,7 +15817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:20">
+    <row r="173" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>41</v>
       </c>
@@ -15870,7 +15870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:20">
+    <row r="174" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>177</v>
       </c>
@@ -15928,7 +15928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:20">
+    <row r="175" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>319</v>
       </c>
@@ -15985,7 +15985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="60">
+    <row r="176" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>313</v>
       </c>
@@ -16047,7 +16047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:20">
+    <row r="177" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>27</v>
       </c>
@@ -16101,7 +16101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:20">
+    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>28</v>
       </c>
@@ -16156,7 +16156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:20">
+    <row r="179" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>29</v>
       </c>
@@ -16210,7 +16210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:20">
+    <row r="180" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>30</v>
       </c>
@@ -16264,7 +16264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:20">
+    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>31</v>
       </c>
@@ -16318,7 +16318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:20">
+    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>32</v>
       </c>
@@ -16372,7 +16372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:20">
+    <row r="183" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>33</v>
       </c>
@@ -16426,7 +16426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:20">
+    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>34</v>
       </c>
@@ -16480,7 +16480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:20">
+    <row r="185" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>35</v>
       </c>
@@ -16534,7 +16534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:20">
+    <row r="186" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>36</v>
       </c>
@@ -16588,7 +16588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:20">
+    <row r="187" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>37</v>
       </c>
@@ -16656,14 +16656,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD156"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D92" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C102" sqref="C102"/>
+      <selection pane="bottomRight" activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="30" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" style="30" customWidth="1"/>
@@ -16678,7 +16678,7 @@
     <col min="29" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="29" customFormat="1">
+    <row r="1" spans="1:30" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>193</v>
       </c>
@@ -16766,7 +16766,7 @@
       <c r="AC1" s="19"/>
       <c r="AD1" s="19"/>
     </row>
-    <row r="2" spans="1:30" s="31" customFormat="1">
+    <row r="2" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>194</v>
       </c>
@@ -16846,7 +16846,7 @@
       <c r="AC2" s="20"/>
       <c r="AD2" s="20"/>
     </row>
-    <row r="3" spans="1:30" ht="15" customHeight="1">
+    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>194</v>
       </c>
@@ -16912,7 +16912,7 @@
       <c r="AC3" s="22"/>
       <c r="AD3" s="22"/>
     </row>
-    <row r="4" spans="1:30" ht="15" customHeight="1">
+    <row r="4" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>194</v>
       </c>
@@ -16978,7 +16978,7 @@
       <c r="AC4" s="22"/>
       <c r="AD4" s="22"/>
     </row>
-    <row r="5" spans="1:30" ht="30">
+    <row r="5" spans="1:30" ht="33" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>194</v>
       </c>
@@ -17044,7 +17044,7 @@
       <c r="AC5" s="22"/>
       <c r="AD5" s="22"/>
     </row>
-    <row r="6" spans="1:30" ht="15" customHeight="1">
+    <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>194</v>
       </c>
@@ -17082,7 +17082,7 @@
       <c r="AC6" s="22"/>
       <c r="AD6" s="22"/>
     </row>
-    <row r="7" spans="1:30" ht="15" customHeight="1">
+    <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>194</v>
       </c>
@@ -17124,7 +17124,7 @@
       <c r="AC7" s="22"/>
       <c r="AD7" s="22"/>
     </row>
-    <row r="8" spans="1:30" ht="15" customHeight="1">
+    <row r="8" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>194</v>
       </c>
@@ -17162,7 +17162,7 @@
       <c r="AC8" s="22"/>
       <c r="AD8" s="22"/>
     </row>
-    <row r="9" spans="1:30" ht="15" customHeight="1">
+    <row r="9" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>194</v>
       </c>
@@ -17200,7 +17200,7 @@
       <c r="AC9" s="22"/>
       <c r="AD9" s="22"/>
     </row>
-    <row r="10" spans="1:30" ht="15" customHeight="1">
+    <row r="10" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>194</v>
       </c>
@@ -17238,7 +17238,7 @@
       <c r="AC10" s="22"/>
       <c r="AD10" s="22"/>
     </row>
-    <row r="11" spans="1:30" ht="15" customHeight="1">
+    <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>194</v>
       </c>
@@ -17278,7 +17278,7 @@
       <c r="AC11" s="22"/>
       <c r="AD11" s="22"/>
     </row>
-    <row r="12" spans="1:30" ht="15" customHeight="1">
+    <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>194</v>
       </c>
@@ -17318,7 +17318,7 @@
       <c r="AC12" s="22"/>
       <c r="AD12" s="22"/>
     </row>
-    <row r="13" spans="1:30" ht="15" customHeight="1">
+    <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>194</v>
       </c>
@@ -17358,7 +17358,7 @@
       <c r="AC13" s="22"/>
       <c r="AD13" s="22"/>
     </row>
-    <row r="14" spans="1:30" ht="15" customHeight="1">
+    <row r="14" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>194</v>
       </c>
@@ -17398,7 +17398,7 @@
       <c r="AC14" s="22"/>
       <c r="AD14" s="22"/>
     </row>
-    <row r="15" spans="1:30" ht="15" customHeight="1">
+    <row r="15" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>194</v>
       </c>
@@ -17438,7 +17438,7 @@
       <c r="AC15" s="22"/>
       <c r="AD15" s="22"/>
     </row>
-    <row r="16" spans="1:30" ht="15" customHeight="1">
+    <row r="16" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>194</v>
       </c>
@@ -17478,7 +17478,7 @@
       <c r="AC16" s="22"/>
       <c r="AD16" s="22"/>
     </row>
-    <row r="17" spans="1:30" ht="15" customHeight="1">
+    <row r="17" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>194</v>
       </c>
@@ -17518,7 +17518,7 @@
       <c r="AC17" s="22"/>
       <c r="AD17" s="22"/>
     </row>
-    <row r="18" spans="1:30" ht="15" customHeight="1">
+    <row r="18" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>194</v>
       </c>
@@ -17558,7 +17558,7 @@
       <c r="AC18" s="22"/>
       <c r="AD18" s="22"/>
     </row>
-    <row r="19" spans="1:30" ht="15" customHeight="1">
+    <row r="19" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>194</v>
       </c>
@@ -17598,7 +17598,7 @@
       <c r="AC19" s="22"/>
       <c r="AD19" s="22"/>
     </row>
-    <row r="20" spans="1:30" ht="15" customHeight="1">
+    <row r="20" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>194</v>
       </c>
@@ -17638,7 +17638,7 @@
       <c r="AC20" s="22"/>
       <c r="AD20" s="22"/>
     </row>
-    <row r="21" spans="1:30" ht="15" customHeight="1">
+    <row r="21" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>194</v>
       </c>
@@ -17678,7 +17678,7 @@
       <c r="AC21" s="22"/>
       <c r="AD21" s="22"/>
     </row>
-    <row r="22" spans="1:30" ht="15" customHeight="1">
+    <row r="22" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>194</v>
       </c>
@@ -17722,7 +17722,7 @@
       <c r="AC22" s="22"/>
       <c r="AD22" s="22"/>
     </row>
-    <row r="23" spans="1:30" ht="15" customHeight="1">
+    <row r="23" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
         <v>194</v>
       </c>
@@ -17766,7 +17766,7 @@
       <c r="AC23" s="22"/>
       <c r="AD23" s="22"/>
     </row>
-    <row r="24" spans="1:30" ht="15" customHeight="1">
+    <row r="24" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
         <v>194</v>
       </c>
@@ -17810,7 +17810,7 @@
       <c r="AC24" s="22"/>
       <c r="AD24" s="22"/>
     </row>
-    <row r="25" spans="1:30" ht="15" customHeight="1">
+    <row r="25" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
         <v>194</v>
       </c>
@@ -17848,7 +17848,7 @@
       <c r="AC25" s="22"/>
       <c r="AD25" s="22"/>
     </row>
-    <row r="26" spans="1:30" ht="15" customHeight="1">
+    <row r="26" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
         <v>194</v>
       </c>
@@ -17888,7 +17888,7 @@
       <c r="AC26" s="22"/>
       <c r="AD26" s="22"/>
     </row>
-    <row r="27" spans="1:30" ht="15" customHeight="1">
+    <row r="27" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
         <v>194</v>
       </c>
@@ -17926,7 +17926,7 @@
       <c r="AC27" s="22"/>
       <c r="AD27" s="22"/>
     </row>
-    <row r="28" spans="1:30" ht="15" customHeight="1">
+    <row r="28" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
         <v>194</v>
       </c>
@@ -17964,7 +17964,7 @@
       <c r="AC28" s="22"/>
       <c r="AD28" s="22"/>
     </row>
-    <row r="29" spans="1:30" ht="15" customHeight="1">
+    <row r="29" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
         <v>194</v>
       </c>
@@ -18002,7 +18002,7 @@
       <c r="AC29" s="22"/>
       <c r="AD29" s="22"/>
     </row>
-    <row r="30" spans="1:30" ht="15" customHeight="1">
+    <row r="30" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
         <v>194</v>
       </c>
@@ -18040,7 +18040,7 @@
       <c r="AC30" s="22"/>
       <c r="AD30" s="22"/>
     </row>
-    <row r="31" spans="1:30" ht="15" customHeight="1">
+    <row r="31" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
         <v>194</v>
       </c>
@@ -18078,7 +18078,7 @@
       <c r="AC31" s="22"/>
       <c r="AD31" s="22"/>
     </row>
-    <row r="32" spans="1:30" ht="15" customHeight="1">
+    <row r="32" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
         <v>194</v>
       </c>
@@ -18120,7 +18120,7 @@
       <c r="AC32" s="22"/>
       <c r="AD32" s="22"/>
     </row>
-    <row r="33" spans="1:30" ht="15" customHeight="1">
+    <row r="33" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
         <v>194</v>
       </c>
@@ -18158,7 +18158,7 @@
       <c r="AC33" s="22"/>
       <c r="AD33" s="22"/>
     </row>
-    <row r="34" spans="1:30" ht="15" customHeight="1">
+    <row r="34" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
         <v>194</v>
       </c>
@@ -18196,7 +18196,7 @@
       <c r="AC34" s="22"/>
       <c r="AD34" s="22"/>
     </row>
-    <row r="35" spans="1:30" ht="15" customHeight="1">
+    <row r="35" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
         <v>194</v>
       </c>
@@ -18234,7 +18234,7 @@
       <c r="AC35" s="22"/>
       <c r="AD35" s="22"/>
     </row>
-    <row r="36" spans="1:30" ht="15" customHeight="1">
+    <row r="36" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
         <v>194</v>
       </c>
@@ -18274,7 +18274,7 @@
       <c r="AC36" s="22"/>
       <c r="AD36" s="22"/>
     </row>
-    <row r="37" spans="1:30" ht="15" customHeight="1">
+    <row r="37" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
         <v>194</v>
       </c>
@@ -18314,7 +18314,7 @@
       <c r="AC37" s="22"/>
       <c r="AD37" s="22"/>
     </row>
-    <row r="38" spans="1:30" ht="15" customHeight="1">
+    <row r="38" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="30" t="s">
         <v>194</v>
       </c>
@@ -18354,7 +18354,7 @@
       <c r="AC38" s="22"/>
       <c r="AD38" s="22"/>
     </row>
-    <row r="39" spans="1:30" ht="15" customHeight="1">
+    <row r="39" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
         <v>194</v>
       </c>
@@ -18394,7 +18394,7 @@
       <c r="AC39" s="22"/>
       <c r="AD39" s="22"/>
     </row>
-    <row r="40" spans="1:30" ht="15" customHeight="1">
+    <row r="40" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="30" t="s">
         <v>194</v>
       </c>
@@ -18434,7 +18434,7 @@
       <c r="AC40" s="22"/>
       <c r="AD40" s="22"/>
     </row>
-    <row r="41" spans="1:30" ht="15" customHeight="1">
+    <row r="41" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="30" t="s">
         <v>194</v>
       </c>
@@ -18474,7 +18474,7 @@
       <c r="AC41" s="22"/>
       <c r="AD41" s="22"/>
     </row>
-    <row r="42" spans="1:30" ht="15" customHeight="1">
+    <row r="42" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
         <v>194</v>
       </c>
@@ -18514,7 +18514,7 @@
       <c r="AC42" s="22"/>
       <c r="AD42" s="22"/>
     </row>
-    <row r="43" spans="1:30" ht="15" customHeight="1">
+    <row r="43" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
         <v>194</v>
       </c>
@@ -18554,7 +18554,7 @@
       <c r="AC43" s="22"/>
       <c r="AD43" s="22"/>
     </row>
-    <row r="44" spans="1:30" ht="15" customHeight="1">
+    <row r="44" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="30" t="s">
         <v>194</v>
       </c>
@@ -18594,7 +18594,7 @@
       <c r="AC44" s="22"/>
       <c r="AD44" s="22"/>
     </row>
-    <row r="45" spans="1:30" ht="15" customHeight="1">
+    <row r="45" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="30" t="s">
         <v>194</v>
       </c>
@@ -18634,7 +18634,7 @@
       <c r="AC45" s="22"/>
       <c r="AD45" s="22"/>
     </row>
-    <row r="46" spans="1:30" ht="15" customHeight="1">
+    <row r="46" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="30" t="s">
         <v>194</v>
       </c>
@@ -18674,7 +18674,7 @@
       <c r="AC46" s="22"/>
       <c r="AD46" s="22"/>
     </row>
-    <row r="47" spans="1:30" ht="15" customHeight="1">
+    <row r="47" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="30" t="s">
         <v>194</v>
       </c>
@@ -18718,7 +18718,7 @@
       <c r="AC47" s="22"/>
       <c r="AD47" s="22"/>
     </row>
-    <row r="48" spans="1:30" ht="15" customHeight="1">
+    <row r="48" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="30" t="s">
         <v>194</v>
       </c>
@@ -18762,7 +18762,7 @@
       <c r="AC48" s="22"/>
       <c r="AD48" s="22"/>
     </row>
-    <row r="49" spans="1:30" ht="15" customHeight="1">
+    <row r="49" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="30" t="s">
         <v>194</v>
       </c>
@@ -18806,7 +18806,7 @@
       <c r="AC49" s="22"/>
       <c r="AD49" s="22"/>
     </row>
-    <row r="50" spans="1:30" ht="15" customHeight="1">
+    <row r="50" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="30" t="s">
         <v>194</v>
       </c>
@@ -18844,7 +18844,7 @@
       <c r="AC50" s="22"/>
       <c r="AD50" s="22"/>
     </row>
-    <row r="51" spans="1:30" ht="15" customHeight="1">
+    <row r="51" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="30" t="s">
         <v>194</v>
       </c>
@@ -18884,7 +18884,7 @@
       <c r="AC51" s="22"/>
       <c r="AD51" s="22"/>
     </row>
-    <row r="52" spans="1:30" ht="15" customHeight="1">
+    <row r="52" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="30" t="s">
         <v>194</v>
       </c>
@@ -18922,7 +18922,7 @@
       <c r="AC52" s="22"/>
       <c r="AD52" s="22"/>
     </row>
-    <row r="53" spans="1:30" ht="15" customHeight="1">
+    <row r="53" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="30" t="s">
         <v>194</v>
       </c>
@@ -18960,7 +18960,7 @@
       <c r="AC53" s="22"/>
       <c r="AD53" s="22"/>
     </row>
-    <row r="54" spans="1:30" ht="15" customHeight="1">
+    <row r="54" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="30" t="s">
         <v>194</v>
       </c>
@@ -18998,7 +18998,7 @@
       <c r="AC54" s="22"/>
       <c r="AD54" s="22"/>
     </row>
-    <row r="55" spans="1:30" ht="15" customHeight="1">
+    <row r="55" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="30" t="s">
         <v>194</v>
       </c>
@@ -19036,7 +19036,7 @@
       <c r="AC55" s="22"/>
       <c r="AD55" s="22"/>
     </row>
-    <row r="56" spans="1:30" s="31" customFormat="1">
+    <row r="56" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="30" t="s">
         <v>195</v>
       </c>
@@ -19100,7 +19100,7 @@
       <c r="AC56" s="20"/>
       <c r="AD56" s="20"/>
     </row>
-    <row r="57" spans="1:30" s="31" customFormat="1">
+    <row r="57" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="30" t="s">
         <v>195</v>
       </c>
@@ -19166,7 +19166,7 @@
       <c r="AC57" s="20"/>
       <c r="AD57" s="20"/>
     </row>
-    <row r="58" spans="1:30" s="31" customFormat="1">
+    <row r="58" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="30" t="s">
         <v>195</v>
       </c>
@@ -19232,7 +19232,7 @@
       <c r="AC58" s="20"/>
       <c r="AD58" s="20"/>
     </row>
-    <row r="59" spans="1:30" s="31" customFormat="1">
+    <row r="59" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="30" t="s">
         <v>195</v>
       </c>
@@ -19298,7 +19298,7 @@
       <c r="AC59" s="20"/>
       <c r="AD59" s="20"/>
     </row>
-    <row r="60" spans="1:30" s="31" customFormat="1">
+    <row r="60" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="30" t="s">
         <v>195</v>
       </c>
@@ -19364,7 +19364,7 @@
       <c r="AC60" s="20"/>
       <c r="AD60" s="20"/>
     </row>
-    <row r="61" spans="1:30" s="31" customFormat="1" ht="30">
+    <row r="61" spans="1:30" s="31" customFormat="1" ht="33" x14ac:dyDescent="0.25">
       <c r="A61" s="30" t="s">
         <v>195</v>
       </c>
@@ -19430,7 +19430,7 @@
       <c r="AC61" s="20"/>
       <c r="AD61" s="20"/>
     </row>
-    <row r="62" spans="1:30" s="31" customFormat="1" ht="42.75">
+    <row r="62" spans="1:30" s="31" customFormat="1" ht="33" x14ac:dyDescent="0.25">
       <c r="A62" s="30" t="s">
         <v>195</v>
       </c>
@@ -19496,7 +19496,7 @@
       <c r="AC62" s="20"/>
       <c r="AD62" s="20"/>
     </row>
-    <row r="63" spans="1:30" s="31" customFormat="1" ht="30">
+    <row r="63" spans="1:30" s="31" customFormat="1" ht="33" x14ac:dyDescent="0.25">
       <c r="A63" s="30" t="s">
         <v>195</v>
       </c>
@@ -19562,7 +19562,7 @@
       <c r="AC63" s="20"/>
       <c r="AD63" s="20"/>
     </row>
-    <row r="64" spans="1:30" s="31" customFormat="1">
+    <row r="64" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="30" t="s">
         <v>195</v>
       </c>
@@ -19628,7 +19628,7 @@
       <c r="AC64" s="20"/>
       <c r="AD64" s="20"/>
     </row>
-    <row r="65" spans="1:30" s="31" customFormat="1">
+    <row r="65" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="30" t="s">
         <v>195</v>
       </c>
@@ -19694,7 +19694,7 @@
       <c r="AC65" s="20"/>
       <c r="AD65" s="20"/>
     </row>
-    <row r="66" spans="1:30" s="31" customFormat="1">
+    <row r="66" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="30" t="s">
         <v>195</v>
       </c>
@@ -19760,7 +19760,7 @@
       <c r="AC66" s="20"/>
       <c r="AD66" s="20"/>
     </row>
-    <row r="67" spans="1:30" s="31" customFormat="1" ht="30">
+    <row r="67" spans="1:30" s="31" customFormat="1" ht="33" x14ac:dyDescent="0.25">
       <c r="A67" s="30" t="s">
         <v>195</v>
       </c>
@@ -19826,7 +19826,7 @@
       <c r="AC67" s="20"/>
       <c r="AD67" s="20"/>
     </row>
-    <row r="68" spans="1:30" s="31" customFormat="1" ht="60">
+    <row r="68" spans="1:30" s="31" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A68" s="30" t="s">
         <v>195</v>
       </c>
@@ -19892,7 +19892,7 @@
       <c r="AC68" s="20"/>
       <c r="AD68" s="20"/>
     </row>
-    <row r="69" spans="1:30" s="31" customFormat="1" ht="57">
+    <row r="69" spans="1:30" s="31" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A69" s="30" t="s">
         <v>195</v>
       </c>
@@ -19958,7 +19958,7 @@
       <c r="AC69" s="20"/>
       <c r="AD69" s="20"/>
     </row>
-    <row r="70" spans="1:30" s="31" customFormat="1" ht="28.5">
+    <row r="70" spans="1:30" s="31" customFormat="1" ht="33" x14ac:dyDescent="0.25">
       <c r="A70" s="30" t="s">
         <v>195</v>
       </c>
@@ -20024,7 +20024,7 @@
       <c r="AC70" s="20"/>
       <c r="AD70" s="20"/>
     </row>
-    <row r="71" spans="1:30" s="31" customFormat="1">
+    <row r="71" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="30" t="s">
         <v>195</v>
       </c>
@@ -20090,7 +20090,7 @@
       <c r="AC71" s="20"/>
       <c r="AD71" s="20"/>
     </row>
-    <row r="72" spans="1:30" s="31" customFormat="1" ht="60">
+    <row r="72" spans="1:30" s="31" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A72" s="30" t="s">
         <v>195</v>
       </c>
@@ -20156,7 +20156,7 @@
       <c r="AC72" s="20"/>
       <c r="AD72" s="20"/>
     </row>
-    <row r="73" spans="1:30" s="31" customFormat="1">
+    <row r="73" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="30" t="s">
         <v>195</v>
       </c>
@@ -20222,7 +20222,7 @@
       <c r="AC73" s="20"/>
       <c r="AD73" s="20"/>
     </row>
-    <row r="74" spans="1:30" s="31" customFormat="1" ht="30">
+    <row r="74" spans="1:30" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="30" t="s">
         <v>195</v>
       </c>
@@ -20288,7 +20288,7 @@
       <c r="AC74" s="20"/>
       <c r="AD74" s="20"/>
     </row>
-    <row r="75" spans="1:30" s="31" customFormat="1" ht="30">
+    <row r="75" spans="1:30" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="30" t="s">
         <v>195</v>
       </c>
@@ -20354,7 +20354,7 @@
       <c r="AC75" s="20"/>
       <c r="AD75" s="20"/>
     </row>
-    <row r="76" spans="1:30" s="31" customFormat="1">
+    <row r="76" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="30" t="s">
         <v>195</v>
       </c>
@@ -20420,7 +20420,7 @@
       <c r="AC76" s="20"/>
       <c r="AD76" s="20"/>
     </row>
-    <row r="77" spans="1:30" ht="15" customHeight="1">
+    <row r="77" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="30" t="s">
         <v>194</v>
       </c>
@@ -20486,7 +20486,7 @@
       <c r="AC77" s="22"/>
       <c r="AD77" s="22"/>
     </row>
-    <row r="78" spans="1:30" ht="15" customHeight="1">
+    <row r="78" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="30" t="s">
         <v>194</v>
       </c>
@@ -20552,7 +20552,7 @@
       <c r="AC78" s="22"/>
       <c r="AD78" s="22"/>
     </row>
-    <row r="79" spans="1:30" ht="15" customHeight="1">
+    <row r="79" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="30" t="s">
         <v>194</v>
       </c>
@@ -20618,7 +20618,7 @@
       <c r="AC79" s="22"/>
       <c r="AD79" s="22"/>
     </row>
-    <row r="80" spans="1:30">
+    <row r="80" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A80" s="30" t="s">
         <v>194</v>
       </c>
@@ -20684,7 +20684,7 @@
       <c r="AC80" s="22"/>
       <c r="AD80" s="22"/>
     </row>
-    <row r="81" spans="1:30" ht="30">
+    <row r="81" spans="1:30" ht="33" x14ac:dyDescent="0.25">
       <c r="A81" s="30" t="s">
         <v>194</v>
       </c>
@@ -20750,7 +20750,7 @@
       <c r="AC81" s="22"/>
       <c r="AD81" s="22"/>
     </row>
-    <row r="82" spans="1:30" ht="238.5" customHeight="1">
+    <row r="82" spans="1:30" ht="238.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="30" t="s">
         <v>194</v>
       </c>
@@ -20816,7 +20816,7 @@
       <c r="AC82" s="22"/>
       <c r="AD82" s="22"/>
     </row>
-    <row r="83" spans="1:30" ht="238.5" customHeight="1">
+    <row r="83" spans="1:30" ht="238.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="30" t="s">
         <v>194</v>
       </c>
@@ -20824,7 +20824,7 @@
         <v>378</v>
       </c>
       <c r="C83" s="23" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="D83" s="22"/>
       <c r="E83" s="22" t="s">
@@ -20882,7 +20882,7 @@
       <c r="AC83" s="22"/>
       <c r="AD83" s="22"/>
     </row>
-    <row r="84" spans="1:30" ht="45">
+    <row r="84" spans="1:30" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A84" s="30" t="s">
         <v>194</v>
       </c>
@@ -20948,7 +20948,7 @@
       <c r="AC84" s="22"/>
       <c r="AD84" s="22"/>
     </row>
-    <row r="85" spans="1:30">
+    <row r="85" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A85" s="30" t="s">
         <v>194</v>
       </c>
@@ -21014,7 +21014,7 @@
       <c r="AC85" s="22"/>
       <c r="AD85" s="22"/>
     </row>
-    <row r="86" spans="1:30">
+    <row r="86" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A86" s="30" t="s">
         <v>194</v>
       </c>
@@ -21080,7 +21080,7 @@
       <c r="AC86" s="22"/>
       <c r="AD86" s="22"/>
     </row>
-    <row r="87" spans="1:30" ht="199.5">
+    <row r="87" spans="1:30" ht="231" x14ac:dyDescent="0.25">
       <c r="A87" s="30" t="s">
         <v>194</v>
       </c>
@@ -21146,7 +21146,7 @@
       <c r="AC87" s="22"/>
       <c r="AD87" s="22"/>
     </row>
-    <row r="88" spans="1:30">
+    <row r="88" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A88" s="30" t="s">
         <v>194</v>
       </c>
@@ -21212,7 +21212,7 @@
       <c r="AC88" s="22"/>
       <c r="AD88" s="22"/>
     </row>
-    <row r="89" spans="1:30" ht="57">
+    <row r="89" spans="1:30" ht="66" x14ac:dyDescent="0.25">
       <c r="A89" s="30" t="s">
         <v>194</v>
       </c>
@@ -21220,7 +21220,7 @@
         <v>272</v>
       </c>
       <c r="C89" s="23" t="s">
-        <v>1442</v>
+        <v>1446</v>
       </c>
       <c r="D89" s="22"/>
       <c r="E89" s="22" t="s">
@@ -21278,7 +21278,7 @@
       <c r="AC89" s="22"/>
       <c r="AD89" s="22"/>
     </row>
-    <row r="90" spans="1:30">
+    <row r="90" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A90" s="30" t="s">
         <v>194</v>
       </c>
@@ -21344,7 +21344,7 @@
       <c r="AC90" s="22"/>
       <c r="AD90" s="22"/>
     </row>
-    <row r="91" spans="1:30" ht="60">
+    <row r="91" spans="1:30" ht="66" x14ac:dyDescent="0.25">
       <c r="A91" s="30" t="s">
         <v>194</v>
       </c>
@@ -21410,7 +21410,7 @@
       <c r="AC91" s="22"/>
       <c r="AD91" s="22"/>
     </row>
-    <row r="92" spans="1:30">
+    <row r="92" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A92" s="30" t="s">
         <v>194</v>
       </c>
@@ -21476,7 +21476,7 @@
       <c r="AC92" s="22"/>
       <c r="AD92" s="22"/>
     </row>
-    <row r="93" spans="1:30" ht="30">
+    <row r="93" spans="1:30" ht="33" x14ac:dyDescent="0.25">
       <c r="A93" s="30" t="s">
         <v>194</v>
       </c>
@@ -21542,7 +21542,7 @@
       <c r="AC93" s="22"/>
       <c r="AD93" s="22"/>
     </row>
-    <row r="94" spans="1:30" ht="30">
+    <row r="94" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="30" t="s">
         <v>194</v>
       </c>
@@ -21608,7 +21608,7 @@
       <c r="AC94" s="22"/>
       <c r="AD94" s="22"/>
     </row>
-    <row r="95" spans="1:30" ht="30">
+    <row r="95" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="30" t="s">
         <v>194</v>
       </c>
@@ -21674,7 +21674,7 @@
       <c r="AC95" s="22"/>
       <c r="AD95" s="22"/>
     </row>
-    <row r="96" spans="1:30" ht="42.75">
+    <row r="96" spans="1:30" ht="33" x14ac:dyDescent="0.25">
       <c r="A96" s="30" t="s">
         <v>194</v>
       </c>
@@ -21740,7 +21740,7 @@
       <c r="AC96" s="22"/>
       <c r="AD96" s="22"/>
     </row>
-    <row r="97" spans="1:30" ht="42.75">
+    <row r="97" spans="1:30" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A97" s="30" t="s">
         <v>194</v>
       </c>
@@ -21806,7 +21806,7 @@
       <c r="AC97" s="22"/>
       <c r="AD97" s="22"/>
     </row>
-    <row r="98" spans="1:30" ht="42.75">
+    <row r="98" spans="1:30" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A98" s="30" t="s">
         <v>194</v>
       </c>
@@ -21872,7 +21872,7 @@
       <c r="AC98" s="22"/>
       <c r="AD98" s="22"/>
     </row>
-    <row r="99" spans="1:30" ht="45">
+    <row r="99" spans="1:30" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A99" s="30" t="s">
         <v>194</v>
       </c>
@@ -21938,7 +21938,7 @@
       <c r="AC99" s="22"/>
       <c r="AD99" s="22"/>
     </row>
-    <row r="100" spans="1:30" ht="30">
+    <row r="100" spans="1:30" ht="33" x14ac:dyDescent="0.25">
       <c r="A100" s="30" t="s">
         <v>194</v>
       </c>
@@ -22004,7 +22004,7 @@
       <c r="AC100" s="22"/>
       <c r="AD100" s="22"/>
     </row>
-    <row r="101" spans="1:30" ht="30">
+    <row r="101" spans="1:30" ht="33" x14ac:dyDescent="0.25">
       <c r="A101" s="30" t="s">
         <v>194</v>
       </c>
@@ -22070,7 +22070,7 @@
       <c r="AC101" s="22"/>
       <c r="AD101" s="22"/>
     </row>
-    <row r="102" spans="1:30" ht="270.75">
+    <row r="102" spans="1:30" ht="280.5" x14ac:dyDescent="0.25">
       <c r="A102" s="30" t="s">
         <v>194</v>
       </c>
@@ -22078,7 +22078,7 @@
         <v>85</v>
       </c>
       <c r="C102" s="24" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="D102" s="22"/>
       <c r="E102" s="22" t="s">
@@ -22136,7 +22136,7 @@
       <c r="AC102" s="22"/>
       <c r="AD102" s="22"/>
     </row>
-    <row r="103" spans="1:30">
+    <row r="103" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A103" s="30" t="s">
         <v>194</v>
       </c>
@@ -22202,7 +22202,7 @@
       <c r="AC103" s="22"/>
       <c r="AD103" s="22"/>
     </row>
-    <row r="104" spans="1:30">
+    <row r="104" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A104" s="30" t="s">
         <v>194</v>
       </c>
@@ -22268,7 +22268,7 @@
       <c r="AC104" s="22"/>
       <c r="AD104" s="22"/>
     </row>
-    <row r="105" spans="1:30">
+    <row r="105" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A105" s="30" t="s">
         <v>194</v>
       </c>
@@ -22334,7 +22334,7 @@
       <c r="AC105" s="22"/>
       <c r="AD105" s="22"/>
     </row>
-    <row r="106" spans="1:30">
+    <row r="106" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A106" s="30" t="s">
         <v>194</v>
       </c>
@@ -22400,7 +22400,7 @@
       <c r="AC106" s="22"/>
       <c r="AD106" s="22"/>
     </row>
-    <row r="107" spans="1:30">
+    <row r="107" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A107" s="30" t="s">
         <v>194</v>
       </c>
@@ -22466,7 +22466,7 @@
       <c r="AC107" s="22"/>
       <c r="AD107" s="22"/>
     </row>
-    <row r="108" spans="1:30">
+    <row r="108" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A108" s="30" t="s">
         <v>194</v>
       </c>
@@ -22532,7 +22532,7 @@
       <c r="AC108" s="22"/>
       <c r="AD108" s="22"/>
     </row>
-    <row r="109" spans="1:30">
+    <row r="109" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A109" s="30" t="s">
         <v>194</v>
       </c>
@@ -22598,7 +22598,7 @@
       <c r="AC109" s="22"/>
       <c r="AD109" s="22"/>
     </row>
-    <row r="110" spans="1:30">
+    <row r="110" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A110" s="30" t="s">
         <v>194</v>
       </c>
@@ -22664,7 +22664,7 @@
       <c r="AC110" s="22"/>
       <c r="AD110" s="22"/>
     </row>
-    <row r="111" spans="1:30">
+    <row r="111" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A111" s="30" t="s">
         <v>194</v>
       </c>
@@ -22730,7 +22730,7 @@
       <c r="AC111" s="22"/>
       <c r="AD111" s="22"/>
     </row>
-    <row r="112" spans="1:30" ht="30">
+    <row r="112" spans="1:30" ht="33" x14ac:dyDescent="0.25">
       <c r="A112" s="30" t="s">
         <v>194</v>
       </c>
@@ -22796,7 +22796,7 @@
       <c r="AC112" s="22"/>
       <c r="AD112" s="22"/>
     </row>
-    <row r="113" spans="1:30">
+    <row r="113" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A113" s="30" t="s">
         <v>194</v>
       </c>
@@ -22862,7 +22862,7 @@
       <c r="AC113" s="22"/>
       <c r="AD113" s="22"/>
     </row>
-    <row r="114" spans="1:30">
+    <row r="114" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A114" s="30" t="s">
         <v>194</v>
       </c>
@@ -22928,7 +22928,7 @@
       <c r="AC114" s="22"/>
       <c r="AD114" s="22"/>
     </row>
-    <row r="115" spans="1:30">
+    <row r="115" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A115" s="30" t="s">
         <v>194</v>
       </c>
@@ -22994,7 +22994,7 @@
       <c r="AC115" s="22"/>
       <c r="AD115" s="22"/>
     </row>
-    <row r="116" spans="1:30">
+    <row r="116" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A116" s="30" t="s">
         <v>194</v>
       </c>
@@ -23060,7 +23060,7 @@
       <c r="AC116" s="22"/>
       <c r="AD116" s="22"/>
     </row>
-    <row r="117" spans="1:30">
+    <row r="117" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A117" s="30" t="s">
         <v>194</v>
       </c>
@@ -23126,7 +23126,7 @@
       <c r="AC117" s="22"/>
       <c r="AD117" s="22"/>
     </row>
-    <row r="118" spans="1:30">
+    <row r="118" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A118" s="30" t="s">
         <v>194</v>
       </c>
@@ -23192,7 +23192,7 @@
       <c r="AC118" s="22"/>
       <c r="AD118" s="22"/>
     </row>
-    <row r="119" spans="1:30">
+    <row r="119" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A119" s="30" t="s">
         <v>194</v>
       </c>
@@ -23258,7 +23258,7 @@
       <c r="AC119" s="22"/>
       <c r="AD119" s="22"/>
     </row>
-    <row r="120" spans="1:30">
+    <row r="120" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A120" s="30" t="s">
         <v>194</v>
       </c>
@@ -23324,7 +23324,7 @@
       <c r="AC120" s="22"/>
       <c r="AD120" s="22"/>
     </row>
-    <row r="121" spans="1:30" ht="270.75">
+    <row r="121" spans="1:30" ht="297" x14ac:dyDescent="0.25">
       <c r="A121" s="30" t="s">
         <v>194</v>
       </c>
@@ -23390,7 +23390,7 @@
       <c r="AC121" s="22"/>
       <c r="AD121" s="22"/>
     </row>
-    <row r="122" spans="1:30" ht="30">
+    <row r="122" spans="1:30" ht="33" x14ac:dyDescent="0.25">
       <c r="A122" s="30" t="s">
         <v>194</v>
       </c>
@@ -23456,7 +23456,7 @@
       <c r="AC122" s="22"/>
       <c r="AD122" s="22"/>
     </row>
-    <row r="123" spans="1:30">
+    <row r="123" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A123" s="30" t="s">
         <v>194</v>
       </c>
@@ -23522,7 +23522,7 @@
       <c r="AC123" s="22"/>
       <c r="AD123" s="22"/>
     </row>
-    <row r="124" spans="1:30" ht="30">
+    <row r="124" spans="1:30" ht="33" x14ac:dyDescent="0.25">
       <c r="A124" s="30" t="s">
         <v>194</v>
       </c>
@@ -23588,7 +23588,7 @@
       <c r="AC124" s="22"/>
       <c r="AD124" s="22"/>
     </row>
-    <row r="125" spans="1:30" ht="30">
+    <row r="125" spans="1:30" ht="33" x14ac:dyDescent="0.25">
       <c r="A125" s="30" t="s">
         <v>194</v>
       </c>
@@ -23654,7 +23654,7 @@
       <c r="AC125" s="22"/>
       <c r="AD125" s="22"/>
     </row>
-    <row r="126" spans="1:30" ht="228">
+    <row r="126" spans="1:30" ht="264" x14ac:dyDescent="0.25">
       <c r="A126" s="30" t="s">
         <v>194</v>
       </c>
@@ -23720,7 +23720,7 @@
       <c r="AC126" s="22"/>
       <c r="AD126" s="22"/>
     </row>
-    <row r="127" spans="1:30" ht="30">
+    <row r="127" spans="1:30" ht="33" x14ac:dyDescent="0.25">
       <c r="A127" s="30" t="s">
         <v>194</v>
       </c>
@@ -23786,7 +23786,7 @@
       <c r="AC127" s="22"/>
       <c r="AD127" s="22"/>
     </row>
-    <row r="128" spans="1:30" ht="327.75">
+    <row r="128" spans="1:30" ht="396" x14ac:dyDescent="0.25">
       <c r="A128" s="30" t="s">
         <v>194</v>
       </c>
@@ -23852,7 +23852,7 @@
       <c r="AC128" s="22"/>
       <c r="AD128" s="22"/>
     </row>
-    <row r="129" spans="1:30" ht="76.5" customHeight="1">
+    <row r="129" spans="1:30" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="30" t="s">
         <v>194</v>
       </c>
@@ -23918,7 +23918,7 @@
       <c r="AC129" s="22"/>
       <c r="AD129" s="22"/>
     </row>
-    <row r="130" spans="1:30" ht="238.5" customHeight="1">
+    <row r="130" spans="1:30" ht="238.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="30" t="s">
         <v>194</v>
       </c>
@@ -23984,7 +23984,7 @@
       <c r="AC130" s="22"/>
       <c r="AD130" s="22"/>
     </row>
-    <row r="131" spans="1:30" ht="238.5" customHeight="1">
+    <row r="131" spans="1:30" ht="238.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="30" t="s">
         <v>194</v>
       </c>
@@ -24050,7 +24050,7 @@
       <c r="AC131" s="22"/>
       <c r="AD131" s="22"/>
     </row>
-    <row r="132" spans="1:30" ht="30">
+    <row r="132" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="30" t="s">
         <v>194</v>
       </c>
@@ -24089,7 +24089,7 @@
       <c r="AC132" s="22"/>
       <c r="AD132" s="22"/>
     </row>
-    <row r="133" spans="1:30" ht="30">
+    <row r="133" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="30" t="s">
         <v>194</v>
       </c>
@@ -24132,7 +24132,7 @@
       <c r="AC133" s="22"/>
       <c r="AD133" s="22"/>
     </row>
-    <row r="134" spans="1:30" ht="30">
+    <row r="134" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="30" t="s">
         <v>194</v>
       </c>
@@ -24171,7 +24171,7 @@
       <c r="AC134" s="22"/>
       <c r="AD134" s="22"/>
     </row>
-    <row r="135" spans="1:30" ht="30">
+    <row r="135" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="30" t="s">
         <v>194</v>
       </c>
@@ -24210,7 +24210,7 @@
       <c r="AC135" s="22"/>
       <c r="AD135" s="22"/>
     </row>
-    <row r="136" spans="1:30" ht="30">
+    <row r="136" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="30" t="s">
         <v>194</v>
       </c>
@@ -24249,7 +24249,7 @@
       <c r="AC136" s="22"/>
       <c r="AD136" s="22"/>
     </row>
-    <row r="137" spans="1:30" ht="30">
+    <row r="137" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="30" t="s">
         <v>194</v>
       </c>
@@ -24290,7 +24290,7 @@
       <c r="AC137" s="22"/>
       <c r="AD137" s="22"/>
     </row>
-    <row r="138" spans="1:30" ht="30">
+    <row r="138" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="30" t="s">
         <v>194</v>
       </c>
@@ -24331,7 +24331,7 @@
       <c r="AC138" s="22"/>
       <c r="AD138" s="22"/>
     </row>
-    <row r="139" spans="1:30" ht="42.75">
+    <row r="139" spans="1:30" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A139" s="30" t="s">
         <v>194</v>
       </c>
@@ -24372,7 +24372,7 @@
       <c r="AC139" s="22"/>
       <c r="AD139" s="22"/>
     </row>
-    <row r="140" spans="1:30" ht="30">
+    <row r="140" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="30" t="s">
         <v>194</v>
       </c>
@@ -24413,7 +24413,7 @@
       <c r="AC140" s="22"/>
       <c r="AD140" s="22"/>
     </row>
-    <row r="141" spans="1:30" ht="30">
+    <row r="141" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="30" t="s">
         <v>194</v>
       </c>
@@ -24454,7 +24454,7 @@
       <c r="AC141" s="22"/>
       <c r="AD141" s="22"/>
     </row>
-    <row r="142" spans="1:30" ht="30">
+    <row r="142" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" s="30" t="s">
         <v>194</v>
       </c>
@@ -24495,7 +24495,7 @@
       <c r="AC142" s="22"/>
       <c r="AD142" s="22"/>
     </row>
-    <row r="143" spans="1:30" ht="30">
+    <row r="143" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="30" t="s">
         <v>194</v>
       </c>
@@ -24536,7 +24536,7 @@
       <c r="AC143" s="22"/>
       <c r="AD143" s="22"/>
     </row>
-    <row r="144" spans="1:30" ht="30">
+    <row r="144" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="30" t="s">
         <v>194</v>
       </c>
@@ -24577,7 +24577,7 @@
       <c r="AC144" s="22"/>
       <c r="AD144" s="22"/>
     </row>
-    <row r="145" spans="1:30" ht="30">
+    <row r="145" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="30" t="s">
         <v>194</v>
       </c>
@@ -24618,7 +24618,7 @@
       <c r="AC145" s="22"/>
       <c r="AD145" s="22"/>
     </row>
-    <row r="146" spans="1:30" ht="30">
+    <row r="146" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="30" t="s">
         <v>194</v>
       </c>
@@ -24659,7 +24659,7 @@
       <c r="AC146" s="22"/>
       <c r="AD146" s="22"/>
     </row>
-    <row r="147" spans="1:30" ht="30">
+    <row r="147" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="30" t="s">
         <v>194</v>
       </c>
@@ -24700,7 +24700,7 @@
       <c r="AC147" s="22"/>
       <c r="AD147" s="22"/>
     </row>
-    <row r="148" spans="1:30" ht="30">
+    <row r="148" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="30" t="s">
         <v>194</v>
       </c>
@@ -24745,7 +24745,7 @@
       <c r="AC148" s="22"/>
       <c r="AD148" s="22"/>
     </row>
-    <row r="149" spans="1:30" ht="30">
+    <row r="149" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="30" t="s">
         <v>194</v>
       </c>
@@ -24790,7 +24790,7 @@
       <c r="AC149" s="22"/>
       <c r="AD149" s="22"/>
     </row>
-    <row r="150" spans="1:30" ht="30">
+    <row r="150" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="30" t="s">
         <v>194</v>
       </c>
@@ -24835,7 +24835,7 @@
       <c r="AC150" s="22"/>
       <c r="AD150" s="22"/>
     </row>
-    <row r="151" spans="1:30" ht="30">
+    <row r="151" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="30" t="s">
         <v>194</v>
       </c>
@@ -24874,7 +24874,7 @@
       <c r="AC151" s="22"/>
       <c r="AD151" s="22"/>
     </row>
-    <row r="152" spans="1:30" ht="30">
+    <row r="152" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="30" t="s">
         <v>194</v>
       </c>
@@ -24915,7 +24915,7 @@
       <c r="AC152" s="22"/>
       <c r="AD152" s="22"/>
     </row>
-    <row r="153" spans="1:30" ht="30">
+    <row r="153" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="30" t="s">
         <v>194</v>
       </c>
@@ -24954,7 +24954,7 @@
       <c r="AC153" s="22"/>
       <c r="AD153" s="22"/>
     </row>
-    <row r="154" spans="1:30" ht="105">
+    <row r="154" spans="1:30" ht="105" x14ac:dyDescent="0.25">
       <c r="A154" s="30" t="s">
         <v>194</v>
       </c>
@@ -24993,7 +24993,7 @@
       <c r="AC154" s="22"/>
       <c r="AD154" s="22"/>
     </row>
-    <row r="155" spans="1:30" ht="30">
+    <row r="155" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="30" t="s">
         <v>194</v>
       </c>
@@ -25032,7 +25032,7 @@
       <c r="AC155" s="22"/>
       <c r="AD155" s="22"/>
     </row>
-    <row r="156" spans="1:30" ht="30">
+    <row r="156" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="30" t="s">
         <v>194</v>
       </c>
@@ -25089,11 +25089,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
@@ -25102,7 +25102,7 @@
     <col min="6" max="6" width="78.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>184</v>
       </c>
@@ -25122,7 +25122,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>637</v>
       </c>
@@ -25133,13 +25133,13 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="F2" t="s">
         <v>895</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>637</v>
       </c>
@@ -25159,7 +25159,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>637</v>
       </c>
@@ -25179,7 +25179,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>637</v>
       </c>
@@ -25199,7 +25199,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>566</v>
       </c>
@@ -25216,7 +25216,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>566</v>
       </c>
@@ -25236,7 +25236,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>566</v>
       </c>
@@ -25256,7 +25256,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>566</v>
       </c>
@@ -25276,7 +25276,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>217</v>
       </c>
@@ -25293,7 +25293,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>217</v>
       </c>
@@ -25313,7 +25313,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>217</v>
       </c>
@@ -25333,7 +25333,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -25353,7 +25353,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>291</v>
       </c>
@@ -25361,7 +25361,7 @@
         <v>226</v>
       </c>
       <c r="C14" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="E14" t="s">
         <v>894</v>
@@ -25370,7 +25370,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>291</v>
       </c>
@@ -25378,7 +25378,7 @@
         <v>226</v>
       </c>
       <c r="C15" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="D15" t="s">
         <v>38</v>
@@ -25390,7 +25390,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>291</v>
       </c>
@@ -25398,7 +25398,7 @@
         <v>226</v>
       </c>
       <c r="C16" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
@@ -25410,7 +25410,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>291</v>
       </c>
@@ -25418,7 +25418,7 @@
         <v>226</v>
       </c>
       <c r="C17" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="D17" t="s">
         <v>188</v>
@@ -25444,13 +25444,13 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" customWidth="1"/>
     <col min="2" max="17" width="11.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="5" customFormat="1" ht="45">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="15" t="s">
         <v>302</v>
@@ -25501,7 +25501,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75">
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>247</v>
       </c>
@@ -25524,7 +25524,7 @@
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75">
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>248</v>
       </c>
@@ -25547,7 +25547,7 @@
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75">
+    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>249</v>
       </c>
@@ -25570,7 +25570,7 @@
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:17" ht="15.75">
+    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>265</v>
       </c>
@@ -25593,7 +25593,7 @@
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
     </row>
-    <row r="6" spans="1:17" ht="15.75">
+    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>237</v>
       </c>
@@ -25616,7 +25616,7 @@
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
     </row>
-    <row r="7" spans="1:17" ht="15.75">
+    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>266</v>
       </c>
@@ -25639,7 +25639,7 @@
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
     </row>
-    <row r="8" spans="1:17" ht="15.75">
+    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>267</v>
       </c>
@@ -25664,7 +25664,7 @@
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
     </row>
-    <row r="9" spans="1:17" ht="15.75">
+    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>256</v>
       </c>
@@ -25691,7 +25691,7 @@
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
     </row>
-    <row r="10" spans="1:17" ht="15.75">
+    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>259</v>
       </c>
@@ -25716,7 +25716,7 @@
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
     </row>
-    <row r="11" spans="1:17" ht="15.75">
+    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>254</v>
       </c>
@@ -25741,7 +25741,7 @@
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
     </row>
-    <row r="12" spans="1:17" ht="15.75">
+    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>258</v>
       </c>
@@ -25766,7 +25766,7 @@
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
     </row>
-    <row r="13" spans="1:17" ht="15.75">
+    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>255</v>
       </c>
@@ -25791,7 +25791,7 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
     </row>
-    <row r="14" spans="1:17" ht="15.75">
+    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>263</v>
       </c>
@@ -25816,7 +25816,7 @@
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
     </row>
-    <row r="15" spans="1:17" ht="15.75">
+    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>260</v>
       </c>
@@ -25843,7 +25843,7 @@
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
     </row>
-    <row r="16" spans="1:17" ht="15.75">
+    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>261</v>
       </c>
@@ -25870,7 +25870,7 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
     </row>
-    <row r="17" spans="1:17" ht="15.75">
+    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>262</v>
       </c>
@@ -25895,7 +25895,7 @@
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
     </row>
-    <row r="18" spans="1:17" ht="15.75">
+    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>264</v>
       </c>
@@ -25920,7 +25920,7 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>257</v>
       </c>
@@ -25947,7 +25947,7 @@
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
     </row>
-    <row r="20" spans="1:17" ht="15.75">
+    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>251</v>
       </c>
@@ -25972,7 +25972,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="1:17" ht="15.75">
+    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>240</v>
       </c>
@@ -25997,7 +25997,7 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
     </row>
-    <row r="22" spans="1:17" ht="15.75">
+    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>250</v>
       </c>
@@ -26022,7 +26022,7 @@
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
     </row>
-    <row r="23" spans="1:17" ht="15.75">
+    <row r="23" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>239</v>
       </c>
@@ -26047,7 +26047,7 @@
       </c>
       <c r="Q23" s="7"/>
     </row>
-    <row r="24" spans="1:17" ht="15.75">
+    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>253</v>
       </c>
@@ -26072,7 +26072,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="15.75">
+    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>246</v>
       </c>
@@ -26097,7 +26097,7 @@
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
     </row>
-    <row r="26" spans="1:17" ht="15.75">
+    <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>252</v>
       </c>

</xml_diff>

<commit_message>
amended Policy presence scoring, with half marks for national/sub-national presence each
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06134FD6-7394-45E8-9DB1-CE28D28220A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E955DE6E-AA8D-4F44-8DD9-72F40F274D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16657,10 +16657,10 @@
   <dimension ref="A1:AD156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D109" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C122" sqref="C122"/>
+      <selection pane="bottomRight" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
corrected scaling of policy presence rating bar, which was impeded due to over-large xtick label; this was effectively an axis title however, so replaced it with this so it was just set centered, and so didn't overflow.  (problem solved!)
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E955DE6E-AA8D-4F44-8DD9-72F40F274D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E580FA-39C5-4EA6-9EAD-D254A9C079CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16660,7 +16660,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F65" sqref="F65"/>
+      <selection pane="bottomRight" activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated Maiduguri summary, and corrected some typos
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9A3F75-5548-4E84-81DF-B39D08452CD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89A987D-FC34-4740-9C6F-3DFAF496AAA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17970" yWindow="4920" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17970" yWindow="5685" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
@@ -3504,10 +3504,6 @@
     <t>(above) {:.1f}% of population meet minimum threshold* for neighbourhood population density ({:,} {})</t>
   </si>
   <si>
-    <t xml:space="preserve">While the availability and quality of urban and transport policies and neighbourhood infrastructure supporting health and sustainability in Maiduguri was found to be well below average compared with other cities,  data availability for Maiduguri was limited and this may partially explain our findings. Although Maiduguri has an air pollution policy related to land use, it appears to lack city planning requirements that include other specific health-focussed actions, and specific and measureable standards to create walkable neighbourhoods and equitable access to public transport and public open space. Relative to the 25 cities in this international study, the majority of neighbourhoods in Maiduguri do not appear to be walkable, and any walkable neighbourhoods appear to be spatially patterned along major road networks. In terms of thresholds for built environment interventions to achieve WHO targets to increase physical activity, 95.9% of residents in Maiduguri live in neighbourhoods that meet the density threshold, although only 29% live in neighbourhoods that meet street connectivity thresholds. The latter could reflect lack of data that on informal routes. Notably, many Maiduguri residents may live in neighbourhoods that exceed levels of density and street connectivity that encourage physical activity. Only 10% of residents have access to public transport stops, with evidence that access is spatially patterned along major road networks. Very few residents have access to public open space within 500m, and only 0.5% of residents have access to larger public open space, concentrated in the city's northeast.
-</t>
-  </si>
-  <si>
     <t>The availability  of policies supporting health and sustainability in Baltimore is below average, and the quality of those available is well below average compared with other cities. Baltimore  does not appear to require health impact assessment of transport and land use interventions,  and has few specific and measureable public transport and public open space policies.   Apart from the inner city,  the majority of neighbourhoods in  Baltimore have low walkability relative to the 25 cities in this international study.   Less than one third of neighbourhoods meet minimum density thresholds to achieve WHO targets to increase physical activity, and only half meet street connectivity thresholds.  A minority of residents have access to public transport stops with regular services with 500m.  While just over half have public open space within 500m, only around 40 percent have access to larger public open space. The percentage of Baltimore's population with access within 500m to a food market, convenience store, any public open space or a larger open space and public transport is well below average compared with other cities studied.</t>
   </si>
   <si>
@@ -4633,12 +4629,6 @@
     <t>No geral, a disponibilidade e a qualidade das políticas urbanas e de transporte que apoiam a saúde e a sustentabilidade em Auckland estão abaixo da média em comparação com outras cidades. Auckland não parece ter políticas de planejamento de transportes incorporando ações focadas em saúde ou gestão da poluição do ar; nem requisitos para avaliação de impacto na saúde ou densidade habitacional e padrões de conectividade de rua.  Em relação às 25 cidades deste estudo internacional, a maioria dos bairros de Auckland tem baixa caminhabilidade.  Apenas um em cada cinco bairros atende a densidade e limites de conectividade de rua para atingir metas da OMS para aumentar a atividade física. Apenas 56% dos moradores têm acesso a paradas de transporte público com serviços regulares.  A maioria dos moradores tem algum espaço público aberto dentro de 500m, embora isso caia para dois terços tendo acesso a maior espaço público aberto.   Em comparação com outras cidades estudadas, o percentual da população com acesso a um mercado de alimentos ou paradas de transporte público com serviço regular é ligeiramente abaixo da média.</t>
   </si>
   <si>
-    <t>(acima) {:.1f}% da população cumpre o limiar mínimo* para a densidade populacional do bairro ({:}} {}}</t>
-  </si>
-  <si>
-    <t>(acima) {:.1f}% da população cumpre o limiar mínimo* para a densidade de intersecção de rua do bairro ({:}} {}}</t>
-  </si>
-  <si>
     <t>(acima) {:.1f}% da população vive em bairros com pontuações de walkability superiores às 25 medianas da cidade internacional</t>
   </si>
   <si>
@@ -4757,15 +4747,6 @@
   </si>
   <si>
     <t>25 நகரங்களுக்கு ஒப்பிடுகையில் அண்டை நடைபயிற்சி</t>
-  </si>
-  <si>
-    <t>(மேலே) {:.1எஃப்}% மக்கள் தொகை, அக்கம்பக்க மக்கள்தொகை அடர்த்திக்கான குறைந்தபட்ச வரம்பு* ({:,} {})</t>
-  </si>
-  <si>
-    <t>(மேலே) {:.1எஃப்}% மக்கள் தொகை, அக்கம்பக்க தெரு வெட்டு அடர்த்திக்கான குறைந்தபட்ச வரம்பு* ({:,} {})</t>
-  </si>
-  <si>
-    <t>(மேலே) {:.1எஃப்}% மக்கள் 25 சர்வதேச நகர சராசரியை விட அதிகமான நடைத்திறன் மதிப்பெண்களுடன் சுற்றுப்புறங்களில் வாழ்கின்றனர்</t>
   </si>
   <si>
     <t>சர்வதேச அளவில் 25 நகரங்களுக்கான சராசரி மதிப்பெண்</t>
@@ -5754,6 +5735,24 @@
   </si>
   <si>
     <t>The availability and quality of urban and transport policies supporting health and sustainability in Mexico City is just below average compared with other cities. Mexico City does not appear to have specific health-focussed actions in its metropolitan transport policy nor requirements for health impact assessment for urban or transport interventions.  It also lacks air pollution policies related to land use.  Many available policy standards lack specificity, measurability and/or consistency with health evidence. Nonetheless, relative to the 25 cities in this international study, the majority of neighbourhoods in Mexico City are walkable.  In terms of thresholds for built environment interventions to achieve WHO targets to increase physical activity, 98.1% of residents in Mexico City live in neighbourhoods that meet the minimum density threshold and 77% meet the street connectivity threshold.  However, notably many residents in Mexico City live in neighbourhoods that may exceed levels of density and street connectivity that encourage physical activity.  Only 20% of residents have access to public transport stops with regular services, with evidence that access is spatially patterned favouring the inner city.  Only 50% of residents have access to some public open space within 500m, and even fewer (20%) have access to larger public open space.  The proportion of the population with access within 500m to amenities is below average compared with other cities studied.</t>
+  </si>
+  <si>
+    <t>(acima) {:.1f}% da população cumpre o limiar mínimo* para a densidade populacional do bairro ({:,} {})</t>
+  </si>
+  <si>
+    <t>(acima) {:.1f}% da população cumpre o limiar mínimo* para a densidade de intersecção de rua do bairro ({:,} {})</t>
+  </si>
+  <si>
+    <t>While the availability and quality of urban and transport policies and neighbourhood infrastructure supporting health and sustainability in Maiduguri was found to be well below average compared with other cities,  data availability for Maiduguri was limited and this may partially explain our findings. Although Maiduguri has an air pollution policy related to land use, it appears to lack city planning requirements that include other specific health-focussed actions, and specific and measureable standards to create walkable neighbourhoods and equitable access to public transport and public open space. Relative to the 25 cities in this international study, the majority of neighbourhoods in Maiduguri were found to lack access to amenities and infrastructure which support walkability.  Walkable neighbourhoods appear to be spatially patterned along major road networks. In terms of thresholds for built environment interventions to achieve WHO targets to increase physical activity, 95.9% of residents in Maiduguri live in neighbourhoods that meet the density threshold, although only 29% live in neighbourhoods that meet street connectivity thresholds. The latter could reflect lack of data that on informal routes. Notably, many Maiduguri residents may live in neighbourhoods that exceed levels of density and street connectivity that encourage physical activity. Only 10% of residents have access to public transport stops, with evidence that access is spatially patterned along major road networks. Very few residents have access to public open space within 500m, and only 0.5% of residents have access to larger public open space, concentrated in the city's northeast.</t>
+  </si>
+  <si>
+    <t>(மேலே) {:.1f}% மக்கள் 25 சர்வதேச நகர சராசரியை விட அதிகமான நடைத்திறன் மதிப்பெண்களுடன் சுற்றுப்புறங்களில் வாழ்கின்றனர்</t>
+  </si>
+  <si>
+    <t>(மேலே) {:.1f}% மக்கள் தொகை, அக்கம்பக்க மக்கள்தொகை அடர்த்திக்கான குறைந்தபட்ச வரம்பு* ({:,} {})</t>
+  </si>
+  <si>
+    <t>(மேலே) {:.1f}% மக்கள் தொகை, அக்கம்பக்க தெரு வெட்டு அடர்த்திக்கான குறைந்தபட்ச வரம்பு* ({:,} {})</t>
   </si>
 </sst>
 </file>
@@ -18233,10 +18232,10 @@
   <dimension ref="A1:AG157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="R134" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AA69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C135" sqref="C135"/>
+      <selection pane="bottomRight" activeCell="AA81" sqref="AA81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18302,7 +18301,7 @@
         <v>289</v>
       </c>
       <c r="R1" s="19" t="s">
-        <v>1719</v>
+        <v>1713</v>
       </c>
       <c r="S1" s="19" t="s">
         <v>1110</v>
@@ -18391,7 +18390,7 @@
       <c r="P2" s="20"/>
       <c r="Q2" s="20"/>
       <c r="R2" s="20" t="s">
-        <v>1844</v>
+        <v>1838</v>
       </c>
       <c r="S2" s="20" t="s">
         <v>725</v>
@@ -18447,7 +18446,7 @@
       </c>
       <c r="F3" s="22"/>
       <c r="G3" s="22" t="s">
-        <v>1873</v>
+        <v>1867</v>
       </c>
       <c r="H3" s="23"/>
       <c r="I3" s="23" t="s">
@@ -18468,7 +18467,7 @@
       <c r="P3" s="37"/>
       <c r="Q3" s="37"/>
       <c r="R3" s="37" t="s">
-        <v>1720</v>
+        <v>1714</v>
       </c>
       <c r="S3" s="22" t="s">
         <v>834</v>
@@ -18497,7 +18496,7 @@
       </c>
       <c r="AD3" s="22"/>
       <c r="AE3" s="22" t="s">
-        <v>1639</v>
+        <v>1633</v>
       </c>
       <c r="AF3" s="22"/>
       <c r="AG3" s="22"/>
@@ -18539,7 +18538,7 @@
       <c r="P4" s="37"/>
       <c r="Q4" s="37"/>
       <c r="R4" s="37" t="s">
-        <v>1721</v>
+        <v>1715</v>
       </c>
       <c r="S4" s="22" t="s">
         <v>835</v>
@@ -18610,7 +18609,7 @@
       <c r="P5" s="37"/>
       <c r="Q5" s="37"/>
       <c r="R5" s="37" t="s">
-        <v>1722</v>
+        <v>1716</v>
       </c>
       <c r="S5" s="22" t="s">
         <v>726</v>
@@ -18639,7 +18638,7 @@
       </c>
       <c r="AD5" s="22"/>
       <c r="AE5" s="22" t="s">
-        <v>1640</v>
+        <v>1634</v>
       </c>
       <c r="AF5" s="22"/>
       <c r="AG5" s="22"/>
@@ -19699,7 +19698,7 @@
       <c r="P30" s="37"/>
       <c r="Q30" s="37"/>
       <c r="R30" s="37" t="s">
-        <v>1701</v>
+        <v>1695</v>
       </c>
       <c r="S30" s="22"/>
       <c r="T30" s="22"/>
@@ -20772,7 +20771,7 @@
       <c r="P55" s="37"/>
       <c r="Q55" s="37"/>
       <c r="R55" s="37" t="s">
-        <v>1702</v>
+        <v>1696</v>
       </c>
       <c r="S55" s="22"/>
       <c r="T55" s="22"/>
@@ -20806,7 +20805,7 @@
       </c>
       <c r="F56" s="20"/>
       <c r="G56" s="20" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="H56" s="21"/>
       <c r="I56" s="21" t="s">
@@ -20827,7 +20826,7 @@
       <c r="P56" s="37"/>
       <c r="Q56" s="37"/>
       <c r="R56" s="37" t="s">
-        <v>1882</v>
+        <v>1876</v>
       </c>
       <c r="S56" s="20" t="s">
         <v>727</v>
@@ -20898,7 +20897,7 @@
       <c r="P57" s="37"/>
       <c r="Q57" s="37"/>
       <c r="R57" s="37" t="s">
-        <v>1723</v>
+        <v>1717</v>
       </c>
       <c r="S57" s="20" t="s">
         <v>728</v>
@@ -20969,7 +20968,7 @@
       <c r="P58" s="37"/>
       <c r="Q58" s="37"/>
       <c r="R58" s="37" t="s">
-        <v>1724</v>
+        <v>1718</v>
       </c>
       <c r="S58" s="20" t="s">
         <v>368</v>
@@ -21040,7 +21039,7 @@
       <c r="P59" s="37"/>
       <c r="Q59" s="37"/>
       <c r="R59" s="37" t="s">
-        <v>1725</v>
+        <v>1719</v>
       </c>
       <c r="S59" s="20" t="s">
         <v>729</v>
@@ -21111,7 +21110,7 @@
       <c r="P60" s="37"/>
       <c r="Q60" s="37"/>
       <c r="R60" s="37" t="s">
-        <v>1726</v>
+        <v>1720</v>
       </c>
       <c r="S60" s="20" t="s">
         <v>370</v>
@@ -21182,7 +21181,7 @@
       <c r="P61" s="37"/>
       <c r="Q61" s="37"/>
       <c r="R61" s="37" t="s">
-        <v>1727</v>
+        <v>1721</v>
       </c>
       <c r="S61" s="20" t="s">
         <v>371</v>
@@ -21253,7 +21252,7 @@
       <c r="P62" s="37"/>
       <c r="Q62" s="37"/>
       <c r="R62" s="37" t="s">
-        <v>1728</v>
+        <v>1722</v>
       </c>
       <c r="S62" s="20" t="s">
         <v>372</v>
@@ -21303,7 +21302,7 @@
       </c>
       <c r="F63" s="20"/>
       <c r="G63" s="20" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="H63" s="21"/>
       <c r="I63" s="21" t="s">
@@ -21315,16 +21314,16 @@
       </c>
       <c r="L63" s="37"/>
       <c r="M63" s="37" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="N63" s="20"/>
       <c r="O63" s="37" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="P63" s="37"/>
       <c r="Q63" s="37"/>
       <c r="R63" s="37" t="s">
-        <v>1729</v>
+        <v>1723</v>
       </c>
       <c r="S63" s="20" t="s">
         <v>730</v>
@@ -21333,11 +21332,11 @@
         <v>1111</v>
       </c>
       <c r="U63" s="20" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="V63" s="20"/>
       <c r="W63" s="37" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="X63" s="20"/>
       <c r="Y63" s="37" t="s">
@@ -21345,11 +21344,11 @@
       </c>
       <c r="Z63" s="20"/>
       <c r="AA63" s="39" t="s">
-        <v>1555</v>
+        <v>1552</v>
       </c>
       <c r="AB63" s="20"/>
       <c r="AC63" s="20" t="s">
-        <v>1593</v>
+        <v>1587</v>
       </c>
       <c r="AD63" s="20"/>
       <c r="AE63" s="20" t="s">
@@ -21395,7 +21394,7 @@
       <c r="P64" s="37"/>
       <c r="Q64" s="37"/>
       <c r="R64" s="37" t="s">
-        <v>1730</v>
+        <v>1724</v>
       </c>
       <c r="S64" s="20" t="s">
         <v>373</v>
@@ -21466,7 +21465,7 @@
       <c r="P65" s="37"/>
       <c r="Q65" s="37"/>
       <c r="R65" s="37" t="s">
-        <v>1731</v>
+        <v>1725</v>
       </c>
       <c r="S65" s="20" t="s">
         <v>374</v>
@@ -21537,7 +21536,7 @@
       <c r="P66" s="37"/>
       <c r="Q66" s="37"/>
       <c r="R66" s="37" t="s">
-        <v>1732</v>
+        <v>1726</v>
       </c>
       <c r="S66" s="20" t="s">
         <v>375</v>
@@ -21608,7 +21607,7 @@
       <c r="P67" s="37"/>
       <c r="Q67" s="37"/>
       <c r="R67" s="37" t="s">
-        <v>1733</v>
+        <v>1727</v>
       </c>
       <c r="S67" s="20" t="s">
         <v>747</v>
@@ -21637,7 +21636,7 @@
       </c>
       <c r="AD67" s="20"/>
       <c r="AE67" s="20" t="s">
-        <v>1641</v>
+        <v>1635</v>
       </c>
       <c r="AF67" s="20"/>
       <c r="AG67" s="20"/>
@@ -21679,7 +21678,7 @@
       <c r="P68" s="37"/>
       <c r="Q68" s="37"/>
       <c r="R68" s="37" t="s">
-        <v>1704</v>
+        <v>1698</v>
       </c>
       <c r="S68" s="20" t="s">
         <v>750</v>
@@ -21688,7 +21687,7 @@
         <v>750</v>
       </c>
       <c r="U68" s="20" t="s">
-        <v>1705</v>
+        <v>1699</v>
       </c>
       <c r="V68" s="20"/>
       <c r="W68" s="37" t="s">
@@ -21700,15 +21699,15 @@
       </c>
       <c r="Z68" s="20"/>
       <c r="AA68" s="39" t="s">
-        <v>1706</v>
+        <v>1700</v>
       </c>
       <c r="AB68" s="20"/>
       <c r="AC68" s="20" t="s">
-        <v>1707</v>
+        <v>1701</v>
       </c>
       <c r="AD68" s="20"/>
       <c r="AE68" s="20" t="s">
-        <v>1708</v>
+        <v>1702</v>
       </c>
       <c r="AF68" s="20"/>
       <c r="AG68" s="20"/>
@@ -21725,7 +21724,7 @@
       </c>
       <c r="D69" s="20"/>
       <c r="E69" s="20" t="s">
-        <v>1709</v>
+        <v>1703</v>
       </c>
       <c r="F69" s="20"/>
       <c r="G69" s="20" t="s">
@@ -21737,7 +21736,7 @@
       </c>
       <c r="J69" s="20"/>
       <c r="K69" s="37" t="s">
-        <v>1710</v>
+        <v>1704</v>
       </c>
       <c r="L69" s="37"/>
       <c r="M69" s="37" t="s">
@@ -21745,29 +21744,29 @@
       </c>
       <c r="N69" s="20"/>
       <c r="O69" s="37" t="s">
-        <v>1711</v>
+        <v>1705</v>
       </c>
       <c r="P69" s="37"/>
       <c r="Q69" s="37"/>
       <c r="R69" s="37" t="s">
-        <v>1712</v>
+        <v>1706</v>
       </c>
       <c r="S69" s="20" t="s">
-        <v>1713</v>
+        <v>1707</v>
       </c>
       <c r="T69" s="22" t="s">
-        <v>1713</v>
+        <v>1707</v>
       </c>
       <c r="U69" s="20" t="s">
-        <v>1714</v>
+        <v>1708</v>
       </c>
       <c r="V69" s="20"/>
       <c r="W69" s="37" t="s">
-        <v>1715</v>
+        <v>1709</v>
       </c>
       <c r="X69" s="20"/>
       <c r="Y69" s="37" t="s">
-        <v>1716</v>
+        <v>1710</v>
       </c>
       <c r="Z69" s="20"/>
       <c r="AA69" s="39" t="s">
@@ -21775,11 +21774,11 @@
       </c>
       <c r="AB69" s="20"/>
       <c r="AC69" s="20" t="s">
-        <v>1717</v>
+        <v>1711</v>
       </c>
       <c r="AD69" s="20"/>
       <c r="AE69" s="20" t="s">
-        <v>1718</v>
+        <v>1712</v>
       </c>
       <c r="AF69" s="20"/>
       <c r="AG69" s="20"/>
@@ -21796,61 +21795,61 @@
       </c>
       <c r="D70" s="20"/>
       <c r="E70" s="20" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="F70" s="20"/>
       <c r="G70" s="20" t="s">
-        <v>1880</v>
+        <v>1874</v>
       </c>
       <c r="H70" s="21"/>
       <c r="I70" s="21" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="J70" s="20"/>
       <c r="K70" s="37" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="L70" s="37"/>
       <c r="M70" s="37" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="N70" s="20"/>
       <c r="O70" s="37" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="P70" s="37"/>
       <c r="Q70" s="37"/>
       <c r="R70" s="37" t="s">
-        <v>1734</v>
+        <v>1728</v>
       </c>
       <c r="S70" s="20" t="s">
+        <v>1447</v>
+      </c>
+      <c r="T70" s="22" t="s">
         <v>1448</v>
       </c>
-      <c r="T70" s="22" t="s">
-        <v>1449</v>
-      </c>
       <c r="U70" s="20" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="V70" s="20"/>
       <c r="W70" s="37" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="X70" s="20"/>
       <c r="Y70" s="37" t="s">
-        <v>1514</v>
+        <v>1878</v>
       </c>
       <c r="Z70" s="20"/>
       <c r="AA70" s="39" t="s">
-        <v>1556</v>
+        <v>1882</v>
       </c>
       <c r="AB70" s="20"/>
       <c r="AC70" s="20" t="s">
-        <v>1594</v>
+        <v>1588</v>
       </c>
       <c r="AD70" s="20"/>
       <c r="AE70" s="20" t="s">
-        <v>1642</v>
+        <v>1636</v>
       </c>
       <c r="AF70" s="20"/>
       <c r="AG70" s="20"/>
@@ -21867,61 +21866,61 @@
       </c>
       <c r="D71" s="20"/>
       <c r="E71" s="20" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="F71" s="20"/>
       <c r="G71" s="20" t="s">
-        <v>1881</v>
+        <v>1875</v>
       </c>
       <c r="H71" s="21"/>
       <c r="I71" s="21" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="J71" s="20"/>
       <c r="K71" s="37" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="L71" s="37"/>
       <c r="M71" s="37" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="N71" s="20"/>
       <c r="O71" s="37" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="P71" s="37"/>
       <c r="Q71" s="37"/>
       <c r="R71" s="37" t="s">
-        <v>1735</v>
+        <v>1729</v>
       </c>
       <c r="S71" s="20" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="T71" s="22" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="U71" s="20" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="V71" s="20"/>
       <c r="W71" s="37" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="X71" s="20"/>
       <c r="Y71" s="37" t="s">
-        <v>1515</v>
+        <v>1879</v>
       </c>
       <c r="Z71" s="20"/>
       <c r="AA71" s="39" t="s">
-        <v>1557</v>
+        <v>1883</v>
       </c>
       <c r="AB71" s="20"/>
       <c r="AC71" s="20" t="s">
-        <v>1595</v>
+        <v>1589</v>
       </c>
       <c r="AD71" s="20"/>
       <c r="AE71" s="20" t="s">
-        <v>1643</v>
+        <v>1637</v>
       </c>
       <c r="AF71" s="20"/>
       <c r="AG71" s="20"/>
@@ -21938,61 +21937,61 @@
       </c>
       <c r="D72" s="20"/>
       <c r="E72" s="20" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="F72" s="20"/>
       <c r="G72" s="20" t="s">
-        <v>1874</v>
+        <v>1868</v>
       </c>
       <c r="H72" s="21"/>
       <c r="I72" s="21" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="J72" s="20"/>
       <c r="K72" s="37" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="L72" s="37"/>
       <c r="M72" s="37" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="N72" s="20"/>
       <c r="O72" s="37" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="P72" s="37"/>
       <c r="Q72" s="37"/>
       <c r="R72" s="37" t="s">
-        <v>1736</v>
+        <v>1730</v>
       </c>
       <c r="S72" s="20" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="T72" s="20" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="U72" s="20" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="V72" s="20"/>
       <c r="W72" s="37" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="X72" s="20"/>
       <c r="Y72" s="37" t="s">
-        <v>1516</v>
+        <v>1513</v>
       </c>
       <c r="Z72" s="20"/>
       <c r="AA72" s="39" t="s">
-        <v>1558</v>
+        <v>1881</v>
       </c>
       <c r="AB72" s="20"/>
       <c r="AC72" s="20" t="s">
-        <v>1596</v>
+        <v>1590</v>
       </c>
       <c r="AD72" s="20"/>
       <c r="AE72" s="20" t="s">
-        <v>1644</v>
+        <v>1638</v>
       </c>
       <c r="AF72" s="20"/>
       <c r="AG72" s="20"/>
@@ -22034,7 +22033,7 @@
       <c r="P73" s="37"/>
       <c r="Q73" s="37"/>
       <c r="R73" s="37" t="s">
-        <v>1737</v>
+        <v>1731</v>
       </c>
       <c r="S73" s="20" t="s">
         <v>376</v>
@@ -22105,7 +22104,7 @@
       <c r="P74" s="37"/>
       <c r="Q74" s="37"/>
       <c r="R74" s="37" t="s">
-        <v>1703</v>
+        <v>1697</v>
       </c>
       <c r="S74" s="20" t="s">
         <v>731</v>
@@ -22176,7 +22175,7 @@
       <c r="P75" s="37"/>
       <c r="Q75" s="37"/>
       <c r="R75" s="37" t="s">
-        <v>1738</v>
+        <v>1732</v>
       </c>
       <c r="S75" s="20" t="s">
         <v>836</v>
@@ -22247,7 +22246,7 @@
       <c r="P76" s="37"/>
       <c r="Q76" s="37"/>
       <c r="R76" s="37" t="s">
-        <v>1739</v>
+        <v>1733</v>
       </c>
       <c r="S76" s="20" t="s">
         <v>1113</v>
@@ -22318,7 +22317,7 @@
       <c r="P77" s="37"/>
       <c r="Q77" s="37"/>
       <c r="R77" s="37" t="s">
-        <v>1740</v>
+        <v>1734</v>
       </c>
       <c r="S77" s="20" t="s">
         <v>1115</v>
@@ -22364,61 +22363,61 @@
       </c>
       <c r="D78" s="20"/>
       <c r="E78" s="20" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="F78" s="20"/>
       <c r="G78" s="20" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="H78" s="21"/>
       <c r="I78" s="21" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="J78" s="20"/>
       <c r="K78" s="37" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="L78" s="37"/>
       <c r="M78" s="37" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="N78" s="20"/>
       <c r="O78" s="37" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="P78" s="37"/>
       <c r="Q78" s="37"/>
       <c r="R78" s="37" t="s">
-        <v>1741</v>
+        <v>1735</v>
       </c>
       <c r="S78" s="20" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="T78" s="22" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="U78" s="20" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="V78" s="20"/>
       <c r="W78" s="37" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="X78" s="20"/>
       <c r="Y78" s="37" t="s">
-        <v>1517</v>
+        <v>1514</v>
       </c>
       <c r="Z78" s="20"/>
       <c r="AA78" s="39" t="s">
-        <v>1559</v>
+        <v>1553</v>
       </c>
       <c r="AB78" s="20"/>
       <c r="AC78" s="20" t="s">
-        <v>1597</v>
+        <v>1591</v>
       </c>
       <c r="AD78" s="20"/>
       <c r="AE78" s="20" t="s">
-        <v>1645</v>
+        <v>1639</v>
       </c>
       <c r="AF78" s="20"/>
       <c r="AG78" s="20"/>
@@ -22435,61 +22434,61 @@
       </c>
       <c r="D79" s="22"/>
       <c r="E79" s="22" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="F79" s="22"/>
       <c r="G79" s="22" t="s">
-        <v>1875</v>
+        <v>1869</v>
       </c>
       <c r="H79" s="23"/>
       <c r="I79" s="23" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="J79" s="22"/>
       <c r="K79" s="37" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="L79" s="37"/>
       <c r="M79" s="37" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="N79" s="22"/>
       <c r="O79" s="37" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="P79" s="37"/>
       <c r="Q79" s="37"/>
       <c r="R79" s="37" t="s">
-        <v>1742</v>
+        <v>1736</v>
       </c>
       <c r="S79" s="22" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="T79" s="22" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="U79" s="22" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="V79" s="22"/>
       <c r="W79" s="37" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="X79" s="22"/>
       <c r="Y79" s="37" t="s">
-        <v>1518</v>
+        <v>1515</v>
       </c>
       <c r="Z79" s="22"/>
       <c r="AA79" s="39" t="s">
-        <v>1560</v>
+        <v>1554</v>
       </c>
       <c r="AB79" s="22"/>
       <c r="AC79" s="22" t="s">
-        <v>1598</v>
+        <v>1592</v>
       </c>
       <c r="AD79" s="22"/>
       <c r="AE79" s="22" t="s">
-        <v>1646</v>
+        <v>1640</v>
       </c>
       <c r="AF79" s="22"/>
       <c r="AG79" s="22"/>
@@ -22506,61 +22505,61 @@
       </c>
       <c r="D80" s="22"/>
       <c r="E80" s="22" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="F80" s="22"/>
       <c r="G80" s="22" t="s">
-        <v>1876</v>
+        <v>1870</v>
       </c>
       <c r="H80" s="23"/>
       <c r="I80" s="23" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="J80" s="22"/>
       <c r="K80" s="37" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="L80" s="37"/>
       <c r="M80" s="37" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="N80" s="22"/>
       <c r="O80" s="37" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="P80" s="37"/>
       <c r="Q80" s="37"/>
       <c r="R80" s="37" t="s">
-        <v>1743</v>
+        <v>1737</v>
       </c>
       <c r="S80" s="22" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="T80" s="22" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="U80" s="22" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="V80" s="22"/>
       <c r="W80" s="37" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="X80" s="22"/>
       <c r="Y80" s="37" t="s">
-        <v>1519</v>
+        <v>1516</v>
       </c>
       <c r="Z80" s="22"/>
       <c r="AA80" s="39" t="s">
-        <v>1561</v>
+        <v>1555</v>
       </c>
       <c r="AB80" s="22"/>
       <c r="AC80" s="22" t="s">
-        <v>1599</v>
+        <v>1593</v>
       </c>
       <c r="AD80" s="22"/>
       <c r="AE80" s="22" t="s">
-        <v>1647</v>
+        <v>1641</v>
       </c>
       <c r="AF80" s="22"/>
       <c r="AG80" s="22"/>
@@ -22602,7 +22601,7 @@
       <c r="P81" s="37"/>
       <c r="Q81" s="37"/>
       <c r="R81" s="37" t="s">
-        <v>1744</v>
+        <v>1738</v>
       </c>
       <c r="S81" s="22" t="s">
         <v>558</v>
@@ -22673,7 +22672,7 @@
       <c r="P82" s="37"/>
       <c r="Q82" s="37"/>
       <c r="R82" s="37" t="s">
-        <v>1745</v>
+        <v>1739</v>
       </c>
       <c r="S82" s="22" t="s">
         <v>732</v>
@@ -22719,23 +22718,23 @@
       </c>
       <c r="D83" s="22"/>
       <c r="E83" s="22" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="F83" s="22"/>
       <c r="G83" s="22" t="s">
-        <v>1877</v>
+        <v>1871</v>
       </c>
       <c r="H83" s="23"/>
       <c r="I83" s="23" t="s">
-        <v>1831</v>
+        <v>1825</v>
       </c>
       <c r="J83" s="22"/>
       <c r="K83" s="37" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="L83" s="37"/>
       <c r="M83" s="37" t="s">
-        <v>1838</v>
+        <v>1832</v>
       </c>
       <c r="N83" s="22"/>
       <c r="O83" s="37" t="s">
@@ -22744,36 +22743,36 @@
       <c r="P83" s="37"/>
       <c r="Q83" s="37"/>
       <c r="R83" s="37" t="s">
-        <v>1746</v>
+        <v>1740</v>
       </c>
       <c r="S83" s="22" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="T83" s="22" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="U83" s="22" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="V83" s="22"/>
       <c r="W83" s="37" t="s">
-        <v>1520</v>
+        <v>1517</v>
       </c>
       <c r="X83" s="22"/>
       <c r="Y83" s="37" t="s">
-        <v>1520</v>
+        <v>1517</v>
       </c>
       <c r="Z83" s="22"/>
       <c r="AA83" s="39" t="s">
-        <v>1855</v>
+        <v>1849</v>
       </c>
       <c r="AB83" s="22"/>
       <c r="AC83" s="22" t="s">
-        <v>1600</v>
+        <v>1594</v>
       </c>
       <c r="AD83" s="22"/>
       <c r="AE83" s="22" t="s">
-        <v>1648</v>
+        <v>1642</v>
       </c>
       <c r="AF83" s="22"/>
       <c r="AG83" s="22"/>
@@ -22790,61 +22789,61 @@
       </c>
       <c r="D84" s="22"/>
       <c r="E84" s="22" t="s">
-        <v>1822</v>
+        <v>1816</v>
       </c>
       <c r="F84" s="22"/>
       <c r="G84" s="22" t="s">
-        <v>1823</v>
+        <v>1817</v>
       </c>
       <c r="H84" s="23"/>
       <c r="I84" s="23" t="s">
-        <v>1832</v>
+        <v>1826</v>
       </c>
       <c r="J84" s="22"/>
       <c r="K84" s="37" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="L84" s="37"/>
       <c r="M84" s="37" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="N84" s="22"/>
       <c r="O84" s="37" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="P84" s="37"/>
       <c r="Q84" s="37"/>
       <c r="R84" s="37" t="s">
-        <v>1747</v>
+        <v>1741</v>
       </c>
       <c r="S84" s="22" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="T84" s="22" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="U84" s="22" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="V84" s="22"/>
       <c r="W84" s="37" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="X84" s="22"/>
       <c r="Y84" s="37" t="s">
-        <v>1521</v>
+        <v>1518</v>
       </c>
       <c r="Z84" s="22"/>
       <c r="AA84" s="39" t="s">
-        <v>1851</v>
+        <v>1845</v>
       </c>
       <c r="AB84" s="22"/>
       <c r="AC84" s="22" t="s">
-        <v>1601</v>
+        <v>1595</v>
       </c>
       <c r="AD84" s="22"/>
       <c r="AE84" s="22" t="s">
-        <v>1861</v>
+        <v>1855</v>
       </c>
       <c r="AF84" s="22"/>
       <c r="AG84" s="22"/>
@@ -22861,61 +22860,61 @@
       </c>
       <c r="D85" s="22"/>
       <c r="E85" s="22" t="s">
-        <v>1821</v>
+        <v>1815</v>
       </c>
       <c r="F85" s="22"/>
       <c r="G85" s="22" t="s">
-        <v>1824</v>
+        <v>1818</v>
       </c>
       <c r="H85" s="23"/>
       <c r="I85" s="23" t="s">
-        <v>1833</v>
+        <v>1827</v>
       </c>
       <c r="J85" s="22"/>
       <c r="K85" s="37" t="s">
-        <v>1834</v>
+        <v>1828</v>
       </c>
       <c r="L85" s="37"/>
       <c r="M85" s="37" t="s">
-        <v>1835</v>
+        <v>1829</v>
       </c>
       <c r="N85" s="22"/>
       <c r="O85" s="37" t="s">
-        <v>1843</v>
+        <v>1837</v>
       </c>
       <c r="P85" s="37"/>
       <c r="Q85" s="37"/>
       <c r="R85" s="37" t="s">
-        <v>1748</v>
+        <v>1742</v>
       </c>
       <c r="S85" s="22" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="T85" s="22" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="U85" s="22" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="V85" s="22"/>
       <c r="W85" s="37" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="X85" s="22"/>
       <c r="Y85" s="37" t="s">
-        <v>1522</v>
+        <v>1519</v>
       </c>
       <c r="Z85" s="22"/>
       <c r="AA85" s="39" t="s">
-        <v>1852</v>
+        <v>1846</v>
       </c>
       <c r="AB85" s="22"/>
       <c r="AC85" s="22" t="s">
-        <v>1602</v>
+        <v>1596</v>
       </c>
       <c r="AD85" s="22"/>
       <c r="AE85" s="22" t="s">
-        <v>1862</v>
+        <v>1856</v>
       </c>
       <c r="AF85" s="22"/>
       <c r="AG85" s="22"/>
@@ -22932,61 +22931,61 @@
       </c>
       <c r="D86" s="22"/>
       <c r="E86" s="22" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="F86" s="22"/>
       <c r="G86" s="22" t="s">
-        <v>1830</v>
+        <v>1824</v>
       </c>
       <c r="H86" s="23"/>
       <c r="I86" s="23" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="J86" s="22"/>
       <c r="K86" s="37" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="L86" s="37"/>
       <c r="M86" s="37" t="s">
-        <v>1839</v>
+        <v>1833</v>
       </c>
       <c r="N86" s="22"/>
       <c r="O86" s="37" t="s">
-        <v>1842</v>
+        <v>1836</v>
       </c>
       <c r="P86" s="37"/>
       <c r="Q86" s="37"/>
       <c r="R86" s="37" t="s">
-        <v>1749</v>
+        <v>1743</v>
       </c>
       <c r="S86" s="22" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="T86" s="22" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="U86" s="22" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="V86" s="22"/>
       <c r="W86" s="37" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="X86" s="22"/>
       <c r="Y86" s="37" t="s">
-        <v>1523</v>
+        <v>1520</v>
       </c>
       <c r="Z86" s="22"/>
       <c r="AA86" s="39" t="s">
-        <v>1856</v>
+        <v>1850</v>
       </c>
       <c r="AB86" s="22"/>
       <c r="AC86" s="22" t="s">
-        <v>1603</v>
+        <v>1597</v>
       </c>
       <c r="AD86" s="22"/>
       <c r="AE86" s="22" t="s">
-        <v>1649</v>
+        <v>1643</v>
       </c>
       <c r="AF86" s="22"/>
       <c r="AG86" s="22"/>
@@ -23003,45 +23002,45 @@
       </c>
       <c r="D87" s="22"/>
       <c r="E87" s="22" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="F87" s="22"/>
       <c r="G87" s="22" t="s">
-        <v>1825</v>
+        <v>1819</v>
       </c>
       <c r="H87" s="23"/>
       <c r="I87" s="23" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="J87" s="22"/>
       <c r="K87" s="37" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="L87" s="37"/>
       <c r="M87" s="37" t="s">
-        <v>1836</v>
+        <v>1830</v>
       </c>
       <c r="N87" s="22"/>
       <c r="O87" s="37" t="s">
-        <v>1840</v>
+        <v>1834</v>
       </c>
       <c r="P87" s="37"/>
       <c r="Q87" s="37"/>
       <c r="R87" s="37" t="s">
-        <v>1750</v>
+        <v>1744</v>
       </c>
       <c r="S87" s="22" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="T87" s="22" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="U87" s="22" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="V87" s="22"/>
       <c r="W87" s="37" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="X87" s="22"/>
       <c r="Y87" s="37" t="s">
@@ -23049,15 +23048,15 @@
       </c>
       <c r="Z87" s="22"/>
       <c r="AA87" s="39" t="s">
-        <v>1857</v>
+        <v>1851</v>
       </c>
       <c r="AB87" s="22"/>
       <c r="AC87" s="22" t="s">
-        <v>1860</v>
+        <v>1854</v>
       </c>
       <c r="AD87" s="22"/>
       <c r="AE87" s="22" t="s">
-        <v>1650</v>
+        <v>1644</v>
       </c>
       <c r="AF87" s="22"/>
       <c r="AG87" s="22"/>
@@ -23074,61 +23073,61 @@
       </c>
       <c r="D88" s="22"/>
       <c r="E88" s="22" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="F88" s="22"/>
       <c r="G88" s="22" t="s">
-        <v>1826</v>
+        <v>1820</v>
       </c>
       <c r="H88" s="23"/>
       <c r="I88" s="23" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="J88" s="22"/>
       <c r="K88" s="37" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="L88" s="37"/>
       <c r="M88" s="37" t="s">
-        <v>1837</v>
+        <v>1831</v>
       </c>
       <c r="N88" s="22"/>
       <c r="O88" s="37" t="s">
-        <v>1841</v>
+        <v>1835</v>
       </c>
       <c r="P88" s="37"/>
       <c r="Q88" s="37"/>
       <c r="R88" s="37" t="s">
-        <v>1751</v>
+        <v>1745</v>
       </c>
       <c r="S88" s="22" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="T88" s="22" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="U88" s="22" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="V88" s="22"/>
       <c r="W88" s="37" t="s">
-        <v>1849</v>
+        <v>1843</v>
       </c>
       <c r="X88" s="22"/>
       <c r="Y88" s="37" t="s">
-        <v>1849</v>
+        <v>1843</v>
       </c>
       <c r="Z88" s="22"/>
       <c r="AA88" s="39" t="s">
-        <v>1858</v>
+        <v>1852</v>
       </c>
       <c r="AB88" s="22"/>
       <c r="AC88" s="22" t="s">
-        <v>1604</v>
+        <v>1598</v>
       </c>
       <c r="AD88" s="22"/>
       <c r="AE88" s="22" t="s">
-        <v>1651</v>
+        <v>1645</v>
       </c>
       <c r="AF88" s="22"/>
       <c r="AG88" s="22"/>
@@ -23145,61 +23144,61 @@
       </c>
       <c r="D89" s="22"/>
       <c r="E89" s="22" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="F89" s="22"/>
       <c r="G89" s="22" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="H89" s="23"/>
       <c r="I89" s="23" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="J89" s="22"/>
       <c r="K89" s="37" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="L89" s="37"/>
       <c r="M89" s="37" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="N89" s="22"/>
       <c r="O89" s="37" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="P89" s="37"/>
       <c r="Q89" s="37"/>
       <c r="R89" s="37" t="s">
-        <v>1752</v>
+        <v>1746</v>
       </c>
       <c r="S89" s="22" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="T89" s="22" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="U89" s="22" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="V89" s="22"/>
       <c r="W89" s="37" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="X89" s="22"/>
       <c r="Y89" s="37" t="s">
-        <v>1524</v>
+        <v>1521</v>
       </c>
       <c r="Z89" s="22"/>
       <c r="AA89" s="39" t="s">
-        <v>1562</v>
+        <v>1556</v>
       </c>
       <c r="AB89" s="22"/>
       <c r="AC89" s="22" t="s">
-        <v>1605</v>
+        <v>1599</v>
       </c>
       <c r="AD89" s="22"/>
       <c r="AE89" s="22" t="s">
-        <v>1652</v>
+        <v>1646</v>
       </c>
       <c r="AF89" s="22"/>
       <c r="AG89" s="22"/>
@@ -23241,7 +23240,7 @@
       <c r="P90" s="37"/>
       <c r="Q90" s="37"/>
       <c r="R90" s="37" t="s">
-        <v>1753</v>
+        <v>1747</v>
       </c>
       <c r="S90" s="22" t="s">
         <v>1035</v>
@@ -23270,7 +23269,7 @@
       </c>
       <c r="AD90" s="22"/>
       <c r="AE90" s="22" t="s">
-        <v>1653</v>
+        <v>1647</v>
       </c>
       <c r="AF90" s="22"/>
       <c r="AG90" s="22"/>
@@ -23287,32 +23286,32 @@
       </c>
       <c r="D91" s="22"/>
       <c r="E91" s="22" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="F91" s="22"/>
       <c r="G91" s="22" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="H91" s="23"/>
       <c r="I91" s="23" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="J91" s="22"/>
       <c r="K91" s="37" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="L91" s="37"/>
       <c r="M91" s="37" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="N91" s="22"/>
       <c r="O91" s="37" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="P91" s="37"/>
       <c r="Q91" s="37"/>
       <c r="R91" s="37" t="s">
-        <v>1754</v>
+        <v>1748</v>
       </c>
       <c r="S91" s="22" t="s">
         <v>733</v>
@@ -23321,27 +23320,27 @@
         <v>733</v>
       </c>
       <c r="U91" s="22" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="V91" s="22"/>
       <c r="W91" s="37" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="X91" s="22"/>
       <c r="Y91" s="37" t="s">
-        <v>1525</v>
+        <v>1522</v>
       </c>
       <c r="Z91" s="22"/>
       <c r="AA91" s="39" t="s">
-        <v>1563</v>
+        <v>1557</v>
       </c>
       <c r="AB91" s="22"/>
       <c r="AC91" s="22" t="s">
-        <v>1606</v>
+        <v>1600</v>
       </c>
       <c r="AD91" s="22"/>
       <c r="AE91" s="22" t="s">
-        <v>1654</v>
+        <v>1648</v>
       </c>
       <c r="AF91" s="22"/>
       <c r="AG91" s="22"/>
@@ -23383,7 +23382,7 @@
       <c r="P92" s="37"/>
       <c r="Q92" s="37"/>
       <c r="R92" s="37" t="s">
-        <v>1755</v>
+        <v>1749</v>
       </c>
       <c r="S92" s="22" t="s">
         <v>1036</v>
@@ -23412,7 +23411,7 @@
       </c>
       <c r="AD92" s="22"/>
       <c r="AE92" s="22" t="s">
-        <v>1655</v>
+        <v>1649</v>
       </c>
       <c r="AF92" s="22"/>
       <c r="AG92" s="22"/>
@@ -23454,7 +23453,7 @@
       <c r="P93" s="37"/>
       <c r="Q93" s="37"/>
       <c r="R93" s="37" t="s">
-        <v>1756</v>
+        <v>1750</v>
       </c>
       <c r="S93" s="22" t="s">
         <v>734</v>
@@ -23525,7 +23524,7 @@
       <c r="P94" s="37"/>
       <c r="Q94" s="37"/>
       <c r="R94" s="37" t="s">
-        <v>1757</v>
+        <v>1751</v>
       </c>
       <c r="S94" s="22" t="s">
         <v>735</v>
@@ -23571,61 +23570,61 @@
       </c>
       <c r="D95" s="22"/>
       <c r="E95" s="22" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="F95" s="22"/>
       <c r="G95" s="22" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="H95" s="23"/>
       <c r="I95" s="23" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="J95" s="22"/>
       <c r="K95" s="37" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="L95" s="37"/>
       <c r="M95" s="37" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="N95" s="22"/>
       <c r="O95" s="37" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="P95" s="37"/>
       <c r="Q95" s="37"/>
       <c r="R95" s="37" t="s">
-        <v>1758</v>
+        <v>1752</v>
       </c>
       <c r="S95" s="22" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="T95" s="22" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="U95" s="22" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="V95" s="22"/>
       <c r="W95" s="37" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="X95" s="22"/>
       <c r="Y95" s="37" t="s">
-        <v>1526</v>
+        <v>1523</v>
       </c>
       <c r="Z95" s="22"/>
       <c r="AA95" s="39" t="s">
-        <v>1564</v>
+        <v>1558</v>
       </c>
       <c r="AB95" s="22"/>
       <c r="AC95" s="22" t="s">
-        <v>1607</v>
+        <v>1601</v>
       </c>
       <c r="AD95" s="22"/>
       <c r="AE95" s="22" t="s">
-        <v>1656</v>
+        <v>1650</v>
       </c>
       <c r="AF95" s="22"/>
       <c r="AG95" s="22"/>
@@ -23667,7 +23666,7 @@
       <c r="P96" s="37"/>
       <c r="Q96" s="37"/>
       <c r="R96" s="37" t="s">
-        <v>1759</v>
+        <v>1753</v>
       </c>
       <c r="S96" s="22" t="s">
         <v>736</v>
@@ -23738,7 +23737,7 @@
       <c r="P97" s="37"/>
       <c r="Q97" s="37"/>
       <c r="R97" s="37" t="s">
-        <v>1760</v>
+        <v>1754</v>
       </c>
       <c r="S97" s="22" t="s">
         <v>737</v>
@@ -23809,7 +23808,7 @@
       <c r="P98" s="37"/>
       <c r="Q98" s="37"/>
       <c r="R98" s="37" t="s">
-        <v>1761</v>
+        <v>1755</v>
       </c>
       <c r="S98" s="22" t="s">
         <v>738</v>
@@ -23880,7 +23879,7 @@
       <c r="P99" s="37"/>
       <c r="Q99" s="37"/>
       <c r="R99" s="37" t="s">
-        <v>1762</v>
+        <v>1756</v>
       </c>
       <c r="S99" s="22" t="s">
         <v>739</v>
@@ -23909,7 +23908,7 @@
       </c>
       <c r="AD99" s="22"/>
       <c r="AE99" s="22" t="s">
-        <v>1657</v>
+        <v>1651</v>
       </c>
       <c r="AF99" s="22"/>
       <c r="AG99" s="22"/>
@@ -23951,7 +23950,7 @@
       <c r="P100" s="37"/>
       <c r="Q100" s="37"/>
       <c r="R100" s="37" t="s">
-        <v>1763</v>
+        <v>1757</v>
       </c>
       <c r="S100" s="22" t="s">
         <v>740</v>
@@ -23980,7 +23979,7 @@
       </c>
       <c r="AD100" s="22"/>
       <c r="AE100" s="22" t="s">
-        <v>1658</v>
+        <v>1652</v>
       </c>
       <c r="AF100" s="22"/>
       <c r="AG100" s="22"/>
@@ -24022,7 +24021,7 @@
       <c r="P101" s="37"/>
       <c r="Q101" s="37"/>
       <c r="R101" s="37" t="s">
-        <v>1764</v>
+        <v>1758</v>
       </c>
       <c r="S101" s="22" t="s">
         <v>386</v>
@@ -24093,7 +24092,7 @@
       <c r="P102" s="37"/>
       <c r="Q102" s="37"/>
       <c r="R102" s="37" t="s">
-        <v>1765</v>
+        <v>1759</v>
       </c>
       <c r="S102" s="22" t="s">
         <v>387</v>
@@ -24122,7 +24121,7 @@
       </c>
       <c r="AD102" s="22"/>
       <c r="AE102" s="22" t="s">
-        <v>1659</v>
+        <v>1653</v>
       </c>
       <c r="AF102" s="22"/>
       <c r="AG102" s="22"/>
@@ -24164,7 +24163,7 @@
       <c r="P103" s="37"/>
       <c r="Q103" s="37"/>
       <c r="R103" s="37" t="s">
-        <v>1766</v>
+        <v>1760</v>
       </c>
       <c r="S103" s="22" t="s">
         <v>388</v>
@@ -24206,65 +24205,65 @@
         <v>84</v>
       </c>
       <c r="C104" s="24" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="D104" s="22"/>
       <c r="E104" s="22" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="F104" s="22"/>
       <c r="G104" s="22" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="H104" s="24"/>
       <c r="I104" s="24" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="J104" s="25"/>
       <c r="K104" s="37" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="L104" s="37"/>
       <c r="M104" s="37" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="N104" s="25"/>
       <c r="O104" s="37" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="P104" s="37"/>
       <c r="Q104" s="37"/>
       <c r="R104" s="37" t="s">
-        <v>1767</v>
+        <v>1761</v>
       </c>
       <c r="S104" s="22" t="s">
         <v>1108</v>
       </c>
       <c r="T104" s="25" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="U104" s="22" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="V104" s="22"/>
       <c r="W104" s="37" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="X104" s="22"/>
       <c r="Y104" s="37" t="s">
-        <v>1527</v>
+        <v>1524</v>
       </c>
       <c r="Z104" s="22"/>
       <c r="AA104" s="39" t="s">
-        <v>1565</v>
+        <v>1559</v>
       </c>
       <c r="AB104" s="22"/>
       <c r="AC104" s="22" t="s">
-        <v>1608</v>
+        <v>1602</v>
       </c>
       <c r="AD104" s="22"/>
       <c r="AE104" s="22" t="s">
-        <v>1660</v>
+        <v>1654</v>
       </c>
       <c r="AF104" s="22"/>
       <c r="AG104" s="22"/>
@@ -24306,7 +24305,7 @@
       <c r="P105" s="37"/>
       <c r="Q105" s="37"/>
       <c r="R105" s="37" t="s">
-        <v>1768</v>
+        <v>1762</v>
       </c>
       <c r="S105" s="22" t="s">
         <v>1032</v>
@@ -24335,7 +24334,7 @@
       </c>
       <c r="AD105" s="22"/>
       <c r="AE105" s="22" t="s">
-        <v>1661</v>
+        <v>1655</v>
       </c>
       <c r="AF105" s="22"/>
       <c r="AG105" s="22"/>
@@ -24377,7 +24376,7 @@
       <c r="P106" s="37"/>
       <c r="Q106" s="37"/>
       <c r="R106" s="37" t="s">
-        <v>1769</v>
+        <v>1763</v>
       </c>
       <c r="S106" s="22" t="s">
         <v>1033</v>
@@ -24406,7 +24405,7 @@
       </c>
       <c r="AD106" s="22"/>
       <c r="AE106" s="22" t="s">
-        <v>1662</v>
+        <v>1656</v>
       </c>
       <c r="AF106" s="22"/>
       <c r="AG106" s="22"/>
@@ -24448,7 +24447,7 @@
       <c r="P107" s="37"/>
       <c r="Q107" s="37"/>
       <c r="R107" s="37" t="s">
-        <v>1770</v>
+        <v>1764</v>
       </c>
       <c r="S107" s="22" t="s">
         <v>1034</v>
@@ -24477,7 +24476,7 @@
       </c>
       <c r="AD107" s="22"/>
       <c r="AE107" s="22" t="s">
-        <v>1663</v>
+        <v>1657</v>
       </c>
       <c r="AF107" s="22"/>
       <c r="AG107" s="22"/>
@@ -24519,7 +24518,7 @@
       <c r="P108" s="37"/>
       <c r="Q108" s="37"/>
       <c r="R108" s="37" t="s">
-        <v>1771</v>
+        <v>1765</v>
       </c>
       <c r="S108" s="22" t="s">
         <v>389</v>
@@ -24590,7 +24589,7 @@
       <c r="P109" s="37"/>
       <c r="Q109" s="37"/>
       <c r="R109" s="37" t="s">
-        <v>1772</v>
+        <v>1766</v>
       </c>
       <c r="S109" s="22" t="s">
         <v>741</v>
@@ -24661,7 +24660,7 @@
       <c r="P110" s="37"/>
       <c r="Q110" s="37"/>
       <c r="R110" s="37" t="s">
-        <v>1773</v>
+        <v>1767</v>
       </c>
       <c r="S110" s="22" t="s">
         <v>391</v>
@@ -24732,7 +24731,7 @@
       <c r="P111" s="37"/>
       <c r="Q111" s="37"/>
       <c r="R111" s="37" t="s">
-        <v>1774</v>
+        <v>1768</v>
       </c>
       <c r="S111" s="22" t="s">
         <v>392</v>
@@ -24803,7 +24802,7 @@
       <c r="P112" s="37"/>
       <c r="Q112" s="37"/>
       <c r="R112" s="37" t="s">
-        <v>1775</v>
+        <v>1769</v>
       </c>
       <c r="S112" s="22" t="s">
         <v>742</v>
@@ -24874,7 +24873,7 @@
       <c r="P113" s="37"/>
       <c r="Q113" s="37"/>
       <c r="R113" s="37" t="s">
-        <v>1776</v>
+        <v>1770</v>
       </c>
       <c r="S113" s="22" t="s">
         <v>394</v>
@@ -24945,7 +24944,7 @@
       <c r="P114" s="37"/>
       <c r="Q114" s="37"/>
       <c r="R114" s="37" t="s">
-        <v>1777</v>
+        <v>1771</v>
       </c>
       <c r="S114" s="22" t="s">
         <v>395</v>
@@ -25016,7 +25015,7 @@
       <c r="P115" s="37"/>
       <c r="Q115" s="37"/>
       <c r="R115" s="37" t="s">
-        <v>1778</v>
+        <v>1772</v>
       </c>
       <c r="S115" s="22" t="s">
         <v>396</v>
@@ -25087,7 +25086,7 @@
       <c r="P116" s="37"/>
       <c r="Q116" s="37"/>
       <c r="R116" s="37" t="s">
-        <v>1779</v>
+        <v>1773</v>
       </c>
       <c r="S116" s="22" t="s">
         <v>397</v>
@@ -25158,7 +25157,7 @@
       <c r="P117" s="37"/>
       <c r="Q117" s="37"/>
       <c r="R117" s="37" t="s">
-        <v>1780</v>
+        <v>1774</v>
       </c>
       <c r="S117" s="22" t="s">
         <v>398</v>
@@ -25229,7 +25228,7 @@
       <c r="P118" s="37"/>
       <c r="Q118" s="37"/>
       <c r="R118" s="37" t="s">
-        <v>1781</v>
+        <v>1775</v>
       </c>
       <c r="S118" s="22" t="s">
         <v>399</v>
@@ -25258,7 +25257,7 @@
       </c>
       <c r="AD118" s="22"/>
       <c r="AE118" s="22" t="s">
-        <v>1664</v>
+        <v>1658</v>
       </c>
       <c r="AF118" s="22"/>
       <c r="AG118" s="22"/>
@@ -25275,61 +25274,61 @@
       </c>
       <c r="D119" s="22"/>
       <c r="E119" s="22" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="F119" s="22"/>
       <c r="G119" s="22" t="s">
-        <v>1827</v>
+        <v>1821</v>
       </c>
       <c r="H119" s="23"/>
       <c r="I119" s="23" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="J119" s="22"/>
       <c r="K119" s="37" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="L119" s="37"/>
       <c r="M119" s="37" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="N119" s="22"/>
       <c r="O119" s="37" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="P119" s="37"/>
       <c r="Q119" s="37"/>
       <c r="R119" s="37" t="s">
-        <v>1782</v>
+        <v>1776</v>
       </c>
       <c r="S119" s="22" t="s">
-        <v>1845</v>
+        <v>1839</v>
       </c>
       <c r="T119" s="22" t="s">
-        <v>1845</v>
+        <v>1839</v>
       </c>
       <c r="U119" s="22" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="V119" s="22"/>
       <c r="W119" s="37" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="X119" s="22"/>
       <c r="Y119" s="37" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="Z119" s="22"/>
       <c r="AA119" s="39" t="s">
-        <v>1853</v>
+        <v>1847</v>
       </c>
       <c r="AB119" s="22"/>
       <c r="AC119" s="22" t="s">
-        <v>1609</v>
+        <v>1603</v>
       </c>
       <c r="AD119" s="22"/>
       <c r="AE119" s="22" t="s">
-        <v>1665</v>
+        <v>1659</v>
       </c>
       <c r="AF119" s="22"/>
       <c r="AG119" s="22"/>
@@ -25346,61 +25345,61 @@
       </c>
       <c r="D120" s="22"/>
       <c r="E120" s="22" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="F120" s="25"/>
       <c r="G120" s="25" t="s">
-        <v>1828</v>
+        <v>1822</v>
       </c>
       <c r="H120" s="23"/>
       <c r="I120" s="23" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="J120" s="22"/>
       <c r="K120" s="37" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="L120" s="37"/>
       <c r="M120" s="37" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="N120" s="22"/>
       <c r="O120" s="37" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="P120" s="37"/>
       <c r="Q120" s="37"/>
       <c r="R120" s="37" t="s">
-        <v>1783</v>
+        <v>1777</v>
       </c>
       <c r="S120" s="22" t="s">
-        <v>1847</v>
+        <v>1841</v>
       </c>
       <c r="T120" s="22" t="s">
-        <v>1847</v>
+        <v>1841</v>
       </c>
       <c r="U120" s="22" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="V120" s="22"/>
       <c r="W120" s="37" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="X120" s="22"/>
       <c r="Y120" s="37" t="s">
-        <v>1528</v>
+        <v>1525</v>
       </c>
       <c r="Z120" s="25"/>
       <c r="AA120" s="39" t="s">
-        <v>1859</v>
+        <v>1853</v>
       </c>
       <c r="AB120" s="22"/>
       <c r="AC120" s="22" t="s">
-        <v>1610</v>
+        <v>1604</v>
       </c>
       <c r="AD120" s="22"/>
       <c r="AE120" s="22" t="s">
-        <v>1666</v>
+        <v>1660</v>
       </c>
       <c r="AF120" s="22"/>
       <c r="AG120" s="22"/>
@@ -25417,61 +25416,61 @@
       </c>
       <c r="D121" s="22"/>
       <c r="E121" s="22" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="F121" s="22"/>
       <c r="G121" s="22" t="s">
-        <v>1829</v>
+        <v>1823</v>
       </c>
       <c r="H121" s="23"/>
       <c r="I121" s="23" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="J121" s="22"/>
       <c r="K121" s="37" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="L121" s="37"/>
       <c r="M121" s="37" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="N121" s="22"/>
       <c r="O121" s="37" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="P121" s="37"/>
       <c r="Q121" s="37"/>
       <c r="R121" s="37" t="s">
-        <v>1784</v>
+        <v>1778</v>
       </c>
       <c r="S121" s="22" t="s">
-        <v>1846</v>
+        <v>1840</v>
       </c>
       <c r="T121" s="22" t="s">
-        <v>1846</v>
+        <v>1840</v>
       </c>
       <c r="U121" s="22" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="V121" s="22"/>
       <c r="W121" s="37" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="X121" s="22"/>
       <c r="Y121" s="37" t="s">
-        <v>1850</v>
+        <v>1844</v>
       </c>
       <c r="Z121" s="22"/>
       <c r="AA121" s="39" t="s">
-        <v>1854</v>
+        <v>1848</v>
       </c>
       <c r="AB121" s="22"/>
       <c r="AC121" s="22" t="s">
-        <v>1611</v>
+        <v>1605</v>
       </c>
       <c r="AD121" s="22"/>
       <c r="AE121" s="22" t="s">
-        <v>1667</v>
+        <v>1661</v>
       </c>
       <c r="AF121" s="22"/>
       <c r="AG121" s="22"/>
@@ -25513,7 +25512,7 @@
       <c r="P122" s="37"/>
       <c r="Q122" s="37"/>
       <c r="R122" s="37" t="s">
-        <v>1785</v>
+        <v>1779</v>
       </c>
       <c r="S122" s="22" t="s">
         <v>743</v>
@@ -25542,7 +25541,7 @@
       </c>
       <c r="AD122" s="22"/>
       <c r="AE122" s="22" t="s">
-        <v>1668</v>
+        <v>1662</v>
       </c>
       <c r="AF122" s="22"/>
       <c r="AG122" s="22"/>
@@ -25559,32 +25558,32 @@
       </c>
       <c r="D123" s="22"/>
       <c r="E123" s="22" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="F123" s="22"/>
       <c r="G123" s="22" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="H123" s="23"/>
       <c r="I123" s="23" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="J123" s="22"/>
       <c r="K123" s="37" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="L123" s="37"/>
       <c r="M123" s="37" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="N123" s="22"/>
       <c r="O123" s="37" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="P123" s="37"/>
       <c r="Q123" s="37"/>
       <c r="R123" s="37" t="s">
-        <v>1786</v>
+        <v>1780</v>
       </c>
       <c r="S123" s="22" t="s">
         <v>401</v>
@@ -25593,27 +25592,27 @@
         <v>401</v>
       </c>
       <c r="U123" s="22" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="V123" s="22"/>
       <c r="W123" s="37" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="X123" s="22"/>
       <c r="Y123" s="37" t="s">
-        <v>1529</v>
+        <v>1526</v>
       </c>
       <c r="Z123" s="22"/>
       <c r="AA123" s="39" t="s">
-        <v>1566</v>
+        <v>1560</v>
       </c>
       <c r="AB123" s="22"/>
       <c r="AC123" s="22" t="s">
-        <v>1612</v>
+        <v>1606</v>
       </c>
       <c r="AD123" s="22"/>
       <c r="AE123" s="22" t="s">
-        <v>1669</v>
+        <v>1663</v>
       </c>
       <c r="AF123" s="22"/>
       <c r="AG123" s="22"/>
@@ -25655,7 +25654,7 @@
       <c r="P124" s="37"/>
       <c r="Q124" s="37"/>
       <c r="R124" s="37" t="s">
-        <v>1787</v>
+        <v>1781</v>
       </c>
       <c r="S124" s="22" t="s">
         <v>402</v>
@@ -25726,7 +25725,7 @@
       <c r="P125" s="37"/>
       <c r="Q125" s="37"/>
       <c r="R125" s="37" t="s">
-        <v>1788</v>
+        <v>1782</v>
       </c>
       <c r="S125" s="22" t="s">
         <v>403</v>
@@ -25755,7 +25754,7 @@
       </c>
       <c r="AD125" s="22"/>
       <c r="AE125" s="22" t="s">
-        <v>1670</v>
+        <v>1664</v>
       </c>
       <c r="AF125" s="22"/>
       <c r="AG125" s="22"/>
@@ -25797,7 +25796,7 @@
       <c r="P126" s="37"/>
       <c r="Q126" s="37"/>
       <c r="R126" s="37" t="s">
-        <v>1789</v>
+        <v>1783</v>
       </c>
       <c r="S126" s="22" t="s">
         <v>404</v>
@@ -25868,7 +25867,7 @@
       <c r="P127" s="37"/>
       <c r="Q127" s="37"/>
       <c r="R127" s="37" t="s">
-        <v>1790</v>
+        <v>1784</v>
       </c>
       <c r="S127" s="22" t="s">
         <v>744</v>
@@ -25897,7 +25896,7 @@
       </c>
       <c r="AD127" s="22"/>
       <c r="AE127" s="22" t="s">
-        <v>1671</v>
+        <v>1665</v>
       </c>
       <c r="AF127" s="22"/>
       <c r="AG127" s="22"/>
@@ -25939,7 +25938,7 @@
       <c r="P128" s="37"/>
       <c r="Q128" s="37"/>
       <c r="R128" s="37" t="s">
-        <v>1791</v>
+        <v>1785</v>
       </c>
       <c r="S128" s="22" t="s">
         <v>745</v>
@@ -25968,7 +25967,7 @@
       </c>
       <c r="AD128" s="22"/>
       <c r="AE128" s="22" t="s">
-        <v>1672</v>
+        <v>1666</v>
       </c>
       <c r="AF128" s="22"/>
       <c r="AG128" s="22"/>
@@ -25989,7 +25988,7 @@
       </c>
       <c r="F129" s="22"/>
       <c r="G129" s="22" t="s">
-        <v>1878</v>
+        <v>1872</v>
       </c>
       <c r="H129" s="23"/>
       <c r="I129" s="23" t="s">
@@ -26010,7 +26009,7 @@
       <c r="P129" s="37"/>
       <c r="Q129" s="37"/>
       <c r="R129" s="37" t="s">
-        <v>1792</v>
+        <v>1786</v>
       </c>
       <c r="S129" s="22" t="s">
         <v>746</v>
@@ -26039,7 +26038,7 @@
       </c>
       <c r="AD129" s="22"/>
       <c r="AE129" s="22" t="s">
-        <v>1673</v>
+        <v>1667</v>
       </c>
       <c r="AF129" s="22"/>
       <c r="AG129" s="22"/>
@@ -26056,61 +26055,61 @@
       </c>
       <c r="D130" s="22"/>
       <c r="E130" s="22" t="s">
-        <v>1872</v>
+        <v>1866</v>
       </c>
       <c r="F130" s="22"/>
       <c r="G130" s="22" t="s">
-        <v>1879</v>
+        <v>1873</v>
       </c>
       <c r="H130" s="23"/>
       <c r="I130" s="23" t="s">
-        <v>1871</v>
+        <v>1865</v>
       </c>
       <c r="J130" s="22"/>
       <c r="K130" s="37" t="s">
-        <v>1870</v>
+        <v>1864</v>
       </c>
       <c r="L130" s="37"/>
       <c r="M130" s="37" t="s">
-        <v>1869</v>
+        <v>1863</v>
       </c>
       <c r="N130" s="22"/>
       <c r="O130" s="37" t="s">
-        <v>1868</v>
+        <v>1862</v>
       </c>
       <c r="P130" s="37"/>
       <c r="Q130" s="37"/>
       <c r="R130" s="37" t="s">
-        <v>1793</v>
+        <v>1787</v>
       </c>
       <c r="S130" s="22" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="T130" s="22" t="s">
-        <v>1848</v>
+        <v>1842</v>
       </c>
       <c r="U130" s="22" t="s">
-        <v>1867</v>
+        <v>1861</v>
       </c>
       <c r="V130" s="22"/>
       <c r="W130" s="37" t="s">
-        <v>1866</v>
+        <v>1860</v>
       </c>
       <c r="X130" s="22"/>
       <c r="Y130" s="37" t="s">
-        <v>1866</v>
+        <v>1860</v>
       </c>
       <c r="Z130" s="22"/>
       <c r="AA130" s="39" t="s">
-        <v>1865</v>
+        <v>1859</v>
       </c>
       <c r="AB130" s="22"/>
       <c r="AC130" s="22" t="s">
-        <v>1864</v>
+        <v>1858</v>
       </c>
       <c r="AD130" s="22"/>
       <c r="AE130" s="22" t="s">
-        <v>1863</v>
+        <v>1857</v>
       </c>
       <c r="AF130" s="22"/>
       <c r="AG130" s="22"/>
@@ -26127,15 +26126,15 @@
       </c>
       <c r="D131" s="22"/>
       <c r="E131" s="22" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="F131" s="22"/>
       <c r="G131" s="22" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="H131" s="23"/>
       <c r="I131" s="23" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="J131" s="22"/>
       <c r="K131" s="38" t="s">
@@ -26143,16 +26142,16 @@
       </c>
       <c r="L131" s="38"/>
       <c r="M131" s="38" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="N131" s="22"/>
       <c r="O131" s="38" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="P131" s="38"/>
       <c r="Q131" s="38"/>
       <c r="R131" s="38" t="s">
-        <v>1794</v>
+        <v>1788</v>
       </c>
       <c r="S131" s="22" t="s">
         <v>1045</v>
@@ -26165,23 +26164,23 @@
       </c>
       <c r="V131" s="22"/>
       <c r="W131" s="38" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="X131" s="22"/>
       <c r="Y131" s="38" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="Z131" s="22"/>
       <c r="AA131" s="40" t="s">
-        <v>1567</v>
+        <v>1561</v>
       </c>
       <c r="AB131" s="22"/>
       <c r="AC131" s="22" t="s">
-        <v>1613</v>
+        <v>1607</v>
       </c>
       <c r="AD131" s="22"/>
       <c r="AE131" s="22" t="s">
-        <v>1674</v>
+        <v>1668</v>
       </c>
       <c r="AF131" s="22"/>
       <c r="AG131" s="22"/>
@@ -26223,7 +26222,7 @@
       <c r="P132" s="37"/>
       <c r="Q132" s="37"/>
       <c r="R132" s="37" t="s">
-        <v>1795</v>
+        <v>1789</v>
       </c>
       <c r="S132" s="22" t="s">
         <v>562</v>
@@ -26252,7 +26251,7 @@
       </c>
       <c r="AD132" s="22"/>
       <c r="AE132" s="22" t="s">
-        <v>1675</v>
+        <v>1669</v>
       </c>
       <c r="AF132" s="22"/>
       <c r="AG132" s="22"/>
@@ -26266,61 +26265,61 @@
         <v>Maiduguri - Summary</v>
       </c>
       <c r="C133" s="23" t="s">
-        <v>1138</v>
+        <v>1880</v>
       </c>
       <c r="D133" s="22"/>
       <c r="E133" s="22" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="F133" s="22"/>
       <c r="G133" s="22" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="H133" s="23"/>
       <c r="I133" s="23" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="J133" s="22"/>
       <c r="K133" s="37" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="L133" s="37"/>
       <c r="M133" s="37" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="N133" s="22"/>
       <c r="O133" s="37" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="P133" s="37"/>
       <c r="Q133" s="37"/>
       <c r="R133" s="37" t="s">
-        <v>1796</v>
+        <v>1790</v>
       </c>
       <c r="S133" s="22"/>
       <c r="T133" s="22"/>
       <c r="U133" s="22" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="V133" s="22"/>
       <c r="W133" s="37" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="X133" s="22"/>
       <c r="Y133" s="37" t="s">
-        <v>1530</v>
+        <v>1527</v>
       </c>
       <c r="Z133" s="22"/>
       <c r="AA133" s="39" t="s">
-        <v>1568</v>
+        <v>1562</v>
       </c>
       <c r="AB133" s="22"/>
       <c r="AC133" s="22" t="s">
-        <v>1614</v>
+        <v>1608</v>
       </c>
       <c r="AD133" s="22"/>
       <c r="AE133" s="22" t="s">
-        <v>1676</v>
+        <v>1670</v>
       </c>
       <c r="AF133" s="22"/>
       <c r="AG133" s="22"/>
@@ -26334,63 +26333,63 @@
         <v>Mexico City - Summary</v>
       </c>
       <c r="C134" s="23" t="s">
-        <v>1883</v>
+        <v>1877</v>
       </c>
       <c r="D134" s="22"/>
       <c r="E134" s="22" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="F134" s="22"/>
       <c r="G134" s="22" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="H134" s="23"/>
       <c r="I134" s="23" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="J134" s="22"/>
       <c r="K134" s="37" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="L134" s="37"/>
       <c r="M134" s="37" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="N134" s="22"/>
       <c r="O134" s="37" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="P134" s="37"/>
       <c r="Q134" s="37"/>
       <c r="R134" s="37" t="s">
-        <v>1797</v>
+        <v>1791</v>
       </c>
       <c r="S134" s="22" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="T134" s="22"/>
       <c r="U134" s="22" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="V134" s="22"/>
       <c r="W134" s="37" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="X134" s="22"/>
       <c r="Y134" s="37" t="s">
-        <v>1531</v>
+        <v>1528</v>
       </c>
       <c r="Z134" s="22"/>
       <c r="AA134" s="39" t="s">
-        <v>1569</v>
+        <v>1563</v>
       </c>
       <c r="AB134" s="22"/>
       <c r="AC134" s="22" t="s">
-        <v>1615</v>
+        <v>1609</v>
       </c>
       <c r="AD134" s="22"/>
       <c r="AE134" s="22" t="s">
-        <v>1677</v>
+        <v>1671</v>
       </c>
       <c r="AF134" s="22"/>
       <c r="AG134" s="22"/>
@@ -26404,61 +26403,61 @@
         <v>Baltimore - Summary</v>
       </c>
       <c r="C135" s="23" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="D135" s="22"/>
       <c r="E135" s="22" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="F135" s="22"/>
       <c r="G135" s="22" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="H135" s="23"/>
       <c r="I135" s="23" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="J135" s="22"/>
       <c r="K135" s="37" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="L135" s="37"/>
       <c r="M135" s="37" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="N135" s="22"/>
       <c r="O135" s="37" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="P135" s="37"/>
       <c r="Q135" s="37"/>
       <c r="R135" s="37" t="s">
-        <v>1798</v>
+        <v>1792</v>
       </c>
       <c r="S135" s="22"/>
       <c r="T135" s="22"/>
       <c r="U135" s="22" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="V135" s="22"/>
       <c r="W135" s="37" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="X135" s="22"/>
       <c r="Y135" s="37" t="s">
-        <v>1532</v>
+        <v>1529</v>
       </c>
       <c r="Z135" s="22"/>
       <c r="AA135" s="39" t="s">
-        <v>1570</v>
+        <v>1564</v>
       </c>
       <c r="AB135" s="22"/>
       <c r="AC135" s="22" t="s">
-        <v>1616</v>
+        <v>1610</v>
       </c>
       <c r="AD135" s="22"/>
       <c r="AE135" s="22" t="s">
-        <v>1678</v>
+        <v>1672</v>
       </c>
       <c r="AF135" s="22"/>
       <c r="AG135" s="22"/>
@@ -26472,61 +26471,61 @@
         <v>Phoenix - Summary</v>
       </c>
       <c r="C136" s="23" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="D136" s="22"/>
       <c r="E136" s="22" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="F136" s="22"/>
       <c r="G136" s="22" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="H136" s="23"/>
       <c r="I136" s="23" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="J136" s="22"/>
       <c r="K136" s="37" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="L136" s="37"/>
       <c r="M136" s="37" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="N136" s="22"/>
       <c r="O136" s="37" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="P136" s="37"/>
       <c r="Q136" s="37"/>
       <c r="R136" s="37" t="s">
-        <v>1799</v>
+        <v>1793</v>
       </c>
       <c r="S136" s="22"/>
       <c r="T136" s="22"/>
       <c r="U136" s="22" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="V136" s="22"/>
       <c r="W136" s="37" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="X136" s="22"/>
       <c r="Y136" s="37" t="s">
-        <v>1533</v>
+        <v>1530</v>
       </c>
       <c r="Z136" s="22"/>
       <c r="AA136" s="39" t="s">
-        <v>1571</v>
+        <v>1565</v>
       </c>
       <c r="AB136" s="22"/>
       <c r="AC136" s="22" t="s">
-        <v>1617</v>
+        <v>1611</v>
       </c>
       <c r="AD136" s="22"/>
       <c r="AE136" s="22" t="s">
-        <v>1679</v>
+        <v>1673</v>
       </c>
       <c r="AF136" s="22"/>
       <c r="AG136" s="22"/>
@@ -26540,61 +26539,61 @@
         <v>Seattle - Summary</v>
       </c>
       <c r="C137" s="23" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="D137" s="22"/>
       <c r="E137" s="22" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="F137" s="22"/>
       <c r="G137" s="22" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="H137" s="23"/>
       <c r="I137" s="23" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="J137" s="22"/>
       <c r="K137" s="37" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="L137" s="37"/>
       <c r="M137" s="37" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="N137" s="22"/>
       <c r="O137" s="37" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="P137" s="37"/>
       <c r="Q137" s="37"/>
       <c r="R137" s="37" t="s">
-        <v>1800</v>
+        <v>1794</v>
       </c>
       <c r="S137" s="22"/>
       <c r="T137" s="22"/>
       <c r="U137" s="22" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="V137" s="22"/>
       <c r="W137" s="37" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="X137" s="22"/>
       <c r="Y137" s="37" t="s">
-        <v>1534</v>
+        <v>1531</v>
       </c>
       <c r="Z137" s="22"/>
       <c r="AA137" s="39" t="s">
-        <v>1572</v>
+        <v>1566</v>
       </c>
       <c r="AB137" s="22"/>
       <c r="AC137" s="22" t="s">
-        <v>1618</v>
+        <v>1612</v>
       </c>
       <c r="AD137" s="22"/>
       <c r="AE137" s="22" t="s">
-        <v>1680</v>
+        <v>1674</v>
       </c>
       <c r="AF137" s="22"/>
       <c r="AG137" s="22"/>
@@ -26608,61 +26607,61 @@
         <v>Sao Paulo - Summary</v>
       </c>
       <c r="C138" s="23" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="D138" s="22"/>
       <c r="E138" s="22" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="F138" s="22"/>
       <c r="G138" s="22" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="H138" s="23"/>
       <c r="I138" s="23" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="J138" s="22"/>
       <c r="K138" s="37" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="L138" s="37"/>
       <c r="M138" s="37" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="N138" s="22"/>
       <c r="O138" s="37" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="P138" s="37"/>
       <c r="Q138" s="37"/>
       <c r="R138" s="37" t="s">
-        <v>1801</v>
+        <v>1795</v>
       </c>
       <c r="S138" s="22"/>
       <c r="T138" s="22"/>
       <c r="U138" s="22" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="V138" s="22"/>
       <c r="W138" s="37" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="X138" s="22"/>
       <c r="Y138" s="37" t="s">
-        <v>1535</v>
+        <v>1532</v>
       </c>
       <c r="Z138" s="22"/>
       <c r="AA138" s="39" t="s">
-        <v>1573</v>
+        <v>1567</v>
       </c>
       <c r="AB138" s="22"/>
       <c r="AC138" s="22" t="s">
-        <v>1619</v>
+        <v>1613</v>
       </c>
       <c r="AD138" s="22"/>
       <c r="AE138" s="22" t="s">
-        <v>1681</v>
+        <v>1675</v>
       </c>
       <c r="AF138" s="22"/>
       <c r="AG138" s="22"/>
@@ -26676,61 +26675,61 @@
         <v>Hong Kong - Summary</v>
       </c>
       <c r="C139" s="23" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="D139" s="22"/>
       <c r="E139" s="22" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="F139" s="22"/>
       <c r="G139" s="22" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="H139" s="23"/>
       <c r="I139" s="23" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="J139" s="22"/>
       <c r="K139" s="37" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="L139" s="37"/>
       <c r="M139" s="37" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="N139" s="22"/>
       <c r="O139" s="37" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="P139" s="37"/>
       <c r="Q139" s="37"/>
       <c r="R139" s="37" t="s">
-        <v>1802</v>
+        <v>1796</v>
       </c>
       <c r="S139" s="22"/>
       <c r="T139" s="22"/>
       <c r="U139" s="22" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="V139" s="22"/>
       <c r="W139" s="37" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="X139" s="22"/>
       <c r="Y139" s="37" t="s">
-        <v>1536</v>
+        <v>1533</v>
       </c>
       <c r="Z139" s="22"/>
       <c r="AA139" s="39" t="s">
-        <v>1574</v>
+        <v>1568</v>
       </c>
       <c r="AB139" s="22"/>
       <c r="AC139" s="22" t="s">
-        <v>1620</v>
+        <v>1614</v>
       </c>
       <c r="AD139" s="22"/>
       <c r="AE139" s="22" t="s">
-        <v>1682</v>
+        <v>1676</v>
       </c>
       <c r="AF139" s="22"/>
       <c r="AG139" s="22"/>
@@ -26744,61 +26743,61 @@
         <v>Chennai - Summary</v>
       </c>
       <c r="C140" s="23" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="D140" s="22"/>
       <c r="E140" s="22" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="F140" s="22"/>
       <c r="G140" s="22" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="H140" s="23"/>
       <c r="I140" s="23" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="J140" s="22"/>
       <c r="K140" s="37" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="L140" s="37"/>
       <c r="M140" s="37" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="N140" s="22"/>
       <c r="O140" s="37" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="P140" s="37"/>
       <c r="Q140" s="37"/>
       <c r="R140" s="37" t="s">
-        <v>1803</v>
+        <v>1797</v>
       </c>
       <c r="S140" s="22"/>
       <c r="T140" s="22"/>
       <c r="U140" s="22" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="V140" s="22"/>
       <c r="W140" s="37" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="X140" s="22"/>
       <c r="Y140" s="37" t="s">
-        <v>1537</v>
+        <v>1534</v>
       </c>
       <c r="Z140" s="22"/>
       <c r="AA140" s="39" t="s">
-        <v>1575</v>
+        <v>1569</v>
       </c>
       <c r="AB140" s="22"/>
       <c r="AC140" s="22" t="s">
-        <v>1621</v>
+        <v>1615</v>
       </c>
       <c r="AD140" s="22"/>
       <c r="AE140" s="22" t="s">
-        <v>1683</v>
+        <v>1677</v>
       </c>
       <c r="AF140" s="22"/>
       <c r="AG140" s="22"/>
@@ -26812,61 +26811,61 @@
         <v>Bangkok - Summary</v>
       </c>
       <c r="C141" s="23" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="D141" s="22"/>
       <c r="E141" s="22" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="F141" s="22"/>
       <c r="G141" s="22" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="H141" s="23"/>
       <c r="I141" s="23" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="J141" s="22"/>
       <c r="K141" s="37" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="L141" s="37"/>
       <c r="M141" s="37" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="N141" s="22"/>
       <c r="O141" s="37" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="P141" s="37"/>
       <c r="Q141" s="37"/>
       <c r="R141" s="37" t="s">
-        <v>1804</v>
+        <v>1798</v>
       </c>
       <c r="S141" s="22"/>
       <c r="T141" s="22"/>
       <c r="U141" s="22" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="V141" s="22"/>
       <c r="W141" s="37" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="X141" s="22"/>
       <c r="Y141" s="37" t="s">
-        <v>1538</v>
+        <v>1535</v>
       </c>
       <c r="Z141" s="22"/>
       <c r="AA141" s="39" t="s">
-        <v>1576</v>
+        <v>1570</v>
       </c>
       <c r="AB141" s="22"/>
       <c r="AC141" s="22" t="s">
-        <v>1622</v>
+        <v>1616</v>
       </c>
       <c r="AD141" s="22"/>
       <c r="AE141" s="22" t="s">
-        <v>1684</v>
+        <v>1678</v>
       </c>
       <c r="AF141" s="22"/>
       <c r="AG141" s="22"/>
@@ -26880,61 +26879,61 @@
         <v>Hanoi - Summary</v>
       </c>
       <c r="C142" s="23" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="D142" s="22"/>
       <c r="E142" s="22" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="F142" s="22"/>
       <c r="G142" s="22" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="H142" s="23"/>
       <c r="I142" s="23" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="J142" s="22"/>
       <c r="K142" s="37" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="L142" s="37"/>
       <c r="M142" s="37" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="N142" s="22"/>
       <c r="O142" s="37" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="P142" s="37"/>
       <c r="Q142" s="37"/>
       <c r="R142" s="37" t="s">
-        <v>1805</v>
+        <v>1799</v>
       </c>
       <c r="S142" s="22"/>
       <c r="T142" s="22"/>
       <c r="U142" s="22" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="V142" s="22"/>
       <c r="W142" s="37" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="X142" s="22"/>
       <c r="Y142" s="37" t="s">
-        <v>1539</v>
+        <v>1536</v>
       </c>
       <c r="Z142" s="22"/>
       <c r="AA142" s="39" t="s">
-        <v>1577</v>
+        <v>1571</v>
       </c>
       <c r="AB142" s="22"/>
       <c r="AC142" s="22" t="s">
-        <v>1623</v>
+        <v>1617</v>
       </c>
       <c r="AD142" s="22"/>
       <c r="AE142" s="22" t="s">
-        <v>1685</v>
+        <v>1679</v>
       </c>
       <c r="AF142" s="22"/>
       <c r="AG142" s="22"/>
@@ -26948,61 +26947,61 @@
         <v>Graz - Summary</v>
       </c>
       <c r="C143" s="23" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="D143" s="22"/>
       <c r="E143" s="22" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F143" s="22"/>
       <c r="G143" s="22" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="H143" s="23"/>
       <c r="I143" s="23" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="J143" s="22"/>
       <c r="K143" s="37" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="L143" s="37"/>
       <c r="M143" s="37" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="N143" s="22"/>
       <c r="O143" s="37" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="P143" s="37"/>
       <c r="Q143" s="37"/>
       <c r="R143" s="37" t="s">
-        <v>1806</v>
+        <v>1800</v>
       </c>
       <c r="S143" s="22"/>
       <c r="T143" s="22"/>
       <c r="U143" s="22" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="V143" s="22"/>
       <c r="W143" s="37" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="X143" s="22"/>
       <c r="Y143" s="37" t="s">
-        <v>1540</v>
+        <v>1537</v>
       </c>
       <c r="Z143" s="22"/>
       <c r="AA143" s="39" t="s">
-        <v>1578</v>
+        <v>1572</v>
       </c>
       <c r="AB143" s="22"/>
       <c r="AC143" s="22" t="s">
-        <v>1624</v>
+        <v>1618</v>
       </c>
       <c r="AD143" s="22"/>
       <c r="AE143" s="22" t="s">
-        <v>1686</v>
+        <v>1680</v>
       </c>
       <c r="AF143" s="22"/>
       <c r="AG143" s="22"/>
@@ -27016,61 +27015,61 @@
         <v>Ghent - Summary</v>
       </c>
       <c r="C144" s="23" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="D144" s="22"/>
       <c r="E144" s="22" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="F144" s="22"/>
       <c r="G144" s="22" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="H144" s="23"/>
       <c r="I144" s="23" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="J144" s="22"/>
       <c r="K144" s="37" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="L144" s="37"/>
       <c r="M144" s="37" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="N144" s="22"/>
       <c r="O144" s="37" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="P144" s="37"/>
       <c r="Q144" s="37"/>
       <c r="R144" s="37" t="s">
-        <v>1807</v>
+        <v>1801</v>
       </c>
       <c r="S144" s="22"/>
       <c r="T144" s="22"/>
       <c r="U144" s="22" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="V144" s="22"/>
       <c r="W144" s="37" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="X144" s="22"/>
       <c r="Y144" s="37" t="s">
-        <v>1541</v>
+        <v>1538</v>
       </c>
       <c r="Z144" s="22"/>
       <c r="AA144" s="39" t="s">
-        <v>1579</v>
+        <v>1573</v>
       </c>
       <c r="AB144" s="22"/>
       <c r="AC144" s="22" t="s">
-        <v>1625</v>
+        <v>1619</v>
       </c>
       <c r="AD144" s="22"/>
       <c r="AE144" s="22" t="s">
-        <v>1687</v>
+        <v>1681</v>
       </c>
       <c r="AF144" s="22"/>
       <c r="AG144" s="22"/>
@@ -27084,61 +27083,61 @@
         <v>Bern - Summary</v>
       </c>
       <c r="C145" s="23" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="D145" s="22"/>
       <c r="E145" s="22" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="F145" s="22"/>
       <c r="G145" s="22" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="H145" s="23"/>
       <c r="I145" s="23" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="J145" s="22"/>
       <c r="K145" s="37" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="L145" s="37"/>
       <c r="M145" s="37" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="N145" s="22"/>
       <c r="O145" s="37" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="P145" s="37"/>
       <c r="Q145" s="37"/>
       <c r="R145" s="37" t="s">
-        <v>1808</v>
+        <v>1802</v>
       </c>
       <c r="S145" s="22"/>
       <c r="T145" s="22"/>
       <c r="U145" s="22" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="V145" s="22"/>
       <c r="W145" s="37" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="X145" s="22"/>
       <c r="Y145" s="37" t="s">
-        <v>1542</v>
+        <v>1539</v>
       </c>
       <c r="Z145" s="22"/>
       <c r="AA145" s="39" t="s">
-        <v>1580</v>
+        <v>1574</v>
       </c>
       <c r="AB145" s="22"/>
       <c r="AC145" s="22" t="s">
-        <v>1626</v>
+        <v>1620</v>
       </c>
       <c r="AD145" s="22"/>
       <c r="AE145" s="22" t="s">
-        <v>1688</v>
+        <v>1682</v>
       </c>
       <c r="AF145" s="22"/>
       <c r="AG145" s="22"/>
@@ -27152,61 +27151,61 @@
         <v>Olomouc - Summary</v>
       </c>
       <c r="C146" s="23" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="D146" s="22"/>
       <c r="E146" s="22" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="F146" s="22"/>
       <c r="G146" s="22" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="H146" s="23"/>
       <c r="I146" s="23" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="J146" s="22"/>
       <c r="K146" s="37" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="L146" s="37"/>
       <c r="M146" s="37" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="N146" s="22"/>
       <c r="O146" s="37" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="P146" s="37"/>
       <c r="Q146" s="37"/>
       <c r="R146" s="37" t="s">
-        <v>1809</v>
+        <v>1803</v>
       </c>
       <c r="S146" s="22"/>
       <c r="T146" s="22"/>
       <c r="U146" s="22" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="V146" s="22"/>
       <c r="W146" s="37" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="X146" s="22"/>
       <c r="Y146" s="37" t="s">
-        <v>1543</v>
+        <v>1540</v>
       </c>
       <c r="Z146" s="22"/>
       <c r="AA146" s="39" t="s">
-        <v>1581</v>
+        <v>1575</v>
       </c>
       <c r="AB146" s="22"/>
       <c r="AC146" s="22" t="s">
-        <v>1627</v>
+        <v>1621</v>
       </c>
       <c r="AD146" s="22"/>
       <c r="AE146" s="22" t="s">
-        <v>1689</v>
+        <v>1683</v>
       </c>
       <c r="AF146" s="22"/>
       <c r="AG146" s="22"/>
@@ -27220,61 +27219,61 @@
         <v>Cologne - Summary</v>
       </c>
       <c r="C147" s="23" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D147" s="22"/>
       <c r="E147" s="22" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="F147" s="22"/>
       <c r="G147" s="22" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="H147" s="23"/>
       <c r="I147" s="23" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="J147" s="22"/>
       <c r="K147" s="37" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="L147" s="37"/>
       <c r="M147" s="37" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="N147" s="22"/>
       <c r="O147" s="37" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="P147" s="37"/>
       <c r="Q147" s="37"/>
       <c r="R147" s="37" t="s">
-        <v>1810</v>
+        <v>1804</v>
       </c>
       <c r="S147" s="22"/>
       <c r="T147" s="22"/>
       <c r="U147" s="22" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="V147" s="22"/>
       <c r="W147" s="37" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="X147" s="22"/>
       <c r="Y147" s="37" t="s">
-        <v>1544</v>
+        <v>1541</v>
       </c>
       <c r="Z147" s="22"/>
       <c r="AA147" s="39" t="s">
-        <v>1582</v>
+        <v>1576</v>
       </c>
       <c r="AB147" s="22"/>
       <c r="AC147" s="22" t="s">
-        <v>1628</v>
+        <v>1622</v>
       </c>
       <c r="AD147" s="22"/>
       <c r="AE147" s="22" t="s">
-        <v>1690</v>
+        <v>1684</v>
       </c>
       <c r="AF147" s="22"/>
       <c r="AG147" s="22"/>
@@ -27288,61 +27287,61 @@
         <v>Odense - Summary</v>
       </c>
       <c r="C148" s="23" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="D148" s="22"/>
       <c r="E148" s="22" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="F148" s="22"/>
       <c r="G148" s="22" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="H148" s="23"/>
       <c r="I148" s="23" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="J148" s="22"/>
       <c r="K148" s="37" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="L148" s="37"/>
       <c r="M148" s="37" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="N148" s="22"/>
       <c r="O148" s="37" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="P148" s="37"/>
       <c r="Q148" s="37"/>
       <c r="R148" s="37" t="s">
-        <v>1811</v>
+        <v>1805</v>
       </c>
       <c r="S148" s="22"/>
       <c r="T148" s="22"/>
       <c r="U148" s="22" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="V148" s="22"/>
       <c r="W148" s="37" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="X148" s="22"/>
       <c r="Y148" s="37" t="s">
-        <v>1545</v>
+        <v>1542</v>
       </c>
       <c r="Z148" s="22"/>
       <c r="AA148" s="39" t="s">
-        <v>1583</v>
+        <v>1577</v>
       </c>
       <c r="AB148" s="22"/>
       <c r="AC148" s="22" t="s">
-        <v>1629</v>
+        <v>1623</v>
       </c>
       <c r="AD148" s="22"/>
       <c r="AE148" s="22" t="s">
-        <v>1691</v>
+        <v>1685</v>
       </c>
       <c r="AF148" s="22"/>
       <c r="AG148" s="22"/>
@@ -27356,63 +27355,63 @@
         <v>Barcelona - Summary</v>
       </c>
       <c r="C149" s="23" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="D149" s="22"/>
       <c r="E149" s="22" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="F149" s="22"/>
       <c r="G149" s="22" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="H149" s="23"/>
       <c r="I149" s="23" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="J149" s="22"/>
       <c r="K149" s="37" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="L149" s="37"/>
       <c r="M149" s="37" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="N149" s="22"/>
       <c r="O149" s="37" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="P149" s="37"/>
       <c r="Q149" s="37"/>
       <c r="R149" s="37" t="s">
-        <v>1812</v>
+        <v>1806</v>
       </c>
       <c r="S149" s="22"/>
       <c r="T149" s="22" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="U149" s="22" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="V149" s="22"/>
       <c r="W149" s="37" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="X149" s="22"/>
       <c r="Y149" s="37" t="s">
-        <v>1546</v>
+        <v>1543</v>
       </c>
       <c r="Z149" s="22"/>
       <c r="AA149" s="39" t="s">
-        <v>1584</v>
+        <v>1578</v>
       </c>
       <c r="AB149" s="22"/>
       <c r="AC149" s="22" t="s">
-        <v>1630</v>
+        <v>1624</v>
       </c>
       <c r="AD149" s="22"/>
       <c r="AE149" s="22" t="s">
-        <v>1692</v>
+        <v>1686</v>
       </c>
       <c r="AF149" s="22"/>
       <c r="AG149" s="22"/>
@@ -27426,63 +27425,63 @@
         <v>Valencia - Summary</v>
       </c>
       <c r="C150" s="23" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="D150" s="22"/>
       <c r="E150" s="22" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="F150" s="22"/>
       <c r="G150" s="22" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="H150" s="23"/>
       <c r="I150" s="23" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="J150" s="22"/>
       <c r="K150" s="37" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="L150" s="37"/>
       <c r="M150" s="37" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="N150" s="22"/>
       <c r="O150" s="37" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="P150" s="37"/>
       <c r="Q150" s="37"/>
       <c r="R150" s="37" t="s">
-        <v>1813</v>
+        <v>1807</v>
       </c>
       <c r="S150" s="22"/>
       <c r="T150" s="22" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="U150" s="22" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="V150" s="22"/>
       <c r="W150" s="37" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="X150" s="22"/>
       <c r="Y150" s="37" t="s">
-        <v>1547</v>
+        <v>1544</v>
       </c>
       <c r="Z150" s="22"/>
       <c r="AA150" s="39" t="s">
-        <v>1585</v>
+        <v>1579</v>
       </c>
       <c r="AB150" s="22"/>
       <c r="AC150" s="22" t="s">
-        <v>1631</v>
+        <v>1625</v>
       </c>
       <c r="AD150" s="22"/>
       <c r="AE150" s="22" t="s">
-        <v>1693</v>
+        <v>1687</v>
       </c>
       <c r="AF150" s="22"/>
       <c r="AG150" s="22"/>
@@ -27496,63 +27495,63 @@
         <v>Vic - Summary</v>
       </c>
       <c r="C151" s="23" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="D151" s="22"/>
       <c r="E151" s="22" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="F151" s="22"/>
       <c r="G151" s="22" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="H151" s="23"/>
       <c r="I151" s="23" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="J151" s="22"/>
       <c r="K151" s="37" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="L151" s="37"/>
       <c r="M151" s="37" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="N151" s="22"/>
       <c r="O151" s="37" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="P151" s="37"/>
       <c r="Q151" s="37"/>
       <c r="R151" s="37" t="s">
-        <v>1814</v>
+        <v>1808</v>
       </c>
       <c r="S151" s="22"/>
       <c r="T151" s="22" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="U151" s="22" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="V151" s="22"/>
       <c r="W151" s="37" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="X151" s="22"/>
       <c r="Y151" s="37" t="s">
-        <v>1548</v>
+        <v>1545</v>
       </c>
       <c r="Z151" s="22"/>
       <c r="AA151" s="39" t="s">
-        <v>1586</v>
+        <v>1580</v>
       </c>
       <c r="AB151" s="22"/>
       <c r="AC151" s="22" t="s">
-        <v>1632</v>
+        <v>1626</v>
       </c>
       <c r="AD151" s="22"/>
       <c r="AE151" s="22" t="s">
-        <v>1694</v>
+        <v>1688</v>
       </c>
       <c r="AF151" s="22"/>
       <c r="AG151" s="22"/>
@@ -27566,61 +27565,61 @@
         <v>Belfast - Summary</v>
       </c>
       <c r="C152" s="23" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="D152" s="22"/>
       <c r="E152" s="22" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="F152" s="22"/>
       <c r="G152" s="22" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="H152" s="23"/>
       <c r="I152" s="23" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="J152" s="22"/>
       <c r="K152" s="37" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="L152" s="37"/>
       <c r="M152" s="37" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="N152" s="22"/>
       <c r="O152" s="37" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="P152" s="37"/>
       <c r="Q152" s="37"/>
       <c r="R152" s="37" t="s">
-        <v>1815</v>
+        <v>1809</v>
       </c>
       <c r="S152" s="22"/>
       <c r="T152" s="22"/>
       <c r="U152" s="22" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="V152" s="22"/>
       <c r="W152" s="37" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="X152" s="22"/>
       <c r="Y152" s="37" t="s">
-        <v>1549</v>
+        <v>1546</v>
       </c>
       <c r="Z152" s="22"/>
       <c r="AA152" s="39" t="s">
-        <v>1587</v>
+        <v>1581</v>
       </c>
       <c r="AB152" s="22"/>
       <c r="AC152" s="22" t="s">
-        <v>1633</v>
+        <v>1627</v>
       </c>
       <c r="AD152" s="22"/>
       <c r="AE152" s="22" t="s">
-        <v>1695</v>
+        <v>1689</v>
       </c>
       <c r="AF152" s="22"/>
       <c r="AG152" s="22"/>
@@ -27634,61 +27633,61 @@
         <v>Lisbon - Summary</v>
       </c>
       <c r="C153" s="23" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="D153" s="22"/>
       <c r="E153" s="22" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="F153" s="22"/>
       <c r="G153" s="22" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="H153" s="23"/>
       <c r="I153" s="23" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="J153" s="22"/>
       <c r="K153" s="37" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="L153" s="37"/>
       <c r="M153" s="37" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="N153" s="22"/>
       <c r="O153" s="37" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="P153" s="37"/>
       <c r="Q153" s="37"/>
       <c r="R153" s="37" t="s">
-        <v>1816</v>
+        <v>1810</v>
       </c>
       <c r="S153" s="22"/>
       <c r="T153" s="22"/>
       <c r="U153" s="22" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="V153" s="22"/>
       <c r="W153" s="37" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="X153" s="22"/>
       <c r="Y153" s="37" t="s">
-        <v>1550</v>
+        <v>1547</v>
       </c>
       <c r="Z153" s="22"/>
       <c r="AA153" s="39" t="s">
-        <v>1588</v>
+        <v>1582</v>
       </c>
       <c r="AB153" s="22"/>
       <c r="AC153" s="22" t="s">
-        <v>1634</v>
+        <v>1628</v>
       </c>
       <c r="AD153" s="22"/>
       <c r="AE153" s="22" t="s">
-        <v>1696</v>
+        <v>1690</v>
       </c>
       <c r="AF153" s="22"/>
       <c r="AG153" s="22"/>
@@ -27702,61 +27701,61 @@
         <v>Adelaide - Summary</v>
       </c>
       <c r="C154" s="23" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="D154" s="22"/>
       <c r="E154" s="22" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="F154" s="22"/>
       <c r="G154" s="22" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="H154" s="23"/>
       <c r="I154" s="23" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="J154" s="22"/>
       <c r="K154" s="37" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="L154" s="37"/>
       <c r="M154" s="37" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="N154" s="22"/>
       <c r="O154" s="37" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="P154" s="37"/>
       <c r="Q154" s="37"/>
       <c r="R154" s="37" t="s">
-        <v>1817</v>
+        <v>1811</v>
       </c>
       <c r="S154" s="22"/>
       <c r="T154" s="22"/>
       <c r="U154" s="22" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="V154" s="22"/>
       <c r="W154" s="37" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="X154" s="22"/>
       <c r="Y154" s="37" t="s">
-        <v>1551</v>
+        <v>1548</v>
       </c>
       <c r="Z154" s="22"/>
       <c r="AA154" s="39" t="s">
-        <v>1589</v>
+        <v>1583</v>
       </c>
       <c r="AB154" s="22"/>
       <c r="AC154" s="22" t="s">
-        <v>1635</v>
+        <v>1629</v>
       </c>
       <c r="AD154" s="22"/>
       <c r="AE154" s="22" t="s">
-        <v>1697</v>
+        <v>1691</v>
       </c>
       <c r="AF154" s="22"/>
       <c r="AG154" s="22"/>
@@ -27770,61 +27769,61 @@
         <v>Melbourne - Summary</v>
       </c>
       <c r="C155" s="23" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="D155" s="22"/>
       <c r="E155" s="22" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="F155" s="22"/>
       <c r="G155" s="22" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="H155" s="23"/>
       <c r="I155" s="23" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="J155" s="22"/>
       <c r="K155" s="37" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="L155" s="37"/>
       <c r="M155" s="37" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="N155" s="22"/>
       <c r="O155" s="37" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="P155" s="37"/>
       <c r="Q155" s="37"/>
       <c r="R155" s="37" t="s">
-        <v>1818</v>
+        <v>1812</v>
       </c>
       <c r="S155" s="22"/>
       <c r="T155" s="22"/>
       <c r="U155" s="22" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="V155" s="22"/>
       <c r="W155" s="37" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="X155" s="22"/>
       <c r="Y155" s="37" t="s">
-        <v>1552</v>
+        <v>1549</v>
       </c>
       <c r="Z155" s="22"/>
       <c r="AA155" s="39" t="s">
-        <v>1590</v>
+        <v>1584</v>
       </c>
       <c r="AB155" s="22"/>
       <c r="AC155" s="22" t="s">
-        <v>1636</v>
+        <v>1630</v>
       </c>
       <c r="AD155" s="22"/>
       <c r="AE155" s="22" t="s">
-        <v>1698</v>
+        <v>1692</v>
       </c>
       <c r="AF155" s="22"/>
       <c r="AG155" s="22"/>
@@ -27838,61 +27837,61 @@
         <v>Sydney - Summary</v>
       </c>
       <c r="C156" s="23" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="D156" s="22"/>
       <c r="E156" s="22" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="F156" s="22"/>
       <c r="G156" s="22" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="H156" s="23"/>
       <c r="I156" s="23" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="J156" s="22"/>
       <c r="K156" s="37" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="L156" s="37"/>
       <c r="M156" s="37" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="N156" s="22"/>
       <c r="O156" s="37" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="P156" s="37"/>
       <c r="Q156" s="37"/>
       <c r="R156" s="37" t="s">
-        <v>1819</v>
+        <v>1813</v>
       </c>
       <c r="S156" s="22"/>
       <c r="T156" s="22"/>
       <c r="U156" s="22" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="V156" s="22"/>
       <c r="W156" s="37" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="X156" s="22"/>
       <c r="Y156" s="37" t="s">
-        <v>1553</v>
+        <v>1550</v>
       </c>
       <c r="Z156" s="22"/>
       <c r="AA156" s="39" t="s">
-        <v>1591</v>
+        <v>1585</v>
       </c>
       <c r="AB156" s="22"/>
       <c r="AC156" s="22" t="s">
-        <v>1637</v>
+        <v>1631</v>
       </c>
       <c r="AD156" s="22"/>
       <c r="AE156" s="22" t="s">
-        <v>1699</v>
+        <v>1693</v>
       </c>
       <c r="AF156" s="22"/>
       <c r="AG156" s="22"/>
@@ -27906,61 +27905,61 @@
         <v>Auckland - Summary</v>
       </c>
       <c r="C157" s="26" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="D157" s="22"/>
       <c r="E157" s="22" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="F157" s="22"/>
       <c r="G157" s="22" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="H157" s="26"/>
       <c r="I157" s="26" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="J157" s="22"/>
       <c r="K157" s="37" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="L157" s="37"/>
       <c r="M157" s="37" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="N157" s="22"/>
       <c r="O157" s="37" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="P157" s="37"/>
       <c r="Q157" s="37"/>
       <c r="R157" s="37" t="s">
-        <v>1820</v>
+        <v>1814</v>
       </c>
       <c r="S157" s="22"/>
       <c r="T157" s="22"/>
       <c r="U157" s="22" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="V157" s="22"/>
       <c r="W157" s="37" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="X157" s="22"/>
       <c r="Y157" s="37" t="s">
-        <v>1554</v>
+        <v>1551</v>
       </c>
       <c r="Z157" s="22"/>
       <c r="AA157" s="39" t="s">
-        <v>1592</v>
+        <v>1586</v>
       </c>
       <c r="AB157" s="22"/>
       <c r="AC157" s="22" t="s">
-        <v>1638</v>
+        <v>1632</v>
       </c>
       <c r="AD157" s="22"/>
       <c r="AE157" s="22" t="s">
-        <v>1700</v>
+        <v>1694</v>
       </c>
       <c r="AF157" s="22"/>
       <c r="AG157" s="22"/>

</xml_diff>

<commit_message>
further update to Maiduguri prose
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\global-indicators\analysis\global_scorecards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BA851C-3438-41C7-8E89-FB22A6E580EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF4CBD5-8716-4FCA-8EF9-C62BE5B05005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32475" yWindow="3225" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
@@ -5752,14 +5752,14 @@
     <t>(மேலே) {:.1f}% மக்கள் தொகை, அக்கம்பக்க தெரு வெட்டு அடர்த்திக்கான குறைந்தபட்ச வரம்பு* ({:,} {})</t>
   </si>
   <si>
-    <t>The availability and quality of urban and transport policies and neighbourhood infrastructure supporting health and sustainability in Maiduguri was found to be below average compared with other cities.   Although Maiduguri has air pollution policy related to land use, it appears to lack city planning requirements that include other specific health-focussed actions, and specific and measureable standards to create walkable neighbourhoods and equitable access to public transport and public open space. Spatial data availability for Maiduguri was limited and this may partially explain our spatial findings that follow. Relative to the 25 cities in this international study, the majority of neighbourhoods in Maiduguri do not appear to be walkable, and any walkable neighbourhoods appear to be spatially patterned along major road networks. In terms of thresholds for built environment interventions to achieve WHO targets to increase physical activity, 95.9% of residents in Maiduguri live in neighbourhoods that meet the density threshold, although only 29% live in neighbourhoods that meet street connectivity thresholds. The latter could reflect lack of data that on informal routes. Notably, many Maiduguri residents may live in neighbourhoods that exceed levels of population density that encourage physical activity. Only 10% of residents have access to public transport stops, with evidence that access is spatially patterned along major road networks. Very few residents have access to public open space within 500m, and only 0.5% of residents have access to larger public open space, concentrated in the city's northeast.</t>
+    <t>The availability and quality of urban and transport policies and neighbourhood infrastructure supporting health and sustainability in Maiduguri was found to be below average compared with other cities.   Although Maiduguri has air pollution policy related to land use, it appears to lack city planning requirements that include other specific health-focussed actions, and specific and measureable standards to create walkable neighbourhoods and equitable access to public transport and public open space. Spatial data availability for Maiduguri was limited and this may partially explain our spatial findings that follow. Relative to the 25 cities in this international study, the majority of neighbourhoods in Maiduguri do not appear to be walkable, and any walkable neighbourhoods appear to be spatially patterned along major road networks. In terms of thresholds for built environment interventions to achieve WHO targets to increase physical activity, 95.9% of residents in Maiduguri live in neighbourhoods that meet the density threshold, although only 29% live in neighbourhoods that meet street connectivity thresholds. The latter could reflect lack of data on informal routes. Notably, many Maiduguri residents appear to live in neighbourhoods that exceed levels of population density that encourage physical activity. Only 10% of residents have access to public transport stops, with evidence that access is spatially patterned along major road networks. Very few residents have access to public open space within 500m, and only 0.5% of residents have access to larger public open space, concentrated in the city's northeast.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6907,13 +6907,13 @@
       <selection pane="bottomLeft" activeCell="L185" sqref="L185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.140625" customWidth="1"/>
     <col min="16" max="16" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="4" customFormat="1">
+    <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -6975,7 +6975,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -7035,7 +7035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>569</v>
       </c>
@@ -7092,7 +7092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>570</v>
       </c>
@@ -7148,7 +7148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -7205,7 +7205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>239</v>
       </c>
@@ -7263,7 +7263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -7316,7 +7316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -7373,7 +7373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -7426,7 +7426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>225</v>
       </c>
@@ -7483,7 +7483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>225</v>
       </c>
@@ -7536,7 +7536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -7592,7 +7592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>238</v>
       </c>
@@ -7655,7 +7655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>363</v>
       </c>
@@ -7715,7 +7715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -7775,7 +7775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -7832,7 +7832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -7888,7 +7888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -7944,7 +7944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>268</v>
       </c>
@@ -8003,7 +8003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>104</v>
       </c>
@@ -8060,7 +8060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -8119,7 +8119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>269</v>
       </c>
@@ -8178,7 +8178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>105</v>
       </c>
@@ -8235,7 +8235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -8294,7 +8294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -8353,7 +8353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>240</v>
       </c>
@@ -8413,7 +8413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -8473,7 +8473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>271</v>
       </c>
@@ -8535,7 +8535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>270</v>
       </c>
@@ -8597,7 +8597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>86</v>
       </c>
@@ -8654,7 +8654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -8710,7 +8710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>102</v>
       </c>
@@ -8766,7 +8766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -8829,7 +8829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -8892,7 +8892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A34,LEN("policy2_text")+1,1),"_middle")</f>
         <v>policy2_text1_middle</v>
@@ -8956,7 +8956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A35,LEN("policy2_text")+1,1),"_upper")</f>
         <v>policy2_text1_upper</v>
@@ -9020,7 +9020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>58</v>
       </c>
@@ -9080,7 +9080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>59</v>
       </c>
@@ -9143,7 +9143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -9206,7 +9206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A39,LEN("policy2_text")+1,1),"_middle")</f>
         <v>policy2_text2_middle</v>
@@ -9270,7 +9270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A40,LEN("policy2_text")+1,1),"_upper")</f>
         <v>policy2_text2_upper</v>
@@ -9334,7 +9334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -9394,7 +9394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -9457,7 +9457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -9520,7 +9520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A44,LEN("policy2_text")+1,1),"_middle")</f>
         <v>policy2_text3_middle</v>
@@ -9584,7 +9584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A45,LEN("policy2_text")+1,1),"_upper")</f>
         <v>policy2_text3_upper</v>
@@ -9648,7 +9648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>66</v>
       </c>
@@ -9708,7 +9708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>67</v>
       </c>
@@ -9771,7 +9771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>68</v>
       </c>
@@ -9834,7 +9834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A49,LEN("policy2_text")+1,1),"_middle")</f>
         <v>policy2_text4_middle</v>
@@ -9898,7 +9898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A50,LEN("policy2_text")+1,1),"_upper")</f>
         <v>policy2_text4_upper</v>
@@ -9962,7 +9962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:20">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>70</v>
       </c>
@@ -10022,7 +10022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:20">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>71</v>
       </c>
@@ -10085,7 +10085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:20">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>72</v>
       </c>
@@ -10148,7 +10148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:20">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A54,LEN("policy2_text")+1,1),"_middle")</f>
         <v>policy2_text5_middle</v>
@@ -10212,7 +10212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:20">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A55,LEN("policy2_text")+1,1),"_upper")</f>
         <v>policy2_text5_upper</v>
@@ -10276,7 +10276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:20">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>73</v>
       </c>
@@ -10336,7 +10336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:20">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>74</v>
       </c>
@@ -10399,7 +10399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:20">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>75</v>
       </c>
@@ -10462,7 +10462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:20">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A59,LEN("policy2_text")+1,1),"_middle")</f>
         <v>policy2_text6_middle</v>
@@ -10526,7 +10526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:20">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f>_xlfn.CONCAT("policy2_text",MID(A60,LEN("policy2_text")+1,1),"_upper")</f>
         <v>policy2_text6_upper</v>
@@ -10590,7 +10590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:20">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>76</v>
       </c>
@@ -10650,7 +10650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:20">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>45</v>
       </c>
@@ -10708,7 +10708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:20">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>84</v>
       </c>
@@ -10768,7 +10768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:20">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>46</v>
       </c>
@@ -10824,7 +10824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:20">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>1132</v>
       </c>
@@ -10884,7 +10884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:20">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>77</v>
       </c>
@@ -10942,7 +10942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:20">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>228</v>
       </c>
@@ -11002,7 +11002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:20">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>96</v>
       </c>
@@ -11062,7 +11062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:20">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>97</v>
       </c>
@@ -11122,7 +11122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:20">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>98</v>
       </c>
@@ -11182,7 +11182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:20">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>99</v>
       </c>
@@ -11242,7 +11242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:20">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>86</v>
       </c>
@@ -11299,7 +11299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:20">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>87</v>
       </c>
@@ -11356,7 +11356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:20">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>88</v>
       </c>
@@ -11413,7 +11413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:20">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>102</v>
       </c>
@@ -11470,7 +11470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:20">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>107</v>
       </c>
@@ -11530,7 +11530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:20">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>108</v>
       </c>
@@ -11590,7 +11590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:20">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>109</v>
       </c>
@@ -11650,7 +11650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:20">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>110</v>
       </c>
@@ -11710,7 +11710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:20">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>111</v>
       </c>
@@ -11770,7 +11770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:20">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>112</v>
       </c>
@@ -11830,7 +11830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:20">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>113</v>
       </c>
@@ -11890,7 +11890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:20">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>114</v>
       </c>
@@ -11950,7 +11950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:20">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>115</v>
       </c>
@@ -12010,7 +12010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:20">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>116</v>
       </c>
@@ -12070,7 +12070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:20">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>117</v>
       </c>
@@ -12130,7 +12130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:20">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>118</v>
       </c>
@@ -12190,7 +12190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:20">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>119</v>
       </c>
@@ -12250,7 +12250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:20">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>120</v>
       </c>
@@ -12310,7 +12310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:20">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>121</v>
       </c>
@@ -12370,7 +12370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:20">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>122</v>
       </c>
@@ -12430,7 +12430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:20">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>123</v>
       </c>
@@ -12490,7 +12490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:20">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>124</v>
       </c>
@@ -12550,7 +12550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:20">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>125</v>
       </c>
@@ -12610,7 +12610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:20">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>126</v>
       </c>
@@ -12670,7 +12670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:20">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>127</v>
       </c>
@@ -12730,7 +12730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:20">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>128</v>
       </c>
@@ -12790,7 +12790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:20">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>129</v>
       </c>
@@ -12850,7 +12850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:20">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>130</v>
       </c>
@@ -12910,7 +12910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:20">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>131</v>
       </c>
@@ -12970,7 +12970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:20">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>132</v>
       </c>
@@ -13030,7 +13030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:20">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>133</v>
       </c>
@@ -13090,7 +13090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:20">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>134</v>
       </c>
@@ -13150,7 +13150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:20">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>135</v>
       </c>
@@ -13210,7 +13210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:20">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>136</v>
       </c>
@@ -13270,7 +13270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:20">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>137</v>
       </c>
@@ -13330,7 +13330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:20">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>138</v>
       </c>
@@ -13390,7 +13390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:20">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>139</v>
       </c>
@@ -13450,7 +13450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:20">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>140</v>
       </c>
@@ -13510,7 +13510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:20">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>141</v>
       </c>
@@ -13570,7 +13570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:20">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>47</v>
       </c>
@@ -13627,7 +13627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:20">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>48</v>
       </c>
@@ -13682,7 +13682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:20">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>1128</v>
       </c>
@@ -13742,7 +13742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:20">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>78</v>
       </c>
@@ -13799,7 +13799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:20">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>79</v>
       </c>
@@ -13855,7 +13855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:20">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>1129</v>
       </c>
@@ -13915,7 +13915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:20">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>307</v>
       </c>
@@ -13975,7 +13975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:20">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>1131</v>
       </c>
@@ -14032,7 +14032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:20">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>241</v>
       </c>
@@ -14086,7 +14086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:20">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>242</v>
       </c>
@@ -14143,7 +14143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:20">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>80</v>
       </c>
@@ -14199,7 +14199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:20">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>162</v>
       </c>
@@ -14258,7 +14258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:20">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>178</v>
       </c>
@@ -14314,7 +14314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:20">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>171</v>
       </c>
@@ -14373,7 +14373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:20">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>231</v>
       </c>
@@ -14433,7 +14433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:20">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>96</v>
       </c>
@@ -14493,7 +14493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:20">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>97</v>
       </c>
@@ -14553,7 +14553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:20">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>98</v>
       </c>
@@ -14613,7 +14613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:20">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>99</v>
       </c>
@@ -14673,7 +14673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:20">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>86</v>
       </c>
@@ -14730,7 +14730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:20">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>87</v>
       </c>
@@ -14787,7 +14787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:20">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>88</v>
       </c>
@@ -14844,7 +14844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:20">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>102</v>
       </c>
@@ -14900,7 +14900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:20">
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>142</v>
       </c>
@@ -14960,7 +14960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:20">
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>143</v>
       </c>
@@ -15020,7 +15020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:20">
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>144</v>
       </c>
@@ -15080,7 +15080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:20">
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>145</v>
       </c>
@@ -15140,7 +15140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:20">
+    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>146</v>
       </c>
@@ -15200,7 +15200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:20">
+    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>147</v>
       </c>
@@ -15260,7 +15260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:20">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>148</v>
       </c>
@@ -15320,7 +15320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:20">
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>149</v>
       </c>
@@ -15380,7 +15380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:20">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>150</v>
       </c>
@@ -15440,7 +15440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:20">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>151</v>
       </c>
@@ -15500,7 +15500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:20">
+    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>152</v>
       </c>
@@ -15560,7 +15560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:20">
+    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>153</v>
       </c>
@@ -15620,7 +15620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:20">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>154</v>
       </c>
@@ -15680,7 +15680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:20">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>155</v>
       </c>
@@ -15740,7 +15740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:20">
+    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>156</v>
       </c>
@@ -15800,7 +15800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:20">
+    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>157</v>
       </c>
@@ -15860,7 +15860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:20">
+    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>158</v>
       </c>
@@ -15920,7 +15920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:20">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>159</v>
       </c>
@@ -15980,7 +15980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:20">
+    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>160</v>
       </c>
@@ -16040,7 +16040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:20">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>161</v>
       </c>
@@ -16100,7 +16100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:20">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>81</v>
       </c>
@@ -16158,7 +16158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:20">
+    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>173</v>
       </c>
@@ -16217,7 +16217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:20">
+    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>82</v>
       </c>
@@ -16273,7 +16273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:20">
+    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>172</v>
       </c>
@@ -16332,7 +16332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:20">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>232</v>
       </c>
@@ -16391,7 +16391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:20">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>96</v>
       </c>
@@ -16451,7 +16451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:20">
+    <row r="161" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>97</v>
       </c>
@@ -16511,7 +16511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:20">
+    <row r="162" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>98</v>
       </c>
@@ -16571,7 +16571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:20">
+    <row r="163" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>99</v>
       </c>
@@ -16631,7 +16631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:20">
+    <row r="164" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>86</v>
       </c>
@@ -16688,7 +16688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:20">
+    <row r="165" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>87</v>
       </c>
@@ -16745,7 +16745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:20">
+    <row r="166" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>88</v>
       </c>
@@ -16802,7 +16802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:20">
+    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>102</v>
       </c>
@@ -16859,7 +16859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:20">
+    <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>165</v>
       </c>
@@ -16919,7 +16919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:20">
+    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>166</v>
       </c>
@@ -16979,7 +16979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:20">
+    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>167</v>
       </c>
@@ -17039,7 +17039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:20">
+    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>168</v>
       </c>
@@ -17099,7 +17099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:20">
+    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>169</v>
       </c>
@@ -17159,7 +17159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:20">
+    <row r="173" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>364</v>
       </c>
@@ -17216,7 +17216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:20">
+    <row r="174" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>365</v>
       </c>
@@ -17275,7 +17275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:20">
+    <row r="175" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>235</v>
       </c>
@@ -17335,7 +17335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:20">
+    <row r="176" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>83</v>
       </c>
@@ -17392,7 +17392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:20">
+    <row r="177" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>41</v>
       </c>
@@ -17445,7 +17445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:20">
+    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>176</v>
       </c>
@@ -17503,7 +17503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:20">
+    <row r="179" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>314</v>
       </c>
@@ -17560,7 +17560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="18" customHeight="1">
+    <row r="180" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>308</v>
       </c>
@@ -17622,7 +17622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:20">
+    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>27</v>
       </c>
@@ -17676,7 +17676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:20">
+    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>28</v>
       </c>
@@ -17731,7 +17731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:20">
+    <row r="183" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>29</v>
       </c>
@@ -17785,7 +17785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:20">
+    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>30</v>
       </c>
@@ -17839,7 +17839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:20">
+    <row r="185" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>31</v>
       </c>
@@ -17893,7 +17893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:20">
+    <row r="186" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>32</v>
       </c>
@@ -17947,7 +17947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:20">
+    <row r="187" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>33</v>
       </c>
@@ -18001,7 +18001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:20">
+    <row r="188" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>34</v>
       </c>
@@ -18055,7 +18055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:20">
+    <row r="189" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>35</v>
       </c>
@@ -18109,7 +18109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:20">
+    <row r="190" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>36</v>
       </c>
@@ -18163,7 +18163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:20">
+    <row r="191" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>37</v>
       </c>
@@ -18232,13 +18232,13 @@
   <dimension ref="A1:AG157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AA132" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D133" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA133" sqref="AA133"/>
+      <selection pane="bottomRight" activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="30" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" style="30" customWidth="1"/>
@@ -18248,7 +18248,7 @@
     <col min="34" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="29" customFormat="1">
+    <row r="1" spans="1:33" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>190</v>
       </c>
@@ -18345,7 +18345,7 @@
       <c r="AF1" s="19"/>
       <c r="AG1" s="19"/>
     </row>
-    <row r="2" spans="1:33" s="31" customFormat="1">
+    <row r="2" spans="1:33" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>191</v>
       </c>
@@ -18430,7 +18430,7 @@
       <c r="AF2" s="20"/>
       <c r="AG2" s="20"/>
     </row>
-    <row r="3" spans="1:33" ht="15" customHeight="1">
+    <row r="3" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>191</v>
       </c>
@@ -18501,7 +18501,7 @@
       <c r="AF3" s="22"/>
       <c r="AG3" s="22"/>
     </row>
-    <row r="4" spans="1:33" ht="15" customHeight="1">
+    <row r="4" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>191</v>
       </c>
@@ -18572,7 +18572,7 @@
       <c r="AF4" s="22"/>
       <c r="AG4" s="22"/>
     </row>
-    <row r="5" spans="1:33" ht="42.75">
+    <row r="5" spans="1:33" ht="33" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>191</v>
       </c>
@@ -18643,7 +18643,7 @@
       <c r="AF5" s="22"/>
       <c r="AG5" s="22"/>
     </row>
-    <row r="6" spans="1:33" ht="15" customHeight="1">
+    <row r="6" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>191</v>
       </c>
@@ -18684,7 +18684,7 @@
       <c r="AF6" s="22"/>
       <c r="AG6" s="22"/>
     </row>
-    <row r="7" spans="1:33" ht="15" customHeight="1">
+    <row r="7" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>191</v>
       </c>
@@ -18729,7 +18729,7 @@
       <c r="AF7" s="22"/>
       <c r="AG7" s="22"/>
     </row>
-    <row r="8" spans="1:33" ht="15" customHeight="1">
+    <row r="8" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>191</v>
       </c>
@@ -18770,7 +18770,7 @@
       <c r="AF8" s="22"/>
       <c r="AG8" s="22"/>
     </row>
-    <row r="9" spans="1:33" ht="15" customHeight="1">
+    <row r="9" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>191</v>
       </c>
@@ -18811,7 +18811,7 @@
       <c r="AF9" s="22"/>
       <c r="AG9" s="22"/>
     </row>
-    <row r="10" spans="1:33" ht="15" customHeight="1">
+    <row r="10" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>191</v>
       </c>
@@ -18852,7 +18852,7 @@
       <c r="AF10" s="22"/>
       <c r="AG10" s="22"/>
     </row>
-    <row r="11" spans="1:33" ht="15" customHeight="1">
+    <row r="11" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>191</v>
       </c>
@@ -18895,7 +18895,7 @@
       <c r="AF11" s="22"/>
       <c r="AG11" s="22"/>
     </row>
-    <row r="12" spans="1:33" ht="15" customHeight="1">
+    <row r="12" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>191</v>
       </c>
@@ -18938,7 +18938,7 @@
       <c r="AF12" s="22"/>
       <c r="AG12" s="22"/>
     </row>
-    <row r="13" spans="1:33" ht="15" customHeight="1">
+    <row r="13" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>191</v>
       </c>
@@ -18981,7 +18981,7 @@
       <c r="AF13" s="22"/>
       <c r="AG13" s="22"/>
     </row>
-    <row r="14" spans="1:33" ht="15" customHeight="1">
+    <row r="14" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>191</v>
       </c>
@@ -19024,7 +19024,7 @@
       <c r="AF14" s="22"/>
       <c r="AG14" s="22"/>
     </row>
-    <row r="15" spans="1:33" ht="15" customHeight="1">
+    <row r="15" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>191</v>
       </c>
@@ -19067,7 +19067,7 @@
       <c r="AF15" s="22"/>
       <c r="AG15" s="22"/>
     </row>
-    <row r="16" spans="1:33" ht="15" customHeight="1">
+    <row r="16" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>191</v>
       </c>
@@ -19110,7 +19110,7 @@
       <c r="AF16" s="22"/>
       <c r="AG16" s="22"/>
     </row>
-    <row r="17" spans="1:33" ht="15" customHeight="1">
+    <row r="17" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>191</v>
       </c>
@@ -19153,7 +19153,7 @@
       <c r="AF17" s="22"/>
       <c r="AG17" s="22"/>
     </row>
-    <row r="18" spans="1:33" ht="15" customHeight="1">
+    <row r="18" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>191</v>
       </c>
@@ -19196,7 +19196,7 @@
       <c r="AF18" s="22"/>
       <c r="AG18" s="22"/>
     </row>
-    <row r="19" spans="1:33" ht="15" customHeight="1">
+    <row r="19" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>191</v>
       </c>
@@ -19239,7 +19239,7 @@
       <c r="AF19" s="22"/>
       <c r="AG19" s="22"/>
     </row>
-    <row r="20" spans="1:33" ht="15" customHeight="1">
+    <row r="20" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>191</v>
       </c>
@@ -19282,7 +19282,7 @@
       <c r="AF20" s="22"/>
       <c r="AG20" s="22"/>
     </row>
-    <row r="21" spans="1:33" ht="15" customHeight="1">
+    <row r="21" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>191</v>
       </c>
@@ -19325,7 +19325,7 @@
       <c r="AF21" s="22"/>
       <c r="AG21" s="22"/>
     </row>
-    <row r="22" spans="1:33" ht="15" customHeight="1">
+    <row r="22" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>191</v>
       </c>
@@ -19372,7 +19372,7 @@
       <c r="AF22" s="22"/>
       <c r="AG22" s="22"/>
     </row>
-    <row r="23" spans="1:33" ht="15" customHeight="1">
+    <row r="23" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
         <v>191</v>
       </c>
@@ -19419,7 +19419,7 @@
       <c r="AF23" s="22"/>
       <c r="AG23" s="22"/>
     </row>
-    <row r="24" spans="1:33" ht="15" customHeight="1">
+    <row r="24" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
         <v>191</v>
       </c>
@@ -19466,7 +19466,7 @@
       <c r="AF24" s="22"/>
       <c r="AG24" s="22"/>
     </row>
-    <row r="25" spans="1:33" ht="15" customHeight="1">
+    <row r="25" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
         <v>191</v>
       </c>
@@ -19507,7 +19507,7 @@
       <c r="AF25" s="22"/>
       <c r="AG25" s="22"/>
     </row>
-    <row r="26" spans="1:33" ht="15" customHeight="1">
+    <row r="26" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
         <v>191</v>
       </c>
@@ -19550,7 +19550,7 @@
       <c r="AF26" s="22"/>
       <c r="AG26" s="22"/>
     </row>
-    <row r="27" spans="1:33" ht="15" customHeight="1">
+    <row r="27" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
         <v>191</v>
       </c>
@@ -19591,7 +19591,7 @@
       <c r="AF27" s="22"/>
       <c r="AG27" s="22"/>
     </row>
-    <row r="28" spans="1:33" ht="15" customHeight="1">
+    <row r="28" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
         <v>191</v>
       </c>
@@ -19632,7 +19632,7 @@
       <c r="AF28" s="22"/>
       <c r="AG28" s="22"/>
     </row>
-    <row r="29" spans="1:33" ht="15" customHeight="1">
+    <row r="29" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
         <v>191</v>
       </c>
@@ -19673,7 +19673,7 @@
       <c r="AF29" s="22"/>
       <c r="AG29" s="22"/>
     </row>
-    <row r="30" spans="1:33" ht="15" customHeight="1">
+    <row r="30" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
         <v>191</v>
       </c>
@@ -19716,7 +19716,7 @@
       <c r="AF30" s="22"/>
       <c r="AG30" s="22"/>
     </row>
-    <row r="31" spans="1:33" ht="15" customHeight="1">
+    <row r="31" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
         <v>191</v>
       </c>
@@ -19757,7 +19757,7 @@
       <c r="AF31" s="22"/>
       <c r="AG31" s="22"/>
     </row>
-    <row r="32" spans="1:33" ht="15" customHeight="1">
+    <row r="32" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
         <v>191</v>
       </c>
@@ -19802,7 +19802,7 @@
       <c r="AF32" s="22"/>
       <c r="AG32" s="22"/>
     </row>
-    <row r="33" spans="1:33" ht="15" customHeight="1">
+    <row r="33" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
         <v>191</v>
       </c>
@@ -19843,7 +19843,7 @@
       <c r="AF33" s="22"/>
       <c r="AG33" s="22"/>
     </row>
-    <row r="34" spans="1:33" ht="15" customHeight="1">
+    <row r="34" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
         <v>191</v>
       </c>
@@ -19884,7 +19884,7 @@
       <c r="AF34" s="22"/>
       <c r="AG34" s="22"/>
     </row>
-    <row r="35" spans="1:33" ht="15" customHeight="1">
+    <row r="35" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
         <v>191</v>
       </c>
@@ -19925,7 +19925,7 @@
       <c r="AF35" s="22"/>
       <c r="AG35" s="22"/>
     </row>
-    <row r="36" spans="1:33" ht="15" customHeight="1">
+    <row r="36" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
         <v>191</v>
       </c>
@@ -19968,7 +19968,7 @@
       <c r="AF36" s="22"/>
       <c r="AG36" s="22"/>
     </row>
-    <row r="37" spans="1:33" ht="15" customHeight="1">
+    <row r="37" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
         <v>191</v>
       </c>
@@ -20011,7 +20011,7 @@
       <c r="AF37" s="22"/>
       <c r="AG37" s="22"/>
     </row>
-    <row r="38" spans="1:33" ht="15" customHeight="1">
+    <row r="38" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="30" t="s">
         <v>191</v>
       </c>
@@ -20054,7 +20054,7 @@
       <c r="AF38" s="22"/>
       <c r="AG38" s="22"/>
     </row>
-    <row r="39" spans="1:33" ht="15" customHeight="1">
+    <row r="39" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
         <v>191</v>
       </c>
@@ -20097,7 +20097,7 @@
       <c r="AF39" s="22"/>
       <c r="AG39" s="22"/>
     </row>
-    <row r="40" spans="1:33" ht="15" customHeight="1">
+    <row r="40" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="30" t="s">
         <v>191</v>
       </c>
@@ -20140,7 +20140,7 @@
       <c r="AF40" s="22"/>
       <c r="AG40" s="22"/>
     </row>
-    <row r="41" spans="1:33" ht="15" customHeight="1">
+    <row r="41" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="30" t="s">
         <v>191</v>
       </c>
@@ -20183,7 +20183,7 @@
       <c r="AF41" s="22"/>
       <c r="AG41" s="22"/>
     </row>
-    <row r="42" spans="1:33" ht="15" customHeight="1">
+    <row r="42" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
         <v>191</v>
       </c>
@@ -20226,7 +20226,7 @@
       <c r="AF42" s="22"/>
       <c r="AG42" s="22"/>
     </row>
-    <row r="43" spans="1:33" ht="15" customHeight="1">
+    <row r="43" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
         <v>191</v>
       </c>
@@ -20269,7 +20269,7 @@
       <c r="AF43" s="22"/>
       <c r="AG43" s="22"/>
     </row>
-    <row r="44" spans="1:33" ht="15" customHeight="1">
+    <row r="44" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="30" t="s">
         <v>191</v>
       </c>
@@ -20312,7 +20312,7 @@
       <c r="AF44" s="22"/>
       <c r="AG44" s="22"/>
     </row>
-    <row r="45" spans="1:33" ht="15" customHeight="1">
+    <row r="45" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="30" t="s">
         <v>191</v>
       </c>
@@ -20355,7 +20355,7 @@
       <c r="AF45" s="22"/>
       <c r="AG45" s="22"/>
     </row>
-    <row r="46" spans="1:33" ht="15" customHeight="1">
+    <row r="46" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="30" t="s">
         <v>191</v>
       </c>
@@ -20398,7 +20398,7 @@
       <c r="AF46" s="22"/>
       <c r="AG46" s="22"/>
     </row>
-    <row r="47" spans="1:33" ht="15" customHeight="1">
+    <row r="47" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="30" t="s">
         <v>191</v>
       </c>
@@ -20445,7 +20445,7 @@
       <c r="AF47" s="22"/>
       <c r="AG47" s="22"/>
     </row>
-    <row r="48" spans="1:33" ht="15" customHeight="1">
+    <row r="48" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="30" t="s">
         <v>191</v>
       </c>
@@ -20492,7 +20492,7 @@
       <c r="AF48" s="22"/>
       <c r="AG48" s="22"/>
     </row>
-    <row r="49" spans="1:33" ht="15" customHeight="1">
+    <row r="49" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="30" t="s">
         <v>191</v>
       </c>
@@ -20539,7 +20539,7 @@
       <c r="AF49" s="22"/>
       <c r="AG49" s="22"/>
     </row>
-    <row r="50" spans="1:33" ht="15" customHeight="1">
+    <row r="50" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="30" t="s">
         <v>191</v>
       </c>
@@ -20580,7 +20580,7 @@
       <c r="AF50" s="22"/>
       <c r="AG50" s="22"/>
     </row>
-    <row r="51" spans="1:33" ht="15" customHeight="1">
+    <row r="51" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="30" t="s">
         <v>191</v>
       </c>
@@ -20623,7 +20623,7 @@
       <c r="AF51" s="22"/>
       <c r="AG51" s="22"/>
     </row>
-    <row r="52" spans="1:33" ht="15" customHeight="1">
+    <row r="52" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="30" t="s">
         <v>191</v>
       </c>
@@ -20664,7 +20664,7 @@
       <c r="AF52" s="22"/>
       <c r="AG52" s="22"/>
     </row>
-    <row r="53" spans="1:33" ht="15" customHeight="1">
+    <row r="53" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="30" t="s">
         <v>191</v>
       </c>
@@ -20705,7 +20705,7 @@
       <c r="AF53" s="22"/>
       <c r="AG53" s="22"/>
     </row>
-    <row r="54" spans="1:33" ht="15" customHeight="1">
+    <row r="54" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="30" t="s">
         <v>191</v>
       </c>
@@ -20746,7 +20746,7 @@
       <c r="AF54" s="22"/>
       <c r="AG54" s="22"/>
     </row>
-    <row r="55" spans="1:33" ht="15" customHeight="1">
+    <row r="55" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="30" t="s">
         <v>191</v>
       </c>
@@ -20789,7 +20789,7 @@
       <c r="AF55" s="22"/>
       <c r="AG55" s="22"/>
     </row>
-    <row r="56" spans="1:33" s="31" customFormat="1">
+    <row r="56" spans="1:33" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="30" t="s">
         <v>192</v>
       </c>
@@ -20860,7 +20860,7 @@
       <c r="AF56" s="20"/>
       <c r="AG56" s="20"/>
     </row>
-    <row r="57" spans="1:33" s="31" customFormat="1">
+    <row r="57" spans="1:33" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="30" t="s">
         <v>192</v>
       </c>
@@ -20931,7 +20931,7 @@
       <c r="AF57" s="20"/>
       <c r="AG57" s="20"/>
     </row>
-    <row r="58" spans="1:33" s="31" customFormat="1">
+    <row r="58" spans="1:33" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="30" t="s">
         <v>192</v>
       </c>
@@ -21002,7 +21002,7 @@
       <c r="AF58" s="20"/>
       <c r="AG58" s="20"/>
     </row>
-    <row r="59" spans="1:33" s="31" customFormat="1">
+    <row r="59" spans="1:33" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="30" t="s">
         <v>192</v>
       </c>
@@ -21073,7 +21073,7 @@
       <c r="AF59" s="20"/>
       <c r="AG59" s="20"/>
     </row>
-    <row r="60" spans="1:33" s="31" customFormat="1">
+    <row r="60" spans="1:33" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="30" t="s">
         <v>192</v>
       </c>
@@ -21144,7 +21144,7 @@
       <c r="AF60" s="20"/>
       <c r="AG60" s="20"/>
     </row>
-    <row r="61" spans="1:33" s="31" customFormat="1" ht="30">
+    <row r="61" spans="1:33" s="31" customFormat="1" ht="33" x14ac:dyDescent="0.25">
       <c r="A61" s="30" t="s">
         <v>192</v>
       </c>
@@ -21215,7 +21215,7 @@
       <c r="AF61" s="20"/>
       <c r="AG61" s="20"/>
     </row>
-    <row r="62" spans="1:33" s="31" customFormat="1" ht="42.75">
+    <row r="62" spans="1:33" s="31" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A62" s="30" t="s">
         <v>192</v>
       </c>
@@ -21286,7 +21286,7 @@
       <c r="AF62" s="20"/>
       <c r="AG62" s="20"/>
     </row>
-    <row r="63" spans="1:33" s="31" customFormat="1" ht="30">
+    <row r="63" spans="1:33" s="31" customFormat="1" ht="33" x14ac:dyDescent="0.25">
       <c r="A63" s="30" t="s">
         <v>192</v>
       </c>
@@ -21357,7 +21357,7 @@
       <c r="AF63" s="20"/>
       <c r="AG63" s="20"/>
     </row>
-    <row r="64" spans="1:33" s="31" customFormat="1">
+    <row r="64" spans="1:33" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="30" t="s">
         <v>192</v>
       </c>
@@ -21428,7 +21428,7 @@
       <c r="AF64" s="20"/>
       <c r="AG64" s="20"/>
     </row>
-    <row r="65" spans="1:33" s="31" customFormat="1">
+    <row r="65" spans="1:33" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="30" t="s">
         <v>192</v>
       </c>
@@ -21499,7 +21499,7 @@
       <c r="AF65" s="20"/>
       <c r="AG65" s="20"/>
     </row>
-    <row r="66" spans="1:33" s="31" customFormat="1">
+    <row r="66" spans="1:33" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="30" t="s">
         <v>192</v>
       </c>
@@ -21570,7 +21570,7 @@
       <c r="AF66" s="20"/>
       <c r="AG66" s="20"/>
     </row>
-    <row r="67" spans="1:33" s="31" customFormat="1" ht="30">
+    <row r="67" spans="1:33" s="31" customFormat="1" ht="33" x14ac:dyDescent="0.25">
       <c r="A67" s="30" t="s">
         <v>192</v>
       </c>
@@ -21641,7 +21641,7 @@
       <c r="AF67" s="20"/>
       <c r="AG67" s="20"/>
     </row>
-    <row r="68" spans="1:33" s="31" customFormat="1" ht="43.5" customHeight="1">
+    <row r="68" spans="1:33" s="31" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="30" t="s">
         <v>192</v>
       </c>
@@ -21712,7 +21712,7 @@
       <c r="AF68" s="20"/>
       <c r="AG68" s="20"/>
     </row>
-    <row r="69" spans="1:33" s="31" customFormat="1" ht="43.5" customHeight="1">
+    <row r="69" spans="1:33" s="31" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="30" t="s">
         <v>192</v>
       </c>
@@ -21783,7 +21783,7 @@
       <c r="AF69" s="20"/>
       <c r="AG69" s="20"/>
     </row>
-    <row r="70" spans="1:33" s="31" customFormat="1" ht="45">
+    <row r="70" spans="1:33" s="31" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A70" s="30" t="s">
         <v>192</v>
       </c>
@@ -21854,7 +21854,7 @@
       <c r="AF70" s="20"/>
       <c r="AG70" s="20"/>
     </row>
-    <row r="71" spans="1:33" s="31" customFormat="1" ht="45">
+    <row r="71" spans="1:33" s="31" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A71" s="30" t="s">
         <v>192</v>
       </c>
@@ -21925,7 +21925,7 @@
       <c r="AF71" s="20"/>
       <c r="AG71" s="20"/>
     </row>
-    <row r="72" spans="1:33" s="31" customFormat="1" ht="57">
+    <row r="72" spans="1:33" s="31" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A72" s="30" t="s">
         <v>192</v>
       </c>
@@ -21996,7 +21996,7 @@
       <c r="AF72" s="20"/>
       <c r="AG72" s="20"/>
     </row>
-    <row r="73" spans="1:33" s="31" customFormat="1">
+    <row r="73" spans="1:33" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="30" t="s">
         <v>192</v>
       </c>
@@ -22067,7 +22067,7 @@
       <c r="AF73" s="20"/>
       <c r="AG73" s="20"/>
     </row>
-    <row r="74" spans="1:33" s="31" customFormat="1" ht="60">
+    <row r="74" spans="1:33" s="31" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A74" s="30" t="s">
         <v>192</v>
       </c>
@@ -22138,7 +22138,7 @@
       <c r="AF74" s="20"/>
       <c r="AG74" s="20"/>
     </row>
-    <row r="75" spans="1:33" s="31" customFormat="1">
+    <row r="75" spans="1:33" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="30" t="s">
         <v>192</v>
       </c>
@@ -22209,7 +22209,7 @@
       <c r="AF75" s="20"/>
       <c r="AG75" s="20"/>
     </row>
-    <row r="76" spans="1:33" s="31" customFormat="1" ht="30">
+    <row r="76" spans="1:33" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="30" t="s">
         <v>192</v>
       </c>
@@ -22280,7 +22280,7 @@
       <c r="AF76" s="20"/>
       <c r="AG76" s="20"/>
     </row>
-    <row r="77" spans="1:33" s="31" customFormat="1" ht="30">
+    <row r="77" spans="1:33" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="30" t="s">
         <v>192</v>
       </c>
@@ -22351,7 +22351,7 @@
       <c r="AF77" s="20"/>
       <c r="AG77" s="20"/>
     </row>
-    <row r="78" spans="1:33" s="31" customFormat="1" ht="28.5">
+    <row r="78" spans="1:33" s="31" customFormat="1" ht="33" x14ac:dyDescent="0.25">
       <c r="A78" s="30" t="s">
         <v>192</v>
       </c>
@@ -22422,7 +22422,7 @@
       <c r="AF78" s="20"/>
       <c r="AG78" s="20"/>
     </row>
-    <row r="79" spans="1:33" ht="80.25" customHeight="1">
+    <row r="79" spans="1:33" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="30" t="s">
         <v>191</v>
       </c>
@@ -22493,7 +22493,7 @@
       <c r="AF79" s="22"/>
       <c r="AG79" s="22"/>
     </row>
-    <row r="80" spans="1:33" ht="67.5" customHeight="1">
+    <row r="80" spans="1:33" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="30" t="s">
         <v>191</v>
       </c>
@@ -22564,7 +22564,7 @@
       <c r="AF80" s="22"/>
       <c r="AG80" s="22"/>
     </row>
-    <row r="81" spans="1:33" ht="15" customHeight="1">
+    <row r="81" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="30" t="s">
         <v>191</v>
       </c>
@@ -22635,7 +22635,7 @@
       <c r="AF81" s="22"/>
       <c r="AG81" s="22"/>
     </row>
-    <row r="82" spans="1:33">
+    <row r="82" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A82" s="30" t="s">
         <v>191</v>
       </c>
@@ -22706,7 +22706,7 @@
       <c r="AF82" s="22"/>
       <c r="AG82" s="22"/>
     </row>
-    <row r="83" spans="1:33" ht="30">
+    <row r="83" spans="1:33" ht="33" x14ac:dyDescent="0.25">
       <c r="A83" s="30" t="s">
         <v>191</v>
       </c>
@@ -22777,7 +22777,7 @@
       <c r="AF83" s="22"/>
       <c r="AG83" s="22"/>
     </row>
-    <row r="84" spans="1:33" ht="238.5" customHeight="1">
+    <row r="84" spans="1:33" ht="238.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="30" t="s">
         <v>191</v>
       </c>
@@ -22848,7 +22848,7 @@
       <c r="AF84" s="22"/>
       <c r="AG84" s="22"/>
     </row>
-    <row r="85" spans="1:33" ht="238.5" customHeight="1">
+    <row r="85" spans="1:33" ht="238.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="30" t="s">
         <v>191</v>
       </c>
@@ -22919,7 +22919,7 @@
       <c r="AF85" s="22"/>
       <c r="AG85" s="22"/>
     </row>
-    <row r="86" spans="1:33" ht="45">
+    <row r="86" spans="1:33" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A86" s="30" t="s">
         <v>191</v>
       </c>
@@ -22990,7 +22990,7 @@
       <c r="AF86" s="22"/>
       <c r="AG86" s="22"/>
     </row>
-    <row r="87" spans="1:33">
+    <row r="87" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A87" s="30" t="s">
         <v>191</v>
       </c>
@@ -23061,7 +23061,7 @@
       <c r="AF87" s="22"/>
       <c r="AG87" s="22"/>
     </row>
-    <row r="88" spans="1:33">
+    <row r="88" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A88" s="30" t="s">
         <v>191</v>
       </c>
@@ -23132,7 +23132,7 @@
       <c r="AF88" s="22"/>
       <c r="AG88" s="22"/>
     </row>
-    <row r="89" spans="1:33" ht="228">
+    <row r="89" spans="1:33" ht="247.5" x14ac:dyDescent="0.25">
       <c r="A89" s="30" t="s">
         <v>191</v>
       </c>
@@ -23203,7 +23203,7 @@
       <c r="AF89" s="22"/>
       <c r="AG89" s="22"/>
     </row>
-    <row r="90" spans="1:33">
+    <row r="90" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A90" s="30" t="s">
         <v>191</v>
       </c>
@@ -23274,7 +23274,7 @@
       <c r="AF90" s="22"/>
       <c r="AG90" s="22"/>
     </row>
-    <row r="91" spans="1:33" ht="42.75">
+    <row r="91" spans="1:33" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A91" s="30" t="s">
         <v>191</v>
       </c>
@@ -23345,7 +23345,7 @@
       <c r="AF91" s="22"/>
       <c r="AG91" s="22"/>
     </row>
-    <row r="92" spans="1:33">
+    <row r="92" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A92" s="30" t="s">
         <v>191</v>
       </c>
@@ -23416,7 +23416,7 @@
       <c r="AF92" s="22"/>
       <c r="AG92" s="22"/>
     </row>
-    <row r="93" spans="1:33" ht="71.25">
+    <row r="93" spans="1:33" ht="66" x14ac:dyDescent="0.25">
       <c r="A93" s="30" t="s">
         <v>191</v>
       </c>
@@ -23487,7 +23487,7 @@
       <c r="AF93" s="22"/>
       <c r="AG93" s="22"/>
     </row>
-    <row r="94" spans="1:33">
+    <row r="94" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A94" s="30" t="s">
         <v>191</v>
       </c>
@@ -23558,7 +23558,7 @@
       <c r="AF94" s="22"/>
       <c r="AG94" s="22"/>
     </row>
-    <row r="95" spans="1:33" ht="42.75">
+    <row r="95" spans="1:33" ht="33" x14ac:dyDescent="0.25">
       <c r="A95" s="30" t="s">
         <v>191</v>
       </c>
@@ -23629,7 +23629,7 @@
       <c r="AF95" s="22"/>
       <c r="AG95" s="22"/>
     </row>
-    <row r="96" spans="1:33" ht="30">
+    <row r="96" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="30" t="s">
         <v>191</v>
       </c>
@@ -23700,7 +23700,7 @@
       <c r="AF96" s="22"/>
       <c r="AG96" s="22"/>
     </row>
-    <row r="97" spans="1:33" ht="30">
+    <row r="97" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="30" t="s">
         <v>191</v>
       </c>
@@ -23771,7 +23771,7 @@
       <c r="AF97" s="22"/>
       <c r="AG97" s="22"/>
     </row>
-    <row r="98" spans="1:33" ht="42.75">
+    <row r="98" spans="1:33" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A98" s="30" t="s">
         <v>191</v>
       </c>
@@ -23842,7 +23842,7 @@
       <c r="AF98" s="22"/>
       <c r="AG98" s="22"/>
     </row>
-    <row r="99" spans="1:33" ht="42.75">
+    <row r="99" spans="1:33" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A99" s="30" t="s">
         <v>191</v>
       </c>
@@ -23913,7 +23913,7 @@
       <c r="AF99" s="22"/>
       <c r="AG99" s="22"/>
     </row>
-    <row r="100" spans="1:33" ht="45">
+    <row r="100" spans="1:33" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A100" s="30" t="s">
         <v>191</v>
       </c>
@@ -23984,7 +23984,7 @@
       <c r="AF100" s="22"/>
       <c r="AG100" s="22"/>
     </row>
-    <row r="101" spans="1:33" ht="42.75">
+    <row r="101" spans="1:33" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A101" s="30" t="s">
         <v>191</v>
       </c>
@@ -24055,7 +24055,7 @@
       <c r="AF101" s="22"/>
       <c r="AG101" s="22"/>
     </row>
-    <row r="102" spans="1:33" ht="30">
+    <row r="102" spans="1:33" ht="33" x14ac:dyDescent="0.25">
       <c r="A102" s="30" t="s">
         <v>191</v>
       </c>
@@ -24126,7 +24126,7 @@
       <c r="AF102" s="22"/>
       <c r="AG102" s="22"/>
     </row>
-    <row r="103" spans="1:33" ht="42.75">
+    <row r="103" spans="1:33" ht="33" x14ac:dyDescent="0.25">
       <c r="A103" s="30" t="s">
         <v>191</v>
       </c>
@@ -24197,7 +24197,7 @@
       <c r="AF103" s="22"/>
       <c r="AG103" s="22"/>
     </row>
-    <row r="104" spans="1:33" ht="285">
+    <row r="104" spans="1:33" ht="313.5" x14ac:dyDescent="0.25">
       <c r="A104" s="30" t="s">
         <v>191</v>
       </c>
@@ -24268,7 +24268,7 @@
       <c r="AF104" s="22"/>
       <c r="AG104" s="22"/>
     </row>
-    <row r="105" spans="1:33">
+    <row r="105" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A105" s="30" t="s">
         <v>191</v>
       </c>
@@ -24339,7 +24339,7 @@
       <c r="AF105" s="22"/>
       <c r="AG105" s="22"/>
     </row>
-    <row r="106" spans="1:33">
+    <row r="106" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A106" s="30" t="s">
         <v>191</v>
       </c>
@@ -24410,7 +24410,7 @@
       <c r="AF106" s="22"/>
       <c r="AG106" s="22"/>
     </row>
-    <row r="107" spans="1:33">
+    <row r="107" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A107" s="30" t="s">
         <v>191</v>
       </c>
@@ -24481,7 +24481,7 @@
       <c r="AF107" s="22"/>
       <c r="AG107" s="22"/>
     </row>
-    <row r="108" spans="1:33">
+    <row r="108" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A108" s="30" t="s">
         <v>191</v>
       </c>
@@ -24552,7 +24552,7 @@
       <c r="AF108" s="22"/>
       <c r="AG108" s="22"/>
     </row>
-    <row r="109" spans="1:33">
+    <row r="109" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A109" s="30" t="s">
         <v>191</v>
       </c>
@@ -24623,7 +24623,7 @@
       <c r="AF109" s="22"/>
       <c r="AG109" s="22"/>
     </row>
-    <row r="110" spans="1:33">
+    <row r="110" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A110" s="30" t="s">
         <v>191</v>
       </c>
@@ -24694,7 +24694,7 @@
       <c r="AF110" s="22"/>
       <c r="AG110" s="22"/>
     </row>
-    <row r="111" spans="1:33">
+    <row r="111" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A111" s="30" t="s">
         <v>191</v>
       </c>
@@ -24765,7 +24765,7 @@
       <c r="AF111" s="22"/>
       <c r="AG111" s="22"/>
     </row>
-    <row r="112" spans="1:33">
+    <row r="112" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A112" s="30" t="s">
         <v>191</v>
       </c>
@@ -24836,7 +24836,7 @@
       <c r="AF112" s="22"/>
       <c r="AG112" s="22"/>
     </row>
-    <row r="113" spans="1:33">
+    <row r="113" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A113" s="30" t="s">
         <v>191</v>
       </c>
@@ -24907,7 +24907,7 @@
       <c r="AF113" s="22"/>
       <c r="AG113" s="22"/>
     </row>
-    <row r="114" spans="1:33" ht="30">
+    <row r="114" spans="1:33" ht="33" x14ac:dyDescent="0.25">
       <c r="A114" s="30" t="s">
         <v>191</v>
       </c>
@@ -24978,7 +24978,7 @@
       <c r="AF114" s="22"/>
       <c r="AG114" s="22"/>
     </row>
-    <row r="115" spans="1:33">
+    <row r="115" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A115" s="30" t="s">
         <v>191</v>
       </c>
@@ -25049,7 +25049,7 @@
       <c r="AF115" s="22"/>
       <c r="AG115" s="22"/>
     </row>
-    <row r="116" spans="1:33" ht="28.5">
+    <row r="116" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A116" s="30" t="s">
         <v>191</v>
       </c>
@@ -25120,7 +25120,7 @@
       <c r="AF116" s="22"/>
       <c r="AG116" s="22"/>
     </row>
-    <row r="117" spans="1:33">
+    <row r="117" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A117" s="30" t="s">
         <v>191</v>
       </c>
@@ -25191,7 +25191,7 @@
       <c r="AF117" s="22"/>
       <c r="AG117" s="22"/>
     </row>
-    <row r="118" spans="1:33">
+    <row r="118" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A118" s="30" t="s">
         <v>191</v>
       </c>
@@ -25262,7 +25262,7 @@
       <c r="AF118" s="22"/>
       <c r="AG118" s="22"/>
     </row>
-    <row r="119" spans="1:33">
+    <row r="119" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A119" s="30" t="s">
         <v>191</v>
       </c>
@@ -25333,7 +25333,7 @@
       <c r="AF119" s="22"/>
       <c r="AG119" s="22"/>
     </row>
-    <row r="120" spans="1:33">
+    <row r="120" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A120" s="30" t="s">
         <v>191</v>
       </c>
@@ -25404,7 +25404,7 @@
       <c r="AF120" s="22"/>
       <c r="AG120" s="22"/>
     </row>
-    <row r="121" spans="1:33">
+    <row r="121" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A121" s="30" t="s">
         <v>191</v>
       </c>
@@ -25475,7 +25475,7 @@
       <c r="AF121" s="22"/>
       <c r="AG121" s="22"/>
     </row>
-    <row r="122" spans="1:33" ht="270.75">
+    <row r="122" spans="1:33" ht="313.5" x14ac:dyDescent="0.25">
       <c r="A122" s="30" t="s">
         <v>191</v>
       </c>
@@ -25546,7 +25546,7 @@
       <c r="AF122" s="22"/>
       <c r="AG122" s="22"/>
     </row>
-    <row r="123" spans="1:33" ht="30">
+    <row r="123" spans="1:33" ht="33" x14ac:dyDescent="0.25">
       <c r="A123" s="30" t="s">
         <v>191</v>
       </c>
@@ -25617,7 +25617,7 @@
       <c r="AF123" s="22"/>
       <c r="AG123" s="22"/>
     </row>
-    <row r="124" spans="1:33">
+    <row r="124" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A124" s="30" t="s">
         <v>191</v>
       </c>
@@ -25688,7 +25688,7 @@
       <c r="AF124" s="22"/>
       <c r="AG124" s="22"/>
     </row>
-    <row r="125" spans="1:33" ht="30">
+    <row r="125" spans="1:33" ht="33" x14ac:dyDescent="0.25">
       <c r="A125" s="30" t="s">
         <v>191</v>
       </c>
@@ -25759,7 +25759,7 @@
       <c r="AF125" s="22"/>
       <c r="AG125" s="22"/>
     </row>
-    <row r="126" spans="1:33" ht="30">
+    <row r="126" spans="1:33" ht="33" x14ac:dyDescent="0.25">
       <c r="A126" s="30" t="s">
         <v>191</v>
       </c>
@@ -25830,7 +25830,7 @@
       <c r="AF126" s="22"/>
       <c r="AG126" s="22"/>
     </row>
-    <row r="127" spans="1:33" ht="242.25">
+    <row r="127" spans="1:33" ht="264" x14ac:dyDescent="0.25">
       <c r="A127" s="30" t="s">
         <v>191</v>
       </c>
@@ -25901,7 +25901,7 @@
       <c r="AF127" s="22"/>
       <c r="AG127" s="22"/>
     </row>
-    <row r="128" spans="1:33" ht="30">
+    <row r="128" spans="1:33" ht="33" x14ac:dyDescent="0.25">
       <c r="A128" s="30" t="s">
         <v>191</v>
       </c>
@@ -25972,7 +25972,7 @@
       <c r="AF128" s="22"/>
       <c r="AG128" s="22"/>
     </row>
-    <row r="129" spans="1:33" ht="356.25">
+    <row r="129" spans="1:33" ht="396" x14ac:dyDescent="0.25">
       <c r="A129" s="30" t="s">
         <v>191</v>
       </c>
@@ -26043,7 +26043,7 @@
       <c r="AF129" s="22"/>
       <c r="AG129" s="22"/>
     </row>
-    <row r="130" spans="1:33" ht="76.5" customHeight="1">
+    <row r="130" spans="1:33" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="30" t="s">
         <v>191</v>
       </c>
@@ -26114,7 +26114,7 @@
       <c r="AF130" s="22"/>
       <c r="AG130" s="22"/>
     </row>
-    <row r="131" spans="1:33" ht="238.5" customHeight="1">
+    <row r="131" spans="1:33" ht="238.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="30" t="s">
         <v>191</v>
       </c>
@@ -26185,7 +26185,7 @@
       <c r="AF131" s="22"/>
       <c r="AG131" s="22"/>
     </row>
-    <row r="132" spans="1:33" ht="238.5" customHeight="1">
+    <row r="132" spans="1:33" ht="238.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="30" t="s">
         <v>191</v>
       </c>
@@ -26256,7 +26256,7 @@
       <c r="AF132" s="22"/>
       <c r="AG132" s="22"/>
     </row>
-    <row r="133" spans="1:33" ht="390.75" customHeight="1">
+    <row r="133" spans="1:33" ht="390.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="30" t="s">
         <v>191</v>
       </c>
@@ -26324,7 +26324,7 @@
       <c r="AF133" s="22"/>
       <c r="AG133" s="22"/>
     </row>
-    <row r="134" spans="1:33" ht="409.5">
+    <row r="134" spans="1:33" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A134" s="30" t="s">
         <v>191</v>
       </c>
@@ -26394,7 +26394,7 @@
       <c r="AF134" s="22"/>
       <c r="AG134" s="22"/>
     </row>
-    <row r="135" spans="1:33" ht="409.5" customHeight="1">
+    <row r="135" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="30" t="s">
         <v>191</v>
       </c>
@@ -26462,7 +26462,7 @@
       <c r="AF135" s="22"/>
       <c r="AG135" s="22"/>
     </row>
-    <row r="136" spans="1:33" ht="409.5" customHeight="1">
+    <row r="136" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="30" t="s">
         <v>191</v>
       </c>
@@ -26530,7 +26530,7 @@
       <c r="AF136" s="22"/>
       <c r="AG136" s="22"/>
     </row>
-    <row r="137" spans="1:33" ht="409.5" customHeight="1">
+    <row r="137" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="30" t="s">
         <v>191</v>
       </c>
@@ -26598,7 +26598,7 @@
       <c r="AF137" s="22"/>
       <c r="AG137" s="22"/>
     </row>
-    <row r="138" spans="1:33" ht="409.5" customHeight="1">
+    <row r="138" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="30" t="s">
         <v>191</v>
       </c>
@@ -26666,7 +26666,7 @@
       <c r="AF138" s="22"/>
       <c r="AG138" s="22"/>
     </row>
-    <row r="139" spans="1:33" ht="409.5" customHeight="1">
+    <row r="139" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="30" t="s">
         <v>191</v>
       </c>
@@ -26734,7 +26734,7 @@
       <c r="AF139" s="22"/>
       <c r="AG139" s="22"/>
     </row>
-    <row r="140" spans="1:33" ht="409.5" customHeight="1">
+    <row r="140" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="30" t="s">
         <v>191</v>
       </c>
@@ -26802,7 +26802,7 @@
       <c r="AF140" s="22"/>
       <c r="AG140" s="22"/>
     </row>
-    <row r="141" spans="1:33" ht="409.5" customHeight="1">
+    <row r="141" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="30" t="s">
         <v>191</v>
       </c>
@@ -26870,7 +26870,7 @@
       <c r="AF141" s="22"/>
       <c r="AG141" s="22"/>
     </row>
-    <row r="142" spans="1:33" ht="409.5" customHeight="1">
+    <row r="142" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="30" t="s">
         <v>191</v>
       </c>
@@ -26938,7 +26938,7 @@
       <c r="AF142" s="22"/>
       <c r="AG142" s="22"/>
     </row>
-    <row r="143" spans="1:33" ht="409.5" customHeight="1">
+    <row r="143" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="30" t="s">
         <v>191</v>
       </c>
@@ -27006,7 +27006,7 @@
       <c r="AF143" s="22"/>
       <c r="AG143" s="22"/>
     </row>
-    <row r="144" spans="1:33" ht="409.5" customHeight="1">
+    <row r="144" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="30" t="s">
         <v>191</v>
       </c>
@@ -27074,7 +27074,7 @@
       <c r="AF144" s="22"/>
       <c r="AG144" s="22"/>
     </row>
-    <row r="145" spans="1:33" ht="409.5" customHeight="1">
+    <row r="145" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="30" t="s">
         <v>191</v>
       </c>
@@ -27142,7 +27142,7 @@
       <c r="AF145" s="22"/>
       <c r="AG145" s="22"/>
     </row>
-    <row r="146" spans="1:33" ht="409.5" customHeight="1">
+    <row r="146" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="30" t="s">
         <v>191</v>
       </c>
@@ -27210,7 +27210,7 @@
       <c r="AF146" s="22"/>
       <c r="AG146" s="22"/>
     </row>
-    <row r="147" spans="1:33" ht="409.5" customHeight="1">
+    <row r="147" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="30" t="s">
         <v>191</v>
       </c>
@@ -27278,7 +27278,7 @@
       <c r="AF147" s="22"/>
       <c r="AG147" s="22"/>
     </row>
-    <row r="148" spans="1:33" ht="409.5" customHeight="1">
+    <row r="148" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="30" t="s">
         <v>191</v>
       </c>
@@ -27346,7 +27346,7 @@
       <c r="AF148" s="22"/>
       <c r="AG148" s="22"/>
     </row>
-    <row r="149" spans="1:33" ht="409.5" customHeight="1">
+    <row r="149" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="30" t="s">
         <v>191</v>
       </c>
@@ -27416,7 +27416,7 @@
       <c r="AF149" s="22"/>
       <c r="AG149" s="22"/>
     </row>
-    <row r="150" spans="1:33" ht="409.5" customHeight="1">
+    <row r="150" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="30" t="s">
         <v>191</v>
       </c>
@@ -27486,7 +27486,7 @@
       <c r="AF150" s="22"/>
       <c r="AG150" s="22"/>
     </row>
-    <row r="151" spans="1:33" ht="409.5" customHeight="1">
+    <row r="151" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="30" t="s">
         <v>191</v>
       </c>
@@ -27556,7 +27556,7 @@
       <c r="AF151" s="22"/>
       <c r="AG151" s="22"/>
     </row>
-    <row r="152" spans="1:33" ht="409.5" customHeight="1">
+    <row r="152" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="30" t="s">
         <v>191</v>
       </c>
@@ -27624,7 +27624,7 @@
       <c r="AF152" s="22"/>
       <c r="AG152" s="22"/>
     </row>
-    <row r="153" spans="1:33" ht="409.5" customHeight="1">
+    <row r="153" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="30" t="s">
         <v>191</v>
       </c>
@@ -27692,7 +27692,7 @@
       <c r="AF153" s="22"/>
       <c r="AG153" s="22"/>
     </row>
-    <row r="154" spans="1:33" ht="409.5" customHeight="1">
+    <row r="154" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="30" t="s">
         <v>191</v>
       </c>
@@ -27760,7 +27760,7 @@
       <c r="AF154" s="22"/>
       <c r="AG154" s="22"/>
     </row>
-    <row r="155" spans="1:33" ht="409.5" customHeight="1">
+    <row r="155" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="30" t="s">
         <v>191</v>
       </c>
@@ -27828,7 +27828,7 @@
       <c r="AF155" s="22"/>
       <c r="AG155" s="22"/>
     </row>
-    <row r="156" spans="1:33" ht="409.5" customHeight="1">
+    <row r="156" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="30" t="s">
         <v>191</v>
       </c>
@@ -27896,7 +27896,7 @@
       <c r="AF156" s="22"/>
       <c r="AG156" s="22"/>
     </row>
-    <row r="157" spans="1:33" ht="409.5" customHeight="1">
+    <row r="157" spans="1:33" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="30" t="s">
         <v>191</v>
       </c>
@@ -27997,7 +27997,7 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
@@ -28006,7 +28006,7 @@
     <col min="6" max="6" width="78.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>181</v>
       </c>
@@ -28026,7 +28026,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>567</v>
       </c>
@@ -28043,7 +28043,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>567</v>
       </c>
@@ -28063,7 +28063,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>567</v>
       </c>
@@ -28083,7 +28083,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>567</v>
       </c>
@@ -28103,7 +28103,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>512</v>
       </c>
@@ -28120,7 +28120,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>512</v>
       </c>
@@ -28140,7 +28140,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>512</v>
       </c>
@@ -28160,7 +28160,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>512</v>
       </c>
@@ -28180,7 +28180,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>214</v>
       </c>
@@ -28197,7 +28197,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>214</v>
       </c>
@@ -28217,7 +28217,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>214</v>
       </c>
@@ -28237,7 +28237,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>214</v>
       </c>
@@ -28257,7 +28257,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>287</v>
       </c>
@@ -28274,7 +28274,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>287</v>
       </c>
@@ -28294,7 +28294,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>287</v>
       </c>
@@ -28314,7 +28314,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>287</v>
       </c>
@@ -28348,13 +28348,13 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" customWidth="1"/>
     <col min="2" max="17" width="11.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="5" customFormat="1" ht="45">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="15" t="s">
         <v>298</v>
@@ -28405,7 +28405,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75">
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>244</v>
       </c>
@@ -28428,7 +28428,7 @@
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75">
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>245</v>
       </c>
@@ -28451,7 +28451,7 @@
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75">
+    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>246</v>
       </c>
@@ -28474,7 +28474,7 @@
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:17" ht="15.75">
+    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>262</v>
       </c>
@@ -28497,7 +28497,7 @@
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
     </row>
-    <row r="6" spans="1:17" ht="15.75">
+    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>234</v>
       </c>
@@ -28520,7 +28520,7 @@
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
     </row>
-    <row r="7" spans="1:17" ht="15.75">
+    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>263</v>
       </c>
@@ -28543,7 +28543,7 @@
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
     </row>
-    <row r="8" spans="1:17" ht="15.75">
+    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>264</v>
       </c>
@@ -28568,7 +28568,7 @@
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
     </row>
-    <row r="9" spans="1:17" ht="15.75">
+    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>253</v>
       </c>
@@ -28595,7 +28595,7 @@
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
     </row>
-    <row r="10" spans="1:17" ht="15.75">
+    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>256</v>
       </c>
@@ -28620,7 +28620,7 @@
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
     </row>
-    <row r="11" spans="1:17" ht="15.75">
+    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>251</v>
       </c>
@@ -28645,7 +28645,7 @@
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
     </row>
-    <row r="12" spans="1:17" ht="15.75">
+    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>255</v>
       </c>
@@ -28670,7 +28670,7 @@
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
     </row>
-    <row r="13" spans="1:17" ht="15.75">
+    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>252</v>
       </c>
@@ -28695,7 +28695,7 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
     </row>
-    <row r="14" spans="1:17" ht="15.75">
+    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>260</v>
       </c>
@@ -28720,7 +28720,7 @@
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
     </row>
-    <row r="15" spans="1:17" ht="15.75">
+    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>257</v>
       </c>
@@ -28747,7 +28747,7 @@
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
     </row>
-    <row r="16" spans="1:17" ht="15.75">
+    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>258</v>
       </c>
@@ -28774,7 +28774,7 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
     </row>
-    <row r="17" spans="1:17" ht="15.75">
+    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>259</v>
       </c>
@@ -28799,7 +28799,7 @@
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
     </row>
-    <row r="18" spans="1:17" ht="15.75">
+    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>261</v>
       </c>
@@ -28824,7 +28824,7 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>254</v>
       </c>
@@ -28851,7 +28851,7 @@
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
     </row>
-    <row r="20" spans="1:17" ht="15.75">
+    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>248</v>
       </c>
@@ -28876,7 +28876,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="1:17" ht="15.75">
+    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>237</v>
       </c>
@@ -28901,7 +28901,7 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
     </row>
-    <row r="22" spans="1:17" ht="15.75">
+    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>247</v>
       </c>
@@ -28926,7 +28926,7 @@
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
     </row>
-    <row r="23" spans="1:17" ht="15.75">
+    <row r="23" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>236</v>
       </c>
@@ -28951,7 +28951,7 @@
       </c>
       <c r="Q23" s="7"/>
     </row>
-    <row r="24" spans="1:17" ht="15.75">
+    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>250</v>
       </c>
@@ -28976,7 +28976,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="15.75">
+    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>243</v>
       </c>
@@ -29001,7 +29001,7 @@
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
     </row>
-    <row r="26" spans="1:17" ht="15.75">
+    <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>249</v>
       </c>

</xml_diff>

<commit_message>
provided more space for summary box - ie. more flexibility for translations
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\global-indicators\analysis\global_scorecards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB697FB7-5466-45D7-95F0-EE9FE9A75FBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231A612F-AC6D-43B7-BD03-9539C1F81FB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4284,9 +4284,6 @@
     <t>Si bien se encontró que la disponibilidad y la calidad de las políticas urbanas y de transporte y la infraestructura vecinal que respaldan la salud y la sostenibilidad en Maiduguri estaban muy por debajo del promedio en comparación con otras ciudades, la disponibilidad de datos para Maiduguri fue limitada y esto puede explicar parcialmente nuestros hallazgos. Aunque Maiduguri tiene una política de contaminación del aire relacionada con el uso de la tierra, parece carecer de requisitos de planificación urbana que incluyan otras acciones específicas centradas en la salud y estándares específicos y medibles para crear vecindarios transitables y un acceso equitativo al transporte público y al espacio público abierto. En relación con las 25 ciudades de este estudio internacional, la mayoría de los barrios de Maiduguri no parecen ser transitables, y los barrios transitables parecen tener un patrón espacial a lo largo de las principales redes de carreteras. En cuanto a los umbrales para las intervenciones en entornos construidos para alcanzar los objetivos de la OMS de aumentar la actividad física, el 95,9% de los residentes en Maiduguri viven en barrios que cumplen con el umbral de densidad, aunque solo el 29% vive en barrios que cumplen con los umbrales de conectividad de las calles. Esto último podría reflejar la falta de datos sobre las rutas informales. En particular, muchos residentes de Maiduguri pueden vivir en vecindarios que exceden los niveles de densidad y conectividad de la calle que fomentan la actividad física. Solo el 10% de los residentes tienen acceso a paradas de transporte público, con evidencia de que el acceso está modelado espacialmente a lo largo de las principales redes de carreteras. Muy pocos residentes tienen acceso a espacios abiertos públicos dentro de los 500 m, y solo el 0.5% de los residentes tienen acceso a espacios abiertos públicos más grandes, concentrados en el noreste de la ciudad.</t>
   </si>
   <si>
-    <t>La disponibilidad y calidad de las políticas urbanas y de transporte que apoyan la salud y la sostenibilidad en la Ciudad de México está justo por debajo del promedio en comparación con otras ciudades. La Ciudad de México no parece tener acciones específicas centradas en la salud en su política de transporte metropolitano ni requisitos para la evaluación del impacto en la salud para las intervenciones urbanas o de transporte.  También carece de políticas de contaminación del aire relacionadas con el uso de la tierra.  Muchos estándares de políticas disponibles carecen de especificidad, mensurabilidad y/o consistencia con la evidencia de salud. Sin embargo, en relación con las 25 ciudades en este estudio internacional, la mayoría de los barrios de la Ciudad de México son transitables.  En términos de umbrales para las intervenciones en entornos construidos para alcanzar los objetivos de la OMS de aumentar la actividad física, el 98.1% de los residentes en la Ciudad de México viven en vecindarios que cumplen con el umbral de densidad mínima y el 77% cumple con el umbral de conectividad vial.  Sin embargo, en particular, muchos residentes en la Ciudad de México viven en vecindarios que pueden exceder los niveles de densidad y conectividad de las calles que fomentan la actividad física.  Solo el 20% de los residentes tiene acceso a paradas de transporte público con servicios regulares, con evidencia de que el acceso está diseñado espacialmente favoreciendo el centro de la ciudad.  Solo el 50% de los residentes tienen acceso a algún espacio público abierto dentro de los 500 m, y aún menos (20%) tienen acceso a un espacio abierto público más grande.  ¿La proporción de la población con acceso a menos de 500 metros de un mercado de alimentos, tienda de conveniencia, cualquier espacio público abierto, transporte público y grande? espacio público abierto, está muy por debajo de la media en comparación con otras ciudades estudiadas.</t>
-  </si>
-  <si>
     <t>La disponibilidad de políticas que apoyen la salud y la sostenibilidad en Baltimore está por debajo del promedio, y la calidad de las disponibles está muy por debajo del promedio en comparación con otras ciudades. Baltimore no parece requerir una evaluación del impacto en la salud de las intervenciones de transporte y uso de la tierra, y tiene pocas políticas específicas y medibles de transporte público y espacios abiertos.   Aparte del centro de la ciudad, la mayoría de los barrios de Baltimore tienen una baja transitabilidad en relación con las 25 ciudades de este estudio internacional.   Menos de un tercio de los barrios cumplen con los umbrales mínimos de densidad para alcanzar los objetivos de la OMS de aumentar la actividad física, y solo la mitad cumple con los umbrales de conectividad de las calles.  Una minoría de residentes tiene acceso a paradas de transporte público con servicios regulares a 500 metros.  Mientras que poco más de la mitad tiene espacio público abierto dentro de los 500 m, solo alrededor del 40 por ciento tiene acceso a espacios abiertos públicos más grandes. El porcentaje de la población de Baltimore con acceso a menos de 500 metros a un mercado de alimentos, tienda de conveniencia, cualquier espacio abierto público o un espacio abierto más grande y transporte público está muy por debajo del promedio en comparación con otras ciudades estudiadas.</t>
   </si>
   <si>
@@ -5759,6 +5756,9 @@
   </si>
   <si>
     <t>Kết nối đường phố trong</t>
+  </si>
+  <si>
+    <t>La disponibilidad y calidad de las políticas urbanas y de transporte que apoyan la salud y la sustentabilidad en la Ciudad de México está justo por debajo del promedio en comparación con otras ciudades. La Ciudad de México no parece tener acciones específicas centradas en la salud en su política de transporte metropolitano ni requisitos para la evaluación del impacto en la salud de las intervenciones urbanas o de transporte. También carece de políticas de contaminación del aire relacionadas con el uso de la tierra. Muchos estándares de políticas disponibles carecen de especificidad, mensurabilidad y/o consistencia con la evidencia de salud. No obstante, en relación con las 25 ciudades de este estudio internacional, la mayoría de los barrios de la Ciudad de México son transitables. En cuanto a los umbrales para las intervenciones en el entorno construido para lograr los objetivos de la OMS de aumentar la actividad física, el 98,1 % de los residentes de la Ciudad de México vive en barrios que alcanzan el umbral de densidad mínima y el 77 % alcanza el umbral de conectividad de calles. Sin embargo, en particular, muchos residentes de la Ciudad de México viven en vecindarios que pueden superar los niveles de densidad y conectividad de las calles que fomentan la actividad física. Solo el 20% de los residentes tiene acceso a paradas de transporte público con servicios regulares, con evidencia de que el acceso tiene un patrón espacial que favorece el centro de la ciudad. Solo el 50 % de los residentes tiene acceso a algún espacio público abierto dentro de los 500 m, y aún menos (20 %) tiene acceso a un espacio público abierto más grande. La proporción de la población con acceso a servicios dentro de los 500 m está por debajo del promedio en comparación con otras ciudades estudiadas.</t>
   </si>
 </sst>
 </file>
@@ -6909,8 +6909,8 @@
   <dimension ref="A1:V194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
+      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E158" sqref="E158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7058,7 +7058,7 @@
         <v>5</v>
       </c>
       <c r="F3">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G3">
         <f>E3+3</f>
@@ -7080,7 +7080,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="N3" t="s">
         <v>21</v>
@@ -7122,7 +7122,7 @@
         <v>5</v>
       </c>
       <c r="F4">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G4">
         <f>E4+3</f>
@@ -7144,7 +7144,7 @@
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="N4" t="s">
         <v>21</v>
@@ -7186,7 +7186,7 @@
         <v>5</v>
       </c>
       <c r="F5">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G5">
         <f>E5+3</f>
@@ -7208,7 +7208,7 @@
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="N5" t="s">
         <v>21</v>
@@ -16312,15 +16312,15 @@
         <v>7</v>
       </c>
       <c r="E158">
-        <f>G128+11</f>
-        <v>135</v>
+        <f>G128+4</f>
+        <v>128</v>
       </c>
       <c r="F158">
         <v>203</v>
       </c>
       <c r="G158">
         <f>E158+3</f>
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="H158" t="s">
         <v>266</v>
@@ -16371,14 +16371,14 @@
       </c>
       <c r="E159">
         <f>G158+4</f>
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="F159">
         <v>205</v>
       </c>
       <c r="G159">
         <f>E159+4</f>
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="H159" t="s">
         <v>266</v>
@@ -16430,7 +16430,7 @@
       </c>
       <c r="E160">
         <f>G158+4</f>
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="F160">
         <f>D160+88</f>
@@ -16438,7 +16438,7 @@
       </c>
       <c r="G160">
         <f>E160+80</f>
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="I160">
         <v>0</v>
@@ -16486,7 +16486,7 @@
       </c>
       <c r="E161">
         <f>G160-28</f>
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F161">
         <f>F166</f>
@@ -16494,7 +16494,7 @@
       </c>
       <c r="G161">
         <f>G160+4</f>
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="I161">
         <v>0</v>
@@ -16546,14 +16546,14 @@
       </c>
       <c r="E162">
         <f>E161+2</f>
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="F162">
         <v>174</v>
       </c>
       <c r="G162">
         <f>E162+3</f>
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="H162" t="s">
         <v>266</v>
@@ -16605,7 +16605,7 @@
       </c>
       <c r="E163">
         <f>E161+7</f>
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="F163">
         <f>D163+18</f>
@@ -16613,7 +16613,7 @@
       </c>
       <c r="G163">
         <f>E163+3</f>
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="H163" t="s">
         <v>266</v>
@@ -16665,7 +16665,7 @@
       </c>
       <c r="E164">
         <f>E163</f>
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="F164">
         <f>D168-1</f>
@@ -16673,7 +16673,7 @@
       </c>
       <c r="G164">
         <f>E164+3</f>
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="H164" t="s">
         <v>266</v>
@@ -16725,7 +16725,7 @@
       </c>
       <c r="E165">
         <f>E164</f>
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="F165">
         <f>D169+1</f>
@@ -16733,7 +16733,7 @@
       </c>
       <c r="G165">
         <f>E165+3</f>
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="H165" t="s">
         <v>266</v>
@@ -16785,7 +16785,7 @@
       </c>
       <c r="E166">
         <f>E165</f>
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="F166">
         <f>D166+18</f>
@@ -16793,7 +16793,7 @@
       </c>
       <c r="G166">
         <f>E166+3</f>
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="H166" t="s">
         <v>266</v>
@@ -16845,7 +16845,7 @@
       </c>
       <c r="E167">
         <f>E163</f>
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="F167">
         <f>F163+1</f>
@@ -16853,7 +16853,7 @@
       </c>
       <c r="G167">
         <f>G175+3</f>
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="I167">
         <v>0</v>
@@ -16902,7 +16902,7 @@
       </c>
       <c r="E168">
         <f>E163</f>
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="F168">
         <f t="shared" ref="F168:F169" si="5">D168</f>
@@ -16910,7 +16910,7 @@
       </c>
       <c r="G168">
         <f>G167</f>
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="I168">
         <v>0</v>
@@ -16959,7 +16959,7 @@
       </c>
       <c r="E169">
         <f>E163</f>
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="F169">
         <f t="shared" si="5"/>
@@ -16967,7 +16967,7 @@
       </c>
       <c r="G169">
         <f>G168</f>
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="I169">
         <v>0</v>
@@ -17016,7 +17016,7 @@
       </c>
       <c r="E170">
         <f>E163+10</f>
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="F170">
         <f>F161</f>
@@ -17024,7 +17024,7 @@
       </c>
       <c r="G170">
         <f>E170</f>
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="I170">
         <v>0</v>
@@ -17073,7 +17073,7 @@
       </c>
       <c r="E171">
         <f>E170+2</f>
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="F171">
         <f>D171+36</f>
@@ -17081,7 +17081,7 @@
       </c>
       <c r="G171">
         <f>E171+4</f>
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="H171" t="s">
         <v>266</v>
@@ -17133,7 +17133,7 @@
       </c>
       <c r="E172">
         <f>E171+1</f>
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F172">
         <f>D172+4</f>
@@ -17141,7 +17141,7 @@
       </c>
       <c r="G172">
         <f>E172+3</f>
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="H172" t="s">
         <v>20</v>
@@ -17193,7 +17193,7 @@
       </c>
       <c r="E173">
         <f>E172</f>
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F173">
         <f>D173+4</f>
@@ -17201,7 +17201,7 @@
       </c>
       <c r="G173">
         <f>E173+3</f>
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="H173" t="s">
         <v>20</v>
@@ -17253,7 +17253,7 @@
       </c>
       <c r="E174">
         <f>E173</f>
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F174">
         <f>D174+4</f>
@@ -17261,7 +17261,7 @@
       </c>
       <c r="G174">
         <f>E174+3</f>
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="H174" t="s">
         <v>20</v>
@@ -17313,7 +17313,7 @@
       </c>
       <c r="E175">
         <f>E174</f>
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F175">
         <f>D175+4</f>
@@ -17321,7 +17321,7 @@
       </c>
       <c r="G175">
         <f>E175+3</f>
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="H175" t="s">
         <v>20</v>
@@ -17372,10 +17372,10 @@
       </c>
       <c r="E176">
         <f>G161+4</f>
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F176">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="G176">
         <v>298</v>
@@ -17429,15 +17429,15 @@
       </c>
       <c r="E177">
         <f>E176+3</f>
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="F177">
         <f>F176-14</f>
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="G177">
         <f>E177+4</f>
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="H177" t="s">
         <v>266</v>
@@ -17489,15 +17489,15 @@
       </c>
       <c r="E178">
         <f>G177+2</f>
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="F178">
         <f>F177</f>
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="G178">
         <f>E178+4</f>
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="H178" t="s">
         <v>266</v>
@@ -18430,10 +18430,10 @@
   <dimension ref="A1:AG157"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AC106" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="S134" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE120" sqref="AE120"/>
+      <selection pane="bottomRight" activeCell="T134" sqref="T134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18499,7 +18499,7 @@
         <v>289</v>
       </c>
       <c r="R1" s="19" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="S1" s="19" t="s">
         <v>1106</v>
@@ -18588,7 +18588,7 @@
       <c r="P2" s="20"/>
       <c r="Q2" s="20"/>
       <c r="R2" s="20" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="S2" s="20" t="s">
         <v>725</v>
@@ -18644,7 +18644,7 @@
       </c>
       <c r="F3" s="22"/>
       <c r="G3" s="22" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="H3" s="23"/>
       <c r="I3" s="23" t="s">
@@ -18665,7 +18665,7 @@
       <c r="P3" s="37"/>
       <c r="Q3" s="37"/>
       <c r="R3" s="37" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="S3" s="22" t="s">
         <v>834</v>
@@ -18694,7 +18694,7 @@
       </c>
       <c r="AD3" s="22"/>
       <c r="AE3" s="22" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="AF3" s="22"/>
       <c r="AG3" s="22"/>
@@ -18736,7 +18736,7 @@
       <c r="P4" s="37"/>
       <c r="Q4" s="37"/>
       <c r="R4" s="37" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="S4" s="22" t="s">
         <v>835</v>
@@ -18807,7 +18807,7 @@
       <c r="P5" s="37"/>
       <c r="Q5" s="37"/>
       <c r="R5" s="37" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="S5" s="22" t="s">
         <v>726</v>
@@ -18836,7 +18836,7 @@
       </c>
       <c r="AD5" s="22"/>
       <c r="AE5" s="22" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="AF5" s="22"/>
       <c r="AG5" s="22"/>
@@ -19896,7 +19896,7 @@
       <c r="P30" s="37"/>
       <c r="Q30" s="37"/>
       <c r="R30" s="37" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="S30" s="22"/>
       <c r="T30" s="22"/>
@@ -20969,7 +20969,7 @@
       <c r="P55" s="37"/>
       <c r="Q55" s="37"/>
       <c r="R55" s="37" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="S55" s="22"/>
       <c r="T55" s="22"/>
@@ -21024,7 +21024,7 @@
       <c r="P56" s="37"/>
       <c r="Q56" s="37"/>
       <c r="R56" s="37" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="S56" s="20" t="s">
         <v>727</v>
@@ -21095,7 +21095,7 @@
       <c r="P57" s="37"/>
       <c r="Q57" s="37"/>
       <c r="R57" s="37" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="S57" s="20" t="s">
         <v>728</v>
@@ -21166,7 +21166,7 @@
       <c r="P58" s="37"/>
       <c r="Q58" s="37"/>
       <c r="R58" s="37" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="S58" s="20" t="s">
         <v>368</v>
@@ -21237,7 +21237,7 @@
       <c r="P59" s="37"/>
       <c r="Q59" s="37"/>
       <c r="R59" s="37" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="S59" s="20" t="s">
         <v>729</v>
@@ -21308,7 +21308,7 @@
       <c r="P60" s="37"/>
       <c r="Q60" s="37"/>
       <c r="R60" s="37" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="S60" s="20" t="s">
         <v>370</v>
@@ -21379,7 +21379,7 @@
       <c r="P61" s="37"/>
       <c r="Q61" s="37"/>
       <c r="R61" s="37" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="S61" s="20" t="s">
         <v>371</v>
@@ -21450,7 +21450,7 @@
       <c r="P62" s="37"/>
       <c r="Q62" s="37"/>
       <c r="R62" s="37" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="S62" s="20" t="s">
         <v>372</v>
@@ -21521,7 +21521,7 @@
       <c r="P63" s="37"/>
       <c r="Q63" s="37"/>
       <c r="R63" s="37" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="S63" s="20" t="s">
         <v>730</v>
@@ -21534,7 +21534,7 @@
       </c>
       <c r="V63" s="20"/>
       <c r="W63" s="37" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="X63" s="20"/>
       <c r="Y63" s="37" t="s">
@@ -21542,11 +21542,11 @@
       </c>
       <c r="Z63" s="20"/>
       <c r="AA63" s="39" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="AB63" s="20"/>
       <c r="AC63" s="20" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="AD63" s="20"/>
       <c r="AE63" s="20" t="s">
@@ -21592,7 +21592,7 @@
       <c r="P64" s="37"/>
       <c r="Q64" s="37"/>
       <c r="R64" s="37" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="S64" s="20" t="s">
         <v>373</v>
@@ -21663,7 +21663,7 @@
       <c r="P65" s="37"/>
       <c r="Q65" s="37"/>
       <c r="R65" s="37" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="S65" s="20" t="s">
         <v>374</v>
@@ -21734,7 +21734,7 @@
       <c r="P66" s="37"/>
       <c r="Q66" s="37"/>
       <c r="R66" s="37" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="S66" s="20" t="s">
         <v>375</v>
@@ -21805,7 +21805,7 @@
       <c r="P67" s="37"/>
       <c r="Q67" s="37"/>
       <c r="R67" s="37" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="S67" s="20" t="s">
         <v>747</v>
@@ -21834,7 +21834,7 @@
       </c>
       <c r="AD67" s="20"/>
       <c r="AE67" s="20" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="AF67" s="20"/>
       <c r="AG67" s="20"/>
@@ -21876,7 +21876,7 @@
       <c r="P68" s="37"/>
       <c r="Q68" s="37"/>
       <c r="R68" s="37" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="S68" s="20" t="s">
         <v>750</v>
@@ -21885,7 +21885,7 @@
         <v>750</v>
       </c>
       <c r="U68" s="20" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="V68" s="20"/>
       <c r="W68" s="37" t="s">
@@ -21897,15 +21897,15 @@
       </c>
       <c r="Z68" s="20"/>
       <c r="AA68" s="39" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="AB68" s="20"/>
       <c r="AC68" s="20" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="AD68" s="20"/>
       <c r="AE68" s="20" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="AF68" s="20"/>
       <c r="AG68" s="20"/>
@@ -21922,7 +21922,7 @@
       </c>
       <c r="D69" s="20"/>
       <c r="E69" s="20" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="F69" s="20"/>
       <c r="G69" s="20" t="s">
@@ -21934,7 +21934,7 @@
       </c>
       <c r="J69" s="20"/>
       <c r="K69" s="37" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="L69" s="37"/>
       <c r="M69" s="37" t="s">
@@ -21942,29 +21942,29 @@
       </c>
       <c r="N69" s="20"/>
       <c r="O69" s="37" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="P69" s="37"/>
       <c r="Q69" s="37"/>
       <c r="R69" s="37" t="s">
+        <v>1660</v>
+      </c>
+      <c r="S69" s="20" t="s">
         <v>1661</v>
       </c>
-      <c r="S69" s="20" t="s">
+      <c r="T69" s="22" t="s">
+        <v>1661</v>
+      </c>
+      <c r="U69" s="20" t="s">
         <v>1662</v>
-      </c>
-      <c r="T69" s="22" t="s">
-        <v>1662</v>
-      </c>
-      <c r="U69" s="20" t="s">
-        <v>1663</v>
       </c>
       <c r="V69" s="20"/>
       <c r="W69" s="37" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="X69" s="20"/>
       <c r="Y69" s="37" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="Z69" s="20"/>
       <c r="AA69" s="39" t="s">
@@ -21972,11 +21972,11 @@
       </c>
       <c r="AB69" s="20"/>
       <c r="AC69" s="20" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="AD69" s="20"/>
       <c r="AE69" s="20" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="AF69" s="20"/>
       <c r="AG69" s="20"/>
@@ -21997,7 +21997,7 @@
       </c>
       <c r="F70" s="20"/>
       <c r="G70" s="20" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="H70" s="21"/>
       <c r="I70" s="21" t="s">
@@ -22018,36 +22018,36 @@
       <c r="P70" s="37"/>
       <c r="Q70" s="37"/>
       <c r="R70" s="37" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="S70" s="20" t="s">
+        <v>1421</v>
+      </c>
+      <c r="T70" s="22" t="s">
         <v>1422</v>
-      </c>
-      <c r="T70" s="22" t="s">
-        <v>1423</v>
       </c>
       <c r="U70" s="20" t="s">
         <v>1386</v>
       </c>
       <c r="V70" s="20"/>
       <c r="W70" s="37" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="X70" s="20"/>
       <c r="Y70" s="37" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="Z70" s="20"/>
       <c r="AA70" s="39" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="AB70" s="20"/>
       <c r="AC70" s="20" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="AD70" s="20"/>
       <c r="AE70" s="20" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="AF70" s="20"/>
       <c r="AG70" s="20"/>
@@ -22068,7 +22068,7 @@
       </c>
       <c r="F71" s="20"/>
       <c r="G71" s="20" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="H71" s="21"/>
       <c r="I71" s="21" t="s">
@@ -22089,36 +22089,36 @@
       <c r="P71" s="37"/>
       <c r="Q71" s="37"/>
       <c r="R71" s="37" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="S71" s="20" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="T71" s="22" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="U71" s="20" t="s">
         <v>1387</v>
       </c>
       <c r="V71" s="20"/>
       <c r="W71" s="37" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="X71" s="20"/>
       <c r="Y71" s="37" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="Z71" s="20"/>
       <c r="AA71" s="39" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="AB71" s="20"/>
       <c r="AC71" s="20" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="AD71" s="20"/>
       <c r="AE71" s="20" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="AF71" s="20"/>
       <c r="AG71" s="20"/>
@@ -22139,7 +22139,7 @@
       </c>
       <c r="F72" s="20"/>
       <c r="G72" s="20" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="H72" s="21"/>
       <c r="I72" s="21" t="s">
@@ -22160,7 +22160,7 @@
       <c r="P72" s="37"/>
       <c r="Q72" s="37"/>
       <c r="R72" s="37" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="S72" s="20" t="s">
         <v>1388</v>
@@ -22173,23 +22173,23 @@
       </c>
       <c r="V72" s="20"/>
       <c r="W72" s="37" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="X72" s="20"/>
       <c r="Y72" s="37" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="Z72" s="20"/>
       <c r="AA72" s="39" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="AB72" s="20"/>
       <c r="AC72" s="20" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="AD72" s="20"/>
       <c r="AE72" s="20" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="AF72" s="20"/>
       <c r="AG72" s="20"/>
@@ -22231,7 +22231,7 @@
       <c r="P73" s="37"/>
       <c r="Q73" s="37"/>
       <c r="R73" s="37" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="S73" s="20" t="s">
         <v>376</v>
@@ -22302,7 +22302,7 @@
       <c r="P74" s="37"/>
       <c r="Q74" s="37"/>
       <c r="R74" s="37" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="S74" s="20" t="s">
         <v>731</v>
@@ -22373,7 +22373,7 @@
       <c r="P75" s="37"/>
       <c r="Q75" s="37"/>
       <c r="R75" s="37" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="S75" s="20" t="s">
         <v>836</v>
@@ -22444,7 +22444,7 @@
       <c r="P76" s="37"/>
       <c r="Q76" s="37"/>
       <c r="R76" s="37" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="S76" s="20" t="s">
         <v>1109</v>
@@ -22515,7 +22515,7 @@
       <c r="P77" s="37"/>
       <c r="Q77" s="37"/>
       <c r="R77" s="37" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="S77" s="20" t="s">
         <v>1111</v>
@@ -22586,36 +22586,36 @@
       <c r="P78" s="37"/>
       <c r="Q78" s="37"/>
       <c r="R78" s="37" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="S78" s="20" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="T78" s="22" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="U78" s="20" t="s">
         <v>1389</v>
       </c>
       <c r="V78" s="20"/>
       <c r="W78" s="37" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="X78" s="20"/>
       <c r="Y78" s="37" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="Z78" s="20"/>
       <c r="AA78" s="39" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="AB78" s="20"/>
       <c r="AC78" s="20" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="AD78" s="20"/>
       <c r="AE78" s="20" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="AF78" s="20"/>
       <c r="AG78" s="20"/>
@@ -22636,7 +22636,7 @@
       </c>
       <c r="F79" s="22"/>
       <c r="G79" s="22" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="H79" s="23"/>
       <c r="I79" s="23" t="s">
@@ -22657,36 +22657,36 @@
       <c r="P79" s="37"/>
       <c r="Q79" s="37"/>
       <c r="R79" s="37" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="S79" s="22" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="T79" s="22" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="U79" s="22" t="s">
         <v>1390</v>
       </c>
       <c r="V79" s="22"/>
       <c r="W79" s="37" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="X79" s="22"/>
       <c r="Y79" s="37" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="Z79" s="22"/>
       <c r="AA79" s="39" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="AB79" s="22"/>
       <c r="AC79" s="22" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="AD79" s="22"/>
       <c r="AE79" s="22" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="AF79" s="22"/>
       <c r="AG79" s="22"/>
@@ -22707,7 +22707,7 @@
       </c>
       <c r="F80" s="22"/>
       <c r="G80" s="22" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="H80" s="23"/>
       <c r="I80" s="23" t="s">
@@ -22728,36 +22728,36 @@
       <c r="P80" s="37"/>
       <c r="Q80" s="37"/>
       <c r="R80" s="37" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="S80" s="22" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="T80" s="22" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="U80" s="22" t="s">
         <v>1391</v>
       </c>
       <c r="V80" s="22"/>
       <c r="W80" s="37" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="X80" s="22"/>
       <c r="Y80" s="37" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="Z80" s="22"/>
       <c r="AA80" s="39" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="AB80" s="22"/>
       <c r="AC80" s="22" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="AD80" s="22"/>
       <c r="AE80" s="22" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="AF80" s="22"/>
       <c r="AG80" s="22"/>
@@ -22799,7 +22799,7 @@
       <c r="P81" s="37"/>
       <c r="Q81" s="37"/>
       <c r="R81" s="37" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="S81" s="22" t="s">
         <v>558</v>
@@ -22870,7 +22870,7 @@
       <c r="P82" s="37"/>
       <c r="Q82" s="37"/>
       <c r="R82" s="37" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="S82" s="22" t="s">
         <v>732</v>
@@ -22912,65 +22912,65 @@
         <v>42</v>
       </c>
       <c r="C83" s="23" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="D83" s="22"/>
       <c r="E83" s="22" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="F83" s="22"/>
       <c r="G83" s="22" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="H83" s="23"/>
       <c r="I83" s="23" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="J83" s="22"/>
       <c r="K83" s="37" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="L83" s="37"/>
       <c r="M83" s="37" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="N83" s="22"/>
       <c r="O83" s="37" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="P83" s="37"/>
       <c r="Q83" s="37"/>
       <c r="R83" s="37" t="s">
+        <v>1820</v>
+      </c>
+      <c r="S83" s="22" t="s">
         <v>1821</v>
       </c>
-      <c r="S83" s="22" t="s">
-        <v>1822</v>
-      </c>
       <c r="T83" s="22" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="U83" s="22" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="V83" s="22"/>
       <c r="W83" s="37" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="X83" s="22"/>
       <c r="Y83" s="37" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="Z83" s="22"/>
       <c r="AA83" s="39" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="AB83" s="22"/>
       <c r="AC83" s="22" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="AD83" s="22"/>
       <c r="AE83" s="22" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="AF83" s="22"/>
       <c r="AG83" s="22"/>
@@ -22987,15 +22987,15 @@
       </c>
       <c r="D84" s="22"/>
       <c r="E84" s="22" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="F84" s="22"/>
       <c r="G84" s="22" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="H84" s="23"/>
       <c r="I84" s="23" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="J84" s="22"/>
       <c r="K84" s="37" t="s">
@@ -23012,36 +23012,36 @@
       <c r="P84" s="37"/>
       <c r="Q84" s="37"/>
       <c r="R84" s="37" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="S84" s="22" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="T84" s="22" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="U84" s="22" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="V84" s="22"/>
       <c r="W84" s="37" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="X84" s="22"/>
       <c r="Y84" s="37" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="Z84" s="22"/>
       <c r="AA84" s="39" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="AB84" s="22"/>
       <c r="AC84" s="22" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="AD84" s="22"/>
       <c r="AE84" s="22" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="AF84" s="22"/>
       <c r="AG84" s="22"/>
@@ -23058,61 +23058,61 @@
       </c>
       <c r="D85" s="22"/>
       <c r="E85" s="22" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="F85" s="22"/>
       <c r="G85" s="22" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="H85" s="23"/>
       <c r="I85" s="23" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="J85" s="22"/>
       <c r="K85" s="37" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="L85" s="37"/>
       <c r="M85" s="37" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="N85" s="22"/>
       <c r="O85" s="37" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="P85" s="37"/>
       <c r="Q85" s="37"/>
       <c r="R85" s="37" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="S85" s="22" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="T85" s="22" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="U85" s="22" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="V85" s="22"/>
       <c r="W85" s="37" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="X85" s="22"/>
       <c r="Y85" s="37" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="Z85" s="22"/>
       <c r="AA85" s="39" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="AB85" s="22"/>
       <c r="AC85" s="22" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="AD85" s="22"/>
       <c r="AE85" s="22" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="AF85" s="22"/>
       <c r="AG85" s="22"/>
@@ -23133,7 +23133,7 @@
       </c>
       <c r="F86" s="22"/>
       <c r="G86" s="22" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="H86" s="23"/>
       <c r="I86" s="23" t="s">
@@ -23145,45 +23145,45 @@
       </c>
       <c r="L86" s="37"/>
       <c r="M86" s="37" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="N86" s="22"/>
       <c r="O86" s="37" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="P86" s="37"/>
       <c r="Q86" s="37"/>
       <c r="R86" s="37" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="S86" s="22" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="T86" s="22" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="U86" s="22" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="V86" s="22"/>
       <c r="W86" s="37" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="X86" s="22"/>
       <c r="Y86" s="37" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="Z86" s="22"/>
       <c r="AA86" s="39" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="AB86" s="22"/>
       <c r="AC86" s="22" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="AD86" s="22"/>
       <c r="AE86" s="22" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="AF86" s="22"/>
       <c r="AG86" s="22"/>
@@ -23204,7 +23204,7 @@
       </c>
       <c r="F87" s="22"/>
       <c r="G87" s="22" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="H87" s="23"/>
       <c r="I87" s="23" t="s">
@@ -23216,29 +23216,29 @@
       </c>
       <c r="L87" s="37"/>
       <c r="M87" s="37" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="N87" s="22"/>
       <c r="O87" s="37" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="P87" s="37"/>
       <c r="Q87" s="37"/>
       <c r="R87" s="37" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="S87" s="22" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="T87" s="22" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="U87" s="22" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="V87" s="22"/>
       <c r="W87" s="37" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="X87" s="22"/>
       <c r="Y87" s="37" t="s">
@@ -23246,15 +23246,15 @@
       </c>
       <c r="Z87" s="22"/>
       <c r="AA87" s="39" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="AB87" s="22"/>
       <c r="AC87" s="22" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="AD87" s="22"/>
       <c r="AE87" s="22" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="AF87" s="22"/>
       <c r="AG87" s="22"/>
@@ -23267,65 +23267,65 @@
         <v>47</v>
       </c>
       <c r="C88" s="23" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="D88" s="22"/>
       <c r="E88" s="22" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="F88" s="22"/>
       <c r="G88" s="22" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="H88" s="23"/>
       <c r="I88" s="23" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="J88" s="22"/>
       <c r="K88" s="37" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="L88" s="37"/>
       <c r="M88" s="37" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="N88" s="22"/>
       <c r="O88" s="37" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="P88" s="37"/>
       <c r="Q88" s="37"/>
       <c r="R88" s="37" t="s">
+        <v>1835</v>
+      </c>
+      <c r="S88" s="22" t="s">
         <v>1836</v>
       </c>
-      <c r="S88" s="22" t="s">
-        <v>1837</v>
-      </c>
       <c r="T88" s="22" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="U88" s="22" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="V88" s="22"/>
       <c r="W88" s="37" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="X88" s="22"/>
       <c r="Y88" s="37" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="Z88" s="22"/>
       <c r="AA88" s="39" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="AB88" s="22"/>
       <c r="AC88" s="22" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="AD88" s="22"/>
       <c r="AE88" s="22" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="AF88" s="22"/>
       <c r="AG88" s="22"/>
@@ -23367,7 +23367,7 @@
       <c r="P89" s="37"/>
       <c r="Q89" s="37"/>
       <c r="R89" s="37" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="S89" s="22" t="s">
         <v>1392</v>
@@ -23380,23 +23380,23 @@
       </c>
       <c r="V89" s="22"/>
       <c r="W89" s="37" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="X89" s="22"/>
       <c r="Y89" s="37" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="Z89" s="22"/>
       <c r="AA89" s="39" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="AB89" s="22"/>
       <c r="AC89" s="22" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="AD89" s="22"/>
       <c r="AE89" s="22" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="AF89" s="22"/>
       <c r="AG89" s="22"/>
@@ -23438,7 +23438,7 @@
       <c r="P90" s="37"/>
       <c r="Q90" s="37"/>
       <c r="R90" s="37" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="S90" s="22" t="s">
         <v>1035</v>
@@ -23467,7 +23467,7 @@
       </c>
       <c r="AD90" s="22"/>
       <c r="AE90" s="22" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="AF90" s="22"/>
       <c r="AG90" s="22"/>
@@ -23509,7 +23509,7 @@
       <c r="P91" s="37"/>
       <c r="Q91" s="37"/>
       <c r="R91" s="37" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="S91" s="22" t="s">
         <v>733</v>
@@ -23522,23 +23522,23 @@
       </c>
       <c r="V91" s="22"/>
       <c r="W91" s="37" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="X91" s="22"/>
       <c r="Y91" s="37" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="Z91" s="22"/>
       <c r="AA91" s="39" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="AB91" s="22"/>
       <c r="AC91" s="22" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="AD91" s="22"/>
       <c r="AE91" s="22" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="AF91" s="22"/>
       <c r="AG91" s="22"/>
@@ -23580,7 +23580,7 @@
       <c r="P92" s="37"/>
       <c r="Q92" s="37"/>
       <c r="R92" s="37" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="S92" s="22" t="s">
         <v>1036</v>
@@ -23609,7 +23609,7 @@
       </c>
       <c r="AD92" s="22"/>
       <c r="AE92" s="22" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="AF92" s="22"/>
       <c r="AG92" s="22"/>
@@ -23651,7 +23651,7 @@
       <c r="P93" s="37"/>
       <c r="Q93" s="37"/>
       <c r="R93" s="37" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="S93" s="22" t="s">
         <v>734</v>
@@ -23722,7 +23722,7 @@
       <c r="P94" s="37"/>
       <c r="Q94" s="37"/>
       <c r="R94" s="37" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="S94" s="22" t="s">
         <v>735</v>
@@ -23793,7 +23793,7 @@
       <c r="P95" s="37"/>
       <c r="Q95" s="37"/>
       <c r="R95" s="37" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="S95" s="22" t="s">
         <v>1394</v>
@@ -23806,23 +23806,23 @@
       </c>
       <c r="V95" s="22"/>
       <c r="W95" s="37" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="X95" s="22"/>
       <c r="Y95" s="37" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="Z95" s="22"/>
       <c r="AA95" s="39" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="AB95" s="22"/>
       <c r="AC95" s="22" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="AD95" s="22"/>
       <c r="AE95" s="22" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="AF95" s="22"/>
       <c r="AG95" s="22"/>
@@ -23864,7 +23864,7 @@
       <c r="P96" s="37"/>
       <c r="Q96" s="37"/>
       <c r="R96" s="37" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="S96" s="22" t="s">
         <v>736</v>
@@ -23935,7 +23935,7 @@
       <c r="P97" s="37"/>
       <c r="Q97" s="37"/>
       <c r="R97" s="37" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="S97" s="22" t="s">
         <v>737</v>
@@ -24006,7 +24006,7 @@
       <c r="P98" s="37"/>
       <c r="Q98" s="37"/>
       <c r="R98" s="37" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="S98" s="22" t="s">
         <v>738</v>
@@ -24077,7 +24077,7 @@
       <c r="P99" s="37"/>
       <c r="Q99" s="37"/>
       <c r="R99" s="37" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="S99" s="22" t="s">
         <v>739</v>
@@ -24106,7 +24106,7 @@
       </c>
       <c r="AD99" s="22"/>
       <c r="AE99" s="22" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="AF99" s="22"/>
       <c r="AG99" s="22"/>
@@ -24148,7 +24148,7 @@
       <c r="P100" s="37"/>
       <c r="Q100" s="37"/>
       <c r="R100" s="37" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="S100" s="22" t="s">
         <v>740</v>
@@ -24177,7 +24177,7 @@
       </c>
       <c r="AD100" s="22"/>
       <c r="AE100" s="22" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="AF100" s="22"/>
       <c r="AG100" s="22"/>
@@ -24219,7 +24219,7 @@
       <c r="P101" s="37"/>
       <c r="Q101" s="37"/>
       <c r="R101" s="37" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="S101" s="22" t="s">
         <v>386</v>
@@ -24290,7 +24290,7 @@
       <c r="P102" s="37"/>
       <c r="Q102" s="37"/>
       <c r="R102" s="37" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="S102" s="22" t="s">
         <v>387</v>
@@ -24319,7 +24319,7 @@
       </c>
       <c r="AD102" s="22"/>
       <c r="AE102" s="22" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="AF102" s="22"/>
       <c r="AG102" s="22"/>
@@ -24361,7 +24361,7 @@
       <c r="P103" s="37"/>
       <c r="Q103" s="37"/>
       <c r="R103" s="37" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="S103" s="22" t="s">
         <v>388</v>
@@ -24403,7 +24403,7 @@
         <v>84</v>
       </c>
       <c r="C104" s="24" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="D104" s="22"/>
       <c r="E104" s="22" t="s">
@@ -24432,36 +24432,36 @@
       <c r="P104" s="37"/>
       <c r="Q104" s="37"/>
       <c r="R104" s="37" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="S104" s="22" t="s">
         <v>1104</v>
       </c>
       <c r="T104" s="25" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="U104" s="22" t="s">
         <v>1395</v>
       </c>
       <c r="V104" s="22"/>
       <c r="W104" s="37" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="X104" s="22"/>
       <c r="Y104" s="37" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="Z104" s="22"/>
       <c r="AA104" s="39" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="AB104" s="22"/>
       <c r="AC104" s="22" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="AD104" s="22"/>
       <c r="AE104" s="22" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="AF104" s="22"/>
       <c r="AG104" s="22"/>
@@ -24503,7 +24503,7 @@
       <c r="P105" s="37"/>
       <c r="Q105" s="37"/>
       <c r="R105" s="37" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="S105" s="22" t="s">
         <v>1032</v>
@@ -24532,7 +24532,7 @@
       </c>
       <c r="AD105" s="22"/>
       <c r="AE105" s="22" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="AF105" s="22"/>
       <c r="AG105" s="22"/>
@@ -24574,7 +24574,7 @@
       <c r="P106" s="37"/>
       <c r="Q106" s="37"/>
       <c r="R106" s="37" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="S106" s="22" t="s">
         <v>1033</v>
@@ -24603,7 +24603,7 @@
       </c>
       <c r="AD106" s="22"/>
       <c r="AE106" s="22" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="AF106" s="22"/>
       <c r="AG106" s="22"/>
@@ -24645,7 +24645,7 @@
       <c r="P107" s="37"/>
       <c r="Q107" s="37"/>
       <c r="R107" s="37" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="S107" s="22" t="s">
         <v>1034</v>
@@ -24674,7 +24674,7 @@
       </c>
       <c r="AD107" s="22"/>
       <c r="AE107" s="22" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="AF107" s="22"/>
       <c r="AG107" s="22"/>
@@ -24716,7 +24716,7 @@
       <c r="P108" s="37"/>
       <c r="Q108" s="37"/>
       <c r="R108" s="37" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="S108" s="22" t="s">
         <v>389</v>
@@ -24787,7 +24787,7 @@
       <c r="P109" s="37"/>
       <c r="Q109" s="37"/>
       <c r="R109" s="37" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="S109" s="22" t="s">
         <v>741</v>
@@ -24858,7 +24858,7 @@
       <c r="P110" s="37"/>
       <c r="Q110" s="37"/>
       <c r="R110" s="37" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="S110" s="22" t="s">
         <v>391</v>
@@ -24929,7 +24929,7 @@
       <c r="P111" s="37"/>
       <c r="Q111" s="37"/>
       <c r="R111" s="37" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="S111" s="22" t="s">
         <v>392</v>
@@ -25000,7 +25000,7 @@
       <c r="P112" s="37"/>
       <c r="Q112" s="37"/>
       <c r="R112" s="37" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="S112" s="22" t="s">
         <v>742</v>
@@ -25071,7 +25071,7 @@
       <c r="P113" s="37"/>
       <c r="Q113" s="37"/>
       <c r="R113" s="37" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="S113" s="22" t="s">
         <v>394</v>
@@ -25142,7 +25142,7 @@
       <c r="P114" s="37"/>
       <c r="Q114" s="37"/>
       <c r="R114" s="37" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="S114" s="22" t="s">
         <v>395</v>
@@ -25213,7 +25213,7 @@
       <c r="P115" s="37"/>
       <c r="Q115" s="37"/>
       <c r="R115" s="37" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="S115" s="22" t="s">
         <v>396</v>
@@ -25284,7 +25284,7 @@
       <c r="P116" s="37"/>
       <c r="Q116" s="37"/>
       <c r="R116" s="37" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="S116" s="22" t="s">
         <v>397</v>
@@ -25355,7 +25355,7 @@
       <c r="P117" s="37"/>
       <c r="Q117" s="37"/>
       <c r="R117" s="37" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="S117" s="22" t="s">
         <v>398</v>
@@ -25426,7 +25426,7 @@
       <c r="P118" s="37"/>
       <c r="Q118" s="37"/>
       <c r="R118" s="37" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="S118" s="22" t="s">
         <v>399</v>
@@ -25455,7 +25455,7 @@
       </c>
       <c r="AD118" s="22"/>
       <c r="AE118" s="22" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="AF118" s="22"/>
       <c r="AG118" s="22"/>
@@ -25468,65 +25468,65 @@
         <v>78</v>
       </c>
       <c r="C119" s="23" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="D119" s="22"/>
       <c r="E119" s="22" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="F119" s="22"/>
       <c r="G119" s="22" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="H119" s="23"/>
       <c r="I119" s="23" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="J119" s="22"/>
       <c r="K119" s="37" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="L119" s="37"/>
       <c r="M119" s="37" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="N119" s="22"/>
       <c r="O119" s="37" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="P119" s="37"/>
       <c r="Q119" s="37"/>
       <c r="R119" s="37" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="S119" s="22" t="s">
+        <v>1859</v>
+      </c>
+      <c r="T119" s="22" t="s">
+        <v>1859</v>
+      </c>
+      <c r="U119" s="22" t="s">
         <v>1860</v>
-      </c>
-      <c r="T119" s="22" t="s">
-        <v>1860</v>
-      </c>
-      <c r="U119" s="22" t="s">
-        <v>1861</v>
       </c>
       <c r="V119" s="22"/>
       <c r="W119" s="37" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="X119" s="22"/>
       <c r="Y119" s="37" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="Z119" s="22"/>
       <c r="AA119" s="39" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="AB119" s="22"/>
       <c r="AC119" s="22" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="AD119" s="22"/>
       <c r="AE119" s="22" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="AF119" s="22"/>
       <c r="AG119" s="22"/>
@@ -25539,65 +25539,65 @@
         <v>80</v>
       </c>
       <c r="C120" s="23" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="D120" s="22"/>
       <c r="E120" s="22" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="F120" s="25"/>
       <c r="G120" s="25" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="H120" s="23"/>
       <c r="I120" s="23" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="J120" s="22"/>
       <c r="K120" s="37" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="L120" s="37"/>
       <c r="M120" s="37" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="N120" s="22"/>
       <c r="O120" s="37" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="P120" s="37"/>
       <c r="Q120" s="37"/>
       <c r="R120" s="37" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="S120" s="22" t="s">
+        <v>1861</v>
+      </c>
+      <c r="T120" s="22" t="s">
+        <v>1861</v>
+      </c>
+      <c r="U120" s="22" t="s">
         <v>1862</v>
-      </c>
-      <c r="T120" s="22" t="s">
-        <v>1862</v>
-      </c>
-      <c r="U120" s="22" t="s">
-        <v>1863</v>
       </c>
       <c r="V120" s="22"/>
       <c r="W120" s="37" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="X120" s="22"/>
       <c r="Y120" s="37" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="Z120" s="25"/>
       <c r="AA120" s="39" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="AB120" s="22"/>
       <c r="AC120" s="22" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="AD120" s="22"/>
       <c r="AE120" s="22" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="AF120" s="22"/>
       <c r="AG120" s="22"/>
@@ -25610,65 +25610,65 @@
         <v>81</v>
       </c>
       <c r="C121" s="23" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="D121" s="22"/>
       <c r="E121" s="22" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="F121" s="22"/>
       <c r="G121" s="22" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="H121" s="23"/>
       <c r="I121" s="23" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="J121" s="22"/>
       <c r="K121" s="37" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="L121" s="37"/>
       <c r="M121" s="37" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="N121" s="22"/>
       <c r="O121" s="37" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="P121" s="37"/>
       <c r="Q121" s="37"/>
       <c r="R121" s="37" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="S121" s="22" t="s">
+        <v>1863</v>
+      </c>
+      <c r="T121" s="22" t="s">
+        <v>1863</v>
+      </c>
+      <c r="U121" s="22" t="s">
         <v>1864</v>
-      </c>
-      <c r="T121" s="22" t="s">
-        <v>1864</v>
-      </c>
-      <c r="U121" s="22" t="s">
-        <v>1865</v>
       </c>
       <c r="V121" s="22"/>
       <c r="W121" s="37" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="X121" s="22"/>
       <c r="Y121" s="37" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="Z121" s="22"/>
       <c r="AA121" s="39" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="AB121" s="22"/>
       <c r="AC121" s="22" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="AD121" s="22"/>
       <c r="AE121" s="22" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="AF121" s="22"/>
       <c r="AG121" s="22"/>
@@ -25710,7 +25710,7 @@
       <c r="P122" s="37"/>
       <c r="Q122" s="37"/>
       <c r="R122" s="37" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="S122" s="22" t="s">
         <v>743</v>
@@ -25739,7 +25739,7 @@
       </c>
       <c r="AD122" s="22"/>
       <c r="AE122" s="22" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="AF122" s="22"/>
       <c r="AG122" s="22"/>
@@ -25781,7 +25781,7 @@
       <c r="P123" s="37"/>
       <c r="Q123" s="37"/>
       <c r="R123" s="37" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="S123" s="22" t="s">
         <v>401</v>
@@ -25794,23 +25794,23 @@
       </c>
       <c r="V123" s="22"/>
       <c r="W123" s="37" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="X123" s="22"/>
       <c r="Y123" s="37" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="Z123" s="22"/>
       <c r="AA123" s="39" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="AB123" s="22"/>
       <c r="AC123" s="22" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="AD123" s="22"/>
       <c r="AE123" s="22" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="AF123" s="22"/>
       <c r="AG123" s="22"/>
@@ -25852,7 +25852,7 @@
       <c r="P124" s="37"/>
       <c r="Q124" s="37"/>
       <c r="R124" s="37" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="S124" s="22" t="s">
         <v>402</v>
@@ -25923,7 +25923,7 @@
       <c r="P125" s="37"/>
       <c r="Q125" s="37"/>
       <c r="R125" s="37" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="S125" s="22" t="s">
         <v>403</v>
@@ -25952,7 +25952,7 @@
       </c>
       <c r="AD125" s="22"/>
       <c r="AE125" s="22" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="AF125" s="22"/>
       <c r="AG125" s="22"/>
@@ -25994,7 +25994,7 @@
       <c r="P126" s="37"/>
       <c r="Q126" s="37"/>
       <c r="R126" s="37" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="S126" s="22" t="s">
         <v>404</v>
@@ -26065,7 +26065,7 @@
       <c r="P127" s="37"/>
       <c r="Q127" s="37"/>
       <c r="R127" s="37" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="S127" s="22" t="s">
         <v>744</v>
@@ -26094,7 +26094,7 @@
       </c>
       <c r="AD127" s="22"/>
       <c r="AE127" s="22" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="AF127" s="22"/>
       <c r="AG127" s="22"/>
@@ -26136,7 +26136,7 @@
       <c r="P128" s="37"/>
       <c r="Q128" s="37"/>
       <c r="R128" s="37" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="S128" s="22" t="s">
         <v>745</v>
@@ -26165,7 +26165,7 @@
       </c>
       <c r="AD128" s="22"/>
       <c r="AE128" s="22" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="AF128" s="22"/>
       <c r="AG128" s="22"/>
@@ -26186,7 +26186,7 @@
       </c>
       <c r="F129" s="22"/>
       <c r="G129" s="22" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="H129" s="23"/>
       <c r="I129" s="23" t="s">
@@ -26207,7 +26207,7 @@
       <c r="P129" s="37"/>
       <c r="Q129" s="37"/>
       <c r="R129" s="37" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="S129" s="22" t="s">
         <v>746</v>
@@ -26236,7 +26236,7 @@
       </c>
       <c r="AD129" s="22"/>
       <c r="AE129" s="22" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="AF129" s="22"/>
       <c r="AG129" s="22"/>
@@ -26253,61 +26253,61 @@
       </c>
       <c r="D130" s="22"/>
       <c r="E130" s="22" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="F130" s="22"/>
       <c r="G130" s="22" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="H130" s="23"/>
       <c r="I130" s="23" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="J130" s="22"/>
       <c r="K130" s="37" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="L130" s="37"/>
       <c r="M130" s="37" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="N130" s="22"/>
       <c r="O130" s="37" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="P130" s="37"/>
       <c r="Q130" s="37"/>
       <c r="R130" s="37" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="S130" s="22" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="T130" s="22" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="U130" s="22" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="V130" s="22"/>
       <c r="W130" s="37" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="X130" s="22"/>
       <c r="Y130" s="37" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="Z130" s="22"/>
       <c r="AA130" s="39" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="AB130" s="22"/>
       <c r="AC130" s="22" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="AD130" s="22"/>
       <c r="AE130" s="22" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="AF130" s="22"/>
       <c r="AG130" s="22"/>
@@ -26349,7 +26349,7 @@
       <c r="P131" s="38"/>
       <c r="Q131" s="38"/>
       <c r="R131" s="38" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="S131" s="22" t="s">
         <v>1045</v>
@@ -26362,23 +26362,23 @@
       </c>
       <c r="V131" s="22"/>
       <c r="W131" s="38" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="X131" s="22"/>
       <c r="Y131" s="38" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="Z131" s="22"/>
       <c r="AA131" s="40" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="AB131" s="22"/>
       <c r="AC131" s="22" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="AD131" s="22"/>
       <c r="AE131" s="22" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="AF131" s="22"/>
       <c r="AG131" s="22"/>
@@ -26420,7 +26420,7 @@
       <c r="P132" s="37"/>
       <c r="Q132" s="37"/>
       <c r="R132" s="37" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="S132" s="22" t="s">
         <v>562</v>
@@ -26449,7 +26449,7 @@
       </c>
       <c r="AD132" s="22"/>
       <c r="AE132" s="22" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="AF132" s="22"/>
       <c r="AG132" s="22"/>
@@ -26463,7 +26463,7 @@
         <v>Maiduguri - Summary</v>
       </c>
       <c r="C133" s="23" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="D133" s="22"/>
       <c r="E133" s="22" t="s">
@@ -26492,7 +26492,7 @@
       <c r="P133" s="37"/>
       <c r="Q133" s="37"/>
       <c r="R133" s="37" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="S133" s="22"/>
       <c r="T133" s="22"/>
@@ -26501,23 +26501,23 @@
       </c>
       <c r="V133" s="22"/>
       <c r="W133" s="37" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="X133" s="22"/>
       <c r="Y133" s="37" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="Z133" s="22"/>
       <c r="AA133" s="39" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="AB133" s="22"/>
       <c r="AC133" s="22" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="AD133" s="22"/>
       <c r="AE133" s="22" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="AF133" s="22"/>
       <c r="AG133" s="22"/>
@@ -26531,7 +26531,7 @@
         <v>Mexico City - Summary</v>
       </c>
       <c r="C134" s="23" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="D134" s="22"/>
       <c r="E134" s="22" t="s">
@@ -26560,34 +26560,34 @@
       <c r="P134" s="37"/>
       <c r="Q134" s="37"/>
       <c r="R134" s="37" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="S134" s="22" t="s">
-        <v>1398</v>
+        <v>1885</v>
       </c>
       <c r="T134" s="22"/>
       <c r="U134" s="22" t="s">
-        <v>1398</v>
+        <v>1885</v>
       </c>
       <c r="V134" s="22"/>
       <c r="W134" s="37" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="X134" s="22"/>
       <c r="Y134" s="37" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="Z134" s="22"/>
       <c r="AA134" s="39" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="AB134" s="22"/>
       <c r="AC134" s="22" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="AD134" s="22"/>
       <c r="AE134" s="22" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="AF134" s="22"/>
       <c r="AG134" s="22"/>
@@ -26630,32 +26630,32 @@
       <c r="P135" s="37"/>
       <c r="Q135" s="37"/>
       <c r="R135" s="37" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="S135" s="22"/>
       <c r="T135" s="22"/>
       <c r="U135" s="22" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="V135" s="22"/>
       <c r="W135" s="37" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="X135" s="22"/>
       <c r="Y135" s="37" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="Z135" s="22"/>
       <c r="AA135" s="39" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="AB135" s="22"/>
       <c r="AC135" s="22" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="AD135" s="22"/>
       <c r="AE135" s="22" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="AF135" s="22"/>
       <c r="AG135" s="22"/>
@@ -26698,32 +26698,32 @@
       <c r="P136" s="37"/>
       <c r="Q136" s="37"/>
       <c r="R136" s="37" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="S136" s="22"/>
       <c r="T136" s="22"/>
       <c r="U136" s="22" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="V136" s="22"/>
       <c r="W136" s="37" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="X136" s="22"/>
       <c r="Y136" s="37" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="Z136" s="22"/>
       <c r="AA136" s="39" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="AB136" s="22"/>
       <c r="AC136" s="22" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="AD136" s="22"/>
       <c r="AE136" s="22" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="AF136" s="22"/>
       <c r="AG136" s="22"/>
@@ -26766,32 +26766,32 @@
       <c r="P137" s="37"/>
       <c r="Q137" s="37"/>
       <c r="R137" s="37" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="S137" s="22"/>
       <c r="T137" s="22"/>
       <c r="U137" s="22" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="V137" s="22"/>
       <c r="W137" s="37" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="X137" s="22"/>
       <c r="Y137" s="37" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="Z137" s="22"/>
       <c r="AA137" s="39" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="AB137" s="22"/>
       <c r="AC137" s="22" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="AD137" s="22"/>
       <c r="AE137" s="22" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="AF137" s="22"/>
       <c r="AG137" s="22"/>
@@ -26834,32 +26834,32 @@
       <c r="P138" s="37"/>
       <c r="Q138" s="37"/>
       <c r="R138" s="37" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="S138" s="22"/>
       <c r="T138" s="22"/>
       <c r="U138" s="22" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="V138" s="22"/>
       <c r="W138" s="37" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="X138" s="22"/>
       <c r="Y138" s="37" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="Z138" s="22"/>
       <c r="AA138" s="39" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="AB138" s="22"/>
       <c r="AC138" s="22" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="AD138" s="22"/>
       <c r="AE138" s="22" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="AF138" s="22"/>
       <c r="AG138" s="22"/>
@@ -26902,32 +26902,32 @@
       <c r="P139" s="37"/>
       <c r="Q139" s="37"/>
       <c r="R139" s="37" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="S139" s="22"/>
       <c r="T139" s="22"/>
       <c r="U139" s="22" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="V139" s="22"/>
       <c r="W139" s="37" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="X139" s="22"/>
       <c r="Y139" s="37" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="Z139" s="22"/>
       <c r="AA139" s="39" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="AB139" s="22"/>
       <c r="AC139" s="22" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="AD139" s="22"/>
       <c r="AE139" s="22" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="AF139" s="22"/>
       <c r="AG139" s="22"/>
@@ -26970,32 +26970,32 @@
       <c r="P140" s="37"/>
       <c r="Q140" s="37"/>
       <c r="R140" s="37" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="S140" s="22"/>
       <c r="T140" s="22"/>
       <c r="U140" s="22" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="V140" s="22"/>
       <c r="W140" s="37" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="X140" s="22"/>
       <c r="Y140" s="37" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="Z140" s="22"/>
       <c r="AA140" s="39" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="AB140" s="22"/>
       <c r="AC140" s="22" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="AD140" s="22"/>
       <c r="AE140" s="22" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="AF140" s="22"/>
       <c r="AG140" s="22"/>
@@ -27038,32 +27038,32 @@
       <c r="P141" s="37"/>
       <c r="Q141" s="37"/>
       <c r="R141" s="37" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="S141" s="22"/>
       <c r="T141" s="22"/>
       <c r="U141" s="22" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="V141" s="22"/>
       <c r="W141" s="37" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="X141" s="22"/>
       <c r="Y141" s="37" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="Z141" s="22"/>
       <c r="AA141" s="39" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="AB141" s="22"/>
       <c r="AC141" s="22" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="AD141" s="22"/>
       <c r="AE141" s="22" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="AF141" s="22"/>
       <c r="AG141" s="22"/>
@@ -27106,32 +27106,32 @@
       <c r="P142" s="37"/>
       <c r="Q142" s="37"/>
       <c r="R142" s="37" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="S142" s="22"/>
       <c r="T142" s="22"/>
       <c r="U142" s="22" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="V142" s="22"/>
       <c r="W142" s="37" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="X142" s="22"/>
       <c r="Y142" s="37" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="Z142" s="22"/>
       <c r="AA142" s="39" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="AB142" s="22"/>
       <c r="AC142" s="22" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="AD142" s="22"/>
       <c r="AE142" s="22" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="AF142" s="22"/>
       <c r="AG142" s="22"/>
@@ -27174,32 +27174,32 @@
       <c r="P143" s="37"/>
       <c r="Q143" s="37"/>
       <c r="R143" s="37" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="S143" s="22"/>
       <c r="T143" s="22"/>
       <c r="U143" s="22" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="V143" s="22"/>
       <c r="W143" s="37" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="X143" s="22"/>
       <c r="Y143" s="37" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="Z143" s="22"/>
       <c r="AA143" s="39" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="AB143" s="22"/>
       <c r="AC143" s="22" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="AD143" s="22"/>
       <c r="AE143" s="22" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="AF143" s="22"/>
       <c r="AG143" s="22"/>
@@ -27242,32 +27242,32 @@
       <c r="P144" s="37"/>
       <c r="Q144" s="37"/>
       <c r="R144" s="37" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="S144" s="22"/>
       <c r="T144" s="22"/>
       <c r="U144" s="22" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="V144" s="22"/>
       <c r="W144" s="37" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="X144" s="22"/>
       <c r="Y144" s="37" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="Z144" s="22"/>
       <c r="AA144" s="39" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="AB144" s="22"/>
       <c r="AC144" s="22" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="AD144" s="22"/>
       <c r="AE144" s="22" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="AF144" s="22"/>
       <c r="AG144" s="22"/>
@@ -27310,32 +27310,32 @@
       <c r="P145" s="37"/>
       <c r="Q145" s="37"/>
       <c r="R145" s="37" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="S145" s="22"/>
       <c r="T145" s="22"/>
       <c r="U145" s="22" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="V145" s="22"/>
       <c r="W145" s="37" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="X145" s="22"/>
       <c r="Y145" s="37" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="Z145" s="22"/>
       <c r="AA145" s="39" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="AB145" s="22"/>
       <c r="AC145" s="22" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="AD145" s="22"/>
       <c r="AE145" s="22" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="AF145" s="22"/>
       <c r="AG145" s="22"/>
@@ -27378,32 +27378,32 @@
       <c r="P146" s="37"/>
       <c r="Q146" s="37"/>
       <c r="R146" s="37" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="S146" s="22"/>
       <c r="T146" s="22"/>
       <c r="U146" s="22" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="V146" s="22"/>
       <c r="W146" s="37" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="X146" s="22"/>
       <c r="Y146" s="37" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="Z146" s="22"/>
       <c r="AA146" s="39" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="AB146" s="22"/>
       <c r="AC146" s="22" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="AD146" s="22"/>
       <c r="AE146" s="22" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="AF146" s="22"/>
       <c r="AG146" s="22"/>
@@ -27446,32 +27446,32 @@
       <c r="P147" s="37"/>
       <c r="Q147" s="37"/>
       <c r="R147" s="37" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="S147" s="22"/>
       <c r="T147" s="22"/>
       <c r="U147" s="22" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="V147" s="22"/>
       <c r="W147" s="37" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="X147" s="22"/>
       <c r="Y147" s="37" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="Z147" s="22"/>
       <c r="AA147" s="39" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="AB147" s="22"/>
       <c r="AC147" s="22" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="AD147" s="22"/>
       <c r="AE147" s="22" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="AF147" s="22"/>
       <c r="AG147" s="22"/>
@@ -27514,32 +27514,32 @@
       <c r="P148" s="37"/>
       <c r="Q148" s="37"/>
       <c r="R148" s="37" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="S148" s="22"/>
       <c r="T148" s="22"/>
       <c r="U148" s="22" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="V148" s="22"/>
       <c r="W148" s="37" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="X148" s="22"/>
       <c r="Y148" s="37" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="Z148" s="22"/>
       <c r="AA148" s="39" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="AB148" s="22"/>
       <c r="AC148" s="22" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="AD148" s="22"/>
       <c r="AE148" s="22" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="AF148" s="22"/>
       <c r="AG148" s="22"/>
@@ -27582,34 +27582,34 @@
       <c r="P149" s="37"/>
       <c r="Q149" s="37"/>
       <c r="R149" s="37" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="S149" s="22"/>
       <c r="T149" s="22" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="U149" s="22" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="V149" s="22"/>
       <c r="W149" s="37" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="X149" s="22"/>
       <c r="Y149" s="37" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="Z149" s="22"/>
       <c r="AA149" s="39" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="AB149" s="22"/>
       <c r="AC149" s="22" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="AD149" s="22"/>
       <c r="AE149" s="22" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="AF149" s="22"/>
       <c r="AG149" s="22"/>
@@ -27652,34 +27652,34 @@
       <c r="P150" s="37"/>
       <c r="Q150" s="37"/>
       <c r="R150" s="37" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="S150" s="22"/>
       <c r="T150" s="22" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="U150" s="22" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="V150" s="22"/>
       <c r="W150" s="37" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="X150" s="22"/>
       <c r="Y150" s="37" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="Z150" s="22"/>
       <c r="AA150" s="39" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="AB150" s="22"/>
       <c r="AC150" s="22" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="AD150" s="22"/>
       <c r="AE150" s="22" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="AF150" s="22"/>
       <c r="AG150" s="22"/>
@@ -27722,34 +27722,34 @@
       <c r="P151" s="37"/>
       <c r="Q151" s="37"/>
       <c r="R151" s="37" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="S151" s="22"/>
       <c r="T151" s="22" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="U151" s="22" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="V151" s="22"/>
       <c r="W151" s="37" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="X151" s="22"/>
       <c r="Y151" s="37" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="Z151" s="22"/>
       <c r="AA151" s="39" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="AB151" s="22"/>
       <c r="AC151" s="22" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="AD151" s="22"/>
       <c r="AE151" s="22" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="AF151" s="22"/>
       <c r="AG151" s="22"/>
@@ -27792,32 +27792,32 @@
       <c r="P152" s="37"/>
       <c r="Q152" s="37"/>
       <c r="R152" s="37" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="S152" s="22"/>
       <c r="T152" s="22"/>
       <c r="U152" s="22" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="V152" s="22"/>
       <c r="W152" s="37" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="X152" s="22"/>
       <c r="Y152" s="37" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="Z152" s="22"/>
       <c r="AA152" s="39" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="AB152" s="22"/>
       <c r="AC152" s="22" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="AD152" s="22"/>
       <c r="AE152" s="22" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="AF152" s="22"/>
       <c r="AG152" s="22"/>
@@ -27860,32 +27860,32 @@
       <c r="P153" s="37"/>
       <c r="Q153" s="37"/>
       <c r="R153" s="37" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="S153" s="22"/>
       <c r="T153" s="22"/>
       <c r="U153" s="22" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="V153" s="22"/>
       <c r="W153" s="37" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="X153" s="22"/>
       <c r="Y153" s="37" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="Z153" s="22"/>
       <c r="AA153" s="39" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="AB153" s="22"/>
       <c r="AC153" s="22" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="AD153" s="22"/>
       <c r="AE153" s="22" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="AF153" s="22"/>
       <c r="AG153" s="22"/>
@@ -27928,32 +27928,32 @@
       <c r="P154" s="37"/>
       <c r="Q154" s="37"/>
       <c r="R154" s="37" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="S154" s="22"/>
       <c r="T154" s="22"/>
       <c r="U154" s="22" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="V154" s="22"/>
       <c r="W154" s="37" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="X154" s="22"/>
       <c r="Y154" s="37" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="Z154" s="22"/>
       <c r="AA154" s="39" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="AB154" s="22"/>
       <c r="AC154" s="22" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="AD154" s="22"/>
       <c r="AE154" s="22" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="AF154" s="22"/>
       <c r="AG154" s="22"/>
@@ -27996,32 +27996,32 @@
       <c r="P155" s="37"/>
       <c r="Q155" s="37"/>
       <c r="R155" s="37" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="S155" s="22"/>
       <c r="T155" s="22"/>
       <c r="U155" s="22" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="V155" s="22"/>
       <c r="W155" s="37" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="X155" s="22"/>
       <c r="Y155" s="37" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="Z155" s="22"/>
       <c r="AA155" s="39" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="AB155" s="22"/>
       <c r="AC155" s="22" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="AD155" s="22"/>
       <c r="AE155" s="22" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="AF155" s="22"/>
       <c r="AG155" s="22"/>
@@ -28064,32 +28064,32 @@
       <c r="P156" s="37"/>
       <c r="Q156" s="37"/>
       <c r="R156" s="37" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="S156" s="22"/>
       <c r="T156" s="22"/>
       <c r="U156" s="22" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="V156" s="22"/>
       <c r="W156" s="37" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="X156" s="22"/>
       <c r="Y156" s="37" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="Z156" s="22"/>
       <c r="AA156" s="39" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="AB156" s="22"/>
       <c r="AC156" s="22" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="AD156" s="22"/>
       <c r="AE156" s="22" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="AF156" s="22"/>
       <c r="AG156" s="22"/>
@@ -28132,32 +28132,32 @@
       <c r="P157" s="37"/>
       <c r="Q157" s="37"/>
       <c r="R157" s="37" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="S157" s="22"/>
       <c r="T157" s="22"/>
       <c r="U157" s="22" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="V157" s="22"/>
       <c r="W157" s="37" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="X157" s="22"/>
       <c r="Y157" s="37" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="Z157" s="22"/>
       <c r="AA157" s="39" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="AB157" s="22"/>
       <c r="AC157" s="22" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="AD157" s="22"/>
       <c r="AE157" s="22" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="AF157" s="22"/>
       <c r="AG157" s="22"/>

</xml_diff>

<commit_message>
re-factored code to abstract the formatting of phrases and font setup from the generate_scorecards() function addressing issue #4
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/analysis/global_scorecards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1333" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3350F65-2C42-4B92-9306-A08CD9977BAF}"/>
+  <xr:revisionPtr revIDLastSave="1334" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E440BEFE-B6B8-49FC-9FE8-598B9B621BEB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4365" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
@@ -7019,6 +7019,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -7027,9 +7030,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -26277,7 +26277,7 @@
       <c r="X131" s="11"/>
       <c r="Y131" s="11"/>
     </row>
-    <row r="132" spans="1:25" ht="75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A132" s="19" t="s">
         <v>150</v>
       </c>
@@ -28121,7 +28121,10 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28180,7 +28183,7 @@
       <c r="F2" s="18" t="s">
         <v>1358</v>
       </c>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="55" t="s">
         <v>2002</v>
       </c>
     </row>
@@ -28203,7 +28206,7 @@
       <c r="F3" s="20" t="s">
         <v>1972</v>
       </c>
-      <c r="G3" s="58" t="str">
+      <c r="G3" s="55" t="str">
         <f>"https://doi.org/INSERT-"&amp;A3&amp;"-DOI-HERE"</f>
         <v>https://doi.org/INSERT-Maiduguri-DOI-HERE</v>
       </c>
@@ -28227,7 +28230,7 @@
       <c r="F4" s="20" t="s">
         <v>1455</v>
       </c>
-      <c r="G4" s="58" t="str">
+      <c r="G4" s="55" t="str">
         <f t="shared" ref="G4:G27" si="0">"https://doi.org/INSERT-"&amp;A4&amp;"-DOI-HERE"</f>
         <v>https://doi.org/INSERT-Mexico City-DOI-HERE</v>
       </c>
@@ -28251,7 +28254,7 @@
       <c r="F5" s="20" t="s">
         <v>1456</v>
       </c>
-      <c r="G5" s="58" t="str">
+      <c r="G5" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Baltimore-DOI-HERE</v>
       </c>
@@ -28275,7 +28278,7 @@
       <c r="F6" s="20" t="s">
         <v>1358</v>
       </c>
-      <c r="G6" s="58" t="str">
+      <c r="G6" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Phoenix-DOI-HERE</v>
       </c>
@@ -28299,7 +28302,7 @@
       <c r="F7" s="20" t="s">
         <v>1967</v>
       </c>
-      <c r="G7" s="58" t="str">
+      <c r="G7" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Seattle-DOI-HERE</v>
       </c>
@@ -28326,7 +28329,7 @@
       <c r="F8" s="20" t="s">
         <v>1976</v>
       </c>
-      <c r="G8" s="58" t="str">
+      <c r="G8" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Sao Paulo-DOI-HERE</v>
       </c>
@@ -28350,7 +28353,7 @@
       <c r="F9" s="20" t="s">
         <v>1909</v>
       </c>
-      <c r="G9" s="58" t="str">
+      <c r="G9" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Hong Kong-DOI-HERE</v>
       </c>
@@ -28374,7 +28377,7 @@
       <c r="F10" s="20" t="s">
         <v>1358</v>
       </c>
-      <c r="G10" s="58" t="str">
+      <c r="G10" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Chennai-DOI-HERE</v>
       </c>
@@ -28398,7 +28401,7 @@
       <c r="F11" s="20" t="s">
         <v>1457</v>
       </c>
-      <c r="G11" s="58" t="str">
+      <c r="G11" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Bangkok-DOI-HERE</v>
       </c>
@@ -28422,7 +28425,7 @@
       <c r="F12" s="20" t="s">
         <v>1594</v>
       </c>
-      <c r="G12" s="58" t="str">
+      <c r="G12" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Hanoi-DOI-HERE</v>
       </c>
@@ -28446,7 +28449,7 @@
       <c r="F13" s="20" t="s">
         <v>1358</v>
       </c>
-      <c r="G13" s="58" t="str">
+      <c r="G13" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Graz-DOI-HERE</v>
       </c>
@@ -28470,7 +28473,7 @@
       <c r="F14" s="20" t="s">
         <v>1890</v>
       </c>
-      <c r="G14" s="58" t="str">
+      <c r="G14" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Ghent-DOI-HERE</v>
       </c>
@@ -28494,7 +28497,7 @@
       <c r="F15" s="20" t="s">
         <v>1358</v>
       </c>
-      <c r="G15" s="58" t="str">
+      <c r="G15" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Bern-DOI-HERE</v>
       </c>
@@ -28518,7 +28521,7 @@
       <c r="F16" s="20" t="s">
         <v>1854</v>
       </c>
-      <c r="G16" s="58" t="str">
+      <c r="G16" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Olomouc-DOI-HERE</v>
       </c>
@@ -28540,7 +28543,7 @@
       <c r="F17" s="20" t="s">
         <v>1358</v>
       </c>
-      <c r="G17" s="58" t="str">
+      <c r="G17" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Cologne-DOI-HERE</v>
       </c>
@@ -28564,7 +28567,7 @@
       <c r="F18" s="37" t="s">
         <v>1852</v>
       </c>
-      <c r="G18" s="58" t="str">
+      <c r="G18" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Odense-DOI-HERE</v>
       </c>
@@ -28588,7 +28591,7 @@
       <c r="F19" s="20" t="s">
         <v>1446</v>
       </c>
-      <c r="G19" s="58" t="str">
+      <c r="G19" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Barcelona-DOI-HERE</v>
       </c>
@@ -28612,7 +28615,7 @@
       <c r="F20" s="20" t="s">
         <v>1454</v>
       </c>
-      <c r="G20" s="58" t="str">
+      <c r="G20" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Valencia-DOI-HERE</v>
       </c>
@@ -28636,7 +28639,7 @@
       <c r="F21" s="20" t="s">
         <v>1883</v>
       </c>
-      <c r="G21" s="58" t="str">
+      <c r="G21" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Vic-DOI-HERE</v>
       </c>
@@ -28660,7 +28663,7 @@
       <c r="F22" s="20" t="s">
         <v>1449</v>
       </c>
-      <c r="G22" s="58" t="str">
+      <c r="G22" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Belfast-DOI-HERE</v>
       </c>
@@ -28684,7 +28687,7 @@
       <c r="F23" s="20" t="s">
         <v>1874</v>
       </c>
-      <c r="G23" s="58" t="str">
+      <c r="G23" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Lisbon-DOI-HERE</v>
       </c>
@@ -28700,7 +28703,7 @@
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="38"/>
-      <c r="G24" s="58" t="str">
+      <c r="G24" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Adelaide-DOI-HERE</v>
       </c>
@@ -28724,7 +28727,7 @@
       <c r="F25" s="20" t="s">
         <v>1591</v>
       </c>
-      <c r="G25" s="58" t="str">
+      <c r="G25" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Melbourne-DOI-HERE</v>
       </c>
@@ -28748,7 +28751,7 @@
       <c r="F26" s="20" t="s">
         <v>1858</v>
       </c>
-      <c r="G26" s="58" t="str">
+      <c r="G26" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Sydney-DOI-HERE</v>
       </c>
@@ -28772,7 +28775,7 @@
       <c r="F27" s="20" t="s">
         <v>1876</v>
       </c>
-      <c r="G27" s="58" t="str">
+      <c r="G27" s="55" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Auckland-DOI-HERE</v>
       </c>
@@ -29242,30 +29245,30 @@
       <c r="C2" s="39" t="s">
         <v>1015</v>
       </c>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="56" t="s">
         <v>1016</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="56" t="s">
         <v>1615</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="58" t="s">
         <v>1017</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="58"/>
       <c r="V2" s="30" t="s">
         <v>1018</v>
       </c>
@@ -29274,8 +29277,8 @@
       <c r="A3" s="31"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
       <c r="F3" s="32" t="s">
         <v>1019</v>
       </c>

</xml_diff>

<commit_message>
implemented city-specific prose exceptions, addressing issue #3
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/analysis/global_scorecards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1334" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E440BEFE-B6B8-49FC-9FE8-598B9B621BEB}"/>
+  <xr:revisionPtr revIDLastSave="1347" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22C2F0E7-CB45-4C07-BA63-AE473B2B6005}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4365" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
@@ -6107,9 +6107,6 @@
     <t>exceptions_json</t>
   </si>
   <si>
-    <t>{'English':{'series_intro'='This brief report outlines how the Seattle metropolitan area performs on a selection of spatial and policy indicators of healthy and sustainable cities. Our collaborative study examined the spatial distribution of urban design and transport features and the presence and quality of city planning policies that promote health and sustainability for 25 cities across 19 countries. Further details of the study are available at {study_doi}'}}</t>
-  </si>
-  <si>
     <t>credit_image1</t>
   </si>
   <si>
@@ -6123,6 +6120,9 @@
   </si>
   <si>
     <t>https://doi.org/INSERT-STUDY-DOI-HERE</t>
+  </si>
+  <si>
+    <t>{"English":"{'series_intro':'This brief report outlines how the Seattle metropolitan area performs on a selection of spatial and policy indicators of healthy and sustainable cities. Our collaborative study examined the spatial distribution of urban design and transport features and the presence and quality of city planning policies that promote health and sustainability for 25 cities across 19 countries. Further details of the study are available at {study_doi}'}"}</t>
   </si>
 </sst>
 </file>
@@ -8218,7 +8218,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -14989,7 +14989,7 @@
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="B125">
         <v>3</v>
@@ -26285,67 +26285,67 @@
         <v>899</v>
       </c>
       <c r="C132" s="12" t="s">
+        <v>1999</v>
+      </c>
+      <c r="D132" s="12" t="s">
+        <v>1999</v>
+      </c>
+      <c r="E132" s="12" t="s">
+        <v>1999</v>
+      </c>
+      <c r="F132" s="12" t="s">
+        <v>1999</v>
+      </c>
+      <c r="G132" s="12" t="s">
+        <v>1999</v>
+      </c>
+      <c r="H132" s="12" t="s">
         <v>2000</v>
       </c>
-      <c r="D132" s="12" t="s">
-        <v>2000</v>
-      </c>
-      <c r="E132" s="12" t="s">
-        <v>2000</v>
-      </c>
-      <c r="F132" s="12" t="s">
-        <v>2000</v>
-      </c>
-      <c r="G132" s="12" t="s">
-        <v>2000</v>
-      </c>
-      <c r="H132" s="12" t="s">
-        <v>2001</v>
-      </c>
       <c r="I132" s="12" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="J132" s="12" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="K132" s="12" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="L132" s="12" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="M132" s="12" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="N132" s="12" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="O132" s="12" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="P132" s="12" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="Q132" s="12" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="R132" s="12" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="S132" s="12" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="T132" s="12" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="U132" s="12" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="V132" s="12" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="W132" s="12" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="X132" s="11"/>
       <c r="Y132" s="11"/>
@@ -28121,10 +28121,10 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28149,13 +28149,13 @@
         <v>1440</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>1441</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="G1" s="18" t="s">
         <v>1995</v>
@@ -28184,7 +28184,7 @@
         <v>1358</v>
       </c>
       <c r="G2" s="55" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -28307,7 +28307,7 @@
         <v>https://doi.org/INSERT-Seattle-DOI-HERE</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>1997</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated Chinese and Thai translations
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/analysis/global_scorecards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1992" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B93DC9A-D0FB-4C4A-98C9-F7060DE9EAE8}"/>
+  <xr:revisionPtr revIDLastSave="1996" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F349153F-A0C8-4129-ACE9-843FC6FDC138}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4121" uniqueCount="1991">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4121" uniqueCount="1992">
   <si>
     <t>name</t>
   </si>
@@ -4990,10 +4990,6 @@
 （按國家收入）</t>
   </si>
   <si>
-    <t>针对具体、可衡量的政策
-，及作为健康城市所具备的条 件的效能评级</t>
-  </si>
-  <si>
     <t>500米范围內可搭乘平日班次平均为二十分钟或更频
  密的公共交通的人口百分比</t>
   </si>
@@ -5213,12 +5209,6 @@
   </si>
   <si>
     <t>人口數據</t>
-  </si>
-  <si>
-    <t>在全球25個城市中，⾹港就⼈⼝健康和可持續發展相關⽅⾯⽽制定的市區和運輸政策的整體表現平均。現有的政策在具體性、可衡量性和符合健康要素等⽅⾯則⾼於平均指標。然⽽，⾹港在都市市區或運輸政策中幾乎沒有以健康為重點的具體措施，對⼈⼝健康的影響亦未被納⼊制定市區和交通規劃政策所須要評估的範圍內。雖然現有政策已確⽴不同的標準，但當中許多缺乏素質可衡量的⽬標。儘管如此，和這項全球性研究中的25個城市相⽐，⾹港絕⼤多數社區都⾮常適合步⾏。就為達到世界衛⽣組織所訂⽴有關增加⾝體活動的⽬標⽽設定的閾值⽽⾔，⾹港近乎100%的⼈⼝都居住在密度達到閾值的社區，⽽92%的⼈⼝居住在街道連接性亦達到閾值的社區。但我們不能忽視，這當中有部分居⺠居住在密度和街道連接性超過可以促進⾝體活動的⽔平的社區。分析結果同時顯⽰，絕⼤多數居⺠(83.6%)可以⽅便使⽤提供定期服務的公共交通站。此外，雖然近90%的居⺠可以使⽤500⽶範圍內的一些公共開放空間，但責際上只有54%的居⺠居住在⼤型公共開放空間的500⽶範圍內。最後，與研究中的其他城市相⽐，⽐例較多的⾹港居⺠可以在500⽶範圍內使⽤所有⽣活服務設施。</t>
-  </si>
-  <si>
-    <t>在全球25个城市中，⾹港就⼈⼝健康和可持续发展相关⽅⾯⽽制定的市区和交通运输政策的整体表现平均。现有的政策在具体性、可衡量性和符合健康要素等⽅⾯则⾼于平均指标。然⽽，⾹港在都市市区或交通运输政策中几乎没有以健康为重点的具体措施，对⼈⼝健康的影响亦未被纳⼊制定市区和交通规划政策所须要评估的范围内。虽然现有政策已确⽴不同的标准，但当中许多缺乏质素可衡量的⽬标。尽管如此，和这项全球性研究中的25个城市相⽐，⾹港绝⼤多数社区都⾮常适合步⾏。就为达到世界卫 ⽣组织所制定有关增加⾝体活动的⽬标⽽设定的阈值⽽⾔，⾹港近乎100%的⼈⼝都居住在密度达到阈值的社区，⽽92%的⼈⼝居住在街道连接性亦达到阈值的社区。但我们不能忽视，这当中有部分居⺠居住在密度和街道连接性超过可以促进⾝体活动的⽔平的社区。分析结果同时显⽰，绝⼤多数居⺠(83.6%)可以⽅便使⽤提供定期服务的公共交通站。此外，虽然近90%的居⺠可以使⽤500⽶范围内的一些公共开放空间，但实际上只有54%的居⺠居住在⼤型公共开放空间的500⽶范围内。最后，与研究中的其他城市相⽐，⽐例较多的⾹港居⺠可以在500⽶范围内使⽤所有⽣活服务设施。</t>
   </si>
   <si>
     <t>{}</t>
@@ -6099,6 +6089,18 @@
   </si>
   <si>
     <t>vi</t>
+  </si>
+  <si>
+    <t>在全球25個城市中，⾹港就⼈⼝健康和可持續發展相關⽅⾯⽽制定的市區和運輸政策的整體表現平均。現有的政策在具體性、可衡量性和符合健康要素等⽅⾯則⾼於平均指標。然⽽，⾹港在都市市區或運輸政策中幾乎沒有以健康為重點的具體措施，對⼈⼝健康的影響亦未被納⼊制定市區和交通規劃政策所須要評估的範圍內。雖然現有政策已確⽴不同的標準，但當中許多缺乏素質可衡量的⽬標。儘管如此，和這項全球性研究中的25個城市相⽐，⾹港絕⼤多數社區都⾮常適合步⾏。就為達到世界衛⽣組織所訂⽴有關增加⾝體活動的⽬標⽽設定的閾值⽽⾔，⾹港近乎100%的⼈⼝都居住在密度達到閾值的社區，⽽92%的⼈⼝居住在街道連接性亦達到閾值的社區。但我們不能忽視，這當中有部分居⺠居住在密度和街道連接性超過可以促進⾝體活動的⽔平的社區。分析結果同時顯⽰，絕⼤多數居⺠(83.6%)可以⽅便使⽤提供定期服務的公共交通站。此外，雖然近90%的居⺠可以使⽤500⽶範圍內的一些公共開放空間，但實際上只有54%的居⺠居住在⼤型公共開放空間的500⽶範圍內。最後，與研究中的其他城市相⽐，⽐例較多的⾹港居⺠可以在500⽶範圍內使⽤所有⽣活服務設施。</t>
+  </si>
+  <si>
+    <t>针对具体、可衡量的政策，及作为健康城市所具备的条 件的效能评级</t>
+  </si>
+  <si>
+    <t>在全球25个城市中，⾹港就⼈⼝健康和可持续发展相关⽅⾯⽽制定的市区和交通运输政策的整体表现平均。现有的政策在具体性、可衡量性和符合健康要素等⽅⾯则⾼于平均指标。然⽽，⾹港在都市市区或交通运输政策中几乎没有以健康为重点的具体措施，对⼈⼝健康的影响亦未被纳⼊制定市区和交通规划政策所须要评估的范围内。虽然现有政策已确⽴不同的标准，但当中许多缺乏质素可衡量的⽬标。尽管如此，和这项全球性研究中的25个城市相⽐，⾹港绝⼤多数社区都⾮常适合步⾏。就为达到世界卫⽣组织所制定有关增加⾝体活动的⽬标⽽设定的阈值⽽⾔，⾹港近乎100%的⼈⼝都居住在密度达到阈值的社区，⽽92%的⼈⼝居住在街道连接性亦达到阈值的社区。但我们不能忽视，这当中有部分居⺠居住在密度和街道连接性超过可以促进⾝体活动的⽔平的社区。分析结果同时显⽰，绝⼤多数居⺠(83.6%)可以⽅便使⽤提供定期服务的公共交通站。此外，虽然近90%的居⺠可以使⽤500⽶范围内的一些公共开放空间，但实际上只有54%的居⺠居住在⼤型公共开放空间的500⽶范围内。最后，与研究中的其他城市相⽐，⽐例较多的⾹港居⺠可以在500⽶范围内使⽤所有⽣活服务设施。</t>
+  </si>
+  <si>
+    <t>{city} {country}</t>
   </si>
 </sst>
 </file>
@@ -7512,7 +7514,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H62" sqref="H62"/>
+      <selection pane="bottomLeft" activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8179,7 +8181,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -14951,7 +14953,7 @@
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="B125">
         <v>3</v>
@@ -18368,7 +18370,7 @@
     </row>
     <row r="183" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="B183">
         <v>5</v>
@@ -18424,7 +18426,7 @@
     </row>
     <row r="184" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="B184">
         <v>5</v>
@@ -18468,7 +18470,7 @@
         <v>213</v>
       </c>
       <c r="P184" s="1" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="Q184">
         <v>2</v>
@@ -18706,7 +18708,7 @@
     </row>
     <row r="189" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>1726</v>
+        <v>1723</v>
       </c>
       <c r="B189">
         <v>5</v>
@@ -19117,10 +19119,10 @@
   <dimension ref="A1:W170"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="S83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="T88" sqref="T88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19219,10 +19221,10 @@
         <v>864</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>1701</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>1702</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>1703</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>510</v>
@@ -19234,7 +19236,7 @@
         <v>509</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="K2" s="9"/>
       <c r="L2" s="9" t="s">
@@ -19257,7 +19259,7 @@
         <v>360</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>1768</v>
+        <v>1765</v>
       </c>
       <c r="T2" s="9" t="s">
         <v>361</v>
@@ -19273,64 +19275,64 @@
         <v>150</v>
       </c>
       <c r="B3" s="19" t="s">
+        <v>1979</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>1841</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>1974</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>1975</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>1976</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>1977</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>1978</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>1980</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>1953</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>1981</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>1981</v>
+      </c>
+      <c r="M3" s="9" t="s">
         <v>1982</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>1844</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>1977</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>1978</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>1979</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>1980</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>1981</v>
-      </c>
-      <c r="I3" s="9" t="s">
+      <c r="N3" s="9" t="s">
+        <v>1982</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>1983</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>1956</v>
-      </c>
-      <c r="K3" s="9" t="s">
+      <c r="P3" s="9" t="s">
+        <v>1983</v>
+      </c>
+      <c r="Q3" s="9" t="s">
         <v>1984</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="R3" s="9" t="s">
         <v>1984</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="S3" s="9" t="s">
         <v>1985</v>
       </c>
-      <c r="N3" s="9" t="s">
-        <v>1985</v>
-      </c>
-      <c r="O3" s="9" t="s">
+      <c r="T3" s="9" t="s">
         <v>1986</v>
       </c>
-      <c r="P3" s="9" t="s">
-        <v>1986</v>
-      </c>
-      <c r="Q3" s="9" t="s">
+      <c r="U3" s="9" t="s">
         <v>1987</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>1987</v>
-      </c>
-      <c r="S3" s="9" t="s">
-        <v>1988</v>
-      </c>
-      <c r="T3" s="9" t="s">
-        <v>1989</v>
-      </c>
-      <c r="U3" s="9" t="s">
-        <v>1990</v>
       </c>
       <c r="V3" s="9"/>
       <c r="W3" s="9"/>
@@ -19387,7 +19389,7 @@
         <v>492</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>1769</v>
+        <v>1766</v>
       </c>
       <c r="T4" s="11" t="s">
         <v>707</v>
@@ -19427,7 +19429,7 @@
         <v>1241</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="K5" s="22"/>
       <c r="L5" s="22" t="s">
@@ -19450,7 +19452,7 @@
         <v>494</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>1770</v>
+        <v>1767</v>
       </c>
       <c r="T5" s="11" t="s">
         <v>865</v>
@@ -21313,7 +21315,7 @@
         <v>1620</v>
       </c>
       <c r="T57" s="12" t="s">
-        <v>1621</v>
+        <v>1991</v>
       </c>
       <c r="U57" s="11" t="s">
         <v>1622</v>
@@ -21341,7 +21343,7 @@
         <v>1625</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>1752</v>
+        <v>1749</v>
       </c>
       <c r="H58" s="12" t="s">
         <v>1624</v>
@@ -21452,60 +21454,60 @@
         <v>151</v>
       </c>
       <c r="B60" s="19" t="s">
+        <v>1638</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>1638</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>1638</v>
+      </c>
+      <c r="E60" s="12" t="s">
         <v>1639</v>
       </c>
-      <c r="C60" s="12" t="s">
+      <c r="F60" s="12" t="s">
         <v>1639</v>
       </c>
-      <c r="D60" s="12" t="s">
-        <v>1639</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>1640</v>
-      </c>
-      <c r="F60" s="12" t="s">
-        <v>1640</v>
-      </c>
       <c r="G60" s="12" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="J60" s="11" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="K60" s="22"/>
       <c r="L60" s="12" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="M60" s="22"/>
       <c r="N60" s="12" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="O60" s="12" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="P60" s="12" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="Q60" s="12" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="R60" s="12" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="S60" s="11" t="s">
+        <v>1640</v>
+      </c>
+      <c r="T60" s="12" t="s">
         <v>1641</v>
       </c>
-      <c r="T60" s="12" t="s">
-        <v>1642</v>
-      </c>
       <c r="U60" s="11" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="V60" s="11"/>
       <c r="W60" s="11"/>
@@ -21590,7 +21592,7 @@
         <v>1025</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>1375</v>
@@ -21659,13 +21661,13 @@
         <v>1376</v>
       </c>
       <c r="H63" s="9" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="I63" s="22" t="s">
         <v>514</v>
       </c>
       <c r="J63" s="9" t="s">
-        <v>1750</v>
+        <v>1747</v>
       </c>
       <c r="K63" s="22"/>
       <c r="L63" s="22" t="s">
@@ -21688,7 +21690,7 @@
         <v>292</v>
       </c>
       <c r="S63" s="9" t="s">
-        <v>1771</v>
+        <v>1768</v>
       </c>
       <c r="T63" s="9" t="s">
         <v>331</v>
@@ -21751,7 +21753,7 @@
         <v>293</v>
       </c>
       <c r="S64" s="9" t="s">
-        <v>1772</v>
+        <v>1769</v>
       </c>
       <c r="T64" s="9" t="s">
         <v>868</v>
@@ -21854,7 +21856,7 @@
         <v>1246</v>
       </c>
       <c r="J66" s="9" t="s">
-        <v>1767</v>
+        <v>1764</v>
       </c>
       <c r="K66" s="22"/>
       <c r="L66" s="22" t="s">
@@ -22003,7 +22005,7 @@
         <v>315</v>
       </c>
       <c r="S68" s="9" t="s">
-        <v>1773</v>
+        <v>1770</v>
       </c>
       <c r="T68" s="9" t="s">
         <v>871</v>
@@ -22022,7 +22024,7 @@
         <v>161</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="D69" s="9" t="s">
         <v>801</v>
@@ -22043,7 +22045,7 @@
         <v>1247</v>
       </c>
       <c r="J69" s="9" t="s">
-        <v>1748</v>
+        <v>1745</v>
       </c>
       <c r="K69" s="22"/>
       <c r="L69" s="22" t="s">
@@ -22066,7 +22068,7 @@
         <v>1136</v>
       </c>
       <c r="S69" s="9" t="s">
-        <v>1774</v>
+        <v>1771</v>
       </c>
       <c r="T69" s="9" t="s">
         <v>872</v>
@@ -22318,7 +22320,7 @@
         <v>495</v>
       </c>
       <c r="S73" s="9" t="s">
-        <v>1775</v>
+        <v>1772</v>
       </c>
       <c r="T73" s="9" t="s">
         <v>874</v>
@@ -22346,7 +22348,7 @@
         <v>1634</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="G74" s="10" t="s">
         <v>1387</v>
@@ -22358,7 +22360,7 @@
         <v>1249</v>
       </c>
       <c r="J74" s="9" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="K74" s="22"/>
       <c r="L74" s="22" t="s">
@@ -22381,7 +22383,7 @@
         <v>1594</v>
       </c>
       <c r="S74" s="9" t="s">
-        <v>1776</v>
+        <v>1773</v>
       </c>
       <c r="T74" s="9" t="s">
         <v>875</v>
@@ -22421,7 +22423,7 @@
         <v>1250</v>
       </c>
       <c r="J75" s="9" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="K75" s="22"/>
       <c r="L75" s="22" t="s">
@@ -22444,7 +22446,7 @@
         <v>1595</v>
       </c>
       <c r="S75" s="9" t="s">
-        <v>1777</v>
+        <v>1774</v>
       </c>
       <c r="T75" s="9" t="s">
         <v>876</v>
@@ -22463,57 +22465,57 @@
         <v>605</v>
       </c>
       <c r="C76" s="10" t="s">
+        <v>1862</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>1863</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>1857</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>1858</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>1864</v>
+      </c>
+      <c r="H76" s="9" t="s">
+        <v>1889</v>
+      </c>
+      <c r="I76" s="22" t="s">
         <v>1865</v>
       </c>
-      <c r="D76" s="9" t="s">
+      <c r="J76" s="9" t="s">
         <v>1866</v>
-      </c>
-      <c r="E76" s="9" t="s">
-        <v>1860</v>
-      </c>
-      <c r="F76" s="9" t="s">
-        <v>1861</v>
-      </c>
-      <c r="G76" s="10" t="s">
-        <v>1867</v>
-      </c>
-      <c r="H76" s="9" t="s">
-        <v>1892</v>
-      </c>
-      <c r="I76" s="22" t="s">
-        <v>1868</v>
-      </c>
-      <c r="J76" s="9" t="s">
-        <v>1869</v>
       </c>
       <c r="K76" s="22"/>
       <c r="L76" s="22" t="s">
-        <v>1870</v>
+        <v>1867</v>
       </c>
       <c r="M76" s="22"/>
       <c r="N76" s="22" t="s">
+        <v>1868</v>
+      </c>
+      <c r="O76" s="9" t="s">
+        <v>1869</v>
+      </c>
+      <c r="P76" s="11" t="s">
+        <v>1870</v>
+      </c>
+      <c r="Q76" s="9" t="s">
         <v>1871</v>
       </c>
-      <c r="O76" s="9" t="s">
+      <c r="R76" s="9" t="s">
         <v>1872</v>
       </c>
-      <c r="P76" s="11" t="s">
+      <c r="S76" s="9" t="s">
         <v>1873</v>
       </c>
-      <c r="Q76" s="9" t="s">
+      <c r="T76" s="9" t="s">
         <v>1874</v>
       </c>
-      <c r="R76" s="9" t="s">
+      <c r="U76" s="9" t="s">
         <v>1875</v>
-      </c>
-      <c r="S76" s="9" t="s">
-        <v>1876</v>
-      </c>
-      <c r="T76" s="9" t="s">
-        <v>1877</v>
-      </c>
-      <c r="U76" s="9" t="s">
-        <v>1878</v>
       </c>
       <c r="V76" s="9"/>
       <c r="W76" s="9"/>
@@ -22526,57 +22528,57 @@
         <v>606</v>
       </c>
       <c r="C77" s="10" t="s">
+        <v>1876</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>1877</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>1859</v>
+      </c>
+      <c r="F77" s="9" t="s">
+        <v>1860</v>
+      </c>
+      <c r="G77" s="10" t="s">
+        <v>1878</v>
+      </c>
+      <c r="H77" s="9" t="s">
+        <v>1861</v>
+      </c>
+      <c r="I77" s="22" t="s">
         <v>1879</v>
       </c>
-      <c r="D77" s="9" t="s">
+      <c r="J77" s="9" t="s">
         <v>1880</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>1862</v>
-      </c>
-      <c r="F77" s="9" t="s">
-        <v>1863</v>
-      </c>
-      <c r="G77" s="10" t="s">
-        <v>1881</v>
-      </c>
-      <c r="H77" s="9" t="s">
-        <v>1864</v>
-      </c>
-      <c r="I77" s="22" t="s">
-        <v>1882</v>
-      </c>
-      <c r="J77" s="9" t="s">
-        <v>1883</v>
       </c>
       <c r="K77" s="22"/>
       <c r="L77" s="22" t="s">
-        <v>1884</v>
+        <v>1881</v>
       </c>
       <c r="M77" s="22"/>
       <c r="N77" s="22" t="s">
+        <v>1882</v>
+      </c>
+      <c r="O77" s="9" t="s">
+        <v>1883</v>
+      </c>
+      <c r="P77" s="11" t="s">
+        <v>1884</v>
+      </c>
+      <c r="Q77" s="9" t="s">
         <v>1885</v>
       </c>
-      <c r="O77" s="9" t="s">
+      <c r="R77" s="9" t="s">
         <v>1886</v>
       </c>
-      <c r="P77" s="11" t="s">
+      <c r="S77" s="9" t="s">
         <v>1887</v>
       </c>
-      <c r="Q77" s="9" t="s">
+      <c r="T77" s="9" t="s">
         <v>1888</v>
       </c>
-      <c r="R77" s="9" t="s">
-        <v>1889</v>
-      </c>
-      <c r="S77" s="9" t="s">
+      <c r="U77" s="9" t="s">
         <v>1890</v>
-      </c>
-      <c r="T77" s="9" t="s">
-        <v>1891</v>
-      </c>
-      <c r="U77" s="9" t="s">
-        <v>1893</v>
       </c>
       <c r="V77" s="9"/>
       <c r="W77" s="9"/>
@@ -22589,57 +22591,57 @@
         <v>604</v>
       </c>
       <c r="C78" s="10" t="s">
+        <v>1842</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>1843</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>1844</v>
+      </c>
+      <c r="F78" s="9" t="s">
         <v>1845</v>
       </c>
-      <c r="D78" s="9" t="s">
+      <c r="G78" s="10" t="s">
         <v>1846</v>
       </c>
-      <c r="E78" s="9" t="s">
+      <c r="H78" s="9" t="s">
+        <v>1891</v>
+      </c>
+      <c r="I78" s="22" t="s">
         <v>1847</v>
       </c>
-      <c r="F78" s="9" t="s">
-        <v>1848</v>
-      </c>
-      <c r="G78" s="10" t="s">
-        <v>1849</v>
-      </c>
-      <c r="H78" s="9" t="s">
-        <v>1894</v>
-      </c>
-      <c r="I78" s="22" t="s">
-        <v>1850</v>
-      </c>
       <c r="J78" s="9" t="s">
-        <v>1895</v>
+        <v>1892</v>
       </c>
       <c r="K78" s="22"/>
       <c r="L78" s="22" t="s">
-        <v>1851</v>
+        <v>1848</v>
       </c>
       <c r="M78" s="22"/>
       <c r="N78" s="22" t="s">
+        <v>1849</v>
+      </c>
+      <c r="O78" s="9" t="s">
+        <v>1850</v>
+      </c>
+      <c r="P78" s="9" t="s">
+        <v>1851</v>
+      </c>
+      <c r="Q78" s="9" t="s">
         <v>1852</v>
       </c>
-      <c r="O78" s="9" t="s">
+      <c r="R78" s="9" t="s">
         <v>1853</v>
       </c>
-      <c r="P78" s="9" t="s">
+      <c r="S78" s="9" t="s">
         <v>1854</v>
       </c>
-      <c r="Q78" s="9" t="s">
+      <c r="T78" s="9" t="s">
         <v>1855</v>
       </c>
-      <c r="R78" s="9" t="s">
+      <c r="U78" s="9" t="s">
         <v>1856</v>
-      </c>
-      <c r="S78" s="9" t="s">
-        <v>1857</v>
-      </c>
-      <c r="T78" s="9" t="s">
-        <v>1858</v>
-      </c>
-      <c r="U78" s="9" t="s">
-        <v>1859</v>
       </c>
       <c r="V78" s="9"/>
       <c r="W78" s="9"/>
@@ -22696,7 +22698,7 @@
         <v>275</v>
       </c>
       <c r="S79" s="9" t="s">
-        <v>1778</v>
+        <v>1775</v>
       </c>
       <c r="T79" s="9" t="s">
         <v>335</v>
@@ -22715,10 +22717,10 @@
         <v>171</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>1759</v>
+        <v>1756</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>1760</v>
+        <v>1757</v>
       </c>
       <c r="E80" s="9" t="s">
         <v>1040</v>
@@ -22727,45 +22729,45 @@
         <v>1041</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>1761</v>
+        <v>1758</v>
       </c>
       <c r="H80" s="9" t="s">
-        <v>1762</v>
+        <v>1759</v>
       </c>
       <c r="I80" s="22" t="s">
         <v>1252</v>
       </c>
       <c r="J80" s="9" t="s">
-        <v>1766</v>
+        <v>1763</v>
       </c>
       <c r="K80" s="22"/>
       <c r="L80" s="22" t="s">
-        <v>1763</v>
+        <v>1760</v>
       </c>
       <c r="M80" s="22"/>
       <c r="N80" s="22" t="s">
+        <v>1752</v>
+      </c>
+      <c r="O80" s="9" t="s">
+        <v>1753</v>
+      </c>
+      <c r="P80" s="11" t="s">
+        <v>1754</v>
+      </c>
+      <c r="Q80" s="9" t="s">
         <v>1755</v>
       </c>
-      <c r="O80" s="9" t="s">
-        <v>1756</v>
-      </c>
-      <c r="P80" s="11" t="s">
-        <v>1757</v>
-      </c>
-      <c r="Q80" s="9" t="s">
-        <v>1758</v>
-      </c>
       <c r="R80" s="9" t="s">
-        <v>1764</v>
+        <v>1761</v>
       </c>
       <c r="S80" s="9" t="s">
-        <v>1779</v>
+        <v>1776</v>
       </c>
       <c r="T80" s="9" t="s">
-        <v>1837</v>
+        <v>1834</v>
       </c>
       <c r="U80" s="9" t="s">
-        <v>1765</v>
+        <v>1762</v>
       </c>
       <c r="V80" s="9"/>
       <c r="W80" s="9"/>
@@ -22862,7 +22864,7 @@
         <v>1253</v>
       </c>
       <c r="J82" s="9" t="s">
-        <v>1738</v>
+        <v>1735</v>
       </c>
       <c r="K82" s="22"/>
       <c r="L82" s="22" t="s">
@@ -22885,7 +22887,7 @@
         <v>1596</v>
       </c>
       <c r="S82" s="9" t="s">
-        <v>1780</v>
+        <v>1777</v>
       </c>
       <c r="T82" s="9" t="s">
         <v>879</v>
@@ -22925,7 +22927,7 @@
         <v>1254</v>
       </c>
       <c r="J83" s="9" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="K83" s="22"/>
       <c r="L83" s="22" t="s">
@@ -22988,7 +22990,7 @@
         <v>1255</v>
       </c>
       <c r="J84" s="11" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="K84" s="22"/>
       <c r="L84" s="22" t="s">
@@ -23051,7 +23053,7 @@
         <v>1256</v>
       </c>
       <c r="J85" s="11" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="K85" s="22"/>
       <c r="L85" s="22" t="s">
@@ -23156,57 +23158,57 @@
         <v>186</v>
       </c>
       <c r="C87" s="12" t="s">
+        <v>1678</v>
+      </c>
+      <c r="D87" s="11" t="s">
         <v>1679</v>
       </c>
-      <c r="D87" s="11" t="s">
+      <c r="E87" s="11" t="s">
+        <v>1893</v>
+      </c>
+      <c r="F87" s="11" t="s">
+        <v>1704</v>
+      </c>
+      <c r="G87" s="12" t="s">
         <v>1680</v>
       </c>
-      <c r="E87" s="11" t="s">
-        <v>1896</v>
-      </c>
-      <c r="F87" s="11" t="s">
-        <v>1705</v>
-      </c>
-      <c r="G87" s="12" t="s">
+      <c r="H87" s="11" t="s">
         <v>1681</v>
       </c>
-      <c r="H87" s="11" t="s">
+      <c r="I87" s="22" t="s">
         <v>1682</v>
       </c>
-      <c r="I87" s="22" t="s">
-        <v>1683</v>
-      </c>
       <c r="J87" s="11" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="K87" s="22"/>
       <c r="L87" s="22" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="M87" s="22"/>
       <c r="N87" s="22" t="s">
+        <v>1685</v>
+      </c>
+      <c r="O87" s="11" t="s">
+        <v>1894</v>
+      </c>
+      <c r="P87" s="11" t="s">
+        <v>1895</v>
+      </c>
+      <c r="Q87" s="11" t="s">
+        <v>1896</v>
+      </c>
+      <c r="R87" s="11" t="s">
         <v>1686</v>
       </c>
-      <c r="O87" s="11" t="s">
-        <v>1897</v>
-      </c>
-      <c r="P87" s="11" t="s">
-        <v>1898</v>
-      </c>
-      <c r="Q87" s="11" t="s">
-        <v>1899</v>
-      </c>
-      <c r="R87" s="11" t="s">
+      <c r="S87" s="11" t="s">
+        <v>1784</v>
+      </c>
+      <c r="T87" s="11" t="s">
+        <v>1824</v>
+      </c>
+      <c r="U87" s="11" t="s">
         <v>1687</v>
-      </c>
-      <c r="S87" s="11" t="s">
-        <v>1787</v>
-      </c>
-      <c r="T87" s="11" t="s">
-        <v>1827</v>
-      </c>
-      <c r="U87" s="11" t="s">
-        <v>1688</v>
       </c>
       <c r="V87" s="11"/>
       <c r="W87" s="11"/>
@@ -23225,7 +23227,7 @@
         <v>920</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="F88" s="11" t="s">
         <v>1049</v>
@@ -23240,7 +23242,7 @@
         <v>1617</v>
       </c>
       <c r="J88" s="11" t="s">
-        <v>1751</v>
+        <v>1748</v>
       </c>
       <c r="K88" s="22"/>
       <c r="L88" s="22" t="s">
@@ -23263,10 +23265,10 @@
         <v>1597</v>
       </c>
       <c r="S88" s="11" t="s">
-        <v>1781</v>
+        <v>1778</v>
       </c>
       <c r="T88" s="11" t="s">
-        <v>1812</v>
+        <v>1809</v>
       </c>
       <c r="U88" s="11" t="s">
         <v>1352</v>
@@ -23288,10 +23290,10 @@
         <v>607</v>
       </c>
       <c r="E89" s="11" t="s">
+        <v>1642</v>
+      </c>
+      <c r="F89" s="11" t="s">
         <v>1643</v>
-      </c>
-      <c r="F89" s="11" t="s">
-        <v>1644</v>
       </c>
       <c r="G89" s="12" t="s">
         <v>1435</v>
@@ -23314,7 +23316,7 @@
         <v>660</v>
       </c>
       <c r="O89" s="11" t="s">
-        <v>1900</v>
+        <v>1897</v>
       </c>
       <c r="P89" s="11" t="s">
         <v>831</v>
@@ -23326,10 +23328,10 @@
         <v>1598</v>
       </c>
       <c r="S89" s="11" t="s">
-        <v>1782</v>
+        <v>1779</v>
       </c>
       <c r="T89" s="11" t="s">
-        <v>1813</v>
+        <v>1810</v>
       </c>
       <c r="U89" s="11" t="s">
         <v>1312</v>
@@ -23366,7 +23368,7 @@
         <v>1258</v>
       </c>
       <c r="J90" s="11" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="K90" s="22"/>
       <c r="L90" s="22" t="s">
@@ -23389,10 +23391,10 @@
         <v>1139</v>
       </c>
       <c r="S90" s="11" t="s">
-        <v>1783</v>
+        <v>1780</v>
       </c>
       <c r="T90" s="11" t="s">
-        <v>1814</v>
+        <v>1811</v>
       </c>
       <c r="U90" s="11" t="s">
         <v>1313</v>
@@ -23471,28 +23473,28 @@
         <v>246</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>1901</v>
+        <v>1898</v>
       </c>
       <c r="D92" s="11" t="s">
         <v>1371</v>
       </c>
       <c r="E92" s="11" t="s">
+        <v>1706</v>
+      </c>
+      <c r="F92" s="11" t="s">
         <v>1707</v>
-      </c>
-      <c r="F92" s="11" t="s">
-        <v>1708</v>
       </c>
       <c r="G92" s="12" t="s">
         <v>1397</v>
       </c>
       <c r="H92" s="11" t="s">
-        <v>1902</v>
+        <v>1899</v>
       </c>
       <c r="I92" s="22" t="s">
-        <v>1903</v>
+        <v>1900</v>
       </c>
       <c r="J92" s="11" t="s">
-        <v>1904</v>
+        <v>1901</v>
       </c>
       <c r="K92" s="22"/>
       <c r="L92" s="22" t="s">
@@ -23500,28 +23502,28 @@
       </c>
       <c r="M92" s="22"/>
       <c r="N92" s="22" t="s">
-        <v>1905</v>
+        <v>1902</v>
       </c>
       <c r="O92" s="11" t="s">
-        <v>1906</v>
+        <v>1903</v>
       </c>
       <c r="P92" s="11" t="s">
-        <v>1907</v>
+        <v>1904</v>
       </c>
       <c r="Q92" s="11" t="s">
         <v>1181</v>
       </c>
       <c r="R92" s="11" t="s">
-        <v>1908</v>
+        <v>1905</v>
       </c>
       <c r="S92" s="11" t="s">
-        <v>1909</v>
+        <v>1906</v>
       </c>
       <c r="T92" s="11" t="s">
         <v>884</v>
       </c>
       <c r="U92" s="11" t="s">
-        <v>1910</v>
+        <v>1907</v>
       </c>
       <c r="V92" s="11"/>
       <c r="W92" s="11"/>
@@ -23555,7 +23557,7 @@
         <v>526</v>
       </c>
       <c r="J93" s="11" t="s">
-        <v>1739</v>
+        <v>1736</v>
       </c>
       <c r="K93" s="22"/>
       <c r="L93" s="22" t="s">
@@ -23581,7 +23583,7 @@
         <v>534</v>
       </c>
       <c r="T93" s="11" t="s">
-        <v>1815</v>
+        <v>1812</v>
       </c>
       <c r="U93" s="11" t="s">
         <v>1315</v>
@@ -23618,7 +23620,7 @@
         <v>1259</v>
       </c>
       <c r="J94" s="11" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="K94" s="22"/>
       <c r="L94" s="22" t="s">
@@ -23641,7 +23643,7 @@
         <v>1599</v>
       </c>
       <c r="S94" s="11" t="s">
-        <v>1784</v>
+        <v>1781</v>
       </c>
       <c r="T94" s="11" t="s">
         <v>885</v>
@@ -23681,7 +23683,7 @@
         <v>527</v>
       </c>
       <c r="J95" s="11" t="s">
-        <v>1740</v>
+        <v>1737</v>
       </c>
       <c r="K95" s="22"/>
       <c r="L95" s="22" t="s">
@@ -23707,7 +23709,7 @@
         <v>535</v>
       </c>
       <c r="T95" s="11" t="s">
-        <v>1816</v>
+        <v>1813</v>
       </c>
       <c r="U95" s="11" t="s">
         <v>629</v>
@@ -23732,19 +23734,19 @@
         <v>1053</v>
       </c>
       <c r="F96" s="11" t="s">
-        <v>1637</v>
+        <v>1989</v>
       </c>
       <c r="G96" s="12" t="s">
         <v>1399</v>
       </c>
       <c r="H96" s="11" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="I96" s="22" t="s">
         <v>1260</v>
       </c>
       <c r="J96" s="11" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="K96" s="22"/>
       <c r="L96" s="22" t="s">
@@ -23767,7 +23769,7 @@
         <v>1140</v>
       </c>
       <c r="S96" s="11" t="s">
-        <v>1785</v>
+        <v>1782</v>
       </c>
       <c r="T96" s="11" t="s">
         <v>886</v>
@@ -23807,7 +23809,7 @@
         <v>521</v>
       </c>
       <c r="J97" s="11" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="K97" s="22"/>
       <c r="L97" s="22" t="s">
@@ -23849,7 +23851,7 @@
         <v>41</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="D98" s="11" t="s">
         <v>923</v>
@@ -23870,7 +23872,7 @@
         <v>1618</v>
       </c>
       <c r="J98" s="11" t="s">
-        <v>1747</v>
+        <v>1744</v>
       </c>
       <c r="K98" s="22"/>
       <c r="L98" s="22" t="s">
@@ -23893,7 +23895,7 @@
         <v>621</v>
       </c>
       <c r="S98" s="11" t="s">
-        <v>1786</v>
+        <v>1783</v>
       </c>
       <c r="T98" s="11" t="s">
         <v>888</v>
@@ -23933,7 +23935,7 @@
         <v>1289</v>
       </c>
       <c r="J99" s="11" t="s">
-        <v>1954</v>
+        <v>1951</v>
       </c>
       <c r="K99" s="22"/>
       <c r="L99" s="22" t="s">
@@ -23996,7 +23998,7 @@
         <v>1290</v>
       </c>
       <c r="J100" s="11" t="s">
-        <v>1746</v>
+        <v>1743</v>
       </c>
       <c r="K100" s="22"/>
       <c r="L100" s="22" t="s">
@@ -24059,7 +24061,7 @@
         <v>1261</v>
       </c>
       <c r="J101" s="11" t="s">
-        <v>1911</v>
+        <v>1908</v>
       </c>
       <c r="K101" s="22"/>
       <c r="L101" s="22" t="s">
@@ -24085,7 +24087,7 @@
         <v>387</v>
       </c>
       <c r="T101" s="11" t="s">
-        <v>1821</v>
+        <v>1818</v>
       </c>
       <c r="U101" s="11" t="s">
         <v>1319</v>
@@ -24110,7 +24112,7 @@
         <v>1058</v>
       </c>
       <c r="F102" s="11" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="G102" s="12" t="s">
         <v>1405</v>
@@ -24211,7 +24213,7 @@
         <v>389</v>
       </c>
       <c r="T103" s="11" t="s">
-        <v>1822</v>
+        <v>1819</v>
       </c>
       <c r="U103" s="11" t="s">
         <v>1321</v>
@@ -24274,7 +24276,7 @@
         <v>390</v>
       </c>
       <c r="T104" s="11" t="s">
-        <v>1823</v>
+        <v>1820</v>
       </c>
       <c r="U104" s="11" t="s">
         <v>1353</v>
@@ -24311,7 +24313,7 @@
         <v>1265</v>
       </c>
       <c r="J105" s="11" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="K105" s="22"/>
       <c r="L105" s="22" t="s">
@@ -24337,7 +24339,7 @@
         <v>391</v>
       </c>
       <c r="T105" s="11" t="s">
-        <v>1824</v>
+        <v>1821</v>
       </c>
       <c r="U105" s="11" t="s">
         <v>1322</v>
@@ -24374,7 +24376,7 @@
         <v>1266</v>
       </c>
       <c r="J106" s="11" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="K106" s="22"/>
       <c r="L106" s="22" t="s">
@@ -24397,10 +24399,10 @@
         <v>323</v>
       </c>
       <c r="S106" s="11" t="s">
-        <v>1788</v>
+        <v>1785</v>
       </c>
       <c r="T106" s="11" t="s">
-        <v>1825</v>
+        <v>1822</v>
       </c>
       <c r="U106" s="11" t="s">
         <v>1323</v>
@@ -24416,7 +24418,7 @@
         <v>52</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>1912</v>
+        <v>1909</v>
       </c>
       <c r="D107" s="11" t="s">
         <v>927</v>
@@ -24437,7 +24439,7 @@
         <v>1267</v>
       </c>
       <c r="J107" s="14" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="K107" s="22"/>
       <c r="L107" s="22" t="s">
@@ -24460,10 +24462,10 @@
         <v>1600</v>
       </c>
       <c r="S107" s="11" t="s">
-        <v>1789</v>
+        <v>1786</v>
       </c>
       <c r="T107" s="11" t="s">
-        <v>1817</v>
+        <v>1814</v>
       </c>
       <c r="U107" s="11" t="s">
         <v>1324</v>
@@ -24491,7 +24493,7 @@
         <v>1070</v>
       </c>
       <c r="G108" s="12" t="s">
-        <v>1753</v>
+        <v>1750</v>
       </c>
       <c r="H108" s="11" t="s">
         <v>1560</v>
@@ -24500,7 +24502,7 @@
         <v>1268</v>
       </c>
       <c r="J108" s="11" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="K108" s="22"/>
       <c r="L108" s="22" t="s">
@@ -24563,7 +24565,7 @@
         <v>528</v>
       </c>
       <c r="J109" s="11" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="K109" s="22"/>
       <c r="L109" s="22" t="s">
@@ -24626,7 +24628,7 @@
         <v>1269</v>
       </c>
       <c r="J110" s="11" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="K110" s="22"/>
       <c r="L110" s="22" t="s">
@@ -24646,7 +24648,7 @@
         <v>1193</v>
       </c>
       <c r="R110" s="11" t="s">
-        <v>1913</v>
+        <v>1910</v>
       </c>
       <c r="S110" s="11" t="s">
         <v>449</v>
@@ -24712,10 +24714,10 @@
         <v>279</v>
       </c>
       <c r="S111" s="11" t="s">
-        <v>1790</v>
+        <v>1787</v>
       </c>
       <c r="T111" s="11" t="s">
-        <v>1818</v>
+        <v>1815</v>
       </c>
       <c r="U111" s="11" t="s">
         <v>1326</v>
@@ -24872,13 +24874,13 @@
         <v>1412</v>
       </c>
       <c r="H114" s="11" t="s">
-        <v>1736</v>
+        <v>1733</v>
       </c>
       <c r="I114" s="22" t="s">
         <v>1270</v>
       </c>
       <c r="J114" s="11" t="s">
-        <v>1955</v>
+        <v>1952</v>
       </c>
       <c r="K114" s="22"/>
       <c r="L114" s="22" t="s">
@@ -24901,10 +24903,10 @@
         <v>1142</v>
       </c>
       <c r="S114" s="11" t="s">
-        <v>1791</v>
+        <v>1788</v>
       </c>
       <c r="T114" s="11" t="s">
-        <v>1833</v>
+        <v>1830</v>
       </c>
       <c r="U114" s="11" t="s">
         <v>1327</v>
@@ -24941,7 +24943,7 @@
         <v>1271</v>
       </c>
       <c r="J115" s="11" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="K115" s="22"/>
       <c r="L115" s="22" t="s">
@@ -24964,10 +24966,10 @@
         <v>304</v>
       </c>
       <c r="S115" s="11" t="s">
-        <v>1792</v>
+        <v>1789</v>
       </c>
       <c r="T115" s="11" t="s">
-        <v>1819</v>
+        <v>1816</v>
       </c>
       <c r="U115" s="11" t="s">
         <v>1328</v>
@@ -25067,7 +25069,7 @@
         <v>525</v>
       </c>
       <c r="J117" s="11" t="s">
-        <v>1741</v>
+        <v>1738</v>
       </c>
       <c r="K117" s="22"/>
       <c r="L117" s="22" t="s">
@@ -25090,7 +25092,7 @@
         <v>306</v>
       </c>
       <c r="S117" s="11" t="s">
-        <v>1793</v>
+        <v>1790</v>
       </c>
       <c r="T117" s="11" t="s">
         <v>891</v>
@@ -25153,7 +25155,7 @@
         <v>325</v>
       </c>
       <c r="S118" s="11" t="s">
-        <v>1794</v>
+        <v>1791</v>
       </c>
       <c r="T118" s="11" t="s">
         <v>892</v>
@@ -25256,7 +25258,7 @@
         <v>1275</v>
       </c>
       <c r="J120" s="11" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="K120" s="22"/>
       <c r="L120" s="22" t="s">
@@ -25319,7 +25321,7 @@
         <v>1276</v>
       </c>
       <c r="J121" s="11" t="s">
-        <v>1742</v>
+        <v>1739</v>
       </c>
       <c r="K121" s="22"/>
       <c r="L121" s="22" t="s">
@@ -25345,7 +25347,7 @@
         <v>397</v>
       </c>
       <c r="T121" s="11" t="s">
-        <v>1820</v>
+        <v>1817</v>
       </c>
       <c r="U121" s="11" t="s">
         <v>1332</v>
@@ -25382,7 +25384,7 @@
         <v>1277</v>
       </c>
       <c r="J122" s="11" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="K122" s="22"/>
       <c r="L122" s="22" t="s">
@@ -25405,7 +25407,7 @@
         <v>731</v>
       </c>
       <c r="S122" s="11" t="s">
-        <v>1795</v>
+        <v>1792</v>
       </c>
       <c r="T122" s="11" t="s">
         <v>894</v>
@@ -25508,7 +25510,7 @@
         <v>1279</v>
       </c>
       <c r="J124" s="11" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="K124" s="22"/>
       <c r="L124" s="22" t="s">
@@ -25528,10 +25530,10 @@
         <v>1200</v>
       </c>
       <c r="R124" s="11" t="s">
-        <v>1914</v>
+        <v>1911</v>
       </c>
       <c r="S124" s="11" t="s">
-        <v>1796</v>
+        <v>1793</v>
       </c>
       <c r="T124" s="11" t="s">
         <v>896</v>
@@ -25568,10 +25570,10 @@
         <v>1574</v>
       </c>
       <c r="I125" s="22" t="s">
-        <v>1915</v>
+        <v>1912</v>
       </c>
       <c r="J125" s="14" t="s">
-        <v>1745</v>
+        <v>1742</v>
       </c>
       <c r="K125" s="22"/>
       <c r="L125" s="22" t="s">
@@ -25594,13 +25596,13 @@
         <v>1602</v>
       </c>
       <c r="S125" s="11" t="s">
-        <v>1797</v>
+        <v>1794</v>
       </c>
       <c r="T125" s="11" t="s">
-        <v>1826</v>
+        <v>1823</v>
       </c>
       <c r="U125" s="11" t="s">
-        <v>1916</v>
+        <v>1913</v>
       </c>
       <c r="V125" s="11"/>
       <c r="W125" s="11"/>
@@ -25657,10 +25659,10 @@
         <v>622</v>
       </c>
       <c r="S126" s="11" t="s">
-        <v>1798</v>
+        <v>1795</v>
       </c>
       <c r="T126" s="11" t="s">
-        <v>1828</v>
+        <v>1825</v>
       </c>
       <c r="U126" s="11" t="s">
         <v>1335</v>
@@ -25723,7 +25725,7 @@
         <v>398</v>
       </c>
       <c r="T127" s="11" t="s">
-        <v>1829</v>
+        <v>1826</v>
       </c>
       <c r="U127" s="11" t="s">
         <v>1336</v>
@@ -25786,7 +25788,7 @@
         <v>399</v>
       </c>
       <c r="T128" s="11" t="s">
-        <v>1830</v>
+        <v>1827</v>
       </c>
       <c r="U128" s="11" t="s">
         <v>1337</v>
@@ -25849,7 +25851,7 @@
         <v>400</v>
       </c>
       <c r="T129" s="11" t="s">
-        <v>1831</v>
+        <v>1828</v>
       </c>
       <c r="U129" s="11" t="s">
         <v>1338</v>
@@ -25906,13 +25908,13 @@
         <v>1202</v>
       </c>
       <c r="R130" s="11" t="s">
-        <v>1917</v>
+        <v>1914</v>
       </c>
       <c r="S130" s="11" t="s">
-        <v>1799</v>
+        <v>1796</v>
       </c>
       <c r="T130" s="11" t="s">
-        <v>1832</v>
+        <v>1829</v>
       </c>
       <c r="U130" s="11" t="s">
         <v>1356</v>
@@ -25975,7 +25977,7 @@
         <v>401</v>
       </c>
       <c r="T131" s="11" t="s">
-        <v>1834</v>
+        <v>1831</v>
       </c>
       <c r="U131" s="11" t="s">
         <v>1339</v>
@@ -26012,7 +26014,7 @@
         <v>1285</v>
       </c>
       <c r="J132" s="11" t="s">
-        <v>1743</v>
+        <v>1740</v>
       </c>
       <c r="K132" s="22"/>
       <c r="L132" s="22" t="s">
@@ -26060,7 +26062,7 @@
         <v>744</v>
       </c>
       <c r="E133" s="11" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="F133" s="11" t="s">
         <v>1111</v>
@@ -26201,7 +26203,7 @@
         <v>1287</v>
       </c>
       <c r="J135" s="11" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="K135" s="22"/>
       <c r="L135" s="22" t="s">
@@ -26287,7 +26289,7 @@
         <v>770</v>
       </c>
       <c r="S136" s="11" t="s">
-        <v>1800</v>
+        <v>1797</v>
       </c>
       <c r="T136" s="11" t="s">
         <v>775</v>
@@ -26545,7 +26547,7 @@
         <v>902</v>
       </c>
       <c r="U140" s="11" t="s">
-        <v>1918</v>
+        <v>1915</v>
       </c>
       <c r="V140" s="11"/>
       <c r="W140" s="11"/>
@@ -26559,7 +26561,7 @@
         <v>Maiduguri - Summary</v>
       </c>
       <c r="C141" s="12" t="s">
-        <v>1942</v>
+        <v>1939</v>
       </c>
       <c r="D141" s="11"/>
       <c r="E141" s="11"/>
@@ -26595,7 +26597,7 @@
         <v>Mexico City - Summary</v>
       </c>
       <c r="C142" s="12" t="s">
-        <v>1919</v>
+        <v>1916</v>
       </c>
       <c r="D142" s="11"/>
       <c r="E142" s="11"/>
@@ -26609,7 +26611,7 @@
       <c r="M142" s="22"/>
       <c r="N142" s="22"/>
       <c r="O142" s="11" t="s">
-        <v>1920</v>
+        <v>1917</v>
       </c>
       <c r="P142" s="11"/>
       <c r="Q142" s="11"/>
@@ -26631,7 +26633,7 @@
         <v>Baltimore - Summary</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>1943</v>
+        <v>1940</v>
       </c>
       <c r="D143" s="11"/>
       <c r="E143" s="11"/>
@@ -26665,7 +26667,7 @@
         <v>Phoenix - Summary</v>
       </c>
       <c r="C144" s="12" t="s">
-        <v>1921</v>
+        <v>1918</v>
       </c>
       <c r="D144" s="11"/>
       <c r="E144" s="11"/>
@@ -26699,7 +26701,7 @@
         <v>Seattle - Summary</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>1922</v>
+        <v>1919</v>
       </c>
       <c r="D145" s="11"/>
       <c r="E145" s="11"/>
@@ -26733,7 +26735,7 @@
         <v>Sao Paulo - Summary</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>1923</v>
+        <v>1920</v>
       </c>
       <c r="D146" s="11"/>
       <c r="E146" s="11"/>
@@ -26769,14 +26771,14 @@
         <v>Hong Kong - Summary</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>1924</v>
+        <v>1921</v>
       </c>
       <c r="D147" s="11"/>
       <c r="E147" s="11" t="s">
-        <v>1711</v>
+        <v>1988</v>
       </c>
       <c r="F147" s="11" t="s">
-        <v>1712</v>
+        <v>1990</v>
       </c>
       <c r="G147" s="12"/>
       <c r="H147" s="11"/>
@@ -26807,7 +26809,7 @@
         <v>Chennai - Summary</v>
       </c>
       <c r="C148" s="12" t="s">
-        <v>1925</v>
+        <v>1922</v>
       </c>
       <c r="D148" s="11"/>
       <c r="E148" s="11"/>
@@ -26827,7 +26829,7 @@
         <v>1135</v>
       </c>
       <c r="S148" s="11" t="s">
-        <v>1926</v>
+        <v>1923</v>
       </c>
       <c r="T148" s="11"/>
       <c r="U148" s="11"/>
@@ -26843,7 +26845,7 @@
         <v>Bangkok - Summary</v>
       </c>
       <c r="C149" s="12" t="s">
-        <v>1944</v>
+        <v>1941</v>
       </c>
       <c r="D149" s="11"/>
       <c r="E149" s="11"/>
@@ -26864,7 +26866,7 @@
       </c>
       <c r="S149" s="11"/>
       <c r="T149" s="11" t="s">
-        <v>1836</v>
+        <v>1833</v>
       </c>
       <c r="U149" s="11"/>
       <c r="V149" s="11"/>
@@ -26879,7 +26881,7 @@
         <v>Hanoi - Summary</v>
       </c>
       <c r="C150" s="12" t="s">
-        <v>1927</v>
+        <v>1924</v>
       </c>
       <c r="D150" s="11"/>
       <c r="E150" s="11"/>
@@ -26901,7 +26903,7 @@
       <c r="S150" s="11"/>
       <c r="T150" s="11"/>
       <c r="U150" s="11" t="s">
-        <v>1928</v>
+        <v>1925</v>
       </c>
       <c r="V150" s="11"/>
       <c r="W150" s="11"/>
@@ -26915,7 +26917,7 @@
         <v>Graz - Summary</v>
       </c>
       <c r="C151" s="12" t="s">
-        <v>1929</v>
+        <v>1926</v>
       </c>
       <c r="D151" s="11"/>
       <c r="E151" s="11"/>
@@ -26924,7 +26926,7 @@
       <c r="H151" s="11"/>
       <c r="I151" s="22"/>
       <c r="J151" s="11" t="s">
-        <v>1930</v>
+        <v>1927</v>
       </c>
       <c r="K151" s="22"/>
       <c r="L151" s="22"/>
@@ -26951,7 +26953,7 @@
         <v>Ghent - Summary</v>
       </c>
       <c r="C152" s="12" t="s">
-        <v>1931</v>
+        <v>1928</v>
       </c>
       <c r="D152" s="11"/>
       <c r="E152" s="11"/>
@@ -26959,7 +26961,7 @@
       <c r="G152" s="12"/>
       <c r="H152" s="11"/>
       <c r="I152" s="22" t="s">
-        <v>1932</v>
+        <v>1929</v>
       </c>
       <c r="J152" s="11"/>
       <c r="K152" s="22"/>
@@ -26987,7 +26989,7 @@
         <v>Bern - Summary</v>
       </c>
       <c r="C153" s="12" t="s">
-        <v>1933</v>
+        <v>1930</v>
       </c>
       <c r="D153" s="11"/>
       <c r="E153" s="11"/>
@@ -26996,7 +26998,7 @@
       <c r="H153" s="11"/>
       <c r="I153" s="22"/>
       <c r="J153" s="11" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="K153" s="22"/>
       <c r="L153" s="22"/>
@@ -27023,7 +27025,7 @@
         <v>Olomouc - Summary</v>
       </c>
       <c r="C154" s="12" t="s">
-        <v>1934</v>
+        <v>1931</v>
       </c>
       <c r="D154" s="11"/>
       <c r="E154" s="11"/>
@@ -27059,7 +27061,7 @@
         <v>Cologne - Summary</v>
       </c>
       <c r="C155" s="12" t="s">
-        <v>1935</v>
+        <v>1932</v>
       </c>
       <c r="D155" s="11"/>
       <c r="E155" s="11"/>
@@ -27068,7 +27070,7 @@
       <c r="H155" s="11"/>
       <c r="I155" s="22"/>
       <c r="J155" s="11" t="s">
-        <v>1744</v>
+        <v>1741</v>
       </c>
       <c r="K155" s="22"/>
       <c r="L155" s="22"/>
@@ -27095,7 +27097,7 @@
         <v>Odense - Summary</v>
       </c>
       <c r="C156" s="12" t="s">
-        <v>1945</v>
+        <v>1942</v>
       </c>
       <c r="D156" s="11"/>
       <c r="E156" s="11"/>
@@ -27131,10 +27133,10 @@
         <v>Barcelona - Summary</v>
       </c>
       <c r="C157" s="12" t="s">
-        <v>1946</v>
+        <v>1943</v>
       </c>
       <c r="D157" s="11" t="s">
-        <v>1936</v>
+        <v>1933</v>
       </c>
       <c r="E157" s="11"/>
       <c r="F157" s="11"/>
@@ -27169,10 +27171,10 @@
         <v>Valencia - Summary</v>
       </c>
       <c r="C158" s="12" t="s">
-        <v>1937</v>
+        <v>1934</v>
       </c>
       <c r="D158" s="11" t="s">
-        <v>1938</v>
+        <v>1935</v>
       </c>
       <c r="E158" s="11"/>
       <c r="F158" s="11"/>
@@ -27207,10 +27209,10 @@
         <v>Vic - Summary</v>
       </c>
       <c r="C159" s="12" t="s">
-        <v>1947</v>
+        <v>1944</v>
       </c>
       <c r="D159" s="11" t="s">
-        <v>1939</v>
+        <v>1936</v>
       </c>
       <c r="E159" s="11"/>
       <c r="F159" s="11"/>
@@ -27245,7 +27247,7 @@
         <v>Belfast - Summary</v>
       </c>
       <c r="C160" s="12" t="s">
-        <v>1948</v>
+        <v>1945</v>
       </c>
       <c r="D160" s="11"/>
       <c r="E160" s="11"/>
@@ -27279,7 +27281,7 @@
         <v>Lisbon - Summary</v>
       </c>
       <c r="C161" s="12" t="s">
-        <v>1949</v>
+        <v>1946</v>
       </c>
       <c r="D161" s="11"/>
       <c r="E161" s="11"/>
@@ -27296,7 +27298,7 @@
       <c r="P161" s="11"/>
       <c r="Q161" s="11"/>
       <c r="R161" s="11" t="s">
-        <v>1950</v>
+        <v>1947</v>
       </c>
       <c r="S161" s="11"/>
       <c r="T161" s="11"/>
@@ -27313,7 +27315,7 @@
         <v>Adelaide - Summary</v>
       </c>
       <c r="C162" s="12" t="s">
-        <v>1951</v>
+        <v>1948</v>
       </c>
       <c r="D162" s="11"/>
       <c r="E162" s="11"/>
@@ -27347,7 +27349,7 @@
         <v>Melbourne - Summary</v>
       </c>
       <c r="C163" s="12" t="s">
-        <v>1940</v>
+        <v>1937</v>
       </c>
       <c r="D163" s="11"/>
       <c r="E163" s="11"/>
@@ -27381,7 +27383,7 @@
         <v>Sydney - Summary</v>
       </c>
       <c r="C164" s="12" t="s">
-        <v>1941</v>
+        <v>1938</v>
       </c>
       <c r="D164" s="11"/>
       <c r="E164" s="11"/>
@@ -27415,7 +27417,7 @@
         <v>Auckland - Summary</v>
       </c>
       <c r="C165" s="15" t="s">
-        <v>1952</v>
+        <v>1949</v>
       </c>
       <c r="E165" s="11"/>
       <c r="F165" s="11"/>
@@ -27427,7 +27429,7 @@
       <c r="L165" s="22"/>
       <c r="M165" s="22"/>
       <c r="N165" s="22" t="s">
-        <v>1953</v>
+        <v>1950</v>
       </c>
       <c r="O165" s="11"/>
       <c r="P165" s="11"/>
@@ -27452,10 +27454,10 @@
         <v>1160</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>1729</v>
+        <v>1726</v>
       </c>
       <c r="F166" s="2" t="s">
-        <v>1730</v>
+        <v>1727</v>
       </c>
       <c r="G166" s="2" t="s">
         <v>1441</v>
@@ -27467,7 +27469,7 @@
         <v>1291</v>
       </c>
       <c r="J166" s="2" t="s">
-        <v>1749</v>
+        <v>1746</v>
       </c>
       <c r="K166" s="2" t="s">
         <v>919</v>
@@ -27488,7 +27490,7 @@
         <v>917</v>
       </c>
       <c r="T166" s="2" t="s">
-        <v>1835</v>
+        <v>1832</v>
       </c>
       <c r="U166" s="2" t="s">
         <v>1341</v>
@@ -27499,13 +27501,13 @@
         <v>150</v>
       </c>
       <c r="B167" s="19" t="s">
-        <v>1726</v>
+        <v>1723</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>1727</v>
+        <v>1724</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>1728</v>
+        <v>1725</v>
       </c>
       <c r="H167" s="3"/>
     </row>
@@ -27532,7 +27534,7 @@
         <v>970</v>
       </c>
       <c r="H168" s="3" t="s">
-        <v>1737</v>
+        <v>1734</v>
       </c>
       <c r="I168" s="3" t="s">
         <v>969</v>
@@ -27573,58 +27575,58 @@
         <v>150</v>
       </c>
       <c r="B169" s="19" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="E169" s="3" t="s">
+        <v>1712</v>
+      </c>
+      <c r="F169" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="G169" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="H169" s="3" t="s">
         <v>1715</v>
       </c>
-      <c r="F169" s="3" t="s">
+      <c r="I169" s="3" t="s">
+        <v>1698</v>
+      </c>
+      <c r="J169" s="3" t="s">
+        <v>1718</v>
+      </c>
+      <c r="L169" s="3" t="s">
         <v>1716</v>
       </c>
-      <c r="G169" s="3" t="s">
+      <c r="N169" s="3" t="s">
         <v>1717</v>
       </c>
-      <c r="H169" s="3" t="s">
-        <v>1718</v>
-      </c>
-      <c r="I169" s="3" t="s">
-        <v>1699</v>
-      </c>
-      <c r="J169" s="3" t="s">
+      <c r="O169" s="3" t="s">
+        <v>1719</v>
+      </c>
+      <c r="P169" s="3" t="s">
+        <v>1719</v>
+      </c>
+      <c r="Q169" s="3" t="s">
+        <v>1719</v>
+      </c>
+      <c r="R169" s="3" t="s">
+        <v>1719</v>
+      </c>
+      <c r="S169" s="3" t="s">
+        <v>1720</v>
+      </c>
+      <c r="T169" s="3" t="s">
         <v>1721</v>
       </c>
-      <c r="L169" s="3" t="s">
-        <v>1719</v>
-      </c>
-      <c r="N169" s="3" t="s">
-        <v>1720</v>
-      </c>
-      <c r="O169" s="3" t="s">
+      <c r="U169" s="3" t="s">
         <v>1722</v>
-      </c>
-      <c r="P169" s="3" t="s">
-        <v>1722</v>
-      </c>
-      <c r="Q169" s="3" t="s">
-        <v>1722</v>
-      </c>
-      <c r="R169" s="3" t="s">
-        <v>1722</v>
-      </c>
-      <c r="S169" s="3" t="s">
-        <v>1723</v>
-      </c>
-      <c r="T169" s="3" t="s">
-        <v>1724</v>
-      </c>
-      <c r="U169" s="3" t="s">
-        <v>1725</v>
       </c>
     </row>
     <row r="170" spans="1:23" x14ac:dyDescent="0.25">
@@ -27641,10 +27643,10 @@
         <v>1150</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>1805</v>
+        <v>1802</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>1804</v>
+        <v>1801</v>
       </c>
       <c r="G170" s="3" t="s">
         <v>1151</v>
@@ -27742,7 +27744,7 @@
         <v>844</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>1957</v>
+        <v>1954</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>1206</v>
@@ -27751,24 +27753,24 @@
         <v>1208</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>1209</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="H1" s="18" t="s">
+        <v>1689</v>
+      </c>
+      <c r="I1" s="30" t="s">
         <v>1690</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>1691</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="18" t="s">
@@ -27787,10 +27789,10 @@
         <v>1135</v>
       </c>
       <c r="H2" s="49" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -27798,29 +27800,29 @@
         <v>191</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1958</v>
+        <v>1955</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>1365</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>1735</v>
+        <v>1732</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>1735</v>
+        <v>1732</v>
       </c>
       <c r="H3" s="49" t="str">
         <f>"https://doi.org/INSERT-"&amp;A3&amp;"-DOI-HERE"</f>
         <v>https://doi.org/INSERT-Maiduguri-DOI-HERE</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -27828,7 +27830,7 @@
         <v>185</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1959</v>
+        <v>1956</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>915</v>
@@ -27850,7 +27852,7 @@
         <v>https://doi.org/INSERT-Mexico City-DOI-HERE</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -27858,7 +27860,7 @@
         <v>192</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1960</v>
+        <v>1957</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1146</v>
@@ -27880,7 +27882,7 @@
         <v>https://doi.org/INSERT-Baltimore-DOI-HERE</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -27888,7 +27890,7 @@
         <v>193</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1960</v>
+        <v>1957</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>1145</v>
@@ -27910,7 +27912,7 @@
         <v>https://doi.org/INSERT-Phoenix-DOI-HERE</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -27918,29 +27920,29 @@
         <v>194</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>1960</v>
+        <v>1957</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="F7" s="20" t="s">
         <v>1616</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="H7" s="49" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Seattle-DOI-HERE</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -27948,7 +27950,7 @@
         <v>195</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1961</v>
+        <v>1958</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>905</v>
@@ -27957,20 +27959,20 @@
         <v>1210</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>1608</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="H8" s="49" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Sao Paulo-DOI-HERE</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -27978,7 +27980,7 @@
         <v>196</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1962</v>
+        <v>1959</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>1632</v>
@@ -28000,7 +28002,7 @@
         <v>https://doi.org/INSERT-Hong Kong-DOI-HERE</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>1714</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -28008,7 +28010,7 @@
         <v>197</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1963</v>
+        <v>1960</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>914</v>
@@ -28030,7 +28032,7 @@
         <v>https://doi.org/INSERT-Chennai-DOI-HERE</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -28038,7 +28040,7 @@
         <v>184</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1964</v>
+        <v>1961</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>903</v>
@@ -28060,7 +28062,7 @@
         <v>https://doi.org/INSERT-Bangkok-DOI-HERE</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -28068,7 +28070,7 @@
         <v>198</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>1965</v>
+        <v>1962</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1361</v>
@@ -28090,7 +28092,7 @@
         <v>https://doi.org/INSERT-Hanoi-DOI-HERE</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -28098,7 +28100,7 @@
         <v>199</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>1966</v>
+        <v>1963</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>908</v>
@@ -28120,7 +28122,7 @@
         <v>https://doi.org/INSERT-Graz-DOI-HERE</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -28128,7 +28130,7 @@
         <v>200</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1967</v>
+        <v>1964</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>911</v>
@@ -28137,20 +28139,20 @@
         <v>1345</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>1733</v>
+        <v>1730</v>
       </c>
       <c r="F14" s="20" t="s">
         <v>1344</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>1734</v>
+        <v>1731</v>
       </c>
       <c r="H14" s="49" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Ghent-DOI-HERE</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -28158,7 +28160,7 @@
         <v>201</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>1968</v>
+        <v>1965</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>910</v>
@@ -28180,7 +28182,7 @@
         <v>https://doi.org/INSERT-Bern-DOI-HERE</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -28188,10 +28190,10 @@
         <v>202</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>1969</v>
+        <v>1966</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>1754</v>
+        <v>1751</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>1591</v>
@@ -28210,7 +28212,7 @@
         <v>https://doi.org/INSERT-Olomouc-DOI-HERE</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -28218,7 +28220,7 @@
         <v>203</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>1970</v>
+        <v>1967</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>909</v>
@@ -28238,7 +28240,7 @@
         <v>https://doi.org/INSERT-Cologne-DOI-HERE</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -28246,7 +28248,7 @@
         <v>204</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>1971</v>
+        <v>1968</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>912</v>
@@ -28255,20 +28257,20 @@
         <v>1588</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>1732</v>
+        <v>1729</v>
       </c>
       <c r="F18" s="31" t="s">
         <v>1587</v>
       </c>
       <c r="G18" s="31" t="s">
-        <v>1731</v>
+        <v>1728</v>
       </c>
       <c r="H18" s="49" t="str">
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Odense-DOI-HERE</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -28276,7 +28278,7 @@
         <v>205</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>1972</v>
+        <v>1969</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>1148</v>
@@ -28298,7 +28300,7 @@
         <v>https://doi.org/INSERT-Barcelona-DOI-HERE</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -28306,7 +28308,7 @@
         <v>206</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>1972</v>
+        <v>1969</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>1147</v>
@@ -28328,7 +28330,7 @@
         <v>https://doi.org/INSERT-Valencia-DOI-HERE</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -28336,7 +28338,7 @@
         <v>207</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>1972</v>
+        <v>1969</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>1148</v>
@@ -28358,7 +28360,7 @@
         <v>https://doi.org/INSERT-Vic-DOI-HERE</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -28366,7 +28368,7 @@
         <v>208</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>1973</v>
+        <v>1970</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>913</v>
@@ -28388,7 +28390,7 @@
         <v>https://doi.org/INSERT-Belfast-DOI-HERE</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -28396,7 +28398,7 @@
         <v>209</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>1974</v>
+        <v>1971</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>918</v>
@@ -28418,7 +28420,7 @@
         <v>https://doi.org/INSERT-Lisbon-DOI-HERE</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -28426,7 +28428,7 @@
         <v>210</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>1975</v>
+        <v>1972</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>906</v>
@@ -28440,7 +28442,7 @@
         <v>https://doi.org/INSERT-Adelaide-DOI-HERE</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -28448,7 +28450,7 @@
         <v>182</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>1975</v>
+        <v>1972</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>906</v>
@@ -28470,7 +28472,7 @@
         <v>https://doi.org/INSERT-Melbourne-DOI-HERE</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -28478,7 +28480,7 @@
         <v>211</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>1975</v>
+        <v>1972</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>906</v>
@@ -28500,7 +28502,7 @@
         <v>https://doi.org/INSERT-Sydney-DOI-HERE</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -28508,7 +28510,7 @@
         <v>212</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>1976</v>
+        <v>1973</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>907</v>
@@ -28530,7 +28532,7 @@
         <v>https://doi.org/INSERT-Auckland-DOI-HERE</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
     </row>
   </sheetData>
@@ -28591,7 +28593,7 @@
         <v>598</v>
       </c>
       <c r="F2" s="50" t="s">
-        <v>1802</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -28611,7 +28613,7 @@
         <v>145</v>
       </c>
       <c r="F3" s="50" t="s">
-        <v>1802</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -28631,7 +28633,7 @@
         <v>146</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>1802</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -28651,7 +28653,7 @@
         <v>147</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>1802</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -28668,7 +28670,7 @@
         <v>1129</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>1801</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -28688,7 +28690,7 @@
         <v>1129</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>1801</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -28708,7 +28710,7 @@
         <v>1129</v>
       </c>
       <c r="F8" s="50" t="s">
-        <v>1801</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -28728,7 +28730,7 @@
         <v>1129</v>
       </c>
       <c r="F9" s="50" t="s">
-        <v>1801</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -28816,13 +28818,13 @@
         <v>175</v>
       </c>
       <c r="C14" t="s">
-        <v>1806</v>
+        <v>1803</v>
       </c>
       <c r="E14" t="s">
-        <v>1808</v>
+        <v>1805</v>
       </c>
       <c r="F14" t="s">
-        <v>1807</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -28833,16 +28835,16 @@
         <v>175</v>
       </c>
       <c r="C15" t="s">
-        <v>1806</v>
+        <v>1803</v>
       </c>
       <c r="D15" t="s">
         <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>1809</v>
+        <v>1806</v>
       </c>
       <c r="F15" t="s">
-        <v>1807</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -28853,16 +28855,16 @@
         <v>175</v>
       </c>
       <c r="C16" t="s">
-        <v>1806</v>
+        <v>1803</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>1810</v>
+        <v>1807</v>
       </c>
       <c r="F16" t="s">
-        <v>1807</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -28873,16 +28875,16 @@
         <v>175</v>
       </c>
       <c r="C17" t="s">
-        <v>1806</v>
+        <v>1803</v>
       </c>
       <c r="D17" t="s">
         <v>144</v>
       </c>
       <c r="E17" t="s">
-        <v>1811</v>
+        <v>1808</v>
       </c>
       <c r="F17" t="s">
-        <v>1807</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -28893,13 +28895,13 @@
         <v>175</v>
       </c>
       <c r="C18" t="s">
-        <v>1839</v>
+        <v>1836</v>
       </c>
       <c r="E18" t="s">
-        <v>1838</v>
+        <v>1835</v>
       </c>
       <c r="F18" t="s">
-        <v>1843</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -28910,16 +28912,16 @@
         <v>175</v>
       </c>
       <c r="C19" t="s">
-        <v>1839</v>
+        <v>1836</v>
       </c>
       <c r="D19" t="s">
         <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>1840</v>
+        <v>1837</v>
       </c>
       <c r="F19" t="s">
-        <v>1803</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -28930,16 +28932,16 @@
         <v>175</v>
       </c>
       <c r="C20" t="s">
-        <v>1839</v>
+        <v>1836</v>
       </c>
       <c r="D20" t="s">
         <v>25</v>
       </c>
       <c r="E20" t="s">
-        <v>1841</v>
+        <v>1838</v>
       </c>
       <c r="F20" t="s">
-        <v>1803</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -28950,16 +28952,16 @@
         <v>175</v>
       </c>
       <c r="C21" t="s">
-        <v>1839</v>
+        <v>1836</v>
       </c>
       <c r="D21" t="s">
         <v>144</v>
       </c>
       <c r="E21" t="s">
-        <v>1842</v>
+        <v>1839</v>
       </c>
       <c r="F21" t="s">
-        <v>1803</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated custom contact information for Belfast
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/analysis/global_scorecards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2124" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89068B3E-D86A-4D0C-963C-104B7F64D207}"/>
+  <xr:revisionPtr revIDLastSave="2130" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF274732-A797-416B-B8BF-A7D8B2893F4B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4136" uniqueCount="1996">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4120" uniqueCount="1997">
   <si>
     <t>name</t>
   </si>
@@ -6111,6 +6111,9 @@
   </si>
   <si>
     <t>partial</t>
+  </si>
+  <si>
+    <t>{"English":"{'local_collaborators_names':'Claire Cleland, Sara Ferguson &amp; Ruth Hunter||For further information, please contact ruth.hunter@qub.ac.uk'}"}</t>
   </si>
 </sst>
 </file>
@@ -7000,6 +7003,12 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -7008,12 +7017,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -19140,11 +19143,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W170"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22920,7 +22923,7 @@
       <c r="V82" s="9"/>
       <c r="W82" s="9"/>
     </row>
-    <row r="83" spans="1:23" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="19" t="s">
         <v>151</v>
       </c>
@@ -24243,7 +24246,7 @@
       <c r="V103" s="11"/>
       <c r="W103" s="11"/>
     </row>
-    <row r="104" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="19" t="s">
         <v>150</v>
       </c>
@@ -24432,7 +24435,7 @@
       <c r="V106" s="11"/>
       <c r="W106" s="11"/>
     </row>
-    <row r="107" spans="1:23" ht="225" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:23" ht="210" x14ac:dyDescent="0.25">
       <c r="A107" s="19" t="s">
         <v>150</v>
       </c>
@@ -27743,10 +27746,10 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27920,13 +27923,13 @@
       <c r="D6" s="20" t="s">
         <v>1985</v>
       </c>
-      <c r="E6" s="55" t="s">
+      <c r="E6" s="52" t="s">
         <v>1984</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>1986</v>
       </c>
-      <c r="G6" s="55" t="s">
+      <c r="G6" s="52" t="s">
         <v>1984</v>
       </c>
       <c r="H6" s="49" t="str">
@@ -28411,8 +28414,8 @@
         <f t="shared" si="0"/>
         <v>https://doi.org/INSERT-Belfast-DOI-HERE</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>1699</v>
+      <c r="I22" s="3" t="s">
+        <v>1996</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -28567,7 +28570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -29026,30 +29029,30 @@
       <c r="C2" s="33" t="s">
         <v>844</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="54" t="s">
         <v>845</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="54" t="s">
         <v>1363</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="56" t="s">
         <v>846</v>
       </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
       <c r="V2" s="24" t="s">
         <v>847</v>
       </c>
@@ -29058,8 +29061,8 @@
       <c r="A3" s="25"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
       <c r="F3" s="26" t="s">
         <v>848</v>
       </c>
@@ -29790,11 +29793,11 @@
       <c r="A14" s="41" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="56" t="str">
+      <c r="B14" s="53" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A14,city_details!A:A,0))</f>
         <v>candidates sent, none chosen</v>
       </c>
-      <c r="C14" s="56" t="str">
+      <c r="C14" s="53" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A14,city_details!A:A,0))</f>
         <v>candidates sent, none chosen</v>
       </c>
@@ -29924,11 +29927,11 @@
       <c r="A16" s="41" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="56" t="str">
+      <c r="B16" s="53" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A16,city_details!A:A,0))</f>
         <v>candidates sent, none chosen</v>
       </c>
-      <c r="C16" s="56" t="str">
+      <c r="C16" s="53" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A16,city_details!A:A,0))</f>
         <v>candidates sent, none chosen</v>
       </c>
@@ -30062,11 +30065,11 @@
       <c r="A18" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="B18" s="56" t="str">
+      <c r="B18" s="53" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A18,city_details!A:A,0))</f>
         <v>candidates sent, none chosen</v>
       </c>
-      <c r="C18" s="56" t="str">
+      <c r="C18" s="53" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A18,city_details!A:A,0))</f>
         <v>candidates sent, none chosen</v>
       </c>
@@ -30266,11 +30269,11 @@
       <c r="A21" s="41" t="s">
         <v>206</v>
       </c>
-      <c r="B21" s="56" t="str">
+      <c r="B21" s="53" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A21,city_details!A:A,0))</f>
         <v>To be updated on sunny day</v>
       </c>
-      <c r="C21" s="56" t="str">
+      <c r="C21" s="53" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A21,city_details!A:A,0))</f>
         <v>To be updated on sunny day</v>
       </c>

</xml_diff>

<commit_message>
updated code to allow for localisation of percentage sign spacing, addressing issue #10
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/analysis/global_scorecards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2324" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C88C8720-0630-4F36-B642-8D3BA62579D8}"/>
+  <xr:revisionPtr revIDLastSave="2325" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FB95881-A91C-498A-BD7D-C7833DDE6783}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
@@ -5474,154 +5474,13 @@
     <t>en</t>
   </si>
   <si>
-    <t>(above) {}% of population live in neighbourhoods with walkability scores greater than the 25 international city median</t>
-  </si>
-  <si>
-    <t>(a dalt) {}% de població que viu en barris amb puntuacions de caminabilitat superiors a la mediana de les 25 ciutats internacionals</t>
-  </si>
-  <si>
-    <t>(上圖) {}%的人口居住在比25個城市可步行性中位數高的社區</t>
-  </si>
-  <si>
-    <t>(上图) {}%的人口居住在比25个城市可步行性中位数高的社区</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(výše) {}% obyvatel žije v oblastech s vyšší úrovní podmínek pro chůzi (walkability), než je medián 25 srovnávaných měst. </t>
-  </si>
-  <si>
-    <t>(boven) {}% van de bevolking woont in buurten met bewegingsvriendelijkheidsscores die groter zijn dan de mediaan van de 25 internationale steden</t>
-  </si>
-  <si>
-    <t>(a sama) {}% na yawan jama'a suna rayuwa ne a unguwannin da ke da maki mai iya tafiya fiye da 25 na duniya na tsakiya</t>
-  </si>
-  <si>
-    <t>(i runga) {}% o te iwi whānui e noho ana i ngā rohe me ngā tapeke hīkoi nui ake i te taone ao whānui e 25</t>
-  </si>
-  <si>
-    <t>(arriba) {}% de la población vive en colonias con puntuaciones de caminabilidad superiores a la mediana de las 25 ciudades internacionales</t>
-  </si>
-  <si>
-    <t>(arriba) {}% de la población que vive en barrios con puntuaciones de caminabilidad superiores a la mediana de las 25 ciudades internacionales</t>
-  </si>
-  <si>
-    <t>(acima) {}% da população que vive em bairros com pontuação de caminhabilidade maior que a mediana de 25 cidades internacionais</t>
-  </si>
-  <si>
-    <t>(acima) {}% da população residente em bairros com pontuações de caminhabilidade superiores às 25 medianas da cidade internacional</t>
-  </si>
-  <si>
-    <t>(மேலே) {}% மக்கள் 25 சர்வதேச நகர சராசரியை விட அதிகமான நடைத்திறன் மதிப்பெண்களுடன் சுற்றுப்புறங்களில் வாழ்கின்றனர்</t>
-  </si>
-  <si>
     <t>(บน) ร้อยละ{}ของประชากรที่อาศัยอยู่ในย่านที่มีคะแนนความสามารถในการเดินมากกว่าค่าเฉลี่ยของ 25 เมืองในระดับสากล</t>
   </si>
   <si>
-    <t>(trên) {}% dân số sống trong các khu dân cư có điểm số khả năng đi bộ lớn hơn mức trung bình của 25 thành phố quốc tế</t>
-  </si>
-  <si>
-    <t>(上圖) {}%的人口符合鄰里人口密度的最小閾值</t>
-  </si>
-  <si>
-    <t>(上图) {}%的人口符合邻里人口密度的最小阈值</t>
-  </si>
-  <si>
-    <t>(上圖) {}%的人口符合鄰里街道交匯處密度的最小閾值</t>
-  </si>
-  <si>
-    <t>(上图) {}%的人口符合邻里街道交汇处密度的最小阈值</t>
-  </si>
-  <si>
-    <t>(ovenfor) {} % af indbyggere, der opfylder minimumgrænsen* for tætheden af vejkryds i nærområdet ({:}{})</t>
-  </si>
-  <si>
-    <t>(above) {}% of population meet minimum threshold* for neighbourhood population density ({} people {})</t>
-  </si>
-  <si>
-    <t>(a dalt) {}% de població que compleix el llindar mínim* de densitat de població a nivell de barri ({} {})</t>
-  </si>
-  <si>
-    <t>(výše) {}% obyvatel žije v oblasti, která dosahuje mezní hodnoty* hustoty zalidnění({} obyv. {})</t>
-  </si>
-  <si>
-    <t>(boven) {}% van de bevolking voldoet aan minimumdrempel* voor buurtgerelateerde bevolkingsdichtheid ({} {})</t>
-  </si>
-  <si>
-    <t>(oben) {}% der Bevölkerung erreichen die Mindestschwelle* für die Bevölkerungsdichte in der Nachbarschaft ({} {})</t>
-  </si>
-  <si>
-    <t>(a sama) {}% na yawan jama'a sun cika mafi ƙarancin ƙima* don yawan yawan jama'ar unguwa ({} {})</t>
-  </si>
-  <si>
-    <t>(i runga) {}% o te iwi whānui e tūtaki ana ki te paepae mōkito* mō te kiato o te iwi whānui paetata ({} {})</t>
-  </si>
-  <si>
-    <t>(arriba) {}% de la población cumple con el umbral mínimo* de densidad de población en la colonia ({} {})</t>
-  </si>
-  <si>
-    <t>(arriba) {}% de la población cumple con el umbral mínimo* de densidad de población a nivel de barrio ({} {})</t>
-  </si>
-  <si>
-    <t>(acima) {}% da população cumpre o limite mínimo* para a densidade populacional da vizinhança ({} {})</t>
-  </si>
-  <si>
-    <t>(acima) {}% da população cumpre o limiar mínimo* para a densidade populacional do bairro ({} {})</t>
-  </si>
-  <si>
-    <t>(மேலே) {}% மக்கள் தொகை, அக்கம்பக்க மக்கள்தொகை அடர்த்திக்கான குறைந்தபட்ச வரம்பு* ({} {})</t>
-  </si>
-  <si>
     <t xml:space="preserve">(บน) {} ร้อยละของประชากรตรงตามเกณฑ์ขั้นต่ำ* สำหรับย่านที่มีประชากรหนาแน่น ({} {}) </t>
   </si>
   <si>
-    <t>(trên) {}% dân số đáp ứng ngưỡng tối thiểu* đối với mật độ dân số khu dân cư ({} {})</t>
-  </si>
-  <si>
-    <t>(above) {}% of population meet minimum threshold* for neighbourhood street intersection density ({} intersections {})</t>
-  </si>
-  <si>
-    <t>(a dalt) {}% de població que compleix el llindar mínim* de densitat d'interseccions de carrers a nivell de barri ({} {})</t>
-  </si>
-  <si>
-    <t>(výše) {}% obyvatel žije v oblasti, která dosahuje mezní hodnoty* pro hustotu křižovatek ({} křížovatek {})</t>
-  </si>
-  <si>
-    <t>(boven) {}% van de bevolking voldoet aan minimumdrempel* voor de dichtheid van kruispunten in straten in de buurt ({} {})</t>
-  </si>
-  <si>
-    <t>(a sama) {}% na yawan jama'a suna saduwa da mafi ƙanƙanta kofa* don yawan mahadar titin unguwa ({} {})</t>
-  </si>
-  <si>
-    <t>(i runga) {}% o te iwi whānui e tūtaki ana ki te paepae mōkito* mō te kiato o te tiriti paetata ({} {})</t>
-  </si>
-  <si>
-    <t>(arriba) {}% de la población cumple con el umbral mínimo* de densidad de intersección de calles en la colonia ({} {})</t>
-  </si>
-  <si>
-    <t>(arriba) {}% de la población cumple con el umbral mínimo* de densidad de intersecciones de calles a nivel de barrio ({} {})</t>
-  </si>
-  <si>
-    <t>(acima) {}% da população cumpre o limite mínimo* para a densidade de intersecção de ruas da vizinhança ({} {})</t>
-  </si>
-  <si>
-    <t>(acima) {}% da população cumpre o limiar mínimo* para a densidade de intersecção de rua do bairro ({} {})</t>
-  </si>
-  <si>
-    <t>(மேலே) {}% மக்கள் தொகை, அக்கம்பக்க தெரு வெட்டு அடர்த்திக்கான குறைந்தபட்ச வரம்பு* ({} {})</t>
-  </si>
-  <si>
     <t>(บน) {} ร้อยละของประชากรตรงตามเกณฑ์ขั้นต่ำ* สำหรับย่านที่มีทางแยกหนาแน่น ({} {})</t>
-  </si>
-  <si>
-    <t>(ovenfor) % af indbyggere, der opfylder minimumsgrænsen* for befolkningstæthed i nærområdet ({} {})</t>
-  </si>
-  <si>
-    <t>(trên) {}% dân số đáp ứng ngưỡng tối thiểu* đối với mật độ giao lộ đường xá trong khu dân cư ({} {})</t>
-  </si>
-  <si>
-    <t>(ovenfor) {} % af indbyggere, der bor i kvarterer med et walkability indeks, der er større end mediaen for de 25 internationale byer</t>
-  </si>
-  <si>
-    <t>(oben) {}% der Bevölkerung leben in Stadtteilen mit Begehbarkeitswerten, die über dem Median der 25 Städte in 19 Ländern liegen</t>
   </si>
   <si>
     <t>這份報告概述了香港在健康和可持續城市，有關空間和政策的指標的表現。我們的研究 團隊涵蓋了19個國家一共25個城市，就各城市規劃的空間分佈，運輸系統，以及該城 市有關促進健康和可持續性的規劃政策和效能作出分析。詳細研究內容可參考此連結: https://doi.org/INSERT-DOI-HERE。</t>
@@ -5932,9 +5791,6 @@
   </si>
   <si>
     <t xml:space="preserve">Dieser kurze Bericht beschreibt, wie {city} bei einer Auswahl von räumlichen und stadtplanerischen Indikatoren für gesunde und nachhaltige Städte abschneidet. In unserer kollaborativen Studie wurden die räumliche Verteilung von Stadtgestaltung und Verkehrsmerkmalen sowie das Vorhandensein und die Qualität von Stadtplanungsrichtlinien zur Förderung von Gesundheit und Nachhaltigkeit für 25 Städte in 19 Ländern untersucht. Weitere Details der Studie finden Sie unter {study_doi}. </t>
-  </si>
-  <si>
-    <t>(oben) {}% der Bevölkerung erreichen die Mindestschwelle* für die Nachbarschaftsstraßen-kreuzungsdichte ({} {})</t>
   </si>
   <si>
     <t>Klaus Gebel, Sylvia Titze</t>
@@ -6136,6 +5992,150 @@
   </si>
   <si>
     <t>28</t>
+  </si>
+  <si>
+    <t>(above) {} of population meet minimum threshold* for neighbourhood population density ({} people {})</t>
+  </si>
+  <si>
+    <t>(a dalt) {} de població que compleix el llindar mínim* de densitat de població a nivell de barri ({} {})</t>
+  </si>
+  <si>
+    <t>(上圖) {}的人口符合鄰里人口密度的最小閾值</t>
+  </si>
+  <si>
+    <t>(上图) {}的人口符合邻里人口密度的最小阈值</t>
+  </si>
+  <si>
+    <t>(výše) {} obyvatel žije v oblasti, která dosahuje mezní hodnoty* hustoty zalidnění({} obyv. {})</t>
+  </si>
+  <si>
+    <t>(ovenfor)  af indbyggere, der opfylder minimumsgrænsen* for befolkningstæthed i nærområdet ({} {})</t>
+  </si>
+  <si>
+    <t>(boven) {} van de bevolking voldoet aan minimumdrempel* voor buurtgerelateerde bevolkingsdichtheid ({} {})</t>
+  </si>
+  <si>
+    <t>(oben) {} der Bevölkerung erreichen die Mindestschwelle* für die Bevölkerungsdichte in der Nachbarschaft ({} {})</t>
+  </si>
+  <si>
+    <t>(a sama) {} na yawan jama'a sun cika mafi ƙarancin ƙima* don yawan yawan jama'ar unguwa ({} {})</t>
+  </si>
+  <si>
+    <t>(i runga) {} o te iwi whānui e tūtaki ana ki te paepae mōkito* mō te kiato o te iwi whānui paetata ({} {})</t>
+  </si>
+  <si>
+    <t>(arriba) {} de la población cumple con el umbral mínimo* de densidad de población en la colonia ({} {})</t>
+  </si>
+  <si>
+    <t>(arriba) {} de la población cumple con el umbral mínimo* de densidad de población a nivel de barrio ({} {})</t>
+  </si>
+  <si>
+    <t>(acima) {} da população cumpre o limite mínimo* para a densidade populacional da vizinhança ({} {})</t>
+  </si>
+  <si>
+    <t>(acima) {} da população cumpre o limiar mínimo* para a densidade populacional do bairro ({} {})</t>
+  </si>
+  <si>
+    <t>(மேலே) {} மக்கள் தொகை, அக்கம்பக்க மக்கள்தொகை அடர்த்திக்கான குறைந்தபட்ச வரம்பு* ({} {})</t>
+  </si>
+  <si>
+    <t>(trên) {} dân số đáp ứng ngưỡng tối thiểu* đối với mật độ dân số khu dân cư ({} {})</t>
+  </si>
+  <si>
+    <t>(above) {} of population meet minimum threshold* for neighbourhood street intersection density ({} intersections {})</t>
+  </si>
+  <si>
+    <t>(a dalt) {} de població que compleix el llindar mínim* de densitat d'interseccions de carrers a nivell de barri ({} {})</t>
+  </si>
+  <si>
+    <t>(上圖) {}的人口符合鄰里街道交匯處密度的最小閾值</t>
+  </si>
+  <si>
+    <t>(上图) {}的人口符合邻里街道交汇处密度的最小阈值</t>
+  </si>
+  <si>
+    <t>(výše) {} obyvatel žije v oblasti, která dosahuje mezní hodnoty* pro hustotu křižovatek ({} křížovatek {})</t>
+  </si>
+  <si>
+    <t>(ovenfor) {}  af indbyggere, der opfylder minimumgrænsen* for tætheden af vejkryds i nærområdet ({:}{})</t>
+  </si>
+  <si>
+    <t>(boven) {} van de bevolking voldoet aan minimumdrempel* voor de dichtheid van kruispunten in straten in de buurt ({} {})</t>
+  </si>
+  <si>
+    <t>(oben) {} der Bevölkerung erreichen die Mindestschwelle* für die Nachbarschaftsstraßen-kreuzungsdichte ({} {})</t>
+  </si>
+  <si>
+    <t>(a sama) {} na yawan jama'a suna saduwa da mafi ƙanƙanta kofa* don yawan mahadar titin unguwa ({} {})</t>
+  </si>
+  <si>
+    <t>(i runga) {} o te iwi whānui e tūtaki ana ki te paepae mōkito* mō te kiato o te tiriti paetata ({} {})</t>
+  </si>
+  <si>
+    <t>(arriba) {} de la población cumple con el umbral mínimo* de densidad de intersección de calles en la colonia ({} {})</t>
+  </si>
+  <si>
+    <t>(arriba) {} de la población cumple con el umbral mínimo* de densidad de intersecciones de calles a nivel de barrio ({} {})</t>
+  </si>
+  <si>
+    <t>(acima) {} da população cumpre o limite mínimo* para a densidade de intersecção de ruas da vizinhança ({} {})</t>
+  </si>
+  <si>
+    <t>(acima) {} da população cumpre o limiar mínimo* para a densidade de intersecção de rua do bairro ({} {})</t>
+  </si>
+  <si>
+    <t>(மேலே) {} மக்கள் தொகை, அக்கம்பக்க தெரு வெட்டு அடர்த்திக்கான குறைந்தபட்ச வரம்பு* ({} {})</t>
+  </si>
+  <si>
+    <t>(trên) {} dân số đáp ứng ngưỡng tối thiểu* đối với mật độ giao lộ đường xá trong khu dân cư ({} {})</t>
+  </si>
+  <si>
+    <t>(above) {} of population live in neighbourhoods with walkability scores greater than the 25 international city median</t>
+  </si>
+  <si>
+    <t>(a dalt) {} de població que viu en barris amb puntuacions de caminabilitat superiors a la mediana de les 25 ciutats internacionals</t>
+  </si>
+  <si>
+    <t>(上圖) {}的人口居住在比25個城市可步行性中位數高的社區</t>
+  </si>
+  <si>
+    <t>(上图) {}的人口居住在比25个城市可步行性中位数高的社区</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(výše) {} obyvatel žije v oblastech s vyšší úrovní podmínek pro chůzi (walkability), než je medián 25 srovnávaných měst. </t>
+  </si>
+  <si>
+    <t>(ovenfor) {}  af indbyggere, der bor i kvarterer med et walkability indeks, der er større end mediaen for de 25 internationale byer</t>
+  </si>
+  <si>
+    <t>(boven) {} van de bevolking woont in buurten met bewegingsvriendelijkheidsscores die groter zijn dan de mediaan van de 25 internationale steden</t>
+  </si>
+  <si>
+    <t>(oben) {} der Bevölkerung leben in Stadtteilen mit Begehbarkeitswerten, die über dem Median der 25 Städte in 19 Ländern liegen</t>
+  </si>
+  <si>
+    <t>(a sama) {} na yawan jama'a suna rayuwa ne a unguwannin da ke da maki mai iya tafiya fiye da 25 na duniya na tsakiya</t>
+  </si>
+  <si>
+    <t>(i runga) {} o te iwi whānui e noho ana i ngā rohe me ngā tapeke hīkoi nui ake i te taone ao whānui e 25</t>
+  </si>
+  <si>
+    <t>(arriba) {} de la población vive en colonias con puntuaciones de caminabilidad superiores a la mediana de las 25 ciudades internacionales</t>
+  </si>
+  <si>
+    <t>(arriba) {} de la población que vive en barrios con puntuaciones de caminabilidad superiores a la mediana de las 25 ciudades internacionales</t>
+  </si>
+  <si>
+    <t>(acima) {} da população que vive em bairros com pontuação de caminhabilidade maior que a mediana de 25 cidades internacionais</t>
+  </si>
+  <si>
+    <t>(acima) {} da população residente em bairros com pontuações de caminhabilidade superiores às 25 medianas da cidade internacional</t>
+  </si>
+  <si>
+    <t>(மேலே) {} மக்கள் 25 சர்வதேச நகர சராசரியை விட அதிகமான நடைத்திறன் மதிப்பெண்களுடன் சுற்றுப்புறங்களில் வாழ்கின்றனர்</t>
+  </si>
+  <si>
+    <t>(trên) {} dân số sống trong các khu dân cư có điểm số khả năng đi bộ lớn hơn mức trung bình của 25 thành phố quốc tế</t>
   </si>
 </sst>
 </file>
@@ -7562,8 +7562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V195"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
@@ -9070,10 +9070,10 @@
         <v>0</v>
       </c>
       <c r="M26" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="N26" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O26" t="s">
         <v>26</v>
@@ -9132,7 +9132,7 @@
         <v>0</v>
       </c>
       <c r="N27" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O27" t="s">
         <v>26</v>
@@ -9192,7 +9192,7 @@
         <v>0</v>
       </c>
       <c r="N28" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O28" t="s">
         <v>22</v>
@@ -9249,7 +9249,7 @@
         <v>0</v>
       </c>
       <c r="N29" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O29" t="s">
         <v>26</v>
@@ -9309,7 +9309,7 @@
         <v>0</v>
       </c>
       <c r="N30" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O30" t="s">
         <v>28</v>
@@ -9370,7 +9370,7 @@
       </c>
       <c r="M31" s="2"/>
       <c r="N31" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O31" s="2" t="s">
         <v>28</v>
@@ -9432,7 +9432,7 @@
       </c>
       <c r="M32" s="2"/>
       <c r="N32" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O32" s="2" t="s">
         <v>28</v>
@@ -9490,7 +9490,7 @@
         <v>0</v>
       </c>
       <c r="N33" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O33" t="s">
         <v>26</v>
@@ -9546,7 +9546,7 @@
         <v>0</v>
       </c>
       <c r="N34" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O34" t="s">
         <v>26</v>
@@ -9606,7 +9606,7 @@
         <v>0</v>
       </c>
       <c r="N35" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O35" t="s">
         <v>26</v>
@@ -9669,7 +9669,7 @@
         <v>0</v>
       </c>
       <c r="N36" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O36" t="s">
         <v>26</v>
@@ -9729,7 +9729,7 @@
         <v>0</v>
       </c>
       <c r="N37" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O37" t="s">
         <v>28</v>
@@ -9793,13 +9793,13 @@
         <v>0</v>
       </c>
       <c r="N38" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O38" t="s">
         <v>28</v>
       </c>
       <c r="P38" s="5" t="s">
-        <v>1990</v>
+        <v>1942</v>
       </c>
       <c r="Q38">
         <v>3</v>
@@ -9857,13 +9857,13 @@
         <v>0</v>
       </c>
       <c r="N39" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O39" t="s">
         <v>28</v>
       </c>
       <c r="P39" s="5" t="s">
-        <v>1994</v>
+        <v>1946</v>
       </c>
       <c r="Q39">
         <v>3</v>
@@ -9920,7 +9920,7 @@
         <v>0</v>
       </c>
       <c r="N40" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O40" t="s">
         <v>26</v>
@@ -9983,7 +9983,7 @@
         <v>0</v>
       </c>
       <c r="N41" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O41" t="s">
         <v>26</v>
@@ -10043,7 +10043,7 @@
         <v>0</v>
       </c>
       <c r="N42" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O42" t="s">
         <v>28</v>
@@ -10107,13 +10107,13 @@
         <v>0</v>
       </c>
       <c r="N43" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O43" t="s">
         <v>28</v>
       </c>
       <c r="P43" s="5" t="s">
-        <v>1990</v>
+        <v>1942</v>
       </c>
       <c r="Q43">
         <v>3</v>
@@ -10171,13 +10171,13 @@
         <v>0</v>
       </c>
       <c r="N44" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O44" t="s">
         <v>28</v>
       </c>
       <c r="P44" s="5" t="s">
-        <v>1993</v>
+        <v>1945</v>
       </c>
       <c r="Q44">
         <v>3</v>
@@ -10234,7 +10234,7 @@
         <v>0</v>
       </c>
       <c r="N45" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O45" t="s">
         <v>26</v>
@@ -10297,7 +10297,7 @@
         <v>0</v>
       </c>
       <c r="N46" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O46" t="s">
         <v>26</v>
@@ -10357,7 +10357,7 @@
         <v>0</v>
       </c>
       <c r="N47" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O47" t="s">
         <v>28</v>
@@ -10421,13 +10421,13 @@
         <v>0</v>
       </c>
       <c r="N48" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O48" t="s">
         <v>28</v>
       </c>
       <c r="P48" s="5" t="s">
-        <v>1992</v>
+        <v>1944</v>
       </c>
       <c r="Q48">
         <v>3</v>
@@ -10485,13 +10485,13 @@
         <v>0</v>
       </c>
       <c r="N49" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O49" t="s">
         <v>28</v>
       </c>
       <c r="P49" s="5" t="s">
-        <v>1991</v>
+        <v>1943</v>
       </c>
       <c r="Q49">
         <v>3</v>
@@ -10548,7 +10548,7 @@
         <v>0</v>
       </c>
       <c r="N50" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O50" t="s">
         <v>26</v>
@@ -10611,7 +10611,7 @@
         <v>0</v>
       </c>
       <c r="N51" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O51" t="s">
         <v>26</v>
@@ -10671,7 +10671,7 @@
         <v>0</v>
       </c>
       <c r="N52" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O52" t="s">
         <v>28</v>
@@ -10735,13 +10735,13 @@
         <v>0</v>
       </c>
       <c r="N53" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O53" t="s">
         <v>28</v>
       </c>
       <c r="P53" s="5" t="s">
-        <v>1987</v>
+        <v>1939</v>
       </c>
       <c r="Q53">
         <v>3</v>
@@ -10799,13 +10799,13 @@
         <v>0</v>
       </c>
       <c r="N54" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O54" t="s">
         <v>28</v>
       </c>
       <c r="P54" s="5" t="s">
-        <v>1989</v>
+        <v>1941</v>
       </c>
       <c r="Q54">
         <v>3</v>
@@ -10862,7 +10862,7 @@
         <v>0</v>
       </c>
       <c r="N55" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O55" t="s">
         <v>26</v>
@@ -10925,7 +10925,7 @@
         <v>0</v>
       </c>
       <c r="N56" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O56" t="s">
         <v>26</v>
@@ -10985,7 +10985,7 @@
         <v>0</v>
       </c>
       <c r="N57" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O57" t="s">
         <v>28</v>
@@ -11049,13 +11049,13 @@
         <v>0</v>
       </c>
       <c r="N58" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O58" t="s">
         <v>28</v>
       </c>
       <c r="P58" s="5" t="s">
-        <v>1987</v>
+        <v>1939</v>
       </c>
       <c r="Q58">
         <v>3</v>
@@ -11113,13 +11113,13 @@
         <v>0</v>
       </c>
       <c r="N59" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O59" t="s">
         <v>28</v>
       </c>
       <c r="P59" s="5" t="s">
-        <v>1988</v>
+        <v>1940</v>
       </c>
       <c r="Q59">
         <v>3</v>
@@ -11176,7 +11176,7 @@
         <v>0</v>
       </c>
       <c r="N60" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O60" t="s">
         <v>26</v>
@@ -11239,7 +11239,7 @@
         <v>0</v>
       </c>
       <c r="N61" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O61" t="s">
         <v>26</v>
@@ -11299,7 +11299,7 @@
         <v>0</v>
       </c>
       <c r="N62" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O62" t="s">
         <v>28</v>
@@ -11363,13 +11363,13 @@
         <v>0</v>
       </c>
       <c r="N63" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O63" t="s">
         <v>28</v>
       </c>
       <c r="P63" s="5" t="s">
-        <v>1987</v>
+        <v>1939</v>
       </c>
       <c r="Q63">
         <v>3</v>
@@ -11427,13 +11427,13 @@
         <v>0</v>
       </c>
       <c r="N64" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O64" t="s">
         <v>28</v>
       </c>
       <c r="P64" s="5" t="s">
-        <v>1986</v>
+        <v>1938</v>
       </c>
       <c r="Q64">
         <v>3</v>
@@ -11717,10 +11717,10 @@
         <v>0</v>
       </c>
       <c r="M69" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="N69" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O69" t="s">
         <v>26</v>
@@ -11780,7 +11780,7 @@
         <v>0</v>
       </c>
       <c r="N70" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O70" t="s">
         <v>26</v>
@@ -11840,7 +11840,7 @@
         <v>0</v>
       </c>
       <c r="N71" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O71" t="s">
         <v>28</v>
@@ -11900,7 +11900,7 @@
         <v>0</v>
       </c>
       <c r="N72" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O72" t="s">
         <v>28</v>
@@ -11960,7 +11960,7 @@
         <v>0</v>
       </c>
       <c r="N73" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O73" t="s">
         <v>28</v>
@@ -12020,7 +12020,7 @@
         <v>0</v>
       </c>
       <c r="N74" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O74" t="s">
         <v>28</v>
@@ -12077,7 +12077,7 @@
         <v>0</v>
       </c>
       <c r="N75" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O75" t="s">
         <v>26</v>
@@ -12134,7 +12134,7 @@
         <v>0</v>
       </c>
       <c r="N76" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O76" t="s">
         <v>26</v>
@@ -12191,7 +12191,7 @@
         <v>0</v>
       </c>
       <c r="N77" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O77" t="s">
         <v>26</v>
@@ -12248,7 +12248,7 @@
         <v>0</v>
       </c>
       <c r="N78" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O78" t="s">
         <v>26</v>
@@ -12308,7 +12308,7 @@
         <v>0</v>
       </c>
       <c r="N79" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O79" t="s">
         <v>26</v>
@@ -12368,7 +12368,7 @@
         <v>0</v>
       </c>
       <c r="N80" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O80" t="s">
         <v>26</v>
@@ -12428,7 +12428,7 @@
         <v>0</v>
       </c>
       <c r="N81" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O81" t="s">
         <v>26</v>
@@ -12488,7 +12488,7 @@
         <v>0</v>
       </c>
       <c r="N82" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O82" t="s">
         <v>26</v>
@@ -12548,7 +12548,7 @@
         <v>0</v>
       </c>
       <c r="N83" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O83" t="s">
         <v>26</v>
@@ -12608,7 +12608,7 @@
         <v>0</v>
       </c>
       <c r="N84" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O84" t="s">
         <v>26</v>
@@ -12668,7 +12668,7 @@
         <v>0</v>
       </c>
       <c r="N85" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O85" t="s">
         <v>26</v>
@@ -12728,7 +12728,7 @@
         <v>0</v>
       </c>
       <c r="N86" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O86" t="s">
         <v>26</v>
@@ -12788,7 +12788,7 @@
         <v>0</v>
       </c>
       <c r="N87" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O87" t="s">
         <v>26</v>
@@ -12848,7 +12848,7 @@
         <v>0</v>
       </c>
       <c r="N88" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O88" t="s">
         <v>26</v>
@@ -12908,7 +12908,7 @@
         <v>0</v>
       </c>
       <c r="N89" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O89" t="s">
         <v>26</v>
@@ -12968,7 +12968,7 @@
         <v>0</v>
       </c>
       <c r="N90" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O90" t="s">
         <v>26</v>
@@ -13028,7 +13028,7 @@
         <v>0</v>
       </c>
       <c r="N91" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O91" t="s">
         <v>26</v>
@@ -13088,7 +13088,7 @@
         <v>0</v>
       </c>
       <c r="N92" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O92" t="s">
         <v>26</v>
@@ -13148,7 +13148,7 @@
         <v>0</v>
       </c>
       <c r="N93" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O93" t="s">
         <v>26</v>
@@ -13208,7 +13208,7 @@
         <v>0</v>
       </c>
       <c r="N94" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O94" t="s">
         <v>26</v>
@@ -13268,7 +13268,7 @@
         <v>0</v>
       </c>
       <c r="N95" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O95" t="s">
         <v>26</v>
@@ -13328,7 +13328,7 @@
         <v>0</v>
       </c>
       <c r="N96" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O96" t="s">
         <v>26</v>
@@ -13388,7 +13388,7 @@
         <v>0</v>
       </c>
       <c r="N97" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O97" t="s">
         <v>26</v>
@@ -13448,7 +13448,7 @@
         <v>0</v>
       </c>
       <c r="N98" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O98" t="s">
         <v>26</v>
@@ -13508,7 +13508,7 @@
         <v>0</v>
       </c>
       <c r="N99" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O99" t="s">
         <v>26</v>
@@ -13568,7 +13568,7 @@
         <v>0</v>
       </c>
       <c r="N100" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O100" t="s">
         <v>26</v>
@@ -13628,7 +13628,7 @@
         <v>0</v>
       </c>
       <c r="N101" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O101" t="s">
         <v>26</v>
@@ -13688,7 +13688,7 @@
         <v>0</v>
       </c>
       <c r="N102" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O102" t="s">
         <v>26</v>
@@ -13748,7 +13748,7 @@
         <v>0</v>
       </c>
       <c r="N103" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O103" t="s">
         <v>26</v>
@@ -13808,7 +13808,7 @@
         <v>0</v>
       </c>
       <c r="N104" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O104" t="s">
         <v>26</v>
@@ -13868,7 +13868,7 @@
         <v>0</v>
       </c>
       <c r="N105" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O105" t="s">
         <v>26</v>
@@ -13928,7 +13928,7 @@
         <v>0</v>
       </c>
       <c r="N106" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O106" t="s">
         <v>26</v>
@@ -13988,7 +13988,7 @@
         <v>0</v>
       </c>
       <c r="N107" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O107" t="s">
         <v>26</v>
@@ -14048,7 +14048,7 @@
         <v>0</v>
       </c>
       <c r="N108" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O108" t="s">
         <v>26</v>
@@ -14108,7 +14108,7 @@
         <v>0</v>
       </c>
       <c r="N109" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O109" t="s">
         <v>26</v>
@@ -14168,7 +14168,7 @@
         <v>0</v>
       </c>
       <c r="N110" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O110" t="s">
         <v>26</v>
@@ -14228,7 +14228,7 @@
         <v>0</v>
       </c>
       <c r="N111" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O111" t="s">
         <v>26</v>
@@ -14288,7 +14288,7 @@
         <v>0</v>
       </c>
       <c r="N112" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O112" t="s">
         <v>26</v>
@@ -14348,7 +14348,7 @@
         <v>0</v>
       </c>
       <c r="N113" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O113" t="s">
         <v>26</v>
@@ -15205,10 +15205,10 @@
         <v>0</v>
       </c>
       <c r="M128" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="N128" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O128" t="s">
         <v>26</v>
@@ -15268,7 +15268,7 @@
         <v>0</v>
       </c>
       <c r="N129" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O129" t="s">
         <v>26</v>
@@ -15328,7 +15328,7 @@
         <v>0</v>
       </c>
       <c r="N130" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O130" t="s">
         <v>28</v>
@@ -15388,7 +15388,7 @@
         <v>0</v>
       </c>
       <c r="N131" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O131" t="s">
         <v>28</v>
@@ -15448,7 +15448,7 @@
         <v>0</v>
       </c>
       <c r="N132" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O132" t="s">
         <v>28</v>
@@ -15508,7 +15508,7 @@
         <v>0</v>
       </c>
       <c r="N133" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O133" t="s">
         <v>28</v>
@@ -15565,7 +15565,7 @@
         <v>0</v>
       </c>
       <c r="N134" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O134" t="s">
         <v>26</v>
@@ -15622,7 +15622,7 @@
         <v>0</v>
       </c>
       <c r="N135" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O135" t="s">
         <v>26</v>
@@ -15679,7 +15679,7 @@
         <v>0</v>
       </c>
       <c r="N136" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O136" t="s">
         <v>26</v>
@@ -15736,7 +15736,7 @@
         <v>0</v>
       </c>
       <c r="N137" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O137" t="s">
         <v>26</v>
@@ -15796,7 +15796,7 @@
         <v>0</v>
       </c>
       <c r="N138" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O138" t="s">
         <v>26</v>
@@ -15856,7 +15856,7 @@
         <v>0</v>
       </c>
       <c r="N139" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O139" t="s">
         <v>26</v>
@@ -15916,7 +15916,7 @@
         <v>0</v>
       </c>
       <c r="N140" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O140" t="s">
         <v>26</v>
@@ -15976,7 +15976,7 @@
         <v>0</v>
       </c>
       <c r="N141" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O141" t="s">
         <v>26</v>
@@ -16036,7 +16036,7 @@
         <v>0</v>
       </c>
       <c r="N142" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O142" t="s">
         <v>26</v>
@@ -16096,7 +16096,7 @@
         <v>0</v>
       </c>
       <c r="N143" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O143" t="s">
         <v>26</v>
@@ -16156,7 +16156,7 @@
         <v>0</v>
       </c>
       <c r="N144" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O144" t="s">
         <v>26</v>
@@ -16216,7 +16216,7 @@
         <v>0</v>
       </c>
       <c r="N145" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O145" t="s">
         <v>26</v>
@@ -16276,7 +16276,7 @@
         <v>0</v>
       </c>
       <c r="N146" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O146" t="s">
         <v>26</v>
@@ -16336,7 +16336,7 @@
         <v>0</v>
       </c>
       <c r="N147" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O147" t="s">
         <v>26</v>
@@ -16396,7 +16396,7 @@
         <v>0</v>
       </c>
       <c r="N148" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O148" t="s">
         <v>26</v>
@@ -16456,7 +16456,7 @@
         <v>0</v>
       </c>
       <c r="N149" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O149" t="s">
         <v>26</v>
@@ -16516,7 +16516,7 @@
         <v>0</v>
       </c>
       <c r="N150" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O150" t="s">
         <v>26</v>
@@ -16576,7 +16576,7 @@
         <v>0</v>
       </c>
       <c r="N151" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O151" t="s">
         <v>26</v>
@@ -16636,7 +16636,7 @@
         <v>0</v>
       </c>
       <c r="N152" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O152" t="s">
         <v>26</v>
@@ -16696,7 +16696,7 @@
         <v>0</v>
       </c>
       <c r="N153" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O153" t="s">
         <v>26</v>
@@ -16756,7 +16756,7 @@
         <v>0</v>
       </c>
       <c r="N154" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O154" t="s">
         <v>26</v>
@@ -16816,7 +16816,7 @@
         <v>0</v>
       </c>
       <c r="N155" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O155" t="s">
         <v>26</v>
@@ -16876,7 +16876,7 @@
         <v>0</v>
       </c>
       <c r="N156" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O156" t="s">
         <v>26</v>
@@ -16936,7 +16936,7 @@
         <v>0</v>
       </c>
       <c r="N157" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O157" t="s">
         <v>26</v>
@@ -17164,10 +17164,10 @@
         <v>0</v>
       </c>
       <c r="M161" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="N161" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O161" t="s">
         <v>26</v>
@@ -17227,7 +17227,7 @@
         <v>0</v>
       </c>
       <c r="N162" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O162" t="s">
         <v>26</v>
@@ -17287,7 +17287,7 @@
         <v>0</v>
       </c>
       <c r="N163" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O163" t="s">
         <v>28</v>
@@ -17347,7 +17347,7 @@
         <v>0</v>
       </c>
       <c r="N164" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O164" t="s">
         <v>28</v>
@@ -17407,7 +17407,7 @@
         <v>0</v>
       </c>
       <c r="N165" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O165" t="s">
         <v>28</v>
@@ -17467,7 +17467,7 @@
         <v>0</v>
       </c>
       <c r="N166" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O166" t="s">
         <v>28</v>
@@ -17524,7 +17524,7 @@
         <v>0</v>
       </c>
       <c r="N167" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O167" t="s">
         <v>26</v>
@@ -17581,7 +17581,7 @@
         <v>0</v>
       </c>
       <c r="N168" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O168" t="s">
         <v>26</v>
@@ -17638,7 +17638,7 @@
         <v>0</v>
       </c>
       <c r="N169" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O169" t="s">
         <v>26</v>
@@ -17695,7 +17695,7 @@
         <v>0</v>
       </c>
       <c r="N170" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O170" t="s">
         <v>26</v>
@@ -17755,7 +17755,7 @@
         <v>0</v>
       </c>
       <c r="N171" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O171" t="s">
         <v>26</v>
@@ -17815,7 +17815,7 @@
         <v>0</v>
       </c>
       <c r="N172" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O172" t="s">
         <v>26</v>
@@ -17875,7 +17875,7 @@
         <v>0</v>
       </c>
       <c r="N173" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O173" t="s">
         <v>26</v>
@@ -17935,7 +17935,7 @@
         <v>0</v>
       </c>
       <c r="N174" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O174" t="s">
         <v>26</v>
@@ -17995,7 +17995,7 @@
         <v>0</v>
       </c>
       <c r="N175" t="s">
-        <v>1979</v>
+        <v>1931</v>
       </c>
       <c r="O175" t="s">
         <v>26</v>
@@ -18049,10 +18049,10 @@
         <v>0</v>
       </c>
       <c r="M176" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="N176" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O176" t="s">
         <v>26</v>
@@ -18110,7 +18110,7 @@
         <v>0</v>
       </c>
       <c r="N177" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O177" t="s">
         <v>208</v>
@@ -18170,7 +18170,7 @@
         <v>0</v>
       </c>
       <c r="N178" t="s">
-        <v>1978</v>
+        <v>1930</v>
       </c>
       <c r="O178" t="s">
         <v>208</v>
@@ -18919,7 +18919,7 @@
     </row>
     <row r="192" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>1981</v>
+        <v>1933</v>
       </c>
       <c r="B192">
         <v>6</v>
@@ -19165,11 +19165,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V170"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="E56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomRight" activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19318,61 +19318,61 @@
         <v>146</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>1920</v>
+        <v>1873</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>1786</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>1915</v>
+        <v>1868</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>1916</v>
+        <v>1869</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>1917</v>
+        <v>1870</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>1918</v>
+        <v>1871</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>1919</v>
+        <v>1872</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>1921</v>
+        <v>1874</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>1894</v>
+        <v>1847</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>1922</v>
+        <v>1875</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>1923</v>
+        <v>1876</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>1923</v>
+        <v>1876</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>1924</v>
+        <v>1877</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>1924</v>
+        <v>1877</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>1925</v>
+        <v>1878</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>1925</v>
+        <v>1878</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>1926</v>
+        <v>1879</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>1927</v>
+        <v>1880</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>1928</v>
+        <v>1881</v>
       </c>
       <c r="U3" s="9"/>
       <c r="V3" s="9"/>
@@ -21301,7 +21301,7 @@
         <v>1586</v>
       </c>
       <c r="S57" s="12" t="s">
-        <v>1932</v>
+        <v>1885</v>
       </c>
       <c r="T57" s="11" t="s">
         <v>1588</v>
@@ -21329,7 +21329,7 @@
         <v>1591</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>1945</v>
+        <v>1897</v>
       </c>
       <c r="H58" s="12" t="s">
         <v>1590</v>
@@ -22011,7 +22011,7 @@
         <v>1008</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>1944</v>
+        <v>1896</v>
       </c>
       <c r="H69" s="9" t="s">
         <v>1499</v>
@@ -22395,7 +22395,7 @@
         <v>1614</v>
       </c>
       <c r="K75" s="22" t="s">
-        <v>1976</v>
+        <v>1928</v>
       </c>
       <c r="L75" s="22"/>
       <c r="M75" s="22" t="s">
@@ -22433,56 +22433,56 @@
         <v>588</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>1807</v>
+        <v>1947</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>1808</v>
+        <v>1948</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>1802</v>
+        <v>1949</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>1803</v>
+        <v>1950</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>1809</v>
+        <v>1951</v>
       </c>
       <c r="H76" s="9" t="s">
-        <v>1833</v>
+        <v>1952</v>
       </c>
       <c r="I76" s="22" t="s">
-        <v>1810</v>
+        <v>1953</v>
       </c>
       <c r="J76" s="9" t="s">
-        <v>1811</v>
+        <v>1954</v>
       </c>
       <c r="K76" s="22" t="s">
-        <v>1812</v>
+        <v>1955</v>
       </c>
       <c r="L76" s="22"/>
       <c r="M76" s="22" t="s">
-        <v>1813</v>
+        <v>1956</v>
       </c>
       <c r="N76" s="9" t="s">
-        <v>1814</v>
+        <v>1957</v>
       </c>
       <c r="O76" s="11" t="s">
-        <v>1815</v>
+        <v>1958</v>
       </c>
       <c r="P76" s="9" t="s">
-        <v>1816</v>
+        <v>1959</v>
       </c>
       <c r="Q76" s="9" t="s">
-        <v>1817</v>
+        <v>1960</v>
       </c>
       <c r="R76" s="9" t="s">
-        <v>1818</v>
+        <v>1961</v>
       </c>
       <c r="S76" s="9" t="s">
-        <v>1819</v>
+        <v>1788</v>
       </c>
       <c r="T76" s="9" t="s">
-        <v>1820</v>
+        <v>1962</v>
       </c>
       <c r="U76" s="9"/>
       <c r="V76" s="9"/>
@@ -22495,56 +22495,56 @@
         <v>589</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>1821</v>
+        <v>1963</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>1822</v>
+        <v>1964</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>1804</v>
+        <v>1965</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>1805</v>
+        <v>1966</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>1823</v>
+        <v>1967</v>
       </c>
       <c r="H77" s="9" t="s">
-        <v>1806</v>
+        <v>1968</v>
       </c>
       <c r="I77" s="22" t="s">
-        <v>1824</v>
+        <v>1969</v>
       </c>
       <c r="J77" s="9" t="s">
-        <v>1940</v>
+        <v>1970</v>
       </c>
       <c r="K77" s="22" t="s">
-        <v>1825</v>
+        <v>1971</v>
       </c>
       <c r="L77" s="22"/>
       <c r="M77" s="22" t="s">
-        <v>1826</v>
+        <v>1972</v>
       </c>
       <c r="N77" s="9" t="s">
-        <v>1827</v>
+        <v>1973</v>
       </c>
       <c r="O77" s="11" t="s">
-        <v>1828</v>
+        <v>1974</v>
       </c>
       <c r="P77" s="9" t="s">
-        <v>1829</v>
+        <v>1975</v>
       </c>
       <c r="Q77" s="9" t="s">
-        <v>1830</v>
+        <v>1976</v>
       </c>
       <c r="R77" s="9" t="s">
-        <v>1831</v>
+        <v>1977</v>
       </c>
       <c r="S77" s="9" t="s">
-        <v>1832</v>
+        <v>1789</v>
       </c>
       <c r="T77" s="9" t="s">
-        <v>1834</v>
+        <v>1978</v>
       </c>
       <c r="U77" s="9"/>
       <c r="V77" s="9"/>
@@ -22557,56 +22557,56 @@
         <v>587</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>1787</v>
+        <v>1979</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>1788</v>
+        <v>1980</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>1789</v>
+        <v>1981</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>1790</v>
+        <v>1982</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>1791</v>
+        <v>1983</v>
       </c>
       <c r="H78" s="9" t="s">
-        <v>1835</v>
+        <v>1984</v>
       </c>
       <c r="I78" s="22" t="s">
-        <v>1792</v>
+        <v>1985</v>
       </c>
       <c r="J78" s="9" t="s">
-        <v>1836</v>
+        <v>1986</v>
       </c>
       <c r="K78" s="22" t="s">
-        <v>1793</v>
+        <v>1987</v>
       </c>
       <c r="L78" s="22"/>
       <c r="M78" s="22" t="s">
-        <v>1794</v>
+        <v>1988</v>
       </c>
       <c r="N78" s="9" t="s">
-        <v>1795</v>
+        <v>1989</v>
       </c>
       <c r="O78" s="9" t="s">
-        <v>1796</v>
+        <v>1990</v>
       </c>
       <c r="P78" s="9" t="s">
-        <v>1797</v>
+        <v>1991</v>
       </c>
       <c r="Q78" s="9" t="s">
-        <v>1798</v>
+        <v>1992</v>
       </c>
       <c r="R78" s="9" t="s">
-        <v>1799</v>
+        <v>1993</v>
       </c>
       <c r="S78" s="9" t="s">
-        <v>1800</v>
+        <v>1787</v>
       </c>
       <c r="T78" s="9" t="s">
-        <v>1801</v>
+        <v>1994</v>
       </c>
       <c r="U78" s="9"/>
       <c r="V78" s="9"/>
@@ -23121,7 +23121,7 @@
         <v>1643</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>1837</v>
+        <v>1790</v>
       </c>
       <c r="F87" s="11" t="s">
         <v>1664</v>
@@ -23136,7 +23136,7 @@
         <v>1646</v>
       </c>
       <c r="J87" s="11" t="s">
-        <v>1939</v>
+        <v>1892</v>
       </c>
       <c r="K87" s="22" t="s">
         <v>1647</v>
@@ -23146,13 +23146,13 @@
         <v>1648</v>
       </c>
       <c r="N87" s="11" t="s">
-        <v>1838</v>
+        <v>1791</v>
       </c>
       <c r="O87" s="11" t="s">
-        <v>1839</v>
+        <v>1792</v>
       </c>
       <c r="P87" s="11" t="s">
-        <v>1840</v>
+        <v>1793</v>
       </c>
       <c r="Q87" s="11" t="s">
         <v>1649</v>
@@ -23161,7 +23161,7 @@
         <v>1740</v>
       </c>
       <c r="S87" s="11" t="s">
-        <v>1960</v>
+        <v>1912</v>
       </c>
       <c r="T87" s="11" t="s">
         <v>1650</v>
@@ -23223,7 +23223,7 @@
         <v>1734</v>
       </c>
       <c r="S88" s="11" t="s">
-        <v>1961</v>
+        <v>1913</v>
       </c>
       <c r="T88" s="11" t="s">
         <v>1323</v>
@@ -23270,7 +23270,7 @@
         <v>643</v>
       </c>
       <c r="N89" s="11" t="s">
-        <v>1841</v>
+        <v>1794</v>
       </c>
       <c r="O89" s="11" t="s">
         <v>814</v>
@@ -23425,7 +23425,7 @@
         <v>232</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>1842</v>
+        <v>1795</v>
       </c>
       <c r="D92" s="11" t="s">
         <v>1342</v>
@@ -23440,41 +23440,41 @@
         <v>1367</v>
       </c>
       <c r="H92" s="11" t="s">
-        <v>1843</v>
+        <v>1796</v>
       </c>
       <c r="I92" s="22" t="s">
-        <v>1844</v>
+        <v>1797</v>
       </c>
       <c r="J92" s="11" t="s">
-        <v>1845</v>
+        <v>1798</v>
       </c>
       <c r="K92" s="22" t="s">
         <v>1439</v>
       </c>
       <c r="L92" s="22"/>
       <c r="M92" s="22" t="s">
-        <v>1846</v>
+        <v>1799</v>
       </c>
       <c r="N92" s="11" t="s">
-        <v>1847</v>
+        <v>1800</v>
       </c>
       <c r="O92" s="11" t="s">
-        <v>1848</v>
+        <v>1801</v>
       </c>
       <c r="P92" s="11" t="s">
         <v>1154</v>
       </c>
       <c r="Q92" s="11" t="s">
-        <v>1849</v>
+        <v>1802</v>
       </c>
       <c r="R92" s="11" t="s">
-        <v>1850</v>
+        <v>1803</v>
       </c>
       <c r="S92" s="11" t="s">
         <v>866</v>
       </c>
       <c r="T92" s="11" t="s">
-        <v>1851</v>
+        <v>1804</v>
       </c>
       <c r="U92" s="11"/>
       <c r="V92" s="11"/>
@@ -23595,7 +23595,7 @@
         <v>1737</v>
       </c>
       <c r="S94" s="11" t="s">
-        <v>1963</v>
+        <v>1915</v>
       </c>
       <c r="T94" s="11" t="s">
         <v>1333</v>
@@ -23682,7 +23682,7 @@
         <v>1028</v>
       </c>
       <c r="F96" s="11" t="s">
-        <v>1930</v>
+        <v>1883</v>
       </c>
       <c r="G96" s="12" t="s">
         <v>1369</v>
@@ -23694,7 +23694,7 @@
         <v>1233</v>
       </c>
       <c r="J96" s="11" t="s">
-        <v>1933</v>
+        <v>1886</v>
       </c>
       <c r="K96" s="22" t="s">
         <v>1441</v>
@@ -23843,7 +23843,7 @@
         <v>1739</v>
       </c>
       <c r="S98" s="11" t="s">
-        <v>1966</v>
+        <v>1918</v>
       </c>
       <c r="T98" s="11" t="s">
         <v>1291</v>
@@ -23880,7 +23880,7 @@
         <v>1262</v>
       </c>
       <c r="J99" s="11" t="s">
-        <v>1893</v>
+        <v>1846</v>
       </c>
       <c r="K99" s="22" t="s">
         <v>1444</v>
@@ -24004,7 +24004,7 @@
         <v>1234</v>
       </c>
       <c r="J101" s="11" t="s">
-        <v>1934</v>
+        <v>1887</v>
       </c>
       <c r="K101" s="22" t="s">
         <v>1446</v>
@@ -24091,7 +24091,7 @@
         <v>373</v>
       </c>
       <c r="S102" s="11" t="s">
-        <v>1964</v>
+        <v>1916</v>
       </c>
       <c r="T102" s="11" t="s">
         <v>1293</v>
@@ -24128,7 +24128,7 @@
         <v>1236</v>
       </c>
       <c r="J103" s="11" t="s">
-        <v>1942</v>
+        <v>1894</v>
       </c>
       <c r="K103" s="22" t="s">
         <v>1448</v>
@@ -24153,7 +24153,7 @@
         <v>374</v>
       </c>
       <c r="S103" s="11" t="s">
-        <v>1965</v>
+        <v>1917</v>
       </c>
       <c r="T103" s="11" t="s">
         <v>1294</v>
@@ -24190,7 +24190,7 @@
         <v>1237</v>
       </c>
       <c r="J104" s="11" t="s">
-        <v>1943</v>
+        <v>1895</v>
       </c>
       <c r="K104" s="22" t="s">
         <v>1449</v>
@@ -24355,7 +24355,7 @@
         <v>51</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>1852</v>
+        <v>1805</v>
       </c>
       <c r="D107" s="11" t="s">
         <v>902</v>
@@ -24376,7 +24376,7 @@
         <v>1240</v>
       </c>
       <c r="J107" s="14" t="s">
-        <v>1935</v>
+        <v>1888</v>
       </c>
       <c r="K107" s="22" t="s">
         <v>1452</v>
@@ -24398,10 +24398,10 @@
         <v>1566</v>
       </c>
       <c r="R107" s="11" t="s">
-        <v>1952</v>
+        <v>1904</v>
       </c>
       <c r="S107" s="11" t="s">
-        <v>1962</v>
+        <v>1914</v>
       </c>
       <c r="T107" s="11" t="s">
         <v>1297</v>
@@ -24581,7 +24581,7 @@
         <v>1166</v>
       </c>
       <c r="Q110" s="11" t="s">
-        <v>1853</v>
+        <v>1806</v>
       </c>
       <c r="R110" s="11" t="s">
         <v>434</v>
@@ -24711,7 +24711,7 @@
         <v>377</v>
       </c>
       <c r="S112" s="11" t="s">
-        <v>1968</v>
+        <v>1920</v>
       </c>
       <c r="T112" s="11" t="s">
         <v>359</v>
@@ -24810,7 +24810,7 @@
         <v>1243</v>
       </c>
       <c r="J114" s="11" t="s">
-        <v>1938</v>
+        <v>1891</v>
       </c>
       <c r="K114" s="22" t="s">
         <v>1456</v>
@@ -24835,7 +24835,7 @@
         <v>1743</v>
       </c>
       <c r="S114" s="11" t="s">
-        <v>1967</v>
+        <v>1919</v>
       </c>
       <c r="T114" s="11" t="s">
         <v>1300</v>
@@ -25021,7 +25021,7 @@
         <v>1745</v>
       </c>
       <c r="S117" s="11" t="s">
-        <v>1971</v>
+        <v>1923</v>
       </c>
       <c r="T117" s="11" t="s">
         <v>1325</v>
@@ -25083,7 +25083,7 @@
         <v>1746</v>
       </c>
       <c r="S118" s="11" t="s">
-        <v>1969</v>
+        <v>1921</v>
       </c>
       <c r="T118" s="11" t="s">
         <v>361</v>
@@ -25145,7 +25145,7 @@
         <v>380</v>
       </c>
       <c r="S119" s="11" t="s">
-        <v>1970</v>
+        <v>1922</v>
       </c>
       <c r="T119" s="11" t="s">
         <v>1303</v>
@@ -25449,7 +25449,7 @@
         <v>1173</v>
       </c>
       <c r="Q124" s="11" t="s">
-        <v>1854</v>
+        <v>1807</v>
       </c>
       <c r="R124" s="11" t="s">
         <v>1748</v>
@@ -25489,10 +25489,10 @@
         <v>1540</v>
       </c>
       <c r="I125" s="22" t="s">
-        <v>1855</v>
+        <v>1808</v>
       </c>
       <c r="J125" s="14" t="s">
-        <v>1936</v>
+        <v>1889</v>
       </c>
       <c r="K125" s="22" t="s">
         <v>1467</v>
@@ -25514,13 +25514,13 @@
         <v>1568</v>
       </c>
       <c r="R125" s="11" t="s">
-        <v>1953</v>
+        <v>1905</v>
       </c>
       <c r="S125" s="11" t="s">
-        <v>1972</v>
+        <v>1924</v>
       </c>
       <c r="T125" s="11" t="s">
-        <v>1856</v>
+        <v>1809</v>
       </c>
       <c r="U125" s="11"/>
       <c r="V125" s="11"/>
@@ -25821,13 +25821,13 @@
         <v>1175</v>
       </c>
       <c r="Q130" s="11" t="s">
-        <v>1857</v>
+        <v>1810</v>
       </c>
       <c r="R130" s="11" t="s">
         <v>1750</v>
       </c>
       <c r="S130" s="11" t="s">
-        <v>1973</v>
+        <v>1925</v>
       </c>
       <c r="T130" s="11" t="s">
         <v>1327</v>
@@ -26425,7 +26425,7 @@
         <v>471</v>
       </c>
       <c r="K140" s="22" t="s">
-        <v>1977</v>
+        <v>1929</v>
       </c>
       <c r="L140" s="22"/>
       <c r="M140" s="22" t="s">
@@ -26450,7 +26450,7 @@
         <v>878</v>
       </c>
       <c r="T140" s="11" t="s">
-        <v>1858</v>
+        <v>1811</v>
       </c>
       <c r="U140" s="11"/>
       <c r="V140" s="11"/>
@@ -26464,7 +26464,7 @@
         <v>Maiduguri - Summary</v>
       </c>
       <c r="C141" s="12" t="s">
-        <v>1881</v>
+        <v>1834</v>
       </c>
       <c r="D141" s="11"/>
       <c r="E141" s="11"/>
@@ -26499,7 +26499,7 @@
         <v>Mexico City - Summary</v>
       </c>
       <c r="C142" s="12" t="s">
-        <v>1859</v>
+        <v>1812</v>
       </c>
       <c r="D142" s="11"/>
       <c r="E142" s="11"/>
@@ -26512,7 +26512,7 @@
       <c r="L142" s="22"/>
       <c r="M142" s="22"/>
       <c r="N142" s="11" t="s">
-        <v>1860</v>
+        <v>1813</v>
       </c>
       <c r="O142" s="11"/>
       <c r="P142" s="11"/>
@@ -26534,7 +26534,7 @@
         <v>Baltimore - Summary</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>1882</v>
+        <v>1835</v>
       </c>
       <c r="D143" s="11"/>
       <c r="E143" s="11"/>
@@ -26567,7 +26567,7 @@
         <v>Phoenix - Summary</v>
       </c>
       <c r="C144" s="12" t="s">
-        <v>1861</v>
+        <v>1814</v>
       </c>
       <c r="D144" s="11"/>
       <c r="E144" s="11"/>
@@ -26600,7 +26600,7 @@
         <v>Seattle - Summary</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>1862</v>
+        <v>1815</v>
       </c>
       <c r="D145" s="11"/>
       <c r="E145" s="11"/>
@@ -26633,7 +26633,7 @@
         <v>Sao Paulo - Summary</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>1863</v>
+        <v>1816</v>
       </c>
       <c r="D146" s="11"/>
       <c r="E146" s="11"/>
@@ -26668,14 +26668,14 @@
         <v>Hong Kong - Summary</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>1864</v>
+        <v>1817</v>
       </c>
       <c r="D147" s="11"/>
       <c r="E147" s="11" t="s">
-        <v>1929</v>
+        <v>1882</v>
       </c>
       <c r="F147" s="11" t="s">
-        <v>1931</v>
+        <v>1884</v>
       </c>
       <c r="G147" s="12"/>
       <c r="H147" s="11"/>
@@ -26705,7 +26705,7 @@
         <v>Chennai - Summary</v>
       </c>
       <c r="C148" s="12" t="s">
-        <v>1865</v>
+        <v>1818</v>
       </c>
       <c r="D148" s="11"/>
       <c r="E148" s="11"/>
@@ -26724,7 +26724,7 @@
         <v>1110</v>
       </c>
       <c r="R148" s="11" t="s">
-        <v>1866</v>
+        <v>1819</v>
       </c>
       <c r="S148" s="11"/>
       <c r="T148" s="11"/>
@@ -26740,7 +26740,7 @@
         <v>Bangkok - Summary</v>
       </c>
       <c r="C149" s="12" t="s">
-        <v>1883</v>
+        <v>1836</v>
       </c>
       <c r="D149" s="11"/>
       <c r="E149" s="11"/>
@@ -26760,7 +26760,7 @@
       </c>
       <c r="R149" s="11"/>
       <c r="S149" s="11" t="s">
-        <v>1974</v>
+        <v>1926</v>
       </c>
       <c r="T149" s="11"/>
       <c r="U149" s="11"/>
@@ -26775,7 +26775,7 @@
         <v>Hanoi - Summary</v>
       </c>
       <c r="C150" s="12" t="s">
-        <v>1867</v>
+        <v>1820</v>
       </c>
       <c r="D150" s="11"/>
       <c r="E150" s="11"/>
@@ -26796,7 +26796,7 @@
       <c r="R150" s="11"/>
       <c r="S150" s="11"/>
       <c r="T150" s="11" t="s">
-        <v>1868</v>
+        <v>1821</v>
       </c>
       <c r="U150" s="11"/>
       <c r="V150" s="11"/>
@@ -26810,7 +26810,7 @@
         <v>Graz - Summary</v>
       </c>
       <c r="C151" s="12" t="s">
-        <v>1869</v>
+        <v>1822</v>
       </c>
       <c r="D151" s="11"/>
       <c r="E151" s="11"/>
@@ -26819,7 +26819,7 @@
       <c r="H151" s="11"/>
       <c r="I151" s="22"/>
       <c r="J151" s="11" t="s">
-        <v>1937</v>
+        <v>1890</v>
       </c>
       <c r="K151" s="22"/>
       <c r="L151" s="22"/>
@@ -26845,7 +26845,7 @@
         <v>Ghent - Summary</v>
       </c>
       <c r="C152" s="12" t="s">
-        <v>1870</v>
+        <v>1823</v>
       </c>
       <c r="D152" s="11"/>
       <c r="E152" s="11"/>
@@ -26853,7 +26853,7 @@
       <c r="G152" s="12"/>
       <c r="H152" s="11"/>
       <c r="I152" s="22" t="s">
-        <v>1871</v>
+        <v>1824</v>
       </c>
       <c r="J152" s="11"/>
       <c r="K152" s="22"/>
@@ -26880,7 +26880,7 @@
         <v>Bern - Summary</v>
       </c>
       <c r="C153" s="12" t="s">
-        <v>1872</v>
+        <v>1825</v>
       </c>
       <c r="D153" s="11"/>
       <c r="E153" s="11"/>
@@ -26915,7 +26915,7 @@
         <v>Olomouc - Summary</v>
       </c>
       <c r="C154" s="12" t="s">
-        <v>1873</v>
+        <v>1826</v>
       </c>
       <c r="D154" s="11"/>
       <c r="E154" s="11"/>
@@ -26950,7 +26950,7 @@
         <v>Cologne - Summary</v>
       </c>
       <c r="C155" s="12" t="s">
-        <v>1874</v>
+        <v>1827</v>
       </c>
       <c r="D155" s="11"/>
       <c r="E155" s="11"/>
@@ -26985,7 +26985,7 @@
         <v>Odense - Summary</v>
       </c>
       <c r="C156" s="12" t="s">
-        <v>1884</v>
+        <v>1837</v>
       </c>
       <c r="D156" s="11"/>
       <c r="E156" s="11"/>
@@ -27020,10 +27020,10 @@
         <v>Barcelona - Summary</v>
       </c>
       <c r="C157" s="12" t="s">
-        <v>1885</v>
+        <v>1838</v>
       </c>
       <c r="D157" s="11" t="s">
-        <v>1875</v>
+        <v>1828</v>
       </c>
       <c r="E157" s="11"/>
       <c r="F157" s="11"/>
@@ -27057,10 +27057,10 @@
         <v>Valencia - Summary</v>
       </c>
       <c r="C158" s="12" t="s">
-        <v>1876</v>
+        <v>1829</v>
       </c>
       <c r="D158" s="11" t="s">
-        <v>1877</v>
+        <v>1830</v>
       </c>
       <c r="E158" s="11"/>
       <c r="F158" s="11"/>
@@ -27094,10 +27094,10 @@
         <v>Vic - Summary</v>
       </c>
       <c r="C159" s="12" t="s">
-        <v>1886</v>
+        <v>1839</v>
       </c>
       <c r="D159" s="11" t="s">
-        <v>1878</v>
+        <v>1831</v>
       </c>
       <c r="E159" s="11"/>
       <c r="F159" s="11"/>
@@ -27131,7 +27131,7 @@
         <v>Belfast - Summary</v>
       </c>
       <c r="C160" s="12" t="s">
-        <v>1887</v>
+        <v>1840</v>
       </c>
       <c r="D160" s="11"/>
       <c r="E160" s="11"/>
@@ -27164,7 +27164,7 @@
         <v>Lisbon - Summary</v>
       </c>
       <c r="C161" s="12" t="s">
-        <v>1888</v>
+        <v>1841</v>
       </c>
       <c r="D161" s="11"/>
       <c r="E161" s="11"/>
@@ -27180,7 +27180,7 @@
       <c r="O161" s="11"/>
       <c r="P161" s="11"/>
       <c r="Q161" s="11" t="s">
-        <v>1889</v>
+        <v>1842</v>
       </c>
       <c r="R161" s="11"/>
       <c r="S161" s="11"/>
@@ -27197,7 +27197,7 @@
         <v>Adelaide - Summary</v>
       </c>
       <c r="C162" s="12" t="s">
-        <v>1890</v>
+        <v>1843</v>
       </c>
       <c r="D162" s="11"/>
       <c r="E162" s="11"/>
@@ -27230,7 +27230,7 @@
         <v>Melbourne - Summary</v>
       </c>
       <c r="C163" s="12" t="s">
-        <v>1879</v>
+        <v>1832</v>
       </c>
       <c r="D163" s="11"/>
       <c r="E163" s="11"/>
@@ -27263,7 +27263,7 @@
         <v>Sydney - Summary</v>
       </c>
       <c r="C164" s="12" t="s">
-        <v>1880</v>
+        <v>1833</v>
       </c>
       <c r="D164" s="11"/>
       <c r="E164" s="11"/>
@@ -27296,7 +27296,7 @@
         <v>Auckland - Summary</v>
       </c>
       <c r="C165" s="15" t="s">
-        <v>1891</v>
+        <v>1844</v>
       </c>
       <c r="E165" s="11"/>
       <c r="F165" s="11"/>
@@ -27307,7 +27307,7 @@
       <c r="K165" s="22"/>
       <c r="L165" s="22"/>
       <c r="M165" s="22" t="s">
-        <v>1892</v>
+        <v>1845</v>
       </c>
       <c r="N165" s="11"/>
       <c r="O165" s="11"/>
@@ -27347,10 +27347,10 @@
         <v>1264</v>
       </c>
       <c r="J166" s="2" t="s">
-        <v>1941</v>
+        <v>1893</v>
       </c>
       <c r="K166" s="2" t="s">
-        <v>1975</v>
+        <v>1927</v>
       </c>
       <c r="N166" s="2" t="s">
         <v>892</v>
@@ -27465,7 +27465,7 @@
         <v>1673</v>
       </c>
       <c r="G169" s="3" t="s">
-        <v>1946</v>
+        <v>1898</v>
       </c>
       <c r="H169" s="3" t="s">
         <v>1674</v>
@@ -27616,7 +27616,7 @@
         <v>827</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>1895</v>
+        <v>1848</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>1179</v>
@@ -27661,10 +27661,10 @@
         <v>1110</v>
       </c>
       <c r="H2" s="54" t="s">
-        <v>1983</v>
+        <v>1935</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1982</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -27672,13 +27672,13 @@
         <v>186</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1896</v>
+        <v>1849</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>1637</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>1985</v>
+        <v>1937</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>1691</v>
@@ -27702,7 +27702,7 @@
         <v>181</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1897</v>
+        <v>1850</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>891</v>
@@ -27720,7 +27720,7 @@
         <v>1196</v>
       </c>
       <c r="H4" s="54" t="s">
-        <v>1980</v>
+        <v>1932</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>1670</v>
@@ -27731,7 +27731,7 @@
         <v>187</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1898</v>
+        <v>1851</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1120</v>
@@ -27761,22 +27761,22 @@
         <v>188</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1898</v>
+        <v>1851</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>1951</v>
+        <v>1903</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>1948</v>
+        <v>1900</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>1947</v>
+        <v>1899</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>1949</v>
+        <v>1901</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>1947</v>
+        <v>1899</v>
       </c>
       <c r="H6" s="49" t="str">
         <f t="shared" si="0"/>
@@ -27791,10 +27791,10 @@
         <v>189</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>1898</v>
+        <v>1851</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>1950</v>
+        <v>1902</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>1639</v>
@@ -27821,7 +27821,7 @@
         <v>190</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1899</v>
+        <v>1852</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>881</v>
@@ -27851,7 +27851,7 @@
         <v>191</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1900</v>
+        <v>1853</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>1598</v>
@@ -27881,22 +27881,22 @@
         <v>192</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1901</v>
+        <v>1854</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>890</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>1955</v>
+        <v>1907</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>1954</v>
+        <v>1906</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>1955</v>
+        <v>1907</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>1954</v>
+        <v>1906</v>
       </c>
       <c r="H10" s="49" t="str">
         <f t="shared" si="0"/>
@@ -27911,7 +27911,7 @@
         <v>180</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1902</v>
+        <v>1855</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>879</v>
@@ -27941,7 +27941,7 @@
         <v>193</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>1903</v>
+        <v>1856</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1332</v>
@@ -27971,19 +27971,19 @@
         <v>194</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>1904</v>
+        <v>1857</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>884</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>1956</v>
+        <v>1908</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>1110</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>1956</v>
+        <v>1908</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>1110</v>
@@ -28001,7 +28001,7 @@
         <v>195</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1905</v>
+        <v>1858</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>887</v>
@@ -28031,19 +28031,19 @@
         <v>196</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>1906</v>
+        <v>1859</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>886</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>1956</v>
+        <v>1908</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>1110</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>1956</v>
+        <v>1908</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>1110</v>
@@ -28061,7 +28061,7 @@
         <v>197</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>1907</v>
+        <v>1860</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>1707</v>
@@ -28091,17 +28091,17 @@
         <v>198</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>1908</v>
+        <v>1861</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>885</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>1956</v>
+        <v>1908</v>
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="20" t="s">
-        <v>1956</v>
+        <v>1908</v>
       </c>
       <c r="G17" s="20" t="s">
         <v>1110</v>
@@ -28119,7 +28119,7 @@
         <v>199</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>1909</v>
+        <v>1862</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>888</v>
@@ -28137,7 +28137,7 @@
         <v>1687</v>
       </c>
       <c r="H18" s="54" t="s">
-        <v>1984</v>
+        <v>1936</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>1670</v>
@@ -28148,7 +28148,7 @@
         <v>200</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>1910</v>
+        <v>1863</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>1122</v>
@@ -28178,19 +28178,19 @@
         <v>201</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>1910</v>
+        <v>1863</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>1121</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>1957</v>
+        <v>1909</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>1195</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>1957</v>
+        <v>1909</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>1195</v>
@@ -28208,7 +28208,7 @@
         <v>202</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>1910</v>
+        <v>1863</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>1122</v>
@@ -28238,7 +28238,7 @@
         <v>203</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>1911</v>
+        <v>1864</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>889</v>
@@ -28260,7 +28260,7 @@
         <v>https://doi.org/INSERT-Belfast-DOI-HERE</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>1959</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -28268,7 +28268,7 @@
         <v>204</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>1912</v>
+        <v>1865</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>894</v>
@@ -28298,7 +28298,7 @@
         <v>205</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>1913</v>
+        <v>1866</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>882</v>
@@ -28320,7 +28320,7 @@
         <v>178</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>1913</v>
+        <v>1866</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>882</v>
@@ -28350,7 +28350,7 @@
         <v>206</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>1913</v>
+        <v>1866</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>882</v>
@@ -28380,7 +28380,7 @@
         <v>207</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>1914</v>
+        <v>1867</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>883</v>
@@ -28998,7 +28998,7 @@
         <v>836</v>
       </c>
       <c r="L4" s="42" t="s">
-        <v>1958</v>
+        <v>1910</v>
       </c>
       <c r="M4" s="38" t="s">
         <v>836</v>
@@ -29493,7 +29493,7 @@
         <v>836</v>
       </c>
       <c r="S11" s="42" t="s">
-        <v>1958</v>
+        <v>1910</v>
       </c>
       <c r="T11" s="39" t="s">
         <v>836</v>

</xml_diff>

<commit_message>
added in figshare uploader template files, and added in report DOIs for each city to the configuration file
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/analysis/global_scorecards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2388" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5FC42B7-375A-43CE-A1F9-0ACC14299CFE}"/>
+  <xr:revisionPtr revIDLastSave="2420" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FCFA11F-1782-4A18-B490-611DF85D325B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4117" uniqueCount="1994">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4140" uniqueCount="2017">
   <si>
     <t>name</t>
   </si>
@@ -5928,21 +5928,12 @@
     <t>eceaf8</t>
   </si>
   <si>
-    <t>https://doi.org/10.25439/rmt.19586770</t>
-  </si>
-  <si>
     <t>citation_doi</t>
   </si>
   <si>
     <t>{"study_citations":"||The Lancet Global Health. May 2022. Volume 10. Special Issue 2 - The Global Healthy &amp; Sustainable City-Indicators Study. S1-S5. Available at {study_doi}.","citation_doi":"Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally ({language}). {city_doi}","citations":"{citation_series}: {study_citations}||{citation_population}: Schiavina, M. et al. (2019): GHS population grid multitemporal (1975, 1990, 2000, 2015) R2019A. European Commission, Joint Research Centre (JRC). https://doi.org/10.2905/42E8BE89-54FF-464E-BE7B-BF9E64DA5218 |{citation_boundaries}: Florczyk, A. et al. (2019): GHS Urban Centre Database 2015, multitemporal and multidimensional attributes, R2019A. European Commission, Joint Research Centre (JRC). https://data.jrc.ec.europa.eu/dataset/53473144-b88c-44bc-b4a3-4583ed1f547e |{citation_features}: OpenStreetMap contributors. Openstreetmap (2020). https://planet.osm.org/pbf/planet-200803.osm.pbf.torrent |{citation_colour}: Crameri, F. (2018). Scientific colour-maps (3.0.4). Zenodo. https://doi.org/10.5281/zenodo.1287763"}</t>
   </si>
   <si>
-    <t>https://doi.org/STUDY-DOI-TBA</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.25439/rmt.19586767</t>
-  </si>
-  <si>
     <t>Tricycle taxis, Cyclists and Pedestrians, Maiduguri, Nigeria</t>
   </si>
   <si>
@@ -6133,6 +6124,84 @@
   </si>
   <si>
     <t>La disponibilidad y calidad de las políticas urbanas y de transporte que apoyan la salud y la sostenibilidad en la Ciudad de México (CDMX) está justo por debajo del promedio en comparación con otras ciudades. La política de transporte metropolitano de la CDMX no parece tener acciones específicas centradas en la salud, ni requisitos para la evaluación de impacto de las intervenciones urbanas o de transporte en la salud pública. También carece de políticas de contaminación del aire relacionadas con el uso de suelo. Muchos de los estándares de políticas disponibles carecen de especificidad, mensurabilidad y/o consistencia con la evidencia de salud pública. No obstante, en relación con las 25 ciudades de este estudio internacional, la mayoría de las colonias de la ciudad son caminables. En cuanto a los umbrales para las intervenciones en el entorno construido, para lograr los objetivos de la OMS de aumentar la actividad física, el 98.1% de los residentes de la CDMX vive en colonias que alcanzan el umbral de densidad mínima y el 77% alcanza el umbral de conectividad de calles. Sin embargo, muchos de sus residentes viven en colonias que superan los niveles de densidad y conectividad de calles que fomentan la actividad física. Solo el 20% de los residentes tiene acceso a paradas de transporte público con servicios regulares, con evidencia de que el acceso a este tiene un patrón espacial que favorece al centro de la ciudad. Solo el 50% de los residentes tiene acceso a algún espacio público abierto a 500 m, o menos, y aún menos (20%) tiene acceso a un espacio público grande. La proporción de la población con acceso a servicios a 500 m, o menos, está por debajo del promedio en comparación con otras ciudades estudiadas.</t>
+  </si>
+  <si>
+    <t>STUDY-DOI-TBA</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19586770</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19586767</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614009</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614012</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614078</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614075</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614072</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614069</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614066</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614063</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614060</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614057</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614054</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614051</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614048</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614045</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614039</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614036</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614033</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614030</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614027</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614024</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614021</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614018</t>
+  </si>
+  <si>
+    <t>10.25439/rmt.19614015</t>
   </si>
 </sst>
 </file>
@@ -6873,7 +6942,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -7027,9 +7096,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -9796,7 +9862,7 @@
         <v>28</v>
       </c>
       <c r="P38" s="5" t="s">
-        <v>1935</v>
+        <v>1932</v>
       </c>
       <c r="Q38">
         <v>3</v>
@@ -9860,7 +9926,7 @@
         <v>28</v>
       </c>
       <c r="P39" s="5" t="s">
-        <v>1939</v>
+        <v>1936</v>
       </c>
       <c r="Q39">
         <v>3</v>
@@ -10110,7 +10176,7 @@
         <v>28</v>
       </c>
       <c r="P43" s="5" t="s">
-        <v>1935</v>
+        <v>1932</v>
       </c>
       <c r="Q43">
         <v>3</v>
@@ -10174,7 +10240,7 @@
         <v>28</v>
       </c>
       <c r="P44" s="5" t="s">
-        <v>1938</v>
+        <v>1935</v>
       </c>
       <c r="Q44">
         <v>3</v>
@@ -10424,7 +10490,7 @@
         <v>28</v>
       </c>
       <c r="P48" s="5" t="s">
-        <v>1937</v>
+        <v>1934</v>
       </c>
       <c r="Q48">
         <v>3</v>
@@ -10488,7 +10554,7 @@
         <v>28</v>
       </c>
       <c r="P49" s="5" t="s">
-        <v>1936</v>
+        <v>1933</v>
       </c>
       <c r="Q49">
         <v>3</v>
@@ -10738,7 +10804,7 @@
         <v>28</v>
       </c>
       <c r="P53" s="5" t="s">
-        <v>1932</v>
+        <v>1929</v>
       </c>
       <c r="Q53">
         <v>3</v>
@@ -10802,7 +10868,7 @@
         <v>28</v>
       </c>
       <c r="P54" s="5" t="s">
-        <v>1934</v>
+        <v>1931</v>
       </c>
       <c r="Q54">
         <v>3</v>
@@ -11052,7 +11118,7 @@
         <v>28</v>
       </c>
       <c r="P58" s="5" t="s">
-        <v>1932</v>
+        <v>1929</v>
       </c>
       <c r="Q58">
         <v>3</v>
@@ -11116,7 +11182,7 @@
         <v>28</v>
       </c>
       <c r="P59" s="5" t="s">
-        <v>1933</v>
+        <v>1930</v>
       </c>
       <c r="Q59">
         <v>3</v>
@@ -11366,7 +11432,7 @@
         <v>28</v>
       </c>
       <c r="P63" s="5" t="s">
-        <v>1932</v>
+        <v>1929</v>
       </c>
       <c r="Q63">
         <v>3</v>
@@ -11430,7 +11496,7 @@
         <v>28</v>
       </c>
       <c r="P64" s="5" t="s">
-        <v>1931</v>
+        <v>1928</v>
       </c>
       <c r="Q64">
         <v>3</v>
@@ -18916,7 +18982,7 @@
     </row>
     <row r="192" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="B192">
         <v>6</v>
@@ -19162,11 +19228,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V170"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22430,56 +22496,56 @@
         <v>585</v>
       </c>
       <c r="C76" s="10" t="s">
+        <v>1937</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>1938</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>1939</v>
+      </c>
+      <c r="F76" s="9" t="s">
         <v>1940</v>
       </c>
-      <c r="D76" s="9" t="s">
+      <c r="G76" s="10" t="s">
         <v>1941</v>
       </c>
-      <c r="E76" s="9" t="s">
+      <c r="H76" s="9" t="s">
         <v>1942</v>
       </c>
-      <c r="F76" s="9" t="s">
+      <c r="I76" s="22" t="s">
         <v>1943</v>
       </c>
-      <c r="G76" s="10" t="s">
+      <c r="J76" s="9" t="s">
         <v>1944</v>
       </c>
-      <c r="H76" s="9" t="s">
+      <c r="K76" s="22" t="s">
         <v>1945</v>
-      </c>
-      <c r="I76" s="22" t="s">
-        <v>1946</v>
-      </c>
-      <c r="J76" s="9" t="s">
-        <v>1947</v>
-      </c>
-      <c r="K76" s="22" t="s">
-        <v>1948</v>
       </c>
       <c r="L76" s="22"/>
       <c r="M76" s="22" t="s">
+        <v>1946</v>
+      </c>
+      <c r="N76" s="9" t="s">
+        <v>1947</v>
+      </c>
+      <c r="O76" s="11" t="s">
+        <v>1948</v>
+      </c>
+      <c r="P76" s="9" t="s">
         <v>1949</v>
       </c>
-      <c r="N76" s="9" t="s">
+      <c r="Q76" s="9" t="s">
         <v>1950</v>
       </c>
-      <c r="O76" s="11" t="s">
+      <c r="R76" s="9" t="s">
         <v>1951</v>
-      </c>
-      <c r="P76" s="9" t="s">
-        <v>1952</v>
-      </c>
-      <c r="Q76" s="9" t="s">
-        <v>1953</v>
-      </c>
-      <c r="R76" s="9" t="s">
-        <v>1954</v>
       </c>
       <c r="S76" s="9" t="s">
         <v>1782</v>
       </c>
       <c r="T76" s="9" t="s">
-        <v>1955</v>
+        <v>1952</v>
       </c>
       <c r="U76" s="9"/>
       <c r="V76" s="9"/>
@@ -22492,56 +22558,56 @@
         <v>586</v>
       </c>
       <c r="C77" s="10" t="s">
+        <v>1953</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>1954</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>1955</v>
+      </c>
+      <c r="F77" s="9" t="s">
         <v>1956</v>
       </c>
-      <c r="D77" s="9" t="s">
+      <c r="G77" s="10" t="s">
         <v>1957</v>
       </c>
-      <c r="E77" s="9" t="s">
+      <c r="H77" s="9" t="s">
         <v>1958</v>
       </c>
-      <c r="F77" s="9" t="s">
+      <c r="I77" s="22" t="s">
         <v>1959</v>
       </c>
-      <c r="G77" s="10" t="s">
+      <c r="J77" s="9" t="s">
         <v>1960</v>
       </c>
-      <c r="H77" s="9" t="s">
+      <c r="K77" s="22" t="s">
         <v>1961</v>
-      </c>
-      <c r="I77" s="22" t="s">
-        <v>1962</v>
-      </c>
-      <c r="J77" s="9" t="s">
-        <v>1963</v>
-      </c>
-      <c r="K77" s="22" t="s">
-        <v>1964</v>
       </c>
       <c r="L77" s="22"/>
       <c r="M77" s="22" t="s">
+        <v>1962</v>
+      </c>
+      <c r="N77" s="9" t="s">
+        <v>1963</v>
+      </c>
+      <c r="O77" s="11" t="s">
+        <v>1964</v>
+      </c>
+      <c r="P77" s="9" t="s">
         <v>1965</v>
       </c>
-      <c r="N77" s="9" t="s">
+      <c r="Q77" s="9" t="s">
         <v>1966</v>
       </c>
-      <c r="O77" s="11" t="s">
+      <c r="R77" s="9" t="s">
         <v>1967</v>
-      </c>
-      <c r="P77" s="9" t="s">
-        <v>1968</v>
-      </c>
-      <c r="Q77" s="9" t="s">
-        <v>1969</v>
-      </c>
-      <c r="R77" s="9" t="s">
-        <v>1970</v>
       </c>
       <c r="S77" s="9" t="s">
         <v>1783</v>
       </c>
       <c r="T77" s="9" t="s">
-        <v>1971</v>
+        <v>1968</v>
       </c>
       <c r="U77" s="9"/>
       <c r="V77" s="9"/>
@@ -22554,56 +22620,56 @@
         <v>584</v>
       </c>
       <c r="C78" s="10" t="s">
+        <v>1969</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>1970</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>1971</v>
+      </c>
+      <c r="F78" s="9" t="s">
         <v>1972</v>
       </c>
-      <c r="D78" s="9" t="s">
+      <c r="G78" s="10" t="s">
         <v>1973</v>
       </c>
-      <c r="E78" s="9" t="s">
+      <c r="H78" s="9" t="s">
         <v>1974</v>
       </c>
-      <c r="F78" s="9" t="s">
+      <c r="I78" s="22" t="s">
         <v>1975</v>
       </c>
-      <c r="G78" s="10" t="s">
+      <c r="J78" s="9" t="s">
         <v>1976</v>
       </c>
-      <c r="H78" s="9" t="s">
+      <c r="K78" s="22" t="s">
         <v>1977</v>
-      </c>
-      <c r="I78" s="22" t="s">
-        <v>1978</v>
-      </c>
-      <c r="J78" s="9" t="s">
-        <v>1979</v>
-      </c>
-      <c r="K78" s="22" t="s">
-        <v>1980</v>
       </c>
       <c r="L78" s="22"/>
       <c r="M78" s="22" t="s">
+        <v>1978</v>
+      </c>
+      <c r="N78" s="9" t="s">
+        <v>1979</v>
+      </c>
+      <c r="O78" s="9" t="s">
+        <v>1980</v>
+      </c>
+      <c r="P78" s="9" t="s">
         <v>1981</v>
       </c>
-      <c r="N78" s="9" t="s">
+      <c r="Q78" s="9" t="s">
         <v>1982</v>
       </c>
-      <c r="O78" s="9" t="s">
+      <c r="R78" s="9" t="s">
         <v>1983</v>
-      </c>
-      <c r="P78" s="9" t="s">
-        <v>1984</v>
-      </c>
-      <c r="Q78" s="9" t="s">
-        <v>1985</v>
-      </c>
-      <c r="R78" s="9" t="s">
-        <v>1986</v>
       </c>
       <c r="S78" s="9" t="s">
         <v>1781</v>
       </c>
       <c r="T78" s="9" t="s">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="U78" s="9"/>
       <c r="V78" s="9"/>
@@ -23205,7 +23271,7 @@
         <v>639</v>
       </c>
       <c r="N88" s="11" t="s">
-        <v>1988</v>
+        <v>1985</v>
       </c>
       <c r="O88" s="11" t="s">
         <v>809</v>
@@ -24135,7 +24201,7 @@
         <v>650</v>
       </c>
       <c r="N103" s="11" t="s">
-        <v>1989</v>
+        <v>1986</v>
       </c>
       <c r="O103" s="11" t="s">
         <v>813</v>
@@ -24383,7 +24449,7 @@
         <v>654</v>
       </c>
       <c r="N107" s="11" t="s">
-        <v>1990</v>
+        <v>1987</v>
       </c>
       <c r="O107" s="14" t="s">
         <v>914</v>
@@ -25499,7 +25565,7 @@
         <v>669</v>
       </c>
       <c r="N125" s="11" t="s">
-        <v>1991</v>
+        <v>1988</v>
       </c>
       <c r="O125" s="14" t="s">
         <v>923</v>
@@ -25809,7 +25875,7 @@
         <v>674</v>
       </c>
       <c r="N130" s="11" t="s">
-        <v>1992</v>
+        <v>1989</v>
       </c>
       <c r="O130" s="14" t="s">
         <v>925</v>
@@ -26509,7 +26575,7 @@
       <c r="L142" s="22"/>
       <c r="M142" s="22"/>
       <c r="N142" s="11" t="s">
-        <v>1993</v>
+        <v>1990</v>
       </c>
       <c r="O142" s="11"/>
       <c r="P142" s="11"/>
@@ -27589,11 +27655,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CAA5C4-0A70-4221-8832-C196189F112B}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27657,11 +27723,11 @@
       <c r="G2" s="18" t="s">
         <v>1104</v>
       </c>
-      <c r="H2" s="54" t="s">
-        <v>1928</v>
+      <c r="H2" s="49" t="s">
+        <v>1991</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -27675,7 +27741,7 @@
         <v>1631</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>1930</v>
+        <v>1927</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>1685</v>
@@ -27686,9 +27752,8 @@
       <c r="G3" s="20" t="s">
         <v>1685</v>
       </c>
-      <c r="H3" s="49" t="str">
-        <f>"https://doi.org/INSERT-"&amp;A3&amp;"-DOI-HERE"</f>
-        <v>https://doi.org/INSERT-Maiduguri-DOI-HERE</v>
+      <c r="H3" s="49" t="s">
+        <v>2004</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>1664</v>
@@ -27716,8 +27781,8 @@
       <c r="G4" s="20" t="s">
         <v>1190</v>
       </c>
-      <c r="H4" s="54" t="s">
-        <v>1925</v>
+      <c r="H4" s="49" t="s">
+        <v>1992</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>1664</v>
@@ -27745,9 +27810,8 @@
       <c r="G5" s="20" t="s">
         <v>1191</v>
       </c>
-      <c r="H5" s="49" t="str">
-        <f t="shared" ref="H5:H27" si="0">"https://doi.org/INSERT-"&amp;A5&amp;"-DOI-HERE"</f>
-        <v>https://doi.org/INSERT-Baltimore-DOI-HERE</v>
+      <c r="H5" s="49" t="s">
+        <v>2016</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>1664</v>
@@ -27775,9 +27839,8 @@
       <c r="G6" s="52" t="s">
         <v>1892</v>
       </c>
-      <c r="H6" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Phoenix-DOI-HERE</v>
+      <c r="H6" s="49" t="s">
+        <v>2001</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>1664</v>
@@ -27805,9 +27868,8 @@
       <c r="G7" s="20" t="s">
         <v>1628</v>
       </c>
-      <c r="H7" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Seattle-DOI-HERE</v>
+      <c r="H7" s="49" t="s">
+        <v>1999</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>1650</v>
@@ -27835,9 +27897,8 @@
       <c r="G8" s="20" t="s">
         <v>1635</v>
       </c>
-      <c r="H8" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Sao Paulo-DOI-HERE</v>
+      <c r="H8" s="49" t="s">
+        <v>2000</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>1664</v>
@@ -27865,9 +27926,8 @@
       <c r="G9" s="20" t="s">
         <v>1593</v>
       </c>
-      <c r="H9" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Hong Kong-DOI-HERE</v>
+      <c r="H9" s="49" t="s">
+        <v>2006</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>1665</v>
@@ -27895,9 +27955,8 @@
       <c r="G10" s="20" t="s">
         <v>1899</v>
       </c>
-      <c r="H10" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Chennai-DOI-HERE</v>
+      <c r="H10" s="49" t="s">
+        <v>2011</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>1664</v>
@@ -27925,9 +27984,8 @@
       <c r="G11" s="20" t="s">
         <v>1192</v>
       </c>
-      <c r="H11" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Bangkok-DOI-HERE</v>
+      <c r="H11" s="49" t="s">
+        <v>2015</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>1664</v>
@@ -27955,9 +28013,8 @@
       <c r="G12" s="20" t="s">
         <v>1315</v>
       </c>
-      <c r="H12" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Hanoi-DOI-HERE</v>
+      <c r="H12" s="49" t="s">
+        <v>2007</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>1664</v>
@@ -27985,9 +28042,8 @@
       <c r="G13" s="20" t="s">
         <v>1104</v>
       </c>
-      <c r="H13" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Graz-DOI-HERE</v>
+      <c r="H13" s="49" t="s">
+        <v>2008</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>1664</v>
@@ -28015,9 +28071,8 @@
       <c r="G14" s="20" t="s">
         <v>1684</v>
       </c>
-      <c r="H14" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Ghent-DOI-HERE</v>
+      <c r="H14" s="49" t="s">
+        <v>2009</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>1664</v>
@@ -28045,9 +28100,8 @@
       <c r="G15" s="20" t="s">
         <v>1104</v>
       </c>
-      <c r="H15" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Bern-DOI-HERE</v>
+      <c r="H15" s="49" t="s">
+        <v>2012</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>1664</v>
@@ -28075,9 +28129,8 @@
       <c r="G16" s="20" t="s">
         <v>1549</v>
       </c>
-      <c r="H16" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Olomouc-DOI-HERE</v>
+      <c r="H16" s="49" t="s">
+        <v>2002</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>1664</v>
@@ -28103,9 +28156,8 @@
       <c r="G17" s="20" t="s">
         <v>1104</v>
       </c>
-      <c r="H17" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Cologne-DOI-HERE</v>
+      <c r="H17" s="49" t="s">
+        <v>2010</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>1664</v>
@@ -28133,8 +28185,8 @@
       <c r="G18" s="31" t="s">
         <v>1681</v>
       </c>
-      <c r="H18" s="54" t="s">
-        <v>1929</v>
+      <c r="H18" s="49" t="s">
+        <v>1993</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>1664</v>
@@ -28162,9 +28214,8 @@
       <c r="G19" s="20" t="s">
         <v>1181</v>
       </c>
-      <c r="H19" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Barcelona-DOI-HERE</v>
+      <c r="H19" s="49" t="s">
+        <v>2014</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>1664</v>
@@ -28192,9 +28243,8 @@
       <c r="G20" s="20" t="s">
         <v>1189</v>
       </c>
-      <c r="H20" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Valencia-DOI-HERE</v>
+      <c r="H20" s="49" t="s">
+        <v>1997</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>1664</v>
@@ -28222,9 +28272,8 @@
       <c r="G21" s="20" t="s">
         <v>1573</v>
       </c>
-      <c r="H21" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Vic-DOI-HERE</v>
+      <c r="H21" s="49" t="s">
+        <v>1996</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>1664</v>
@@ -28252,9 +28301,8 @@
       <c r="G22" s="20" t="s">
         <v>1184</v>
       </c>
-      <c r="H22" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Belfast-DOI-HERE</v>
+      <c r="H22" s="49" t="s">
+        <v>2013</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>1904</v>
@@ -28282,9 +28330,8 @@
       <c r="G23" s="20" t="s">
         <v>1565</v>
       </c>
-      <c r="H23" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Lisbon-DOI-HERE</v>
+      <c r="H23" s="49" t="s">
+        <v>2005</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>1664</v>
@@ -28304,9 +28351,8 @@
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="32"/>
-      <c r="H24" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Adelaide-DOI-HERE</v>
+      <c r="H24" s="49" t="s">
+        <v>1994</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>1664</v>
@@ -28334,9 +28380,8 @@
       <c r="G25" s="20" t="s">
         <v>1312</v>
       </c>
-      <c r="H25" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Melbourne-DOI-HERE</v>
+      <c r="H25" s="49" t="s">
+        <v>2003</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>1664</v>
@@ -28364,9 +28409,8 @@
       <c r="G26" s="20" t="s">
         <v>1553</v>
       </c>
-      <c r="H26" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Sydney-DOI-HERE</v>
+      <c r="H26" s="49" t="s">
+        <v>1998</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>1664</v>
@@ -28394,22 +28438,16 @@
       <c r="G27" s="20" t="s">
         <v>1567</v>
       </c>
-      <c r="H27" s="49" t="str">
-        <f t="shared" si="0"/>
-        <v>https://doi.org/INSERT-Auckland-DOI-HERE</v>
+      <c r="H27" s="49" t="s">
+        <v>1995</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>1664</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" xr:uid="{CB394B5B-C4DB-4076-96B4-D5346757EC3D}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{FE22C84B-E880-493B-BEF3-4C05A4D959BC}"/>
-    <hyperlink ref="H18" r:id="rId3" xr:uid="{D1C02A08-CA8B-49B7-8462-F1392E7E9DEE}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -28876,30 +28914,30 @@
       <c r="C2" s="33" t="s">
         <v>825</v>
       </c>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="54" t="s">
         <v>826</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="54" t="s">
         <v>1334</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="56" t="s">
         <v>827</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
       <c r="V2" s="24" t="s">
         <v>828</v>
       </c>
@@ -28908,8 +28946,8 @@
       <c r="A3" s="25"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
       <c r="F3" s="26" t="s">
         <v>829</v>
       </c>

</xml_diff>

<commit_message>
implemented saving to sub-folders by city, as optional alternative to saving by language (issue #13)
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/analysis/global_scorecards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2472" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{291E6DD3-DFA3-4515-BD6E-F9402A7F4456}"/>
+  <xr:revisionPtr revIDLastSave="2480" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36533413-6A2D-4C7F-BB8C-198AF3574B8C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
@@ -7601,11 +7601,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V195"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M37" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B172" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P63" sqref="P63"/>
+      <selection pane="bottomRight" activeCell="N195" sqref="N195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28842,10 +28842,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0E5A34-E8C6-471F-BB3C-81719394AD1E}">
-  <dimension ref="A2:V28"/>
+  <dimension ref="A2:V29"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30637,6 +30637,12 @@
         <v>824</v>
       </c>
       <c r="V28" s="47"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V29" s="2" t="str">
+        <f>COUNTIF(F4:U28,"Yes")&amp;"/"&amp;COUNTIF(F4:U28,"&lt;&gt;-")&amp;" reports for "&amp;COUNTA(A4:A28)&amp;" cities across "&amp;COUNTA(F3:U3)&amp;" languages"</f>
+        <v>43/47 reports for 25 cities across 16 languages</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
updated citation placeholder for series, and added new 'by_language' argument which is True by default -- but allows for optional simultaneous output both by city and by language (as per issue #13)
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/analysis/global_scorecards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2483" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A1E63B7-3531-4BD4-94DC-260245FDA093}"/>
+  <xr:revisionPtr revIDLastSave="2488" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41CBDCD9-C2AD-4CB9-9C25-F93E03246FDC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4106" uniqueCount="2003">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4108" uniqueCount="2005">
   <si>
     <t>name</t>
   </si>
@@ -6160,6 +6160,12 @@
   </si>
   <si>
     <t>{"study_citations":"||The Lancet Global Health. May 2022. Volume 10. Special Issue 2 - Urban Design, Transport and Health. S1-S5. Available at {study_doi}.","citation_doi":"Global Healthy &amp; Sustainable City-Indicators Collaboration. 2022. {city}, {country}—Healthy and Sustainable City Indicators Report: Comparisons with 25 cities internationally ({language}). {city_doi}","citations":"{citation_series}: {study_citations}||{citation_population}: Schiavina, M. et al. (2019): GHS population grid multitemporal (1975, 1990, 2000, 2015) R2019A. European Commission, Joint Research Centre (JRC). https://doi.org/10.2905/42E8BE89-54FF-464E-BE7B-BF9E64DA5218 |{citation_boundaries}: Florczyk, A. et al. (2019): GHS Urban Centre Database 2015, multitemporal and multidimensional attributes, R2019A. European Commission, Joint Research Centre (JRC). https://data.jrc.ec.europa.eu/dataset/53473144-b88c-44bc-b4a3-4583ed1f547e |{citation_features}: OpenStreetMap contributors. Openstreetmap (2020). https://planet.osm.org/pbf/planet-200803.osm.pbf.torrent |{citation_colour}: Crameri, F. (2018). Scientific colour-maps (3.0.4). Zenodo. https://doi.org/10.5281/zenodo.1287763"}</t>
+  </si>
+  <si>
+    <t>© 2016 Jack Alexander (@jackalexander_) on Unsplash</t>
+  </si>
+  <si>
+    <t>Orange cyclist, Rundle Street, Adelaide, Australia</t>
   </si>
 </sst>
 </file>
@@ -6900,7 +6906,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6989,9 +6995,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -19822,7 +19825,7 @@
       <c r="Q14" s="11" t="s">
         <v>1094</v>
       </c>
-      <c r="R14" s="51" t="s">
+      <c r="R14" s="50" t="s">
         <v>363</v>
       </c>
       <c r="S14" s="11"/>
@@ -27592,10 +27595,10 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27659,7 +27662,7 @@
       <c r="G2" s="18" t="s">
         <v>1094</v>
       </c>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="48" t="s">
         <v>1951</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -27688,7 +27691,7 @@
       <c r="G3" s="20" t="s">
         <v>1660</v>
       </c>
-      <c r="H3" s="49" t="s">
+      <c r="H3" s="48" t="s">
         <v>1964</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -27717,7 +27720,7 @@
       <c r="G4" s="20" t="s">
         <v>1179</v>
       </c>
-      <c r="H4" s="49" t="s">
+      <c r="H4" s="48" t="s">
         <v>1952</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -27746,7 +27749,7 @@
       <c r="G5" s="20" t="s">
         <v>1180</v>
       </c>
-      <c r="H5" s="49" t="s">
+      <c r="H5" s="48" t="s">
         <v>1976</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -27766,16 +27769,16 @@
       <c r="D6" s="20" t="s">
         <v>1865</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="51" t="s">
         <v>1864</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>1866</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="G6" s="51" t="s">
         <v>1864</v>
       </c>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="48" t="s">
         <v>1961</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -27804,7 +27807,7 @@
       <c r="G7" s="20" t="s">
         <v>1603</v>
       </c>
-      <c r="H7" s="49" t="s">
+      <c r="H7" s="48" t="s">
         <v>1959</v>
       </c>
       <c r="I7" s="3" t="s">
@@ -27833,7 +27836,7 @@
       <c r="G8" s="20" t="s">
         <v>1610</v>
       </c>
-      <c r="H8" s="49" t="s">
+      <c r="H8" s="48" t="s">
         <v>1960</v>
       </c>
       <c r="I8" s="2" t="s">
@@ -27862,7 +27865,7 @@
       <c r="G9" s="20" t="s">
         <v>1571</v>
       </c>
-      <c r="H9" s="49" t="s">
+      <c r="H9" s="48" t="s">
         <v>1966</v>
       </c>
       <c r="I9" s="3" t="s">
@@ -27891,7 +27894,7 @@
       <c r="G10" s="20" t="s">
         <v>1871</v>
       </c>
-      <c r="H10" s="49" t="s">
+      <c r="H10" s="48" t="s">
         <v>1971</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -27920,7 +27923,7 @@
       <c r="G11" s="20" t="s">
         <v>1181</v>
       </c>
-      <c r="H11" s="49" t="s">
+      <c r="H11" s="48" t="s">
         <v>1975</v>
       </c>
       <c r="I11" s="2" t="s">
@@ -27949,7 +27952,7 @@
       <c r="G12" s="20" t="s">
         <v>1303</v>
       </c>
-      <c r="H12" s="49" t="s">
+      <c r="H12" s="48" t="s">
         <v>1967</v>
       </c>
       <c r="I12" s="2" t="s">
@@ -27978,7 +27981,7 @@
       <c r="G13" s="20" t="s">
         <v>1094</v>
       </c>
-      <c r="H13" s="49" t="s">
+      <c r="H13" s="48" t="s">
         <v>1968</v>
       </c>
       <c r="I13" s="2" t="s">
@@ -28007,7 +28010,7 @@
       <c r="G14" s="20" t="s">
         <v>1659</v>
       </c>
-      <c r="H14" s="49" t="s">
+      <c r="H14" s="48" t="s">
         <v>1969</v>
       </c>
       <c r="I14" s="2" t="s">
@@ -28036,7 +28039,7 @@
       <c r="G15" s="20" t="s">
         <v>1094</v>
       </c>
-      <c r="H15" s="49" t="s">
+      <c r="H15" s="48" t="s">
         <v>1972</v>
       </c>
       <c r="I15" s="2" t="s">
@@ -28065,7 +28068,7 @@
       <c r="G16" s="20" t="s">
         <v>1529</v>
       </c>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="48" t="s">
         <v>1962</v>
       </c>
       <c r="I16" s="2" t="s">
@@ -28092,7 +28095,7 @@
       <c r="G17" s="20" t="s">
         <v>1094</v>
       </c>
-      <c r="H17" s="49" t="s">
+      <c r="H17" s="48" t="s">
         <v>1970</v>
       </c>
       <c r="I17" s="2" t="s">
@@ -28121,7 +28124,7 @@
       <c r="G18" s="31" t="s">
         <v>1656</v>
       </c>
-      <c r="H18" s="49" t="s">
+      <c r="H18" s="48" t="s">
         <v>1953</v>
       </c>
       <c r="I18" s="2" t="s">
@@ -28150,7 +28153,7 @@
       <c r="G19" s="20" t="s">
         <v>1170</v>
       </c>
-      <c r="H19" s="49" t="s">
+      <c r="H19" s="48" t="s">
         <v>1974</v>
       </c>
       <c r="I19" s="2" t="s">
@@ -28179,7 +28182,7 @@
       <c r="G20" s="20" t="s">
         <v>1178</v>
       </c>
-      <c r="H20" s="49" t="s">
+      <c r="H20" s="48" t="s">
         <v>1957</v>
       </c>
       <c r="I20" s="2" t="s">
@@ -28208,7 +28211,7 @@
       <c r="G21" s="20" t="s">
         <v>1552</v>
       </c>
-      <c r="H21" s="49" t="s">
+      <c r="H21" s="48" t="s">
         <v>1956</v>
       </c>
       <c r="I21" s="2" t="s">
@@ -28237,7 +28240,7 @@
       <c r="G22" s="20" t="s">
         <v>1173</v>
       </c>
-      <c r="H22" s="49" t="s">
+      <c r="H22" s="48" t="s">
         <v>1973</v>
       </c>
       <c r="I22" s="3" t="s">
@@ -28266,14 +28269,14 @@
       <c r="G23" s="20" t="s">
         <v>1545</v>
       </c>
-      <c r="H23" s="49" t="s">
+      <c r="H23" s="48" t="s">
         <v>1965</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>1639</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>205</v>
       </c>
@@ -28285,9 +28288,13 @@
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="49" t="s">
+      <c r="F24" s="20" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>2003</v>
+      </c>
+      <c r="H24" s="48" t="s">
         <v>1954</v>
       </c>
       <c r="I24" s="2" t="s">
@@ -28316,7 +28323,7 @@
       <c r="G25" s="20" t="s">
         <v>1300</v>
       </c>
-      <c r="H25" s="49" t="s">
+      <c r="H25" s="48" t="s">
         <v>1963</v>
       </c>
       <c r="I25" s="2" t="s">
@@ -28345,7 +28352,7 @@
       <c r="G26" s="20" t="s">
         <v>1533</v>
       </c>
-      <c r="H26" s="49" t="s">
+      <c r="H26" s="48" t="s">
         <v>1958</v>
       </c>
       <c r="I26" s="2" t="s">
@@ -28374,7 +28381,7 @@
       <c r="G27" s="20" t="s">
         <v>1547</v>
       </c>
-      <c r="H27" s="49" t="s">
+      <c r="H27" s="48" t="s">
         <v>1955</v>
       </c>
       <c r="I27" s="2" t="s">
@@ -28438,7 +28445,7 @@
       <c r="E2" t="s">
         <v>575</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="49" t="s">
         <v>1721</v>
       </c>
     </row>
@@ -28458,7 +28465,7 @@
       <c r="E3" t="s">
         <v>141</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="49" t="s">
         <v>1721</v>
       </c>
     </row>
@@ -28478,7 +28485,7 @@
       <c r="E4" t="s">
         <v>142</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="49" t="s">
         <v>1721</v>
       </c>
     </row>
@@ -28498,7 +28505,7 @@
       <c r="E5" t="s">
         <v>143</v>
       </c>
-      <c r="F5" s="50" t="s">
+      <c r="F5" s="49" t="s">
         <v>1721</v>
       </c>
     </row>
@@ -28515,7 +28522,7 @@
       <c r="E6" t="s">
         <v>1088</v>
       </c>
-      <c r="F6" s="50" t="s">
+      <c r="F6" s="49" t="s">
         <v>1720</v>
       </c>
     </row>
@@ -28535,7 +28542,7 @@
       <c r="E7" t="s">
         <v>1088</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="49" t="s">
         <v>1720</v>
       </c>
     </row>
@@ -28555,7 +28562,7 @@
       <c r="E8" t="s">
         <v>1088</v>
       </c>
-      <c r="F8" s="50" t="s">
+      <c r="F8" s="49" t="s">
         <v>1720</v>
       </c>
     </row>
@@ -28575,7 +28582,7 @@
       <c r="E9" t="s">
         <v>1088</v>
       </c>
-      <c r="F9" s="50" t="s">
+      <c r="F9" s="49" t="s">
         <v>1720</v>
       </c>
     </row>
@@ -28811,7 +28818,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="50"/>
+      <c r="F22" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28834,8 +28841,8 @@
   <cols>
     <col min="1" max="1" width="13.140625" style="2" customWidth="1"/>
     <col min="2" max="3" width="39" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="48" customWidth="1"/>
-    <col min="5" max="20" width="6.7109375" style="48" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="47" customWidth="1"/>
+    <col min="5" max="20" width="6.7109375" style="47" customWidth="1"/>
     <col min="21" max="21" width="108.28515625" style="2" customWidth="1"/>
     <col min="22" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -28844,42 +28851,42 @@
       <c r="A2" s="24" t="s">
         <v>815</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="32" t="s">
         <v>816</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="32" t="s">
         <v>817</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="53" t="s">
         <v>818</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="55" t="s">
         <v>819</v>
       </c>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
       <c r="U2" s="24" t="s">
         <v>820</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="55"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="26" t="s">
         <v>821</v>
       </c>
@@ -28931,1623 +28938,1623 @@
       <c r="U3" s="27"/>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="34" t="s">
         <v>186</v>
       </c>
-      <c r="B4" s="36" t="str">
+      <c r="B4" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A4,city_details!A:A,0))</f>
         <v>Tricycle taxis, Cyclists and Pedestrians, Maiduguri, Nigeria</v>
       </c>
-      <c r="C4" s="36" t="str">
+      <c r="C4" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A4,city_details!A:A,0))</f>
         <v>Market</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="36" t="s">
         <v>823</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="36" t="s">
         <v>823</v>
       </c>
-      <c r="F4" s="38" t="s">
-        <v>824</v>
-      </c>
-      <c r="G4" s="38" t="s">
-        <v>824</v>
-      </c>
-      <c r="H4" s="38" t="s">
-        <v>824</v>
-      </c>
-      <c r="I4" s="38" t="s">
-        <v>824</v>
-      </c>
-      <c r="J4" s="38" t="s">
-        <v>824</v>
-      </c>
-      <c r="K4" s="42" t="s">
+      <c r="F4" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="H4" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="I4" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="K4" s="41" t="s">
         <v>1875</v>
       </c>
-      <c r="L4" s="38" t="s">
-        <v>824</v>
-      </c>
-      <c r="M4" s="38" t="s">
-        <v>824</v>
-      </c>
-      <c r="N4" s="38" t="s">
-        <v>824</v>
-      </c>
-      <c r="O4" s="38" t="s">
-        <v>824</v>
-      </c>
-      <c r="P4" s="38" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q4" s="38" t="s">
-        <v>824</v>
-      </c>
-      <c r="R4" s="38" t="s">
-        <v>824</v>
-      </c>
-      <c r="S4" s="38" t="s">
-        <v>824</v>
-      </c>
-      <c r="T4" s="38" t="s">
-        <v>824</v>
-      </c>
-      <c r="U4" s="40"/>
+      <c r="L4" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="M4" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="N4" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="O4" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="P4" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q4" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="R4" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="S4" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="T4" s="37" t="s">
+        <v>824</v>
+      </c>
+      <c r="U4" s="39"/>
     </row>
     <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="40" t="s">
         <v>181</v>
       </c>
-      <c r="B5" s="36" t="str">
+      <c r="B5" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A5,city_details!A:A,0))</f>
         <v>Pedestrian street</v>
       </c>
-      <c r="C5" s="36" t="str">
+      <c r="C5" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A5,city_details!A:A,0))</f>
         <v>Bus Rapid Transit "Metrobus", Mexico City, Mexico</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F5" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G5" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H5" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I5" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J5" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K5" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L5" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M5" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N5" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O5" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P5" s="39" t="s">
+      <c r="F5" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H5" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I5" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J5" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K5" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L5" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M5" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N5" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O5" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P5" s="38" t="s">
         <v>823</v>
       </c>
-      <c r="Q5" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R5" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S5" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T5" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U5" s="43"/>
+      <c r="Q5" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R5" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S5" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T5" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U5" s="42"/>
     </row>
     <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="40" t="s">
         <v>187</v>
       </c>
-      <c r="B6" s="36" t="str">
+      <c r="B6" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A6,city_details!A:A,0))</f>
         <v>Fed Hill Park</v>
       </c>
-      <c r="C6" s="36" t="str">
+      <c r="C6" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A6,city_details!A:A,0))</f>
         <v>Safe Signage Bike Lane Roland</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F6" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G6" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H6" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I6" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J6" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K6" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L6" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M6" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N6" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O6" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P6" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q6" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R6" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S6" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T6" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U6" s="43"/>
+      <c r="F6" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K6" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L6" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M6" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N6" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O6" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P6" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q6" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R6" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S6" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T6" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U6" s="42"/>
     </row>
     <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="40" t="s">
         <v>188</v>
       </c>
-      <c r="B7" s="36" t="str">
+      <c r="B7" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A7,city_details!A:A,0))</f>
         <v xml:space="preserve">Cyclist Near Hance Park in Downtown Phoenix, Arizona </v>
       </c>
-      <c r="C7" s="36" t="str">
+      <c r="C7" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A7,city_details!A:A,0))</f>
         <v>Pedestrians and cycleway in downtown Phoenix, Arizona</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F7" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G7" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H7" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I7" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J7" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K7" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L7" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M7" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N7" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O7" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P7" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q7" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R7" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S7" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T7" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U7" s="43"/>
+      <c r="F7" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G7" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H7" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I7" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K7" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L7" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M7" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N7" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O7" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P7" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q7" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R7" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S7" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T7" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U7" s="42"/>
     </row>
     <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="B8" s="36" t="str">
+      <c r="B8" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A8,city_details!A:A,0))</f>
         <v>Sunset pedestrians</v>
       </c>
-      <c r="C8" s="36" t="str">
+      <c r="C8" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A8,city_details!A:A,0))</f>
         <v>Leafy Pioneer Sq area</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F8" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G8" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H8" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I8" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J8" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K8" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L8" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M8" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N8" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O8" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P8" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q8" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R8" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S8" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T8" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U8" s="43"/>
+      <c r="F8" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G8" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H8" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J8" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K8" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L8" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M8" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N8" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O8" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P8" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q8" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R8" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S8" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T8" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U8" s="42"/>
     </row>
     <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="40" t="s">
         <v>190</v>
       </c>
-      <c r="B9" s="36" t="str">
+      <c r="B9" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A9,city_details!A:A,0))</f>
         <v>MASP Museum, Paulista Avenue, Sunday</v>
       </c>
-      <c r="C9" s="36" t="str">
+      <c r="C9" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A9,city_details!A:A,0))</f>
         <v>São Paulo cycling</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F9" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G9" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H9" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I9" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J9" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K9" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L9" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M9" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N9" s="39" t="s">
+      <c r="F9" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H9" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I9" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K9" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L9" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M9" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N9" s="38" t="s">
         <v>823</v>
       </c>
-      <c r="O9" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P9" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q9" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R9" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S9" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T9" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U9" s="43"/>
+      <c r="O9" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P9" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q9" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R9" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S9" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T9" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U9" s="42"/>
     </row>
     <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="40" t="s">
         <v>191</v>
       </c>
-      <c r="B10" s="36" t="str">
+      <c r="B10" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A10,city_details!A:A,0))</f>
         <v>Hong Kong skyline as seen from the West Kowloon Cultural District</v>
       </c>
-      <c r="C10" s="36" t="str">
+      <c r="C10" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A10,city_details!A:A,0))</f>
         <v>Avenue of Stars with the Hong Kong skyline in the background</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F10" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G10" s="42" t="s">
+      <c r="F10" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G10" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="H10" s="42" t="s">
+      <c r="H10" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="I10" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J10" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K10" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L10" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M10" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N10" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O10" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P10" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q10" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R10" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S10" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T10" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U10" s="43"/>
+      <c r="I10" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K10" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L10" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M10" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N10" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O10" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P10" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q10" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R10" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S10" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T10" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U10" s="42"/>
     </row>
     <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="40" t="s">
         <v>192</v>
       </c>
-      <c r="B11" s="36" t="str">
+      <c r="B11" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A11,city_details!A:A,0))</f>
         <v>Chennai pedestrian street scene</v>
       </c>
-      <c r="C11" s="36" t="str">
+      <c r="C11" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A11,city_details!A:A,0))</f>
         <v>Chennai pedestrian street scene</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F11" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H11" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I11" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J11" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K11" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L11" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M11" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N11" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O11" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P11" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q11" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R11" s="42" t="s">
+      <c r="F11" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H11" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I11" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J11" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K11" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L11" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M11" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N11" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O11" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P11" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q11" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R11" s="41" t="s">
         <v>1875</v>
       </c>
-      <c r="S11" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T11" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U11" s="43"/>
+      <c r="S11" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T11" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U11" s="42"/>
     </row>
     <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="B12" s="36" t="str">
+      <c r="B12" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A12,city_details!A:A,0))</f>
         <v>Chao Phraya and Bangkok skyline</v>
       </c>
-      <c r="C12" s="36" t="str">
+      <c r="C12" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A12,city_details!A:A,0))</f>
         <v>Lumphini Park, Bangkok</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F12" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G12" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H12" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I12" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J12" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K12" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L12" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M12" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N12" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O12" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P12" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q12" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R12" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S12" s="42" t="s">
+      <c r="F12" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H12" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I12" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K12" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L12" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M12" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N12" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O12" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P12" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q12" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R12" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S12" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="T12" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U12" s="43"/>
+      <c r="T12" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U12" s="42"/>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="40" t="s">
         <v>193</v>
       </c>
-      <c r="B13" s="36" t="str">
+      <c r="B13" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A13,city_details!A:A,0))</f>
         <v>Hoan Kiem Lake, Hanoi, Viet Nam</v>
       </c>
-      <c r="C13" s="36" t="str">
+      <c r="C13" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A13,city_details!A:A,0))</f>
         <v>Pedestrians gather to watch a street performance on Trang Tien St, Hanoi Vietnam</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F13" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G13" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H13" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I13" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J13" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K13" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L13" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M13" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N13" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O13" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P13" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q13" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R13" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S13" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T13" s="39" t="s">
+      <c r="F13" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H13" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I13" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J13" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K13" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L13" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M13" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N13" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O13" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P13" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q13" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R13" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S13" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T13" s="38" t="s">
         <v>823</v>
       </c>
-      <c r="U13" s="43"/>
+      <c r="U13" s="42"/>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="B14" s="53" t="str">
+      <c r="B14" s="52" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A14,city_details!A:A,0))</f>
         <v>candidates sent, none chosen</v>
       </c>
-      <c r="C14" s="53" t="str">
+      <c r="C14" s="52" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A14,city_details!A:A,0))</f>
         <v>candidates sent, none chosen</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F14" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H14" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I14" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="L14" s="42" t="s">
+      <c r="F14" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H14" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="L14" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="M14" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="N14" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O14" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P14" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q14" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R14" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S14" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T14" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U14" s="43"/>
+      <c r="M14" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="N14" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O14" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P14" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q14" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R14" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S14" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T14" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U14" s="42"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="40" t="s">
         <v>195</v>
       </c>
-      <c r="B15" s="36" t="str">
+      <c r="B15" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A15,city_details!A:A,0))</f>
         <v>VisitReeks01</v>
       </c>
-      <c r="C15" s="36" t="str">
+      <c r="C15" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A15,city_details!A:A,0))</f>
         <v>Groenevalleipark</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F15" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G15" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H15" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I15" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J15" s="42" t="s">
+      <c r="F15" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G15" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H15" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I15" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J15" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="K15" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L15" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M15" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N15" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O15" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P15" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q15" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R15" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S15" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T15" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U15" s="43"/>
+      <c r="K15" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L15" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M15" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N15" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O15" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P15" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q15" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R15" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S15" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T15" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U15" s="42"/>
     </row>
     <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="40" t="s">
         <v>196</v>
       </c>
-      <c r="B16" s="53" t="str">
+      <c r="B16" s="52" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A16,city_details!A:A,0))</f>
         <v>candidates sent, none chosen</v>
       </c>
-      <c r="C16" s="53" t="str">
+      <c r="C16" s="52" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A16,city_details!A:A,0))</f>
         <v>candidates sent, none chosen</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F16" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G16" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H16" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I16" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J16" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K16" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="L16" s="42" t="s">
+      <c r="F16" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G16" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H16" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I16" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J16" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K16" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="L16" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="M16" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="N16" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O16" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P16" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q16" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R16" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S16" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T16" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U16" s="43" t="s">
+      <c r="M16" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="N16" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O16" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P16" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q16" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R16" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S16" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T16" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U16" s="42" t="s">
         <v>826</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="40" t="s">
         <v>197</v>
       </c>
-      <c r="B17" s="36" t="str">
+      <c r="B17" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A17,city_details!A:A,0))</f>
         <v>Namesti Hrdinu, Olomouc, Czechia</v>
       </c>
-      <c r="C17" s="36" t="str">
+      <c r="C17" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A17,city_details!A:A,0))</f>
         <v>Tabulovy vrch, Olomouc, Czechia</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F17" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G17" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H17" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I17" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J17" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K17" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L17" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M17" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N17" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O17" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P17" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q17" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R17" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S17" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T17" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U17" s="43"/>
+      <c r="F17" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H17" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I17" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J17" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K17" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L17" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M17" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N17" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O17" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P17" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q17" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R17" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S17" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T17" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U17" s="42"/>
     </row>
     <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="40" t="s">
         <v>198</v>
       </c>
-      <c r="B18" s="53" t="str">
+      <c r="B18" s="52" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A18,city_details!A:A,0))</f>
         <v>candidates sent, none chosen</v>
       </c>
-      <c r="C18" s="53" t="str">
+      <c r="C18" s="52" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A18,city_details!A:A,0))</f>
         <v>candidates sent, none chosen</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F18" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G18" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H18" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I18" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J18" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K18" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="L18" s="42" t="s">
+      <c r="F18" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G18" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H18" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I18" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J18" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K18" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="L18" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="M18" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="N18" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O18" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P18" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q18" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R18" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S18" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T18" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U18" s="43"/>
+      <c r="M18" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="N18" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O18" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P18" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q18" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R18" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S18" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T18" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U18" s="42"/>
     </row>
     <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="40" t="s">
         <v>199</v>
       </c>
-      <c r="B19" s="36" t="str">
+      <c r="B19" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A19,city_details!A:A,0))</f>
         <v>Odense Lightrail</v>
       </c>
-      <c r="C19" s="36" t="str">
+      <c r="C19" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A19,city_details!A:A,0))</f>
         <v>Summer in the city</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F19" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G19" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H19" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I19" s="42" t="s">
+      <c r="F19" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G19" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H19" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I19" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="J19" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K19" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L19" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M19" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N19" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O19" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P19" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q19" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R19" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S19" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T19" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U19" s="43"/>
+      <c r="J19" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K19" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L19" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M19" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N19" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O19" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P19" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q19" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R19" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S19" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T19" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U19" s="42"/>
     </row>
     <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="40" t="s">
         <v>200</v>
       </c>
-      <c r="B20" s="36" t="str">
+      <c r="B20" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A20,city_details!A:A,0))</f>
         <v>Bike, scooter and pedestrians on Carrer de la Diputació at the intersection of Carrer d'Enric Granados, Barcelona</v>
       </c>
-      <c r="C20" s="36" t="str">
+      <c r="C20" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A20,city_details!A:A,0))</f>
         <v>Pedestrians and bikes on Carrer Astúries, Barcelona</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="E20" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F20" s="42" t="s">
+      <c r="F20" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="G20" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H20" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I20" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J20" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K20" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L20" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M20" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N20" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O20" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P20" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q20" s="39" t="s">
+      <c r="G20" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H20" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I20" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J20" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K20" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L20" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M20" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N20" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O20" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P20" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q20" s="38" t="s">
         <v>823</v>
       </c>
-      <c r="R20" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S20" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T20" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U20" s="43"/>
+      <c r="R20" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S20" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T20" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U20" s="42"/>
     </row>
     <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="40" t="s">
         <v>201</v>
       </c>
-      <c r="B21" s="53" t="str">
+      <c r="B21" s="52" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A21,city_details!A:A,0))</f>
         <v>To be updated on sunny day</v>
       </c>
-      <c r="C21" s="53" t="str">
+      <c r="C21" s="52" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A21,city_details!A:A,0))</f>
         <v>To be updated on sunny day</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F21" s="42" t="s">
+      <c r="F21" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="G21" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H21" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I21" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J21" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K21" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L21" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M21" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N21" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O21" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P21" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q21" s="39" t="s">
+      <c r="G21" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H21" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I21" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J21" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K21" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L21" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M21" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N21" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O21" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P21" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q21" s="38" t="s">
         <v>823</v>
       </c>
-      <c r="R21" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S21" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T21" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U21" s="43"/>
+      <c r="R21" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S21" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T21" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U21" s="42"/>
     </row>
     <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="40" t="s">
         <v>202</v>
       </c>
-      <c r="B22" s="36" t="str">
+      <c r="B22" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A22,city_details!A:A,0))</f>
         <v>Cycle way road, Vic</v>
       </c>
-      <c r="C22" s="36" t="str">
+      <c r="C22" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A22,city_details!A:A,0))</f>
         <v>Vic market</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E22" s="42" t="s">
+      <c r="E22" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F22" s="42" t="s">
+      <c r="F22" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="G22" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H22" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I22" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J22" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K22" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L22" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M22" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N22" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O22" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P22" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q22" s="39" t="s">
+      <c r="G22" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H22" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I22" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J22" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K22" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L22" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M22" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N22" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O22" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P22" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q22" s="38" t="s">
         <v>823</v>
       </c>
-      <c r="R22" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S22" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T22" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U22" s="43"/>
+      <c r="R22" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S22" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T22" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U22" s="42"/>
     </row>
     <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="B23" s="36" t="str">
+      <c r="B23" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A23,city_details!A:A,0))</f>
         <v>Dixon Hollow, Connswater Community Greenway, Belfast</v>
       </c>
-      <c r="C23" s="36" t="str">
+      <c r="C23" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A23,city_details!A:A,0))</f>
         <v>Family cycle ride along the Connswater Community Greenway</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E23" s="42" t="s">
+      <c r="E23" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F23" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G23" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H23" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I23" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J23" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K23" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L23" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M23" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N23" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O23" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P23" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q23" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R23" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S23" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T23" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U23" s="43"/>
+      <c r="F23" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G23" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H23" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I23" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J23" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K23" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L23" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M23" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N23" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O23" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P23" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q23" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R23" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S23" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T23" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U23" s="42"/>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="40" t="s">
         <v>204</v>
       </c>
-      <c r="B24" s="36" t="str">
+      <c r="B24" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A24,city_details!A:A,0))</f>
         <v>Pedestrians in Rua Garrett, Lisboa, Portugal</v>
       </c>
-      <c r="C24" s="36" t="str">
+      <c r="C24" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A24,city_details!A:A,0))</f>
         <v>Av. Duque de Ávila, Lisboa, Portugal</v>
       </c>
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E24" s="42" t="s">
+      <c r="E24" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F24" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G24" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H24" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I24" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J24" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K24" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L24" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M24" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N24" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O24" s="42" t="s">
+      <c r="F24" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G24" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H24" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I24" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J24" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K24" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L24" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M24" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N24" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O24" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="P24" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q24" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R24" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S24" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T24" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U24" s="43"/>
+      <c r="P24" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q24" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R24" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S24" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T24" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U24" s="42"/>
     </row>
     <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="41" t="s">
+      <c r="A25" s="40" t="s">
         <v>205</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="42" t="s">
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E25" s="42" t="s">
+      <c r="E25" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F25" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G25" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H25" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I25" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J25" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K25" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L25" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M25" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N25" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O25" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P25" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q25" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R25" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S25" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T25" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U25" s="43"/>
+      <c r="F25" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G25" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H25" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I25" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J25" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K25" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L25" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M25" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N25" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O25" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P25" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q25" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R25" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S25" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T25" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U25" s="42"/>
     </row>
     <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="40" t="s">
         <v>178</v>
       </c>
-      <c r="B26" s="36" t="str">
+      <c r="B26" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A26,city_details!A:A,0))</f>
         <v>Pedestrians on Swanston St</v>
       </c>
-      <c r="C26" s="36" t="str">
+      <c r="C26" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A26,city_details!A:A,0))</f>
         <v>Brunswick neighbourhood</v>
       </c>
-      <c r="D26" s="42" t="s">
+      <c r="D26" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E26" s="42" t="s">
+      <c r="E26" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F26" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G26" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H26" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I26" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J26" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K26" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L26" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M26" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N26" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O26" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P26" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q26" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R26" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S26" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T26" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U26" s="43"/>
+      <c r="F26" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G26" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H26" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I26" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J26" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K26" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L26" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M26" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N26" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O26" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P26" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q26" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R26" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S26" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T26" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U26" s="42"/>
     </row>
     <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="B27" s="36" t="str">
+      <c r="B27" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A27,city_details!A:A,0))</f>
         <v>Sydney botanical gardens</v>
       </c>
-      <c r="C27" s="36" t="str">
+      <c r="C27" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A27,city_details!A:A,0))</f>
         <v>Sydney harbourside</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="E27" s="42" t="s">
+      <c r="E27" s="41" t="s">
         <v>823</v>
       </c>
-      <c r="F27" s="42" t="s">
-        <v>824</v>
-      </c>
-      <c r="G27" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="H27" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="I27" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="J27" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="K27" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="L27" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="M27" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="N27" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="O27" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="P27" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q27" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="R27" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="S27" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="T27" s="39" t="s">
-        <v>824</v>
-      </c>
-      <c r="U27" s="43"/>
+      <c r="F27" s="41" t="s">
+        <v>824</v>
+      </c>
+      <c r="G27" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="H27" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="I27" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="J27" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="K27" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="L27" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="M27" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="N27" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="O27" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="P27" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q27" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="R27" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="S27" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="T27" s="38" t="s">
+        <v>824</v>
+      </c>
+      <c r="U27" s="42"/>
     </row>
     <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="43" t="s">
         <v>207</v>
       </c>
-      <c r="B28" s="36" t="str">
+      <c r="B28" s="35" t="str">
         <f>INDEX(city_details!D:D,MATCH('City tasks for scorecards'!A28,city_details!A:A,0))</f>
         <v>Auckland park</v>
       </c>
-      <c r="C28" s="36" t="str">
+      <c r="C28" s="35" t="str">
         <f>INDEX(city_details!F:F,MATCH('City tasks for scorecards'!A28,city_details!A:A,0))</f>
         <v>Auckland park</v>
       </c>
-      <c r="D28" s="45" t="s">
+      <c r="D28" s="44" t="s">
         <v>823</v>
       </c>
-      <c r="E28" s="45" t="s">
+      <c r="E28" s="44" t="s">
         <v>823</v>
       </c>
-      <c r="F28" s="45" t="s">
-        <v>824</v>
-      </c>
-      <c r="G28" s="46" t="s">
-        <v>824</v>
-      </c>
-      <c r="H28" s="46" t="s">
-        <v>824</v>
-      </c>
-      <c r="I28" s="46" t="s">
-        <v>824</v>
-      </c>
-      <c r="J28" s="46" t="s">
-        <v>824</v>
-      </c>
-      <c r="K28" s="46" t="s">
-        <v>824</v>
-      </c>
-      <c r="L28" s="46" t="s">
-        <v>824</v>
-      </c>
-      <c r="M28" s="42" t="s">
+      <c r="F28" s="44" t="s">
+        <v>824</v>
+      </c>
+      <c r="G28" s="45" t="s">
+        <v>824</v>
+      </c>
+      <c r="H28" s="45" t="s">
+        <v>824</v>
+      </c>
+      <c r="I28" s="45" t="s">
+        <v>824</v>
+      </c>
+      <c r="J28" s="45" t="s">
+        <v>824</v>
+      </c>
+      <c r="K28" s="45" t="s">
+        <v>824</v>
+      </c>
+      <c r="L28" s="45" t="s">
+        <v>824</v>
+      </c>
+      <c r="M28" s="41" t="s">
         <v>825</v>
       </c>
-      <c r="N28" s="46" t="s">
-        <v>824</v>
-      </c>
-      <c r="O28" s="46" t="s">
-        <v>824</v>
-      </c>
-      <c r="P28" s="46" t="s">
-        <v>824</v>
-      </c>
-      <c r="Q28" s="46" t="s">
-        <v>824</v>
-      </c>
-      <c r="R28" s="46" t="s">
-        <v>824</v>
-      </c>
-      <c r="S28" s="46" t="s">
-        <v>824</v>
-      </c>
-      <c r="T28" s="46" t="s">
-        <v>824</v>
-      </c>
-      <c r="U28" s="47"/>
+      <c r="N28" s="45" t="s">
+        <v>824</v>
+      </c>
+      <c r="O28" s="45" t="s">
+        <v>824</v>
+      </c>
+      <c r="P28" s="45" t="s">
+        <v>824</v>
+      </c>
+      <c r="Q28" s="45" t="s">
+        <v>824</v>
+      </c>
+      <c r="R28" s="45" t="s">
+        <v>824</v>
+      </c>
+      <c r="S28" s="45" t="s">
+        <v>824</v>
+      </c>
+      <c r="T28" s="45" t="s">
+        <v>824</v>
+      </c>
+      <c r="U28" s="46"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="U29" s="2" t="str">

</xml_diff>

<commit_message>
minor code change to better accomodate switching of templates, when a new print template is added, as per #14  (ran code and confirmed working same as intended)
</commit_message>
<xml_diff>
--- a/scorecard_template_elements.xlsx
+++ b/scorecard_template_elements.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/analysis/global_scorecards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2592" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{539761EB-8734-498A-BF21-8B59B092FFE9}"/>
+  <xr:revisionPtr revIDLastSave="2593" documentId="13_ncr:1_{359C2F2A-CF47-4184-8CC1-6CC8B0EC5B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C31EA629-BCF8-4D1D-BC36-BA523D022439}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="scorecard_template_elements" sheetId="1" r:id="rId1"/>
+    <sheet name="template_web" sheetId="1" r:id="rId1"/>
     <sheet name="languages" sheetId="2" r:id="rId2"/>
     <sheet name="city_details" sheetId="6" r:id="rId3"/>
     <sheet name="fonts" sheetId="3" r:id="rId4"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">languages!$B$1:$N$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scorecard_template_elements!$A$1:$T$192</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">template_web!$A$1:$T$192</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -7610,8 +7610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V195"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B143" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G182" sqref="G182"/>
@@ -7729,7 +7729,7 @@
         <v>22</v>
       </c>
       <c r="P2" t="str">
-        <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(scorecard_template_elements!A2,languages!B:B,0)),"")</f>
+        <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(template_web!A2,languages!B:B,0)),"")</f>
         <v>{city}, {country}</v>
       </c>
       <c r="Q2">
@@ -7793,7 +7793,7 @@
         <v>22</v>
       </c>
       <c r="P3" t="str">
-        <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(scorecard_template_elements!A3,languages!B:B,0)),"")</f>
+        <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(template_web!A3,languages!B:B,0)),"")</f>
         <v>{city}, {country}</v>
       </c>
       <c r="Q3">
@@ -7857,7 +7857,7 @@
         <v>22</v>
       </c>
       <c r="P4" t="str">
-        <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(scorecard_template_elements!A4,languages!B:B,0)),"")</f>
+        <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(template_web!A4,languages!B:B,0)),"")</f>
         <v>{city}, {country}</v>
       </c>
       <c r="Q4">
@@ -7921,7 +7921,7 @@
         <v>22</v>
       </c>
       <c r="P5" t="str">
-        <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(scorecard_template_elements!A5,languages!B:B,0)),"")</f>
+        <f>_xlfn.IFNA(INDEX(languages!C:C,MATCH(template_web!A5,languages!B:B,0)),"")</f>
         <v>{city}, {country}</v>
       </c>
       <c r="Q5">
@@ -19191,7 +19191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V170"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>